<commit_message>
add bar figures for clang
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,13 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="162" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{C1E3FE52-12C3-4378-8BE1-DE66EA3F8D83}"/>
+  <xr:revisionPtr revIDLastSave="207" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{D0E05F98-814C-4157-A6EE-D345160BC39E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
-    <sheet name="clang" sheetId="1" r:id="rId2"/>
+    <sheet name="clang-1" sheetId="3" r:id="rId1"/>
+    <sheet name="clang-2" sheetId="4" r:id="rId2"/>
+    <sheet name="clang-3" sheetId="5" r:id="rId3"/>
+    <sheet name="clang" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -102,9 +104,6 @@
     <t>Shared ptp</t>
   </si>
   <si>
-    <t>Improvement % (shared ptp / baseline)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Std. dev. </t>
   </si>
   <si>
@@ -112,9 +111,6 @@
   </si>
   <si>
     <t xml:space="preserve">Average </t>
-  </si>
-  <si>
-    <t>std dev. %</t>
   </si>
   <si>
     <t>baseline (Col C/Col B)</t>
@@ -159,18 +155,25 @@
     <t>Super Page</t>
   </si>
   <si>
-    <t>Improvement % (super page / baseline)</t>
+    <t>super_page (col G/col B)</t>
   </si>
   <si>
-    <t>super_page (col G/col B)</t>
+    <t>std dev. (fraction)</t>
+  </si>
+  <si>
+    <t>shared ptp / baseline</t>
+  </si>
+  <si>
+    <t>super page / baseline</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -226,12 +229,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -239,9 +241,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -255,11 +255,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -313,9 +313,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>clang!$A$5:$A$37</c:f>
+              <c:f>clang!$A$5:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="33"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>PAGE_FAULT.ALL</c:v>
                 </c:pt>
@@ -348,187 +348,55 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v> DTLB_LOAD_MISSES.STLB_HIT </c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>DTLB_STORE_MISSES.MISS_CAUSES_A_WALK</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>DTLB_STORE_MISSES.WALK_COMPLETED</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>DTLB_STORE_MISSES.WALK_PENDING</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v> DTLB_STORE_MISSES.STLB_HIT </c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>MEM_UOPS_RETIRED.STLB_MISS_LOADS</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>MEM_UOPS_RETIRED.STLB_MISS_STORES</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>L1D_PEND_MISS.PENDING</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>L2_RQSTS.DEMAND_DATA_RD_MISS</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>L2_RQSTS.RFO_MISS</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>L2_RQSTS.CODE_RD_MISS</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>L2_RQSTS.ALL_DEMAND_MISS</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>L2_RQSTS.PF_MISS</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>L2_RQSTS.MISS</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>llc-misses</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>OFFCORE_REQUESTS.L3_MISS_DEMAND_DATA_RD</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>CYCLE_ACTIVITY.CYCLES_L1D_MISS</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>CYCLE_ACTIVITY.CYCLES_L2_MISS</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>CYCLE_ACTIVITY.CYCLES_L3_MISS</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>CYCLE_ACTIVITY.CYCLES_MEM_ANY</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>MEM_UOPS_RETIRED.ALL_LOADS</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>MEM_UOPS_RETIRED.ALL_STORES</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>ITLB.ITLB_FLUSH</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>clang!$H$5:$H$37</c:f>
+              <c:f>clang!$H$5:$H$15</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-4.4860825822952949E-2</c:v>
+                  <c:v>1.044860825822953</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18948907056069716</c:v>
+                  <c:v>0.81051092943930281</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15247335129807482</c:v>
+                  <c:v>0.84752664870192518</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41628025382962691</c:v>
+                  <c:v>0.58371974617037303</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.42232907831858063</c:v>
+                  <c:v>0.57767092168141942</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.48526970176401646</c:v>
+                  <c:v>0.5147302982359836</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.3934506735885173E-2</c:v>
+                  <c:v>1.0939345067358852</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.24107293035794211</c:v>
+                  <c:v>0.75892706964205792</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.28985942492651895</c:v>
+                  <c:v>0.71014057507348105</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.31684337032445897</c:v>
+                  <c:v>0.68315662967554103</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.24970625416450079</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-4.863323117838312E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-5.2409216674243538E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-2.000260623699769E-4</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-0.14644479699836685</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.259103850475036E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-2.420262228498931E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-3.5375437982295768E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-3.4742853505272783E-3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.9619928911988667E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-7.0380861164368702E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-2.6949414042711995E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.17297425116454435</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9.7501351459879509E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.17488701855787817</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.14978806507995132</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>-1.2193324387846276E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>4.9078571347687339E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>9.7646754264358274E-2</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.15247666324284623</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.21521373730691776</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.19141058265822045</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>-4.3593614374334538E-2</c:v>
+                  <c:v>0.75029374583549924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B35F-4EFB-93BE-4503F66A6546}"/>
+              <c16:uniqueId val="{00000000-F7C8-4AF3-A9A2-1A50C3DA7C30}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -550,9 +418,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>clang!$A$5:$A$37</c:f>
+              <c:f>clang!$A$5:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="33"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>PAGE_FAULT.ALL</c:v>
                 </c:pt>
@@ -585,187 +453,55 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v> DTLB_LOAD_MISSES.STLB_HIT </c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>DTLB_STORE_MISSES.MISS_CAUSES_A_WALK</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>DTLB_STORE_MISSES.WALK_COMPLETED</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>DTLB_STORE_MISSES.WALK_PENDING</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v> DTLB_STORE_MISSES.STLB_HIT </c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>MEM_UOPS_RETIRED.STLB_MISS_LOADS</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>MEM_UOPS_RETIRED.STLB_MISS_STORES</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>L1D_PEND_MISS.PENDING</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>L2_RQSTS.DEMAND_DATA_RD_MISS</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>L2_RQSTS.RFO_MISS</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>L2_RQSTS.CODE_RD_MISS</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>L2_RQSTS.ALL_DEMAND_MISS</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>L2_RQSTS.PF_MISS</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>L2_RQSTS.MISS</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>llc-misses</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>OFFCORE_REQUESTS.L3_MISS_DEMAND_DATA_RD</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>CYCLE_ACTIVITY.CYCLES_L1D_MISS</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>CYCLE_ACTIVITY.CYCLES_L2_MISS</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>CYCLE_ACTIVITY.CYCLES_L3_MISS</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>CYCLE_ACTIVITY.CYCLES_MEM_ANY</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>MEM_UOPS_RETIRED.ALL_LOADS</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>MEM_UOPS_RETIRED.ALL_STORES</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>ITLB.ITLB_FLUSH</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>clang!$I$5:$I$37</c:f>
+              <c:f>clang!$I$5:$I$15</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2.9283232161041221E-2</c:v>
+                  <c:v>0.97071676783895877</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24414482233798318</c:v>
+                  <c:v>0.75585517766201682</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22450702579275056</c:v>
+                  <c:v>0.7754929742072495</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.86341993002718675</c:v>
+                  <c:v>0.13658006997281327</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.90822776881461031</c:v>
+                  <c:v>9.1772231185389685E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.88418891044406767</c:v>
+                  <c:v>0.1158110895559324</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.57578421495130949</c:v>
+                  <c:v>0.42421578504869056</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.50743051941153461</c:v>
+                  <c:v>0.49256948058846534</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.73041581286463397</c:v>
+                  <c:v>0.26958418713536597</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.64348435145058025</c:v>
+                  <c:v>0.35651564854941975</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.61073379990116994</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.6828584084230464E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8.601808003660967E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.10304745668947624</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.47697367675896807</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.73414546085180332</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.16636829339264575</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-0.39880860188709116</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-0.30237784650289645</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>8.6057154250921017E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-2.3178468876686606E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-3.9069227520122762E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.29211220993754289</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.16722710687100004</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.17011655945642648</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-0.19696797211811526</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.11151529586246686</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3.1822694769619701E-3</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-2.8051249864027187E-2</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.22475528390090829</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.27002725125022381</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.24157326657711808</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.54298914947776911</c:v>
+                  <c:v>0.38926620009883006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B35F-4EFB-93BE-4503F66A6546}"/>
+              <c16:uniqueId val="{00000001-F7C8-4AF3-A9A2-1A50C3DA7C30}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -779,11 +515,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="898513040"/>
-        <c:axId val="898511400"/>
+        <c:axId val="793997560"/>
+        <c:axId val="793993624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="898513040"/>
+        <c:axId val="793997560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,7 +547,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -826,7 +562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="898511400"/>
+        <c:crossAx val="793993624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -834,7 +570,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="898511400"/>
+        <c:axId val="793993624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -861,7 +597,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -875,11 +611,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Improvement</a:t>
+                  <a:t>Normalized</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> over the base kernel</a:t>
+                  <a:t> to the baseilne</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -898,7 +634,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -914,7 +650,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -930,7 +666,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -945,7 +681,484 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="898513040"/>
+        <c:crossAx val="793997560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="2000"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>shared_ptp</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>clang!$A$16:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>DTLB_STORE_MISSES.MISS_CAUSES_A_WALK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DTLB_STORE_MISSES.WALK_COMPLETED</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DTLB_STORE_MISSES.WALK_PENDING</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> DTLB_STORE_MISSES.STLB_HIT </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MEM_UOPS_RETIRED.STLB_MISS_LOADS</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MEM_UOPS_RETIRED.STLB_MISS_STORES</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>L1D_PEND_MISS.PENDING</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>L2_RQSTS.DEMAND_DATA_RD_MISS</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>L2_RQSTS.RFO_MISS</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>L2_RQSTS.CODE_RD_MISS</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>L2_RQSTS.ALL_DEMAND_MISS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>clang!$H$16:$H$26</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.048633231178383</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0524092166742436</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.00020002606237</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85355520300163312</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9774089614952497</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0242026222849894</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0353754379822957</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0034742853505272</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.98038007108801128</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0703808611643688</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.026949414042712</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BABD-4844-89CA-D58C5ED593EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>super_page</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>clang!$A$16:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>DTLB_STORE_MISSES.MISS_CAUSES_A_WALK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DTLB_STORE_MISSES.WALK_COMPLETED</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DTLB_STORE_MISSES.WALK_PENDING</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> DTLB_STORE_MISSES.STLB_HIT </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MEM_UOPS_RETIRED.STLB_MISS_LOADS</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MEM_UOPS_RETIRED.STLB_MISS_STORES</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>L1D_PEND_MISS.PENDING</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>L2_RQSTS.DEMAND_DATA_RD_MISS</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>L2_RQSTS.RFO_MISS</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>L2_RQSTS.CODE_RD_MISS</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>L2_RQSTS.ALL_DEMAND_MISS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>clang!$I$16:$I$26</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.94317141591576958</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91398191996339029</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89695254331052376</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.52302632324103193</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26585453914819662</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.83363170660735419</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3988086018870911</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3023778465028963</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.91394284574907902</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0231784688766865</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0390692275201228</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BABD-4844-89CA-D58C5ED593EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="573268776"/>
+        <c:axId val="573269760"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="573268776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="573269760"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="573269760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1500"/>
+                  <a:t>Norliazed to the baseline</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="573268776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1020,7 +1233,569 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>shared_ptp</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>clang!$A$27:$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>L2_RQSTS.PF_MISS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>L2_RQSTS.MISS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>llc-misses</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>OFFCORE_REQUESTS.L3_MISS_DEMAND_DATA_RD</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CYCLE_ACTIVITY.CYCLES_L1D_MISS</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CYCLE_ACTIVITY.CYCLES_L2_MISS</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>CYCLE_ACTIVITY.CYCLES_L3_MISS</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>CYCLE_ACTIVITY.CYCLES_MEM_ANY</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MEM_UOPS_RETIRED.ALL_LOADS</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>MEM_UOPS_RETIRED.ALL_STORES</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>ITLB.ITLB_FLUSH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>clang!$H$27:$H$37</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.82702574883545565</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90249864854012052</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.82511298144212186</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.85021193492004865</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0121933243878463</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95092142865231266</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.90235324573564168</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.84752333675715374</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.78478626269308227</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.80858941734177958</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0435936143743345</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4998-493F-AAE0-22FAC38E88A8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>super_page</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>clang!$A$27:$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>L2_RQSTS.PF_MISS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>L2_RQSTS.MISS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>llc-misses</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>OFFCORE_REQUESTS.L3_MISS_DEMAND_DATA_RD</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CYCLE_ACTIVITY.CYCLES_L1D_MISS</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CYCLE_ACTIVITY.CYCLES_L2_MISS</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>CYCLE_ACTIVITY.CYCLES_L3_MISS</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>CYCLE_ACTIVITY.CYCLES_MEM_ANY</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>MEM_UOPS_RETIRED.ALL_LOADS</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>MEM_UOPS_RETIRED.ALL_STORES</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>ITLB.ITLB_FLUSH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>clang!$I$27:$I$37</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.70788779006245717</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83277289312899994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.82988344054357355</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1969679721181152</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88848470413753311</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99681773052303801</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0280512498640273</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.77524471609909174</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.72997274874977625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.75842673342288192</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.45701085052223084</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4998-493F-AAE0-22FAC38E88A8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="367769496"/>
+        <c:axId val="367769824"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="367769496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="367769824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="367769824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Normalized</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> to the baseline</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="367769496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1563,11 +2338,1039 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{796BB575-0175-487A-817A-DB4A779F8297}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{E9530A9A-1391-419E-A1EB-B57952BD057F}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" workbookViewId="0"/>
+    <sheetView zoomScale="91" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39218FA5-E567-4D80-A85E-694142D70167}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="91" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{2D12F0F9-E194-42A8-899D-E6197E229285}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1584,7 +3387,73 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF94D2E9-7B58-4023-9D8D-440FD2B6E495}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6A80051-F159-4407-BFCD-4CF6970A9C88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8661470" cy="6285453"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B31895C-A54E-4919-AF34-3F16748B938F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8661470" cy="6285453"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B669E86-6B6C-4B9C-9BE8-5F041570DE07}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1872,8 +3741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27:I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1892,64 +3761,64 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="11" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>46</v>
+      <c r="K4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
@@ -1968,29 +3837,29 @@
       <c r="E5" s="4">
         <v>63374.740610399997</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>10682599.800000001</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>4082.0953149100001</v>
       </c>
-      <c r="H5" s="5">
-        <f>(B5-D5)/B5</f>
-        <v>-4.4860825822952949E-2</v>
-      </c>
-      <c r="I5" s="5">
-        <f>(B5-F5)/B5</f>
-        <v>2.9283232161041221E-2</v>
-      </c>
-      <c r="J5" s="5">
+      <c r="H5" s="11">
+        <f>D5/B5</f>
+        <v>1.044860825822953</v>
+      </c>
+      <c r="I5" s="11">
+        <f>F5/B5</f>
+        <v>0.97071676783895877</v>
+      </c>
+      <c r="J5" s="11">
         <f>C5/B5</f>
         <v>3.9063064824936943E-3</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="11">
         <f>E5/B5</f>
         <v>5.7587969707486265E-3</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="11">
         <f>G5/B5</f>
         <v>3.7093576884720435E-4</v>
       </c>
@@ -2011,35 +3880,35 @@
       <c r="E6" s="4">
         <v>1644622126.3299999</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <v>283268225665</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="7">
         <v>240501278.76800001</v>
       </c>
-      <c r="H6" s="5">
-        <f>(B6-D6)/B6</f>
-        <v>0.18948907056069716</v>
-      </c>
-      <c r="I6" s="5">
-        <f t="shared" ref="I6:I37" si="0">(B6-F6)/B6</f>
-        <v>0.24414482233798318</v>
-      </c>
-      <c r="J6" s="5">
+      <c r="H6" s="11">
+        <f t="shared" ref="H6:H37" si="0">D6/B6</f>
+        <v>0.81051092943930281</v>
+      </c>
+      <c r="I6" s="11">
+        <f t="shared" ref="I6:I37" si="1">F6/B6</f>
+        <v>0.75585517766201682</v>
+      </c>
+      <c r="J6" s="11">
         <f>C6/B6</f>
         <v>3.9437970145817305E-3</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="11">
         <f>E6/B6</f>
         <v>4.3884065943709553E-3</v>
       </c>
-      <c r="L6" s="5">
-        <f t="shared" ref="L6:L37" si="1">G6/B6</f>
+      <c r="L6" s="11">
+        <f t="shared" ref="L6:L37" si="2">G6/B6</f>
         <v>6.4173853726224586E-4</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="4">
@@ -2054,30 +3923,30 @@
       <c r="E7" s="4">
         <v>1922594830.6800001</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <v>311181991364</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="7">
         <v>34689920.276299998</v>
       </c>
-      <c r="H7" s="7">
-        <f>(B7-D7)/B7</f>
-        <v>0.15247335129807482</v>
-      </c>
-      <c r="I7" s="5">
+      <c r="H7" s="11">
         <f t="shared" si="0"/>
-        <v>0.22450702579275056</v>
-      </c>
-      <c r="J7" s="5">
+        <v>0.84752664870192518</v>
+      </c>
+      <c r="I7" s="11">
+        <f t="shared" si="1"/>
+        <v>0.7754929742072495</v>
+      </c>
+      <c r="J7" s="11">
         <f>C7/B7</f>
         <v>4.604518976025926E-3</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="11">
         <f>E7/B7</f>
         <v>4.7912759247545657E-3</v>
       </c>
-      <c r="L7" s="5">
-        <f t="shared" si="1"/>
+      <c r="L7" s="11">
+        <f t="shared" si="2"/>
         <v>8.645034159001936E-5</v>
       </c>
     </row>
@@ -2097,73 +3966,73 @@
       <c r="E8" s="4">
         <v>432735.30819299998</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>18320543.800000001</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="7">
         <v>38405.694501700003</v>
       </c>
-      <c r="H8" s="5">
-        <f>(B8-D8)/B8</f>
-        <v>0.41628025382962691</v>
-      </c>
-      <c r="I8" s="5">
+      <c r="H8" s="11">
         <f t="shared" si="0"/>
-        <v>0.86341993002718675</v>
-      </c>
-      <c r="J8" s="5">
+        <v>0.58371974617037303</v>
+      </c>
+      <c r="I8" s="11">
+        <f t="shared" si="1"/>
+        <v>0.13658006997281327</v>
+      </c>
+      <c r="J8" s="11">
         <f>C8/B8</f>
         <v>4.4096319903338052E-3</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="11">
         <f>E8/B8</f>
         <v>3.226051547263944E-3</v>
       </c>
-      <c r="L8" s="5">
-        <f t="shared" si="1"/>
+      <c r="L8" s="11">
+        <f t="shared" si="2"/>
         <v>2.8631532446087525E-4</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="9">
+        <v>35</v>
+      </c>
+      <c r="B9" s="7">
         <v>99303188.799999997</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <v>392074.22467999998</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="7">
         <v>57364564.600000001</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="7">
         <v>220994.854758</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>9113275.1999999993</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>12871.3087664</v>
       </c>
-      <c r="H9" s="5">
-        <f>(B9-D9)/B9</f>
-        <v>0.42232907831858063</v>
-      </c>
-      <c r="I9" s="5">
+      <c r="H9" s="11">
         <f t="shared" si="0"/>
-        <v>0.90822776881461031</v>
-      </c>
-      <c r="J9" s="5">
+        <v>0.57767092168141942</v>
+      </c>
+      <c r="I9" s="11">
+        <f t="shared" si="1"/>
+        <v>9.1772231185389685E-2</v>
+      </c>
+      <c r="J9" s="11">
         <f>C9/B9</f>
         <v>3.948254123738673E-3</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="11">
         <f>E9/B9</f>
         <v>2.2254557726549061E-3</v>
       </c>
-      <c r="L9" s="5">
-        <f t="shared" si="1"/>
+      <c r="L9" s="11">
+        <f t="shared" si="2"/>
         <v>1.2961626833880686E-4</v>
       </c>
     </row>
@@ -2183,73 +4052,73 @@
       <c r="E10" s="4">
         <v>13604835.5052</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="7">
         <v>596797669.20000005</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="7">
         <v>7630087.2776699997</v>
       </c>
-      <c r="H10" s="5">
-        <f>(B10-D10)/B10</f>
-        <v>0.48526970176401646</v>
-      </c>
-      <c r="I10" s="5">
+      <c r="H10" s="11">
         <f t="shared" si="0"/>
-        <v>0.88418891044406767</v>
-      </c>
-      <c r="J10" s="5">
+        <v>0.5147302982359836</v>
+      </c>
+      <c r="I10" s="11">
+        <f t="shared" si="1"/>
+        <v>0.1158110895559324</v>
+      </c>
+      <c r="J10" s="11">
         <f>C10/B10</f>
         <v>3.3968885657673907E-3</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="11">
         <f>E10/B10</f>
         <v>2.6400753628922618E-3</v>
       </c>
-      <c r="L10" s="5">
-        <f t="shared" si="1"/>
+      <c r="L10" s="11">
+        <f t="shared" si="2"/>
         <v>1.4806504224762491E-3</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="9">
+      <c r="A11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="7">
         <v>52956603.200000003</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <v>36629.741328099997</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="7">
         <v>57931055.600000001</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="7">
         <v>165906.74316300001</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <v>22465027</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="7">
         <v>12980.253464400001</v>
       </c>
-      <c r="H11" s="5">
-        <f>(D11-B11)/B11</f>
-        <v>9.3934506735885173E-2</v>
-      </c>
-      <c r="I11" s="5">
+      <c r="H11" s="11">
         <f t="shared" si="0"/>
-        <v>0.57578421495130949</v>
-      </c>
-      <c r="J11" s="5">
+        <v>1.0939345067358852</v>
+      </c>
+      <c r="I11" s="11">
+        <f t="shared" si="1"/>
+        <v>0.42421578504869056</v>
+      </c>
+      <c r="J11" s="11">
         <f>C11/B11</f>
         <v>6.9169355877606584E-4</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="11">
         <f>E11/B11</f>
         <v>3.1328811354539446E-3</v>
       </c>
-      <c r="L11" s="5">
-        <f t="shared" si="1"/>
+      <c r="L11" s="11">
+        <f t="shared" si="2"/>
         <v>2.4511114157714709E-4</v>
       </c>
     </row>
@@ -2269,73 +4138,73 @@
       <c r="E12" s="4">
         <v>170033.10279100001</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="7">
         <v>47613462.600000001</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="7">
         <v>65408.676163299999</v>
       </c>
-      <c r="H12" s="5">
-        <f>(B12-D12)/B12</f>
-        <v>0.24107293035794211</v>
-      </c>
-      <c r="I12" s="5">
+      <c r="H12" s="11">
         <f t="shared" si="0"/>
-        <v>0.50743051941153461</v>
-      </c>
-      <c r="J12" s="5">
+        <v>0.75892706964205792</v>
+      </c>
+      <c r="I12" s="11">
+        <f t="shared" si="1"/>
+        <v>0.49256948058846534</v>
+      </c>
+      <c r="J12" s="11">
         <f>C12/B12</f>
         <v>1.6895812240578505E-3</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="11">
         <f>E12/B12</f>
         <v>1.7590217671883417E-3</v>
       </c>
-      <c r="L12" s="5">
-        <f t="shared" si="1"/>
+      <c r="L12" s="11">
+        <f t="shared" si="2"/>
         <v>6.7666403333026682E-4</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="9">
+        <v>36</v>
+      </c>
+      <c r="B13" s="7">
         <v>52189010.600000001</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="7">
         <v>184496.05991800001</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="7">
         <v>37061534</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="7">
         <v>184451.52224399999</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="7">
         <v>14069332</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="7">
         <v>23007.3089865</v>
       </c>
-      <c r="H13" s="5">
-        <f>(B13-D13)/B13</f>
-        <v>0.28985942492651895</v>
-      </c>
-      <c r="I13" s="5">
+      <c r="H13" s="11">
         <f t="shared" si="0"/>
-        <v>0.73041581286463397</v>
-      </c>
-      <c r="J13" s="5">
+        <v>0.71014057507348105</v>
+      </c>
+      <c r="I13" s="11">
+        <f t="shared" si="1"/>
+        <v>0.26958418713536597</v>
+      </c>
+      <c r="J13" s="11">
         <f>C13/B13</f>
         <v>3.5351515155568019E-3</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="11">
         <f>E13/B13</f>
         <v>3.5342981237509795E-3</v>
       </c>
-      <c r="L13" s="5">
-        <f t="shared" si="1"/>
+      <c r="L13" s="11">
+        <f t="shared" si="2"/>
         <v>4.4084585474973538E-4</v>
       </c>
     </row>
@@ -2355,73 +4224,73 @@
       <c r="E14" s="4">
         <v>9860683.1170700006</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <v>1117094704.2</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="7">
         <v>2439070.8690800001</v>
       </c>
-      <c r="H14" s="5">
-        <f>(B14-D14)/B14</f>
-        <v>0.31684337032445897</v>
-      </c>
-      <c r="I14" s="5">
+      <c r="H14" s="11">
         <f t="shared" si="0"/>
-        <v>0.64348435145058025</v>
-      </c>
-      <c r="J14" s="5">
+        <v>0.68315662967554103</v>
+      </c>
+      <c r="I14" s="11">
+        <f t="shared" si="1"/>
+        <v>0.35651564854941975</v>
+      </c>
+      <c r="J14" s="11">
         <f>C14/B14</f>
         <v>6.2110148138080972E-3</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="11">
         <f>E14/B14</f>
         <v>3.146991766593432E-3</v>
       </c>
-      <c r="L14" s="5">
-        <f t="shared" si="1"/>
+      <c r="L14" s="11">
+        <f t="shared" si="2"/>
         <v>7.784182750832999E-4</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A15" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="9">
+      <c r="A15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="7">
         <v>1888639030.5999999</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="7">
         <v>330987876.43599999</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="7">
         <v>1417034052.8</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <v>52230323.976099998</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="7">
         <v>735183338.79999995</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="7">
         <v>15665738.5373</v>
       </c>
-      <c r="H15" s="5">
-        <f>(D15-B15)/B15</f>
-        <v>-0.24970625416450079</v>
-      </c>
-      <c r="I15" s="5">
+      <c r="H15" s="11">
         <f t="shared" si="0"/>
-        <v>0.61073379990116994</v>
-      </c>
-      <c r="J15" s="5">
+        <v>0.75029374583549924</v>
+      </c>
+      <c r="I15" s="11">
+        <f t="shared" si="1"/>
+        <v>0.38926620009883006</v>
+      </c>
+      <c r="J15" s="11">
         <f>C15/B15</f>
         <v>0.17525205773749616</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K15" s="11">
         <f>E15/B15</f>
         <v>2.7655006133970976E-2</v>
       </c>
-      <c r="L15" s="5">
-        <f t="shared" si="1"/>
+      <c r="L15" s="11">
+        <f t="shared" si="2"/>
         <v>8.2947234932040804E-3</v>
       </c>
     </row>
@@ -2441,73 +4310,73 @@
       <c r="E16" s="4">
         <v>86536.287661499999</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="7">
         <v>52971565.799999997</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="7">
         <v>57292.834345700001</v>
       </c>
-      <c r="H16" s="5">
-        <f>(B16-D16)/B16</f>
-        <v>-4.863323117838312E-2</v>
-      </c>
-      <c r="I16" s="5">
+      <c r="H16" s="11">
         <f t="shared" si="0"/>
-        <v>5.6828584084230464E-2</v>
-      </c>
-      <c r="J16" s="5">
+        <v>1.048633231178383</v>
+      </c>
+      <c r="I16" s="11">
+        <f t="shared" si="1"/>
+        <v>0.94317141591576958</v>
+      </c>
+      <c r="J16" s="11">
         <f>C16/B16</f>
         <v>1.5940226211917812E-3</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K16" s="11">
         <f>E16/B16</f>
         <v>1.540799327509992E-3</v>
       </c>
-      <c r="L16" s="5">
-        <f t="shared" si="1"/>
+      <c r="L16" s="11">
+        <f t="shared" si="2"/>
         <v>1.0201126373285629E-3</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="9">
+        <v>37</v>
+      </c>
+      <c r="B17" s="7">
         <v>42798674.399999999</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="7">
         <v>169110.16664700001</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="7">
         <v>45041719.399999999</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="7">
         <v>164677.76881099999</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="7">
         <v>39117214.600000001</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="7">
         <v>9703.0218303399997</v>
       </c>
-      <c r="H17" s="5">
-        <f>(B17-D17)/B17</f>
-        <v>-5.2409216674243538E-2</v>
-      </c>
-      <c r="I17" s="5">
+      <c r="H17" s="11">
         <f t="shared" si="0"/>
-        <v>8.601808003660967E-2</v>
-      </c>
-      <c r="J17" s="5">
+        <v>1.0524092166742436</v>
+      </c>
+      <c r="I17" s="11">
+        <f t="shared" si="1"/>
+        <v>0.91398191996339029</v>
+      </c>
+      <c r="J17" s="11">
         <f>C17/B17</f>
         <v>3.9512944972660185E-3</v>
       </c>
-      <c r="K17" s="5">
+      <c r="K17" s="11">
         <f>E17/B17</f>
         <v>3.84773059258583E-3</v>
       </c>
-      <c r="L17" s="5">
-        <f t="shared" si="1"/>
+      <c r="L17" s="11">
+        <f t="shared" si="2"/>
         <v>2.2671313928218301E-4</v>
       </c>
     </row>
@@ -2527,159 +4396,159 @@
       <c r="E18" s="4">
         <v>4191937.8707599998</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="7">
         <v>1625018710.8</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="7">
         <v>3109857.0395399998</v>
       </c>
-      <c r="H18" s="5">
-        <f>(B18-D18)/B18</f>
-        <v>-2.000260623699769E-4</v>
-      </c>
-      <c r="I18" s="5">
+      <c r="H18" s="11">
         <f t="shared" si="0"/>
-        <v>0.10304745668947624</v>
-      </c>
-      <c r="J18" s="5">
+        <v>1.00020002606237</v>
+      </c>
+      <c r="I18" s="11">
+        <f t="shared" si="1"/>
+        <v>0.89695254331052376</v>
+      </c>
+      <c r="J18" s="11">
         <f>C18/B18</f>
         <v>6.178671081599578E-3</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K18" s="11">
         <f>E18/B18</f>
         <v>2.3138006409334469E-3</v>
       </c>
-      <c r="L18" s="5">
-        <f t="shared" si="1"/>
+      <c r="L18" s="11">
+        <f t="shared" si="2"/>
         <v>1.7165305004853233E-3</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A19" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="9">
+      <c r="A19" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="7">
         <v>374259407.80000001</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="7">
         <v>36671339.376199998</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="7">
         <v>319451064.80000001</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="7">
         <v>11498265.4856</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="7">
         <v>195747522</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="7">
         <v>1477896.6923199999</v>
       </c>
-      <c r="H19" s="5">
-        <f>(D19-B19)/B19</f>
-        <v>-0.14644479699836685</v>
-      </c>
-      <c r="I19" s="5">
+      <c r="H19" s="11">
         <f t="shared" si="0"/>
-        <v>0.47697367675896807</v>
-      </c>
-      <c r="J19" s="5">
+        <v>0.85355520300163312</v>
+      </c>
+      <c r="I19" s="11">
+        <f t="shared" si="1"/>
+        <v>0.52302632324103193</v>
+      </c>
+      <c r="J19" s="11">
         <f>C19/B19</f>
         <v>9.7983747667865564E-2</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K19" s="11">
         <f>E19/B19</f>
         <v>3.0722715971764011E-2</v>
       </c>
-      <c r="L19" s="5">
-        <f t="shared" si="1"/>
+      <c r="L19" s="11">
+        <f t="shared" si="2"/>
         <v>3.9488564923657746E-3</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="9">
+        <v>38</v>
+      </c>
+      <c r="B20" s="7">
         <v>28546124.600000001</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="7">
         <v>116019.715939</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="7">
         <v>27901238</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="7">
         <v>128736.181753</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="7">
         <v>7589116.7999999998</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="7">
         <v>72091.823232299997</v>
       </c>
-      <c r="H20" s="5">
-        <f>(B20-D20)/B20</f>
-        <v>2.259103850475036E-2</v>
-      </c>
-      <c r="I20" s="5">
+      <c r="H20" s="11">
         <f t="shared" si="0"/>
-        <v>0.73414546085180332</v>
-      </c>
-      <c r="J20" s="5">
+        <v>0.9774089614952497</v>
+      </c>
+      <c r="I20" s="11">
+        <f t="shared" si="1"/>
+        <v>0.26585453914819662</v>
+      </c>
+      <c r="J20" s="11">
         <f>C20/B20</f>
         <v>4.0642895511988344E-3</v>
       </c>
-      <c r="K20" s="5">
+      <c r="K20" s="11">
         <f>E20/B20</f>
         <v>4.5097603810290935E-3</v>
       </c>
-      <c r="L20" s="5">
-        <f t="shared" si="1"/>
+      <c r="L20" s="11">
+        <f t="shared" si="2"/>
         <v>2.5254504505420675E-3</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="9">
+        <v>39</v>
+      </c>
+      <c r="B21" s="7">
         <v>10800565.199999999</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="7">
         <v>181427.34367599999</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="7">
         <v>11061967.199999999</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="7">
         <v>18989.8155167</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="7">
         <v>9003693.5999999996</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="7">
         <v>6686.3842725300001</v>
       </c>
-      <c r="H21" s="5">
-        <f>(B21-D21)/B21</f>
-        <v>-2.420262228498931E-2</v>
-      </c>
-      <c r="I21" s="5">
+      <c r="H21" s="11">
         <f t="shared" si="0"/>
-        <v>0.16636829339264575</v>
-      </c>
-      <c r="J21" s="5">
+        <v>1.0242026222849894</v>
+      </c>
+      <c r="I21" s="11">
+        <f t="shared" si="1"/>
+        <v>0.83363170660735419</v>
+      </c>
+      <c r="J21" s="11">
         <f>C21/B21</f>
         <v>1.679794902548248E-2</v>
       </c>
-      <c r="K21" s="5">
+      <c r="K21" s="11">
         <f>E21/B21</f>
         <v>1.7582242378111844E-3</v>
       </c>
-      <c r="L21" s="5">
-        <f t="shared" si="1"/>
+      <c r="L21" s="11">
+        <f t="shared" si="2"/>
         <v>6.1907725648746614E-4</v>
       </c>
     </row>
@@ -2699,30 +4568,30 @@
       <c r="E22" s="4">
         <v>174702521.64199999</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="7">
         <v>58861111648.400002</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="7">
         <v>66290083.325000003</v>
       </c>
-      <c r="H22" s="5">
-        <f>(B22-D22)/B22</f>
-        <v>-3.5375437982295768E-2</v>
-      </c>
-      <c r="I22" s="5">
+      <c r="H22" s="11">
         <f t="shared" si="0"/>
-        <v>-0.39880860188709116</v>
-      </c>
-      <c r="J22" s="5">
+        <v>1.0353754379822957</v>
+      </c>
+      <c r="I22" s="11">
+        <f t="shared" si="1"/>
+        <v>1.3988086018870911</v>
+      </c>
+      <c r="J22" s="11">
         <f>C22/B22</f>
         <v>4.7587655326600609E-3</v>
       </c>
-      <c r="K22" s="5">
+      <c r="K22" s="11">
         <f>E22/B22</f>
         <v>4.1517290992386154E-3</v>
       </c>
-      <c r="L22" s="5">
-        <f t="shared" si="1"/>
+      <c r="L22" s="11">
+        <f t="shared" si="2"/>
         <v>1.5753548680615616E-3</v>
       </c>
     </row>
@@ -2742,30 +4611,30 @@
       <c r="E23" s="4">
         <v>950876.60208999994</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="7">
         <v>623199667.60000002</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="7">
         <v>630923.81415300001</v>
       </c>
-      <c r="H23" s="5">
-        <f>(B23-D23)/B23</f>
-        <v>-3.4742853505272783E-3</v>
-      </c>
-      <c r="I23" s="5">
+      <c r="H23" s="11">
         <f t="shared" si="0"/>
-        <v>-0.30237784650289645</v>
-      </c>
-      <c r="J23" s="5">
+        <v>1.0034742853505272</v>
+      </c>
+      <c r="I23" s="11">
+        <f t="shared" si="1"/>
+        <v>1.3023778465028963</v>
+      </c>
+      <c r="J23" s="11">
         <f>C23/B23</f>
         <v>5.2417397361807314E-3</v>
       </c>
-      <c r="K23" s="5">
+      <c r="K23" s="11">
         <f>E23/B23</f>
         <v>1.9871650864146991E-3</v>
       </c>
-      <c r="L23" s="5">
-        <f t="shared" si="1"/>
+      <c r="L23" s="11">
+        <f t="shared" si="2"/>
         <v>1.3185199561296713E-3</v>
       </c>
     </row>
@@ -2785,30 +4654,30 @@
       <c r="E24" s="4">
         <v>904688.83650099998</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="7">
         <v>743078715.20000005</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="7">
         <v>636582.43804000004</v>
       </c>
-      <c r="H24" s="5">
-        <f>(B24-D24)/B24</f>
-        <v>1.9619928911988667E-2</v>
-      </c>
-      <c r="I24" s="5">
+      <c r="H24" s="11">
         <f t="shared" si="0"/>
-        <v>8.6057154250921017E-2</v>
-      </c>
-      <c r="J24" s="5">
+        <v>0.98038007108801128</v>
+      </c>
+      <c r="I24" s="11">
+        <f t="shared" si="1"/>
+        <v>0.91394284574907902</v>
+      </c>
+      <c r="J24" s="11">
         <f>C24/B24</f>
         <v>7.7284880920492282E-4</v>
       </c>
-      <c r="K24" s="5">
+      <c r="K24" s="11">
         <f>E24/B24</f>
         <v>1.1127137311780009E-3</v>
       </c>
-      <c r="L24" s="5">
-        <f t="shared" si="1"/>
+      <c r="L24" s="11">
+        <f t="shared" si="2"/>
         <v>7.8295872708394377E-4</v>
       </c>
     </row>
@@ -2828,30 +4697,30 @@
       <c r="E25" s="4">
         <v>1618224.4899599999</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="7">
         <v>1271852242.8</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="7">
         <v>3537843.5832600002</v>
       </c>
-      <c r="H25" s="5">
-        <f>(B25-D25)/B25</f>
-        <v>-7.0380861164368702E-2</v>
-      </c>
-      <c r="I25" s="5">
+      <c r="H25" s="11">
         <f t="shared" si="0"/>
-        <v>-2.3178468876686606E-2</v>
-      </c>
-      <c r="J25" s="5">
+        <v>1.0703808611643688</v>
+      </c>
+      <c r="I25" s="11">
+        <f t="shared" si="1"/>
+        <v>1.0231784688766865</v>
+      </c>
+      <c r="J25" s="11">
         <f>C25/B25</f>
         <v>2.6873954202269782E-3</v>
       </c>
-      <c r="K25" s="5">
+      <c r="K25" s="11">
         <f>E25/B25</f>
         <v>1.3018276810920367E-3</v>
       </c>
-      <c r="L25" s="5">
-        <f t="shared" si="1"/>
+      <c r="L25" s="11">
+        <f t="shared" si="2"/>
         <v>2.8461210027636847E-3</v>
       </c>
     </row>
@@ -2871,30 +4740,30 @@
       <c r="E26" s="4">
         <v>2931767.1285799998</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="7">
         <v>2633088051.4000001</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="7">
         <v>4171767.29519</v>
       </c>
-      <c r="H26" s="5">
-        <f>(B26-D26)/B26</f>
-        <v>-2.6949414042711995E-2</v>
-      </c>
-      <c r="I26" s="5">
+      <c r="H26" s="11">
         <f t="shared" si="0"/>
-        <v>-3.9069227520122762E-2</v>
-      </c>
-      <c r="J26" s="5">
+        <v>1.026949414042712</v>
+      </c>
+      <c r="I26" s="11">
+        <f t="shared" si="1"/>
+        <v>1.0390692275201228</v>
+      </c>
+      <c r="J26" s="11">
         <f>C26/B26</f>
         <v>5.3539846245207097E-4</v>
       </c>
-      <c r="K26" s="5">
+      <c r="K26" s="11">
         <f>E26/B26</f>
         <v>1.1569339673023092E-3</v>
       </c>
-      <c r="L26" s="5">
-        <f t="shared" si="1"/>
+      <c r="L26" s="11">
+        <f t="shared" si="2"/>
         <v>1.6462628427872045E-3</v>
       </c>
     </row>
@@ -2914,30 +4783,30 @@
       <c r="E27" s="4">
         <v>6077712.8282199996</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="7">
         <v>2957131855.4000001</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="7">
         <v>5873061.8385899998</v>
       </c>
-      <c r="H27" s="5">
-        <f>(B27-D27)/B27</f>
-        <v>0.17297425116454435</v>
-      </c>
-      <c r="I27" s="5">
+      <c r="H27" s="11">
         <f t="shared" si="0"/>
-        <v>0.29211220993754289</v>
-      </c>
-      <c r="J27" s="5">
+        <v>0.82702574883545565</v>
+      </c>
+      <c r="I27" s="11">
+        <f t="shared" si="1"/>
+        <v>0.70788779006245717</v>
+      </c>
+      <c r="J27" s="11">
         <f>C27/B27</f>
         <v>1.0467924332309708E-3</v>
       </c>
-      <c r="K27" s="5">
+      <c r="K27" s="11">
         <f>E27/B27</f>
         <v>1.4549025586216007E-3</v>
       </c>
-      <c r="L27" s="5">
-        <f t="shared" si="1"/>
+      <c r="L27" s="11">
+        <f t="shared" si="2"/>
         <v>1.4059125426645073E-3</v>
       </c>
     </row>
@@ -2957,30 +4826,30 @@
       <c r="E28" s="4">
         <v>7828922.0355799999</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="7">
         <v>5589016638.1999998</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="7">
         <v>9536877.7356800009</v>
       </c>
-      <c r="H28" s="5">
-        <f>(B28-D28)/B28</f>
-        <v>9.7501351459879509E-2</v>
-      </c>
-      <c r="I28" s="5">
+      <c r="H28" s="11">
         <f t="shared" si="0"/>
-        <v>0.16722710687100004</v>
-      </c>
-      <c r="J28" s="5">
+        <v>0.90249864854012052</v>
+      </c>
+      <c r="I28" s="11">
+        <f t="shared" si="1"/>
+        <v>0.83277289312899994</v>
+      </c>
+      <c r="J28" s="11">
         <f>C28/B28</f>
         <v>5.503195732221186E-4</v>
       </c>
-      <c r="K28" s="5">
+      <c r="K28" s="11">
         <f>E28/B28</f>
         <v>1.1665225701942225E-3</v>
       </c>
-      <c r="L28" s="5">
-        <f t="shared" si="1"/>
+      <c r="L28" s="11">
+        <f t="shared" si="2"/>
         <v>1.4210108463584034E-3</v>
       </c>
     </row>
@@ -3000,30 +4869,30 @@
       <c r="E29" s="4">
         <v>7596027.7199299997</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="7">
         <v>2129407451.8</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="7">
         <v>7064432.3703699997</v>
       </c>
-      <c r="H29" s="5">
-        <f>(B29-D29)/B29</f>
-        <v>0.17488701855787817</v>
-      </c>
-      <c r="I29" s="5">
+      <c r="H29" s="11">
         <f t="shared" si="0"/>
-        <v>0.17011655945642648</v>
-      </c>
-      <c r="J29" s="5">
+        <v>0.82511298144212186</v>
+      </c>
+      <c r="I29" s="11">
+        <f t="shared" si="1"/>
+        <v>0.82988344054357355</v>
+      </c>
+      <c r="J29" s="11">
         <f>C29/B29</f>
         <v>7.4889909165773922E-3</v>
       </c>
-      <c r="K29" s="5">
+      <c r="K29" s="11">
         <f>E29/B29</f>
         <v>2.9603623361753582E-3</v>
       </c>
-      <c r="L29" s="5">
-        <f t="shared" si="1"/>
+      <c r="L29" s="11">
+        <f t="shared" si="2"/>
         <v>2.7531863082635088E-3</v>
       </c>
     </row>
@@ -3043,30 +4912,30 @@
       <c r="E30" s="4">
         <v>628746.94184999994</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30" s="7">
         <v>53724671.200000003</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="7">
         <v>336920.660569</v>
       </c>
-      <c r="H30" s="5">
-        <f>(B30-D30)/B30</f>
-        <v>0.14978806507995132</v>
-      </c>
-      <c r="I30" s="5">
+      <c r="H30" s="11">
         <f t="shared" si="0"/>
-        <v>-0.19696797211811526</v>
-      </c>
-      <c r="J30" s="5">
+        <v>0.85021193492004865</v>
+      </c>
+      <c r="I30" s="11">
+        <f t="shared" si="1"/>
+        <v>1.1969679721181152</v>
+      </c>
+      <c r="J30" s="11">
         <f>C30/B30</f>
         <v>1.6678227708957955E-2</v>
       </c>
-      <c r="K30" s="5">
+      <c r="K30" s="11">
         <f>E30/B30</f>
         <v>1.4008274693017776E-2</v>
       </c>
-      <c r="L30" s="5">
-        <f t="shared" si="1"/>
+      <c r="L30" s="11">
+        <f t="shared" si="2"/>
         <v>7.5064813025039366E-3</v>
       </c>
     </row>
@@ -3086,30 +4955,30 @@
       <c r="E31" s="4">
         <v>1015290207.74</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F31" s="7">
         <v>231792565363</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="7">
         <v>387485934.45300001</v>
       </c>
-      <c r="H31" s="5">
-        <f>(B31-D31)/B31</f>
-        <v>-1.2193324387846276E-2</v>
-      </c>
-      <c r="I31" s="5">
+      <c r="H31" s="11">
         <f t="shared" si="0"/>
-        <v>0.11151529586246686</v>
-      </c>
-      <c r="J31" s="5">
+        <v>1.0121933243878463</v>
+      </c>
+      <c r="I31" s="11">
+        <f t="shared" si="1"/>
+        <v>0.88848470413753311</v>
+      </c>
+      <c r="J31" s="11">
         <f>C31/B31</f>
         <v>6.2644680006298673E-3</v>
       </c>
-      <c r="K31" s="5">
+      <c r="K31" s="11">
         <f>E31/B31</f>
         <v>3.8917116190716346E-3</v>
       </c>
-      <c r="L31" s="5">
-        <f t="shared" si="1"/>
+      <c r="L31" s="11">
+        <f t="shared" si="2"/>
         <v>1.485273374884889E-3</v>
       </c>
     </row>
@@ -3129,30 +4998,30 @@
       <c r="E32" s="4">
         <v>95384807.631999999</v>
       </c>
-      <c r="F32" s="9">
+      <c r="F32" s="7">
         <v>20365516610</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="7">
         <v>27671094.960200001</v>
       </c>
-      <c r="H32" s="5">
-        <f>(B32-D32)/B32</f>
-        <v>4.9078571347687339E-2</v>
-      </c>
-      <c r="I32" s="5">
+      <c r="H32" s="11">
         <f t="shared" si="0"/>
-        <v>3.1822694769619701E-3</v>
-      </c>
-      <c r="J32" s="5">
+        <v>0.95092142865231266</v>
+      </c>
+      <c r="I32" s="11">
+        <f t="shared" si="1"/>
+        <v>0.99681773052303801</v>
+      </c>
+      <c r="J32" s="11">
         <f>C32/B32</f>
         <v>1.0404746419487972E-2</v>
       </c>
-      <c r="K32" s="5">
+      <c r="K32" s="11">
         <f>E32/B32</f>
         <v>4.6687383036195318E-3</v>
       </c>
-      <c r="L32" s="5">
-        <f t="shared" si="1"/>
+      <c r="L32" s="11">
+        <f t="shared" si="2"/>
         <v>1.3543991349460808E-3</v>
       </c>
     </row>
@@ -3172,30 +5041,30 @@
       <c r="E33" s="4">
         <v>265266356.43599999</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33" s="7">
         <v>18640519393.200001</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="7">
         <v>115354906.141</v>
       </c>
-      <c r="H33" s="5">
-        <f>(B33-D33)/B33</f>
-        <v>9.7646754264358274E-2</v>
-      </c>
-      <c r="I33" s="5">
+      <c r="H33" s="11">
         <f t="shared" si="0"/>
-        <v>-2.8051249864027187E-2</v>
-      </c>
-      <c r="J33" s="5">
+        <v>0.90235324573564168</v>
+      </c>
+      <c r="I33" s="11">
+        <f t="shared" si="1"/>
+        <v>1.0280512498640273</v>
+      </c>
+      <c r="J33" s="11">
         <f>C33/B33</f>
         <v>1.4981741252244824E-2</v>
       </c>
-      <c r="K33" s="5">
+      <c r="K33" s="11">
         <f>E33/B33</f>
         <v>1.4629818168070418E-2</v>
       </c>
-      <c r="L33" s="5">
-        <f t="shared" si="1"/>
+      <c r="L33" s="11">
+        <f t="shared" si="2"/>
         <v>6.3619877179744311E-3</v>
       </c>
     </row>
@@ -3215,116 +5084,116 @@
       <c r="E34" s="4">
         <v>2840499643.3800001</v>
       </c>
-      <c r="F34" s="9">
+      <c r="F34" s="7">
         <v>3286567960500</v>
       </c>
-      <c r="G34" s="9">
+      <c r="G34" s="7">
         <v>817621597.70899999</v>
       </c>
-      <c r="H34" s="5">
-        <f>(B34-D34)/B34</f>
-        <v>0.15247666324284623</v>
-      </c>
-      <c r="I34" s="5">
+      <c r="H34" s="11">
         <f t="shared" si="0"/>
-        <v>0.22475528390090829</v>
-      </c>
-      <c r="J34" s="5">
+        <v>0.84752333675715374</v>
+      </c>
+      <c r="I34" s="11">
+        <f t="shared" si="1"/>
+        <v>0.77524471609909174</v>
+      </c>
+      <c r="J34" s="11">
         <f>C34/B34</f>
         <v>5.5720605010201442E-4</v>
       </c>
-      <c r="K34" s="5">
+      <c r="K34" s="11">
         <f>E34/B34</f>
         <v>6.7002489103456327E-4</v>
       </c>
-      <c r="L34" s="5">
-        <f t="shared" si="1"/>
+      <c r="L34" s="11">
+        <f t="shared" si="2"/>
         <v>1.9286283777194982E-4</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="9">
+        <v>40</v>
+      </c>
+      <c r="B35" s="7">
         <v>97611105037.600006</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="7">
         <v>1720235606.3699999</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="7">
         <v>76603854319.800003</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="7">
         <v>85021399.524900004</v>
       </c>
-      <c r="F35" s="9">
+      <c r="F35" s="7">
         <v>71253446652.800003</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="7">
         <v>21376046.0966</v>
       </c>
-      <c r="H35" s="5">
-        <f>(B35-D35)/B35</f>
-        <v>0.21521373730691776</v>
-      </c>
-      <c r="I35" s="5">
+      <c r="H35" s="11">
         <f t="shared" si="0"/>
-        <v>0.27002725125022381</v>
-      </c>
-      <c r="J35" s="5">
+        <v>0.78478626269308227</v>
+      </c>
+      <c r="I35" s="11">
+        <f t="shared" si="1"/>
+        <v>0.72997274874977625</v>
+      </c>
+      <c r="J35" s="11">
         <f>C35/B35</f>
         <v>1.7623359613717738E-2</v>
       </c>
-      <c r="K35" s="5">
+      <c r="K35" s="11">
         <f>E35/B35</f>
         <v>8.7102179093402924E-4</v>
       </c>
-      <c r="L35" s="5">
-        <f t="shared" si="1"/>
+      <c r="L35" s="11">
+        <f t="shared" si="2"/>
         <v>2.1899194859402422E-4</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="9">
+        <v>41</v>
+      </c>
+      <c r="B36" s="7">
         <v>57947321369.400002</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="7">
         <v>1048962277.62</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="7">
         <v>46855590822.599998</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="7">
         <v>12043897.4486</v>
       </c>
-      <c r="F36" s="9">
+      <c r="F36" s="7">
         <v>43948797656.800003</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="7">
         <v>13728941.7732</v>
       </c>
-      <c r="H36" s="5">
-        <f>(B36-D36)/B36</f>
-        <v>0.19141058265822045</v>
-      </c>
-      <c r="I36" s="5">
+      <c r="H36" s="11">
         <f t="shared" si="0"/>
-        <v>0.24157326657711808</v>
-      </c>
-      <c r="J36" s="5">
+        <v>0.80858941734177958</v>
+      </c>
+      <c r="I36" s="11">
+        <f t="shared" si="1"/>
+        <v>0.75842673342288192</v>
+      </c>
+      <c r="J36" s="11">
         <f>C36/B36</f>
         <v>1.8101997690853078E-2</v>
       </c>
-      <c r="K36" s="5">
+      <c r="K36" s="11">
         <f>E36/B36</f>
         <v>2.0784217741184443E-4</v>
       </c>
-      <c r="L36" s="5">
-        <f t="shared" si="1"/>
+      <c r="L36" s="11">
+        <f t="shared" si="2"/>
         <v>2.3692107674281186E-4</v>
       </c>
     </row>
@@ -3344,30 +5213,30 @@
       <c r="E37" s="4">
         <v>7882.1990687899997</v>
       </c>
-      <c r="F37" s="9">
+      <c r="F37" s="7">
         <v>1071864.2</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="7">
         <v>846.37637018099997</v>
       </c>
-      <c r="H37" s="5">
-        <f>(B37-D37)/B37</f>
-        <v>-4.3593614374334538E-2</v>
-      </c>
-      <c r="I37" s="5">
+      <c r="H37" s="11">
         <f t="shared" si="0"/>
-        <v>0.54298914947776911</v>
-      </c>
-      <c r="J37" s="5">
+        <v>1.0435936143743345</v>
+      </c>
+      <c r="I37" s="11">
+        <f t="shared" si="1"/>
+        <v>0.45701085052223084</v>
+      </c>
+      <c r="J37" s="11">
         <f>C37/B37</f>
         <v>1.6132415794718484E-3</v>
       </c>
-      <c r="K37" s="5">
+      <c r="K37" s="11">
         <f>E37/B37</f>
         <v>3.3607340374025496E-3</v>
       </c>
-      <c r="L37" s="5">
-        <f t="shared" si="1"/>
+      <c r="L37" s="11">
+        <f t="shared" si="2"/>
         <v>3.6086958105172029E-4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add os and user level hw counter values
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,15 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="207" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{D0E05F98-814C-4157-A6EE-D345160BC39E}"/>
+  <xr:revisionPtr revIDLastSave="259" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{8B016830-57E2-41D7-B39B-C8244CC0FBA6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="clang-1" sheetId="3" r:id="rId1"/>
-    <sheet name="clang-2" sheetId="4" r:id="rId2"/>
-    <sheet name="clang-3" sheetId="5" r:id="rId3"/>
-    <sheet name="clang" sheetId="1" r:id="rId4"/>
+    <sheet name="clang-os" sheetId="6" r:id="rId1"/>
+    <sheet name="clang-usr" sheetId="7" r:id="rId2"/>
+    <sheet name="clang-all" sheetId="1" r:id="rId3"/>
+    <sheet name="clang-part1" sheetId="3" r:id="rId4"/>
+    <sheet name="clang-part2" sheetId="4" r:id="rId5"/>
+    <sheet name="clang-part3" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="47">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -173,7 +175,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -233,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -242,20 +244,21 @@
     </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -313,7 +316,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>clang!$A$5:$A$15</c:f>
+              <c:f>'clang-all'!$A$5:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -354,7 +357,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>clang!$H$5:$H$15</c:f>
+              <c:f>'clang-all'!$H$5:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -364,7 +367,7 @@
                 <c:pt idx="1">
                   <c:v>0.81051092943930281</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="2" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
                   <c:v>0.84752664870192518</c:v>
                 </c:pt>
                 <c:pt idx="3">
@@ -418,7 +421,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>clang!$A$5:$A$15</c:f>
+              <c:f>'clang-all'!$A$5:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -459,7 +462,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>clang!$I$5:$I$15</c:f>
+              <c:f>'clang-all'!$I$5:$I$15</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -469,7 +472,7 @@
                 <c:pt idx="1">
                   <c:v>0.75585517766201682</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="2" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
                   <c:v>0.7754929742072495</c:v>
                 </c:pt>
                 <c:pt idx="3">
@@ -795,7 +798,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>clang!$A$16:$A$26</c:f>
+              <c:f>'clang-all'!$A$16:$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -836,7 +839,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>clang!$H$16:$H$26</c:f>
+              <c:f>'clang-all'!$H$16:$H$26</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -900,7 +903,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>clang!$A$16:$A$26</c:f>
+              <c:f>'clang-all'!$A$16:$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -941,7 +944,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>clang!$I$16:$I$26</c:f>
+              <c:f>'clang-all'!$I$16:$I$26</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1272,7 +1275,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>clang!$A$27:$A$37</c:f>
+              <c:f>'clang-all'!$A$27:$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -1313,7 +1316,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>clang!$H$27:$H$37</c:f>
+              <c:f>'clang-all'!$H$27:$H$37</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1377,7 +1380,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>clang!$A$27:$A$37</c:f>
+              <c:f>'clang-all'!$A$27:$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -1418,7 +1421,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>clang!$I$27:$I$37</c:f>
+              <c:f>'clang-all'!$I$27:$I$37</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3370,7 +3373,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{2D12F0F9-E194-42A8-899D-E6197E229285}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="91" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3381,7 +3384,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661470" cy="6285453"/>
+    <xdr:ext cx="8651875" cy="6276731"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3414,7 +3417,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661470" cy="6285453"/>
+    <xdr:ext cx="8656236" cy="6285453"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3447,7 +3450,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661470" cy="6285453"/>
+    <xdr:ext cx="8656236" cy="6285453"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3738,11 +3741,3039 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670D2A71-BD87-4620-9FEC-7336DAF0F286}">
+  <dimension ref="A1:L37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.65">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+    </row>
+    <row r="4" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="6">
+        <v>11042963</v>
+      </c>
+      <c r="C5" s="6">
+        <v>36350.102217200001</v>
+      </c>
+      <c r="D5" s="6">
+        <v>11490479</v>
+      </c>
+      <c r="E5" s="6">
+        <v>50127.715224200001</v>
+      </c>
+      <c r="F5" s="6">
+        <v>11749421.199999999</v>
+      </c>
+      <c r="G5" s="6">
+        <v>3389.7836155099999</v>
+      </c>
+      <c r="H5" s="6">
+        <f>D5/B5</f>
+        <v>1.0405249931562752</v>
+      </c>
+      <c r="I5" s="6">
+        <f>F5/B5</f>
+        <v>1.0639736092568632</v>
+      </c>
+      <c r="J5" s="6">
+        <f>C5/B5</f>
+        <v>3.2916982713063515E-3</v>
+      </c>
+      <c r="K5" s="6">
+        <f>E5/B5</f>
+        <v>4.5393356134762024E-3</v>
+      </c>
+      <c r="L5" s="6">
+        <f>G5/B5</f>
+        <v>3.0696323219682979E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6">
+        <v>157808861394</v>
+      </c>
+      <c r="C6" s="6">
+        <v>496799761.12900001</v>
+      </c>
+      <c r="D6" s="6">
+        <v>76807903909.800003</v>
+      </c>
+      <c r="E6" s="6">
+        <v>338973495.222</v>
+      </c>
+      <c r="F6" s="6">
+        <v>80568006264</v>
+      </c>
+      <c r="G6" s="6">
+        <v>22781067.6855</v>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" ref="H6:H37" si="0">D6/B6</f>
+        <v>0.48671477147303144</v>
+      </c>
+      <c r="I6" s="6">
+        <f t="shared" ref="I6:I37" si="1">F6/B6</f>
+        <v>0.51054171199452836</v>
+      </c>
+      <c r="J6" s="6">
+        <f t="shared" ref="J6:J37" si="2">C6/B6</f>
+        <v>3.1481106747779162E-3</v>
+      </c>
+      <c r="K6" s="6">
+        <f t="shared" ref="K6:K37" si="3">E6/B6</f>
+        <v>2.1480003862120764E-3</v>
+      </c>
+      <c r="L6" s="6">
+        <f t="shared" ref="L6:L37" si="4">G6/B6</f>
+        <v>1.4435860878954515E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6">
+        <v>138485683363</v>
+      </c>
+      <c r="C7" s="6">
+        <v>543084960.44099998</v>
+      </c>
+      <c r="D7" s="6">
+        <v>107843598232</v>
+      </c>
+      <c r="E7" s="6">
+        <v>776016455.204</v>
+      </c>
+      <c r="F7" s="6">
+        <v>109535573413</v>
+      </c>
+      <c r="G7" s="6">
+        <v>118205810.941</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="0"/>
+        <v>0.77873463605129001</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" si="1"/>
+        <v>0.79095232628404122</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" si="2"/>
+        <v>3.921596422479719E-3</v>
+      </c>
+      <c r="K7" s="6">
+        <f t="shared" si="3"/>
+        <v>5.6035861351089863E-3</v>
+      </c>
+      <c r="L7" s="6">
+        <f t="shared" si="4"/>
+        <v>8.5355979095079308E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6">
+        <v>5635082.2000000002</v>
+      </c>
+      <c r="C8" s="6">
+        <v>24595.531296599998</v>
+      </c>
+      <c r="D8" s="6">
+        <v>4746928.4000000004</v>
+      </c>
+      <c r="E8" s="6">
+        <v>29787.6946379</v>
+      </c>
+      <c r="F8" s="6">
+        <v>5513902.4000000004</v>
+      </c>
+      <c r="G8" s="6">
+        <v>13202.382278999999</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.84238849257602666</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" si="1"/>
+        <v>0.97849546897470285</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="2"/>
+        <v>4.3647156196940651E-3</v>
+      </c>
+      <c r="K8" s="6">
+        <f t="shared" si="3"/>
+        <v>5.2861153716444453E-3</v>
+      </c>
+      <c r="L8" s="6">
+        <f t="shared" si="4"/>
+        <v>2.3428908062778568E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2352445.6</v>
+      </c>
+      <c r="C9" s="6">
+        <v>20876.667527199999</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1984880.2</v>
+      </c>
+      <c r="E9" s="6">
+        <v>14028.128576499999</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1738382.2</v>
+      </c>
+      <c r="G9" s="6">
+        <v>11607.4450832</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="0"/>
+        <v>0.8437517960032741</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="1"/>
+        <v>0.73896807645626317</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="2"/>
+        <v>8.8744528363163839E-3</v>
+      </c>
+      <c r="K9" s="6">
+        <f t="shared" si="3"/>
+        <v>5.9632106164325327E-3</v>
+      </c>
+      <c r="L9" s="6">
+        <f t="shared" si="4"/>
+        <v>4.934203402280588E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6">
+        <v>159890048.59999999</v>
+      </c>
+      <c r="C10" s="6">
+        <v>373621.64579799998</v>
+      </c>
+      <c r="D10" s="6">
+        <v>137003438.19999999</v>
+      </c>
+      <c r="E10" s="6">
+        <v>478934.21460200002</v>
+      </c>
+      <c r="F10" s="6">
+        <v>139969464.40000001</v>
+      </c>
+      <c r="G10" s="6">
+        <v>294426.80045899999</v>
+      </c>
+      <c r="H10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.85686031994864242</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="1"/>
+        <v>0.87541073147187731</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="2"/>
+        <v>2.3367410859489852E-3</v>
+      </c>
+      <c r="K10" s="6">
+        <f t="shared" si="3"/>
+        <v>2.9953972670316645E-3</v>
+      </c>
+      <c r="L10" s="6">
+        <f t="shared" si="4"/>
+        <v>1.8414329286719599E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="6">
+        <v>4372762.2</v>
+      </c>
+      <c r="C11" s="6">
+        <v>3117.0640930200002</v>
+      </c>
+      <c r="D11" s="6">
+        <v>4552725.2</v>
+      </c>
+      <c r="E11" s="6">
+        <v>5667.8894978600001</v>
+      </c>
+      <c r="F11" s="6">
+        <v>8427265.4000000004</v>
+      </c>
+      <c r="G11" s="6">
+        <v>4205.9492436299997</v>
+      </c>
+      <c r="H11" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0411554508955461</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="1"/>
+        <v>1.9272178578565282</v>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" si="2"/>
+        <v>7.1283640647552252E-4</v>
+      </c>
+      <c r="K11" s="6">
+        <f t="shared" si="3"/>
+        <v>1.2961805921803842E-3</v>
+      </c>
+      <c r="L11" s="6">
+        <f t="shared" si="4"/>
+        <v>9.6185181156889792E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="6">
+        <v>17849745</v>
+      </c>
+      <c r="C12" s="6">
+        <v>121261.041488</v>
+      </c>
+      <c r="D12" s="6">
+        <v>17575590.199999999</v>
+      </c>
+      <c r="E12" s="6">
+        <v>39122.121805399998</v>
+      </c>
+      <c r="F12" s="6">
+        <v>14195115.6</v>
+      </c>
+      <c r="G12" s="6">
+        <v>72961.760325800002</v>
+      </c>
+      <c r="H12" s="6">
+        <f t="shared" si="0"/>
+        <v>0.98464096826033087</v>
+      </c>
+      <c r="I12" s="6">
+        <f t="shared" si="1"/>
+        <v>0.79525593222760327</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" si="2"/>
+        <v>6.793432706629703E-3</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" si="3"/>
+        <v>2.1917468179741503E-3</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="4"/>
+        <v>4.0875519692746311E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="6">
+        <v>3933218.4</v>
+      </c>
+      <c r="C13" s="6">
+        <v>40695.104273600002</v>
+      </c>
+      <c r="D13" s="6">
+        <v>3949440.6</v>
+      </c>
+      <c r="E13" s="6">
+        <v>41038.642485299999</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1798863.6</v>
+      </c>
+      <c r="G13" s="6">
+        <v>68914.215713700003</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0041244086522121</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="1"/>
+        <v>0.45735156735766319</v>
+      </c>
+      <c r="J13" s="6">
+        <f t="shared" si="2"/>
+        <v>1.0346515279599018E-2</v>
+      </c>
+      <c r="K13" s="6">
+        <f t="shared" si="3"/>
+        <v>1.0433858055098085E-2</v>
+      </c>
+      <c r="L13" s="6">
+        <f t="shared" si="4"/>
+        <v>1.752107528880166E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="6">
+        <v>491359952.39999998</v>
+      </c>
+      <c r="C14" s="6">
+        <v>9169742.7574700005</v>
+      </c>
+      <c r="D14" s="6">
+        <v>471227525.39999998</v>
+      </c>
+      <c r="E14" s="6">
+        <v>3672817.92307</v>
+      </c>
+      <c r="F14" s="6">
+        <v>305508096.39999998</v>
+      </c>
+      <c r="G14" s="6">
+        <v>2437082.1589700002</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="0"/>
+        <v>0.95902713092170999</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="1"/>
+        <v>0.62176026944763274</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8661966065165226E-2</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="3"/>
+        <v>7.4748011211139154E-3</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="4"/>
+        <v>4.9598713673475198E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="6">
+        <v>827068603.39999998</v>
+      </c>
+      <c r="C15" s="6">
+        <v>149806870.93599999</v>
+      </c>
+      <c r="D15" s="6">
+        <v>431549641.60000002</v>
+      </c>
+      <c r="E15" s="6">
+        <v>3294993.7427300001</v>
+      </c>
+      <c r="F15" s="6">
+        <v>518062177</v>
+      </c>
+      <c r="G15" s="6">
+        <v>4674219.7722199997</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" si="0"/>
+        <v>0.52178215909289838</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" si="1"/>
+        <v>0.62638356101331361</v>
+      </c>
+      <c r="J15" s="6">
+        <f t="shared" si="2"/>
+        <v>0.18112992116997098</v>
+      </c>
+      <c r="K15" s="6">
+        <f t="shared" si="3"/>
+        <v>3.9839424797224752E-3</v>
+      </c>
+      <c r="L15" s="6">
+        <f t="shared" si="4"/>
+        <v>5.651550249888255E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="6">
+        <v>6136437</v>
+      </c>
+      <c r="C16" s="6">
+        <v>14595.562626999999</v>
+      </c>
+      <c r="D16" s="6">
+        <v>6183005.7999999998</v>
+      </c>
+      <c r="E16" s="6">
+        <v>23508.9007944</v>
+      </c>
+      <c r="F16" s="6">
+        <v>5271526</v>
+      </c>
+      <c r="G16" s="6">
+        <v>55955.4177538</v>
+      </c>
+      <c r="H16" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0075888989001272</v>
+      </c>
+      <c r="I16" s="6">
+        <f t="shared" si="1"/>
+        <v>0.85905322583772958</v>
+      </c>
+      <c r="J16" s="6">
+        <f t="shared" si="2"/>
+        <v>2.3785076954265152E-3</v>
+      </c>
+      <c r="K16" s="6">
+        <f t="shared" si="3"/>
+        <v>3.8310343273140423E-3</v>
+      </c>
+      <c r="L16" s="6">
+        <f t="shared" si="4"/>
+        <v>9.1185516536387481E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1076924.2</v>
+      </c>
+      <c r="C17" s="6">
+        <v>14553.050421100001</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1147012</v>
+      </c>
+      <c r="E17" s="6">
+        <v>19796.770049700001</v>
+      </c>
+      <c r="F17" s="6">
+        <v>680652.6</v>
+      </c>
+      <c r="G17" s="6">
+        <v>9832.5468033500001</v>
+      </c>
+      <c r="H17" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0650814607007624</v>
+      </c>
+      <c r="I17" s="6">
+        <f t="shared" si="1"/>
+        <v>0.63203389802179211</v>
+      </c>
+      <c r="J17" s="6">
+        <f t="shared" si="2"/>
+        <v>1.3513532726908729E-2</v>
+      </c>
+      <c r="K17" s="6">
+        <f t="shared" si="3"/>
+        <v>1.8382695875624303E-2</v>
+      </c>
+      <c r="L17" s="6">
+        <f t="shared" si="4"/>
+        <v>9.1302125101748108E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="6">
+        <v>142122988.40000001</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1688359.3844900001</v>
+      </c>
+      <c r="D18" s="6">
+        <v>143348534.59999999</v>
+      </c>
+      <c r="E18" s="6">
+        <v>2386850.5735499999</v>
+      </c>
+      <c r="F18" s="6">
+        <v>97369622</v>
+      </c>
+      <c r="G18" s="6">
+        <v>1822551.4533800001</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0086231384084798</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="1"/>
+        <v>0.6851081805707373</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" si="2"/>
+        <v>1.1879565744411269E-2</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" si="3"/>
+        <v>1.6794261086266322E-2</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="4"/>
+        <v>1.2823762530594241E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="6">
+        <v>147012341.40000001</v>
+      </c>
+      <c r="C19" s="6">
+        <v>7606800.8915200001</v>
+      </c>
+      <c r="D19" s="6">
+        <v>79703584.200000003</v>
+      </c>
+      <c r="E19" s="6">
+        <v>8290771.0046100002</v>
+      </c>
+      <c r="F19" s="6">
+        <v>83981813.400000006</v>
+      </c>
+      <c r="G19" s="6">
+        <v>1750299.80644</v>
+      </c>
+      <c r="H19" s="6">
+        <f t="shared" si="0"/>
+        <v>0.54215573632105962</v>
+      </c>
+      <c r="I19" s="6">
+        <f t="shared" si="1"/>
+        <v>0.57125689313047023</v>
+      </c>
+      <c r="J19" s="6">
+        <f t="shared" si="2"/>
+        <v>5.1742600784943353E-2</v>
+      </c>
+      <c r="K19" s="6">
+        <f t="shared" si="3"/>
+        <v>5.6395068098752152E-2</v>
+      </c>
+      <c r="L19" s="6">
+        <f t="shared" si="4"/>
+        <v>1.1905801851544417E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="6">
+        <v>2898308.6</v>
+      </c>
+      <c r="C20" s="6">
+        <v>36388.156362200003</v>
+      </c>
+      <c r="D20" s="6">
+        <v>2883458.6</v>
+      </c>
+      <c r="E20" s="6">
+        <v>39483.321585700003</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1164719.2</v>
+      </c>
+      <c r="G20" s="6">
+        <v>45536.9098486</v>
+      </c>
+      <c r="H20" s="6">
+        <f t="shared" si="0"/>
+        <v>0.99487632200380594</v>
+      </c>
+      <c r="I20" s="6">
+        <f t="shared" si="1"/>
+        <v>0.40186169271277733</v>
+      </c>
+      <c r="J20" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2554962698658108E-2</v>
+      </c>
+      <c r="K20" s="6">
+        <f t="shared" si="3"/>
+        <v>1.3622883907427941E-2</v>
+      </c>
+      <c r="L20" s="6">
+        <f t="shared" si="4"/>
+        <v>1.5711546330366612E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="6">
+        <v>524441.59999999998</v>
+      </c>
+      <c r="C21" s="6">
+        <v>15199.6411352</v>
+      </c>
+      <c r="D21" s="6">
+        <v>527874.6</v>
+      </c>
+      <c r="E21" s="6">
+        <v>7304.8818635199996</v>
+      </c>
+      <c r="F21" s="6">
+        <v>171678</v>
+      </c>
+      <c r="G21" s="6">
+        <v>8760.4336650599998</v>
+      </c>
+      <c r="H21" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0065460100800547</v>
+      </c>
+      <c r="I21" s="6">
+        <f t="shared" si="1"/>
+        <v>0.32735389412281557</v>
+      </c>
+      <c r="J21" s="6">
+        <f t="shared" si="2"/>
+        <v>2.8982523764705163E-2</v>
+      </c>
+      <c r="K21" s="6">
+        <f t="shared" si="3"/>
+        <v>1.3928875709936053E-2</v>
+      </c>
+      <c r="L21" s="6">
+        <f t="shared" si="4"/>
+        <v>1.6704307333857575E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="6">
+        <v>22343582893.799999</v>
+      </c>
+      <c r="C22" s="6">
+        <v>36130395.837800004</v>
+      </c>
+      <c r="D22" s="6">
+        <v>25119837726.799999</v>
+      </c>
+      <c r="E22" s="6">
+        <v>55201502.9027</v>
+      </c>
+      <c r="F22" s="6">
+        <v>42836296043.599998</v>
+      </c>
+      <c r="G22" s="6">
+        <v>80425547.617799997</v>
+      </c>
+      <c r="H22" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1242528938261898</v>
+      </c>
+      <c r="I22" s="6">
+        <f t="shared" si="1"/>
+        <v>1.9171632520711981</v>
+      </c>
+      <c r="J22" s="6">
+        <f t="shared" si="2"/>
+        <v>1.6170368024470074E-3</v>
+      </c>
+      <c r="K22" s="6">
+        <f t="shared" si="3"/>
+        <v>2.470575250400757E-3</v>
+      </c>
+      <c r="L22" s="6">
+        <f t="shared" si="4"/>
+        <v>3.5994919883738452E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="6">
+        <v>212878332.19999999</v>
+      </c>
+      <c r="C23" s="6">
+        <v>397135.33510700002</v>
+      </c>
+      <c r="D23" s="6">
+        <v>216692924.80000001</v>
+      </c>
+      <c r="E23" s="6">
+        <v>2671681.7472000001</v>
+      </c>
+      <c r="F23" s="6">
+        <v>423024331.39999998</v>
+      </c>
+      <c r="G23" s="6">
+        <v>637180.44013500004</v>
+      </c>
+      <c r="H23" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0179191210330236</v>
+      </c>
+      <c r="I23" s="6">
+        <f t="shared" si="1"/>
+        <v>1.9871648139490639</v>
+      </c>
+      <c r="J23" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8655507632119642E-3</v>
+      </c>
+      <c r="K23" s="6">
+        <f t="shared" si="3"/>
+        <v>1.2550275641439849E-2</v>
+      </c>
+      <c r="L23" s="6">
+        <f t="shared" si="4"/>
+        <v>2.9931671934387699E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="6">
+        <v>709259220</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1579941.92038</v>
+      </c>
+      <c r="D24" s="6">
+        <v>684113708.79999995</v>
+      </c>
+      <c r="E24" s="6">
+        <v>478306.96039199998</v>
+      </c>
+      <c r="F24" s="6">
+        <v>640069622.20000005</v>
+      </c>
+      <c r="G24" s="6">
+        <v>1361179.1296999999</v>
+      </c>
+      <c r="H24" s="6">
+        <f t="shared" si="0"/>
+        <v>0.96454679686786438</v>
+      </c>
+      <c r="I24" s="6">
+        <f t="shared" si="1"/>
+        <v>0.90244808125300091</v>
+      </c>
+      <c r="J24" s="6">
+        <f t="shared" si="2"/>
+        <v>2.2275944757968744E-3</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" si="3"/>
+        <v>6.7437538618391173E-4</v>
+      </c>
+      <c r="L24" s="6">
+        <f t="shared" si="4"/>
+        <v>1.9191560593318758E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="6">
+        <v>557809444.79999995</v>
+      </c>
+      <c r="C25" s="6">
+        <v>303447.01951800002</v>
+      </c>
+      <c r="D25" s="6">
+        <v>589765440.60000002</v>
+      </c>
+      <c r="E25" s="6">
+        <v>754401.82024599996</v>
+      </c>
+      <c r="F25" s="6">
+        <v>555224957.20000005</v>
+      </c>
+      <c r="G25" s="6">
+        <v>1604658.79428</v>
+      </c>
+      <c r="H25" s="6">
+        <f t="shared" si="0"/>
+        <v>1.057288373472159</v>
+      </c>
+      <c r="I25" s="6">
+        <f t="shared" si="1"/>
+        <v>0.99536671954178446</v>
+      </c>
+      <c r="J25" s="6">
+        <f t="shared" si="2"/>
+        <v>5.4399763637347437E-4</v>
+      </c>
+      <c r="K25" s="6">
+        <f t="shared" si="3"/>
+        <v>1.3524364409363619E-3</v>
+      </c>
+      <c r="L25" s="6">
+        <f t="shared" si="4"/>
+        <v>2.8767149951276698E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="6">
+        <v>1480365255.8</v>
+      </c>
+      <c r="C26" s="6">
+        <v>747950.06621399999</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1489458102</v>
+      </c>
+      <c r="E26" s="6">
+        <v>1423514.07947</v>
+      </c>
+      <c r="F26" s="6">
+        <v>1615958912</v>
+      </c>
+      <c r="G26" s="6">
+        <v>3696074.7233500001</v>
+      </c>
+      <c r="H26" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0061422991146103</v>
+      </c>
+      <c r="I26" s="6">
+        <f t="shared" si="1"/>
+        <v>1.0915947301983417</v>
+      </c>
+      <c r="J26" s="6">
+        <f t="shared" si="2"/>
+        <v>5.0524697420691793E-4</v>
+      </c>
+      <c r="K26" s="6">
+        <f t="shared" si="3"/>
+        <v>9.6159652078616419E-4</v>
+      </c>
+      <c r="L26" s="6">
+        <f t="shared" si="4"/>
+        <v>2.4967316065200511E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="6">
+        <v>2809106711.8000002</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1625417.0842299999</v>
+      </c>
+      <c r="D27" s="6">
+        <v>2026142191</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1372255.2624299999</v>
+      </c>
+      <c r="F27" s="6">
+        <v>1700852976.4000001</v>
+      </c>
+      <c r="G27" s="6">
+        <v>3260068.4286600002</v>
+      </c>
+      <c r="H27" s="6">
+        <f t="shared" si="0"/>
+        <v>0.72127633403492264</v>
+      </c>
+      <c r="I27" s="6">
+        <f t="shared" si="1"/>
+        <v>0.60547823593007588</v>
+      </c>
+      <c r="J27" s="6">
+        <f t="shared" si="2"/>
+        <v>5.7862418590302553E-4</v>
+      </c>
+      <c r="K27" s="6">
+        <f t="shared" si="3"/>
+        <v>4.8850236150363099E-4</v>
+      </c>
+      <c r="L27" s="6">
+        <f t="shared" si="4"/>
+        <v>1.1605356304072321E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="6">
+        <v>4289303031.1999998</v>
+      </c>
+      <c r="C28" s="6">
+        <v>1861084.3700600001</v>
+      </c>
+      <c r="D28" s="6">
+        <v>3515418335.1999998</v>
+      </c>
+      <c r="E28" s="6">
+        <v>2787594.4441300002</v>
+      </c>
+      <c r="F28" s="6">
+        <v>3316703760.4000001</v>
+      </c>
+      <c r="G28" s="6">
+        <v>6826824.3310099998</v>
+      </c>
+      <c r="H28" s="6">
+        <f t="shared" si="0"/>
+        <v>0.81957798496146506</v>
+      </c>
+      <c r="I28" s="6">
+        <f t="shared" si="1"/>
+        <v>0.77325004465168323</v>
+      </c>
+      <c r="J28" s="6">
+        <f t="shared" si="2"/>
+        <v>4.3388969175706213E-4</v>
+      </c>
+      <c r="K28" s="6">
+        <f t="shared" si="3"/>
+        <v>6.498944989088651E-4</v>
+      </c>
+      <c r="L28" s="6">
+        <f t="shared" si="4"/>
+        <v>1.5915929187917714E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="6">
+        <v>1761233472.5999999</v>
+      </c>
+      <c r="C29" s="6">
+        <v>2709142.0694300001</v>
+      </c>
+      <c r="D29" s="6">
+        <v>1398700815.2</v>
+      </c>
+      <c r="E29" s="6">
+        <v>1047197.5988799999</v>
+      </c>
+      <c r="F29" s="6">
+        <v>1395896628.8</v>
+      </c>
+      <c r="G29" s="6">
+        <v>1064847.9888800001</v>
+      </c>
+      <c r="H29" s="6">
+        <f t="shared" si="0"/>
+        <v>0.79415979593845931</v>
+      </c>
+      <c r="I29" s="6">
+        <f t="shared" si="1"/>
+        <v>0.79256762406367631</v>
+      </c>
+      <c r="J29" s="6">
+        <f t="shared" si="2"/>
+        <v>1.5382072346323634E-3</v>
+      </c>
+      <c r="K29" s="6">
+        <f t="shared" si="3"/>
+        <v>5.9458193088624814E-4</v>
+      </c>
+      <c r="L29" s="6">
+        <f t="shared" si="4"/>
+        <v>6.04603538057922E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="6">
+        <v>23773682</v>
+      </c>
+      <c r="C30" s="6">
+        <v>104006.54266200001</v>
+      </c>
+      <c r="D30" s="6">
+        <v>20807231.800000001</v>
+      </c>
+      <c r="E30" s="6">
+        <v>251232.72346800001</v>
+      </c>
+      <c r="F30" s="6">
+        <v>36443818.399999999</v>
+      </c>
+      <c r="G30" s="6">
+        <v>169420.30880500001</v>
+      </c>
+      <c r="H30" s="6">
+        <f t="shared" si="0"/>
+        <v>0.87522125516779437</v>
+      </c>
+      <c r="I30" s="6">
+        <f t="shared" si="1"/>
+        <v>1.5329480052774322</v>
+      </c>
+      <c r="J30" s="6">
+        <f t="shared" si="2"/>
+        <v>4.3748605143284075E-3</v>
+      </c>
+      <c r="K30" s="6">
+        <f t="shared" si="3"/>
+        <v>1.0567682509928416E-2</v>
+      </c>
+      <c r="L30" s="6">
+        <f t="shared" si="4"/>
+        <v>7.1263807097697368E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="6">
+        <v>132607255038</v>
+      </c>
+      <c r="C31" s="6">
+        <v>225116431.33000001</v>
+      </c>
+      <c r="D31" s="6">
+        <v>144831816170</v>
+      </c>
+      <c r="E31" s="6">
+        <v>235396070.604</v>
+      </c>
+      <c r="F31" s="6">
+        <v>131505963283</v>
+      </c>
+      <c r="G31" s="6">
+        <v>122990431.06999999</v>
+      </c>
+      <c r="H31" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0921862165723657</v>
+      </c>
+      <c r="I31" s="6">
+        <f t="shared" si="1"/>
+        <v>0.99169508670785456</v>
+      </c>
+      <c r="J31" s="6">
+        <f t="shared" si="2"/>
+        <v>1.6976177605477962E-3</v>
+      </c>
+      <c r="K31" s="6">
+        <f t="shared" si="3"/>
+        <v>1.7751371939381808E-3</v>
+      </c>
+      <c r="L31" s="6">
+        <f t="shared" si="4"/>
+        <v>9.2747890026647327E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="6">
+        <v>10270371487.799999</v>
+      </c>
+      <c r="C32" s="6">
+        <v>28108011.878800001</v>
+      </c>
+      <c r="D32" s="6">
+        <v>10284664219</v>
+      </c>
+      <c r="E32" s="6">
+        <v>35210784.745399997</v>
+      </c>
+      <c r="F32" s="6">
+        <v>12743590795.200001</v>
+      </c>
+      <c r="G32" s="6">
+        <v>14444039.3672</v>
+      </c>
+      <c r="H32" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0013916469542488</v>
+      </c>
+      <c r="I32" s="6">
+        <f t="shared" si="1"/>
+        <v>1.2408110855910028</v>
+      </c>
+      <c r="J32" s="6">
+        <f t="shared" si="2"/>
+        <v>2.7368057632763364E-3</v>
+      </c>
+      <c r="K32" s="6">
+        <f t="shared" si="3"/>
+        <v>3.4283847266115245E-3</v>
+      </c>
+      <c r="L32" s="6">
+        <f t="shared" si="4"/>
+        <v>1.4063794463869035E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="6">
+        <v>9607753811.2000008</v>
+      </c>
+      <c r="C33" s="6">
+        <v>73322321.484699994</v>
+      </c>
+      <c r="D33" s="6">
+        <v>9501860354.3999996</v>
+      </c>
+      <c r="E33" s="6">
+        <v>57971605.242200002</v>
+      </c>
+      <c r="F33" s="6">
+        <v>12104774641.200001</v>
+      </c>
+      <c r="G33" s="6">
+        <v>45363358.215300001</v>
+      </c>
+      <c r="H33" s="6">
+        <f t="shared" si="0"/>
+        <v>0.98897833365832521</v>
+      </c>
+      <c r="I33" s="6">
+        <f t="shared" si="1"/>
+        <v>1.2598964210645323</v>
+      </c>
+      <c r="J33" s="6">
+        <f t="shared" si="2"/>
+        <v>7.6315778823585504E-3</v>
+      </c>
+      <c r="K33" s="6">
+        <f t="shared" si="3"/>
+        <v>6.0338354189114467E-3</v>
+      </c>
+      <c r="L33" s="6">
+        <f t="shared" si="4"/>
+        <v>4.7215362827489182E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="6">
+        <v>1563931880510</v>
+      </c>
+      <c r="C34" s="6">
+        <v>854308712.37699997</v>
+      </c>
+      <c r="D34" s="6">
+        <v>1076152871170</v>
+      </c>
+      <c r="E34" s="6">
+        <v>215388522.50600001</v>
+      </c>
+      <c r="F34" s="6">
+        <v>990270689373</v>
+      </c>
+      <c r="G34" s="6">
+        <v>439518725.89099997</v>
+      </c>
+      <c r="H34" s="6">
+        <f t="shared" si="0"/>
+        <v>0.68810725363502745</v>
+      </c>
+      <c r="I34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.63319298091811493</v>
+      </c>
+      <c r="J34" s="6">
+        <f t="shared" si="2"/>
+        <v>5.4625698409473491E-4</v>
+      </c>
+      <c r="K34" s="6">
+        <f t="shared" si="3"/>
+        <v>1.3772244506951388E-4</v>
+      </c>
+      <c r="L34" s="6">
+        <f t="shared" si="4"/>
+        <v>2.8103444361507127E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="6">
+        <v>42873465287.800003</v>
+      </c>
+      <c r="C35" s="6">
+        <v>8506146.6524400003</v>
+      </c>
+      <c r="D35" s="6">
+        <v>20444634090.799999</v>
+      </c>
+      <c r="E35" s="6">
+        <v>6658858.1248500003</v>
+      </c>
+      <c r="F35" s="6">
+        <v>19627802173.200001</v>
+      </c>
+      <c r="G35" s="6">
+        <v>4395208.3865200002</v>
+      </c>
+      <c r="H35" s="6">
+        <f t="shared" si="0"/>
+        <v>0.47685984684372335</v>
+      </c>
+      <c r="I35" s="6">
+        <f t="shared" si="1"/>
+        <v>0.45780769157433265</v>
+      </c>
+      <c r="J35" s="6">
+        <f t="shared" si="2"/>
+        <v>1.9840119279699312E-4</v>
+      </c>
+      <c r="K35" s="6">
+        <f t="shared" si="3"/>
+        <v>1.5531420378900031E-4</v>
+      </c>
+      <c r="L35" s="6">
+        <f t="shared" si="4"/>
+        <v>1.025158185142243E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="6">
+        <v>22897412817.799999</v>
+      </c>
+      <c r="C36" s="6">
+        <v>3508026.8909300002</v>
+      </c>
+      <c r="D36" s="6">
+        <v>10743890735.799999</v>
+      </c>
+      <c r="E36" s="6">
+        <v>1942872.9863700001</v>
+      </c>
+      <c r="F36" s="6">
+        <v>10553539604.6</v>
+      </c>
+      <c r="G36" s="6">
+        <v>2829252.8361900002</v>
+      </c>
+      <c r="H36" s="6">
+        <f t="shared" si="0"/>
+        <v>0.46921854540037422</v>
+      </c>
+      <c r="I36" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46090532972336007</v>
+      </c>
+      <c r="J36" s="6">
+        <f t="shared" si="2"/>
+        <v>1.5320625604491565E-4</v>
+      </c>
+      <c r="K36" s="6">
+        <f t="shared" si="3"/>
+        <v>8.4851201392484345E-5</v>
+      </c>
+      <c r="L36" s="6">
+        <f t="shared" si="4"/>
+        <v>1.2356211851107451E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="6">
+        <v>1120133</v>
+      </c>
+      <c r="C37" s="6">
+        <v>687.77583557399998</v>
+      </c>
+      <c r="D37" s="6">
+        <v>1163122.6000000001</v>
+      </c>
+      <c r="E37" s="6">
+        <v>2091.8385788599999</v>
+      </c>
+      <c r="F37" s="6">
+        <v>1062673.6000000001</v>
+      </c>
+      <c r="G37" s="6">
+        <v>863.63385760400001</v>
+      </c>
+      <c r="H37" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0383790139206683</v>
+      </c>
+      <c r="I37" s="6">
+        <f t="shared" si="1"/>
+        <v>0.94870305579783842</v>
+      </c>
+      <c r="J37" s="6">
+        <f t="shared" si="2"/>
+        <v>6.1401265347418561E-4</v>
+      </c>
+      <c r="K37" s="6">
+        <f t="shared" si="3"/>
+        <v>1.8674912522530806E-3</v>
+      </c>
+      <c r="L37" s="6">
+        <f t="shared" si="4"/>
+        <v>7.7101010112549137E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="J3:L3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440270B8-E650-47B8-847B-14A2543F142D}">
+  <dimension ref="A1:L37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="42.86328125" customWidth="1"/>
+    <col min="2" max="2" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.65">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+    </row>
+    <row r="4" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="6">
+        <v>10993802.800000001</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1773.7289984700001</v>
+      </c>
+      <c r="D5" s="6">
+        <v>11506634.800000001</v>
+      </c>
+      <c r="E5" s="6">
+        <v>6242.3846533200003</v>
+      </c>
+      <c r="F5" s="6">
+        <v>11497720.6</v>
+      </c>
+      <c r="G5" s="6">
+        <v>484210.22772099997</v>
+      </c>
+      <c r="H5" s="6">
+        <f>D5/B5</f>
+        <v>1.0466473711898852</v>
+      </c>
+      <c r="I5" s="6">
+        <f>F5/B5</f>
+        <v>1.0458365325599617</v>
+      </c>
+      <c r="J5" s="6">
+        <f>C5/B5</f>
+        <v>1.6133898622140103E-4</v>
+      </c>
+      <c r="K5" s="6">
+        <f>E5/B5</f>
+        <v>5.6780940743452303E-4</v>
+      </c>
+      <c r="L5" s="6">
+        <f>G5/B5</f>
+        <v>4.4043925157635166E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6">
+        <v>216409745713</v>
+      </c>
+      <c r="C6" s="6">
+        <v>35294538.0647</v>
+      </c>
+      <c r="D6" s="6">
+        <v>226534065733</v>
+      </c>
+      <c r="E6" s="6">
+        <v>124032309.205</v>
+      </c>
+      <c r="F6" s="6">
+        <v>226361265032</v>
+      </c>
+      <c r="G6" s="6">
+        <v>9553146491.4699993</v>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" ref="H6:H37" si="0">D6/B6</f>
+        <v>1.0467831057545198</v>
+      </c>
+      <c r="I6" s="6">
+        <f t="shared" ref="I6:I37" si="1">F6/B6</f>
+        <v>1.0459846172186607</v>
+      </c>
+      <c r="J6" s="6">
+        <f t="shared" ref="J6:J37" si="2">C6/B6</f>
+        <v>1.6309125981556853E-4</v>
+      </c>
+      <c r="K6" s="6">
+        <f t="shared" ref="K6:K37" si="3">E6/B6</f>
+        <v>5.7313643059998852E-4</v>
+      </c>
+      <c r="L6" s="6">
+        <f t="shared" ref="L6:L37" si="4">G6/B6</f>
+        <v>4.4143790567266167E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6">
+        <v>262280845319</v>
+      </c>
+      <c r="C7" s="6">
+        <v>98838550.429100007</v>
+      </c>
+      <c r="D7" s="6">
+        <v>232783010668</v>
+      </c>
+      <c r="E7" s="6">
+        <v>123231903.88500001</v>
+      </c>
+      <c r="F7" s="6">
+        <v>230464705735</v>
+      </c>
+      <c r="G7" s="6">
+        <v>9731083983.8999996</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="0"/>
+        <v>0.88753340101857936</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" si="1"/>
+        <v>0.87869438370421782</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" si="2"/>
+        <v>3.7684242747077954E-4</v>
+      </c>
+      <c r="K7" s="6">
+        <f t="shared" si="3"/>
+        <v>4.6984713555852227E-4</v>
+      </c>
+      <c r="L7" s="6">
+        <f t="shared" si="4"/>
+        <v>3.7101771469679891E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6">
+        <v>128350330.8</v>
+      </c>
+      <c r="C8" s="6">
+        <v>22670.2774522</v>
+      </c>
+      <c r="D8" s="6">
+        <v>73650716.200000003</v>
+      </c>
+      <c r="E8" s="6">
+        <v>49848.839623</v>
+      </c>
+      <c r="F8" s="6">
+        <v>14298501.800000001</v>
+      </c>
+      <c r="G8" s="6">
+        <v>617578.60468800005</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.57382568273053491</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" si="1"/>
+        <v>0.11140214217507885</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="2"/>
+        <v>1.7662811861019373E-4</v>
+      </c>
+      <c r="K8" s="6">
+        <f t="shared" si="3"/>
+        <v>3.8838107632676238E-4</v>
+      </c>
+      <c r="L8" s="6">
+        <f t="shared" si="4"/>
+        <v>4.811663521540375E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="6">
+        <v>96803733.599999994</v>
+      </c>
+      <c r="C9" s="6">
+        <v>20212.253249900001</v>
+      </c>
+      <c r="D9" s="6">
+        <v>55276355.600000001</v>
+      </c>
+      <c r="E9" s="6">
+        <v>33047.157951000001</v>
+      </c>
+      <c r="F9" s="6">
+        <v>7311102.5999999996</v>
+      </c>
+      <c r="G9" s="6">
+        <v>18140.853691</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="0"/>
+        <v>0.57101470722612713</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="1"/>
+        <v>7.5525006403265427E-2</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="2"/>
+        <v>2.0879621578872659E-4</v>
+      </c>
+      <c r="K9" s="6">
+        <f t="shared" si="3"/>
+        <v>3.4138309259385842E-4</v>
+      </c>
+      <c r="L9" s="6">
+        <f t="shared" si="4"/>
+        <v>1.8739828533844899E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6">
+        <v>5006461781.8000002</v>
+      </c>
+      <c r="C10" s="6">
+        <v>6887086.4564300003</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2566553087</v>
+      </c>
+      <c r="E10" s="6">
+        <v>3096266.9693800001</v>
+      </c>
+      <c r="F10" s="6">
+        <v>455642359</v>
+      </c>
+      <c r="G10" s="6">
+        <v>3153803.81819</v>
+      </c>
+      <c r="H10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.51264809337608352</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="1"/>
+        <v>9.1010853344850748E-2</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="2"/>
+        <v>1.3756394748615955E-3</v>
+      </c>
+      <c r="K10" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1845413074676113E-4</v>
+      </c>
+      <c r="L10" s="6">
+        <f t="shared" si="4"/>
+        <v>6.2994664808089195E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="6">
+        <v>48028447.200000003</v>
+      </c>
+      <c r="C11" s="6">
+        <v>14656.2248263</v>
+      </c>
+      <c r="D11" s="6">
+        <v>52979508.600000001</v>
+      </c>
+      <c r="E11" s="6">
+        <v>34795.673769000001</v>
+      </c>
+      <c r="F11" s="6">
+        <v>13811065.800000001</v>
+      </c>
+      <c r="G11" s="6">
+        <v>11879.022643300001</v>
+      </c>
+      <c r="H11" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1030860185710938</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="1"/>
+        <v>0.28756011499784651</v>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" si="2"/>
+        <v>3.0515716582025994E-4</v>
+      </c>
+      <c r="K11" s="6">
+        <f t="shared" si="3"/>
+        <v>7.2448050681513598E-4</v>
+      </c>
+      <c r="L11" s="6">
+        <f t="shared" si="4"/>
+        <v>2.4733305646616868E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="6">
+        <v>78414325.200000003</v>
+      </c>
+      <c r="C12" s="6">
+        <v>27868.809327999999</v>
+      </c>
+      <c r="D12" s="6">
+        <v>55528342</v>
+      </c>
+      <c r="E12" s="6">
+        <v>18977.7241417</v>
+      </c>
+      <c r="F12" s="6">
+        <v>32812194.800000001</v>
+      </c>
+      <c r="G12" s="6">
+        <v>27211.579758600001</v>
+      </c>
+      <c r="H12" s="6">
+        <f t="shared" si="0"/>
+        <v>0.70814027740941399</v>
+      </c>
+      <c r="I12" s="6">
+        <f t="shared" si="1"/>
+        <v>0.41844643458080794</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" si="2"/>
+        <v>3.5540456742972774E-4</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" si="3"/>
+        <v>2.420185864419069E-4</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="4"/>
+        <v>3.4702306867011079E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="6">
+        <v>46688745.399999999</v>
+      </c>
+      <c r="C13" s="6">
+        <v>49011.521354099998</v>
+      </c>
+      <c r="D13" s="6">
+        <v>31882429.600000001</v>
+      </c>
+      <c r="E13" s="6">
+        <v>7196.4395530000002</v>
+      </c>
+      <c r="F13" s="6">
+        <v>12104994.800000001</v>
+      </c>
+      <c r="G13" s="6">
+        <v>8342.8682453900001</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" si="0"/>
+        <v>0.68287184260042255</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="1"/>
+        <v>0.25927008096473719</v>
+      </c>
+      <c r="J13" s="6">
+        <f t="shared" si="2"/>
+        <v>1.0497502328280597E-3</v>
+      </c>
+      <c r="K13" s="6">
+        <f t="shared" si="3"/>
+        <v>1.5413649459511928E-4</v>
+      </c>
+      <c r="L13" s="6">
+        <f t="shared" si="4"/>
+        <v>1.7869120649770126E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="6">
+        <v>2608042481.8000002</v>
+      </c>
+      <c r="C14" s="6">
+        <v>4278606.0653799996</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1687621141.5999999</v>
+      </c>
+      <c r="E14" s="6">
+        <v>2627662.3417400001</v>
+      </c>
+      <c r="F14" s="6">
+        <v>803254084.60000002</v>
+      </c>
+      <c r="G14" s="6">
+        <v>4322649.3069700003</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="0"/>
+        <v>0.64708345564802672</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="1"/>
+        <v>0.30799118120407909</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="2"/>
+        <v>1.640543087483384E-3</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="3"/>
+        <v>1.0075228298913517E-3</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="4"/>
+        <v>1.657430558411236E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1029766540.6</v>
+      </c>
+      <c r="C15" s="6">
+        <v>2565880.0191899999</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1077653752.2</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1482132.35543</v>
+      </c>
+      <c r="F15" s="6">
+        <v>422390470.19999999</v>
+      </c>
+      <c r="G15" s="6">
+        <v>136864.071249</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0465029787937159</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" si="1"/>
+        <v>0.41018080656795425</v>
+      </c>
+      <c r="J15" s="6">
+        <f t="shared" si="2"/>
+        <v>2.4917104198151296E-3</v>
+      </c>
+      <c r="K15" s="6">
+        <f t="shared" si="3"/>
+        <v>1.4392896807138694E-3</v>
+      </c>
+      <c r="L15" s="6">
+        <f t="shared" si="4"/>
+        <v>1.3290786392152078E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="6">
+        <v>49756746.399999999</v>
+      </c>
+      <c r="C16" s="6">
+        <v>50574.352984899997</v>
+      </c>
+      <c r="D16" s="6">
+        <v>52434312.600000001</v>
+      </c>
+      <c r="E16" s="6">
+        <v>14407.533732</v>
+      </c>
+      <c r="F16" s="6">
+        <v>47007363.799999997</v>
+      </c>
+      <c r="G16" s="6">
+        <v>10735.658739</v>
+      </c>
+      <c r="H16" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0538131287458941</v>
+      </c>
+      <c r="I16" s="6">
+        <f t="shared" si="1"/>
+        <v>0.94474352125242655</v>
+      </c>
+      <c r="J16" s="6">
+        <f t="shared" si="2"/>
+        <v>1.0164320749256226E-3</v>
+      </c>
+      <c r="K16" s="6">
+        <f t="shared" si="3"/>
+        <v>2.8955940197890432E-4</v>
+      </c>
+      <c r="L16" s="6">
+        <f t="shared" si="4"/>
+        <v>2.1576287671012188E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="6">
+        <v>40443157.799999997</v>
+      </c>
+      <c r="C17" s="6">
+        <v>39378.278516999999</v>
+      </c>
+      <c r="D17" s="6">
+        <v>42567336.200000003</v>
+      </c>
+      <c r="E17" s="6">
+        <v>28097.415812800002</v>
+      </c>
+      <c r="F17" s="6">
+        <v>37941717.399999999</v>
+      </c>
+      <c r="G17" s="6">
+        <v>64778.036835300001</v>
+      </c>
+      <c r="H17" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0525225653868207</v>
+      </c>
+      <c r="I17" s="6">
+        <f t="shared" si="1"/>
+        <v>0.93814923126502259</v>
+      </c>
+      <c r="J17" s="6">
+        <f t="shared" si="2"/>
+        <v>9.7366972954322578E-4</v>
+      </c>
+      <c r="K17" s="6">
+        <f t="shared" si="3"/>
+        <v>6.9473842650338261E-4</v>
+      </c>
+      <c r="L17" s="6">
+        <f t="shared" si="4"/>
+        <v>1.6017057113997168E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1647632761.4000001</v>
+      </c>
+      <c r="C18" s="6">
+        <v>7625281.1434800001</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1659695489.8</v>
+      </c>
+      <c r="E18" s="6">
+        <v>7947517.3408000004</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1520164122.4000001</v>
+      </c>
+      <c r="G18" s="6">
+        <v>7301986.9838899998</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0073212482068821</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="1"/>
+        <v>0.92263528500629632</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" si="2"/>
+        <v>4.6280222887779728E-3</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" si="3"/>
+        <v>4.823597543694727E-3</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="4"/>
+        <v>4.431804923377144E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="6">
+        <v>248860750.40000001</v>
+      </c>
+      <c r="C19" s="6">
+        <v>360608.92223899998</v>
+      </c>
+      <c r="D19" s="6">
+        <v>258500446.40000001</v>
+      </c>
+      <c r="E19" s="6">
+        <v>468561.58675399999</v>
+      </c>
+      <c r="F19" s="6">
+        <v>152979552.40000001</v>
+      </c>
+      <c r="G19" s="6">
+        <v>368523.96054300002</v>
+      </c>
+      <c r="H19" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0387353007033286</v>
+      </c>
+      <c r="I19" s="6">
+        <f t="shared" si="1"/>
+        <v>0.61471948531101106</v>
+      </c>
+      <c r="J19" s="6">
+        <f t="shared" si="2"/>
+        <v>1.44903895716534E-3</v>
+      </c>
+      <c r="K19" s="6">
+        <f t="shared" si="3"/>
+        <v>1.8828263838346121E-3</v>
+      </c>
+      <c r="L19" s="6">
+        <f t="shared" si="4"/>
+        <v>1.4808440461208223E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="6">
+        <v>21592205.800000001</v>
+      </c>
+      <c r="C20" s="6">
+        <v>10532.0337143</v>
+      </c>
+      <c r="D20" s="6">
+        <v>21157315.800000001</v>
+      </c>
+      <c r="E20" s="6">
+        <v>10726.5268265</v>
+      </c>
+      <c r="F20" s="6">
+        <v>4130390</v>
+      </c>
+      <c r="G20" s="6">
+        <v>9405.1766384300008</v>
+      </c>
+      <c r="H20" s="6">
+        <f t="shared" si="0"/>
+        <v>0.97985893594993434</v>
+      </c>
+      <c r="I20" s="6">
+        <f t="shared" si="1"/>
+        <v>0.19129078512210179</v>
+      </c>
+      <c r="J20" s="6">
+        <f t="shared" si="2"/>
+        <v>4.8777016168954814E-4</v>
+      </c>
+      <c r="K20" s="6">
+        <f t="shared" si="3"/>
+        <v>4.9677772275123462E-4</v>
+      </c>
+      <c r="L20" s="6">
+        <f t="shared" si="4"/>
+        <v>4.3558202091747387E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="6">
+        <v>10140875</v>
+      </c>
+      <c r="C21" s="6">
+        <v>2601.2293247600001</v>
+      </c>
+      <c r="D21" s="6">
+        <v>10509476.800000001</v>
+      </c>
+      <c r="E21" s="6">
+        <v>2335.2011819099998</v>
+      </c>
+      <c r="F21" s="6">
+        <v>8718003.8000000007</v>
+      </c>
+      <c r="G21" s="6">
+        <v>3251.50915115</v>
+      </c>
+      <c r="H21" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0363481257781011</v>
+      </c>
+      <c r="I21" s="6">
+        <f t="shared" si="1"/>
+        <v>0.85968950411083866</v>
+      </c>
+      <c r="J21" s="6">
+        <f t="shared" si="2"/>
+        <v>2.5650935691052303E-4</v>
+      </c>
+      <c r="K21" s="6">
+        <f t="shared" si="3"/>
+        <v>2.3027610358179149E-4</v>
+      </c>
+      <c r="L21" s="6">
+        <f t="shared" si="4"/>
+        <v>3.2063398386726985E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="6">
+        <v>19383918445.799999</v>
+      </c>
+      <c r="C22" s="6">
+        <v>62997973.089599997</v>
+      </c>
+      <c r="D22" s="6">
+        <v>18800933710.599998</v>
+      </c>
+      <c r="E22" s="6">
+        <v>26704578.8662</v>
+      </c>
+      <c r="F22" s="6">
+        <v>16532536728</v>
+      </c>
+      <c r="G22" s="6">
+        <v>19505318.508400001</v>
+      </c>
+      <c r="H22" s="6">
+        <f t="shared" si="0"/>
+        <v>0.96992430932733731</v>
+      </c>
+      <c r="I22" s="6">
+        <f t="shared" si="1"/>
+        <v>0.85289962265509733</v>
+      </c>
+      <c r="J22" s="6">
+        <f t="shared" si="2"/>
+        <v>3.2500122854803928E-3</v>
+      </c>
+      <c r="K22" s="6">
+        <f t="shared" si="3"/>
+        <v>1.3776666952489268E-3</v>
+      </c>
+      <c r="L22" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0062629268142791E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="6">
+        <v>266567566.19999999</v>
+      </c>
+      <c r="C23" s="6">
+        <v>1189484.3162100001</v>
+      </c>
+      <c r="D23" s="6">
+        <v>266712849.40000001</v>
+      </c>
+      <c r="E23" s="6">
+        <v>695704.353581</v>
+      </c>
+      <c r="F23" s="6">
+        <v>224736287.80000001</v>
+      </c>
+      <c r="G23" s="6">
+        <v>540123.93872800004</v>
+      </c>
+      <c r="H23" s="6">
+        <f t="shared" si="0"/>
+        <v>1.000545014541983</v>
+      </c>
+      <c r="I23" s="6">
+        <f t="shared" si="1"/>
+        <v>0.84307438824491177</v>
+      </c>
+      <c r="J23" s="6">
+        <f t="shared" si="2"/>
+        <v>4.4622244677642265E-3</v>
+      </c>
+      <c r="K23" s="6">
+        <f t="shared" si="3"/>
+        <v>2.6098612201719538E-3</v>
+      </c>
+      <c r="L23" s="6">
+        <f t="shared" si="4"/>
+        <v>2.0262177669535253E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="6">
+        <v>106382030.59999999</v>
+      </c>
+      <c r="C24" s="6">
+        <v>405252.46255200001</v>
+      </c>
+      <c r="D24" s="6">
+        <v>110517831.8</v>
+      </c>
+      <c r="E24" s="6">
+        <v>149226.160221</v>
+      </c>
+      <c r="F24" s="6">
+        <v>102124974.59999999</v>
+      </c>
+      <c r="G24" s="6">
+        <v>342877.11550199997</v>
+      </c>
+      <c r="H24" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0388768777647304</v>
+      </c>
+      <c r="I24" s="6">
+        <f t="shared" si="1"/>
+        <v>0.95998331695691475</v>
+      </c>
+      <c r="J24" s="6">
+        <f t="shared" si="2"/>
+        <v>3.8094070987962515E-3</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" si="3"/>
+        <v>1.4027384077870762E-3</v>
+      </c>
+      <c r="L24" s="6">
+        <f t="shared" si="4"/>
+        <v>3.2230736109111267E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="6">
+        <v>681044917</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1831684.5776899999</v>
+      </c>
+      <c r="D25" s="6">
+        <v>730846103.60000002</v>
+      </c>
+      <c r="E25" s="6">
+        <v>292445.63308499998</v>
+      </c>
+      <c r="F25" s="6">
+        <v>701091829.39999998</v>
+      </c>
+      <c r="G25" s="6">
+        <v>986734.37677099998</v>
+      </c>
+      <c r="H25" s="6">
+        <f t="shared" si="0"/>
+        <v>1.073124672627136</v>
+      </c>
+      <c r="I25" s="6">
+        <f t="shared" si="1"/>
+        <v>1.0294355216515036</v>
+      </c>
+      <c r="J25" s="6">
+        <f t="shared" si="2"/>
+        <v>2.6895209581161883E-3</v>
+      </c>
+      <c r="K25" s="6">
+        <f t="shared" si="3"/>
+        <v>4.2940726196624707E-4</v>
+      </c>
+      <c r="L25" s="6">
+        <f t="shared" si="4"/>
+        <v>1.4488535956153389E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="6">
+        <v>1052021345.6</v>
+      </c>
+      <c r="C26" s="6">
+        <v>2691768.0032799998</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1107875374.4000001</v>
+      </c>
+      <c r="E26" s="6">
+        <v>1804958.78773</v>
+      </c>
+      <c r="F26" s="6">
+        <v>1023622309.4</v>
+      </c>
+      <c r="G26" s="6">
+        <v>1008649.9608999999</v>
+      </c>
+      <c r="H26" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0530921060048879</v>
+      </c>
+      <c r="I26" s="6">
+        <f t="shared" si="1"/>
+        <v>0.97300526617755723</v>
+      </c>
+      <c r="J26" s="6">
+        <f t="shared" si="2"/>
+        <v>2.5586629154799156E-3</v>
+      </c>
+      <c r="K26" s="6">
+        <f t="shared" si="3"/>
+        <v>1.7157054800067547E-3</v>
+      </c>
+      <c r="L26" s="6">
+        <f t="shared" si="4"/>
+        <v>9.5877328451423769E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="6">
+        <v>1374861547.8</v>
+      </c>
+      <c r="C27" s="6">
+        <v>2302629.2171299998</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1424919565.2</v>
+      </c>
+      <c r="E27" s="6">
+        <v>4422678.1181399999</v>
+      </c>
+      <c r="F27" s="6">
+        <v>1273182891.2</v>
+      </c>
+      <c r="G27" s="6">
+        <v>1206884.79522</v>
+      </c>
+      <c r="H27" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0364094969999713</v>
+      </c>
+      <c r="I27" s="6">
+        <f t="shared" si="1"/>
+        <v>0.92604443933812675</v>
+      </c>
+      <c r="J27" s="6">
+        <f t="shared" si="2"/>
+        <v>1.6748080712669414E-3</v>
+      </c>
+      <c r="K27" s="6">
+        <f t="shared" si="3"/>
+        <v>3.2168170862127881E-3</v>
+      </c>
+      <c r="L27" s="6">
+        <f t="shared" si="4"/>
+        <v>8.7782278670256659E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="6">
+        <v>2425734372.4000001</v>
+      </c>
+      <c r="C28" s="6">
+        <v>4744448.9778300002</v>
+      </c>
+      <c r="D28" s="6">
+        <v>2531609439.5999999</v>
+      </c>
+      <c r="E28" s="6">
+        <v>6114149.9741200004</v>
+      </c>
+      <c r="F28" s="6">
+        <v>2295709162.4000001</v>
+      </c>
+      <c r="G28" s="6">
+        <v>1941376.0869499999</v>
+      </c>
+      <c r="H28" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0436466038510424</v>
+      </c>
+      <c r="I28" s="6">
+        <f t="shared" si="1"/>
+        <v>0.94639758933235785</v>
+      </c>
+      <c r="J28" s="6">
+        <f t="shared" si="2"/>
+        <v>1.9558814979135099E-3</v>
+      </c>
+      <c r="K28" s="6">
+        <f t="shared" si="3"/>
+        <v>2.5205356545575574E-3</v>
+      </c>
+      <c r="L28" s="6">
+        <f t="shared" si="4"/>
+        <v>8.0032509290339966E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="6">
+        <v>823052495.20000005</v>
+      </c>
+      <c r="C29" s="6">
+        <v>1504197.41916</v>
+      </c>
+      <c r="D29" s="6">
+        <v>741578725.60000002</v>
+      </c>
+      <c r="E29" s="6">
+        <v>1782951.4190400001</v>
+      </c>
+      <c r="F29" s="6">
+        <v>754718422.60000002</v>
+      </c>
+      <c r="G29" s="6">
+        <v>1129625.15515</v>
+      </c>
+      <c r="H29" s="6">
+        <f t="shared" si="0"/>
+        <v>0.90101023923121448</v>
+      </c>
+      <c r="I29" s="6">
+        <f t="shared" si="1"/>
+        <v>0.91697483089047072</v>
+      </c>
+      <c r="J29" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8275838150450942E-3</v>
+      </c>
+      <c r="K29" s="6">
+        <f t="shared" si="3"/>
+        <v>2.1662669506964396E-3</v>
+      </c>
+      <c r="L29" s="6">
+        <f t="shared" si="4"/>
+        <v>1.3724825108215042E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="6">
+        <v>22418823.800000001</v>
+      </c>
+      <c r="C30" s="6">
+        <v>96830.0391065</v>
+      </c>
+      <c r="D30" s="6">
+        <v>19659639</v>
+      </c>
+      <c r="E30" s="6">
+        <v>73035.239291699996</v>
+      </c>
+      <c r="F30" s="6">
+        <v>17989552.600000001</v>
+      </c>
+      <c r="G30" s="6">
+        <v>92907.484281099998</v>
+      </c>
+      <c r="H30" s="6">
+        <f t="shared" si="0"/>
+        <v>0.87692553255180139</v>
+      </c>
+      <c r="I30" s="6">
+        <f t="shared" si="1"/>
+        <v>0.80243070557519613</v>
+      </c>
+      <c r="J30" s="6">
+        <f t="shared" si="2"/>
+        <v>4.3191400213645464E-3</v>
+      </c>
+      <c r="K30" s="6">
+        <f t="shared" si="3"/>
+        <v>3.2577640978515561E-3</v>
+      </c>
+      <c r="L30" s="6">
+        <f t="shared" si="4"/>
+        <v>4.1441729998832498E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="6">
+        <v>126615263113</v>
+      </c>
+      <c r="C31" s="6">
+        <v>80667418.787400007</v>
+      </c>
+      <c r="D31" s="6">
+        <v>122487126746</v>
+      </c>
+      <c r="E31" s="6">
+        <v>269928060.46899998</v>
+      </c>
+      <c r="F31" s="6">
+        <v>105825598454</v>
+      </c>
+      <c r="G31" s="6">
+        <v>127948118.845</v>
+      </c>
+      <c r="H31" s="6">
+        <f t="shared" si="0"/>
+        <v>0.96739621854818736</v>
+      </c>
+      <c r="I31" s="6">
+        <f t="shared" si="1"/>
+        <v>0.83580443504314406</v>
+      </c>
+      <c r="J31" s="6">
+        <f t="shared" si="2"/>
+        <v>6.3710659208129558E-4</v>
+      </c>
+      <c r="K31" s="6">
+        <f t="shared" si="3"/>
+        <v>2.1318761564164501E-3</v>
+      </c>
+      <c r="L31" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0105268172195833E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="6">
+        <v>10058070079</v>
+      </c>
+      <c r="C32" s="6">
+        <v>9774353.0615599994</v>
+      </c>
+      <c r="D32" s="6">
+        <v>9523389940.6000004</v>
+      </c>
+      <c r="E32" s="6">
+        <v>30559799.585999999</v>
+      </c>
+      <c r="F32" s="6">
+        <v>8212986135.1999998</v>
+      </c>
+      <c r="G32" s="6">
+        <v>15516289.864399999</v>
+      </c>
+      <c r="H32" s="6">
+        <f t="shared" si="0"/>
+        <v>0.94684068273531463</v>
+      </c>
+      <c r="I32" s="6">
+        <f t="shared" si="1"/>
+        <v>0.81655686137519501</v>
+      </c>
+      <c r="J32" s="6">
+        <f t="shared" si="2"/>
+        <v>9.7179210174401487E-4</v>
+      </c>
+      <c r="K32" s="6">
+        <f t="shared" si="3"/>
+        <v>3.0383363156123821E-3</v>
+      </c>
+      <c r="L32" s="6">
+        <f t="shared" si="4"/>
+        <v>1.5426706855817284E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="6">
+        <v>8579486213.6000004</v>
+      </c>
+      <c r="C33" s="6">
+        <v>43101136.4498</v>
+      </c>
+      <c r="D33" s="6">
+        <v>7395381902.8000002</v>
+      </c>
+      <c r="E33" s="6">
+        <v>35551208.384300001</v>
+      </c>
+      <c r="F33" s="6">
+        <v>6774464324.8000002</v>
+      </c>
+      <c r="G33" s="6">
+        <v>35433495.420999996</v>
+      </c>
+      <c r="H33" s="6">
+        <f t="shared" si="0"/>
+        <v>0.86198423992767936</v>
+      </c>
+      <c r="I33" s="6">
+        <f t="shared" si="1"/>
+        <v>0.78961189005249266</v>
+      </c>
+      <c r="J33" s="6">
+        <f t="shared" si="2"/>
+        <v>5.0237433077842224E-3</v>
+      </c>
+      <c r="K33" s="6">
+        <f t="shared" si="3"/>
+        <v>4.1437456159023906E-3</v>
+      </c>
+      <c r="L33" s="6">
+        <f t="shared" si="4"/>
+        <v>4.1300253347142917E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="6">
+        <v>2673114564790</v>
+      </c>
+      <c r="C34" s="6">
+        <v>453874716.78899997</v>
+      </c>
+      <c r="D34" s="6">
+        <v>2514314023640</v>
+      </c>
+      <c r="E34" s="6">
+        <v>313263102.90899998</v>
+      </c>
+      <c r="F34" s="6">
+        <v>2290553200670</v>
+      </c>
+      <c r="G34" s="6">
+        <v>359877898.81999999</v>
+      </c>
+      <c r="H34" s="6">
+        <f t="shared" si="0"/>
+        <v>0.94059343986161126</v>
+      </c>
+      <c r="I34" s="6">
+        <f t="shared" si="1"/>
+        <v>0.85688553376684251</v>
+      </c>
+      <c r="J34" s="6">
+        <f t="shared" si="2"/>
+        <v>1.6979246709714307E-4</v>
+      </c>
+      <c r="K34" s="6">
+        <f t="shared" si="3"/>
+        <v>1.1719030191794639E-4</v>
+      </c>
+      <c r="L34" s="6">
+        <f t="shared" si="4"/>
+        <v>1.3462868504039295E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="6">
+        <v>52898514759.199997</v>
+      </c>
+      <c r="C35" s="6">
+        <v>6143403.5256000003</v>
+      </c>
+      <c r="D35" s="6">
+        <v>55452465741.400002</v>
+      </c>
+      <c r="E35" s="6">
+        <v>12948877.342700001</v>
+      </c>
+      <c r="F35" s="6">
+        <v>50954489972.400002</v>
+      </c>
+      <c r="G35" s="6">
+        <v>6142005.3834199999</v>
+      </c>
+      <c r="H35" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0482802020779955</v>
+      </c>
+      <c r="I35" s="6">
+        <f t="shared" si="1"/>
+        <v>0.96324991740033883</v>
+      </c>
+      <c r="J35" s="6">
+        <f t="shared" si="2"/>
+        <v>1.1613565245764395E-4</v>
+      </c>
+      <c r="K35" s="6">
+        <f t="shared" si="3"/>
+        <v>2.4478716277091616E-4</v>
+      </c>
+      <c r="L35" s="6">
+        <f t="shared" si="4"/>
+        <v>1.1610922180668211E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="6">
+        <v>34314443757</v>
+      </c>
+      <c r="C36" s="6">
+        <v>4223643.4217600003</v>
+      </c>
+      <c r="D36" s="6">
+        <v>35965253851.400002</v>
+      </c>
+      <c r="E36" s="6">
+        <v>8417536.2666699998</v>
+      </c>
+      <c r="F36" s="6">
+        <v>33059567734.799999</v>
+      </c>
+      <c r="G36" s="6">
+        <v>3783579.49486</v>
+      </c>
+      <c r="H36" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0481083157311342</v>
+      </c>
+      <c r="I36" s="6">
+        <f t="shared" si="1"/>
+        <v>0.96343009284700964</v>
+      </c>
+      <c r="J36" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2308646037423803E-4</v>
+      </c>
+      <c r="K36" s="6">
+        <f t="shared" si="3"/>
+        <v>2.4530592208573564E-4</v>
+      </c>
+      <c r="L36" s="6">
+        <f t="shared" si="4"/>
+        <v>1.1026200866473803E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="6">
+        <v>8957.6</v>
+      </c>
+      <c r="C37" s="6">
+        <v>69.887337908999996</v>
+      </c>
+      <c r="D37" s="6">
+        <v>7938.6</v>
+      </c>
+      <c r="E37" s="6">
+        <v>62.755398174200003</v>
+      </c>
+      <c r="F37" s="6">
+        <v>7214.6</v>
+      </c>
+      <c r="G37" s="6">
+        <v>49.317745285000001</v>
+      </c>
+      <c r="H37" s="6">
+        <f t="shared" si="0"/>
+        <v>0.8862418504956685</v>
+      </c>
+      <c r="I37" s="6">
+        <f t="shared" si="1"/>
+        <v>0.80541662945431813</v>
+      </c>
+      <c r="J37" s="6">
+        <f t="shared" si="2"/>
+        <v>7.8020159316111448E-3</v>
+      </c>
+      <c r="K37" s="6">
+        <f t="shared" si="3"/>
+        <v>7.0058272499553455E-3</v>
+      </c>
+      <c r="L37" s="6">
+        <f t="shared" si="4"/>
+        <v>5.5056873811065461E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="J3:L3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27:I37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3765,29 +6796,29 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="9" t="s">
+      <c r="E3" s="11"/>
+      <c r="F3" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="10" t="s">
+      <c r="G3" s="11"/>
+      <c r="H3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -3814,10 +6845,10 @@
       <c r="J4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3837,29 +6868,29 @@
       <c r="E5" s="4">
         <v>63374.740610399997</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>10682599.800000001</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>4082.0953149100001</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <f>D5/B5</f>
         <v>1.044860825822953</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="10">
         <f>F5/B5</f>
         <v>0.97071676783895877</v>
       </c>
-      <c r="J5" s="11">
-        <f>C5/B5</f>
+      <c r="J5" s="10">
+        <f t="shared" ref="J5:J37" si="0">C5/B5</f>
         <v>3.9063064824936943E-3</v>
       </c>
-      <c r="K5" s="11">
-        <f>E5/B5</f>
+      <c r="K5" s="10">
+        <f t="shared" ref="K5:K37" si="1">E5/B5</f>
         <v>5.7587969707486265E-3</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="10">
         <f>G5/B5</f>
         <v>3.7093576884720435E-4</v>
       </c>
@@ -3880,30 +6911,30 @@
       <c r="E6" s="4">
         <v>1644622126.3299999</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>283268225665</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>240501278.76800001</v>
       </c>
-      <c r="H6" s="11">
-        <f t="shared" ref="H6:H37" si="0">D6/B6</f>
+      <c r="H6" s="10">
+        <f t="shared" ref="H6:H37" si="2">D6/B6</f>
         <v>0.81051092943930281</v>
       </c>
-      <c r="I6" s="11">
-        <f t="shared" ref="I6:I37" si="1">F6/B6</f>
+      <c r="I6" s="10">
+        <f t="shared" ref="I6:I37" si="3">F6/B6</f>
         <v>0.75585517766201682</v>
       </c>
-      <c r="J6" s="11">
-        <f>C6/B6</f>
+      <c r="J6" s="10">
+        <f t="shared" si="0"/>
         <v>3.9437970145817305E-3</v>
       </c>
-      <c r="K6" s="11">
-        <f>E6/B6</f>
+      <c r="K6" s="10">
+        <f t="shared" si="1"/>
         <v>4.3884065943709553E-3</v>
       </c>
-      <c r="L6" s="11">
-        <f t="shared" ref="L6:L37" si="2">G6/B6</f>
+      <c r="L6" s="10">
+        <f t="shared" ref="L6:L37" si="4">G6/B6</f>
         <v>6.4173853726224586E-4</v>
       </c>
     </row>
@@ -3923,30 +6954,30 @@
       <c r="E7" s="4">
         <v>1922594830.6800001</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>311181991364</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>34689920.276299998</v>
       </c>
-      <c r="H7" s="11">
-        <f t="shared" si="0"/>
+      <c r="H7" s="9">
+        <f t="shared" si="2"/>
         <v>0.84752664870192518</v>
       </c>
-      <c r="I7" s="11">
-        <f t="shared" si="1"/>
+      <c r="I7" s="9">
+        <f t="shared" si="3"/>
         <v>0.7754929742072495</v>
       </c>
-      <c r="J7" s="11">
-        <f>C7/B7</f>
+      <c r="J7" s="10">
+        <f t="shared" si="0"/>
         <v>4.604518976025926E-3</v>
       </c>
-      <c r="K7" s="11">
-        <f>E7/B7</f>
+      <c r="K7" s="10">
+        <f t="shared" si="1"/>
         <v>4.7912759247545657E-3</v>
       </c>
-      <c r="L7" s="11">
-        <f t="shared" si="2"/>
+      <c r="L7" s="10">
+        <f t="shared" si="4"/>
         <v>8.645034159001936E-5</v>
       </c>
     </row>
@@ -3966,30 +6997,30 @@
       <c r="E8" s="4">
         <v>432735.30819299998</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>18320543.800000001</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>38405.694501700003</v>
       </c>
-      <c r="H8" s="11">
-        <f t="shared" si="0"/>
+      <c r="H8" s="10">
+        <f t="shared" si="2"/>
         <v>0.58371974617037303</v>
       </c>
-      <c r="I8" s="11">
-        <f t="shared" si="1"/>
+      <c r="I8" s="10">
+        <f t="shared" si="3"/>
         <v>0.13658006997281327</v>
       </c>
-      <c r="J8" s="11">
-        <f>C8/B8</f>
+      <c r="J8" s="10">
+        <f t="shared" si="0"/>
         <v>4.4096319903338052E-3</v>
       </c>
-      <c r="K8" s="11">
-        <f>E8/B8</f>
+      <c r="K8" s="10">
+        <f t="shared" si="1"/>
         <v>3.226051547263944E-3</v>
       </c>
-      <c r="L8" s="11">
-        <f t="shared" si="2"/>
+      <c r="L8" s="10">
+        <f t="shared" si="4"/>
         <v>2.8631532446087525E-4</v>
       </c>
     </row>
@@ -3997,42 +7028,42 @@
       <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>99303188.799999997</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>392074.22467999998</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>57364564.600000001</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>220994.854758</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>9113275.1999999993</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>12871.3087664</v>
       </c>
-      <c r="H9" s="11">
-        <f t="shared" si="0"/>
+      <c r="H9" s="10">
+        <f t="shared" si="2"/>
         <v>0.57767092168141942</v>
       </c>
-      <c r="I9" s="11">
-        <f t="shared" si="1"/>
+      <c r="I9" s="10">
+        <f t="shared" si="3"/>
         <v>9.1772231185389685E-2</v>
       </c>
-      <c r="J9" s="11">
-        <f>C9/B9</f>
+      <c r="J9" s="10">
+        <f t="shared" si="0"/>
         <v>3.948254123738673E-3</v>
       </c>
-      <c r="K9" s="11">
-        <f>E9/B9</f>
+      <c r="K9" s="10">
+        <f t="shared" si="1"/>
         <v>2.2254557726549061E-3</v>
       </c>
-      <c r="L9" s="11">
-        <f t="shared" si="2"/>
+      <c r="L9" s="10">
+        <f t="shared" si="4"/>
         <v>1.2961626833880686E-4</v>
       </c>
     </row>
@@ -4052,73 +7083,73 @@
       <c r="E10" s="4">
         <v>13604835.5052</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>596797669.20000005</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>7630087.2776699997</v>
       </c>
-      <c r="H10" s="11">
-        <f t="shared" si="0"/>
+      <c r="H10" s="10">
+        <f t="shared" si="2"/>
         <v>0.5147302982359836</v>
       </c>
-      <c r="I10" s="11">
-        <f t="shared" si="1"/>
+      <c r="I10" s="10">
+        <f t="shared" si="3"/>
         <v>0.1158110895559324</v>
       </c>
-      <c r="J10" s="11">
-        <f>C10/B10</f>
+      <c r="J10" s="10">
+        <f t="shared" si="0"/>
         <v>3.3968885657673907E-3</v>
       </c>
-      <c r="K10" s="11">
-        <f>E10/B10</f>
+      <c r="K10" s="10">
+        <f t="shared" si="1"/>
         <v>2.6400753628922618E-3</v>
       </c>
-      <c r="L10" s="11">
-        <f t="shared" si="2"/>
+      <c r="L10" s="10">
+        <f t="shared" si="4"/>
         <v>1.4806504224762491E-3</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>52956603.200000003</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>36629.741328099997</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>57931055.600000001</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>165906.74316300001</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>22465027</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>12980.253464400001</v>
       </c>
-      <c r="H11" s="11">
-        <f t="shared" si="0"/>
+      <c r="H11" s="10">
+        <f t="shared" si="2"/>
         <v>1.0939345067358852</v>
       </c>
-      <c r="I11" s="11">
-        <f t="shared" si="1"/>
+      <c r="I11" s="10">
+        <f t="shared" si="3"/>
         <v>0.42421578504869056</v>
       </c>
-      <c r="J11" s="11">
-        <f>C11/B11</f>
+      <c r="J11" s="10">
+        <f t="shared" si="0"/>
         <v>6.9169355877606584E-4</v>
       </c>
-      <c r="K11" s="11">
-        <f>E11/B11</f>
+      <c r="K11" s="10">
+        <f t="shared" si="1"/>
         <v>3.1328811354539446E-3</v>
       </c>
-      <c r="L11" s="11">
-        <f t="shared" si="2"/>
+      <c r="L11" s="10">
+        <f t="shared" si="4"/>
         <v>2.4511114157714709E-4</v>
       </c>
     </row>
@@ -4138,30 +7169,30 @@
       <c r="E12" s="4">
         <v>170033.10279100001</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>47613462.600000001</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <v>65408.676163299999</v>
       </c>
-      <c r="H12" s="11">
-        <f t="shared" si="0"/>
+      <c r="H12" s="10">
+        <f t="shared" si="2"/>
         <v>0.75892706964205792</v>
       </c>
-      <c r="I12" s="11">
-        <f t="shared" si="1"/>
+      <c r="I12" s="10">
+        <f t="shared" si="3"/>
         <v>0.49256948058846534</v>
       </c>
-      <c r="J12" s="11">
-        <f>C12/B12</f>
+      <c r="J12" s="10">
+        <f t="shared" si="0"/>
         <v>1.6895812240578505E-3</v>
       </c>
-      <c r="K12" s="11">
-        <f>E12/B12</f>
+      <c r="K12" s="10">
+        <f t="shared" si="1"/>
         <v>1.7590217671883417E-3</v>
       </c>
-      <c r="L12" s="11">
-        <f t="shared" si="2"/>
+      <c r="L12" s="10">
+        <f t="shared" si="4"/>
         <v>6.7666403333026682E-4</v>
       </c>
     </row>
@@ -4169,42 +7200,42 @@
       <c r="A13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>52189010.600000001</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>184496.05991800001</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>37061534</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>184451.52224399999</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>14069332</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <v>23007.3089865</v>
       </c>
-      <c r="H13" s="11">
-        <f t="shared" si="0"/>
+      <c r="H13" s="10">
+        <f t="shared" si="2"/>
         <v>0.71014057507348105</v>
       </c>
-      <c r="I13" s="11">
-        <f t="shared" si="1"/>
+      <c r="I13" s="10">
+        <f t="shared" si="3"/>
         <v>0.26958418713536597</v>
       </c>
-      <c r="J13" s="11">
-        <f>C13/B13</f>
+      <c r="J13" s="10">
+        <f t="shared" si="0"/>
         <v>3.5351515155568019E-3</v>
       </c>
-      <c r="K13" s="11">
-        <f>E13/B13</f>
+      <c r="K13" s="10">
+        <f t="shared" si="1"/>
         <v>3.5342981237509795E-3</v>
       </c>
-      <c r="L13" s="11">
-        <f t="shared" si="2"/>
+      <c r="L13" s="10">
+        <f t="shared" si="4"/>
         <v>4.4084585474973538E-4</v>
       </c>
     </row>
@@ -4224,73 +7255,73 @@
       <c r="E14" s="4">
         <v>9860683.1170700006</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <v>1117094704.2</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="6">
         <v>2439070.8690800001</v>
       </c>
-      <c r="H14" s="11">
-        <f t="shared" si="0"/>
+      <c r="H14" s="10">
+        <f t="shared" si="2"/>
         <v>0.68315662967554103</v>
       </c>
-      <c r="I14" s="11">
-        <f t="shared" si="1"/>
+      <c r="I14" s="10">
+        <f t="shared" si="3"/>
         <v>0.35651564854941975</v>
       </c>
-      <c r="J14" s="11">
-        <f>C14/B14</f>
+      <c r="J14" s="10">
+        <f t="shared" si="0"/>
         <v>6.2110148138080972E-3</v>
       </c>
-      <c r="K14" s="11">
-        <f>E14/B14</f>
+      <c r="K14" s="10">
+        <f t="shared" si="1"/>
         <v>3.146991766593432E-3</v>
       </c>
-      <c r="L14" s="11">
-        <f t="shared" si="2"/>
+      <c r="L14" s="10">
+        <f t="shared" si="4"/>
         <v>7.784182750832999E-4</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>1888639030.5999999</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>330987876.43599999</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>1417034052.8</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>52230323.976099998</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>735183338.79999995</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <v>15665738.5373</v>
       </c>
-      <c r="H15" s="11">
-        <f t="shared" si="0"/>
+      <c r="H15" s="10">
+        <f t="shared" si="2"/>
         <v>0.75029374583549924</v>
       </c>
-      <c r="I15" s="11">
-        <f t="shared" si="1"/>
+      <c r="I15" s="10">
+        <f t="shared" si="3"/>
         <v>0.38926620009883006</v>
       </c>
-      <c r="J15" s="11">
-        <f>C15/B15</f>
+      <c r="J15" s="10">
+        <f t="shared" si="0"/>
         <v>0.17525205773749616</v>
       </c>
-      <c r="K15" s="11">
-        <f>E15/B15</f>
+      <c r="K15" s="10">
+        <f t="shared" si="1"/>
         <v>2.7655006133970976E-2</v>
       </c>
-      <c r="L15" s="11">
-        <f t="shared" si="2"/>
+      <c r="L15" s="10">
+        <f t="shared" si="4"/>
         <v>8.2947234932040804E-3</v>
       </c>
     </row>
@@ -4310,30 +7341,30 @@
       <c r="E16" s="4">
         <v>86536.287661499999</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>52971565.799999997</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <v>57292.834345700001</v>
       </c>
-      <c r="H16" s="11">
-        <f t="shared" si="0"/>
+      <c r="H16" s="10">
+        <f t="shared" si="2"/>
         <v>1.048633231178383</v>
       </c>
-      <c r="I16" s="11">
-        <f t="shared" si="1"/>
+      <c r="I16" s="10">
+        <f t="shared" si="3"/>
         <v>0.94317141591576958</v>
       </c>
-      <c r="J16" s="11">
-        <f>C16/B16</f>
+      <c r="J16" s="10">
+        <f t="shared" si="0"/>
         <v>1.5940226211917812E-3</v>
       </c>
-      <c r="K16" s="11">
-        <f>E16/B16</f>
+      <c r="K16" s="10">
+        <f t="shared" si="1"/>
         <v>1.540799327509992E-3</v>
       </c>
-      <c r="L16" s="11">
-        <f t="shared" si="2"/>
+      <c r="L16" s="10">
+        <f t="shared" si="4"/>
         <v>1.0201126373285629E-3</v>
       </c>
     </row>
@@ -4341,42 +7372,42 @@
       <c r="A17" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>42798674.399999999</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>169110.16664700001</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>45041719.399999999</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>164677.76881099999</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>39117214.600000001</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <v>9703.0218303399997</v>
       </c>
-      <c r="H17" s="11">
-        <f t="shared" si="0"/>
+      <c r="H17" s="10">
+        <f t="shared" si="2"/>
         <v>1.0524092166742436</v>
       </c>
-      <c r="I17" s="11">
-        <f t="shared" si="1"/>
+      <c r="I17" s="10">
+        <f t="shared" si="3"/>
         <v>0.91398191996339029</v>
       </c>
-      <c r="J17" s="11">
-        <f>C17/B17</f>
+      <c r="J17" s="10">
+        <f t="shared" si="0"/>
         <v>3.9512944972660185E-3</v>
       </c>
-      <c r="K17" s="11">
-        <f>E17/B17</f>
+      <c r="K17" s="10">
+        <f t="shared" si="1"/>
         <v>3.84773059258583E-3</v>
       </c>
-      <c r="L17" s="11">
-        <f t="shared" si="2"/>
+      <c r="L17" s="10">
+        <f t="shared" si="4"/>
         <v>2.2671313928218301E-4</v>
       </c>
     </row>
@@ -4396,73 +7427,73 @@
       <c r="E18" s="4">
         <v>4191937.8707599998</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <v>1625018710.8</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <v>3109857.0395399998</v>
       </c>
-      <c r="H18" s="11">
-        <f t="shared" si="0"/>
+      <c r="H18" s="10">
+        <f t="shared" si="2"/>
         <v>1.00020002606237</v>
       </c>
-      <c r="I18" s="11">
-        <f t="shared" si="1"/>
+      <c r="I18" s="10">
+        <f t="shared" si="3"/>
         <v>0.89695254331052376</v>
       </c>
-      <c r="J18" s="11">
-        <f>C18/B18</f>
+      <c r="J18" s="10">
+        <f t="shared" si="0"/>
         <v>6.178671081599578E-3</v>
       </c>
-      <c r="K18" s="11">
-        <f>E18/B18</f>
+      <c r="K18" s="10">
+        <f t="shared" si="1"/>
         <v>2.3138006409334469E-3</v>
       </c>
-      <c r="L18" s="11">
-        <f t="shared" si="2"/>
+      <c r="L18" s="10">
+        <f t="shared" si="4"/>
         <v>1.7165305004853233E-3</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>374259407.80000001</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>36671339.376199998</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>319451064.80000001</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>11498265.4856</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>195747522</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <v>1477896.6923199999</v>
       </c>
-      <c r="H19" s="11">
-        <f t="shared" si="0"/>
+      <c r="H19" s="10">
+        <f t="shared" si="2"/>
         <v>0.85355520300163312</v>
       </c>
-      <c r="I19" s="11">
-        <f t="shared" si="1"/>
+      <c r="I19" s="10">
+        <f t="shared" si="3"/>
         <v>0.52302632324103193</v>
       </c>
-      <c r="J19" s="11">
-        <f>C19/B19</f>
+      <c r="J19" s="10">
+        <f t="shared" si="0"/>
         <v>9.7983747667865564E-2</v>
       </c>
-      <c r="K19" s="11">
-        <f>E19/B19</f>
+      <c r="K19" s="10">
+        <f t="shared" si="1"/>
         <v>3.0722715971764011E-2</v>
       </c>
-      <c r="L19" s="11">
-        <f t="shared" si="2"/>
+      <c r="L19" s="10">
+        <f t="shared" si="4"/>
         <v>3.9488564923657746E-3</v>
       </c>
     </row>
@@ -4470,42 +7501,42 @@
       <c r="A20" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>28546124.600000001</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <v>116019.715939</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
         <v>27901238</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>128736.181753</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>7589116.7999999998</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="6">
         <v>72091.823232299997</v>
       </c>
-      <c r="H20" s="11">
-        <f t="shared" si="0"/>
+      <c r="H20" s="10">
+        <f t="shared" si="2"/>
         <v>0.9774089614952497</v>
       </c>
-      <c r="I20" s="11">
-        <f t="shared" si="1"/>
+      <c r="I20" s="10">
+        <f t="shared" si="3"/>
         <v>0.26585453914819662</v>
       </c>
-      <c r="J20" s="11">
-        <f>C20/B20</f>
+      <c r="J20" s="10">
+        <f t="shared" si="0"/>
         <v>4.0642895511988344E-3</v>
       </c>
-      <c r="K20" s="11">
-        <f>E20/B20</f>
+      <c r="K20" s="10">
+        <f t="shared" si="1"/>
         <v>4.5097603810290935E-3</v>
       </c>
-      <c r="L20" s="11">
-        <f t="shared" si="2"/>
+      <c r="L20" s="10">
+        <f t="shared" si="4"/>
         <v>2.5254504505420675E-3</v>
       </c>
     </row>
@@ -4513,42 +7544,42 @@
       <c r="A21" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>10800565.199999999</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>181427.34367599999</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>11061967.199999999</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>18989.8155167</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>9003693.5999999996</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="6">
         <v>6686.3842725300001</v>
       </c>
-      <c r="H21" s="11">
-        <f t="shared" si="0"/>
+      <c r="H21" s="10">
+        <f t="shared" si="2"/>
         <v>1.0242026222849894</v>
       </c>
-      <c r="I21" s="11">
-        <f t="shared" si="1"/>
+      <c r="I21" s="10">
+        <f t="shared" si="3"/>
         <v>0.83363170660735419</v>
       </c>
-      <c r="J21" s="11">
-        <f>C21/B21</f>
+      <c r="J21" s="10">
+        <f t="shared" si="0"/>
         <v>1.679794902548248E-2</v>
       </c>
-      <c r="K21" s="11">
-        <f>E21/B21</f>
+      <c r="K21" s="10">
+        <f t="shared" si="1"/>
         <v>1.7582242378111844E-3</v>
       </c>
-      <c r="L21" s="11">
-        <f t="shared" si="2"/>
+      <c r="L21" s="10">
+        <f t="shared" si="4"/>
         <v>6.1907725648746614E-4</v>
       </c>
     </row>
@@ -4568,30 +7599,30 @@
       <c r="E22" s="4">
         <v>174702521.64199999</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="6">
         <v>58861111648.400002</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="6">
         <v>66290083.325000003</v>
       </c>
-      <c r="H22" s="11">
-        <f t="shared" si="0"/>
+      <c r="H22" s="10">
+        <f t="shared" si="2"/>
         <v>1.0353754379822957</v>
       </c>
-      <c r="I22" s="11">
-        <f t="shared" si="1"/>
+      <c r="I22" s="10">
+        <f t="shared" si="3"/>
         <v>1.3988086018870911</v>
       </c>
-      <c r="J22" s="11">
-        <f>C22/B22</f>
+      <c r="J22" s="10">
+        <f t="shared" si="0"/>
         <v>4.7587655326600609E-3</v>
       </c>
-      <c r="K22" s="11">
-        <f>E22/B22</f>
+      <c r="K22" s="10">
+        <f t="shared" si="1"/>
         <v>4.1517290992386154E-3</v>
       </c>
-      <c r="L22" s="11">
-        <f t="shared" si="2"/>
+      <c r="L22" s="10">
+        <f t="shared" si="4"/>
         <v>1.5753548680615616E-3</v>
       </c>
     </row>
@@ -4611,30 +7642,30 @@
       <c r="E23" s="4">
         <v>950876.60208999994</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <v>623199667.60000002</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="6">
         <v>630923.81415300001</v>
       </c>
-      <c r="H23" s="11">
-        <f t="shared" si="0"/>
+      <c r="H23" s="10">
+        <f t="shared" si="2"/>
         <v>1.0034742853505272</v>
       </c>
-      <c r="I23" s="11">
-        <f t="shared" si="1"/>
+      <c r="I23" s="10">
+        <f t="shared" si="3"/>
         <v>1.3023778465028963</v>
       </c>
-      <c r="J23" s="11">
-        <f>C23/B23</f>
+      <c r="J23" s="10">
+        <f t="shared" si="0"/>
         <v>5.2417397361807314E-3</v>
       </c>
-      <c r="K23" s="11">
-        <f>E23/B23</f>
+      <c r="K23" s="10">
+        <f t="shared" si="1"/>
         <v>1.9871650864146991E-3</v>
       </c>
-      <c r="L23" s="11">
-        <f t="shared" si="2"/>
+      <c r="L23" s="10">
+        <f t="shared" si="4"/>
         <v>1.3185199561296713E-3</v>
       </c>
     </row>
@@ -4654,30 +7685,30 @@
       <c r="E24" s="4">
         <v>904688.83650099998</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <v>743078715.20000005</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="6">
         <v>636582.43804000004</v>
       </c>
-      <c r="H24" s="11">
-        <f t="shared" si="0"/>
+      <c r="H24" s="10">
+        <f t="shared" si="2"/>
         <v>0.98038007108801128</v>
       </c>
-      <c r="I24" s="11">
-        <f t="shared" si="1"/>
+      <c r="I24" s="10">
+        <f t="shared" si="3"/>
         <v>0.91394284574907902</v>
       </c>
-      <c r="J24" s="11">
-        <f>C24/B24</f>
+      <c r="J24" s="10">
+        <f t="shared" si="0"/>
         <v>7.7284880920492282E-4</v>
       </c>
-      <c r="K24" s="11">
-        <f>E24/B24</f>
+      <c r="K24" s="10">
+        <f t="shared" si="1"/>
         <v>1.1127137311780009E-3</v>
       </c>
-      <c r="L24" s="11">
-        <f t="shared" si="2"/>
+      <c r="L24" s="10">
+        <f t="shared" si="4"/>
         <v>7.8295872708394377E-4</v>
       </c>
     </row>
@@ -4697,30 +7728,30 @@
       <c r="E25" s="4">
         <v>1618224.4899599999</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="6">
         <v>1271852242.8</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="6">
         <v>3537843.5832600002</v>
       </c>
-      <c r="H25" s="11">
-        <f t="shared" si="0"/>
+      <c r="H25" s="10">
+        <f t="shared" si="2"/>
         <v>1.0703808611643688</v>
       </c>
-      <c r="I25" s="11">
-        <f t="shared" si="1"/>
+      <c r="I25" s="10">
+        <f t="shared" si="3"/>
         <v>1.0231784688766865</v>
       </c>
-      <c r="J25" s="11">
-        <f>C25/B25</f>
+      <c r="J25" s="10">
+        <f t="shared" si="0"/>
         <v>2.6873954202269782E-3</v>
       </c>
-      <c r="K25" s="11">
-        <f>E25/B25</f>
+      <c r="K25" s="10">
+        <f t="shared" si="1"/>
         <v>1.3018276810920367E-3</v>
       </c>
-      <c r="L25" s="11">
-        <f t="shared" si="2"/>
+      <c r="L25" s="10">
+        <f t="shared" si="4"/>
         <v>2.8461210027636847E-3</v>
       </c>
     </row>
@@ -4740,30 +7771,30 @@
       <c r="E26" s="4">
         <v>2931767.1285799998</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="6">
         <v>2633088051.4000001</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="6">
         <v>4171767.29519</v>
       </c>
-      <c r="H26" s="11">
-        <f t="shared" si="0"/>
+      <c r="H26" s="10">
+        <f t="shared" si="2"/>
         <v>1.026949414042712</v>
       </c>
-      <c r="I26" s="11">
-        <f t="shared" si="1"/>
+      <c r="I26" s="10">
+        <f t="shared" si="3"/>
         <v>1.0390692275201228</v>
       </c>
-      <c r="J26" s="11">
-        <f>C26/B26</f>
+      <c r="J26" s="10">
+        <f t="shared" si="0"/>
         <v>5.3539846245207097E-4</v>
       </c>
-      <c r="K26" s="11">
-        <f>E26/B26</f>
+      <c r="K26" s="10">
+        <f t="shared" si="1"/>
         <v>1.1569339673023092E-3</v>
       </c>
-      <c r="L26" s="11">
-        <f t="shared" si="2"/>
+      <c r="L26" s="10">
+        <f t="shared" si="4"/>
         <v>1.6462628427872045E-3</v>
       </c>
     </row>
@@ -4783,30 +7814,30 @@
       <c r="E27" s="4">
         <v>6077712.8282199996</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="6">
         <v>2957131855.4000001</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="6">
         <v>5873061.8385899998</v>
       </c>
-      <c r="H27" s="11">
-        <f t="shared" si="0"/>
+      <c r="H27" s="10">
+        <f t="shared" si="2"/>
         <v>0.82702574883545565</v>
       </c>
-      <c r="I27" s="11">
-        <f t="shared" si="1"/>
+      <c r="I27" s="10">
+        <f t="shared" si="3"/>
         <v>0.70788779006245717</v>
       </c>
-      <c r="J27" s="11">
-        <f>C27/B27</f>
+      <c r="J27" s="10">
+        <f t="shared" si="0"/>
         <v>1.0467924332309708E-3</v>
       </c>
-      <c r="K27" s="11">
-        <f>E27/B27</f>
+      <c r="K27" s="10">
+        <f t="shared" si="1"/>
         <v>1.4549025586216007E-3</v>
       </c>
-      <c r="L27" s="11">
-        <f t="shared" si="2"/>
+      <c r="L27" s="10">
+        <f t="shared" si="4"/>
         <v>1.4059125426645073E-3</v>
       </c>
     </row>
@@ -4826,30 +7857,30 @@
       <c r="E28" s="4">
         <v>7828922.0355799999</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="6">
         <v>5589016638.1999998</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="6">
         <v>9536877.7356800009</v>
       </c>
-      <c r="H28" s="11">
-        <f t="shared" si="0"/>
+      <c r="H28" s="10">
+        <f t="shared" si="2"/>
         <v>0.90249864854012052</v>
       </c>
-      <c r="I28" s="11">
-        <f t="shared" si="1"/>
+      <c r="I28" s="10">
+        <f t="shared" si="3"/>
         <v>0.83277289312899994</v>
       </c>
-      <c r="J28" s="11">
-        <f>C28/B28</f>
+      <c r="J28" s="10">
+        <f t="shared" si="0"/>
         <v>5.503195732221186E-4</v>
       </c>
-      <c r="K28" s="11">
-        <f>E28/B28</f>
+      <c r="K28" s="10">
+        <f t="shared" si="1"/>
         <v>1.1665225701942225E-3</v>
       </c>
-      <c r="L28" s="11">
-        <f t="shared" si="2"/>
+      <c r="L28" s="10">
+        <f t="shared" si="4"/>
         <v>1.4210108463584034E-3</v>
       </c>
     </row>
@@ -4869,30 +7900,30 @@
       <c r="E29" s="4">
         <v>7596027.7199299997</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="6">
         <v>2129407451.8</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="6">
         <v>7064432.3703699997</v>
       </c>
-      <c r="H29" s="11">
-        <f t="shared" si="0"/>
+      <c r="H29" s="10">
+        <f t="shared" si="2"/>
         <v>0.82511298144212186</v>
       </c>
-      <c r="I29" s="11">
-        <f t="shared" si="1"/>
+      <c r="I29" s="10">
+        <f t="shared" si="3"/>
         <v>0.82988344054357355</v>
       </c>
-      <c r="J29" s="11">
-        <f>C29/B29</f>
+      <c r="J29" s="10">
+        <f t="shared" si="0"/>
         <v>7.4889909165773922E-3</v>
       </c>
-      <c r="K29" s="11">
-        <f>E29/B29</f>
+      <c r="K29" s="10">
+        <f t="shared" si="1"/>
         <v>2.9603623361753582E-3</v>
       </c>
-      <c r="L29" s="11">
-        <f t="shared" si="2"/>
+      <c r="L29" s="10">
+        <f t="shared" si="4"/>
         <v>2.7531863082635088E-3</v>
       </c>
     </row>
@@ -4912,30 +7943,30 @@
       <c r="E30" s="4">
         <v>628746.94184999994</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="6">
         <v>53724671.200000003</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="6">
         <v>336920.660569</v>
       </c>
-      <c r="H30" s="11">
-        <f t="shared" si="0"/>
+      <c r="H30" s="10">
+        <f t="shared" si="2"/>
         <v>0.85021193492004865</v>
       </c>
-      <c r="I30" s="11">
-        <f t="shared" si="1"/>
+      <c r="I30" s="10">
+        <f t="shared" si="3"/>
         <v>1.1969679721181152</v>
       </c>
-      <c r="J30" s="11">
-        <f>C30/B30</f>
+      <c r="J30" s="10">
+        <f t="shared" si="0"/>
         <v>1.6678227708957955E-2</v>
       </c>
-      <c r="K30" s="11">
-        <f>E30/B30</f>
+      <c r="K30" s="10">
+        <f t="shared" si="1"/>
         <v>1.4008274693017776E-2</v>
       </c>
-      <c r="L30" s="11">
-        <f t="shared" si="2"/>
+      <c r="L30" s="10">
+        <f t="shared" si="4"/>
         <v>7.5064813025039366E-3</v>
       </c>
     </row>
@@ -4955,30 +7986,30 @@
       <c r="E31" s="4">
         <v>1015290207.74</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="6">
         <v>231792565363</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="6">
         <v>387485934.45300001</v>
       </c>
-      <c r="H31" s="11">
-        <f t="shared" si="0"/>
+      <c r="H31" s="10">
+        <f t="shared" si="2"/>
         <v>1.0121933243878463</v>
       </c>
-      <c r="I31" s="11">
-        <f t="shared" si="1"/>
+      <c r="I31" s="10">
+        <f t="shared" si="3"/>
         <v>0.88848470413753311</v>
       </c>
-      <c r="J31" s="11">
-        <f>C31/B31</f>
+      <c r="J31" s="10">
+        <f t="shared" si="0"/>
         <v>6.2644680006298673E-3</v>
       </c>
-      <c r="K31" s="11">
-        <f>E31/B31</f>
+      <c r="K31" s="10">
+        <f t="shared" si="1"/>
         <v>3.8917116190716346E-3</v>
       </c>
-      <c r="L31" s="11">
-        <f t="shared" si="2"/>
+      <c r="L31" s="10">
+        <f t="shared" si="4"/>
         <v>1.485273374884889E-3</v>
       </c>
     </row>
@@ -4998,30 +8029,30 @@
       <c r="E32" s="4">
         <v>95384807.631999999</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="6">
         <v>20365516610</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="6">
         <v>27671094.960200001</v>
       </c>
-      <c r="H32" s="11">
-        <f t="shared" si="0"/>
+      <c r="H32" s="10">
+        <f t="shared" si="2"/>
         <v>0.95092142865231266</v>
       </c>
-      <c r="I32" s="11">
-        <f t="shared" si="1"/>
+      <c r="I32" s="10">
+        <f t="shared" si="3"/>
         <v>0.99681773052303801</v>
       </c>
-      <c r="J32" s="11">
-        <f>C32/B32</f>
+      <c r="J32" s="10">
+        <f t="shared" si="0"/>
         <v>1.0404746419487972E-2</v>
       </c>
-      <c r="K32" s="11">
-        <f>E32/B32</f>
+      <c r="K32" s="10">
+        <f t="shared" si="1"/>
         <v>4.6687383036195318E-3</v>
       </c>
-      <c r="L32" s="11">
-        <f t="shared" si="2"/>
+      <c r="L32" s="10">
+        <f t="shared" si="4"/>
         <v>1.3543991349460808E-3</v>
       </c>
     </row>
@@ -5041,30 +8072,30 @@
       <c r="E33" s="4">
         <v>265266356.43599999</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="6">
         <v>18640519393.200001</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G33" s="6">
         <v>115354906.141</v>
       </c>
-      <c r="H33" s="11">
-        <f t="shared" si="0"/>
+      <c r="H33" s="10">
+        <f t="shared" si="2"/>
         <v>0.90235324573564168</v>
       </c>
-      <c r="I33" s="11">
-        <f t="shared" si="1"/>
+      <c r="I33" s="10">
+        <f t="shared" si="3"/>
         <v>1.0280512498640273</v>
       </c>
-      <c r="J33" s="11">
-        <f>C33/B33</f>
+      <c r="J33" s="10">
+        <f t="shared" si="0"/>
         <v>1.4981741252244824E-2</v>
       </c>
-      <c r="K33" s="11">
-        <f>E33/B33</f>
+      <c r="K33" s="10">
+        <f t="shared" si="1"/>
         <v>1.4629818168070418E-2</v>
       </c>
-      <c r="L33" s="11">
-        <f t="shared" si="2"/>
+      <c r="L33" s="10">
+        <f t="shared" si="4"/>
         <v>6.3619877179744311E-3</v>
       </c>
     </row>
@@ -5084,30 +8115,30 @@
       <c r="E34" s="4">
         <v>2840499643.3800001</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="6">
         <v>3286567960500</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="6">
         <v>817621597.70899999</v>
       </c>
-      <c r="H34" s="11">
-        <f t="shared" si="0"/>
+      <c r="H34" s="10">
+        <f t="shared" si="2"/>
         <v>0.84752333675715374</v>
       </c>
-      <c r="I34" s="11">
-        <f t="shared" si="1"/>
+      <c r="I34" s="10">
+        <f t="shared" si="3"/>
         <v>0.77524471609909174</v>
       </c>
-      <c r="J34" s="11">
-        <f>C34/B34</f>
+      <c r="J34" s="10">
+        <f t="shared" si="0"/>
         <v>5.5720605010201442E-4</v>
       </c>
-      <c r="K34" s="11">
-        <f>E34/B34</f>
+      <c r="K34" s="10">
+        <f t="shared" si="1"/>
         <v>6.7002489103456327E-4</v>
       </c>
-      <c r="L34" s="11">
-        <f t="shared" si="2"/>
+      <c r="L34" s="10">
+        <f t="shared" si="4"/>
         <v>1.9286283777194982E-4</v>
       </c>
     </row>
@@ -5115,42 +8146,42 @@
       <c r="A35" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35" s="6">
         <v>97611105037.600006</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="6">
         <v>1720235606.3699999</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="6">
         <v>76603854319.800003</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="6">
         <v>85021399.524900004</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="6">
         <v>71253446652.800003</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="6">
         <v>21376046.0966</v>
       </c>
-      <c r="H35" s="11">
-        <f t="shared" si="0"/>
+      <c r="H35" s="10">
+        <f t="shared" si="2"/>
         <v>0.78478626269308227</v>
       </c>
-      <c r="I35" s="11">
-        <f t="shared" si="1"/>
+      <c r="I35" s="10">
+        <f t="shared" si="3"/>
         <v>0.72997274874977625</v>
       </c>
-      <c r="J35" s="11">
-        <f>C35/B35</f>
+      <c r="J35" s="10">
+        <f t="shared" si="0"/>
         <v>1.7623359613717738E-2</v>
       </c>
-      <c r="K35" s="11">
-        <f>E35/B35</f>
+      <c r="K35" s="10">
+        <f t="shared" si="1"/>
         <v>8.7102179093402924E-4</v>
       </c>
-      <c r="L35" s="11">
-        <f t="shared" si="2"/>
+      <c r="L35" s="10">
+        <f t="shared" si="4"/>
         <v>2.1899194859402422E-4</v>
       </c>
     </row>
@@ -5158,42 +8189,42 @@
       <c r="A36" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="6">
         <v>57947321369.400002</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="6">
         <v>1048962277.62</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="6">
         <v>46855590822.599998</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="6">
         <v>12043897.4486</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="6">
         <v>43948797656.800003</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="6">
         <v>13728941.7732</v>
       </c>
-      <c r="H36" s="11">
-        <f t="shared" si="0"/>
+      <c r="H36" s="10">
+        <f t="shared" si="2"/>
         <v>0.80858941734177958</v>
       </c>
-      <c r="I36" s="11">
-        <f t="shared" si="1"/>
+      <c r="I36" s="10">
+        <f t="shared" si="3"/>
         <v>0.75842673342288192</v>
       </c>
-      <c r="J36" s="11">
-        <f>C36/B36</f>
+      <c r="J36" s="10">
+        <f t="shared" si="0"/>
         <v>1.8101997690853078E-2</v>
       </c>
-      <c r="K36" s="11">
-        <f>E36/B36</f>
+      <c r="K36" s="10">
+        <f t="shared" si="1"/>
         <v>2.0784217741184443E-4</v>
       </c>
-      <c r="L36" s="11">
-        <f t="shared" si="2"/>
+      <c r="L36" s="10">
+        <f t="shared" si="4"/>
         <v>2.3692107674281186E-4</v>
       </c>
     </row>
@@ -5213,30 +8244,30 @@
       <c r="E37" s="4">
         <v>7882.1990687899997</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="6">
         <v>1071864.2</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="6">
         <v>846.37637018099997</v>
       </c>
-      <c r="H37" s="11">
-        <f t="shared" si="0"/>
+      <c r="H37" s="10">
+        <f t="shared" si="2"/>
         <v>1.0435936143743345</v>
       </c>
-      <c r="I37" s="11">
-        <f t="shared" si="1"/>
+      <c r="I37" s="10">
+        <f t="shared" si="3"/>
         <v>0.45701085052223084</v>
       </c>
-      <c r="J37" s="11">
-        <f>C37/B37</f>
+      <c r="J37" s="10">
+        <f t="shared" si="0"/>
         <v>1.6132415794718484E-3</v>
       </c>
-      <c r="K37" s="11">
-        <f>E37/B37</f>
+      <c r="K37" s="10">
+        <f t="shared" si="1"/>
         <v>3.3607340374025496E-3</v>
       </c>
-      <c r="L37" s="11">
-        <f t="shared" si="2"/>
+      <c r="L37" s="10">
+        <f t="shared" si="4"/>
         <v>3.6086958105172029E-4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update results by pinning pmcstat on other processes to isolate it from processes being measured
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="259" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{8B016830-57E2-41D7-B39B-C8244CC0FBA6}"/>
+  <xr:revisionPtr revIDLastSave="295" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{D103E7D9-D7A1-49CA-9806-9281BB1C111D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -177,7 +177,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +213,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -235,7 +248,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -259,6 +272,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3744,19 +3764,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670D2A71-BD87-4620-9FEC-7336DAF0F286}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="43.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.46484375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.65">
@@ -3829,85 +3849,85 @@
         <v>0</v>
       </c>
       <c r="B5" s="6">
-        <v>11042963</v>
+        <v>11060181.4</v>
       </c>
       <c r="C5" s="6">
-        <v>36350.102217200001</v>
+        <v>38115.304997300002</v>
       </c>
       <c r="D5" s="6">
-        <v>11490479</v>
+        <v>11558800.800000001</v>
       </c>
       <c r="E5" s="6">
-        <v>50127.715224200001</v>
+        <v>48028.480735500001</v>
       </c>
       <c r="F5" s="6">
-        <v>11749421.199999999</v>
+        <v>10593137.4</v>
       </c>
       <c r="G5" s="6">
-        <v>3389.7836155099999</v>
+        <v>3107.88472116</v>
       </c>
       <c r="H5" s="6">
         <f>D5/B5</f>
-        <v>1.0405249931562752</v>
+        <v>1.0450823889741989</v>
       </c>
       <c r="I5" s="6">
         <f>F5/B5</f>
-        <v>1.0639736092568632</v>
+        <v>0.95777248282745164</v>
       </c>
       <c r="J5" s="6">
         <f>C5/B5</f>
-        <v>3.2916982713063515E-3</v>
+        <v>3.4461735860227393E-3</v>
       </c>
       <c r="K5" s="6">
         <f>E5/B5</f>
-        <v>4.5393356134762024E-3</v>
+        <v>4.3424677225908787E-3</v>
       </c>
       <c r="L5" s="6">
         <f>G5/B5</f>
-        <v>3.0696323219682979E-4</v>
+        <v>2.8099762641867697E-4</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="6">
-        <v>157808861394</v>
+        <v>158167304127</v>
       </c>
       <c r="C6" s="6">
-        <v>496799761.12900001</v>
+        <v>552804965.96500003</v>
       </c>
       <c r="D6" s="6">
-        <v>76807903909.800003</v>
+        <v>77076505682.800003</v>
       </c>
       <c r="E6" s="6">
-        <v>338973495.222</v>
+        <v>342947323.72899997</v>
       </c>
       <c r="F6" s="6">
-        <v>80568006264</v>
+        <v>72706085161.399994</v>
       </c>
       <c r="G6" s="6">
-        <v>22781067.6855</v>
+        <v>12249880.3443</v>
       </c>
       <c r="H6" s="6">
         <f t="shared" ref="H6:H37" si="0">D6/B6</f>
-        <v>0.48671477147303144</v>
+        <v>0.48730997919084235</v>
       </c>
       <c r="I6" s="6">
         <f t="shared" ref="I6:I37" si="1">F6/B6</f>
-        <v>0.51054171199452836</v>
+        <v>0.45967834858600637</v>
       </c>
       <c r="J6" s="6">
         <f t="shared" ref="J6:J37" si="2">C6/B6</f>
-        <v>3.1481106747779162E-3</v>
+        <v>3.4950647291878151E-3</v>
       </c>
       <c r="K6" s="6">
         <f t="shared" ref="K6:K37" si="3">E6/B6</f>
-        <v>2.1480003862120764E-3</v>
+        <v>2.1682567432118041E-3</v>
       </c>
       <c r="L6" s="6">
         <f t="shared" ref="L6:L37" si="4">G6/B6</f>
-        <v>1.4435860878954515E-4</v>
+        <v>7.7448878653605882E-5</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
@@ -3915,171 +3935,171 @@
         <v>2</v>
       </c>
       <c r="B7" s="6">
-        <v>138485683363</v>
+        <v>138115690601</v>
       </c>
       <c r="C7" s="6">
-        <v>543084960.44099998</v>
+        <v>600091493.84000003</v>
       </c>
       <c r="D7" s="6">
-        <v>107843598232</v>
+        <v>107043986904</v>
       </c>
       <c r="E7" s="6">
-        <v>776016455.204</v>
+        <v>643825984.86000001</v>
       </c>
       <c r="F7" s="6">
-        <v>109535573413</v>
+        <v>98269727224</v>
       </c>
       <c r="G7" s="6">
-        <v>118205810.941</v>
+        <v>104851095.565</v>
       </c>
       <c r="H7" s="6">
         <f t="shared" si="0"/>
-        <v>0.77873463605129001</v>
+        <v>0.77503132655099627</v>
       </c>
       <c r="I7" s="6">
         <f t="shared" si="1"/>
-        <v>0.79095232628404122</v>
+        <v>0.71150299286335028</v>
       </c>
       <c r="J7" s="6">
         <f t="shared" si="2"/>
-        <v>3.921596422479719E-3</v>
+        <v>4.3448466371108687E-3</v>
       </c>
       <c r="K7" s="6">
         <f t="shared" si="3"/>
-        <v>5.6035861351089863E-3</v>
+        <v>4.6614977781194869E-3</v>
       </c>
       <c r="L7" s="6">
         <f t="shared" si="4"/>
-        <v>8.5355979095079308E-4</v>
+        <v>7.5915412006230694E-4</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="6">
-        <v>5635082.2000000002</v>
+        <v>5427037.7999999998</v>
       </c>
       <c r="C8" s="6">
-        <v>24595.531296599998</v>
+        <v>18018.001169899999</v>
       </c>
       <c r="D8" s="6">
-        <v>4746928.4000000004</v>
+        <v>4563338.4000000004</v>
       </c>
       <c r="E8" s="6">
-        <v>29787.6946379</v>
+        <v>34264.711851100001</v>
       </c>
       <c r="F8" s="6">
-        <v>5513902.4000000004</v>
+        <v>4818117.2</v>
       </c>
       <c r="G8" s="6">
-        <v>13202.382278999999</v>
+        <v>3934.6960949999998</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" si="0"/>
-        <v>0.84238849257602666</v>
+        <v>0.84085251810849748</v>
       </c>
       <c r="I8" s="6">
         <f t="shared" si="1"/>
-        <v>0.97849546897470285</v>
+        <v>0.88779871774617092</v>
       </c>
       <c r="J8" s="6">
         <f t="shared" si="2"/>
-        <v>4.3647156196940651E-3</v>
+        <v>3.3200434258814264E-3</v>
       </c>
       <c r="K8" s="6">
         <f t="shared" si="3"/>
-        <v>5.2861153716444453E-3</v>
+        <v>6.3137042920725561E-3</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" si="4"/>
-        <v>2.3428908062778568E-3</v>
+        <v>7.2501726356134831E-4</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="A9" s="15" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="6">
-        <v>2352445.6</v>
+        <v>2176628.7999999998</v>
       </c>
       <c r="C9" s="6">
-        <v>20876.667527199999</v>
+        <v>8777.2189992000003</v>
       </c>
       <c r="D9" s="6">
-        <v>1984880.2</v>
+        <v>1766594.6</v>
       </c>
       <c r="E9" s="6">
-        <v>14028.128576499999</v>
+        <v>11426.3262968</v>
       </c>
       <c r="F9" s="6">
-        <v>1738382.2</v>
+        <v>1619907.4</v>
       </c>
       <c r="G9" s="6">
-        <v>11607.4450832</v>
+        <v>12149.9388081</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" si="0"/>
-        <v>0.8437517960032741</v>
+        <v>0.81161960183564619</v>
       </c>
       <c r="I9" s="6">
         <f t="shared" si="1"/>
-        <v>0.73896807645626317</v>
+        <v>0.74422767906038922</v>
       </c>
       <c r="J9" s="6">
         <f t="shared" si="2"/>
-        <v>8.8744528363163839E-3</v>
+        <v>4.0324831680992185E-3</v>
       </c>
       <c r="K9" s="6">
         <f t="shared" si="3"/>
-        <v>5.9632106164325327E-3</v>
+        <v>5.2495521040611063E-3</v>
       </c>
       <c r="L9" s="6">
         <f t="shared" si="4"/>
-        <v>4.934203402280588E-3</v>
+        <v>5.5819985511999107E-3</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="6">
-        <v>159890048.59999999</v>
+        <v>153519617</v>
       </c>
       <c r="C10" s="6">
-        <v>373621.64579799998</v>
+        <v>288303.59377699997</v>
       </c>
       <c r="D10" s="6">
-        <v>137003438.19999999</v>
+        <v>131940813.8</v>
       </c>
       <c r="E10" s="6">
-        <v>478934.21460200002</v>
+        <v>277103.72511599999</v>
       </c>
       <c r="F10" s="6">
-        <v>139969464.40000001</v>
+        <v>136084138.59999999</v>
       </c>
       <c r="G10" s="6">
-        <v>294426.80045899999</v>
+        <v>197541.10542499999</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" si="0"/>
-        <v>0.85686031994864242</v>
+        <v>0.85943944088917312</v>
       </c>
       <c r="I10" s="6">
         <f t="shared" si="1"/>
-        <v>0.87541073147187731</v>
+        <v>0.88642833573510016</v>
       </c>
       <c r="J10" s="6">
         <f t="shared" si="2"/>
-        <v>2.3367410859489852E-3</v>
+        <v>1.8779593084641423E-3</v>
       </c>
       <c r="K10" s="6">
         <f t="shared" si="3"/>
-        <v>2.9953972670316645E-3</v>
+        <v>1.8050053180890882E-3</v>
       </c>
       <c r="L10" s="6">
         <f t="shared" si="4"/>
-        <v>1.8414329286719599E-3</v>
+        <v>1.2867482950077969E-3</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
@@ -4087,42 +4107,42 @@
         <v>34</v>
       </c>
       <c r="B11" s="6">
-        <v>4372762.2</v>
+        <v>4383215.8</v>
       </c>
       <c r="C11" s="6">
-        <v>3117.0640930200002</v>
+        <v>4428.0626644200001</v>
       </c>
       <c r="D11" s="6">
-        <v>4552725.2</v>
+        <v>4509902.8</v>
       </c>
       <c r="E11" s="6">
-        <v>5667.8894978600001</v>
+        <v>6367.88974151</v>
       </c>
       <c r="F11" s="6">
-        <v>8427265.4000000004</v>
+        <v>8433161.5999999996</v>
       </c>
       <c r="G11" s="6">
-        <v>4205.9492436299997</v>
+        <v>6668.6516958100001</v>
       </c>
       <c r="H11" s="6">
         <f t="shared" si="0"/>
-        <v>1.0411554508955461</v>
+        <v>1.028902752175697</v>
       </c>
       <c r="I11" s="6">
         <f t="shared" si="1"/>
-        <v>1.9272178578565282</v>
+        <v>1.9239667825617894</v>
       </c>
       <c r="J11" s="6">
         <f t="shared" si="2"/>
-        <v>7.1283640647552252E-4</v>
+        <v>1.0102314981662551E-3</v>
       </c>
       <c r="K11" s="6">
         <f t="shared" si="3"/>
-        <v>1.2961805921803842E-3</v>
+        <v>1.4527894660148835E-3</v>
       </c>
       <c r="L11" s="6">
         <f t="shared" si="4"/>
-        <v>9.6185181156889792E-4</v>
+        <v>1.5214062003997158E-3</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
@@ -4130,42 +4150,42 @@
         <v>5</v>
       </c>
       <c r="B12" s="6">
-        <v>17849745</v>
+        <v>17775974.600000001</v>
       </c>
       <c r="C12" s="6">
-        <v>121261.041488</v>
+        <v>109609.235453</v>
       </c>
       <c r="D12" s="6">
-        <v>17575590.199999999</v>
+        <v>17466646.399999999</v>
       </c>
       <c r="E12" s="6">
-        <v>39122.121805399998</v>
+        <v>26263.132559500002</v>
       </c>
       <c r="F12" s="6">
-        <v>14195115.6</v>
+        <v>14177905.199999999</v>
       </c>
       <c r="G12" s="6">
-        <v>72961.760325800002</v>
+        <v>83422.891844900005</v>
       </c>
       <c r="H12" s="6">
         <f t="shared" si="0"/>
-        <v>0.98464096826033087</v>
+        <v>0.98259852374001466</v>
       </c>
       <c r="I12" s="6">
         <f t="shared" si="1"/>
-        <v>0.79525593222760327</v>
+        <v>0.79758806586053499</v>
       </c>
       <c r="J12" s="6">
         <f t="shared" si="2"/>
-        <v>6.793432706629703E-3</v>
+        <v>6.166144918602662E-3</v>
       </c>
       <c r="K12" s="6">
         <f t="shared" si="3"/>
-        <v>2.1917468179741503E-3</v>
+        <v>1.4774510624863291E-3</v>
       </c>
       <c r="L12" s="6">
         <f t="shared" si="4"/>
-        <v>4.0875519692746311E-3</v>
+        <v>4.6930136727861881E-3</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
@@ -4173,42 +4193,42 @@
         <v>36</v>
       </c>
       <c r="B13" s="6">
-        <v>3933218.4</v>
+        <v>3778745</v>
       </c>
       <c r="C13" s="6">
-        <v>40695.104273600002</v>
+        <v>37023.3373374</v>
       </c>
       <c r="D13" s="6">
-        <v>3949440.6</v>
+        <v>3744922.4</v>
       </c>
       <c r="E13" s="6">
-        <v>41038.642485299999</v>
+        <v>90744.508086400005</v>
       </c>
       <c r="F13" s="6">
-        <v>1798863.6</v>
+        <v>1685866.6</v>
       </c>
       <c r="G13" s="6">
-        <v>68914.215713700003</v>
+        <v>91067.958599299993</v>
       </c>
       <c r="H13" s="6">
         <f t="shared" si="0"/>
-        <v>1.0041244086522121</v>
+        <v>0.99104925047866421</v>
       </c>
       <c r="I13" s="6">
         <f t="shared" si="1"/>
-        <v>0.45735156735766319</v>
+        <v>0.44614457974803806</v>
       </c>
       <c r="J13" s="6">
         <f t="shared" si="2"/>
-        <v>1.0346515279599018E-2</v>
+        <v>9.7977866559929294E-3</v>
       </c>
       <c r="K13" s="6">
         <f t="shared" si="3"/>
-        <v>1.0433858055098085E-2</v>
+        <v>2.4014456674477904E-2</v>
       </c>
       <c r="L13" s="6">
         <f t="shared" si="4"/>
-        <v>1.752107528880166E-2</v>
+        <v>2.4100054012456514E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
@@ -4216,386 +4236,386 @@
         <v>6</v>
       </c>
       <c r="B14" s="6">
-        <v>491359952.39999998</v>
+        <v>469606679.60000002</v>
       </c>
       <c r="C14" s="6">
-        <v>9169742.7574700005</v>
+        <v>2704649.26914</v>
       </c>
       <c r="D14" s="6">
-        <v>471227525.39999998</v>
+        <v>465798168.80000001</v>
       </c>
       <c r="E14" s="6">
-        <v>3672817.92307</v>
+        <v>4047272.3654299998</v>
       </c>
       <c r="F14" s="6">
-        <v>305508096.39999998</v>
+        <v>299984120.60000002</v>
       </c>
       <c r="G14" s="6">
-        <v>2437082.1589700002</v>
+        <v>3365377.74603</v>
       </c>
       <c r="H14" s="6">
         <f t="shared" si="0"/>
-        <v>0.95902713092170999</v>
+        <v>0.99188999866176519</v>
       </c>
       <c r="I14" s="6">
         <f t="shared" si="1"/>
-        <v>0.62176026944763274</v>
+        <v>0.63879866627007831</v>
       </c>
       <c r="J14" s="6">
         <f t="shared" si="2"/>
-        <v>1.8661966065165226E-2</v>
+        <v>5.7593926718498912E-3</v>
       </c>
       <c r="K14" s="6">
         <f t="shared" si="3"/>
-        <v>7.4748011211139154E-3</v>
+        <v>8.6184301485604329E-3</v>
       </c>
       <c r="L14" s="6">
         <f t="shared" si="4"/>
-        <v>4.9598713673475198E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A15" s="7" t="s">
+        <v>7.166375378000479E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="16" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="6">
-        <v>827068603.39999998</v>
+        <v>643995703.79999995</v>
       </c>
       <c r="C15" s="6">
-        <v>149806870.93599999</v>
+        <v>141094510.22799999</v>
       </c>
       <c r="D15" s="6">
-        <v>431549641.60000002</v>
+        <v>375302332.39999998</v>
       </c>
       <c r="E15" s="6">
-        <v>3294993.7427300001</v>
+        <v>16956708.175900001</v>
       </c>
       <c r="F15" s="6">
-        <v>518062177</v>
+        <v>548955151.20000005</v>
       </c>
       <c r="G15" s="6">
-        <v>4674219.7722199997</v>
-      </c>
-      <c r="H15" s="6">
-        <f t="shared" si="0"/>
-        <v>0.52178215909289838</v>
-      </c>
-      <c r="I15" s="6">
-        <f t="shared" si="1"/>
-        <v>0.62638356101331361</v>
-      </c>
-      <c r="J15" s="6">
-        <f t="shared" si="2"/>
-        <v>0.18112992116997098</v>
-      </c>
-      <c r="K15" s="6">
-        <f t="shared" si="3"/>
-        <v>3.9839424797224752E-3</v>
-      </c>
-      <c r="L15" s="6">
-        <f t="shared" si="4"/>
-        <v>5.651550249888255E-3</v>
+        <v>16014400.234200001</v>
+      </c>
+      <c r="H15" s="13">
+        <f t="shared" si="0"/>
+        <v>0.58277148463175821</v>
+      </c>
+      <c r="I15" s="13">
+        <f t="shared" si="1"/>
+        <v>0.85242051765377025</v>
+      </c>
+      <c r="J15" s="13">
+        <f t="shared" si="2"/>
+        <v>0.21909231598199988</v>
+      </c>
+      <c r="K15" s="13">
+        <f t="shared" si="3"/>
+        <v>2.6330467852260852E-2</v>
+      </c>
+      <c r="L15" s="13">
+        <f t="shared" si="4"/>
+        <v>2.4867247001345603E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="6">
-        <v>6136437</v>
+        <v>6210147.5999999996</v>
       </c>
       <c r="C16" s="6">
-        <v>14595.562626999999</v>
+        <v>25652.449751200002</v>
       </c>
       <c r="D16" s="6">
-        <v>6183005.7999999998</v>
+        <v>6209546.4000000004</v>
       </c>
       <c r="E16" s="6">
-        <v>23508.9007944</v>
+        <v>30482.5218484</v>
       </c>
       <c r="F16" s="6">
-        <v>5271526</v>
+        <v>5369027.4000000004</v>
       </c>
       <c r="G16" s="6">
-        <v>55955.4177538</v>
+        <v>23986.761495499999</v>
       </c>
       <c r="H16" s="6">
         <f t="shared" si="0"/>
-        <v>1.0075888989001272</v>
+        <v>0.99990319070677169</v>
       </c>
       <c r="I16" s="6">
         <f t="shared" si="1"/>
-        <v>0.85905322583772958</v>
+        <v>0.86455713226526221</v>
       </c>
       <c r="J16" s="6">
         <f t="shared" si="2"/>
-        <v>2.3785076954265152E-3</v>
+        <v>4.1307310878086062E-3</v>
       </c>
       <c r="K16" s="6">
         <f t="shared" si="3"/>
-        <v>3.8310343273140423E-3</v>
+        <v>4.9085019892924934E-3</v>
       </c>
       <c r="L16" s="6">
         <f t="shared" si="4"/>
-        <v>9.1185516536387481E-3</v>
+        <v>3.8625106906476749E-3</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+      <c r="A17" s="14" t="s">
         <v>37</v>
       </c>
       <c r="B17" s="6">
-        <v>1076924.2</v>
+        <v>1110071</v>
       </c>
       <c r="C17" s="6">
-        <v>14553.050421100001</v>
+        <v>6416.1450420000001</v>
       </c>
       <c r="D17" s="6">
-        <v>1147012</v>
+        <v>1089568.3999999999</v>
       </c>
       <c r="E17" s="6">
-        <v>19796.770049700001</v>
+        <v>8594.6275917000003</v>
       </c>
       <c r="F17" s="6">
-        <v>680652.6</v>
+        <v>702127.2</v>
       </c>
       <c r="G17" s="6">
-        <v>9832.5468033500001</v>
+        <v>7013.5801813300004</v>
       </c>
       <c r="H17" s="6">
         <f t="shared" si="0"/>
-        <v>1.0650814607007624</v>
+        <v>0.98153037057989978</v>
       </c>
       <c r="I17" s="6">
         <f t="shared" si="1"/>
-        <v>0.63203389802179211</v>
+        <v>0.63250656939961492</v>
       </c>
       <c r="J17" s="6">
         <f t="shared" si="2"/>
-        <v>1.3513532726908729E-2</v>
+        <v>5.7799411407018107E-3</v>
       </c>
       <c r="K17" s="6">
         <f t="shared" si="3"/>
-        <v>1.8382695875624303E-2</v>
+        <v>7.7424125048758145E-3</v>
       </c>
       <c r="L17" s="6">
         <f t="shared" si="4"/>
-        <v>9.1302125101748108E-3</v>
+        <v>6.318136570840965E-3</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="6">
-        <v>142122988.40000001</v>
+        <v>142493877.59999999</v>
       </c>
       <c r="C18" s="6">
-        <v>1688359.3844900001</v>
+        <v>371768.52788299997</v>
       </c>
       <c r="D18" s="6">
-        <v>143348534.59999999</v>
+        <v>140258619.59999999</v>
       </c>
       <c r="E18" s="6">
-        <v>2386850.5735499999</v>
+        <v>1273454.5480599999</v>
       </c>
       <c r="F18" s="6">
-        <v>97369622</v>
+        <v>99214962</v>
       </c>
       <c r="G18" s="6">
-        <v>1822551.4533800001</v>
+        <v>527914.96147800004</v>
       </c>
       <c r="H18" s="6">
         <f t="shared" si="0"/>
-        <v>1.0086231384084798</v>
+        <v>0.98431330498090119</v>
       </c>
       <c r="I18" s="6">
         <f t="shared" si="1"/>
-        <v>0.6851081805707373</v>
+        <v>0.69627526228537417</v>
       </c>
       <c r="J18" s="6">
         <f t="shared" si="2"/>
-        <v>1.1879565744411269E-2</v>
+        <v>2.6090140442848052E-3</v>
       </c>
       <c r="K18" s="6">
         <f t="shared" si="3"/>
-        <v>1.6794261086266322E-2</v>
+        <v>8.936907111439291E-3</v>
       </c>
       <c r="L18" s="6">
         <f t="shared" si="4"/>
-        <v>1.2823762530594241E-2</v>
+        <v>3.7048255712426488E-3</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="17" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="6">
-        <v>147012341.40000001</v>
+        <v>129526124.8</v>
       </c>
       <c r="C19" s="6">
-        <v>7606800.8915200001</v>
+        <v>8081944.83452</v>
       </c>
       <c r="D19" s="6">
-        <v>79703584.200000003</v>
+        <v>58015974</v>
       </c>
       <c r="E19" s="6">
-        <v>8290771.0046100002</v>
+        <v>2038374.7693700001</v>
       </c>
       <c r="F19" s="6">
-        <v>83981813.400000006</v>
+        <v>84578620</v>
       </c>
       <c r="G19" s="6">
-        <v>1750299.80644</v>
+        <v>4502817.2907499997</v>
       </c>
       <c r="H19" s="6">
         <f t="shared" si="0"/>
-        <v>0.54215573632105962</v>
+        <v>0.44790943981055475</v>
       </c>
       <c r="I19" s="6">
         <f t="shared" si="1"/>
-        <v>0.57125689313047023</v>
+        <v>0.65298502623001353</v>
       </c>
       <c r="J19" s="6">
         <f t="shared" si="2"/>
-        <v>5.1742600784943353E-2</v>
+        <v>6.2396252856319535E-2</v>
       </c>
       <c r="K19" s="6">
         <f t="shared" si="3"/>
-        <v>5.6395068098752152E-2</v>
+        <v>1.5737170956958948E-2</v>
       </c>
       <c r="L19" s="6">
         <f t="shared" si="4"/>
-        <v>1.1905801851544417E-2</v>
+        <v>3.4763776787908658E-2</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+      <c r="A20" s="14" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="6">
-        <v>2898308.6</v>
+        <v>2762373</v>
       </c>
       <c r="C20" s="6">
-        <v>36388.156362200003</v>
+        <v>38040.132260500002</v>
       </c>
       <c r="D20" s="6">
-        <v>2883458.6</v>
+        <v>2772015.2</v>
       </c>
       <c r="E20" s="6">
-        <v>39483.321585700003</v>
+        <v>25998.012880999999</v>
       </c>
       <c r="F20" s="6">
-        <v>1164719.2</v>
+        <v>1120678.3999999999</v>
       </c>
       <c r="G20" s="6">
-        <v>45536.9098486</v>
+        <v>49133.758751399997</v>
       </c>
       <c r="H20" s="6">
         <f t="shared" si="0"/>
-        <v>0.99487632200380594</v>
+        <v>1.0034905496107875</v>
       </c>
       <c r="I20" s="6">
         <f t="shared" si="1"/>
-        <v>0.40186169271277733</v>
+        <v>0.40569408982784</v>
       </c>
       <c r="J20" s="6">
         <f t="shared" si="2"/>
-        <v>1.2554962698658108E-2</v>
+        <v>1.3770816707410621E-2</v>
       </c>
       <c r="K20" s="6">
         <f t="shared" si="3"/>
-        <v>1.3622883907427941E-2</v>
+        <v>9.4114780592628143E-3</v>
       </c>
       <c r="L20" s="6">
         <f t="shared" si="4"/>
-        <v>1.5711546330366612E-2</v>
+        <v>1.7786793728218453E-2</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+      <c r="A21" s="14" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="6">
-        <v>524441.59999999998</v>
+        <v>551144.6</v>
       </c>
       <c r="C21" s="6">
-        <v>15199.6411352</v>
+        <v>5290.3938076499999</v>
       </c>
       <c r="D21" s="6">
-        <v>527874.6</v>
+        <v>527654</v>
       </c>
       <c r="E21" s="6">
-        <v>7304.8818635199996</v>
+        <v>4825.0795641100003</v>
       </c>
       <c r="F21" s="6">
-        <v>171678</v>
+        <v>188306.6</v>
       </c>
       <c r="G21" s="6">
-        <v>8760.4336650599998</v>
+        <v>2862.5033519600001</v>
       </c>
       <c r="H21" s="6">
         <f t="shared" si="0"/>
-        <v>1.0065460100800547</v>
+        <v>0.95737851736186841</v>
       </c>
       <c r="I21" s="6">
         <f t="shared" si="1"/>
-        <v>0.32735389412281557</v>
+        <v>0.34166460126797943</v>
       </c>
       <c r="J21" s="6">
         <f t="shared" si="2"/>
-        <v>2.8982523764705163E-2</v>
+        <v>9.5989216036045707E-3</v>
       </c>
       <c r="K21" s="6">
         <f t="shared" si="3"/>
-        <v>1.3928875709936053E-2</v>
+        <v>8.7546527065855331E-3</v>
       </c>
       <c r="L21" s="6">
         <f t="shared" si="4"/>
-        <v>1.6704307333857575E-2</v>
+        <v>5.1937428978892294E-3</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="6">
-        <v>22343582893.799999</v>
+        <v>21921636153.799999</v>
       </c>
       <c r="C22" s="6">
-        <v>36130395.837800004</v>
+        <v>44023942.3477</v>
       </c>
       <c r="D22" s="6">
-        <v>25119837726.799999</v>
+        <v>24100457793</v>
       </c>
       <c r="E22" s="6">
-        <v>55201502.9027</v>
+        <v>45888213.592100002</v>
       </c>
       <c r="F22" s="6">
-        <v>42836296043.599998</v>
+        <v>42672266919.400002</v>
       </c>
       <c r="G22" s="6">
-        <v>80425547.617799997</v>
+        <v>97728438.242799997</v>
       </c>
       <c r="H22" s="6">
         <f t="shared" si="0"/>
-        <v>1.1242528938261898</v>
+        <v>1.0993913786322156</v>
       </c>
       <c r="I22" s="6">
         <f t="shared" si="1"/>
-        <v>1.9171632520711981</v>
+        <v>1.946582208554857</v>
       </c>
       <c r="J22" s="6">
         <f t="shared" si="2"/>
-        <v>1.6170368024470074E-3</v>
+        <v>2.0082416311826561E-3</v>
       </c>
       <c r="K22" s="6">
         <f t="shared" si="3"/>
-        <v>2.470575250400757E-3</v>
+        <v>2.0932841540728486E-3</v>
       </c>
       <c r="L22" s="6">
         <f t="shared" si="4"/>
-        <v>3.5994919883738452E-3</v>
+        <v>4.4580813930651473E-3</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.45">
@@ -4603,42 +4623,42 @@
         <v>10</v>
       </c>
       <c r="B23" s="6">
-        <v>212878332.19999999</v>
+        <v>209163281.19999999</v>
       </c>
       <c r="C23" s="6">
-        <v>397135.33510700002</v>
+        <v>277638.59746100003</v>
       </c>
       <c r="D23" s="6">
-        <v>216692924.80000001</v>
+        <v>210255495.19999999</v>
       </c>
       <c r="E23" s="6">
-        <v>2671681.7472000001</v>
+        <v>759532.77214400005</v>
       </c>
       <c r="F23" s="6">
-        <v>423024331.39999998</v>
+        <v>424145380.60000002</v>
       </c>
       <c r="G23" s="6">
-        <v>637180.44013500004</v>
+        <v>1372976.29354</v>
       </c>
       <c r="H23" s="6">
         <f t="shared" si="0"/>
-        <v>1.0179191210330236</v>
+        <v>1.005221824756878</v>
       </c>
       <c r="I23" s="6">
         <f t="shared" si="1"/>
-        <v>1.9871648139490639</v>
+        <v>2.0278195014278637</v>
       </c>
       <c r="J23" s="6">
         <f t="shared" si="2"/>
-        <v>1.8655507632119642E-3</v>
+        <v>1.3273773286981694E-3</v>
       </c>
       <c r="K23" s="6">
         <f t="shared" si="3"/>
-        <v>1.2550275641439849E-2</v>
+        <v>3.6312911510397558E-3</v>
       </c>
       <c r="L23" s="6">
         <f t="shared" si="4"/>
-        <v>2.9931671934387699E-3</v>
+        <v>6.5641363324529835E-3</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.45">
@@ -4646,42 +4666,42 @@
         <v>11</v>
       </c>
       <c r="B24" s="6">
-        <v>709259220</v>
+        <v>708340622.39999998</v>
       </c>
       <c r="C24" s="6">
-        <v>1579941.92038</v>
+        <v>641845.68573499995</v>
       </c>
       <c r="D24" s="6">
-        <v>684113708.79999995</v>
+        <v>686259407.20000005</v>
       </c>
       <c r="E24" s="6">
-        <v>478306.96039199998</v>
+        <v>1098996.8950100001</v>
       </c>
       <c r="F24" s="6">
-        <v>640069622.20000005</v>
+        <v>638935891.60000002</v>
       </c>
       <c r="G24" s="6">
-        <v>1361179.1296999999</v>
+        <v>723161.32633499999</v>
       </c>
       <c r="H24" s="6">
         <f t="shared" si="0"/>
-        <v>0.96454679686786438</v>
+        <v>0.96882684050339463</v>
       </c>
       <c r="I24" s="6">
         <f t="shared" si="1"/>
-        <v>0.90244808125300091</v>
+        <v>0.90201785891532971</v>
       </c>
       <c r="J24" s="6">
         <f t="shared" si="2"/>
-        <v>2.2275944757968744E-3</v>
+        <v>9.0612576130435401E-4</v>
       </c>
       <c r="K24" s="6">
         <f t="shared" si="3"/>
-        <v>6.7437538618391173E-4</v>
+        <v>1.5515090625275428E-3</v>
       </c>
       <c r="L24" s="6">
         <f t="shared" si="4"/>
-        <v>1.9191560593318758E-3</v>
+        <v>1.0209231314233884E-3</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.45">
@@ -4689,257 +4709,257 @@
         <v>12</v>
       </c>
       <c r="B25" s="6">
-        <v>557809444.79999995</v>
+        <v>556696993.39999998</v>
       </c>
       <c r="C25" s="6">
-        <v>303447.01951800002</v>
+        <v>561072.16255300003</v>
       </c>
       <c r="D25" s="6">
-        <v>589765440.60000002</v>
+        <v>589117249</v>
       </c>
       <c r="E25" s="6">
-        <v>754401.82024599996</v>
+        <v>1712351.1913900001</v>
       </c>
       <c r="F25" s="6">
-        <v>555224957.20000005</v>
+        <v>558449117.39999998</v>
       </c>
       <c r="G25" s="6">
-        <v>1604658.79428</v>
+        <v>1017194.8683</v>
       </c>
       <c r="H25" s="6">
         <f t="shared" si="0"/>
-        <v>1.057288373472159</v>
+        <v>1.0582368074273132</v>
       </c>
       <c r="I25" s="6">
         <f t="shared" si="1"/>
-        <v>0.99536671954178446</v>
+        <v>1.0031473566783593</v>
       </c>
       <c r="J25" s="6">
         <f t="shared" si="2"/>
-        <v>5.4399763637347437E-4</v>
+        <v>1.0078591571444978E-3</v>
       </c>
       <c r="K25" s="6">
         <f t="shared" si="3"/>
-        <v>1.3524364409363619E-3</v>
+        <v>3.0759124114033702E-3</v>
       </c>
       <c r="L25" s="6">
         <f t="shared" si="4"/>
-        <v>2.8767149951276698E-3</v>
+        <v>1.8271966264583747E-3</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="6">
-        <v>1480365255.8</v>
+        <v>1477601681.4000001</v>
       </c>
       <c r="C26" s="6">
-        <v>747950.06621399999</v>
+        <v>1728466.8404600001</v>
       </c>
       <c r="D26" s="6">
-        <v>1489458102</v>
+        <v>1489098104.5999999</v>
       </c>
       <c r="E26" s="6">
-        <v>1423514.07947</v>
+        <v>2668410.3672199999</v>
       </c>
       <c r="F26" s="6">
-        <v>1615958912</v>
+        <v>1620387369.5999999</v>
       </c>
       <c r="G26" s="6">
-        <v>3696074.7233500001</v>
+        <v>817772.39235400001</v>
       </c>
       <c r="H26" s="6">
         <f t="shared" si="0"/>
-        <v>1.0061422991146103</v>
+        <v>1.0077804616390982</v>
       </c>
       <c r="I26" s="6">
         <f t="shared" si="1"/>
-        <v>1.0915947301983417</v>
+        <v>1.0966334093940073</v>
       </c>
       <c r="J26" s="6">
         <f t="shared" si="2"/>
-        <v>5.0524697420691793E-4</v>
+        <v>1.1697786096333553E-3</v>
       </c>
       <c r="K26" s="6">
         <f t="shared" si="3"/>
-        <v>9.6159652078616419E-4</v>
+        <v>1.80590642309755E-3</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="4"/>
-        <v>2.4967316065200511E-3</v>
+        <v>5.5344576461172936E-4</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B27" s="6">
-        <v>2809106711.8000002</v>
+        <v>2789833426.5999999</v>
       </c>
       <c r="C27" s="6">
-        <v>1625417.0842299999</v>
+        <v>2035141.57268</v>
       </c>
       <c r="D27" s="6">
-        <v>2026142191</v>
+        <v>2027571768.2</v>
       </c>
       <c r="E27" s="6">
-        <v>1372255.2624299999</v>
+        <v>5045395.4141699998</v>
       </c>
       <c r="F27" s="6">
-        <v>1700852976.4000001</v>
+        <v>1682159963.2</v>
       </c>
       <c r="G27" s="6">
-        <v>3260068.4286600002</v>
+        <v>1509844.4139099999</v>
       </c>
       <c r="H27" s="6">
         <f t="shared" si="0"/>
-        <v>0.72127633403492264</v>
+        <v>0.7267716233047733</v>
       </c>
       <c r="I27" s="6">
         <f t="shared" si="1"/>
-        <v>0.60547823593007588</v>
+        <v>0.60296071699523168</v>
       </c>
       <c r="J27" s="6">
         <f t="shared" si="2"/>
-        <v>5.7862418590302553E-4</v>
+        <v>7.29484976871988E-4</v>
       </c>
       <c r="K27" s="6">
         <f t="shared" si="3"/>
-        <v>4.8850236150363099E-4</v>
+        <v>1.8084934269064507E-3</v>
       </c>
       <c r="L27" s="6">
         <f t="shared" si="4"/>
-        <v>1.1605356304072321E-3</v>
+        <v>5.4119518373900324E-4</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B28" s="6">
-        <v>4289303031.1999998</v>
+        <v>4267317226.4000001</v>
       </c>
       <c r="C28" s="6">
-        <v>1861084.3700600001</v>
+        <v>3092450.0057700002</v>
       </c>
       <c r="D28" s="6">
-        <v>3515418335.1999998</v>
+        <v>3516513600.4000001</v>
       </c>
       <c r="E28" s="6">
-        <v>2787594.4441300002</v>
+        <v>7286563.9173800005</v>
       </c>
       <c r="F28" s="6">
-        <v>3316703760.4000001</v>
+        <v>3302437286.5999999</v>
       </c>
       <c r="G28" s="6">
-        <v>6826824.3310099998</v>
+        <v>1972912.4042799999</v>
       </c>
       <c r="H28" s="6">
         <f t="shared" si="0"/>
-        <v>0.81957798496146506</v>
+        <v>0.82405722701956374</v>
       </c>
       <c r="I28" s="6">
         <f t="shared" si="1"/>
-        <v>0.77325004465168323</v>
+        <v>0.77389074010464565</v>
       </c>
       <c r="J28" s="6">
         <f t="shared" si="2"/>
-        <v>4.3388969175706213E-4</v>
+        <v>7.2468247418738471E-4</v>
       </c>
       <c r="K28" s="6">
         <f t="shared" si="3"/>
-        <v>6.498944989088651E-4</v>
+        <v>1.7075280629012671E-3</v>
       </c>
       <c r="L28" s="6">
         <f t="shared" si="4"/>
-        <v>1.5915929187917714E-3</v>
+        <v>4.6233085088553185E-4</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B29" s="6">
-        <v>1761233472.5999999</v>
+        <v>1761068036.8</v>
       </c>
       <c r="C29" s="6">
-        <v>2709142.0694300001</v>
+        <v>4653678.0338899996</v>
       </c>
       <c r="D29" s="6">
-        <v>1398700815.2</v>
+        <v>1373532614.5999999</v>
       </c>
       <c r="E29" s="6">
-        <v>1047197.5988799999</v>
+        <v>2175874.9010899998</v>
       </c>
       <c r="F29" s="6">
-        <v>1395896628.8</v>
+        <v>1410393731.4000001</v>
       </c>
       <c r="G29" s="6">
-        <v>1064847.9888800001</v>
+        <v>1459853.02018</v>
       </c>
       <c r="H29" s="6">
         <f t="shared" si="0"/>
-        <v>0.79415979593845931</v>
+        <v>0.77994295841960626</v>
       </c>
       <c r="I29" s="6">
         <f t="shared" si="1"/>
-        <v>0.79256762406367631</v>
+        <v>0.80087407296472046</v>
       </c>
       <c r="J29" s="6">
         <f t="shared" si="2"/>
-        <v>1.5382072346323634E-3</v>
+        <v>2.6425316550211775E-3</v>
       </c>
       <c r="K29" s="6">
         <f t="shared" si="3"/>
-        <v>5.9458193088624814E-4</v>
+        <v>1.2355427817790259E-3</v>
       </c>
       <c r="L29" s="6">
         <f t="shared" si="4"/>
-        <v>6.04603538057922E-4</v>
+        <v>8.2895889861965154E-4</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B30" s="6">
-        <v>23773682</v>
+        <v>23105024.199999999</v>
       </c>
       <c r="C30" s="6">
-        <v>104006.54266200001</v>
+        <v>88711.490000799997</v>
       </c>
       <c r="D30" s="6">
-        <v>20807231.800000001</v>
+        <v>19289191</v>
       </c>
       <c r="E30" s="6">
-        <v>251232.72346800001</v>
+        <v>113025.01339399999</v>
       </c>
       <c r="F30" s="6">
-        <v>36443818.399999999</v>
+        <v>36502679.799999997</v>
       </c>
       <c r="G30" s="6">
-        <v>169420.30880500001</v>
+        <v>92017.848028299995</v>
       </c>
       <c r="H30" s="6">
         <f t="shared" si="0"/>
-        <v>0.87522125516779437</v>
+        <v>0.83484833571392669</v>
       </c>
       <c r="I30" s="6">
         <f t="shared" si="1"/>
-        <v>1.5329480052774322</v>
+        <v>1.5798589728376047</v>
       </c>
       <c r="J30" s="6">
         <f t="shared" si="2"/>
-        <v>4.3748605143284075E-3</v>
+        <v>3.8394891618767487E-3</v>
       </c>
       <c r="K30" s="6">
         <f t="shared" si="3"/>
-        <v>1.0567682509928416E-2</v>
+        <v>4.8917937681277127E-3</v>
       </c>
       <c r="L30" s="6">
         <f t="shared" si="4"/>
-        <v>7.1263807097697368E-3</v>
+        <v>3.9825904198057495E-3</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.45">
@@ -4947,257 +4967,257 @@
         <v>18</v>
       </c>
       <c r="B31" s="6">
-        <v>132607255038</v>
+        <v>130671943206</v>
       </c>
       <c r="C31" s="6">
-        <v>225116431.33000001</v>
+        <v>313480336.10299999</v>
       </c>
       <c r="D31" s="6">
-        <v>144831816170</v>
+        <v>139001519472</v>
       </c>
       <c r="E31" s="6">
-        <v>235396070.604</v>
+        <v>218100109.76300001</v>
       </c>
       <c r="F31" s="6">
-        <v>131505963283</v>
+        <v>130652543017</v>
       </c>
       <c r="G31" s="6">
-        <v>122990431.06999999</v>
+        <v>197662034.19400001</v>
       </c>
       <c r="H31" s="6">
         <f t="shared" si="0"/>
-        <v>1.0921862165723657</v>
+        <v>1.0637441830406447</v>
       </c>
       <c r="I31" s="6">
         <f t="shared" si="1"/>
-        <v>0.99169508670785456</v>
+        <v>0.99985153516107572</v>
       </c>
       <c r="J31" s="6">
         <f t="shared" si="2"/>
-        <v>1.6976177605477962E-3</v>
+        <v>2.3989873297346515E-3</v>
       </c>
       <c r="K31" s="6">
         <f t="shared" si="3"/>
-        <v>1.7751371939381808E-3</v>
+        <v>1.6690660933936859E-3</v>
       </c>
       <c r="L31" s="6">
         <f t="shared" si="4"/>
-        <v>9.2747890026647327E-4</v>
+        <v>1.512658565751887E-3</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B32" s="6">
-        <v>10270371487.799999</v>
+        <v>9231106491.2000008</v>
       </c>
       <c r="C32" s="6">
-        <v>28108011.878800001</v>
+        <v>31595097.076900002</v>
       </c>
       <c r="D32" s="6">
-        <v>10284664219</v>
+        <v>9057620010</v>
       </c>
       <c r="E32" s="6">
-        <v>35210784.745399997</v>
+        <v>20076141.795600001</v>
       </c>
       <c r="F32" s="6">
-        <v>12743590795.200001</v>
+        <v>12030245569.4</v>
       </c>
       <c r="G32" s="6">
-        <v>14444039.3672</v>
+        <v>17225067.5526</v>
       </c>
       <c r="H32" s="6">
         <f t="shared" si="0"/>
-        <v>1.0013916469542488</v>
+        <v>0.98120631785957779</v>
       </c>
       <c r="I32" s="6">
         <f t="shared" si="1"/>
-        <v>1.2408110855910028</v>
+        <v>1.3032289878649341</v>
       </c>
       <c r="J32" s="6">
         <f t="shared" si="2"/>
-        <v>2.7368057632763364E-3</v>
+        <v>3.4226771305281289E-3</v>
       </c>
       <c r="K32" s="6">
         <f t="shared" si="3"/>
-        <v>3.4283847266115245E-3</v>
+        <v>2.1748359001966398E-3</v>
       </c>
       <c r="L32" s="6">
         <f t="shared" si="4"/>
-        <v>1.4063794463869035E-3</v>
+        <v>1.8659808083701158E-3</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B33" s="6">
-        <v>9607753811.2000008</v>
+        <v>9682033494.3999996</v>
       </c>
       <c r="C33" s="6">
-        <v>73322321.484699994</v>
+        <v>102150439.789</v>
       </c>
       <c r="D33" s="6">
-        <v>9501860354.3999996</v>
+        <v>9079195596.3999996</v>
       </c>
       <c r="E33" s="6">
-        <v>57971605.242200002</v>
+        <v>22140042.7073</v>
       </c>
       <c r="F33" s="6">
-        <v>12104774641.200001</v>
+        <v>12507954174.4</v>
       </c>
       <c r="G33" s="6">
-        <v>45363358.215300001</v>
+        <v>34985071.001500003</v>
       </c>
       <c r="H33" s="6">
         <f t="shared" si="0"/>
-        <v>0.98897833365832521</v>
+        <v>0.93773643745927171</v>
       </c>
       <c r="I33" s="6">
         <f t="shared" si="1"/>
-        <v>1.2598964210645323</v>
+        <v>1.2918726403533398</v>
       </c>
       <c r="J33" s="6">
         <f t="shared" si="2"/>
-        <v>7.6315778823585504E-3</v>
+        <v>1.0550515018160482E-2</v>
       </c>
       <c r="K33" s="6">
         <f t="shared" si="3"/>
-        <v>6.0338354189114467E-3</v>
+        <v>2.2867141205518034E-3</v>
       </c>
       <c r="L33" s="6">
         <f t="shared" si="4"/>
-        <v>4.7215362827489182E-3</v>
+        <v>3.6134011539760784E-3</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B34" s="6">
-        <v>1563931880510</v>
+        <v>1579196789850</v>
       </c>
       <c r="C34" s="6">
-        <v>854308712.37699997</v>
+        <v>17815351085.299999</v>
       </c>
       <c r="D34" s="6">
-        <v>1076152871170</v>
+        <v>1074457425660</v>
       </c>
       <c r="E34" s="6">
-        <v>215388522.50600001</v>
+        <v>757369498.28299999</v>
       </c>
       <c r="F34" s="6">
-        <v>990270689373</v>
+        <v>996257070573</v>
       </c>
       <c r="G34" s="6">
-        <v>439518725.89099997</v>
+        <v>218264110.53299999</v>
       </c>
       <c r="H34" s="6">
         <f t="shared" si="0"/>
-        <v>0.68810725363502745</v>
+        <v>0.68038222504369283</v>
       </c>
       <c r="I34" s="6">
         <f t="shared" si="1"/>
-        <v>0.63319298091811493</v>
+        <v>0.63086315586268982</v>
       </c>
       <c r="J34" s="6">
         <f t="shared" si="2"/>
-        <v>5.4625698409473491E-4</v>
+        <v>1.1281273619478539E-2</v>
       </c>
       <c r="K34" s="6">
         <f t="shared" si="3"/>
-        <v>1.3772244506951388E-4</v>
+        <v>4.7959158931353875E-4</v>
       </c>
       <c r="L34" s="6">
         <f t="shared" si="4"/>
-        <v>2.8103444361507127E-4</v>
+        <v>1.382121037326398E-4</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+      <c r="A35" s="15" t="s">
         <v>40</v>
       </c>
       <c r="B35" s="6">
-        <v>42873465287.800003</v>
+        <v>43080528284.400002</v>
       </c>
       <c r="C35" s="6">
-        <v>8506146.6524400003</v>
+        <v>172680137.38299999</v>
       </c>
       <c r="D35" s="6">
-        <v>20444634090.799999</v>
+        <v>20490251939.599998</v>
       </c>
       <c r="E35" s="6">
-        <v>6658858.1248500003</v>
+        <v>3347136.4973900001</v>
       </c>
       <c r="F35" s="6">
-        <v>19627802173.200001</v>
+        <v>19695167716.799999</v>
       </c>
       <c r="G35" s="6">
-        <v>4395208.3865200002</v>
+        <v>3458974.2125200001</v>
       </c>
       <c r="H35" s="6">
         <f t="shared" si="0"/>
-        <v>0.47685984684372335</v>
+        <v>0.47562675657855791</v>
       </c>
       <c r="I35" s="6">
         <f t="shared" si="1"/>
-        <v>0.45780769157433265</v>
+        <v>0.45717098886950897</v>
       </c>
       <c r="J35" s="6">
         <f t="shared" si="2"/>
-        <v>1.9840119279699312E-4</v>
+        <v>4.0083105815935322E-3</v>
       </c>
       <c r="K35" s="6">
         <f t="shared" si="3"/>
-        <v>1.5531420378900031E-4</v>
+        <v>7.7694880510600431E-5</v>
       </c>
       <c r="L35" s="6">
         <f t="shared" si="4"/>
-        <v>1.025158185142243E-4</v>
+        <v>8.0290895916718314E-5</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
+      <c r="A36" s="15" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="6">
-        <v>22897412817.799999</v>
+        <v>22991226992</v>
       </c>
       <c r="C36" s="6">
-        <v>3508026.8909300002</v>
+        <v>103385613.002</v>
       </c>
       <c r="D36" s="6">
-        <v>10743890735.799999</v>
+        <v>10742157139.4</v>
       </c>
       <c r="E36" s="6">
-        <v>1942872.9863700001</v>
+        <v>1698179.0649699999</v>
       </c>
       <c r="F36" s="6">
-        <v>10553539604.6</v>
+        <v>10573749849.4</v>
       </c>
       <c r="G36" s="6">
-        <v>2829252.8361900002</v>
+        <v>1780264.3950700001</v>
       </c>
       <c r="H36" s="6">
         <f t="shared" si="0"/>
-        <v>0.46921854540037422</v>
+        <v>0.46722852778313345</v>
       </c>
       <c r="I36" s="6">
         <f t="shared" si="1"/>
-        <v>0.46090532972336007</v>
+        <v>0.45990367774104568</v>
       </c>
       <c r="J36" s="6">
         <f t="shared" si="2"/>
-        <v>1.5320625604491565E-4</v>
+        <v>4.4967418675816622E-3</v>
       </c>
       <c r="K36" s="6">
         <f t="shared" si="3"/>
-        <v>8.4851201392484345E-5</v>
+        <v>7.3862045969138413E-5</v>
       </c>
       <c r="L36" s="6">
         <f t="shared" si="4"/>
-        <v>1.2356211851107451E-4</v>
+        <v>7.7432335198528493E-5</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.45">
@@ -5205,42 +5225,42 @@
         <v>22</v>
       </c>
       <c r="B37" s="6">
-        <v>1120133</v>
+        <v>1123007.6000000001</v>
       </c>
       <c r="C37" s="6">
-        <v>687.77583557399998</v>
+        <v>807.77313646799996</v>
       </c>
       <c r="D37" s="6">
-        <v>1163122.6000000001</v>
+        <v>1157807.2</v>
       </c>
       <c r="E37" s="6">
-        <v>2091.8385788599999</v>
+        <v>2195.0648646499999</v>
       </c>
       <c r="F37" s="6">
-        <v>1062673.6000000001</v>
+        <v>1063081.3999999999</v>
       </c>
       <c r="G37" s="6">
-        <v>863.63385760400001</v>
+        <v>870.85626827900001</v>
       </c>
       <c r="H37" s="6">
         <f t="shared" si="0"/>
-        <v>1.0383790139206683</v>
+        <v>1.0309878579628489</v>
       </c>
       <c r="I37" s="6">
         <f t="shared" si="1"/>
-        <v>0.94870305579783842</v>
+        <v>0.94663776095549113</v>
       </c>
       <c r="J37" s="6">
         <f t="shared" si="2"/>
-        <v>6.1401265347418561E-4</v>
+        <v>7.1929445220851563E-4</v>
       </c>
       <c r="K37" s="6">
         <f t="shared" si="3"/>
-        <v>1.8674912522530806E-3</v>
+        <v>1.9546304625632093E-3</v>
       </c>
       <c r="L37" s="6">
         <f t="shared" si="4"/>
-        <v>7.7101010112549137E-4</v>
+        <v>7.7546783145456888E-4</v>
       </c>
     </row>
   </sheetData>
@@ -5258,8 +5278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440270B8-E650-47B8-847B-14A2543F142D}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5343,42 +5363,42 @@
         <v>0</v>
       </c>
       <c r="B5" s="6">
-        <v>10993802.800000001</v>
+        <v>11002545.800000001</v>
       </c>
       <c r="C5" s="6">
-        <v>1773.7289984700001</v>
+        <v>6573.4197918600003</v>
       </c>
       <c r="D5" s="6">
-        <v>11506634.800000001</v>
+        <v>11560332.4</v>
       </c>
       <c r="E5" s="6">
-        <v>6242.3846533200003</v>
+        <v>4256.1293965300001</v>
       </c>
       <c r="F5" s="6">
-        <v>11497720.6</v>
+        <v>10826309.4</v>
       </c>
       <c r="G5" s="6">
-        <v>484210.22772099997</v>
+        <v>467713.26683799998</v>
       </c>
       <c r="H5" s="6">
         <f>D5/B5</f>
-        <v>1.0466473711898852</v>
+        <v>1.0506961397970276</v>
       </c>
       <c r="I5" s="6">
         <f>F5/B5</f>
-        <v>1.0458365325599617</v>
+        <v>0.98398221618854786</v>
       </c>
       <c r="J5" s="6">
         <f>C5/B5</f>
-        <v>1.6133898622140103E-4</v>
+        <v>5.9744534686326863E-4</v>
       </c>
       <c r="K5" s="6">
         <f>E5/B5</f>
-        <v>5.6780940743452303E-4</v>
+        <v>3.8683132739424721E-4</v>
       </c>
       <c r="L5" s="6">
         <f>G5/B5</f>
-        <v>4.4043925157635166E-2</v>
+        <v>4.2509549638775415E-2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
@@ -5386,42 +5406,42 @@
         <v>1</v>
       </c>
       <c r="B6" s="6">
-        <v>216409745713</v>
+        <v>216582537657</v>
       </c>
       <c r="C6" s="6">
-        <v>35294538.0647</v>
+        <v>128529104.082</v>
       </c>
       <c r="D6" s="6">
-        <v>226534065733</v>
+        <v>227593422718</v>
       </c>
       <c r="E6" s="6">
-        <v>124032309.205</v>
+        <v>84028567.334299996</v>
       </c>
       <c r="F6" s="6">
-        <v>226361265032</v>
+        <v>213107200915</v>
       </c>
       <c r="G6" s="6">
-        <v>9553146491.4699993</v>
+        <v>9234321385.5200005</v>
       </c>
       <c r="H6" s="6">
         <f t="shared" ref="H6:H37" si="0">D6/B6</f>
-        <v>1.0467831057545198</v>
+        <v>1.05083920975401</v>
       </c>
       <c r="I6" s="6">
         <f t="shared" ref="I6:I37" si="1">F6/B6</f>
-        <v>1.0459846172186607</v>
+        <v>0.98395375370703309</v>
       </c>
       <c r="J6" s="6">
         <f t="shared" ref="J6:J37" si="2">C6/B6</f>
-        <v>1.6309125981556853E-4</v>
+        <v>5.9344167573449754E-4</v>
       </c>
       <c r="K6" s="6">
         <f t="shared" ref="K6:K37" si="3">E6/B6</f>
-        <v>5.7313643059998852E-4</v>
+        <v>3.8797480278569526E-4</v>
       </c>
       <c r="L6" s="6">
         <f t="shared" ref="L6:L37" si="4">G6/B6</f>
-        <v>4.4143790567266167E-2</v>
+        <v>4.2636500086375012E-2</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
@@ -5429,343 +5449,343 @@
         <v>2</v>
       </c>
       <c r="B7" s="6">
-        <v>262280845319</v>
+        <v>262633995191</v>
       </c>
       <c r="C7" s="6">
-        <v>98838550.429100007</v>
+        <v>34496870.1866</v>
       </c>
       <c r="D7" s="6">
-        <v>232783010668</v>
+        <v>233793698998</v>
       </c>
       <c r="E7" s="6">
-        <v>123231903.88500001</v>
+        <v>89588044.305999994</v>
       </c>
       <c r="F7" s="6">
-        <v>230464705735</v>
+        <v>216708555603</v>
       </c>
       <c r="G7" s="6">
-        <v>9731083983.8999996</v>
+        <v>9381839067.5599995</v>
       </c>
       <c r="H7" s="6">
         <f t="shared" si="0"/>
-        <v>0.88753340101857936</v>
+        <v>0.890188259246386</v>
       </c>
       <c r="I7" s="6">
         <f t="shared" si="1"/>
-        <v>0.87869438370421782</v>
+        <v>0.82513520553726938</v>
       </c>
       <c r="J7" s="6">
         <f t="shared" si="2"/>
-        <v>3.7684242747077954E-4</v>
+        <v>1.3134959989285556E-4</v>
       </c>
       <c r="K7" s="6">
         <f t="shared" si="3"/>
-        <v>4.6984713555852227E-4</v>
+        <v>3.4111366367802951E-4</v>
       </c>
       <c r="L7" s="6">
         <f t="shared" si="4"/>
-        <v>3.7101771469679891E-2</v>
+        <v>3.5722104675508889E-2</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="6">
-        <v>128350330.8</v>
+        <v>128461687.8</v>
       </c>
       <c r="C8" s="6">
-        <v>22670.2774522</v>
+        <v>39195.649985199998</v>
       </c>
       <c r="D8" s="6">
-        <v>73650716.200000003</v>
+        <v>73754798.799999997</v>
       </c>
       <c r="E8" s="6">
-        <v>49848.839623</v>
+        <v>36422.227243300003</v>
       </c>
       <c r="F8" s="6">
-        <v>14298501.800000001</v>
+        <v>13394536.6</v>
       </c>
       <c r="G8" s="6">
-        <v>617578.60468800005</v>
+        <v>558742.90630899998</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" si="0"/>
-        <v>0.57382568273053491</v>
+        <v>0.5741384848907457</v>
       </c>
       <c r="I8" s="6">
         <f t="shared" si="1"/>
-        <v>0.11140214217507885</v>
+        <v>0.10426872657047559</v>
       </c>
       <c r="J8" s="6">
         <f t="shared" si="2"/>
-        <v>1.7662811861019373E-4</v>
+        <v>3.0511548350682654E-4</v>
       </c>
       <c r="K8" s="6">
         <f t="shared" si="3"/>
-        <v>3.8838107632676238E-4</v>
+        <v>2.8352599025481594E-4</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" si="4"/>
-        <v>4.811663521540375E-3</v>
+        <v>4.3494906215065313E-3</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="A9" s="15" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="6">
-        <v>96803733.599999994</v>
+        <v>96630828.400000006</v>
       </c>
       <c r="C9" s="6">
-        <v>20212.253249900001</v>
+        <v>40839.880179100001</v>
       </c>
       <c r="D9" s="6">
-        <v>55276355.600000001</v>
+        <v>55614656</v>
       </c>
       <c r="E9" s="6">
-        <v>33047.157951000001</v>
+        <v>5659.3818037000001</v>
       </c>
       <c r="F9" s="6">
-        <v>7311102.5999999996</v>
+        <v>7250000.4000000004</v>
       </c>
       <c r="G9" s="6">
-        <v>18140.853691</v>
+        <v>12245.774089</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" si="0"/>
-        <v>0.57101470722612713</v>
+        <v>0.57553740271981357</v>
       </c>
       <c r="I9" s="6">
         <f t="shared" si="1"/>
-        <v>7.5525006403265427E-2</v>
+        <v>7.502782000366251E-2</v>
       </c>
       <c r="J9" s="6">
         <f t="shared" si="2"/>
-        <v>2.0879621578872659E-4</v>
+        <v>4.2263820827494837E-4</v>
       </c>
       <c r="K9" s="6">
         <f t="shared" si="3"/>
-        <v>3.4138309259385842E-4</v>
+        <v>5.8567042189405463E-5</v>
       </c>
       <c r="L9" s="6">
         <f t="shared" si="4"/>
-        <v>1.8739828533844899E-4</v>
+        <v>1.2672740461573028E-4</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="6">
-        <v>5006461781.8000002</v>
+        <v>5039203216.8000002</v>
       </c>
       <c r="C10" s="6">
-        <v>6887086.4564300003</v>
+        <v>17011315.443100002</v>
       </c>
       <c r="D10" s="6">
-        <v>2566553087</v>
+        <v>2507936418</v>
       </c>
       <c r="E10" s="6">
-        <v>3096266.9693800001</v>
+        <v>12601889.833799999</v>
       </c>
       <c r="F10" s="6">
-        <v>455642359</v>
+        <v>446099674.39999998</v>
       </c>
       <c r="G10" s="6">
-        <v>3153803.81819</v>
+        <v>7846216.0669</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" si="0"/>
-        <v>0.51264809337608352</v>
+        <v>0.49768511213020544</v>
       </c>
       <c r="I10" s="6">
         <f t="shared" si="1"/>
-        <v>9.1010853344850748E-2</v>
+        <v>8.8525835376665488E-2</v>
       </c>
       <c r="J10" s="6">
         <f t="shared" si="2"/>
-        <v>1.3756394748615955E-3</v>
+        <v>3.3757946864271418E-3</v>
       </c>
       <c r="K10" s="6">
         <f t="shared" si="3"/>
-        <v>6.1845413074676113E-4</v>
+        <v>2.5007703185668437E-3</v>
       </c>
       <c r="L10" s="6">
         <f t="shared" si="4"/>
-        <v>6.2994664808089195E-4</v>
+        <v>1.5570350568006089E-3</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="17" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="6">
-        <v>48028447.200000003</v>
+        <v>48085307</v>
       </c>
       <c r="C11" s="6">
-        <v>14656.2248263</v>
+        <v>28597.1906452</v>
       </c>
       <c r="D11" s="6">
-        <v>52979508.600000001</v>
+        <v>53083900.600000001</v>
       </c>
       <c r="E11" s="6">
-        <v>34795.673769000001</v>
+        <v>25807.052420600001</v>
       </c>
       <c r="F11" s="6">
-        <v>13811065.800000001</v>
+        <v>13844000.800000001</v>
       </c>
       <c r="G11" s="6">
-        <v>11879.022643300001</v>
+        <v>11183.2337971</v>
       </c>
       <c r="H11" s="6">
         <f t="shared" si="0"/>
-        <v>1.1030860185710938</v>
+        <v>1.1039526190401572</v>
       </c>
       <c r="I11" s="6">
         <f t="shared" si="1"/>
-        <v>0.28756011499784651</v>
+        <v>0.28790501015206166</v>
       </c>
       <c r="J11" s="6">
         <f t="shared" si="2"/>
-        <v>3.0515716582025994E-4</v>
+        <v>5.9471785519015191E-4</v>
       </c>
       <c r="K11" s="6">
         <f t="shared" si="3"/>
-        <v>7.2448050681513598E-4</v>
+        <v>5.3669309880042984E-4</v>
       </c>
       <c r="L11" s="6">
         <f t="shared" si="4"/>
-        <v>2.4733305646616868E-4</v>
+        <v>2.3257070599757218E-4</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="6">
-        <v>78414325.200000003</v>
+        <v>78557918.599999994</v>
       </c>
       <c r="C12" s="6">
-        <v>27868.809327999999</v>
+        <v>50822.754374800003</v>
       </c>
       <c r="D12" s="6">
-        <v>55528342</v>
+        <v>55750789</v>
       </c>
       <c r="E12" s="6">
-        <v>18977.7241417</v>
+        <v>40786.507793600002</v>
       </c>
       <c r="F12" s="6">
-        <v>32812194.800000001</v>
+        <v>32844615.600000001</v>
       </c>
       <c r="G12" s="6">
-        <v>27211.579758600001</v>
+        <v>20655.4121682</v>
       </c>
       <c r="H12" s="6">
         <f t="shared" si="0"/>
-        <v>0.70814027740941399</v>
+        <v>0.70967752192966072</v>
       </c>
       <c r="I12" s="6">
         <f t="shared" si="1"/>
-        <v>0.41844643458080794</v>
+        <v>0.41809426962083496</v>
       </c>
       <c r="J12" s="6">
         <f t="shared" si="2"/>
-        <v>3.5540456742972774E-4</v>
+        <v>6.4694629491876586E-4</v>
       </c>
       <c r="K12" s="6">
         <f t="shared" si="3"/>
-        <v>2.420185864419069E-4</v>
+        <v>5.1919028050216197E-4</v>
       </c>
       <c r="L12" s="6">
         <f t="shared" si="4"/>
-        <v>3.4702306867011079E-4</v>
+        <v>2.6293227387264311E-4</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+      <c r="A13" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="6">
-        <v>46688745.399999999</v>
+        <v>46745239.200000003</v>
       </c>
       <c r="C13" s="6">
-        <v>49011.521354099998</v>
+        <v>12353.4471691</v>
       </c>
       <c r="D13" s="6">
-        <v>31882429.600000001</v>
+        <v>31998845.199999999</v>
       </c>
       <c r="E13" s="6">
-        <v>7196.4395530000002</v>
+        <v>13433.428309999999</v>
       </c>
       <c r="F13" s="6">
-        <v>12104994.800000001</v>
+        <v>12127936</v>
       </c>
       <c r="G13" s="6">
-        <v>8342.8682453900001</v>
+        <v>17957.665850500001</v>
       </c>
       <c r="H13" s="6">
         <f t="shared" si="0"/>
-        <v>0.68287184260042255</v>
+        <v>0.68453698703075627</v>
       </c>
       <c r="I13" s="6">
         <f t="shared" si="1"/>
-        <v>0.25927008096473719</v>
+        <v>0.25944751182276543</v>
       </c>
       <c r="J13" s="6">
         <f t="shared" si="2"/>
-        <v>1.0497502328280597E-3</v>
+        <v>2.6427177142565567E-4</v>
       </c>
       <c r="K13" s="6">
         <f t="shared" si="3"/>
-        <v>1.5413649459511928E-4</v>
+        <v>2.8737532505770122E-4</v>
       </c>
       <c r="L13" s="6">
         <f t="shared" si="4"/>
-        <v>1.7869120649770126E-4</v>
+        <v>3.8416031574184351E-4</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="6">
-        <v>2608042481.8000002</v>
+        <v>2646392046.1999998</v>
       </c>
       <c r="C14" s="6">
-        <v>4278606.0653799996</v>
+        <v>5413605.6002399996</v>
       </c>
       <c r="D14" s="6">
-        <v>1687621141.5999999</v>
+        <v>1684327798.2</v>
       </c>
       <c r="E14" s="6">
-        <v>2627662.3417400001</v>
+        <v>4267263.9938300001</v>
       </c>
       <c r="F14" s="6">
-        <v>803254084.60000002</v>
+        <v>815922082.60000002</v>
       </c>
       <c r="G14" s="6">
-        <v>4322649.3069700003</v>
+        <v>5208404.7201500004</v>
       </c>
       <c r="H14" s="6">
         <f t="shared" si="0"/>
-        <v>0.64708345564802672</v>
+        <v>0.63646193337776824</v>
       </c>
       <c r="I14" s="6">
         <f t="shared" si="1"/>
-        <v>0.30799118120407909</v>
+        <v>0.30831489377078375</v>
       </c>
       <c r="J14" s="6">
         <f t="shared" si="2"/>
-        <v>1.640543087483384E-3</v>
+        <v>2.0456551809900918E-3</v>
       </c>
       <c r="K14" s="6">
         <f t="shared" si="3"/>
-        <v>1.0075228298913517E-3</v>
+        <v>1.6124836831932889E-3</v>
       </c>
       <c r="L14" s="6">
         <f t="shared" si="4"/>
-        <v>1.657430558411236E-3</v>
+        <v>1.9681153167116108E-3</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.45">
@@ -5773,42 +5793,42 @@
         <v>32</v>
       </c>
       <c r="B15" s="6">
-        <v>1029766540.6</v>
+        <v>1039073381.6</v>
       </c>
       <c r="C15" s="6">
-        <v>2565880.0191899999</v>
+        <v>657280.95011800004</v>
       </c>
       <c r="D15" s="6">
-        <v>1077653752.2</v>
+        <v>1085816176.4000001</v>
       </c>
       <c r="E15" s="6">
-        <v>1482132.35543</v>
+        <v>810893.06372099998</v>
       </c>
       <c r="F15" s="6">
-        <v>422390470.19999999</v>
+        <v>417164919.39999998</v>
       </c>
       <c r="G15" s="6">
-        <v>136864.071249</v>
+        <v>433330.514104</v>
       </c>
       <c r="H15" s="6">
         <f t="shared" si="0"/>
-        <v>1.0465029787937159</v>
+        <v>1.0449850757682042</v>
       </c>
       <c r="I15" s="6">
         <f t="shared" si="1"/>
-        <v>0.41018080656795425</v>
+        <v>0.40147782320978664</v>
       </c>
       <c r="J15" s="6">
         <f t="shared" si="2"/>
-        <v>2.4917104198151296E-3</v>
+        <v>6.3256451542036119E-4</v>
       </c>
       <c r="K15" s="6">
         <f t="shared" si="3"/>
-        <v>1.4392896807138694E-3</v>
+        <v>7.8040018932287497E-4</v>
       </c>
       <c r="L15" s="6">
         <f t="shared" si="4"/>
-        <v>1.3290786392152078E-4</v>
+        <v>4.1703552586126605E-4</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.45">
@@ -5816,42 +5836,42 @@
         <v>7</v>
       </c>
       <c r="B16" s="6">
-        <v>49756746.399999999</v>
+        <v>49825737.399999999</v>
       </c>
       <c r="C16" s="6">
-        <v>50574.352984899997</v>
+        <v>13253.092206699999</v>
       </c>
       <c r="D16" s="6">
-        <v>52434312.600000001</v>
+        <v>52775401.200000003</v>
       </c>
       <c r="E16" s="6">
-        <v>14407.533732</v>
+        <v>15213.783834399999</v>
       </c>
       <c r="F16" s="6">
-        <v>47007363.799999997</v>
+        <v>47038271.799999997</v>
       </c>
       <c r="G16" s="6">
-        <v>10735.658739</v>
+        <v>17094.539928300001</v>
       </c>
       <c r="H16" s="6">
         <f t="shared" si="0"/>
-        <v>1.0538131287458941</v>
+        <v>1.0591996015296303</v>
       </c>
       <c r="I16" s="6">
         <f t="shared" si="1"/>
-        <v>0.94474352125242655</v>
+        <v>0.94405570804457373</v>
       </c>
       <c r="J16" s="6">
         <f t="shared" si="2"/>
-        <v>1.0164320749256226E-3</v>
+        <v>2.6598888241842657E-4</v>
       </c>
       <c r="K16" s="6">
         <f t="shared" si="3"/>
-        <v>2.8955940197890432E-4</v>
+        <v>3.0533986305639703E-4</v>
       </c>
       <c r="L16" s="6">
         <f t="shared" si="4"/>
-        <v>2.1576287671012188E-4</v>
+        <v>3.4308654162135897E-4</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
@@ -5859,42 +5879,42 @@
         <v>37</v>
       </c>
       <c r="B17" s="6">
-        <v>40443157.799999997</v>
+        <v>40402749.799999997</v>
       </c>
       <c r="C17" s="6">
-        <v>39378.278516999999</v>
+        <v>16195.590553</v>
       </c>
       <c r="D17" s="6">
-        <v>42567336.200000003</v>
+        <v>42893098.600000001</v>
       </c>
       <c r="E17" s="6">
-        <v>28097.415812800002</v>
+        <v>40434.638173699997</v>
       </c>
       <c r="F17" s="6">
-        <v>37941717.399999999</v>
+        <v>38035704.399999999</v>
       </c>
       <c r="G17" s="6">
-        <v>64778.036835300001</v>
+        <v>26843.1155688</v>
       </c>
       <c r="H17" s="6">
         <f t="shared" si="0"/>
-        <v>1.0525225653868207</v>
+        <v>1.0616381016719809</v>
       </c>
       <c r="I17" s="6">
         <f t="shared" si="1"/>
-        <v>0.93814923126502259</v>
+        <v>0.94141375496179724</v>
       </c>
       <c r="J17" s="6">
         <f t="shared" si="2"/>
-        <v>9.7366972954322578E-4</v>
+        <v>4.0085367043507519E-4</v>
       </c>
       <c r="K17" s="6">
         <f t="shared" si="3"/>
-        <v>6.9473842650338261E-4</v>
+        <v>1.0007892624600517E-3</v>
       </c>
       <c r="L17" s="6">
         <f t="shared" si="4"/>
-        <v>1.6017057113997168E-3</v>
+        <v>6.6438833251889211E-4</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.45">
@@ -5902,42 +5922,42 @@
         <v>8</v>
       </c>
       <c r="B18" s="6">
-        <v>1647632761.4000001</v>
+        <v>1674362490</v>
       </c>
       <c r="C18" s="6">
-        <v>7625281.1434800001</v>
+        <v>4431275.8451300003</v>
       </c>
       <c r="D18" s="6">
-        <v>1659695489.8</v>
+        <v>1649736121.2</v>
       </c>
       <c r="E18" s="6">
-        <v>7947517.3408000004</v>
+        <v>14836747.9476</v>
       </c>
       <c r="F18" s="6">
-        <v>1520164122.4000001</v>
+        <v>1517711724.4000001</v>
       </c>
       <c r="G18" s="6">
-        <v>7301986.9838899998</v>
+        <v>14123708.362299999</v>
       </c>
       <c r="H18" s="6">
         <f t="shared" si="0"/>
-        <v>1.0073212482068821</v>
+        <v>0.98529209239511817</v>
       </c>
       <c r="I18" s="6">
         <f t="shared" si="1"/>
-        <v>0.92263528500629632</v>
+        <v>0.90644154623889128</v>
       </c>
       <c r="J18" s="6">
         <f t="shared" si="2"/>
-        <v>4.6280222887779728E-3</v>
+        <v>2.6465451009536176E-3</v>
       </c>
       <c r="K18" s="6">
         <f t="shared" si="3"/>
-        <v>4.823597543694727E-3</v>
+        <v>8.8611325422131258E-3</v>
       </c>
       <c r="L18" s="6">
         <f t="shared" si="4"/>
-        <v>4.431804923377144E-3</v>
+        <v>8.435275184825718E-3</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
@@ -5945,42 +5965,42 @@
         <v>33</v>
       </c>
       <c r="B19" s="6">
-        <v>248860750.40000001</v>
+        <v>249333879</v>
       </c>
       <c r="C19" s="6">
-        <v>360608.92223899998</v>
+        <v>156368.42799699999</v>
       </c>
       <c r="D19" s="6">
-        <v>258500446.40000001</v>
+        <v>258588558.19999999</v>
       </c>
       <c r="E19" s="6">
-        <v>468561.58675399999</v>
+        <v>347397.77240999998</v>
       </c>
       <c r="F19" s="6">
-        <v>152979552.40000001</v>
+        <v>152590375.59999999</v>
       </c>
       <c r="G19" s="6">
-        <v>368523.96054300002</v>
+        <v>40210.605026999998</v>
       </c>
       <c r="H19" s="6">
         <f t="shared" si="0"/>
-        <v>1.0387353007033286</v>
+        <v>1.0371176160942011</v>
       </c>
       <c r="I19" s="6">
         <f t="shared" si="1"/>
-        <v>0.61471948531101106</v>
+        <v>0.61199214568029081</v>
       </c>
       <c r="J19" s="6">
         <f t="shared" si="2"/>
-        <v>1.44903895716534E-3</v>
+        <v>6.2714472908432953E-4</v>
       </c>
       <c r="K19" s="6">
         <f t="shared" si="3"/>
-        <v>1.8828263838346121E-3</v>
+        <v>1.3933035245884094E-3</v>
       </c>
       <c r="L19" s="6">
         <f t="shared" si="4"/>
-        <v>1.4808440461208223E-3</v>
+        <v>1.6127212711033144E-4</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.45">
@@ -5988,42 +6008,42 @@
         <v>38</v>
       </c>
       <c r="B20" s="6">
-        <v>21592205.800000001</v>
+        <v>21662034.199999999</v>
       </c>
       <c r="C20" s="6">
-        <v>10532.0337143</v>
+        <v>9819.9218001000008</v>
       </c>
       <c r="D20" s="6">
-        <v>21157315.800000001</v>
+        <v>21259836.800000001</v>
       </c>
       <c r="E20" s="6">
-        <v>10726.5268265</v>
+        <v>11347.152601399999</v>
       </c>
       <c r="F20" s="6">
-        <v>4130390</v>
+        <v>4149866</v>
       </c>
       <c r="G20" s="6">
-        <v>9405.1766384300008</v>
+        <v>9073.3799655900002</v>
       </c>
       <c r="H20" s="6">
         <f t="shared" si="0"/>
-        <v>0.97985893594993434</v>
+        <v>0.98143307335374819</v>
       </c>
       <c r="I20" s="6">
         <f t="shared" si="1"/>
-        <v>0.19129078512210179</v>
+        <v>0.19157323645994428</v>
       </c>
       <c r="J20" s="6">
         <f t="shared" si="2"/>
-        <v>4.8777016168954814E-4</v>
+        <v>4.5332408348335083E-4</v>
       </c>
       <c r="K20" s="6">
         <f t="shared" si="3"/>
-        <v>4.9677772275123462E-4</v>
+        <v>5.238267328282586E-4</v>
       </c>
       <c r="L20" s="6">
         <f t="shared" si="4"/>
-        <v>4.3558202091747387E-4</v>
+        <v>4.1886093807339664E-4</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.45">
@@ -6031,42 +6051,42 @@
         <v>39</v>
       </c>
       <c r="B21" s="6">
-        <v>10140875</v>
+        <v>10160149.6</v>
       </c>
       <c r="C21" s="6">
-        <v>2601.2293247600001</v>
+        <v>2754.4167876299998</v>
       </c>
       <c r="D21" s="6">
-        <v>10509476.800000001</v>
+        <v>10570695.6</v>
       </c>
       <c r="E21" s="6">
-        <v>2335.2011819099998</v>
+        <v>1450.00891032</v>
       </c>
       <c r="F21" s="6">
-        <v>8718003.8000000007</v>
+        <v>8736458.8000000007</v>
       </c>
       <c r="G21" s="6">
-        <v>3251.50915115</v>
+        <v>2317.8196133400002</v>
       </c>
       <c r="H21" s="6">
         <f t="shared" si="0"/>
-        <v>1.0363481257781011</v>
+        <v>1.040407475889922</v>
       </c>
       <c r="I21" s="6">
         <f t="shared" si="1"/>
-        <v>0.85968950411083866</v>
+        <v>0.85987501601354388</v>
       </c>
       <c r="J21" s="6">
         <f t="shared" si="2"/>
-        <v>2.5650935691052303E-4</v>
+        <v>2.7110002274277536E-4</v>
       </c>
       <c r="K21" s="6">
         <f t="shared" si="3"/>
-        <v>2.3027610358179149E-4</v>
+        <v>1.4271531103439658E-4</v>
       </c>
       <c r="L21" s="6">
         <f t="shared" si="4"/>
-        <v>3.2063398386726985E-4</v>
+        <v>2.2812849264936024E-4</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.45">
@@ -6074,42 +6094,42 @@
         <v>9</v>
       </c>
       <c r="B22" s="6">
-        <v>19383918445.799999</v>
+        <v>19314200096.400002</v>
       </c>
       <c r="C22" s="6">
-        <v>62997973.089599997</v>
+        <v>13028476.924000001</v>
       </c>
       <c r="D22" s="6">
-        <v>18800933710.599998</v>
+        <v>18467477105.599998</v>
       </c>
       <c r="E22" s="6">
-        <v>26704578.8662</v>
+        <v>11495438.2388</v>
       </c>
       <c r="F22" s="6">
-        <v>16532536728</v>
+        <v>16333005477</v>
       </c>
       <c r="G22" s="6">
-        <v>19505318.508400001</v>
+        <v>23728707.5559</v>
       </c>
       <c r="H22" s="6">
         <f t="shared" si="0"/>
-        <v>0.96992430932733731</v>
+        <v>0.95616059756169636</v>
       </c>
       <c r="I22" s="6">
         <f t="shared" si="1"/>
-        <v>0.85289962265509733</v>
+        <v>0.845647523349638</v>
       </c>
       <c r="J22" s="6">
         <f t="shared" si="2"/>
-        <v>3.2500122854803928E-3</v>
+        <v>6.7455431024701846E-4</v>
       </c>
       <c r="K22" s="6">
         <f t="shared" si="3"/>
-        <v>1.3776666952489268E-3</v>
+        <v>5.9518065368612655E-4</v>
       </c>
       <c r="L22" s="6">
         <f t="shared" si="4"/>
-        <v>1.0062629268142791E-3</v>
+        <v>1.228562789940383E-3</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.45">
@@ -6117,42 +6137,42 @@
         <v>10</v>
       </c>
       <c r="B23" s="6">
-        <v>266567566.19999999</v>
+        <v>266882992.59999999</v>
       </c>
       <c r="C23" s="6">
-        <v>1189484.3162100001</v>
+        <v>407783.32533600001</v>
       </c>
       <c r="D23" s="6">
-        <v>266712849.40000001</v>
+        <v>265883203</v>
       </c>
       <c r="E23" s="6">
-        <v>695704.353581</v>
+        <v>369115.35095499997</v>
       </c>
       <c r="F23" s="6">
-        <v>224736287.80000001</v>
+        <v>224600323.80000001</v>
       </c>
       <c r="G23" s="6">
-        <v>540123.93872800004</v>
+        <v>457135.46983800002</v>
       </c>
       <c r="H23" s="6">
         <f t="shared" si="0"/>
-        <v>1.000545014541983</v>
+        <v>0.99625382797809647</v>
       </c>
       <c r="I23" s="6">
         <f t="shared" si="1"/>
-        <v>0.84307438824491177</v>
+        <v>0.84156851514561448</v>
       </c>
       <c r="J23" s="6">
         <f t="shared" si="2"/>
-        <v>4.4622244677642265E-3</v>
+        <v>1.5279479646242546E-3</v>
       </c>
       <c r="K23" s="6">
         <f t="shared" si="3"/>
-        <v>2.6098612201719538E-3</v>
+        <v>1.3830605965522284E-3</v>
       </c>
       <c r="L23" s="6">
         <f t="shared" si="4"/>
-        <v>2.0262177669535253E-3</v>
+        <v>1.7128684948581471E-3</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.45">
@@ -6160,42 +6180,42 @@
         <v>11</v>
       </c>
       <c r="B24" s="6">
-        <v>106382030.59999999</v>
+        <v>105071315.8</v>
       </c>
       <c r="C24" s="6">
-        <v>405252.46255200001</v>
+        <v>263536.04715400003</v>
       </c>
       <c r="D24" s="6">
-        <v>110517831.8</v>
+        <v>109889123.8</v>
       </c>
       <c r="E24" s="6">
-        <v>149226.160221</v>
+        <v>578201.78486899997</v>
       </c>
       <c r="F24" s="6">
-        <v>102124974.59999999</v>
+        <v>100617335.2</v>
       </c>
       <c r="G24" s="6">
-        <v>342877.11550199997</v>
+        <v>300773.542051</v>
       </c>
       <c r="H24" s="6">
         <f t="shared" si="0"/>
-        <v>1.0388768777647304</v>
+        <v>1.0458527426188375</v>
       </c>
       <c r="I24" s="6">
         <f t="shared" si="1"/>
-        <v>0.95998331695691475</v>
+        <v>0.95760992839874581</v>
       </c>
       <c r="J24" s="6">
         <f t="shared" si="2"/>
-        <v>3.8094070987962515E-3</v>
+        <v>2.5081635758291325E-3</v>
       </c>
       <c r="K24" s="6">
         <f t="shared" si="3"/>
-        <v>1.4027384077870762E-3</v>
+        <v>5.5029460749267591E-3</v>
       </c>
       <c r="L24" s="6">
         <f t="shared" si="4"/>
-        <v>3.2230736109111267E-3</v>
+        <v>2.8625656751411883E-3</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.45">
@@ -6203,42 +6223,42 @@
         <v>12</v>
       </c>
       <c r="B25" s="6">
-        <v>681044917</v>
+        <v>680378845.60000002</v>
       </c>
       <c r="C25" s="6">
-        <v>1831684.5776899999</v>
+        <v>297553.14436600002</v>
       </c>
       <c r="D25" s="6">
-        <v>730846103.60000002</v>
+        <v>730600031.60000002</v>
       </c>
       <c r="E25" s="6">
-        <v>292445.63308499998</v>
+        <v>289377.389257</v>
       </c>
       <c r="F25" s="6">
-        <v>701091829.39999998</v>
+        <v>701939210.39999998</v>
       </c>
       <c r="G25" s="6">
-        <v>986734.37677099998</v>
+        <v>310710.20237399999</v>
       </c>
       <c r="H25" s="6">
         <f t="shared" si="0"/>
-        <v>1.073124672627136</v>
+        <v>1.0738135618483433</v>
       </c>
       <c r="I25" s="6">
         <f t="shared" si="1"/>
-        <v>1.0294355216515036</v>
+        <v>1.0316887641928179</v>
       </c>
       <c r="J25" s="6">
         <f t="shared" si="2"/>
-        <v>2.6895209581161883E-3</v>
+        <v>4.3733450310848407E-4</v>
       </c>
       <c r="K25" s="6">
         <f t="shared" si="3"/>
-        <v>4.2940726196624707E-4</v>
+        <v>4.2531802851955103E-4</v>
       </c>
       <c r="L25" s="6">
         <f t="shared" si="4"/>
-        <v>1.4488535956153389E-3</v>
+        <v>4.5667234421434218E-4</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.45">
@@ -6246,42 +6266,42 @@
         <v>13</v>
       </c>
       <c r="B26" s="6">
-        <v>1052021345.6</v>
+        <v>1053381920.8</v>
       </c>
       <c r="C26" s="6">
-        <v>2691768.0032799998</v>
+        <v>800804.47900799999</v>
       </c>
       <c r="D26" s="6">
-        <v>1107875374.4000001</v>
+        <v>1107315281.8</v>
       </c>
       <c r="E26" s="6">
-        <v>1804958.78773</v>
+        <v>456946.26999499998</v>
       </c>
       <c r="F26" s="6">
-        <v>1023622309.4</v>
+        <v>1025596072.6</v>
       </c>
       <c r="G26" s="6">
-        <v>1008649.9608999999</v>
+        <v>860153.97551000002</v>
       </c>
       <c r="H26" s="6">
         <f t="shared" si="0"/>
-        <v>1.0530921060048879</v>
+        <v>1.0512001961824442</v>
       </c>
       <c r="I26" s="6">
         <f t="shared" si="1"/>
-        <v>0.97300526617755723</v>
+        <v>0.9736222469255047</v>
       </c>
       <c r="J26" s="6">
         <f t="shared" si="2"/>
-        <v>2.5586629154799156E-3</v>
+        <v>7.6022234974359743E-4</v>
       </c>
       <c r="K26" s="6">
         <f t="shared" si="3"/>
-        <v>1.7157054800067547E-3</v>
+        <v>4.3378974042763919E-4</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="4"/>
-        <v>9.5877328451423769E-4</v>
+        <v>8.1656420954780455E-4</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
@@ -6289,42 +6309,42 @@
         <v>14</v>
       </c>
       <c r="B27" s="6">
-        <v>1374861547.8</v>
+        <v>1383045355.2</v>
       </c>
       <c r="C27" s="6">
-        <v>2302629.2171299998</v>
+        <v>2988266.1227600002</v>
       </c>
       <c r="D27" s="6">
-        <v>1424919565.2</v>
+        <v>1433890951.4000001</v>
       </c>
       <c r="E27" s="6">
-        <v>4422678.1181399999</v>
+        <v>1344823.8539100001</v>
       </c>
       <c r="F27" s="6">
-        <v>1273182891.2</v>
+        <v>1278667054.5999999</v>
       </c>
       <c r="G27" s="6">
-        <v>1206884.79522</v>
+        <v>1421388.46594</v>
       </c>
       <c r="H27" s="6">
         <f t="shared" si="0"/>
-        <v>1.0364094969999713</v>
+        <v>1.0367635059897564</v>
       </c>
       <c r="I27" s="6">
         <f t="shared" si="1"/>
-        <v>0.92604443933812675</v>
+        <v>0.92453009569964095</v>
       </c>
       <c r="J27" s="6">
         <f t="shared" si="2"/>
-        <v>1.6748080712669414E-3</v>
+        <v>2.1606421738265204E-3</v>
       </c>
       <c r="K27" s="6">
         <f t="shared" si="3"/>
-        <v>3.2168170862127881E-3</v>
+        <v>9.7236424594009585E-4</v>
       </c>
       <c r="L27" s="6">
         <f t="shared" si="4"/>
-        <v>8.7782278670256659E-4</v>
+        <v>1.0277236828104277E-3</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.45">
@@ -6332,128 +6352,128 @@
         <v>15</v>
       </c>
       <c r="B28" s="6">
-        <v>2425734372.4000001</v>
+        <v>2435264439</v>
       </c>
       <c r="C28" s="6">
-        <v>4744448.9778300002</v>
+        <v>3760078.2648399998</v>
       </c>
       <c r="D28" s="6">
-        <v>2531609439.5999999</v>
+        <v>2539976353</v>
       </c>
       <c r="E28" s="6">
-        <v>6114149.9741200004</v>
+        <v>1586279.22544</v>
       </c>
       <c r="F28" s="6">
-        <v>2295709162.4000001</v>
+        <v>2303131171.1999998</v>
       </c>
       <c r="G28" s="6">
-        <v>1941376.0869499999</v>
+        <v>2209589.6585599999</v>
       </c>
       <c r="H28" s="6">
         <f t="shared" si="0"/>
-        <v>1.0436466038510424</v>
+        <v>1.0429981698591213</v>
       </c>
       <c r="I28" s="6">
         <f t="shared" si="1"/>
-        <v>0.94639758933235785</v>
+        <v>0.94574171671711416</v>
       </c>
       <c r="J28" s="6">
         <f t="shared" si="2"/>
-        <v>1.9558814979135099E-3</v>
+        <v>1.5440123070922073E-3</v>
       </c>
       <c r="K28" s="6">
         <f t="shared" si="3"/>
-        <v>2.5205356545575574E-3</v>
+        <v>6.5137863471261405E-4</v>
       </c>
       <c r="L28" s="6">
         <f t="shared" si="4"/>
-        <v>8.0032509290339966E-4</v>
+        <v>9.0733048254395339E-4</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B29" s="6">
-        <v>823052495.20000005</v>
+        <v>834676881</v>
       </c>
       <c r="C29" s="6">
-        <v>1504197.41916</v>
+        <v>2432042.3309200001</v>
       </c>
       <c r="D29" s="6">
-        <v>741578725.60000002</v>
+        <v>758239744.60000002</v>
       </c>
       <c r="E29" s="6">
-        <v>1782951.4190400001</v>
+        <v>1964535.52792</v>
       </c>
       <c r="F29" s="6">
-        <v>754718422.60000002</v>
+        <v>760035737.79999995</v>
       </c>
       <c r="G29" s="6">
-        <v>1129625.15515</v>
+        <v>1078473.4463800001</v>
       </c>
       <c r="H29" s="6">
         <f t="shared" si="0"/>
-        <v>0.90101023923121448</v>
+        <v>0.90842308186561604</v>
       </c>
       <c r="I29" s="6">
         <f t="shared" si="1"/>
-        <v>0.91697483089047072</v>
+        <v>0.91057480457518503</v>
       </c>
       <c r="J29" s="6">
         <f t="shared" si="2"/>
-        <v>1.8275838150450942E-3</v>
+        <v>2.9137530777254153E-3</v>
       </c>
       <c r="K29" s="6">
         <f t="shared" si="3"/>
-        <v>2.1662669506964396E-3</v>
+        <v>2.3536479476541296E-3</v>
       </c>
       <c r="L29" s="6">
         <f t="shared" si="4"/>
-        <v>1.3724825108215042E-3</v>
+        <v>1.2920849623724035E-3</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B30" s="6">
-        <v>22418823.800000001</v>
+        <v>23014604.199999999</v>
       </c>
       <c r="C30" s="6">
-        <v>96830.0391065</v>
+        <v>89504.347877399996</v>
       </c>
       <c r="D30" s="6">
-        <v>19659639</v>
+        <v>19450580.600000001</v>
       </c>
       <c r="E30" s="6">
-        <v>73035.239291699996</v>
+        <v>122615.928464</v>
       </c>
       <c r="F30" s="6">
-        <v>17989552.600000001</v>
+        <v>17895330</v>
       </c>
       <c r="G30" s="6">
-        <v>92907.484281099998</v>
+        <v>27670.033277899998</v>
       </c>
       <c r="H30" s="6">
         <f t="shared" si="0"/>
-        <v>0.87692553255180139</v>
+        <v>0.84514078239068746</v>
       </c>
       <c r="I30" s="6">
         <f t="shared" si="1"/>
-        <v>0.80243070557519613</v>
+        <v>0.77756409992920927</v>
       </c>
       <c r="J30" s="6">
         <f t="shared" si="2"/>
-        <v>4.3191400213645464E-3</v>
+        <v>3.8890239910100211E-3</v>
       </c>
       <c r="K30" s="6">
         <f t="shared" si="3"/>
-        <v>3.2577640978515561E-3</v>
+        <v>5.3277443921455753E-3</v>
       </c>
       <c r="L30" s="6">
         <f t="shared" si="4"/>
-        <v>4.1441729998832498E-3</v>
+        <v>1.2022815181805299E-3</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.45">
@@ -6461,42 +6481,42 @@
         <v>18</v>
       </c>
       <c r="B31" s="6">
-        <v>126615263113</v>
+        <v>126656855298</v>
       </c>
       <c r="C31" s="6">
-        <v>80667418.787400007</v>
+        <v>160561026.634</v>
       </c>
       <c r="D31" s="6">
-        <v>122487126746</v>
+        <v>120744289478</v>
       </c>
       <c r="E31" s="6">
-        <v>269928060.46899998</v>
+        <v>144616795.109</v>
       </c>
       <c r="F31" s="6">
-        <v>105825598454</v>
+        <v>104759031280</v>
       </c>
       <c r="G31" s="6">
-        <v>127948118.845</v>
+        <v>79156136.723900005</v>
       </c>
       <c r="H31" s="6">
         <f t="shared" si="0"/>
-        <v>0.96739621854818736</v>
+        <v>0.95331823290505013</v>
       </c>
       <c r="I31" s="6">
         <f t="shared" si="1"/>
-        <v>0.83580443504314406</v>
+        <v>0.82710905014593572</v>
       </c>
       <c r="J31" s="6">
         <f t="shared" si="2"/>
-        <v>6.3710659208129558E-4</v>
+        <v>1.267685244957565E-3</v>
       </c>
       <c r="K31" s="6">
         <f t="shared" si="3"/>
-        <v>2.1318761564164501E-3</v>
+        <v>1.1417999820755348E-3</v>
       </c>
       <c r="L31" s="6">
         <f t="shared" si="4"/>
-        <v>1.0105268172195833E-3</v>
+        <v>6.2496527754190927E-4</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.45">
@@ -6504,85 +6524,85 @@
         <v>19</v>
       </c>
       <c r="B32" s="6">
-        <v>10058070079</v>
+        <v>10005713054.799999</v>
       </c>
       <c r="C32" s="6">
-        <v>9774353.0615599994</v>
+        <v>24222009.424699999</v>
       </c>
       <c r="D32" s="6">
-        <v>9523389940.6000004</v>
+        <v>9239733164.6000004</v>
       </c>
       <c r="E32" s="6">
-        <v>30559799.585999999</v>
+        <v>16534215.9199</v>
       </c>
       <c r="F32" s="6">
-        <v>8212986135.1999998</v>
+        <v>8029807846.6000004</v>
       </c>
       <c r="G32" s="6">
-        <v>15516289.864399999</v>
+        <v>5718257.0913500004</v>
       </c>
       <c r="H32" s="6">
         <f t="shared" si="0"/>
-        <v>0.94684068273531463</v>
+        <v>0.92344574684434522</v>
       </c>
       <c r="I32" s="6">
         <f t="shared" si="1"/>
-        <v>0.81655686137519501</v>
+        <v>0.80252229927260343</v>
       </c>
       <c r="J32" s="6">
         <f t="shared" si="2"/>
-        <v>9.7179210174401487E-4</v>
+        <v>2.4208179159285479E-3</v>
       </c>
       <c r="K32" s="6">
         <f t="shared" si="3"/>
-        <v>3.0383363156123821E-3</v>
+        <v>1.6524775225258044E-3</v>
       </c>
       <c r="L32" s="6">
         <f t="shared" si="4"/>
-        <v>1.5426706855817284E-3</v>
+        <v>5.7149920850536526E-4</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B33" s="6">
-        <v>8579486213.6000004</v>
+        <v>8951417611.6000004</v>
       </c>
       <c r="C33" s="6">
-        <v>43101136.4498</v>
+        <v>22425868.647300001</v>
       </c>
       <c r="D33" s="6">
-        <v>7395381902.8000002</v>
+        <v>7440775666.8000002</v>
       </c>
       <c r="E33" s="6">
-        <v>35551208.384300001</v>
+        <v>31201246.311999999</v>
       </c>
       <c r="F33" s="6">
-        <v>6774464324.8000002</v>
+        <v>6900349354.3999996</v>
       </c>
       <c r="G33" s="6">
-        <v>35433495.420999996</v>
+        <v>28203355.996599998</v>
       </c>
       <c r="H33" s="6">
         <f t="shared" si="0"/>
-        <v>0.86198423992767936</v>
+        <v>0.83123992083193798</v>
       </c>
       <c r="I33" s="6">
         <f t="shared" si="1"/>
-        <v>0.78961189005249266</v>
+        <v>0.77086665529468157</v>
       </c>
       <c r="J33" s="6">
         <f t="shared" si="2"/>
-        <v>5.0237433077842224E-3</v>
+        <v>2.5052868294557808E-3</v>
       </c>
       <c r="K33" s="6">
         <f t="shared" si="3"/>
-        <v>4.1437456159023906E-3</v>
+        <v>3.485620676614037E-3</v>
       </c>
       <c r="L33" s="6">
         <f t="shared" si="4"/>
-        <v>4.1300253347142917E-3</v>
+        <v>3.1507139115095821E-3</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.45">
@@ -6590,42 +6610,42 @@
         <v>21</v>
       </c>
       <c r="B34" s="6">
-        <v>2673114564790</v>
+        <v>2677710204530</v>
       </c>
       <c r="C34" s="6">
-        <v>453874716.78899997</v>
+        <v>749247781.51100004</v>
       </c>
       <c r="D34" s="6">
-        <v>2514314023640</v>
+        <v>2522742123210</v>
       </c>
       <c r="E34" s="6">
-        <v>313263102.90899998</v>
+        <v>850770250.56500006</v>
       </c>
       <c r="F34" s="6">
-        <v>2290553200670</v>
+        <v>2294285926740</v>
       </c>
       <c r="G34" s="6">
-        <v>359877898.81999999</v>
+        <v>580801975.39999998</v>
       </c>
       <c r="H34" s="6">
         <f t="shared" si="0"/>
-        <v>0.94059343986161126</v>
+        <v>0.9421266419876827</v>
       </c>
       <c r="I34" s="6">
         <f t="shared" si="1"/>
-        <v>0.85688553376684251</v>
+        <v>0.85680889696676499</v>
       </c>
       <c r="J34" s="6">
         <f t="shared" si="2"/>
-        <v>1.6979246709714307E-4</v>
+        <v>2.7980913701694255E-4</v>
       </c>
       <c r="K34" s="6">
         <f t="shared" si="3"/>
-        <v>1.1719030191794639E-4</v>
+        <v>3.1772304901617605E-4</v>
       </c>
       <c r="L34" s="6">
         <f t="shared" si="4"/>
-        <v>1.3462868504039295E-4</v>
+        <v>2.169024767569813E-4</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.45">
@@ -6633,42 +6653,42 @@
         <v>40</v>
       </c>
       <c r="B35" s="6">
-        <v>52898514759.199997</v>
+        <v>52935579596.199997</v>
       </c>
       <c r="C35" s="6">
-        <v>6143403.5256000003</v>
+        <v>10795234.912</v>
       </c>
       <c r="D35" s="6">
-        <v>55452465741.400002</v>
+        <v>55687440273.599998</v>
       </c>
       <c r="E35" s="6">
-        <v>12948877.342700001</v>
+        <v>22856364.406399999</v>
       </c>
       <c r="F35" s="6">
-        <v>50954489972.400002</v>
+        <v>51104129086.599998</v>
       </c>
       <c r="G35" s="6">
-        <v>6142005.3834199999</v>
+        <v>9761467.5813999996</v>
       </c>
       <c r="H35" s="6">
         <f t="shared" si="0"/>
-        <v>1.0482802020779955</v>
+        <v>1.0519850863708602</v>
       </c>
       <c r="I35" s="6">
         <f t="shared" si="1"/>
-        <v>0.96324991740033883</v>
+        <v>0.96540227719105831</v>
       </c>
       <c r="J35" s="6">
         <f t="shared" si="2"/>
-        <v>1.1613565245764395E-4</v>
+        <v>2.0393155216864652E-4</v>
       </c>
       <c r="K35" s="6">
         <f t="shared" si="3"/>
-        <v>2.4478716277091616E-4</v>
+        <v>4.3177697459348782E-4</v>
       </c>
       <c r="L35" s="6">
         <f t="shared" si="4"/>
-        <v>1.1610922180668211E-4</v>
+        <v>1.8440277136591002E-4</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.45">
@@ -6676,85 +6696,85 @@
         <v>41</v>
       </c>
       <c r="B36" s="6">
-        <v>34314443757</v>
+        <v>34337939790.200001</v>
       </c>
       <c r="C36" s="6">
-        <v>4223643.4217600003</v>
+        <v>6961540.22762</v>
       </c>
       <c r="D36" s="6">
-        <v>35965253851.400002</v>
+        <v>36116679915.800003</v>
       </c>
       <c r="E36" s="6">
-        <v>8417536.2666699998</v>
+        <v>14063332.4827</v>
       </c>
       <c r="F36" s="6">
-        <v>33059567734.799999</v>
+        <v>33156869516.400002</v>
       </c>
       <c r="G36" s="6">
-        <v>3783579.49486</v>
+        <v>6344968.5749300001</v>
       </c>
       <c r="H36" s="6">
         <f t="shared" si="0"/>
-        <v>1.0481083157311342</v>
+        <v>1.0518010147512593</v>
       </c>
       <c r="I36" s="6">
         <f t="shared" si="1"/>
-        <v>0.96343009284700964</v>
+        <v>0.96560450973424228</v>
       </c>
       <c r="J36" s="6">
         <f t="shared" si="2"/>
-        <v>1.2308646037423803E-4</v>
+        <v>2.0273610677151965E-4</v>
       </c>
       <c r="K36" s="6">
         <f t="shared" si="3"/>
-        <v>2.4530592208573564E-4</v>
+        <v>4.0955667604477701E-4</v>
       </c>
       <c r="L36" s="6">
         <f t="shared" si="4"/>
-        <v>1.1026200866473803E-4</v>
+        <v>1.8478011825103278E-4</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B37" s="6">
-        <v>8957.6</v>
+        <v>8994.4</v>
       </c>
       <c r="C37" s="6">
-        <v>69.887337908999996</v>
+        <v>72.712034767299997</v>
       </c>
       <c r="D37" s="6">
-        <v>7938.6</v>
+        <v>8004.4</v>
       </c>
       <c r="E37" s="6">
-        <v>62.755398174200003</v>
+        <v>52.457983186500002</v>
       </c>
       <c r="F37" s="6">
-        <v>7214.6</v>
+        <v>7248.4</v>
       </c>
       <c r="G37" s="6">
-        <v>49.317745285000001</v>
+        <v>57.119523807500002</v>
       </c>
       <c r="H37" s="6">
         <f t="shared" si="0"/>
-        <v>0.8862418504956685</v>
+        <v>0.88993151294138573</v>
       </c>
       <c r="I37" s="6">
         <f t="shared" si="1"/>
-        <v>0.80541662945431813</v>
+        <v>0.80587921373298943</v>
       </c>
       <c r="J37" s="6">
         <f t="shared" si="2"/>
-        <v>7.8020159316111448E-3</v>
+        <v>8.0841451088788582E-3</v>
       </c>
       <c r="K37" s="6">
         <f t="shared" si="3"/>
-        <v>7.0058272499553455E-3</v>
+        <v>5.8322937812972523E-3</v>
       </c>
       <c r="L37" s="6">
         <f t="shared" si="4"/>
-        <v>5.5056873811065461E-3</v>
+        <v>6.3505652191919422E-3</v>
       </c>
     </row>
   </sheetData>
@@ -6773,7 +6793,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Added disk I/O and large pages statistics
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="311" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{6FA119A9-4793-41C0-81C0-A9A7F872C421}"/>
+  <xr:revisionPtr revIDLastSave="339" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{B2AAFDF8-6FB0-4073-A23A-D21F3165E975}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="clang-part2" sheetId="4" r:id="rId5"/>
     <sheet name="clang-part3" sheetId="5" r:id="rId6"/>
     <sheet name="postgres" sheetId="8" r:id="rId7"/>
+    <sheet name="postgres_stats" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="93">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -183,6 +184,129 @@
   </si>
   <si>
     <t>Running "pgbench -j 1 -c 2 -t 4000000 -S pgbench" on the stock freebsd 11.0</t>
+  </si>
+  <si>
+    <t>4GB/2MB * 2 # of super pages for each iteration</t>
+  </si>
+  <si>
+    <t>Before running the experiments</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.promotions: 2856</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.p_failures: 0</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.mappings: 2330</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.demotions: 53</t>
+  </si>
+  <si>
+    <t>vm.reserv.reclaimed: 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vm.reserv.partpopq: </t>
+  </si>
+  <si>
+    <t>LEVEL     SIZE  NUMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 228548K,    127</t>
+  </si>
+  <si>
+    <t>vm.reserv.fullpop: 2173</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 3455</t>
+  </si>
+  <si>
+    <t>vm.reserv.broken: 0</t>
+  </si>
+  <si>
+    <t>After running two rounds of "pgbench -j 1 -c 2 -t 4000000 -S pgbench"</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.promotions: 2906</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.p_failures: 7010</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.mappings: 3400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 231464K,    130</t>
+  </si>
+  <si>
+    <t>vm.reserv.fullpop: 2493</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 3598</t>
+  </si>
+  <si>
+    <t>After running another two rounds of "pgbench -j 1 -c 2 -t 4000000 -S pgbench"</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.promotions: 3003</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.p_failures: 14223</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.mappings: 4470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 236564K,    134</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 3774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extended device statistics  </t>
+  </si>
+  <si>
+    <t>Disk IO statistics generated by "iostat -x -I 300 (INTERVAL in seconds)" when running "pgbench -j 1 -c 2 -T 300 -S pgbench"</t>
+  </si>
+  <si>
+    <t>device</t>
+  </si>
+  <si>
+    <t>r/i</t>
+  </si>
+  <si>
+    <t>w/i</t>
+  </si>
+  <si>
+    <t>kr/i</t>
+  </si>
+  <si>
+    <t>kw/i</t>
+  </si>
+  <si>
+    <t>qlen</t>
+  </si>
+  <si>
+    <t>tsvc_t/i</t>
+  </si>
+  <si>
+    <t>sb/i</t>
+  </si>
+  <si>
+    <t>ada0</t>
+  </si>
+  <si>
+    <t>pass0</t>
+  </si>
+  <si>
+    <t>pass1</t>
+  </si>
+  <si>
+    <t># of writes</t>
+  </si>
+  <si>
+    <t>KB written</t>
   </si>
 </sst>
 </file>
@@ -193,7 +317,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,14 +361,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -278,6 +394,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -300,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -320,30 +467,34 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3829,1507 +3980,1507 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670D2A71-BD87-4620-9FEC-7336DAF0F286}">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="19.46484375" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.9296875" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.46484375" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.46484375" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.46484375" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.06640625" style="16"/>
+    <col min="1" max="1" width="43.33203125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="19.46484375" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.9296875" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.46484375" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.46484375" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.46484375" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.06640625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.65">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17" t="s">
+      <c r="E3" s="24"/>
+      <c r="F3" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18" t="s">
+      <c r="G3" s="24"/>
+      <c r="H3" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
     </row>
     <row r="4" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18" t="s">
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="15" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="16">
         <v>11060181.4</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="16">
         <v>38115.304997300002</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="16">
         <v>11558800.800000001</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="16">
         <v>48028.480735500001</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="16">
         <v>10593137.4</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="16">
         <v>3107.88472116</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="16">
         <f>D5/B5</f>
         <v>1.0450823889741989</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="16">
         <f>F5/B5</f>
         <v>0.95777248282745164</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="16">
         <f>C5/B5</f>
         <v>3.4461735860227393E-3</v>
       </c>
-      <c r="K5" s="19">
+      <c r="K5" s="16">
         <f>E5/B5</f>
         <v>4.3424677225908787E-3</v>
       </c>
-      <c r="L5" s="19">
+      <c r="L5" s="16">
         <f>G5/B5</f>
         <v>2.8099762641867697E-4</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="16">
         <v>158167304127</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="16">
         <v>552804965.96500003</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="16">
         <v>77076505682.800003</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="16">
         <v>342947323.72899997</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="16">
         <v>72706085161.399994</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="16">
         <v>12249880.3443</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="16">
         <f t="shared" ref="H6:H37" si="0">D6/B6</f>
         <v>0.48730997919084235</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="16">
         <f t="shared" ref="I6:I37" si="1">F6/B6</f>
         <v>0.45967834858600637</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="16">
         <f t="shared" ref="J6:J37" si="2">C6/B6</f>
         <v>3.4950647291878151E-3</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="16">
         <f t="shared" ref="K6:K37" si="3">E6/B6</f>
         <v>2.1682567432118041E-3</v>
       </c>
-      <c r="L6" s="19">
+      <c r="L6" s="16">
         <f t="shared" ref="L6:L37" si="4">G6/B6</f>
         <v>7.7448878653605882E-5</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="16">
         <v>138115690601</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="16">
         <v>600091493.84000003</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="16">
         <v>107043986904</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="16">
         <v>643825984.86000001</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="16">
         <v>98269727224</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="16">
         <v>104851095.565</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="16">
         <f t="shared" si="0"/>
         <v>0.77503132655099627</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="16">
         <f t="shared" si="1"/>
         <v>0.71150299286335028</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="16">
         <f t="shared" si="2"/>
         <v>4.3448466371108687E-3</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="16">
         <f t="shared" si="3"/>
         <v>4.6614977781194869E-3</v>
       </c>
-      <c r="L7" s="19">
+      <c r="L7" s="16">
         <f t="shared" si="4"/>
         <v>7.5915412006230694E-4</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="16">
         <v>5427037.7999999998</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="16">
         <v>18018.001169899999</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="16">
         <v>4563338.4000000004</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="16">
         <v>34264.711851100001</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="16">
         <v>4818117.2</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="16">
         <v>3934.6960949999998</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="16">
         <f t="shared" si="0"/>
         <v>0.84085251810849748</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="16">
         <f t="shared" si="1"/>
         <v>0.88779871774617092</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="16">
         <f t="shared" si="2"/>
         <v>3.3200434258814264E-3</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="16">
         <f t="shared" si="3"/>
         <v>6.3137042920725561E-3</v>
       </c>
-      <c r="L8" s="19">
+      <c r="L8" s="16">
         <f t="shared" si="4"/>
         <v>7.2501726356134831E-4</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="16">
         <v>2176628.7999999998</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="16">
         <v>8777.2189992000003</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="16">
         <v>1766594.6</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="16">
         <v>11426.3262968</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="16">
         <v>1619907.4</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="16">
         <v>12149.9388081</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="16">
         <f t="shared" si="0"/>
         <v>0.81161960183564619</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="16">
         <f t="shared" si="1"/>
         <v>0.74422767906038922</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="16">
         <f t="shared" si="2"/>
         <v>4.0324831680992185E-3</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="16">
         <f t="shared" si="3"/>
         <v>5.2495521040611063E-3</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="16">
         <f t="shared" si="4"/>
         <v>5.5819985511999107E-3</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="16">
         <v>153519617</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="16">
         <v>288303.59377699997</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="16">
         <v>131940813.8</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="16">
         <v>277103.72511599999</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="16">
         <v>136084138.59999999</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="16">
         <v>197541.10542499999</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="16">
         <f t="shared" si="0"/>
         <v>0.85943944088917312</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="16">
         <f t="shared" si="1"/>
         <v>0.88642833573510016</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="16">
         <f t="shared" si="2"/>
         <v>1.8779593084641423E-3</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="16">
         <f t="shared" si="3"/>
         <v>1.8050053180890882E-3</v>
       </c>
-      <c r="L10" s="19">
+      <c r="L10" s="16">
         <f t="shared" si="4"/>
         <v>1.2867482950077969E-3</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="16">
         <v>4383215.8</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="16">
         <v>4428.0626644200001</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="16">
         <v>4509902.8</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="16">
         <v>6367.88974151</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="16">
         <v>8433161.5999999996</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="16">
         <v>6668.6516958100001</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="16">
         <f t="shared" si="0"/>
         <v>1.028902752175697</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="16">
         <f t="shared" si="1"/>
         <v>1.9239667825617894</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="16">
         <f t="shared" si="2"/>
         <v>1.0102314981662551E-3</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="16">
         <f t="shared" si="3"/>
         <v>1.4527894660148835E-3</v>
       </c>
-      <c r="L11" s="19">
+      <c r="L11" s="16">
         <f t="shared" si="4"/>
         <v>1.5214062003997158E-3</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="16">
         <v>17775974.600000001</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="16">
         <v>109609.235453</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="16">
         <v>17466646.399999999</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="16">
         <v>26263.132559500002</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="16">
         <v>14177905.199999999</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="16">
         <v>83422.891844900005</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="16">
         <f t="shared" si="0"/>
         <v>0.98259852374001466</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="16">
         <f t="shared" si="1"/>
         <v>0.79758806586053499</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="16">
         <f t="shared" si="2"/>
         <v>6.166144918602662E-3</v>
       </c>
-      <c r="K12" s="19">
+      <c r="K12" s="16">
         <f t="shared" si="3"/>
         <v>1.4774510624863291E-3</v>
       </c>
-      <c r="L12" s="19">
+      <c r="L12" s="16">
         <f t="shared" si="4"/>
         <v>4.6930136727861881E-3</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="16">
         <v>3778745</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="16">
         <v>37023.3373374</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="16">
         <v>3744922.4</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="16">
         <v>90744.508086400005</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="16">
         <v>1685866.6</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="16">
         <v>91067.958599299993</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="16">
         <f t="shared" si="0"/>
         <v>0.99104925047866421</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="16">
         <f t="shared" si="1"/>
         <v>0.44614457974803806</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13" s="16">
         <f t="shared" si="2"/>
         <v>9.7977866559929294E-3</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K13" s="16">
         <f t="shared" si="3"/>
         <v>2.4014456674477904E-2</v>
       </c>
-      <c r="L13" s="19">
+      <c r="L13" s="16">
         <f t="shared" si="4"/>
         <v>2.4100054012456514E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="16">
         <v>469606679.60000002</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="16">
         <v>2704649.26914</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="16">
         <v>465798168.80000001</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="16">
         <v>4047272.3654299998</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="16">
         <v>299984120.60000002</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="16">
         <v>3365377.74603</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="16">
         <f t="shared" si="0"/>
         <v>0.99188999866176519</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="16">
         <f t="shared" si="1"/>
         <v>0.63879866627007831</v>
       </c>
-      <c r="J14" s="19">
+      <c r="J14" s="16">
         <f t="shared" si="2"/>
         <v>5.7593926718498912E-3</v>
       </c>
-      <c r="K14" s="19">
+      <c r="K14" s="16">
         <f t="shared" si="3"/>
         <v>8.6184301485604329E-3</v>
       </c>
-      <c r="L14" s="19">
+      <c r="L14" s="16">
         <f t="shared" si="4"/>
         <v>7.166375378000479E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="22" t="s">
+    <row r="15" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="16">
         <v>643995703.79999995</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="16">
         <v>141094510.22799999</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="16">
         <v>375302332.39999998</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="16">
         <v>16956708.175900001</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="16">
         <v>548955151.20000005</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="16">
         <v>16014400.234200001</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="20">
         <f t="shared" si="0"/>
         <v>0.58277148463175821</v>
       </c>
-      <c r="I15" s="23">
+      <c r="I15" s="20">
         <f t="shared" si="1"/>
         <v>0.85242051765377025</v>
       </c>
-      <c r="J15" s="23">
+      <c r="J15" s="20">
         <f t="shared" si="2"/>
         <v>0.21909231598199988</v>
       </c>
-      <c r="K15" s="23">
+      <c r="K15" s="20">
         <f t="shared" si="3"/>
         <v>2.6330467852260852E-2</v>
       </c>
-      <c r="L15" s="23">
+      <c r="L15" s="20">
         <f t="shared" si="4"/>
         <v>2.4867247001345603E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="16">
         <v>6210147.5999999996</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="16">
         <v>25652.449751200002</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="16">
         <v>6209546.4000000004</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="16">
         <v>30482.5218484</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="16">
         <v>5369027.4000000004</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="16">
         <v>23986.761495499999</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="16">
         <f t="shared" si="0"/>
         <v>0.99990319070677169</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="16">
         <f t="shared" si="1"/>
         <v>0.86455713226526221</v>
       </c>
-      <c r="J16" s="19">
+      <c r="J16" s="16">
         <f t="shared" si="2"/>
         <v>4.1307310878086062E-3</v>
       </c>
-      <c r="K16" s="19">
+      <c r="K16" s="16">
         <f t="shared" si="3"/>
         <v>4.9085019892924934E-3</v>
       </c>
-      <c r="L16" s="19">
+      <c r="L16" s="16">
         <f t="shared" si="4"/>
         <v>3.8625106906476749E-3</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="16">
         <v>1110071</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="16">
         <v>6416.1450420000001</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="16">
         <v>1089568.3999999999</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="16">
         <v>8594.6275917000003</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="16">
         <v>702127.2</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="16">
         <v>7013.5801813300004</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="16">
         <f t="shared" si="0"/>
         <v>0.98153037057989978</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="16">
         <f t="shared" si="1"/>
         <v>0.63250656939961492</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="16">
         <f t="shared" si="2"/>
         <v>5.7799411407018107E-3</v>
       </c>
-      <c r="K17" s="19">
+      <c r="K17" s="16">
         <f t="shared" si="3"/>
         <v>7.7424125048758145E-3</v>
       </c>
-      <c r="L17" s="19">
+      <c r="L17" s="16">
         <f t="shared" si="4"/>
         <v>6.318136570840965E-3</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="16">
         <v>142493877.59999999</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="16">
         <v>371768.52788299997</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="16">
         <v>140258619.59999999</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="16">
         <v>1273454.5480599999</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="16">
         <v>99214962</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="16">
         <v>527914.96147800004</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="16">
         <f t="shared" si="0"/>
         <v>0.98431330498090119</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="16">
         <f t="shared" si="1"/>
         <v>0.69627526228537417</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J18" s="16">
         <f t="shared" si="2"/>
         <v>2.6090140442848052E-3</v>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="16">
         <f t="shared" si="3"/>
         <v>8.936907111439291E-3</v>
       </c>
-      <c r="L18" s="19">
+      <c r="L18" s="16">
         <f t="shared" si="4"/>
         <v>3.7048255712426488E-3</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="19">
+      <c r="B19" s="16">
         <v>129526124.8</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="16">
         <v>8081944.83452</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="16">
         <v>58015974</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="16">
         <v>2038374.7693700001</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="16">
         <v>84578620</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="16">
         <v>4502817.2907499997</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="16">
         <f t="shared" si="0"/>
         <v>0.44790943981055475</v>
       </c>
-      <c r="I19" s="19">
+      <c r="I19" s="16">
         <f t="shared" si="1"/>
         <v>0.65298502623001353</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J19" s="16">
         <f t="shared" si="2"/>
         <v>6.2396252856319535E-2</v>
       </c>
-      <c r="K19" s="19">
+      <c r="K19" s="16">
         <f t="shared" si="3"/>
         <v>1.5737170956958948E-2</v>
       </c>
-      <c r="L19" s="19">
+      <c r="L19" s="16">
         <f t="shared" si="4"/>
         <v>3.4763776787908658E-2</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="19">
+      <c r="B20" s="16">
         <v>2762373</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="16">
         <v>38040.132260500002</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="16">
         <v>2772015.2</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="16">
         <v>25998.012880999999</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="16">
         <v>1120678.3999999999</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="16">
         <v>49133.758751399997</v>
       </c>
-      <c r="H20" s="19">
+      <c r="H20" s="16">
         <f t="shared" si="0"/>
         <v>1.0034905496107875</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="16">
         <f t="shared" si="1"/>
         <v>0.40569408982784</v>
       </c>
-      <c r="J20" s="19">
+      <c r="J20" s="16">
         <f t="shared" si="2"/>
         <v>1.3770816707410621E-2</v>
       </c>
-      <c r="K20" s="19">
+      <c r="K20" s="16">
         <f t="shared" si="3"/>
         <v>9.4114780592628143E-3</v>
       </c>
-      <c r="L20" s="19">
+      <c r="L20" s="16">
         <f t="shared" si="4"/>
         <v>1.7786793728218453E-2</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="16">
         <v>551144.6</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="16">
         <v>5290.3938076499999</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="16">
         <v>527654</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="16">
         <v>4825.0795641100003</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="16">
         <v>188306.6</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="16">
         <v>2862.5033519600001</v>
       </c>
-      <c r="H21" s="19">
+      <c r="H21" s="16">
         <f t="shared" si="0"/>
         <v>0.95737851736186841</v>
       </c>
-      <c r="I21" s="19">
+      <c r="I21" s="16">
         <f t="shared" si="1"/>
         <v>0.34166460126797943</v>
       </c>
-      <c r="J21" s="19">
+      <c r="J21" s="16">
         <f t="shared" si="2"/>
         <v>9.5989216036045707E-3</v>
       </c>
-      <c r="K21" s="19">
+      <c r="K21" s="16">
         <f t="shared" si="3"/>
         <v>8.7546527065855331E-3</v>
       </c>
-      <c r="L21" s="19">
+      <c r="L21" s="16">
         <f t="shared" si="4"/>
         <v>5.1937428978892294E-3</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="16">
         <v>21921636153.799999</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="16">
         <v>44023942.3477</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="16">
         <v>24100457793</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="16">
         <v>45888213.592100002</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="16">
         <v>42672266919.400002</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="16">
         <v>97728438.242799997</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="16">
         <f t="shared" si="0"/>
         <v>1.0993913786322156</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="16">
         <f t="shared" si="1"/>
         <v>1.946582208554857</v>
       </c>
-      <c r="J22" s="19">
+      <c r="J22" s="16">
         <f t="shared" si="2"/>
         <v>2.0082416311826561E-3</v>
       </c>
-      <c r="K22" s="19">
+      <c r="K22" s="16">
         <f t="shared" si="3"/>
         <v>2.0932841540728486E-3</v>
       </c>
-      <c r="L22" s="19">
+      <c r="L22" s="16">
         <f t="shared" si="4"/>
         <v>4.4580813930651473E-3</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23" s="16">
         <v>209163281.19999999</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="16">
         <v>277638.59746100003</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="16">
         <v>210255495.19999999</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="16">
         <v>759532.77214400005</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="16">
         <v>424145380.60000002</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="16">
         <v>1372976.29354</v>
       </c>
-      <c r="H23" s="19">
+      <c r="H23" s="16">
         <f t="shared" si="0"/>
         <v>1.005221824756878</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I23" s="16">
         <f t="shared" si="1"/>
         <v>2.0278195014278637</v>
       </c>
-      <c r="J23" s="19">
+      <c r="J23" s="16">
         <f t="shared" si="2"/>
         <v>1.3273773286981694E-3</v>
       </c>
-      <c r="K23" s="19">
+      <c r="K23" s="16">
         <f t="shared" si="3"/>
         <v>3.6312911510397558E-3</v>
       </c>
-      <c r="L23" s="19">
+      <c r="L23" s="16">
         <f t="shared" si="4"/>
         <v>6.5641363324529835E-3</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="16">
         <v>708340622.39999998</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="16">
         <v>641845.68573499995</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="16">
         <v>686259407.20000005</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="16">
         <v>1098996.8950100001</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="16">
         <v>638935891.60000002</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="16">
         <v>723161.32633499999</v>
       </c>
-      <c r="H24" s="19">
+      <c r="H24" s="16">
         <f t="shared" si="0"/>
         <v>0.96882684050339463</v>
       </c>
-      <c r="I24" s="19">
+      <c r="I24" s="16">
         <f t="shared" si="1"/>
         <v>0.90201785891532971</v>
       </c>
-      <c r="J24" s="19">
+      <c r="J24" s="16">
         <f t="shared" si="2"/>
         <v>9.0612576130435401E-4</v>
       </c>
-      <c r="K24" s="19">
+      <c r="K24" s="16">
         <f t="shared" si="3"/>
         <v>1.5515090625275428E-3</v>
       </c>
-      <c r="L24" s="19">
+      <c r="L24" s="16">
         <f t="shared" si="4"/>
         <v>1.0209231314233884E-3</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="16">
         <v>556696993.39999998</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="16">
         <v>561072.16255300003</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="16">
         <v>589117249</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="16">
         <v>1712351.1913900001</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="16">
         <v>558449117.39999998</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="16">
         <v>1017194.8683</v>
       </c>
-      <c r="H25" s="19">
+      <c r="H25" s="16">
         <f t="shared" si="0"/>
         <v>1.0582368074273132</v>
       </c>
-      <c r="I25" s="19">
+      <c r="I25" s="16">
         <f t="shared" si="1"/>
         <v>1.0031473566783593</v>
       </c>
-      <c r="J25" s="19">
+      <c r="J25" s="16">
         <f t="shared" si="2"/>
         <v>1.0078591571444978E-3</v>
       </c>
-      <c r="K25" s="19">
+      <c r="K25" s="16">
         <f t="shared" si="3"/>
         <v>3.0759124114033702E-3</v>
       </c>
-      <c r="L25" s="19">
+      <c r="L25" s="16">
         <f t="shared" si="4"/>
         <v>1.8271966264583747E-3</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="16">
         <v>1477601681.4000001</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="16">
         <v>1728466.8404600001</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="16">
         <v>1489098104.5999999</v>
       </c>
-      <c r="E26" s="19">
+      <c r="E26" s="16">
         <v>2668410.3672199999</v>
       </c>
-      <c r="F26" s="19">
+      <c r="F26" s="16">
         <v>1620387369.5999999</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="16">
         <v>817772.39235400001</v>
       </c>
-      <c r="H26" s="19">
+      <c r="H26" s="16">
         <f t="shared" si="0"/>
         <v>1.0077804616390982</v>
       </c>
-      <c r="I26" s="19">
+      <c r="I26" s="16">
         <f t="shared" si="1"/>
         <v>1.0966334093940073</v>
       </c>
-      <c r="J26" s="19">
+      <c r="J26" s="16">
         <f t="shared" si="2"/>
         <v>1.1697786096333553E-3</v>
       </c>
-      <c r="K26" s="19">
+      <c r="K26" s="16">
         <f t="shared" si="3"/>
         <v>1.80590642309755E-3</v>
       </c>
-      <c r="L26" s="19">
+      <c r="L26" s="16">
         <f t="shared" si="4"/>
         <v>5.5344576461172936E-4</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="16">
         <v>2789833426.5999999</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="16">
         <v>2035141.57268</v>
       </c>
-      <c r="D27" s="19">
+      <c r="D27" s="16">
         <v>2027571768.2</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E27" s="16">
         <v>5045395.4141699998</v>
       </c>
-      <c r="F27" s="19">
+      <c r="F27" s="16">
         <v>1682159963.2</v>
       </c>
-      <c r="G27" s="19">
+      <c r="G27" s="16">
         <v>1509844.4139099999</v>
       </c>
-      <c r="H27" s="19">
+      <c r="H27" s="16">
         <f t="shared" si="0"/>
         <v>0.7267716233047733</v>
       </c>
-      <c r="I27" s="19">
+      <c r="I27" s="16">
         <f t="shared" si="1"/>
         <v>0.60296071699523168</v>
       </c>
-      <c r="J27" s="19">
+      <c r="J27" s="16">
         <f t="shared" si="2"/>
         <v>7.29484976871988E-4</v>
       </c>
-      <c r="K27" s="19">
+      <c r="K27" s="16">
         <f t="shared" si="3"/>
         <v>1.8084934269064507E-3</v>
       </c>
-      <c r="L27" s="19">
+      <c r="L27" s="16">
         <f t="shared" si="4"/>
         <v>5.4119518373900324E-4</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B28" s="16">
         <v>4267317226.4000001</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="16">
         <v>3092450.0057700002</v>
       </c>
-      <c r="D28" s="19">
+      <c r="D28" s="16">
         <v>3516513600.4000001</v>
       </c>
-      <c r="E28" s="19">
+      <c r="E28" s="16">
         <v>7286563.9173800005</v>
       </c>
-      <c r="F28" s="19">
+      <c r="F28" s="16">
         <v>3302437286.5999999</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="16">
         <v>1972912.4042799999</v>
       </c>
-      <c r="H28" s="19">
+      <c r="H28" s="16">
         <f t="shared" si="0"/>
         <v>0.82405722701956374</v>
       </c>
-      <c r="I28" s="19">
+      <c r="I28" s="16">
         <f t="shared" si="1"/>
         <v>0.77389074010464565</v>
       </c>
-      <c r="J28" s="19">
+      <c r="J28" s="16">
         <f t="shared" si="2"/>
         <v>7.2468247418738471E-4</v>
       </c>
-      <c r="K28" s="19">
+      <c r="K28" s="16">
         <f t="shared" si="3"/>
         <v>1.7075280629012671E-3</v>
       </c>
-      <c r="L28" s="19">
+      <c r="L28" s="16">
         <f t="shared" si="4"/>
         <v>4.6233085088553185E-4</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="16">
         <v>1761068036.8</v>
       </c>
-      <c r="C29" s="19">
+      <c r="C29" s="16">
         <v>4653678.0338899996</v>
       </c>
-      <c r="D29" s="19">
+      <c r="D29" s="16">
         <v>1373532614.5999999</v>
       </c>
-      <c r="E29" s="19">
+      <c r="E29" s="16">
         <v>2175874.9010899998</v>
       </c>
-      <c r="F29" s="19">
+      <c r="F29" s="16">
         <v>1410393731.4000001</v>
       </c>
-      <c r="G29" s="19">
+      <c r="G29" s="16">
         <v>1459853.02018</v>
       </c>
-      <c r="H29" s="19">
+      <c r="H29" s="16">
         <f t="shared" si="0"/>
         <v>0.77994295841960626</v>
       </c>
-      <c r="I29" s="19">
+      <c r="I29" s="16">
         <f t="shared" si="1"/>
         <v>0.80087407296472046</v>
       </c>
-      <c r="J29" s="19">
+      <c r="J29" s="16">
         <f t="shared" si="2"/>
         <v>2.6425316550211775E-3</v>
       </c>
-      <c r="K29" s="19">
+      <c r="K29" s="16">
         <f t="shared" si="3"/>
         <v>1.2355427817790259E-3</v>
       </c>
-      <c r="L29" s="19">
+      <c r="L29" s="16">
         <f t="shared" si="4"/>
         <v>8.2895889861965154E-4</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="19">
+      <c r="B30" s="16">
         <v>23105024.199999999</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="16">
         <v>88711.490000799997</v>
       </c>
-      <c r="D30" s="19">
+      <c r="D30" s="16">
         <v>19289191</v>
       </c>
-      <c r="E30" s="19">
+      <c r="E30" s="16">
         <v>113025.01339399999</v>
       </c>
-      <c r="F30" s="19">
+      <c r="F30" s="16">
         <v>36502679.799999997</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="16">
         <v>92017.848028299995</v>
       </c>
-      <c r="H30" s="19">
+      <c r="H30" s="16">
         <f t="shared" si="0"/>
         <v>0.83484833571392669</v>
       </c>
-      <c r="I30" s="19">
+      <c r="I30" s="16">
         <f t="shared" si="1"/>
         <v>1.5798589728376047</v>
       </c>
-      <c r="J30" s="19">
+      <c r="J30" s="16">
         <f t="shared" si="2"/>
         <v>3.8394891618767487E-3</v>
       </c>
-      <c r="K30" s="19">
+      <c r="K30" s="16">
         <f t="shared" si="3"/>
         <v>4.8917937681277127E-3</v>
       </c>
-      <c r="L30" s="19">
+      <c r="L30" s="16">
         <f t="shared" si="4"/>
         <v>3.9825904198057495E-3</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="19">
+      <c r="B31" s="16">
         <v>130671943206</v>
       </c>
-      <c r="C31" s="19">
+      <c r="C31" s="16">
         <v>313480336.10299999</v>
       </c>
-      <c r="D31" s="19">
+      <c r="D31" s="16">
         <v>139001519472</v>
       </c>
-      <c r="E31" s="19">
+      <c r="E31" s="16">
         <v>218100109.76300001</v>
       </c>
-      <c r="F31" s="19">
+      <c r="F31" s="16">
         <v>130652543017</v>
       </c>
-      <c r="G31" s="19">
+      <c r="G31" s="16">
         <v>197662034.19400001</v>
       </c>
-      <c r="H31" s="19">
+      <c r="H31" s="16">
         <f t="shared" si="0"/>
         <v>1.0637441830406447</v>
       </c>
-      <c r="I31" s="19">
+      <c r="I31" s="16">
         <f t="shared" si="1"/>
         <v>0.99985153516107572</v>
       </c>
-      <c r="J31" s="19">
+      <c r="J31" s="16">
         <f t="shared" si="2"/>
         <v>2.3989873297346515E-3</v>
       </c>
-      <c r="K31" s="19">
+      <c r="K31" s="16">
         <f t="shared" si="3"/>
         <v>1.6690660933936859E-3</v>
       </c>
-      <c r="L31" s="19">
+      <c r="L31" s="16">
         <f t="shared" si="4"/>
         <v>1.512658565751887E-3</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="19">
+      <c r="B32" s="16">
         <v>9231106491.2000008</v>
       </c>
-      <c r="C32" s="19">
+      <c r="C32" s="16">
         <v>31595097.076900002</v>
       </c>
-      <c r="D32" s="19">
+      <c r="D32" s="16">
         <v>9057620010</v>
       </c>
-      <c r="E32" s="19">
+      <c r="E32" s="16">
         <v>20076141.795600001</v>
       </c>
-      <c r="F32" s="19">
+      <c r="F32" s="16">
         <v>12030245569.4</v>
       </c>
-      <c r="G32" s="19">
+      <c r="G32" s="16">
         <v>17225067.5526</v>
       </c>
-      <c r="H32" s="19">
+      <c r="H32" s="16">
         <f t="shared" si="0"/>
         <v>0.98120631785957779</v>
       </c>
-      <c r="I32" s="19">
+      <c r="I32" s="16">
         <f t="shared" si="1"/>
         <v>1.3032289878649341</v>
       </c>
-      <c r="J32" s="19">
+      <c r="J32" s="16">
         <f t="shared" si="2"/>
         <v>3.4226771305281289E-3</v>
       </c>
-      <c r="K32" s="19">
+      <c r="K32" s="16">
         <f t="shared" si="3"/>
         <v>2.1748359001966398E-3</v>
       </c>
-      <c r="L32" s="19">
+      <c r="L32" s="16">
         <f t="shared" si="4"/>
         <v>1.8659808083701158E-3</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="19">
+      <c r="B33" s="16">
         <v>9682033494.3999996</v>
       </c>
-      <c r="C33" s="19">
+      <c r="C33" s="16">
         <v>102150439.789</v>
       </c>
-      <c r="D33" s="19">
+      <c r="D33" s="16">
         <v>9079195596.3999996</v>
       </c>
-      <c r="E33" s="19">
+      <c r="E33" s="16">
         <v>22140042.7073</v>
       </c>
-      <c r="F33" s="19">
+      <c r="F33" s="16">
         <v>12507954174.4</v>
       </c>
-      <c r="G33" s="19">
+      <c r="G33" s="16">
         <v>34985071.001500003</v>
       </c>
-      <c r="H33" s="19">
+      <c r="H33" s="16">
         <f t="shared" si="0"/>
         <v>0.93773643745927171</v>
       </c>
-      <c r="I33" s="19">
+      <c r="I33" s="16">
         <f t="shared" si="1"/>
         <v>1.2918726403533398</v>
       </c>
-      <c r="J33" s="19">
+      <c r="J33" s="16">
         <f t="shared" si="2"/>
         <v>1.0550515018160482E-2</v>
       </c>
-      <c r="K33" s="19">
+      <c r="K33" s="16">
         <f t="shared" si="3"/>
         <v>2.2867141205518034E-3</v>
       </c>
-      <c r="L33" s="19">
+      <c r="L33" s="16">
         <f t="shared" si="4"/>
         <v>3.6134011539760784E-3</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="19">
+      <c r="B34" s="16">
         <v>1579196789850</v>
       </c>
-      <c r="C34" s="19">
+      <c r="C34" s="16">
         <v>17815351085.299999</v>
       </c>
-      <c r="D34" s="19">
+      <c r="D34" s="16">
         <v>1074457425660</v>
       </c>
-      <c r="E34" s="19">
+      <c r="E34" s="16">
         <v>757369498.28299999</v>
       </c>
-      <c r="F34" s="19">
+      <c r="F34" s="16">
         <v>996257070573</v>
       </c>
-      <c r="G34" s="19">
+      <c r="G34" s="16">
         <v>218264110.53299999</v>
       </c>
-      <c r="H34" s="19">
+      <c r="H34" s="16">
         <f t="shared" si="0"/>
         <v>0.68038222504369283</v>
       </c>
-      <c r="I34" s="19">
+      <c r="I34" s="16">
         <f t="shared" si="1"/>
         <v>0.63086315586268982</v>
       </c>
-      <c r="J34" s="19">
+      <c r="J34" s="16">
         <f t="shared" si="2"/>
         <v>1.1281273619478539E-2</v>
       </c>
-      <c r="K34" s="19">
+      <c r="K34" s="16">
         <f t="shared" si="3"/>
         <v>4.7959158931353875E-4</v>
       </c>
-      <c r="L34" s="19">
+      <c r="L34" s="16">
         <f t="shared" si="4"/>
         <v>1.382121037326398E-4</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="19">
+      <c r="B35" s="16">
         <v>43080528284.400002</v>
       </c>
-      <c r="C35" s="19">
+      <c r="C35" s="16">
         <v>172680137.38299999</v>
       </c>
-      <c r="D35" s="19">
+      <c r="D35" s="16">
         <v>20490251939.599998</v>
       </c>
-      <c r="E35" s="19">
+      <c r="E35" s="16">
         <v>3347136.4973900001</v>
       </c>
-      <c r="F35" s="19">
+      <c r="F35" s="16">
         <v>19695167716.799999</v>
       </c>
-      <c r="G35" s="19">
+      <c r="G35" s="16">
         <v>3458974.2125200001</v>
       </c>
-      <c r="H35" s="19">
+      <c r="H35" s="16">
         <f t="shared" si="0"/>
         <v>0.47562675657855791</v>
       </c>
-      <c r="I35" s="19">
+      <c r="I35" s="16">
         <f t="shared" si="1"/>
         <v>0.45717098886950897</v>
       </c>
-      <c r="J35" s="19">
+      <c r="J35" s="16">
         <f t="shared" si="2"/>
         <v>4.0083105815935322E-3</v>
       </c>
-      <c r="K35" s="19">
+      <c r="K35" s="16">
         <f t="shared" si="3"/>
         <v>7.7694880510600431E-5</v>
       </c>
-      <c r="L35" s="19">
+      <c r="L35" s="16">
         <f t="shared" si="4"/>
         <v>8.0290895916718314E-5</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A36" s="21" t="s">
+      <c r="A36" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="19">
+      <c r="B36" s="16">
         <v>22991226992</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="16">
         <v>103385613.002</v>
       </c>
-      <c r="D36" s="19">
+      <c r="D36" s="16">
         <v>10742157139.4</v>
       </c>
-      <c r="E36" s="19">
+      <c r="E36" s="16">
         <v>1698179.0649699999</v>
       </c>
-      <c r="F36" s="19">
+      <c r="F36" s="16">
         <v>10573749849.4</v>
       </c>
-      <c r="G36" s="19">
+      <c r="G36" s="16">
         <v>1780264.3950700001</v>
       </c>
-      <c r="H36" s="19">
+      <c r="H36" s="16">
         <f t="shared" si="0"/>
         <v>0.46722852778313345</v>
       </c>
-      <c r="I36" s="19">
+      <c r="I36" s="16">
         <f t="shared" si="1"/>
         <v>0.45990367774104568</v>
       </c>
-      <c r="J36" s="19">
+      <c r="J36" s="16">
         <f t="shared" si="2"/>
         <v>4.4967418675816622E-3</v>
       </c>
-      <c r="K36" s="19">
+      <c r="K36" s="16">
         <f t="shared" si="3"/>
         <v>7.3862045969138413E-5</v>
       </c>
-      <c r="L36" s="19">
+      <c r="L36" s="16">
         <f t="shared" si="4"/>
         <v>7.7432335198528493E-5</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="19">
+      <c r="B37" s="16">
         <v>1123007.6000000001</v>
       </c>
-      <c r="C37" s="19">
+      <c r="C37" s="16">
         <v>807.77313646799996</v>
       </c>
-      <c r="D37" s="19">
+      <c r="D37" s="16">
         <v>1157807.2</v>
       </c>
-      <c r="E37" s="19">
+      <c r="E37" s="16">
         <v>2195.0648646499999</v>
       </c>
-      <c r="F37" s="19">
+      <c r="F37" s="16">
         <v>1063081.3999999999</v>
       </c>
-      <c r="G37" s="19">
+      <c r="G37" s="16">
         <v>870.85626827900001</v>
       </c>
-      <c r="H37" s="19">
+      <c r="H37" s="16">
         <f t="shared" si="0"/>
         <v>1.0309878579628489</v>
       </c>
-      <c r="I37" s="19">
+      <c r="I37" s="16">
         <f t="shared" si="1"/>
         <v>0.94663776095549113</v>
       </c>
-      <c r="J37" s="19">
+      <c r="J37" s="16">
         <f t="shared" si="2"/>
         <v>7.1929445220851563E-4</v>
       </c>
-      <c r="K37" s="19">
+      <c r="K37" s="16">
         <f t="shared" si="3"/>
         <v>1.9546304625632093E-3</v>
       </c>
-      <c r="L37" s="19">
+      <c r="L37" s="16">
         <f t="shared" si="4"/>
         <v>7.7546783145456888E-4</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="14" t="s">
         <v>47</v>
       </c>
     </row>
@@ -5370,29 +5521,29 @@
     </row>
     <row r="3" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="13"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="8" t="s">
         <v>45</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
     </row>
     <row r="4" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -6886,29 +7037,29 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="13"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="8" t="s">
         <v>45</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -8375,90 +8526,414 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51140CC8-C0B8-469A-8BAE-C9043CBCBC10}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="27.06640625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="19.19921875" style="28" customWidth="1"/>
+    <col min="3" max="3" width="19.3984375" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.06640625" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="29">
+        <v>155338287274</v>
+      </c>
+      <c r="C4" s="29">
+        <v>945633750833</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="29">
+        <v>331202799523</v>
+      </c>
+      <c r="C5" s="29">
+        <v>1201670139630</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="29">
+        <v>78207622</v>
+      </c>
+      <c r="C6" s="29">
+        <v>412919146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="29">
+        <v>17265918</v>
+      </c>
+      <c r="C7" s="29">
+        <v>258821219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="29">
+        <v>13484423091</v>
+      </c>
+      <c r="C8" s="29">
+        <v>13411232377</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5A357B-AD95-4B57-AFAC-6E90E36724A8}">
+  <dimension ref="A1:H50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.06640625" customWidth="1"/>
-    <col min="2" max="2" width="19.19921875" customWidth="1"/>
-    <col min="3" max="3" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6">
-        <v>155338287274</v>
-      </c>
-      <c r="C4" s="6">
-        <v>945633750833</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6">
-        <v>331202799523</v>
-      </c>
-      <c r="C5" s="6">
-        <v>1201670139630</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="6">
-        <v>78207622</v>
-      </c>
-      <c r="C6" s="6">
-        <v>412919146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="6">
-        <v>17265918</v>
-      </c>
-      <c r="C7" s="6">
-        <v>258821219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="6">
-        <v>13484423091</v>
-      </c>
-      <c r="C8" s="6">
-        <v>13411232377</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A15" s="30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A29" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" t="s">
+        <v>82</v>
+      </c>
+      <c r="D46" t="s">
+        <v>83</v>
+      </c>
+      <c r="E46" t="s">
+        <v>84</v>
+      </c>
+      <c r="F46" t="s">
+        <v>85</v>
+      </c>
+      <c r="G46" t="s">
+        <v>86</v>
+      </c>
+      <c r="H46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>81</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>1934</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="H47">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>90</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E50" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new results for postgres
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="339" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{B2AAFDF8-6FB0-4073-A23A-D21F3165E975}"/>
+  <xr:revisionPtr revIDLastSave="459" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{01092C25-481C-4D28-A6CF-DBC2BCA5FFEC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -14,8 +14,10 @@
     <sheet name="clang-part1" sheetId="3" r:id="rId4"/>
     <sheet name="clang-part2" sheetId="4" r:id="rId5"/>
     <sheet name="clang-part3" sheetId="5" r:id="rId6"/>
-    <sheet name="postgres" sheetId="8" r:id="rId7"/>
-    <sheet name="postgres_stats" sheetId="9" r:id="rId8"/>
+    <sheet name="postgres-os" sheetId="11" r:id="rId7"/>
+    <sheet name="postgres-usr" sheetId="8" r:id="rId8"/>
+    <sheet name="postgres-all" sheetId="12" r:id="rId9"/>
+    <sheet name="postgres_stats" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="117">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -177,24 +179,12 @@
     <t>database size = 4GB</t>
   </si>
   <si>
-    <t>OS</t>
-  </si>
-  <si>
-    <t>usr</t>
-  </si>
-  <si>
     <t>Running "pgbench -j 1 -c 2 -t 4000000 -S pgbench" on the stock freebsd 11.0</t>
   </si>
   <si>
     <t>4GB/2MB * 2 # of super pages for each iteration</t>
   </si>
   <si>
-    <t>Before running the experiments</t>
-  </si>
-  <si>
-    <t>vm.pmap.pde.promotions: 2856</t>
-  </si>
-  <si>
     <t>vm.pmap.pde.p_failures: 0</t>
   </si>
   <si>
@@ -213,57 +203,12 @@
     <t>LEVEL     SIZE  NUMBER</t>
   </si>
   <si>
-    <t xml:space="preserve">   -1: 228548K,    127</t>
-  </si>
-  <si>
-    <t>vm.reserv.fullpop: 2173</t>
-  </si>
-  <si>
-    <t>vm.reserv.freed: 3455</t>
-  </si>
-  <si>
     <t>vm.reserv.broken: 0</t>
   </si>
   <si>
-    <t>After running two rounds of "pgbench -j 1 -c 2 -t 4000000 -S pgbench"</t>
-  </si>
-  <si>
-    <t>vm.pmap.pde.promotions: 2906</t>
-  </si>
-  <si>
-    <t>vm.pmap.pde.p_failures: 7010</t>
-  </si>
-  <si>
     <t>vm.pmap.pde.mappings: 3400</t>
   </si>
   <si>
-    <t xml:space="preserve">   -1: 231464K,    130</t>
-  </si>
-  <si>
-    <t>vm.reserv.fullpop: 2493</t>
-  </si>
-  <si>
-    <t>vm.reserv.freed: 3598</t>
-  </si>
-  <si>
-    <t>After running another two rounds of "pgbench -j 1 -c 2 -t 4000000 -S pgbench"</t>
-  </si>
-  <si>
-    <t>vm.pmap.pde.promotions: 3003</t>
-  </si>
-  <si>
-    <t>vm.pmap.pde.p_failures: 14223</t>
-  </si>
-  <si>
-    <t>vm.pmap.pde.mappings: 4470</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   -1: 236564K,    134</t>
-  </si>
-  <si>
-    <t>vm.reserv.freed: 3774</t>
-  </si>
-  <si>
     <t xml:space="preserve">extended device statistics  </t>
   </si>
   <si>
@@ -307,6 +252,135 @@
   </si>
   <si>
     <t>KB written</t>
+  </si>
+  <si>
+    <t>This feature allows the kernel to remove a great deal of internal memory management page-tracking overhead at the cost of wiring the shared memory into core, making it unswappable.</t>
+  </si>
+  <si>
+    <t>kern.ipc.shm_use_phys="1":</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Setting this parameter to 1 will cause all System V shared memory segments to be mapped to unpageable physical RAM.</t>
+  </si>
+  <si>
+    <t>When the system just boots</t>
+  </si>
+  <si>
+    <t>When postgresql starts and pgbench is initialized</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.promotions: 307</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.mappings: 1080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 215632K,    121</t>
+  </si>
+  <si>
+    <t>vm.reserv.fullpop: 247</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 2645</t>
+  </si>
+  <si>
+    <t>vm.reserv.broken: 1</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.promotions: 2853</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 221676K,    124</t>
+  </si>
+  <si>
+    <t>vm.reserv.fullpop: 2170</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 3471</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.promotions: 2868</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.p_failures: 3501</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.mappings: 2868</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 226720K,    128</t>
+  </si>
+  <si>
+    <t>vm.reserv.fullpop: 2490</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 3542</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.promotions: 2907</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.p_failures: 7115</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.mappings: 3408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 228768K,    129</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 3644</t>
+  </si>
+  <si>
+    <t>kern.ipc.shm_use_phys="0":</t>
+  </si>
+  <si>
+    <t>After running one round of "pgbench -j 1 -c 2 -t 4000000 -S pgbench"</t>
+  </si>
+  <si>
+    <t>After running one rounds of "pgbench -j 1 -c 2 -t 4000000 -S pgbench"</t>
+  </si>
+  <si>
+    <t>After running another round of "pgbench -j 1 -c 2 -t 4000000 -S pgbench"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 219800K,    123</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 2599</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 223752K,    125</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 3399</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.promotions: 2861</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.p_failures: 3432</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.mappings: 2865</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 253404K,    142</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 3460</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.promotions: 2901</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.p_failures: 7039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 253396K,    142</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 3508</t>
   </si>
 </sst>
 </file>
@@ -317,7 +391,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,6 +499,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -447,7 +536,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -495,6 +584,25 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3980,7 +4088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670D2A71-BD87-4620-9FEC-7336DAF0F286}">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
@@ -5499,8 +5607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440270B8-E650-47B8-847B-14A2543F142D}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7013,8 +7121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8525,415 +8633,1559 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51140CC8-C0B8-469A-8BAE-C9043CBCBC10}">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65049047-28B8-4D24-A307-ABB41DE3392E}">
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.06640625" style="28" customWidth="1"/>
-    <col min="2" max="2" width="19.19921875" style="28" customWidth="1"/>
-    <col min="3" max="3" width="19.3984375" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.06640625" style="28"/>
+    <col min="1" max="1" width="32.86328125" customWidth="1"/>
+    <col min="2" max="2" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+        <v>49</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="27" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B3" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="28" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3" s="28" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="28" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+    </row>
+    <row r="5" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A5" s="2"/>
+      <c r="B5" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+    </row>
+    <row r="6" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="29">
-        <v>155338287274</v>
-      </c>
-      <c r="C4" s="29">
-        <v>945633750833</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="28" t="s">
+      <c r="B7" s="6">
+        <v>155488099780</v>
+      </c>
+      <c r="C7" s="6">
+        <v>109256561.01800001</v>
+      </c>
+      <c r="D7" s="6">
+        <v>155651878039</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1240169394.24</v>
+      </c>
+      <c r="F7" s="6">
+        <v>155396097352</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1092945842.3599999</v>
+      </c>
+      <c r="H7" s="6">
+        <f>D7/B7</f>
+        <v>1.0010533170013123</v>
+      </c>
+      <c r="I7" s="6">
+        <f>F7/B7</f>
+        <v>0.99940829923235175</v>
+      </c>
+      <c r="J7" s="6">
+        <f>C7/B7</f>
+        <v>7.0266831463364102E-4</v>
+      </c>
+      <c r="K7" s="6">
+        <f>E7/B7</f>
+        <v>7.9759762708188908E-3</v>
+      </c>
+      <c r="L7" s="6">
+        <f>G7/B7</f>
+        <v>7.0291285565030901E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="29">
-        <v>331202799523</v>
-      </c>
-      <c r="C5" s="29">
-        <v>1201670139630</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="28" t="s">
+      <c r="B8" s="6">
+        <v>333482308492</v>
+      </c>
+      <c r="C8" s="6">
+        <v>396439847.07999998</v>
+      </c>
+      <c r="D8" s="6">
+        <v>328381134082</v>
+      </c>
+      <c r="E8" s="6">
+        <v>10031617594</v>
+      </c>
+      <c r="F8" s="6">
+        <v>331966609845</v>
+      </c>
+      <c r="G8" s="6">
+        <v>3160684862.4499998</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" ref="H8:H11" si="0">D8/B8</f>
+        <v>0.98470331324900739</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" ref="I8:I11" si="1">F8/B8</f>
+        <v>0.99545493536417584</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" ref="J8:J11" si="2">C8/B8</f>
+        <v>1.1887882414893091E-3</v>
+      </c>
+      <c r="K8" s="6">
+        <f t="shared" ref="K8:K11" si="3">E8/B8</f>
+        <v>3.0081408634127442E-2</v>
+      </c>
+      <c r="L8" s="6">
+        <f t="shared" ref="L8:L11" si="4">G8/B8</f>
+        <v>9.477818708712166E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="29">
-        <v>78207622</v>
-      </c>
-      <c r="C6" s="29">
-        <v>412919146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="28" t="s">
+      <c r="B9" s="6">
+        <v>78271163.599999994</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1433465.8790899999</v>
+      </c>
+      <c r="D9" s="6">
+        <v>68326073.599999994</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1214110.2608099999</v>
+      </c>
+      <c r="F9" s="6">
+        <v>62405817.399999999</v>
+      </c>
+      <c r="G9" s="6">
+        <v>806169.35760300001</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="0"/>
+        <v>0.87294056274896104</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="1"/>
+        <v>0.79730279364340517</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="2"/>
+        <v>1.8314099511994478E-2</v>
+      </c>
+      <c r="K9" s="6">
+        <f t="shared" si="3"/>
+        <v>1.5511590794978292E-2</v>
+      </c>
+      <c r="L9" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0299698133055481E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="29">
-        <v>17265918</v>
-      </c>
-      <c r="C7" s="29">
-        <v>258821219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="28" t="s">
+      <c r="B10" s="6">
+        <v>32476392.600000001</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1704563.7003500001</v>
+      </c>
+      <c r="D10" s="6">
+        <v>26894871.600000001</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1063580.79907</v>
+      </c>
+      <c r="F10" s="6">
+        <v>4609278</v>
+      </c>
+      <c r="G10" s="6">
+        <v>257185.27273500001</v>
+      </c>
+      <c r="H10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.82813605350983477</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="1"/>
+        <v>0.1419270316371283</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="2"/>
+        <v>5.2486238891877417E-2</v>
+      </c>
+      <c r="K10" s="6">
+        <f t="shared" si="3"/>
+        <v>3.2749351572686672E-2</v>
+      </c>
+      <c r="L10" s="6">
+        <f t="shared" si="4"/>
+        <v>7.9191453281975653E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="29">
-        <v>13484423091</v>
-      </c>
-      <c r="C8" s="29">
-        <v>13411232377</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="28" t="s">
-        <v>52</v>
+      <c r="B11" s="6">
+        <v>13127022678.4</v>
+      </c>
+      <c r="C11" s="6">
+        <v>210486566.602</v>
+      </c>
+      <c r="D11" s="6">
+        <v>13630958501.799999</v>
+      </c>
+      <c r="E11" s="6">
+        <v>220806167.229</v>
+      </c>
+      <c r="F11" s="6">
+        <v>13408413157</v>
+      </c>
+      <c r="G11" s="6">
+        <v>190294880.90900001</v>
+      </c>
+      <c r="H11" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0383891942404584</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="1"/>
+        <v>1.0214359710875656</v>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" si="2"/>
+        <v>1.6034600667548735E-2</v>
+      </c>
+      <c r="K11" s="6">
+        <f t="shared" si="3"/>
+        <v>1.6820734803203157E-2</v>
+      </c>
+      <c r="L11" s="6">
+        <f t="shared" si="4"/>
+        <v>1.4496423566184795E-2</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="J5:L5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51140CC8-C0B8-469A-8BAE-C9043CBCBC10}">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="35" style="28" customWidth="1"/>
+    <col min="2" max="2" width="19.19921875" style="28" customWidth="1"/>
+    <col min="3" max="3" width="19.46484375" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.86328125" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.3984375" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.9296875" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.06640625" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A1" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A2" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3" s="28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A5" s="2"/>
+      <c r="B5" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+    </row>
+    <row r="6" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6">
+        <v>946914692983</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1638529605.76</v>
+      </c>
+      <c r="D7" s="6">
+        <v>940390725841</v>
+      </c>
+      <c r="E7" s="6">
+        <v>6669456559.4899998</v>
+      </c>
+      <c r="F7" s="6">
+        <v>944522103276</v>
+      </c>
+      <c r="G7" s="6">
+        <v>6985699539.3500004</v>
+      </c>
+      <c r="H7" s="29">
+        <f>D7/B7</f>
+        <v>0.99311029051471578</v>
+      </c>
+      <c r="I7" s="29">
+        <f>F7/B7</f>
+        <v>0.99747327850678624</v>
+      </c>
+      <c r="J7" s="29">
+        <f>C7/B7</f>
+        <v>1.7303877718892007E-3</v>
+      </c>
+      <c r="K7" s="29">
+        <f>E7/B7</f>
+        <v>7.0433552345456497E-3</v>
+      </c>
+      <c r="L7" s="29">
+        <f>G7/B7</f>
+        <v>7.3773272197767189E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1200836800110</v>
+      </c>
+      <c r="C8" s="6">
+        <v>827454901.97399998</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1200772331430</v>
+      </c>
+      <c r="E8" s="6">
+        <v>9214310628.6700001</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1151380231060</v>
+      </c>
+      <c r="G8" s="6">
+        <v>10934220055.700001</v>
+      </c>
+      <c r="H8" s="29">
+        <f t="shared" ref="H8:H11" si="0">D8/B8</f>
+        <v>0.99994631353736485</v>
+      </c>
+      <c r="I8" s="29">
+        <f t="shared" ref="I8:I11" si="1">F8/B8</f>
+        <v>0.95881491219667014</v>
+      </c>
+      <c r="J8" s="29">
+        <f t="shared" ref="J8:J11" si="2">C8/B8</f>
+        <v>6.8906524341875834E-4</v>
+      </c>
+      <c r="K8" s="29">
+        <f t="shared" ref="K8:K11" si="3">E8/B8</f>
+        <v>7.6732413828639687E-3</v>
+      </c>
+      <c r="L8" s="29">
+        <f t="shared" ref="L8:L11" si="4">G8/B8</f>
+        <v>9.1055004765829926E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="6">
+        <v>451472726.19999999</v>
+      </c>
+      <c r="C9" s="6">
+        <v>4509950.1854800005</v>
+      </c>
+      <c r="D9" s="6">
+        <v>414906363.80000001</v>
+      </c>
+      <c r="E9" s="6">
+        <v>5076230.1852000002</v>
+      </c>
+      <c r="F9" s="6">
+        <v>83253569.799999997</v>
+      </c>
+      <c r="G9" s="6">
+        <v>4087614.1338900002</v>
+      </c>
+      <c r="H9" s="29">
+        <f t="shared" si="0"/>
+        <v>0.9190064863767623</v>
+      </c>
+      <c r="I9" s="29">
+        <f t="shared" si="1"/>
+        <v>0.18440442792798764</v>
+      </c>
+      <c r="J9" s="29">
+        <f t="shared" si="2"/>
+        <v>9.9894189034181371E-3</v>
+      </c>
+      <c r="K9" s="29">
+        <f t="shared" si="3"/>
+        <v>1.1243713940210991E-2</v>
+      </c>
+      <c r="L9" s="29">
+        <f t="shared" si="4"/>
+        <v>9.0539558575221859E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="6">
+        <v>266369123.40000001</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3466899.5721100001</v>
+      </c>
+      <c r="D10" s="6">
+        <v>245947677.80000001</v>
+      </c>
+      <c r="E10" s="6">
+        <v>2917717.71747</v>
+      </c>
+      <c r="F10" s="6">
+        <v>127109755.2</v>
+      </c>
+      <c r="G10" s="6">
+        <v>665387.35145299998</v>
+      </c>
+      <c r="H10" s="29">
+        <f t="shared" si="0"/>
+        <v>0.92333403609496578</v>
+      </c>
+      <c r="I10" s="29">
+        <f t="shared" si="1"/>
+        <v>0.47719402901334923</v>
+      </c>
+      <c r="J10" s="29">
+        <f t="shared" si="2"/>
+        <v>1.3015395808108891E-2</v>
+      </c>
+      <c r="K10" s="29">
+        <f t="shared" si="3"/>
+        <v>1.0953663398473309E-2</v>
+      </c>
+      <c r="L10" s="29">
+        <f t="shared" si="4"/>
+        <v>2.4979897931105329E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="6">
+        <v>13444549014</v>
+      </c>
+      <c r="C11" s="6">
+        <v>307569910.05299997</v>
+      </c>
+      <c r="D11" s="6">
+        <v>13667780586.799999</v>
+      </c>
+      <c r="E11" s="6">
+        <v>113540871.403</v>
+      </c>
+      <c r="F11" s="6">
+        <v>13323831275.6</v>
+      </c>
+      <c r="G11" s="6">
+        <v>250385375.715</v>
+      </c>
+      <c r="H11" s="29">
+        <f t="shared" si="0"/>
+        <v>1.0166038721393738</v>
+      </c>
+      <c r="I11" s="29">
+        <f t="shared" si="1"/>
+        <v>0.99102106450173266</v>
+      </c>
+      <c r="J11" s="29">
+        <f t="shared" si="2"/>
+        <v>2.2876922813306944E-2</v>
+      </c>
+      <c r="K11" s="29">
+        <f t="shared" si="3"/>
+        <v>8.4451230967114085E-3</v>
+      </c>
+      <c r="L11" s="29">
+        <f t="shared" si="4"/>
+        <v>1.8623560779485435E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="J5:L5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCFEC93-FC4D-46DA-B16B-8898E424FCC7}">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="34.59765625" customWidth="1"/>
+    <col min="2" max="2" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="9.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A1" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A2" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+    </row>
+    <row r="5" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A5" s="4"/>
+      <c r="B5" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="32"/>
+      <c r="F5" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="32"/>
+      <c r="H5" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+    </row>
+    <row r="6" spans="1:12" ht="57" x14ac:dyDescent="0.45">
+      <c r="A6" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1102402792763</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1747786166.7779999</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1096042603880</v>
+      </c>
+      <c r="E7" s="6">
+        <v>7909625953.7299995</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1099918200628</v>
+      </c>
+      <c r="G7" s="6">
+        <v>8078645381.71</v>
+      </c>
+      <c r="H7" s="29">
+        <f>D7/B7</f>
+        <v>0.99423061250864653</v>
+      </c>
+      <c r="I7" s="29">
+        <f>F7/B7</f>
+        <v>0.99774620297471062</v>
+      </c>
+      <c r="J7" s="29">
+        <f>C7/B7</f>
+        <v>1.5854333626980819E-3</v>
+      </c>
+      <c r="K7" s="29">
+        <f>E7/B7</f>
+        <v>7.1748965130120548E-3</v>
+      </c>
+      <c r="L7" s="29">
+        <f>G7/B7</f>
+        <v>7.3282156347428511E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1534319108602</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1223894749.0539999</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1529153465512</v>
+      </c>
+      <c r="E8" s="6">
+        <v>19245928222.669998</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1483346840905</v>
+      </c>
+      <c r="G8" s="6">
+        <v>14094904918.150002</v>
+      </c>
+      <c r="H8" s="29">
+        <f t="shared" ref="H8:H11" si="0">D8/B8</f>
+        <v>0.99663326679499764</v>
+      </c>
+      <c r="I8" s="29">
+        <f t="shared" ref="I8:I11" si="1">F8/B8</f>
+        <v>0.966778574671182</v>
+      </c>
+      <c r="J8" s="29">
+        <f t="shared" ref="J8:J11" si="2">C8/B8</f>
+        <v>7.97679402017717E-4</v>
+      </c>
+      <c r="K8" s="29">
+        <f t="shared" ref="K8:K11" si="3">E8/B8</f>
+        <v>1.2543628059358519E-2</v>
+      </c>
+      <c r="L8" s="29">
+        <f t="shared" ref="L8:L11" si="4">G8/B8</f>
+        <v>9.1864233712064119E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="6">
+        <v>529743889.79999995</v>
+      </c>
+      <c r="C9" s="6">
+        <v>5943416.0645700004</v>
+      </c>
+      <c r="D9" s="6">
+        <v>483232437.39999998</v>
+      </c>
+      <c r="E9" s="6">
+        <v>6290340.4460100001</v>
+      </c>
+      <c r="F9" s="6">
+        <v>145659387.19999999</v>
+      </c>
+      <c r="G9" s="6">
+        <v>4893783.4914929997</v>
+      </c>
+      <c r="H9" s="29">
+        <f t="shared" si="0"/>
+        <v>0.91220011538488921</v>
+      </c>
+      <c r="I9" s="29">
+        <f t="shared" si="1"/>
+        <v>0.27496190141049554</v>
+      </c>
+      <c r="J9" s="29">
+        <f t="shared" si="2"/>
+        <v>1.1219414096147261E-2</v>
+      </c>
+      <c r="K9" s="29">
+        <f t="shared" si="3"/>
+        <v>1.1874304861514988E-2</v>
+      </c>
+      <c r="L9" s="29">
+        <f t="shared" si="4"/>
+        <v>9.2380178152514491E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="6">
+        <v>298845516</v>
+      </c>
+      <c r="C10" s="6">
+        <v>5171463.2724600006</v>
+      </c>
+      <c r="D10" s="6">
+        <v>272842549.40000004</v>
+      </c>
+      <c r="E10" s="6">
+        <v>3981298.5165400002</v>
+      </c>
+      <c r="F10" s="6">
+        <v>131719033.2</v>
+      </c>
+      <c r="G10" s="6">
+        <v>922572.62418799999</v>
+      </c>
+      <c r="H10" s="29">
+        <f t="shared" si="0"/>
+        <v>0.91298860043796015</v>
+      </c>
+      <c r="I10" s="29">
+        <f t="shared" si="1"/>
+        <v>0.44075961039348505</v>
+      </c>
+      <c r="J10" s="29">
+        <f t="shared" si="2"/>
+        <v>1.7304804641806976E-2</v>
+      </c>
+      <c r="K10" s="29">
+        <f t="shared" si="3"/>
+        <v>1.3322262852824602E-2</v>
+      </c>
+      <c r="L10" s="29">
+        <f t="shared" si="4"/>
+        <v>3.0871221912126667E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="6">
+        <v>26571571692.400002</v>
+      </c>
+      <c r="C11" s="6">
+        <v>518056476.65499997</v>
+      </c>
+      <c r="D11" s="6">
+        <v>27298739088.599998</v>
+      </c>
+      <c r="E11" s="6">
+        <v>334347038.63199997</v>
+      </c>
+      <c r="F11" s="6">
+        <v>26732244432.599998</v>
+      </c>
+      <c r="G11" s="6">
+        <v>440680256.62400001</v>
+      </c>
+      <c r="H11" s="29">
+        <f t="shared" si="0"/>
+        <v>1.0273663675080229</v>
+      </c>
+      <c r="I11" s="29">
+        <f t="shared" si="1"/>
+        <v>1.0060467909862461</v>
+      </c>
+      <c r="J11" s="29">
+        <f t="shared" si="2"/>
+        <v>1.9496644107174679E-2</v>
+      </c>
+      <c r="K11" s="29">
+        <f t="shared" si="3"/>
+        <v>1.2582885291938899E-2</v>
+      </c>
+      <c r="L11" s="29">
+        <f t="shared" si="4"/>
+        <v>1.6584651511225561E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="J5:L5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5A357B-AD95-4B57-AFAC-6E90E36724A8}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="26.46484375" customWidth="1"/>
+    <col min="3" max="3" width="28.06640625" customWidth="1"/>
+    <col min="4" max="4" width="28.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="37"/>
+    </row>
+    <row r="5" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A5" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A19" s="30"/>
+    </row>
+    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A22" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="B35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A48" s="23" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A15" s="30" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A29" s="30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>80</v>
-      </c>
-      <c r="B46" t="s">
-        <v>81</v>
-      </c>
-      <c r="C46" t="s">
-        <v>82</v>
-      </c>
-      <c r="D46" t="s">
-        <v>83</v>
-      </c>
-      <c r="E46" t="s">
-        <v>84</v>
-      </c>
-      <c r="F46" t="s">
-        <v>85</v>
-      </c>
-      <c r="G46" t="s">
-        <v>86</v>
-      </c>
-      <c r="H46" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>88</v>
-      </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
-      <c r="C47">
-        <v>81</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>1934</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="H47">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>89</v>
-      </c>
-      <c r="B48">
-        <v>0</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>90</v>
-      </c>
-      <c r="B49">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" t="s">
+        <v>64</v>
+      </c>
+      <c r="E50" t="s">
+        <v>65</v>
+      </c>
+      <c r="F50" t="s">
+        <v>66</v>
+      </c>
+      <c r="G50" t="s">
+        <v>67</v>
+      </c>
+      <c r="H50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51">
         <v>0</v>
       </c>
-      <c r="C49">
+      <c r="C51">
+        <v>81</v>
+      </c>
+      <c r="D51">
         <v>0</v>
       </c>
-      <c r="D49">
+      <c r="E51">
+        <v>1934</v>
+      </c>
+      <c r="F51">
         <v>0</v>
       </c>
-      <c r="E49">
+      <c r="G51">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="H51">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52">
         <v>0</v>
       </c>
-      <c r="F49">
+      <c r="C52">
         <v>0</v>
       </c>
-      <c r="G49">
+      <c r="D52">
         <v>0</v>
       </c>
-      <c r="H49">
+      <c r="E52">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C50" t="s">
-        <v>91</v>
-      </c>
-      <c r="E50" t="s">
-        <v>92</v>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E54" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated results for clang multicore
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="701" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{749E5523-D324-42A4-9171-E975C9714D0F}"/>
+  <xr:revisionPtr revIDLastSave="727" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{CA48287C-34B7-42BB-902A-03FC98EF6831}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="146">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -304,9 +304,6 @@
     <t>vm.pmap.pde.p_failures: 3501</t>
   </si>
   <si>
-    <t>vm.pmap.pde.mappings: 2868</t>
-  </si>
-  <si>
     <t xml:space="preserve">   -1: 226720K,    128</t>
   </si>
   <si>
@@ -334,9 +331,6 @@
     <t>kern.ipc.shm_use_phys="0":</t>
   </si>
   <si>
-    <t>After running one round of "pgbench -j 1 -c 2 -t 4000000 -S pgbench"</t>
-  </si>
-  <si>
     <t>After running one rounds of "pgbench -j 1 -c 2 -t 4000000 -S pgbench"</t>
   </si>
   <si>
@@ -397,21 +391,12 @@
     <t>Running "pgbench -j 1 -c 2 -t 4000000 -S pgbench"</t>
   </si>
   <si>
-    <t>Compile SQLite by make using clang</t>
-  </si>
-  <si>
     <t>(shared_ptp + super_page) / baseline (col I/col B)</t>
   </si>
   <si>
     <t>Run four instances of "clang -c test.c"concurrently  for 10,000 times per iteration on each thread of the same two cores at 3.5 GHz. The results are system-level averages across 5 iterations</t>
   </si>
   <si>
-    <t xml:space="preserve">   -1: 235520K,    131</t>
-  </si>
-  <si>
-    <t>vm.reserv.freed: 2526</t>
-  </si>
-  <si>
     <t>After executes " dd if=/usr/bin/clang of=/dev/null" to force using super page on clang binary</t>
   </si>
   <si>
@@ -434,6 +419,105 @@
   </si>
   <si>
     <t>vm.reserv.freed: 2605</t>
+  </si>
+  <si>
+    <t>Compile SQLite by make using clang by 1 round</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">vm.pmap.pde.mappings: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2868</t>
+    </r>
+  </si>
+  <si>
+    <t>With superpage mapping forcing patch, after the first round of "pgbench -j 1 -c 2 -t 4000000 -S pgbench"</t>
+  </si>
+  <si>
+    <t>After running one round (first round) of "pgbench -j 1 -c 2 -t 4000000 -S pgbench"</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.promotions: 2857</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 230632K,    130</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 3449</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">vm.pmap.pde.mappings: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7363</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 232672K,    131</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 3529</t>
+  </si>
+  <si>
+    <t>With superpage mapping forcing patch, after running another round of "pgbench -j 1 -c 2 -t 4000000 -S pgbench"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">vm.pmap.pde.mappings: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>12398</t>
+    </r>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 3594</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">vm.pmap.pde.mappings: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>17423</t>
+    </r>
+  </si>
+  <si>
+    <t>vm.pmap.pde.mappings: 1170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 228896K,    139</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 4204</t>
   </si>
 </sst>
 </file>
@@ -445,7 +529,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -575,6 +659,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -615,7 +721,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -702,6 +808,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -723,11 +833,33 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1011,7 +1143,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670D2A71-BD87-4620-9FEC-7336DAF0F286}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1035,22 +1169,22 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="57" x14ac:dyDescent="0.45">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56" t="s">
+      <c r="C3" s="58"/>
+      <c r="D3" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56" t="s">
+      <c r="E3" s="58"/>
+      <c r="F3" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="56"/>
-      <c r="H3" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="I3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="60"/>
       <c r="J3" s="38" t="s">
         <v>45</v>
       </c>
@@ -1058,14 +1192,14 @@
         <v>46</v>
       </c>
       <c r="L3" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="M3" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="M3" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
     </row>
     <row r="4" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
@@ -1108,7 +1242,7 @@
         <v>43</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
@@ -3031,7 +3165,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
@@ -3046,29 +3180,29 @@
     </row>
     <row r="5" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59" t="s">
+      <c r="C5" s="61"/>
+      <c r="D5" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60" t="s">
+      <c r="E5" s="61"/>
+      <c r="F5" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="59"/>
+      <c r="G5" s="61"/>
       <c r="H5" s="8" t="s">
         <v>45</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="60" t="s">
+      <c r="J5" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
     </row>
     <row r="6" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
@@ -3349,8 +3483,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A1" s="63" t="s">
-        <v>120</v>
+      <c r="A1" s="56" t="s">
+        <v>118</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -3412,29 +3546,29 @@
     </row>
     <row r="5" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="4"/>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61" t="s">
+      <c r="C5" s="63"/>
+      <c r="D5" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="61"/>
-      <c r="F5" s="62" t="s">
+      <c r="E5" s="63"/>
+      <c r="F5" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="61"/>
+      <c r="G5" s="63"/>
       <c r="H5" s="29" t="s">
         <v>45</v>
       </c>
       <c r="I5" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="62" t="s">
+      <c r="J5" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
     </row>
     <row r="6" spans="1:12" ht="57" x14ac:dyDescent="0.45">
       <c r="A6" s="30" t="s">
@@ -3701,7 +3835,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3710,27 +3844,30 @@
     <col min="2" max="2" width="26.46484375" customWidth="1"/>
     <col min="3" max="3" width="28.06640625" customWidth="1"/>
     <col min="4" max="4" width="28.73046875" customWidth="1"/>
+    <col min="6" max="6" width="27.73046875" customWidth="1"/>
+    <col min="7" max="7" width="28.53125" customWidth="1"/>
+    <col min="8" max="8" width="29.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="31" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="23" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="32" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="32"/>
     </row>
-    <row r="5" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.45">
       <c r="A5" s="23" t="s">
         <v>76</v>
       </c>
@@ -3738,13 +3875,22 @@
         <v>77</v>
       </c>
       <c r="C5" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="33" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F5" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -3755,10 +3901,19 @@
         <v>88</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+        <v>93</v>
+      </c>
+      <c r="F6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" t="s">
+        <v>133</v>
+      </c>
+      <c r="H6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -3769,10 +3924,19 @@
         <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+        <v>94</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -3780,13 +3944,22 @@
         <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+        <v>95</v>
+      </c>
+      <c r="F8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" t="s">
+        <v>140</v>
+      </c>
+      <c r="H8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -3799,8 +3972,17 @@
       <c r="D9" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -3813,8 +3995,17 @@
       <c r="D10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -3827,8 +4018,17 @@
       <c r="D11" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -3841,8 +4041,17 @@
       <c r="D12" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -3850,13 +4059,22 @@
         <v>85</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+        <v>96</v>
+      </c>
+      <c r="F14" t="s">
+        <v>134</v>
+      </c>
+      <c r="G14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -3864,13 +4082,22 @@
         <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+        <v>91</v>
+      </c>
+      <c r="F16" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -3878,13 +4105,22 @@
         <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+        <v>97</v>
+      </c>
+      <c r="F17" t="s">
+        <v>135</v>
+      </c>
+      <c r="G17" t="s">
+        <v>138</v>
+      </c>
+      <c r="H17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -3897,16 +4133,25 @@
       <c r="D18" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="F18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A19" s="27"/>
     </row>
-    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="31" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A22" s="23" t="s">
         <v>76</v>
       </c>
@@ -3914,13 +4159,13 @@
         <v>77</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -3928,13 +4173,13 @@
         <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D23" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -3942,13 +4187,13 @@
         <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D24" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -3956,13 +4201,13 @@
         <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -3976,7 +4221,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -3990,7 +4235,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -4004,7 +4249,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -4018,18 +4263,18 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" t="s">
         <v>103</v>
       </c>
-      <c r="B31" t="s">
-        <v>105</v>
-      </c>
       <c r="C31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D31" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
@@ -4040,24 +4285,24 @@
         <v>86</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" t="s">
         <v>104</v>
       </c>
-      <c r="B34" t="s">
-        <v>106</v>
-      </c>
       <c r="C34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
@@ -4198,6 +4443,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4205,8 +4451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440270B8-E650-47B8-847B-14A2543F142D}">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4230,22 +4476,22 @@
     </row>
     <row r="3" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59" t="s">
+      <c r="C3" s="61"/>
+      <c r="D3" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60" t="s">
+      <c r="E3" s="61"/>
+      <c r="F3" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="59"/>
-      <c r="H3" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="I3" s="58"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="60"/>
       <c r="J3" s="53" t="s">
         <v>45</v>
       </c>
@@ -4253,13 +4499,13 @@
         <v>46</v>
       </c>
       <c r="L3" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="M3" s="60" t="s">
+        <v>115</v>
+      </c>
+      <c r="M3" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
     </row>
     <row r="4" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -6067,8 +6313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6091,29 +6337,29 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59" t="s">
+      <c r="C3" s="61"/>
+      <c r="D3" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60" t="s">
+      <c r="E3" s="61"/>
+      <c r="F3" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="59"/>
+      <c r="G3" s="61"/>
       <c r="H3" s="8" t="s">
         <v>45</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -7137,7 +7383,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="34" t="s">
         <v>15</v>
       </c>
       <c r="B28" s="37">
@@ -7582,555 +7828,554 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF0FC0F-9CDB-4345-A574-CC78D085172F}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="32.9296875" customWidth="1"/>
-    <col min="2" max="2" width="16.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.9296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.9296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.9296875" style="66" customWidth="1"/>
+    <col min="2" max="2" width="16.9296875" style="66" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" style="66" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.9296875" style="66" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.3984375" style="66" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.9296875" style="66" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" style="66" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.9296875" style="66" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.3984375" style="66" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="66"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="31" t="s">
-        <v>121</v>
+      <c r="A1" s="65" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="31"/>
-      <c r="B2" s="59" t="s">
+      <c r="A2" s="65"/>
+      <c r="B2" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59" t="s">
+      <c r="C2" s="67"/>
+      <c r="D2" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="59"/>
-      <c r="F2" s="60" t="s">
+      <c r="E2" s="67"/>
+      <c r="F2" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="59"/>
-      <c r="H2" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="I2" s="58"/>
-      <c r="J2" s="53" t="s">
+      <c r="G2" s="67"/>
+      <c r="H2" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="68"/>
+      <c r="J2" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="M2" s="60" t="s">
+      <c r="L2" s="71" t="s">
+        <v>115</v>
+      </c>
+      <c r="M2" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
     </row>
     <row r="3" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="31"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="65"/>
+      <c r="B3" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="54"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="3" t="s">
+      <c r="J3" s="69"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="P3" s="64" t="s">
-        <v>122</v>
+      <c r="P3" s="74" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="A4" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="75">
         <v>15493779083.6</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="75">
         <v>269378983.61299998</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="75">
         <v>15367176388.4</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="75">
         <v>233620359.995</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="75">
         <v>15237536778</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="75">
         <v>68019754.890799999</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="75">
         <v>15271385968</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="75">
         <v>75985835.517000005</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="75">
         <f>D4/B4</f>
         <v>0.99182880467593548</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="75">
         <f>F4/B4</f>
         <v>0.98346160067099253</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="75">
         <f>H4/B4</f>
         <v>0.98564629620701116</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="75">
         <f>C4/B4</f>
         <v>1.7386267234062655E-2</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="75">
         <f>E4/B4</f>
         <v>1.5078332970571696E-2</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="75">
         <f>G4/B4</f>
         <v>4.3901332608258358E-3</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="75">
         <f>I4/B4</f>
         <v>4.9042802990156356E-3</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="A5" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="75">
         <v>13359320945</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="75">
         <v>184113319.08199999</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="75">
         <v>13208793116.799999</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="75">
         <v>231210962.28</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="75">
         <v>13138638115.4</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="75">
         <v>78633552.787900001</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="75">
         <v>13096325414.200001</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="75">
         <v>31473296.476199999</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="75">
         <f t="shared" ref="J5:J11" si="0">D5/B5</f>
         <v>0.98873237428610927</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="75">
         <f t="shared" ref="K5:K11" si="1">F5/B5</f>
         <v>0.98348098451197141</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="75">
         <f t="shared" ref="L5:L11" si="2">H5/B5</f>
         <v>0.98031370517388228</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="75">
         <f t="shared" ref="M5:M11" si="3">C5/B5</f>
         <v>1.378163754280551E-2</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="75">
         <f t="shared" ref="N5:N11" si="4">E5/B5</f>
         <v>1.7307089427066685E-2</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="75">
         <f t="shared" ref="O5:O11" si="5">G5/B5</f>
         <v>5.8860441418865849E-3</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="75">
         <f t="shared" ref="P5:P11" si="6">I5/B5</f>
         <v>2.3559054090978725E-3</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="75">
         <v>772108.4</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="75">
         <v>20840.3923053</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="75">
         <v>778058</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="75">
         <v>66931.412634099994</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="75">
         <v>893528</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="75">
         <v>20788.819706800001</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="75">
         <v>883725.4</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="75">
         <v>11119.290581699999</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="75">
         <f t="shared" si="0"/>
         <v>1.0077056537657147</v>
       </c>
-      <c r="K6" s="65">
+      <c r="K6" s="77">
         <f t="shared" si="1"/>
         <v>1.1572571934199913</v>
       </c>
-      <c r="L6" s="65">
+      <c r="L6" s="77">
         <f t="shared" si="2"/>
         <v>1.1445613077127512</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="75">
         <f t="shared" si="3"/>
         <v>2.6991536816980619E-2</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="75">
         <f t="shared" si="4"/>
         <v>8.6686548979521522E-2</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="75">
         <f t="shared" si="5"/>
         <v>2.6924742311830827E-2</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="75">
         <f t="shared" si="6"/>
         <v>1.440120400412688E-2</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="A7" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="75">
         <v>1051803.6000000001</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="75">
         <v>45216.7865714</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="75">
         <v>1010779</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="75">
         <v>128858.43975000001</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="75">
         <v>776760</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="75">
         <v>18222.783508600001</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="75">
         <v>766362.6</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="75">
         <v>6871.7964056000001</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="75">
         <f t="shared" si="0"/>
         <v>0.9609959501945039</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="75">
         <f t="shared" si="1"/>
         <v>0.73850289160447824</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="75">
         <f t="shared" si="2"/>
         <v>0.72861758602081217</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="75">
         <f t="shared" si="3"/>
         <v>4.2989762129926154E-2</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="75">
         <f t="shared" si="4"/>
         <v>0.12251188315955563</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="75">
         <f t="shared" si="5"/>
         <v>1.7325272045655673E-2</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="75">
         <f t="shared" si="6"/>
         <v>6.5333455842896898E-3</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="A8" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="75">
         <v>202052215.80000001</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="75">
         <v>2921223.5882100002</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="75">
         <v>203467213.19999999</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="75">
         <v>4753513.9950299999</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="75">
         <v>197764249.19999999</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="75">
         <v>7106267.3385899998</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="75">
         <v>206681380.19999999</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="75">
         <v>1123113.60931</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="75">
         <f t="shared" si="0"/>
         <v>1.0070031273569433</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="75">
         <f t="shared" si="1"/>
         <v>0.97877792835370614</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="75">
         <f t="shared" si="2"/>
         <v>1.0229107331571268</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="75">
         <f t="shared" si="3"/>
         <v>1.4457765665393906E-2</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="75">
         <f t="shared" si="4"/>
         <v>2.3526166125964355E-2</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="75">
         <f t="shared" si="5"/>
         <v>3.517044992777555E-2</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="75">
         <f t="shared" si="6"/>
         <v>5.5585315155450028E-3</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="75">
         <v>36771523.200000003</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="75">
         <v>803144.46110499999</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="75">
         <v>34548013.799999997</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="75">
         <v>4157049.4423500001</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="75">
         <v>48143153</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="75">
         <v>892664.94822699996</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="75">
         <v>41941492.799999997</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="75">
         <v>594525.30033999996</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="75">
         <f t="shared" si="0"/>
         <v>0.93953175700918456</v>
       </c>
-      <c r="K9" s="65">
+      <c r="K9" s="77">
         <f t="shared" si="1"/>
         <v>1.3092509858280768</v>
       </c>
-      <c r="L9" s="65">
+      <c r="L9" s="77">
         <f t="shared" si="2"/>
         <v>1.1405971020531451</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="75">
         <f t="shared" si="3"/>
         <v>2.1841479253842819E-2</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="75">
         <f t="shared" si="4"/>
         <v>0.11305078170789509</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="75">
         <f t="shared" si="5"/>
         <v>2.4275985070615728E-2</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="75">
         <f t="shared" si="6"/>
         <v>1.6168090103485296E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+      <c r="A10" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="75">
         <v>59642364.200000003</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="75">
         <v>2999024.6089599999</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="75">
         <v>59248842.200000003</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="75">
         <v>8400849.4349600002</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="75">
         <v>43745193</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="75">
         <v>1244984.8977699999</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="75">
         <v>44358163</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="75">
         <v>1172723.6488600001</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="75">
         <f t="shared" si="0"/>
         <v>0.99340197181519507</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="75">
         <f t="shared" si="1"/>
         <v>0.73345839969234483</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="75">
         <f t="shared" si="2"/>
         <v>0.74373582595171506</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="75">
         <f t="shared" si="3"/>
         <v>5.0283462924160874E-2</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="75">
         <f t="shared" si="4"/>
         <v>0.14085372951999781</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="75">
         <f t="shared" si="5"/>
         <v>2.087417080911088E-2</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="75">
         <f t="shared" si="6"/>
         <v>1.9662594945557173E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="A11" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="75">
         <v>248801500.19999999</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="75">
         <v>4715956.1624400001</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="75">
         <v>253422519.59999999</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="75">
         <v>7220355.8324800003</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="75">
         <v>266081221.40000001</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="75">
         <v>4012746.4544000002</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="75">
         <v>271198856.39999998</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="75">
         <v>752691.83418200002</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="75">
         <f t="shared" si="0"/>
         <v>1.0185731171085599</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="75">
         <f t="shared" si="1"/>
         <v>1.069451836850299</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="75">
         <f t="shared" si="2"/>
         <v>1.0900209853316631</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="75">
         <f t="shared" si="3"/>
         <v>1.8954693434923269E-2</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11" s="75">
         <f t="shared" si="4"/>
         <v>2.9020547812918698E-2</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="75">
         <f t="shared" si="5"/>
         <v>1.6128304898380193E-2</v>
       </c>
-      <c r="P11" s="6">
+      <c r="P11" s="75">
         <f t="shared" si="6"/>
         <v>3.0252704809936677E-3</v>
       </c>
@@ -8152,8 +8397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1580D30-4320-4334-B527-1D249D93CFB5}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8172,27 +8417,27 @@
   <sheetData>
     <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="31" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="31"/>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59" t="s">
+      <c r="C2" s="61"/>
+      <c r="D2" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="59"/>
-      <c r="F2" s="60" t="s">
+      <c r="E2" s="61"/>
+      <c r="F2" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="59"/>
-      <c r="H2" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="I2" s="58"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="60"/>
       <c r="J2" s="53" t="s">
         <v>45</v>
       </c>
@@ -8200,13 +8445,13 @@
         <v>46</v>
       </c>
       <c r="L2" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="M2" s="60" t="s">
+        <v>115</v>
+      </c>
+      <c r="M2" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
     </row>
     <row r="3" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="31"/>
@@ -8246,8 +8491,8 @@
       <c r="O3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="P3" s="64" t="s">
-        <v>122</v>
+      <c r="P3" s="57" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
@@ -8723,45 +8968,45 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="B5" sqref="B5:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34.3984375" customWidth="1"/>
-    <col min="2" max="2" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="31"/>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59" t="s">
+      <c r="C3" s="61"/>
+      <c r="D3" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60" t="s">
+      <c r="E3" s="61"/>
+      <c r="F3" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="59"/>
-      <c r="H3" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="I3" s="58"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="60"/>
       <c r="J3" s="53" t="s">
         <v>45</v>
       </c>
@@ -8769,13 +9014,13 @@
         <v>46</v>
       </c>
       <c r="L3" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="M3" s="60" t="s">
+        <v>115</v>
+      </c>
+      <c r="M3" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
     </row>
     <row r="4" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="31"/>
@@ -8815,8 +9060,8 @@
       <c r="O4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="P4" s="64" t="s">
-        <v>122</v>
+      <c r="P4" s="57" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
@@ -8824,56 +9069,56 @@
         <v>1</v>
       </c>
       <c r="B5" s="6">
-        <v>161920530400</v>
+        <v>323833414850</v>
       </c>
       <c r="C5" s="6">
-        <v>1118377832.23</v>
+        <v>2243297199.8099999</v>
       </c>
       <c r="D5" s="6">
-        <v>75824438032.600006</v>
+        <v>151628607505</v>
       </c>
       <c r="E5" s="6">
-        <v>232939406.671</v>
+        <v>453500083.074</v>
       </c>
       <c r="F5" s="6">
-        <v>79870556064.199997</v>
+        <v>159735523498</v>
       </c>
       <c r="G5" s="6">
-        <v>44740481.014700003</v>
+        <v>85430315.095100001</v>
       </c>
       <c r="H5" s="6">
-        <v>67743673836.400002</v>
+        <v>135501610356</v>
       </c>
       <c r="I5" s="6">
-        <v>17972324.0865</v>
+        <v>34339293.133299999</v>
       </c>
       <c r="J5" s="6">
         <f>D5/B5</f>
-        <v>0.46828180370510947</v>
+        <v>0.46823027072494833</v>
       </c>
       <c r="K5" s="6">
         <f>F5/B5</f>
-        <v>0.49327009902260049</v>
+        <v>0.49326448776754456</v>
       </c>
       <c r="L5" s="6">
         <f>H5/B5</f>
-        <v>0.41837606181902676</v>
+        <v>0.41842998326397074</v>
       </c>
       <c r="M5" s="6">
         <f>C5/B5</f>
-        <v>6.9069550937562885E-3</v>
+        <v>6.927318482093942E-3</v>
       </c>
       <c r="N5" s="6">
         <f>E5/B5</f>
-        <v>1.4386032833239781E-3</v>
+        <v>1.4004116384470754E-3</v>
       </c>
       <c r="O5" s="6">
         <f>G5/B5</f>
-        <v>2.7631135412029261E-4</v>
+        <v>2.6380945009850642E-4</v>
       </c>
       <c r="P5" s="6">
         <f>I5/B5</f>
-        <v>1.109947209418232E-4</v>
+        <v>1.0603999327619109E-4</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.45">
@@ -8881,56 +9126,56 @@
         <v>2</v>
       </c>
       <c r="B6" s="6">
-        <v>161912884449</v>
+        <v>344917005871</v>
       </c>
       <c r="C6" s="6">
-        <v>1125010974.4300001</v>
+        <v>5771055084.4899998</v>
       </c>
       <c r="D6" s="6">
-        <v>75804169472.199997</v>
+        <v>268554651948</v>
       </c>
       <c r="E6" s="6">
-        <v>220663959.68799999</v>
+        <v>1527986699.4200001</v>
       </c>
       <c r="F6" s="6">
-        <v>79864967433.600006</v>
+        <v>279199707592</v>
       </c>
       <c r="G6" s="6">
-        <v>41447177.850599997</v>
+        <v>103894355.98100001</v>
       </c>
       <c r="H6" s="6">
-        <v>67757936519.199997</v>
+        <v>249053398032</v>
       </c>
       <c r="I6" s="6">
-        <v>18265238.058899999</v>
+        <v>263643857.17199999</v>
       </c>
       <c r="J6" s="6">
         <f t="shared" ref="J6:J12" si="0">D6/B6</f>
-        <v>0.46817873531292137</v>
+        <v>0.77860658470530808</v>
       </c>
       <c r="K6" s="6">
         <f t="shared" ref="K6:K12" si="1">F6/B6</f>
-        <v>0.49325887624932163</v>
+        <v>0.80946924286018396</v>
       </c>
       <c r="L6" s="6">
         <f t="shared" ref="L6:L12" si="2">H6/B6</f>
-        <v>0.41848390725534063</v>
+        <v>0.72206760986771035</v>
       </c>
       <c r="M6" s="6">
         <f t="shared" ref="M6:M12" si="3">C6/B6</f>
-        <v>6.9482486107173315E-3</v>
+        <v>1.6731720924912562E-2</v>
       </c>
       <c r="N6" s="6">
         <f t="shared" ref="N6:N12" si="4">E6/B6</f>
-        <v>1.3628560842389641E-3</v>
+        <v>4.4300126506127439E-3</v>
       </c>
       <c r="O6" s="6">
         <f t="shared" ref="O6:O12" si="5">G6/B6</f>
-        <v>2.5598443256475491E-4</v>
+        <v>3.0121552203157186E-4</v>
       </c>
       <c r="P6" s="6">
         <f t="shared" ref="P6:P12" si="6">I6/B6</f>
-        <v>1.1280904617972673E-4</v>
+        <v>7.6436897191031392E-4</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.45">
@@ -8938,56 +9183,56 @@
         <v>35</v>
       </c>
       <c r="B7" s="6">
-        <v>172452880170</v>
+        <v>4511528</v>
       </c>
       <c r="C7" s="6">
-        <v>2879684751.0100002</v>
+        <v>208635.12502899999</v>
       </c>
       <c r="D7" s="6">
-        <v>134295608237</v>
+        <v>3782812.6</v>
       </c>
       <c r="E7" s="6">
-        <v>775836367.16299999</v>
+        <v>14869.4190418</v>
       </c>
       <c r="F7" s="6">
-        <v>139532253479</v>
+        <v>3832780.4</v>
       </c>
       <c r="G7" s="6">
-        <v>48827656.841899998</v>
+        <v>16005.149291399999</v>
       </c>
       <c r="H7" s="6">
-        <v>124422036123</v>
+        <v>2827524.8</v>
       </c>
       <c r="I7" s="6">
-        <v>142929596.377</v>
+        <v>7654.0007943600003</v>
       </c>
       <c r="J7" s="6">
         <f t="shared" si="0"/>
-        <v>0.77873798399084171</v>
+        <v>0.83847703039857013</v>
       </c>
       <c r="K7" s="6">
         <f t="shared" si="1"/>
-        <v>0.80910364234828891</v>
+        <v>0.84955261277332206</v>
       </c>
       <c r="L7" s="6">
         <f t="shared" si="2"/>
-        <v>0.72148424543763889</v>
+        <v>0.62673329302178771</v>
       </c>
       <c r="M7" s="6">
         <f t="shared" si="3"/>
-        <v>1.6698385948505323E-2</v>
+        <v>4.6244891980943038E-2</v>
       </c>
       <c r="N7" s="6">
         <f t="shared" si="4"/>
-        <v>4.4988310221215138E-3</v>
+        <v>3.2958720508439714E-3</v>
       </c>
       <c r="O7" s="6">
         <f t="shared" si="5"/>
-        <v>2.8313622128993637E-4</v>
+        <v>3.5476116498445757E-3</v>
       </c>
       <c r="P7" s="6">
         <f t="shared" si="6"/>
-        <v>8.2880376504064978E-4</v>
+        <v>1.696542899514311E-3</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
@@ -8995,56 +9240,56 @@
         <v>36</v>
       </c>
       <c r="B8" s="6">
-        <v>172464125701</v>
+        <v>8358082</v>
       </c>
       <c r="C8" s="6">
-        <v>2891438321.4899998</v>
+        <v>242056.925934</v>
       </c>
       <c r="D8" s="6">
-        <v>134259043711</v>
+        <v>7704912.2000000002</v>
       </c>
       <c r="E8" s="6">
-        <v>752643099.25999999</v>
+        <v>125585.31752900001</v>
       </c>
       <c r="F8" s="6">
-        <v>139667454113</v>
+        <v>5671751.2000000002</v>
       </c>
       <c r="G8" s="6">
-        <v>69845308.633100003</v>
+        <v>119284.504275</v>
       </c>
       <c r="H8" s="6">
-        <v>124631361908</v>
+        <v>3989537</v>
       </c>
       <c r="I8" s="6">
-        <v>128797142.83400001</v>
+        <v>112850.02192499999</v>
       </c>
       <c r="J8" s="6">
         <f t="shared" si="0"/>
-        <v>0.77847519398767073</v>
+        <v>0.92185171191189563</v>
       </c>
       <c r="K8" s="6">
         <f t="shared" si="1"/>
-        <v>0.80983481953308145</v>
+        <v>0.67859482594212406</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" si="2"/>
-        <v>0.72265093625367993</v>
+        <v>0.47732685561113186</v>
       </c>
       <c r="M8" s="6">
         <f t="shared" si="3"/>
-        <v>1.6765447943086254E-2</v>
+        <v>2.8960822104162176E-2</v>
       </c>
       <c r="N8" s="6">
         <f t="shared" si="4"/>
-        <v>4.3640559809223906E-3</v>
+        <v>1.5025614432713151E-2</v>
       </c>
       <c r="O8" s="6">
         <f t="shared" si="5"/>
-        <v>4.0498456330675047E-4</v>
+        <v>1.4271755682105057E-2</v>
       </c>
       <c r="P8" s="6">
         <f t="shared" si="6"/>
-        <v>7.4680541423028941E-4</v>
+        <v>1.3501904136020679E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.45">
@@ -9052,56 +9297,56 @@
         <v>15</v>
       </c>
       <c r="B9" s="6">
-        <v>5468028574</v>
+        <v>10917595034.799999</v>
       </c>
       <c r="C9" s="6">
-        <v>7716121.4217999997</v>
+        <v>12027905.988</v>
       </c>
       <c r="D9" s="6">
-        <v>4257250254.8000002</v>
+        <v>8536499054.6000004</v>
       </c>
       <c r="E9" s="6">
-        <v>2753153.9033400002</v>
+        <v>4210427.8809500001</v>
       </c>
       <c r="F9" s="6">
-        <v>4347945362.3999996</v>
+        <v>8712493051.2000008</v>
       </c>
       <c r="G9" s="6">
-        <v>9050676.7055500001</v>
+        <v>13310563.509299999</v>
       </c>
       <c r="H9" s="6">
-        <v>3911189585</v>
+        <v>7865535338.6000004</v>
       </c>
       <c r="I9" s="6">
-        <v>12046007.275599999</v>
+        <v>15078993.797800001</v>
       </c>
       <c r="J9" s="6">
         <f t="shared" si="0"/>
-        <v>0.77857132551260877</v>
+        <v>0.7819028849659454</v>
       </c>
       <c r="K9" s="6">
         <f t="shared" si="1"/>
-        <v>0.79515776180726294</v>
+        <v>0.79802310155568124</v>
       </c>
       <c r="L9" s="6">
         <f t="shared" si="2"/>
-        <v>0.71528331135600975</v>
+        <v>0.72044578623116973</v>
       </c>
       <c r="M9" s="6">
         <f t="shared" si="3"/>
-        <v>1.4111340709683717E-3</v>
+        <v>1.1016992249356079E-3</v>
       </c>
       <c r="N9" s="6">
         <f t="shared" si="4"/>
-        <v>5.0350027730853631E-4</v>
+        <v>3.8565525351775713E-4</v>
       </c>
       <c r="O9" s="6">
         <f t="shared" si="5"/>
-        <v>1.655199233702834E-3</v>
+        <v>1.2191845792843916E-3</v>
       </c>
       <c r="P9" s="6">
         <f t="shared" si="6"/>
-        <v>2.2029890869403493E-3</v>
+        <v>1.381164418513004E-3</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.45">
@@ -9109,56 +9354,56 @@
         <v>4</v>
       </c>
       <c r="B10" s="6">
-        <v>5449566460.8000002</v>
+        <v>329342557.39999998</v>
       </c>
       <c r="C10" s="6">
-        <v>9858668.6322499998</v>
+        <v>367242.755794</v>
       </c>
       <c r="D10" s="6">
-        <v>4279248799.8000002</v>
+        <v>271117999.39999998</v>
       </c>
       <c r="E10" s="6">
-        <v>5423911.4997699996</v>
+        <v>394928.76964999997</v>
       </c>
       <c r="F10" s="6">
-        <v>4364547688.8000002</v>
+        <v>303310294.60000002</v>
       </c>
       <c r="G10" s="6">
-        <v>5106071.7021199996</v>
+        <v>780989.61561400001</v>
       </c>
       <c r="H10" s="6">
-        <v>3954345753.5999999</v>
+        <v>237234451</v>
       </c>
       <c r="I10" s="6">
-        <v>8442598.5826200005</v>
+        <v>629474.45207300002</v>
       </c>
       <c r="J10" s="6">
         <f t="shared" si="0"/>
-        <v>0.78524573112038043</v>
+        <v>0.82320973499551742</v>
       </c>
       <c r="K10" s="6">
         <f t="shared" si="1"/>
-        <v>0.80089814853992647</v>
+        <v>0.9209568814746808</v>
       </c>
       <c r="L10" s="6">
         <f t="shared" si="2"/>
-        <v>0.72562575060686552</v>
+        <v>0.72032734813517918</v>
       </c>
       <c r="M10" s="6">
         <f t="shared" si="3"/>
-        <v>1.809073933342349E-3</v>
+        <v>1.1150783509219207E-3</v>
       </c>
       <c r="N10" s="6">
         <f t="shared" si="4"/>
-        <v>9.9529229321001166E-4</v>
+        <v>1.1991428401108299E-3</v>
       </c>
       <c r="O10" s="6">
         <f t="shared" si="5"/>
-        <v>9.3696842470849043E-4</v>
+        <v>2.3713595405936449E-3</v>
       </c>
       <c r="P10" s="6">
         <f t="shared" si="6"/>
-        <v>1.5492238957630074E-3</v>
+        <v>1.9113061398514544E-3</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
@@ -9166,56 +9411,56 @@
         <v>6</v>
       </c>
       <c r="B11" s="6">
-        <v>164794158</v>
+        <v>1092598050.4000001</v>
       </c>
       <c r="C11" s="6">
-        <v>121426.907028</v>
+        <v>8337252.7442899998</v>
       </c>
       <c r="D11" s="6">
-        <v>134372748</v>
+        <v>1001825975.6</v>
       </c>
       <c r="E11" s="6">
-        <v>272969.07404500002</v>
+        <v>4196491.25153</v>
       </c>
       <c r="F11" s="6">
-        <v>151156817.80000001</v>
+        <v>771608049.20000005</v>
       </c>
       <c r="G11" s="6">
-        <v>253588.58381400001</v>
+        <v>1932350.86785</v>
       </c>
       <c r="H11" s="6">
-        <v>117893003.40000001</v>
+        <v>666503240.60000002</v>
       </c>
       <c r="I11" s="6">
-        <v>275119.49949800002</v>
+        <v>4503514.2328399997</v>
       </c>
       <c r="J11" s="6">
         <f t="shared" si="0"/>
-        <v>0.81539752155534539</v>
+        <v>0.91692088891539902</v>
       </c>
       <c r="K11" s="6">
         <f t="shared" si="1"/>
-        <v>0.91724621573053589</v>
+        <v>0.70621400881826069</v>
       </c>
       <c r="L11" s="6">
         <f t="shared" si="2"/>
-        <v>0.71539552633898595</v>
+        <v>0.61001686791953658</v>
       </c>
       <c r="M11" s="6">
         <f t="shared" si="3"/>
-        <v>7.3683987649610734E-4</v>
+        <v>7.630667784221043E-3</v>
       </c>
       <c r="N11" s="6">
         <f t="shared" si="4"/>
-        <v>1.6564244592032202E-3</v>
+        <v>3.8408372136428991E-3</v>
       </c>
       <c r="O11" s="6">
         <f t="shared" si="5"/>
-        <v>1.538820228166098E-3</v>
+        <v>1.7685834851550086E-3</v>
       </c>
       <c r="P11" s="6">
         <f t="shared" si="6"/>
-        <v>1.6694736199204345E-3</v>
+        <v>4.1218398945442594E-3</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.45">
@@ -9223,56 +9468,56 @@
         <v>20</v>
       </c>
       <c r="B12" s="6">
-        <v>164548399.40000001</v>
+        <v>21119035550.200001</v>
       </c>
       <c r="C12" s="6">
-        <v>395429.66282500001</v>
+        <v>155785034.61300001</v>
       </c>
       <c r="D12" s="6">
-        <v>136745251.40000001</v>
+        <v>18833330851.200001</v>
       </c>
       <c r="E12" s="6">
-        <v>193717.71436300001</v>
+        <v>75611967.094699994</v>
       </c>
       <c r="F12" s="6">
-        <v>152153476.80000001</v>
+        <v>31370492398.200001</v>
       </c>
       <c r="G12" s="6">
-        <v>660576.02424000006</v>
+        <v>80723893.809499994</v>
       </c>
       <c r="H12" s="6">
-        <v>119341447.59999999</v>
+        <v>27275422816.200001</v>
       </c>
       <c r="I12" s="6">
-        <v>678168.13926900004</v>
+        <v>60382890.618000001</v>
       </c>
       <c r="J12" s="6">
         <f t="shared" si="0"/>
-        <v>0.83103361624069372</v>
+        <v>0.89177040336113478</v>
       </c>
       <c r="K12" s="6">
         <f t="shared" si="1"/>
-        <v>0.92467308922361968</v>
+        <v>1.4854131157472727</v>
       </c>
       <c r="L12" s="6">
         <f t="shared" si="2"/>
-        <v>0.72526653577403311</v>
+        <v>1.2915089210094965</v>
       </c>
       <c r="M12" s="6">
         <f t="shared" si="3"/>
-        <v>2.4031206883012683E-3</v>
+        <v>7.3765222016269911E-3</v>
       </c>
       <c r="N12" s="6">
         <f t="shared" si="4"/>
-        <v>1.1772689073206507E-3</v>
+        <v>3.5802755724791578E-3</v>
       </c>
       <c r="O12" s="6">
         <f t="shared" si="5"/>
-        <v>4.0144785768119725E-3</v>
+        <v>3.8223286104907155E-3</v>
       </c>
       <c r="P12" s="6">
         <f t="shared" si="6"/>
-        <v>4.1213900696806171E-3</v>
+        <v>2.859168946160904E-3</v>
       </c>
     </row>
   </sheetData>
@@ -9291,46 +9536,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EB1957-8C0E-4A2E-90B7-11EE02C0E28A}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="35.86328125" customWidth="1"/>
-    <col min="2" max="2" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.46484375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="31"/>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59" t="s">
+      <c r="C3" s="61"/>
+      <c r="D3" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60" t="s">
+      <c r="E3" s="61"/>
+      <c r="F3" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="59"/>
-      <c r="H3" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="I3" s="58"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="60"/>
       <c r="J3" s="53" t="s">
         <v>45</v>
       </c>
@@ -9338,13 +9583,13 @@
         <v>46</v>
       </c>
       <c r="L3" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="M3" s="60" t="s">
+        <v>115</v>
+      </c>
+      <c r="M3" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
     </row>
     <row r="4" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="31"/>
@@ -9384,8 +9629,8 @@
       <c r="O4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="P4" s="64" t="s">
-        <v>122</v>
+      <c r="P4" s="57" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
@@ -9393,56 +9638,56 @@
         <v>1</v>
       </c>
       <c r="B5" s="6">
-        <v>223368116288</v>
+        <v>446771506254</v>
       </c>
       <c r="C5" s="6">
-        <v>450855524.43599999</v>
+        <v>905336131.699</v>
       </c>
       <c r="D5" s="6">
-        <v>223305075907</v>
+        <v>446614573821</v>
       </c>
       <c r="E5" s="6">
-        <v>114201772.119</v>
+        <v>224275324.10600001</v>
       </c>
       <c r="F5" s="6">
-        <v>229856783383</v>
+        <v>459711545632</v>
       </c>
       <c r="G5" s="6">
-        <v>61051708.182800002</v>
+        <v>123395452.454</v>
       </c>
       <c r="H5" s="6">
-        <v>213355797812</v>
+        <v>426703314244</v>
       </c>
       <c r="I5" s="6">
-        <v>316216619.77999997</v>
+        <v>628741417.37300003</v>
       </c>
       <c r="J5" s="6">
         <f>D5/B5</f>
-        <v>0.99971777359254477</v>
+        <v>0.99964874117797753</v>
       </c>
       <c r="K5" s="6">
         <f>F5/B5</f>
-        <v>1.0290492090045378</v>
+        <v>1.0289634392454816</v>
       </c>
       <c r="L5" s="6">
         <f>H5/B5</f>
-        <v>0.95517570438257804</v>
+        <v>0.9550817549259939</v>
       </c>
       <c r="M5" s="6">
         <f>C5/B5</f>
-        <v>2.0184417182203783E-3</v>
+        <v>2.0263963100285438E-3</v>
       </c>
       <c r="N5" s="6">
         <f>E5/B5</f>
-        <v>5.1127159066763936E-4</v>
+        <v>5.0199110947441274E-4</v>
       </c>
       <c r="O5" s="6">
         <f>G5/B5</f>
-        <v>2.7332328891596549E-4</v>
+        <v>2.7619364871457765E-4</v>
       </c>
       <c r="P5" s="6">
         <f>I5/B5</f>
-        <v>1.4156748287758563E-3</v>
+        <v>1.4072997238448459E-3</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.45">
@@ -9450,56 +9695,56 @@
         <v>2</v>
       </c>
       <c r="B6" s="6">
-        <v>223403389966</v>
+        <v>528624286936</v>
       </c>
       <c r="C6" s="6">
-        <v>455400934.35100001</v>
+        <v>808294894.88800001</v>
       </c>
       <c r="D6" s="6">
-        <v>223309497914</v>
+        <v>451411278250</v>
       </c>
       <c r="E6" s="6">
-        <v>110191719.294</v>
+        <v>269201917.21799999</v>
       </c>
       <c r="F6" s="6">
-        <v>229854762250</v>
+        <v>458572112066</v>
       </c>
       <c r="G6" s="6">
-        <v>62354375.772500001</v>
+        <v>104300790.016</v>
       </c>
       <c r="H6" s="6">
-        <v>213347516432</v>
+        <v>425722742888</v>
       </c>
       <c r="I6" s="6">
-        <v>312708908.85399997</v>
+        <v>605998762.06200004</v>
       </c>
       <c r="J6" s="6">
         <f t="shared" ref="J6:J12" si="0">D6/B6</f>
-        <v>0.99957971966309778</v>
+        <v>0.85393594166181752</v>
       </c>
       <c r="K6" s="6">
         <f t="shared" ref="K6:K12" si="1">F6/B6</f>
-        <v>1.0288776830332871</v>
+        <v>0.86748211044930457</v>
       </c>
       <c r="L6" s="6">
         <f t="shared" ref="L6:L12" si="2">H6/B6</f>
-        <v>0.95498782030330687</v>
+        <v>0.80534086951540651</v>
       </c>
       <c r="M6" s="6">
         <f t="shared" ref="M6:M12" si="3">C6/B6</f>
-        <v>2.0384692211712096E-3</v>
+        <v>1.5290536489971362E-3</v>
       </c>
       <c r="N6" s="6">
         <f t="shared" ref="N6:N12" si="4">E6/B6</f>
-        <v>4.9324103502086604E-4</v>
+        <v>5.0924999828960184E-4</v>
       </c>
       <c r="O6" s="6">
         <f t="shared" ref="O6:O12" si="5">G6/B6</f>
-        <v>2.7911114411464293E-4</v>
+        <v>1.9730608788435706E-4</v>
       </c>
       <c r="P6" s="6">
         <f t="shared" ref="P6:P12" si="6">I6/B6</f>
-        <v>1.3997500615437906E-3</v>
+        <v>1.1463695048414748E-3</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.45">
@@ -9507,56 +9752,56 @@
         <v>35</v>
       </c>
       <c r="B7" s="6">
-        <v>264610863412</v>
+        <v>200378758.80000001</v>
       </c>
       <c r="C7" s="6">
-        <v>409210286.66500002</v>
+        <v>424422.57727900002</v>
       </c>
       <c r="D7" s="6">
-        <v>225885999036</v>
+        <v>110731923.59999999</v>
       </c>
       <c r="E7" s="6">
-        <v>135726616.74900001</v>
+        <v>67603.774890500004</v>
       </c>
       <c r="F7" s="6">
-        <v>229483841336</v>
+        <v>18289506.199999999</v>
       </c>
       <c r="G7" s="6">
-        <v>61668883.782899998</v>
+        <v>21429.9867046</v>
       </c>
       <c r="H7" s="6">
-        <v>212992718012</v>
+        <v>15672405.4</v>
       </c>
       <c r="I7" s="6">
-        <v>281859417.83899999</v>
+        <v>18385.697991599998</v>
       </c>
       <c r="J7" s="6">
         <f t="shared" si="0"/>
-        <v>0.85365353532101496</v>
+        <v>0.55261308265973741</v>
       </c>
       <c r="K7" s="6">
         <f t="shared" si="1"/>
-        <v>0.86725026469791189</v>
+        <v>9.1274675567059149E-2</v>
       </c>
       <c r="L7" s="6">
         <f t="shared" si="2"/>
-        <v>0.80492809427997525</v>
+        <v>7.8213905974149595E-2</v>
       </c>
       <c r="M7" s="6">
         <f t="shared" si="3"/>
-        <v>1.5464606456003971E-3</v>
+        <v>2.1181016382211468E-3</v>
       </c>
       <c r="N7" s="6">
         <f t="shared" si="4"/>
-        <v>5.1292911787099689E-4</v>
+        <v>3.3737994633441156E-4</v>
       </c>
       <c r="O7" s="6">
         <f t="shared" si="5"/>
-        <v>2.3305499626023041E-4</v>
+        <v>1.0694739718389751E-4</v>
       </c>
       <c r="P7" s="6">
         <f t="shared" si="6"/>
-        <v>1.0651846043075862E-3</v>
+        <v>9.1754725409547741E-5</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
@@ -9564,56 +9809,56 @@
         <v>36</v>
       </c>
       <c r="B8" s="6">
-        <v>264013423524</v>
+        <v>98153450</v>
       </c>
       <c r="C8" s="6">
-        <v>456629198.324</v>
+        <v>146248.45193400001</v>
       </c>
       <c r="D8" s="6">
-        <v>225525279214</v>
+        <v>64171459.600000001</v>
       </c>
       <c r="E8" s="6">
-        <v>135554071.308</v>
+        <v>47459.290667300003</v>
       </c>
       <c r="F8" s="6">
-        <v>229088270730</v>
+        <v>28986669.800000001</v>
       </c>
       <c r="G8" s="6">
-        <v>67586969.539700001</v>
+        <v>71447.210502300004</v>
       </c>
       <c r="H8" s="6">
-        <v>212730024875</v>
+        <v>26883251.800000001</v>
       </c>
       <c r="I8" s="6">
-        <v>325594494.15200001</v>
+        <v>31888.826246199998</v>
       </c>
       <c r="J8" s="6">
         <f t="shared" si="0"/>
-        <v>0.85421898706411326</v>
+        <v>0.65378710172693877</v>
       </c>
       <c r="K8" s="6">
         <f t="shared" si="1"/>
-        <v>0.86771448084788327</v>
+        <v>0.29531992813293878</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" si="2"/>
-        <v>0.80575457882224644</v>
+        <v>0.27389003443078158</v>
       </c>
       <c r="M8" s="6">
         <f t="shared" si="3"/>
-        <v>1.7295681114581295E-3</v>
+        <v>1.4899980788652871E-3</v>
       </c>
       <c r="N8" s="6">
         <f t="shared" si="4"/>
-        <v>5.1343628478677536E-4</v>
+        <v>4.8352137054071968E-4</v>
       </c>
       <c r="O8" s="6">
         <f t="shared" si="5"/>
-        <v>2.5599823159581144E-4</v>
+        <v>7.2791338972089115E-4</v>
       </c>
       <c r="P8" s="6">
         <f t="shared" si="6"/>
-        <v>1.2332497711897668E-3</v>
+        <v>3.2488747207764981E-4</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.45">
@@ -9621,56 +9866,56 @@
         <v>15</v>
       </c>
       <c r="B9" s="6">
-        <v>2638098623.5999999</v>
+        <v>5266986648</v>
       </c>
       <c r="C9" s="6">
-        <v>109794568.998</v>
+        <v>218573968.03</v>
       </c>
       <c r="D9" s="6">
-        <v>2556762686.8000002</v>
+        <v>5120191668.8000002</v>
       </c>
       <c r="E9" s="6">
-        <v>2118662.8189099999</v>
+        <v>4540521.1788900001</v>
       </c>
       <c r="F9" s="6">
-        <v>2616025291.8000002</v>
+        <v>5241340864</v>
       </c>
       <c r="G9" s="6">
-        <v>5246679.5850200001</v>
+        <v>7268357.2188100005</v>
       </c>
       <c r="H9" s="6">
-        <v>2424963041.4000001</v>
+        <v>4860084892</v>
       </c>
       <c r="I9" s="6">
-        <v>6528381.8301799996</v>
+        <v>11724740.3805</v>
       </c>
       <c r="J9" s="6">
         <f t="shared" si="0"/>
-        <v>0.96916872778281238</v>
+        <v>0.9721292289100939</v>
       </c>
       <c r="K9" s="6">
         <f t="shared" si="1"/>
-        <v>0.99163286330445144</v>
+        <v>0.99513084317201783</v>
       </c>
       <c r="L9" s="6">
         <f t="shared" si="2"/>
-        <v>0.91920863750379778</v>
+        <v>0.92274486662036437</v>
       </c>
       <c r="M9" s="6">
         <f t="shared" si="3"/>
-        <v>4.1618826535064192E-2</v>
+        <v>4.1498865031867456E-2</v>
       </c>
       <c r="N9" s="6">
         <f t="shared" si="4"/>
-        <v>8.0310220397250803E-4</v>
+        <v>8.6207189847617026E-4</v>
       </c>
       <c r="O9" s="6">
         <f t="shared" si="5"/>
-        <v>1.9888110088394956E-3</v>
+        <v>1.3799839841192626E-3</v>
       </c>
       <c r="P9" s="6">
         <f t="shared" si="6"/>
-        <v>2.4746541966923301E-3</v>
+        <v>2.2260812802614872E-3</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.45">
@@ -9678,56 +9923,56 @@
         <v>4</v>
       </c>
       <c r="B10" s="6">
-        <v>2628888024.4000001</v>
+        <v>11355493836.4</v>
       </c>
       <c r="C10" s="6">
-        <v>108807998.84999999</v>
+        <v>127970604.134</v>
       </c>
       <c r="D10" s="6">
-        <v>2563428982</v>
+        <v>5203680046.8000002</v>
       </c>
       <c r="E10" s="6">
-        <v>4836580.0210699998</v>
+        <v>3470245.6611100002</v>
       </c>
       <c r="F10" s="6">
-        <v>2625315572.1999998</v>
+        <v>1075298464</v>
       </c>
       <c r="G10" s="6">
-        <v>2353283.4302500002</v>
+        <v>2746502.6315899999</v>
       </c>
       <c r="H10" s="6">
-        <v>2435121850.5999999</v>
+        <v>962083587.60000002</v>
       </c>
       <c r="I10" s="6">
-        <v>5986719.8161000004</v>
+        <v>4240447.3037599996</v>
       </c>
       <c r="J10" s="6">
         <f t="shared" si="0"/>
-        <v>0.97510010247966339</v>
+        <v>0.45825220124902188</v>
       </c>
       <c r="K10" s="6">
         <f t="shared" si="1"/>
-        <v>0.99864107859793094</v>
+        <v>9.4694117181688228E-2</v>
       </c>
       <c r="L10" s="6">
         <f t="shared" si="2"/>
-        <v>0.92629348530574096</v>
+        <v>8.4724064092751655E-2</v>
       </c>
       <c r="M10" s="6">
         <f t="shared" si="3"/>
-        <v>4.1389362285536524E-2</v>
+        <v>1.1269488229898962E-2</v>
       </c>
       <c r="N10" s="6">
         <f t="shared" si="4"/>
-        <v>1.8397816781009031E-3</v>
+        <v>3.0560059395973947E-4</v>
       </c>
       <c r="O10" s="6">
         <f t="shared" si="5"/>
-        <v>8.9516305312665339E-4</v>
+        <v>2.4186553849257479E-4</v>
       </c>
       <c r="P10" s="6">
         <f t="shared" si="6"/>
-        <v>2.2772821666553751E-3</v>
+        <v>3.7342693896475545E-4</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
@@ -9735,56 +9980,56 @@
         <v>6</v>
       </c>
       <c r="B11" s="6">
-        <v>5672297848.3999996</v>
+        <v>5786223260</v>
       </c>
       <c r="C11" s="6">
-        <v>63327913.115199998</v>
+        <v>62037027.294799998</v>
       </c>
       <c r="D11" s="6">
-        <v>2599365330.8000002</v>
+        <v>3438909717.4000001</v>
       </c>
       <c r="E11" s="6">
-        <v>2680185.4322500001</v>
+        <v>4621022.9611</v>
       </c>
       <c r="F11" s="6">
-        <v>535336536</v>
+        <v>1887519431</v>
       </c>
       <c r="G11" s="6">
-        <v>1562906.19405</v>
+        <v>7494212.3056699997</v>
       </c>
       <c r="H11" s="6">
-        <v>479455306</v>
+        <v>1737596097.2</v>
       </c>
       <c r="I11" s="6">
-        <v>1861514.7493</v>
+        <v>4339269.4783800002</v>
       </c>
       <c r="J11" s="6">
         <f t="shared" si="0"/>
-        <v>0.45825614244379115</v>
+        <v>0.59432717385329514</v>
       </c>
       <c r="K11" s="6">
         <f t="shared" si="1"/>
-        <v>9.4377367040238164E-2</v>
+        <v>0.32620922943785613</v>
       </c>
       <c r="L11" s="6">
         <f t="shared" si="2"/>
-        <v>8.4525763423237948E-2</v>
+        <v>0.30029883381997258</v>
       </c>
       <c r="M11" s="6">
         <f t="shared" si="3"/>
-        <v>1.1164419571701983E-2</v>
+        <v>1.0721505981917468E-2</v>
       </c>
       <c r="N11" s="6">
         <f t="shared" si="4"/>
-        <v>4.7250435429902664E-4</v>
+        <v>7.9862507087222212E-4</v>
       </c>
       <c r="O11" s="6">
         <f t="shared" si="5"/>
-        <v>2.7553316765459578E-4</v>
+        <v>1.295182015785198E-3</v>
       </c>
       <c r="P11" s="6">
         <f t="shared" si="6"/>
-        <v>3.2817648139282432E-4</v>
+        <v>7.4993122169641276E-4</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.45">
@@ -9792,56 +10037,56 @@
         <v>20</v>
       </c>
       <c r="B12" s="6">
-        <v>5683195988</v>
+        <v>22542731297.200001</v>
       </c>
       <c r="C12" s="6">
-        <v>64691020.842799999</v>
+        <v>819742834.50999999</v>
       </c>
       <c r="D12" s="6">
-        <v>2604314716</v>
+        <v>16749732515.200001</v>
       </c>
       <c r="E12" s="6">
-        <v>4124371.66652</v>
+        <v>32618174.876600001</v>
       </c>
       <c r="F12" s="6">
-        <v>539961928</v>
+        <v>17482337767.599998</v>
       </c>
       <c r="G12" s="6">
-        <v>1561794.7929100001</v>
+        <v>11502241.1653</v>
       </c>
       <c r="H12" s="6">
-        <v>482628281.60000002</v>
+        <v>16155439290.799999</v>
       </c>
       <c r="I12" s="6">
-        <v>2626838.7095900001</v>
+        <v>31441946.857299998</v>
       </c>
       <c r="J12" s="6">
         <f t="shared" si="0"/>
-        <v>0.4582482676119175</v>
+        <v>0.74302143313399027</v>
       </c>
       <c r="K12" s="6">
         <f t="shared" si="1"/>
-        <v>9.5010259920671941E-2</v>
+        <v>0.77551994641268041</v>
       </c>
       <c r="L12" s="6">
         <f t="shared" si="2"/>
-        <v>8.4921984499402067E-2</v>
+        <v>0.71665846865710736</v>
       </c>
       <c r="M12" s="6">
         <f t="shared" si="3"/>
-        <v>1.138285939450167E-2</v>
+        <v>3.6363953582315867E-2</v>
       </c>
       <c r="N12" s="6">
         <f t="shared" si="4"/>
-        <v>7.2571343223576336E-4</v>
+        <v>1.4469486614805836E-3</v>
       </c>
       <c r="O12" s="6">
         <f t="shared" si="5"/>
-        <v>2.7480924399012649E-4</v>
+        <v>5.1024168339036528E-4</v>
       </c>
       <c r="P12" s="6">
         <f t="shared" si="6"/>
-        <v>4.6221152941699329E-4</v>
+        <v>1.3947709548933565E-3</v>
       </c>
     </row>
   </sheetData>
@@ -9860,8 +10105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60957CB0-6CA6-420F-AE12-73B8B97534D5}">
   <dimension ref="A2:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9876,10 +10121,10 @@
         <v>76</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -9906,13 +10151,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s">
         <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -9961,13 +10206,13 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" t="s">
         <v>127</v>
-      </c>
-      <c r="C11" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -9975,21 +10220,21 @@
         <v>81</v>
       </c>
       <c r="B13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="B14" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -10012,7 +10257,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65049047-28B8-4D24-A307-ABB41DE3392E}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -10027,7 +10274,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -10089,29 +10336,29 @@
     </row>
     <row r="5" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59" t="s">
+      <c r="C5" s="61"/>
+      <c r="D5" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60" t="s">
+      <c r="E5" s="61"/>
+      <c r="F5" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="59"/>
+      <c r="G5" s="61"/>
       <c r="H5" s="8" t="s">
         <v>45</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="60" t="s">
+      <c r="J5" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
     </row>
     <row r="6" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">

</xml_diff>

<commit_message>
Added postgresql results with the super-page-mapping patch
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="727" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{CA48287C-34B7-42BB-902A-03FC98EF6831}"/>
+  <xr:revisionPtr revIDLastSave="820" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{61CD0F8D-C78C-4CB9-AA06-9534A67CC54F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="153">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -400,25 +400,7 @@
     <t>After executes " dd if=/usr/bin/clang of=/dev/null" to force using super page on clang binary</t>
   </si>
   <si>
-    <t xml:space="preserve">   -1: 223896K,    125</t>
-  </si>
-  <si>
-    <t>vm.reserv.fullpop: 267</t>
-  </si>
-  <si>
-    <t>vm.reserv.freed: 2582</t>
-  </si>
-  <si>
     <t>After executes "clang -c empty.c"</t>
-  </si>
-  <si>
-    <t>vm.pmap.pde.mappings: 1120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   -1: 227968K,    127</t>
-  </si>
-  <si>
-    <t>vm.reserv.freed: 2605</t>
   </si>
   <si>
     <t>Compile SQLite by make using clang by 1 round</t>
@@ -448,49 +430,10 @@
     <t>vm.pmap.pde.promotions: 2857</t>
   </si>
   <si>
-    <t xml:space="preserve">   -1: 230632K,    130</t>
-  </si>
-  <si>
-    <t>vm.reserv.freed: 3449</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">vm.pmap.pde.mappings: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>7363</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">   -1: 232672K,    131</t>
   </si>
   <si>
-    <t>vm.reserv.freed: 3529</t>
-  </si>
-  <si>
     <t>With superpage mapping forcing patch, after running another round of "pgbench -j 1 -c 2 -t 4000000 -S pgbench"</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">vm.pmap.pde.mappings: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>12398</t>
-    </r>
   </si>
   <si>
     <t>vm.reserv.freed: 3594</t>
@@ -511,13 +454,67 @@
     </r>
   </si>
   <si>
-    <t>vm.pmap.pde.mappings: 1170</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   -1: 228896K,    139</t>
-  </si>
-  <si>
-    <t>vm.reserv.freed: 4204</t>
+    <t>vm.pmap.pde.mappings: 1120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 235520K,    131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 223896K,    125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 227968K,    127</t>
+  </si>
+  <si>
+    <t>vm.reserv.fullpop: 267</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 2526</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 2582</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 2605</t>
+  </si>
+  <si>
+    <t>shared_ptp + super_page</t>
+  </si>
+  <si>
+    <t>With the patch for for forcing super page mappings</t>
+  </si>
+  <si>
+    <t>After postgres is start and pgbench is initialized</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.mappings: 2331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 229564K,    128</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 3444</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.mappings: 7372</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 232548K,    131</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 3495</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.mappings: 12396</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 3571</t>
+  </si>
+  <si>
+    <t>Without the super-page-mapping patch</t>
+  </si>
+  <si>
+    <t>With the super-page-mapping patch</t>
   </si>
 </sst>
 </file>
@@ -721,7 +718,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -812,35 +809,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -860,6 +830,44 @@
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1143,8 +1151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670D2A71-BD87-4620-9FEC-7336DAF0F286}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD33"/>
+    <sheetView topLeftCell="E12" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1169,22 +1177,22 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="57" x14ac:dyDescent="0.45">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58" t="s">
+      <c r="C3" s="71"/>
+      <c r="D3" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58" t="s">
+      <c r="E3" s="71"/>
+      <c r="F3" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="58"/>
-      <c r="H3" s="59" t="s">
+      <c r="G3" s="71"/>
+      <c r="H3" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="60"/>
+      <c r="I3" s="73"/>
       <c r="J3" s="38" t="s">
         <v>45</v>
       </c>
@@ -1194,12 +1202,12 @@
       <c r="L3" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="58" t="s">
+      <c r="M3" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
-      <c r="P3" s="58"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
     </row>
     <row r="4" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
@@ -1387,7 +1395,7 @@
       <c r="I7" s="36">
         <v>160538541.021</v>
       </c>
-      <c r="J7" s="41">
+      <c r="J7" s="69">
         <f t="shared" si="0"/>
         <v>0.77503132655099627</v>
       </c>
@@ -1444,7 +1452,7 @@
       <c r="I8" s="36">
         <v>24405.584675599999</v>
       </c>
-      <c r="J8" s="41">
+      <c r="J8" s="69">
         <f t="shared" si="0"/>
         <v>0.84085251810849748</v>
       </c>
@@ -2869,7 +2877,7 @@
       <c r="I33" s="36">
         <v>65031884.0832</v>
       </c>
-      <c r="J33" s="41">
+      <c r="J33" s="69">
         <f t="shared" si="0"/>
         <v>0.93773643745927171</v>
       </c>
@@ -3145,10 +3153,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51140CC8-C0B8-469A-8BAE-C9043CBCBC10}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3160,305 +3168,576 @@
     <col min="5" max="5" width="15.86328125" style="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.3984375" style="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.9296875" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.06640625" style="25"/>
+    <col min="8" max="8" width="19.59765625" style="25" customWidth="1"/>
+    <col min="9" max="9" width="17" style="25" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="23" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="2"/>
-      <c r="B5" s="61" t="s">
+    <row r="5" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="83" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="2"/>
+      <c r="B6" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61" t="s">
+      <c r="C6" s="74"/>
+      <c r="D6" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="61"/>
-      <c r="F5" s="62" t="s">
+      <c r="E6" s="74"/>
+      <c r="F6" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="61"/>
-      <c r="H5" s="8" t="s">
+      <c r="G6" s="74"/>
+      <c r="H6" s="72" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" s="73"/>
+      <c r="J6" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="K6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="62" t="s">
+      <c r="L6" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
-    </row>
-    <row r="6" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
+      <c r="M6" s="74"/>
+      <c r="N6" s="74"/>
+    </row>
+    <row r="7" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3" t="s">
+      <c r="H7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="M7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="N7" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B8" s="6">
         <v>946914692983</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C8" s="6">
         <v>1638529605.76</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D8" s="6">
         <v>940390725841</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E8" s="6">
         <v>6669456559.4899998</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F8" s="6">
         <v>944522103276</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G8" s="6">
         <v>6985699539.3500004</v>
       </c>
-      <c r="H7" s="26">
-        <f>D7/B7</f>
+      <c r="J8" s="26">
+        <f>D8/B8</f>
         <v>0.99311029051471578</v>
       </c>
-      <c r="I7" s="26">
-        <f>F7/B7</f>
+      <c r="K8" s="26">
+        <f>F8/B8</f>
         <v>0.99747327850678624</v>
       </c>
-      <c r="J7" s="26">
-        <f>C7/B7</f>
+      <c r="L8" s="26">
+        <f>C8/B8</f>
         <v>1.7303877718892007E-3</v>
       </c>
-      <c r="K7" s="26">
-        <f>E7/B7</f>
+      <c r="M8" s="26">
+        <f>E8/B8</f>
         <v>7.0433552345456497E-3</v>
       </c>
-      <c r="L7" s="26">
-        <f>G7/B7</f>
+      <c r="N8" s="26">
+        <f>G8/B8</f>
         <v>7.3773272197767189E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B9" s="6">
         <v>1200836800110</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C9" s="6">
         <v>827454901.97399998</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D9" s="6">
         <v>1200772331430</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E9" s="6">
         <v>9214310628.6700001</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F9" s="6">
         <v>1151380231060</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G9" s="6">
         <v>10934220055.700001</v>
       </c>
-      <c r="H8" s="26">
-        <f t="shared" ref="H8:H11" si="0">D8/B8</f>
+      <c r="J9" s="26">
+        <f>D9/B9</f>
         <v>0.99994631353736485</v>
       </c>
-      <c r="I8" s="26">
-        <f t="shared" ref="I8:I11" si="1">F8/B8</f>
+      <c r="K9" s="26">
+        <f>F9/B9</f>
         <v>0.95881491219667014</v>
       </c>
-      <c r="J8" s="26">
-        <f t="shared" ref="J8:J11" si="2">C8/B8</f>
+      <c r="L9" s="26">
+        <f>C9/B9</f>
         <v>6.8906524341875834E-4</v>
       </c>
-      <c r="K8" s="26">
-        <f t="shared" ref="K8:K11" si="3">E8/B8</f>
+      <c r="M9" s="26">
+        <f>E9/B9</f>
         <v>7.6732413828639687E-3</v>
       </c>
-      <c r="L8" s="26">
-        <f t="shared" ref="L8:L11" si="4">G8/B8</f>
+      <c r="N9" s="26">
+        <f>G9/B9</f>
         <v>9.1055004765829926E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B10" s="6">
         <v>451472726.19999999</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C10" s="6">
         <v>4509950.1854800005</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D10" s="6">
         <v>414906363.80000001</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E10" s="6">
         <v>5076230.1852000002</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F10" s="6">
         <v>83253569.799999997</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G10" s="6">
         <v>4087614.1338900002</v>
       </c>
-      <c r="H9" s="26">
-        <f t="shared" si="0"/>
+      <c r="J10" s="26">
+        <f>D10/B10</f>
         <v>0.9190064863767623</v>
       </c>
-      <c r="I9" s="26">
-        <f t="shared" si="1"/>
+      <c r="K10" s="26">
+        <f>F10/B10</f>
         <v>0.18440442792798764</v>
       </c>
-      <c r="J9" s="26">
-        <f t="shared" si="2"/>
+      <c r="L10" s="26">
+        <f>C10/B10</f>
         <v>9.9894189034181371E-3</v>
       </c>
-      <c r="K9" s="26">
-        <f t="shared" si="3"/>
+      <c r="M10" s="26">
+        <f>E10/B10</f>
         <v>1.1243713940210991E-2</v>
       </c>
-      <c r="L9" s="26">
-        <f t="shared" si="4"/>
+      <c r="N10" s="26">
+        <f>G10/B10</f>
         <v>9.0539558575221859E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B11" s="6">
         <v>266369123.40000001</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C11" s="6">
         <v>3466899.5721100001</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D11" s="6">
         <v>245947677.80000001</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E11" s="6">
         <v>2917717.71747</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F11" s="6">
         <v>127109755.2</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G11" s="6">
         <v>665387.35145299998</v>
       </c>
-      <c r="H10" s="26">
-        <f t="shared" si="0"/>
+      <c r="J11" s="26">
+        <f>D11/B11</f>
         <v>0.92333403609496578</v>
       </c>
-      <c r="I10" s="26">
-        <f t="shared" si="1"/>
+      <c r="K11" s="26">
+        <f>F11/B11</f>
         <v>0.47719402901334923</v>
       </c>
-      <c r="J10" s="26">
-        <f t="shared" si="2"/>
+      <c r="L11" s="26">
+        <f>C11/B11</f>
         <v>1.3015395808108891E-2</v>
       </c>
-      <c r="K10" s="26">
-        <f t="shared" si="3"/>
+      <c r="M11" s="26">
+        <f>E11/B11</f>
         <v>1.0953663398473309E-2</v>
       </c>
-      <c r="L10" s="26">
-        <f t="shared" si="4"/>
+      <c r="N11" s="26">
+        <f>G11/B11</f>
         <v>2.4979897931105329E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B12" s="6">
         <v>13444549014</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C12" s="6">
         <v>307569910.05299997</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D12" s="6">
         <v>13667780586.799999</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E12" s="6">
         <v>113540871.403</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F12" s="6">
         <v>13323831275.6</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G12" s="6">
         <v>250385375.715</v>
       </c>
-      <c r="H11" s="26">
-        <f t="shared" si="0"/>
+      <c r="J12" s="26">
+        <f>D12/B12</f>
         <v>1.0166038721393738</v>
       </c>
-      <c r="I11" s="26">
-        <f t="shared" si="1"/>
+      <c r="K12" s="26">
+        <f>F12/B12</f>
         <v>0.99102106450173266</v>
       </c>
-      <c r="J11" s="26">
-        <f t="shared" si="2"/>
+      <c r="L12" s="26">
+        <f>C12/B12</f>
         <v>2.2876922813306944E-2</v>
       </c>
-      <c r="K11" s="26">
-        <f t="shared" si="3"/>
+      <c r="M12" s="26">
+        <f>E12/B12</f>
         <v>8.4451230967114085E-3</v>
       </c>
-      <c r="L11" s="26">
-        <f t="shared" si="4"/>
+      <c r="N12" s="26">
+        <f>G12/B12</f>
         <v>1.8623560779485435E-2</v>
       </c>
     </row>
+    <row r="15" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="83" t="s">
+        <v>152</v>
+      </c>
+      <c r="M15" s="80"/>
+      <c r="N15" s="80"/>
+    </row>
+    <row r="16" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A16" s="2"/>
+      <c r="B16" s="74" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="74"/>
+      <c r="F16" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="74"/>
+      <c r="H16" s="72" t="s">
+        <v>114</v>
+      </c>
+      <c r="I16" s="73"/>
+      <c r="J16" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="K16" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16" s="75" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" s="74"/>
+      <c r="N16" s="74"/>
+    </row>
+    <row r="17" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M17" s="82" t="s">
+        <v>30</v>
+      </c>
+      <c r="N17" s="82" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A18" s="80" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="81"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="81">
+        <v>947044998803</v>
+      </c>
+      <c r="E18" s="81">
+        <v>4671101663.8400002</v>
+      </c>
+      <c r="H18" s="81">
+        <v>944883191889</v>
+      </c>
+      <c r="I18" s="81">
+        <v>6989132626.8100004</v>
+      </c>
+      <c r="J18" s="81"/>
+      <c r="K18" s="81"/>
+      <c r="L18" s="81"/>
+      <c r="M18" s="80"/>
+      <c r="N18" s="80"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A19" s="80" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="81"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81">
+        <v>1203651140030</v>
+      </c>
+      <c r="E19" s="81">
+        <v>9785263329.6399994</v>
+      </c>
+      <c r="H19" s="81">
+        <v>1145899823710</v>
+      </c>
+      <c r="I19" s="81">
+        <v>10497091805.6</v>
+      </c>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="80"/>
+      <c r="N19" s="80"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A20" s="80" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81">
+        <v>373726151.39999998</v>
+      </c>
+      <c r="E20" s="81">
+        <v>11967060.9714</v>
+      </c>
+      <c r="H20" s="81">
+        <v>109409320.40000001</v>
+      </c>
+      <c r="I20" s="81">
+        <v>3682064.03516</v>
+      </c>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="80"/>
+      <c r="N20" s="80"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A21" s="80" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="81"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81">
+        <v>178376300</v>
+      </c>
+      <c r="E21" s="81">
+        <v>7016479.1470799996</v>
+      </c>
+      <c r="H21" s="81">
+        <v>72696324.200000003</v>
+      </c>
+      <c r="I21" s="81">
+        <v>1204122.4476600001</v>
+      </c>
+      <c r="J21" s="81"/>
+      <c r="K21" s="81"/>
+      <c r="L21" s="81"/>
+      <c r="M21" s="80"/>
+      <c r="N21" s="80"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A22" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="81"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="81">
+        <v>50047193757.599998</v>
+      </c>
+      <c r="E22" s="81">
+        <v>256065872.794</v>
+      </c>
+      <c r="H22" s="81">
+        <v>49480147960.800003</v>
+      </c>
+      <c r="I22" s="81">
+        <v>676041009.45899999</v>
+      </c>
+      <c r="J22" s="81"/>
+      <c r="K22" s="81"/>
+      <c r="L22" s="81"/>
+      <c r="M22" s="80"/>
+      <c r="N22" s="80"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A23" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="81">
+        <v>19963233833.799999</v>
+      </c>
+      <c r="E23" s="81">
+        <v>208319673.255</v>
+      </c>
+      <c r="H23" s="81">
+        <v>8088796149.8000002</v>
+      </c>
+      <c r="I23" s="81">
+        <v>104743077.28399999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A24" s="80" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="81">
+        <v>11291216904.799999</v>
+      </c>
+      <c r="E24" s="81">
+        <v>101645055.061</v>
+      </c>
+      <c r="H24" s="81">
+        <v>4792947991</v>
+      </c>
+      <c r="I24" s="81">
+        <v>250072949.72400001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A25" s="80" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="81">
+        <v>63401290363.800003</v>
+      </c>
+      <c r="E25" s="81">
+        <v>105764495.332</v>
+      </c>
+      <c r="H25" s="81">
+        <v>63760215368.599998</v>
+      </c>
+      <c r="I25" s="81">
+        <v>554303853.73599994</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="J5:L5"/>
+  <mergeCells count="10">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="H6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3546,29 +3825,29 @@
     </row>
     <row r="5" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="4"/>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63" t="s">
+      <c r="C5" s="78"/>
+      <c r="D5" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="63"/>
-      <c r="F5" s="64" t="s">
+      <c r="E5" s="78"/>
+      <c r="F5" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="63"/>
+      <c r="G5" s="78"/>
       <c r="H5" s="29" t="s">
         <v>45</v>
       </c>
       <c r="I5" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="64" t="s">
+      <c r="J5" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="63"/>
-      <c r="L5" s="63"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
     </row>
     <row r="6" spans="1:12" ht="57" x14ac:dyDescent="0.45">
       <c r="A6" s="30" t="s">
@@ -3832,10 +4111,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5A357B-AD95-4B57-AFAC-6E90E36724A8}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D39" sqref="D39:D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3875,19 +4154,13 @@
         <v>77</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D5" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="33" t="s">
-        <v>131</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>139</v>
-      </c>
       <c r="H5" s="33" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
@@ -3903,14 +4176,8 @@
       <c r="D6" t="s">
         <v>93</v>
       </c>
-      <c r="F6" t="s">
-        <v>133</v>
-      </c>
-      <c r="G6" t="s">
-        <v>133</v>
-      </c>
       <c r="H6" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
@@ -3926,12 +4193,6 @@
       <c r="D7" t="s">
         <v>94</v>
       </c>
-      <c r="F7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" t="s">
-        <v>50</v>
-      </c>
       <c r="H7" t="s">
         <v>50</v>
       </c>
@@ -3944,19 +4205,13 @@
         <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D8" t="s">
         <v>95</v>
       </c>
-      <c r="F8" t="s">
-        <v>136</v>
-      </c>
-      <c r="G8" t="s">
-        <v>140</v>
-      </c>
       <c r="H8" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
@@ -3972,12 +4227,6 @@
       <c r="D9" t="s">
         <v>52</v>
       </c>
-      <c r="F9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" t="s">
-        <v>52</v>
-      </c>
       <c r="H9" t="s">
         <v>52</v>
       </c>
@@ -3995,12 +4244,6 @@
       <c r="D10" t="s">
         <v>53</v>
       </c>
-      <c r="F10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" t="s">
-        <v>53</v>
-      </c>
       <c r="H10" t="s">
         <v>53</v>
       </c>
@@ -4018,12 +4261,6 @@
       <c r="D11" t="s">
         <v>54</v>
       </c>
-      <c r="F11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" t="s">
-        <v>54</v>
-      </c>
       <c r="H11" t="s">
         <v>54</v>
       </c>
@@ -4041,12 +4278,6 @@
       <c r="D12" t="s">
         <v>55</v>
       </c>
-      <c r="F12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" t="s">
-        <v>55</v>
-      </c>
       <c r="H12" t="s">
         <v>55</v>
       </c>
@@ -4064,14 +4295,8 @@
       <c r="D14" t="s">
         <v>96</v>
       </c>
-      <c r="F14" t="s">
-        <v>134</v>
-      </c>
-      <c r="G14" t="s">
-        <v>137</v>
-      </c>
       <c r="H14" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
@@ -4087,12 +4312,6 @@
       <c r="D16" t="s">
         <v>91</v>
       </c>
-      <c r="F16" t="s">
-        <v>91</v>
-      </c>
-      <c r="G16" t="s">
-        <v>91</v>
-      </c>
       <c r="H16" t="s">
         <v>91</v>
       </c>
@@ -4110,14 +4329,8 @@
       <c r="D17" t="s">
         <v>97</v>
       </c>
-      <c r="F17" t="s">
-        <v>135</v>
-      </c>
-      <c r="G17" t="s">
-        <v>138</v>
-      </c>
       <c r="H17" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
@@ -4133,12 +4346,6 @@
       <c r="D18" t="s">
         <v>83</v>
       </c>
-      <c r="F18" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" t="s">
-        <v>56</v>
-      </c>
       <c r="H18" t="s">
         <v>56</v>
       </c>
@@ -4319,125 +4526,262 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A48" s="23" t="s">
-        <v>59</v>
+    <row r="37" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="83" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="80" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A38" s="84" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="80" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="80" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="80" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="80" t="s">
+        <v>143</v>
+      </c>
+      <c r="B41" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="80" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="80" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="80" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" t="s">
+        <v>147</v>
+      </c>
+      <c r="C47" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>86</v>
+      </c>
+      <c r="B49" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>145</v>
       </c>
       <c r="B50" t="s">
-        <v>61</v>
+        <v>148</v>
       </c>
       <c r="C50" t="s">
-        <v>62</v>
-      </c>
-      <c r="D50" t="s">
-        <v>63</v>
-      </c>
-      <c r="E50" t="s">
-        <v>64</v>
-      </c>
-      <c r="F50" t="s">
-        <v>65</v>
-      </c>
-      <c r="G50" t="s">
-        <v>66</v>
-      </c>
-      <c r="H50" t="s">
-        <v>67</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A53" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" t="s">
+        <v>62</v>
+      </c>
+      <c r="D55" t="s">
+        <v>63</v>
+      </c>
+      <c r="E55" t="s">
+        <v>64</v>
+      </c>
+      <c r="F55" t="s">
+        <v>65</v>
+      </c>
+      <c r="G55" t="s">
+        <v>66</v>
+      </c>
+      <c r="H55" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
         <v>68</v>
       </c>
-      <c r="B51">
+      <c r="B56">
         <v>0</v>
       </c>
-      <c r="C51">
+      <c r="C56">
         <v>81</v>
       </c>
-      <c r="D51">
+      <c r="D56">
         <v>0</v>
       </c>
-      <c r="E51">
+      <c r="E56">
         <v>1934</v>
       </c>
-      <c r="F51">
+      <c r="F56">
         <v>0</v>
       </c>
-      <c r="G51">
+      <c r="G56">
         <v>19.899999999999999</v>
       </c>
-      <c r="H51">
+      <c r="H56">
         <v>6.5</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
         <v>69</v>
       </c>
-      <c r="B52">
+      <c r="B57">
         <v>0</v>
       </c>
-      <c r="C52">
+      <c r="C57">
         <v>0</v>
       </c>
-      <c r="D52">
+      <c r="D57">
         <v>0</v>
       </c>
-      <c r="E52">
+      <c r="E57">
         <v>0</v>
       </c>
-      <c r="F52">
+      <c r="F57">
         <v>0</v>
       </c>
-      <c r="G52">
+      <c r="G57">
         <v>0</v>
       </c>
-      <c r="H52">
+      <c r="H57">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
         <v>70</v>
       </c>
-      <c r="B53">
+      <c r="B58">
         <v>0</v>
       </c>
-      <c r="C53">
+      <c r="C58">
         <v>0</v>
       </c>
-      <c r="D53">
+      <c r="D58">
         <v>0</v>
       </c>
-      <c r="E53">
+      <c r="E58">
         <v>0</v>
       </c>
-      <c r="F53">
+      <c r="F58">
         <v>0</v>
       </c>
-      <c r="G53">
+      <c r="G58">
         <v>0</v>
       </c>
-      <c r="H53">
+      <c r="H58">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C54" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C59" t="s">
         <v>71</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E59" t="s">
         <v>72</v>
       </c>
     </row>
@@ -4451,8 +4795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440270B8-E650-47B8-847B-14A2543F142D}">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD33"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4476,22 +4820,22 @@
     </row>
     <row r="3" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61" t="s">
+      <c r="C3" s="74"/>
+      <c r="D3" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="61"/>
-      <c r="F3" s="62" t="s">
+      <c r="E3" s="74"/>
+      <c r="F3" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="59" t="s">
+      <c r="G3" s="74"/>
+      <c r="H3" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="60"/>
+      <c r="I3" s="73"/>
       <c r="J3" s="53" t="s">
         <v>45</v>
       </c>
@@ -4501,11 +4845,11 @@
       <c r="L3" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="62" t="s">
+      <c r="M3" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
     </row>
     <row r="4" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -4682,7 +5026,7 @@
       <c r="I7" s="36">
         <v>162123527.46399999</v>
       </c>
-      <c r="J7" s="55">
+      <c r="J7" s="70">
         <f t="shared" si="0"/>
         <v>0.890188259246386</v>
       </c>
@@ -4735,7 +5079,7 @@
       <c r="I8" s="36">
         <v>35659.240431600003</v>
       </c>
-      <c r="J8" s="55">
+      <c r="J8" s="70">
         <f t="shared" si="0"/>
         <v>0.5741384848907457</v>
       </c>
@@ -6060,7 +6404,7 @@
       <c r="I33" s="36">
         <v>33025471.036600001</v>
       </c>
-      <c r="J33" s="55">
+      <c r="J33" s="70">
         <f t="shared" si="0"/>
         <v>0.83123992083193798</v>
       </c>
@@ -6337,29 +6681,29 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61" t="s">
+      <c r="C3" s="74"/>
+      <c r="D3" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="61"/>
-      <c r="F3" s="62" t="s">
+      <c r="E3" s="74"/>
+      <c r="F3" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="61"/>
+      <c r="G3" s="74"/>
       <c r="H3" s="8" t="s">
         <v>45</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="62" t="s">
+      <c r="J3" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -7832,550 +8176,550 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="32.9296875" style="66" customWidth="1"/>
-    <col min="2" max="2" width="16.9296875" style="66" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.3984375" style="66" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.9296875" style="66" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.3984375" style="66" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.9296875" style="66" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" style="66" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.9296875" style="66" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.3984375" style="66" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.06640625" style="66"/>
+    <col min="1" max="1" width="32.9296875" style="59" customWidth="1"/>
+    <col min="2" max="2" width="16.9296875" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" style="59" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.9296875" style="59" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.3984375" style="59" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.9296875" style="59" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" style="59" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.9296875" style="59" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.3984375" style="59" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="59"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="65" t="s">
-        <v>129</v>
+      <c r="A1" s="58" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="65"/>
-      <c r="B2" s="67" t="s">
+      <c r="A2" s="58"/>
+      <c r="B2" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67" t="s">
+      <c r="C2" s="76"/>
+      <c r="D2" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67" t="s">
+      <c r="E2" s="76"/>
+      <c r="F2" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68" t="s">
+      <c r="G2" s="76"/>
+      <c r="H2" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="68"/>
-      <c r="J2" s="69" t="s">
+      <c r="I2" s="77"/>
+      <c r="J2" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="70" t="s">
+      <c r="K2" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="71" t="s">
+      <c r="L2" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="67" t="s">
+      <c r="M2" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
     </row>
     <row r="3" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="65"/>
-      <c r="B3" s="72" t="s">
+      <c r="A3" s="58"/>
+      <c r="B3" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="72" t="s">
+      <c r="D3" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="72" t="s">
+      <c r="E3" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="72" t="s">
+      <c r="F3" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="72" t="s">
+      <c r="G3" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="72" t="s">
+      <c r="H3" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="72" t="s">
+      <c r="I3" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="69"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="72" t="s">
+      <c r="J3" s="60"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="72" t="s">
+      <c r="N3" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="72" t="s">
+      <c r="O3" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="P3" s="74" t="s">
+      <c r="P3" s="65" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="75">
+      <c r="B4" s="66">
         <v>15493779083.6</v>
       </c>
-      <c r="C4" s="75">
+      <c r="C4" s="66">
         <v>269378983.61299998</v>
       </c>
-      <c r="D4" s="75">
+      <c r="D4" s="66">
         <v>15367176388.4</v>
       </c>
-      <c r="E4" s="75">
+      <c r="E4" s="66">
         <v>233620359.995</v>
       </c>
-      <c r="F4" s="75">
+      <c r="F4" s="66">
         <v>15237536778</v>
       </c>
-      <c r="G4" s="75">
+      <c r="G4" s="66">
         <v>68019754.890799999</v>
       </c>
-      <c r="H4" s="75">
+      <c r="H4" s="66">
         <v>15271385968</v>
       </c>
-      <c r="I4" s="75">
+      <c r="I4" s="66">
         <v>75985835.517000005</v>
       </c>
-      <c r="J4" s="75">
+      <c r="J4" s="66">
         <f>D4/B4</f>
         <v>0.99182880467593548</v>
       </c>
-      <c r="K4" s="75">
+      <c r="K4" s="66">
         <f>F4/B4</f>
         <v>0.98346160067099253</v>
       </c>
-      <c r="L4" s="75">
+      <c r="L4" s="66">
         <f>H4/B4</f>
         <v>0.98564629620701116</v>
       </c>
-      <c r="M4" s="75">
+      <c r="M4" s="66">
         <f>C4/B4</f>
         <v>1.7386267234062655E-2</v>
       </c>
-      <c r="N4" s="75">
+      <c r="N4" s="66">
         <f>E4/B4</f>
         <v>1.5078332970571696E-2</v>
       </c>
-      <c r="O4" s="75">
+      <c r="O4" s="66">
         <f>G4/B4</f>
         <v>4.3901332608258358E-3</v>
       </c>
-      <c r="P4" s="75">
+      <c r="P4" s="66">
         <f>I4/B4</f>
         <v>4.9042802990156356E-3</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="75">
+      <c r="B5" s="66">
         <v>13359320945</v>
       </c>
-      <c r="C5" s="75">
+      <c r="C5" s="66">
         <v>184113319.08199999</v>
       </c>
-      <c r="D5" s="75">
+      <c r="D5" s="66">
         <v>13208793116.799999</v>
       </c>
-      <c r="E5" s="75">
+      <c r="E5" s="66">
         <v>231210962.28</v>
       </c>
-      <c r="F5" s="75">
+      <c r="F5" s="66">
         <v>13138638115.4</v>
       </c>
-      <c r="G5" s="75">
+      <c r="G5" s="66">
         <v>78633552.787900001</v>
       </c>
-      <c r="H5" s="75">
+      <c r="H5" s="66">
         <v>13096325414.200001</v>
       </c>
-      <c r="I5" s="75">
+      <c r="I5" s="66">
         <v>31473296.476199999</v>
       </c>
-      <c r="J5" s="75">
+      <c r="J5" s="66">
         <f t="shared" ref="J5:J11" si="0">D5/B5</f>
         <v>0.98873237428610927</v>
       </c>
-      <c r="K5" s="75">
+      <c r="K5" s="66">
         <f t="shared" ref="K5:K11" si="1">F5/B5</f>
         <v>0.98348098451197141</v>
       </c>
-      <c r="L5" s="75">
+      <c r="L5" s="66">
         <f t="shared" ref="L5:L11" si="2">H5/B5</f>
         <v>0.98031370517388228</v>
       </c>
-      <c r="M5" s="75">
+      <c r="M5" s="66">
         <f t="shared" ref="M5:M11" si="3">C5/B5</f>
         <v>1.378163754280551E-2</v>
       </c>
-      <c r="N5" s="75">
+      <c r="N5" s="66">
         <f t="shared" ref="N5:N11" si="4">E5/B5</f>
         <v>1.7307089427066685E-2</v>
       </c>
-      <c r="O5" s="75">
+      <c r="O5" s="66">
         <f t="shared" ref="O5:O11" si="5">G5/B5</f>
         <v>5.8860441418865849E-3</v>
       </c>
-      <c r="P5" s="75">
+      <c r="P5" s="66">
         <f t="shared" ref="P5:P11" si="6">I5/B5</f>
         <v>2.3559054090978725E-3</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="75">
+      <c r="B6" s="66">
         <v>772108.4</v>
       </c>
-      <c r="C6" s="75">
+      <c r="C6" s="66">
         <v>20840.3923053</v>
       </c>
-      <c r="D6" s="75">
+      <c r="D6" s="66">
         <v>778058</v>
       </c>
-      <c r="E6" s="75">
+      <c r="E6" s="66">
         <v>66931.412634099994</v>
       </c>
-      <c r="F6" s="75">
+      <c r="F6" s="66">
         <v>893528</v>
       </c>
-      <c r="G6" s="75">
+      <c r="G6" s="66">
         <v>20788.819706800001</v>
       </c>
-      <c r="H6" s="75">
+      <c r="H6" s="66">
         <v>883725.4</v>
       </c>
-      <c r="I6" s="75">
+      <c r="I6" s="66">
         <v>11119.290581699999</v>
       </c>
-      <c r="J6" s="75">
+      <c r="J6" s="66">
         <f t="shared" si="0"/>
         <v>1.0077056537657147</v>
       </c>
-      <c r="K6" s="77">
+      <c r="K6" s="68">
         <f t="shared" si="1"/>
         <v>1.1572571934199913</v>
       </c>
-      <c r="L6" s="77">
+      <c r="L6" s="68">
         <f t="shared" si="2"/>
         <v>1.1445613077127512</v>
       </c>
-      <c r="M6" s="75">
+      <c r="M6" s="66">
         <f t="shared" si="3"/>
         <v>2.6991536816980619E-2</v>
       </c>
-      <c r="N6" s="75">
+      <c r="N6" s="66">
         <f t="shared" si="4"/>
         <v>8.6686548979521522E-2</v>
       </c>
-      <c r="O6" s="75">
+      <c r="O6" s="66">
         <f t="shared" si="5"/>
         <v>2.6924742311830827E-2</v>
       </c>
-      <c r="P6" s="75">
+      <c r="P6" s="66">
         <f t="shared" si="6"/>
         <v>1.440120400412688E-2</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="75">
+      <c r="B7" s="66">
         <v>1051803.6000000001</v>
       </c>
-      <c r="C7" s="75">
+      <c r="C7" s="66">
         <v>45216.7865714</v>
       </c>
-      <c r="D7" s="75">
+      <c r="D7" s="66">
         <v>1010779</v>
       </c>
-      <c r="E7" s="75">
+      <c r="E7" s="66">
         <v>128858.43975000001</v>
       </c>
-      <c r="F7" s="75">
+      <c r="F7" s="66">
         <v>776760</v>
       </c>
-      <c r="G7" s="75">
+      <c r="G7" s="66">
         <v>18222.783508600001</v>
       </c>
-      <c r="H7" s="75">
+      <c r="H7" s="66">
         <v>766362.6</v>
       </c>
-      <c r="I7" s="75">
+      <c r="I7" s="66">
         <v>6871.7964056000001</v>
       </c>
-      <c r="J7" s="75">
+      <c r="J7" s="66">
         <f t="shared" si="0"/>
         <v>0.9609959501945039</v>
       </c>
-      <c r="K7" s="75">
+      <c r="K7" s="66">
         <f t="shared" si="1"/>
         <v>0.73850289160447824</v>
       </c>
-      <c r="L7" s="75">
+      <c r="L7" s="66">
         <f t="shared" si="2"/>
         <v>0.72861758602081217</v>
       </c>
-      <c r="M7" s="75">
+      <c r="M7" s="66">
         <f t="shared" si="3"/>
         <v>4.2989762129926154E-2</v>
       </c>
-      <c r="N7" s="75">
+      <c r="N7" s="66">
         <f t="shared" si="4"/>
         <v>0.12251188315955563</v>
       </c>
-      <c r="O7" s="75">
+      <c r="O7" s="66">
         <f t="shared" si="5"/>
         <v>1.7325272045655673E-2</v>
       </c>
-      <c r="P7" s="75">
+      <c r="P7" s="66">
         <f t="shared" si="6"/>
         <v>6.5333455842896898E-3</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="75">
+      <c r="B8" s="66">
         <v>202052215.80000001</v>
       </c>
-      <c r="C8" s="75">
+      <c r="C8" s="66">
         <v>2921223.5882100002</v>
       </c>
-      <c r="D8" s="75">
+      <c r="D8" s="66">
         <v>203467213.19999999</v>
       </c>
-      <c r="E8" s="75">
+      <c r="E8" s="66">
         <v>4753513.9950299999</v>
       </c>
-      <c r="F8" s="75">
+      <c r="F8" s="66">
         <v>197764249.19999999</v>
       </c>
-      <c r="G8" s="75">
+      <c r="G8" s="66">
         <v>7106267.3385899998</v>
       </c>
-      <c r="H8" s="75">
+      <c r="H8" s="66">
         <v>206681380.19999999</v>
       </c>
-      <c r="I8" s="75">
+      <c r="I8" s="66">
         <v>1123113.60931</v>
       </c>
-      <c r="J8" s="75">
+      <c r="J8" s="66">
         <f t="shared" si="0"/>
         <v>1.0070031273569433</v>
       </c>
-      <c r="K8" s="75">
+      <c r="K8" s="66">
         <f t="shared" si="1"/>
         <v>0.97877792835370614</v>
       </c>
-      <c r="L8" s="75">
+      <c r="L8" s="66">
         <f t="shared" si="2"/>
         <v>1.0229107331571268</v>
       </c>
-      <c r="M8" s="75">
+      <c r="M8" s="66">
         <f t="shared" si="3"/>
         <v>1.4457765665393906E-2</v>
       </c>
-      <c r="N8" s="75">
+      <c r="N8" s="66">
         <f t="shared" si="4"/>
         <v>2.3526166125964355E-2</v>
       </c>
-      <c r="O8" s="75">
+      <c r="O8" s="66">
         <f t="shared" si="5"/>
         <v>3.517044992777555E-2</v>
       </c>
-      <c r="P8" s="75">
+      <c r="P8" s="66">
         <f t="shared" si="6"/>
         <v>5.5585315155450028E-3</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="75">
+      <c r="B9" s="66">
         <v>36771523.200000003</v>
       </c>
-      <c r="C9" s="75">
+      <c r="C9" s="66">
         <v>803144.46110499999</v>
       </c>
-      <c r="D9" s="75">
+      <c r="D9" s="66">
         <v>34548013.799999997</v>
       </c>
-      <c r="E9" s="75">
+      <c r="E9" s="66">
         <v>4157049.4423500001</v>
       </c>
-      <c r="F9" s="75">
+      <c r="F9" s="66">
         <v>48143153</v>
       </c>
-      <c r="G9" s="75">
+      <c r="G9" s="66">
         <v>892664.94822699996</v>
       </c>
-      <c r="H9" s="75">
+      <c r="H9" s="66">
         <v>41941492.799999997</v>
       </c>
-      <c r="I9" s="75">
+      <c r="I9" s="66">
         <v>594525.30033999996</v>
       </c>
-      <c r="J9" s="75">
+      <c r="J9" s="66">
         <f t="shared" si="0"/>
         <v>0.93953175700918456</v>
       </c>
-      <c r="K9" s="77">
+      <c r="K9" s="68">
         <f t="shared" si="1"/>
         <v>1.3092509858280768</v>
       </c>
-      <c r="L9" s="77">
+      <c r="L9" s="68">
         <f t="shared" si="2"/>
         <v>1.1405971020531451</v>
       </c>
-      <c r="M9" s="75">
+      <c r="M9" s="66">
         <f t="shared" si="3"/>
         <v>2.1841479253842819E-2</v>
       </c>
-      <c r="N9" s="75">
+      <c r="N9" s="66">
         <f t="shared" si="4"/>
         <v>0.11305078170789509</v>
       </c>
-      <c r="O9" s="75">
+      <c r="O9" s="66">
         <f t="shared" si="5"/>
         <v>2.4275985070615728E-2</v>
       </c>
-      <c r="P9" s="75">
+      <c r="P9" s="66">
         <f t="shared" si="6"/>
         <v>1.6168090103485296E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A10" s="66" t="s">
+      <c r="A10" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="75">
+      <c r="B10" s="66">
         <v>59642364.200000003</v>
       </c>
-      <c r="C10" s="75">
+      <c r="C10" s="66">
         <v>2999024.6089599999</v>
       </c>
-      <c r="D10" s="75">
+      <c r="D10" s="66">
         <v>59248842.200000003</v>
       </c>
-      <c r="E10" s="75">
+      <c r="E10" s="66">
         <v>8400849.4349600002</v>
       </c>
-      <c r="F10" s="75">
+      <c r="F10" s="66">
         <v>43745193</v>
       </c>
-      <c r="G10" s="75">
+      <c r="G10" s="66">
         <v>1244984.8977699999</v>
       </c>
-      <c r="H10" s="75">
+      <c r="H10" s="66">
         <v>44358163</v>
       </c>
-      <c r="I10" s="75">
+      <c r="I10" s="66">
         <v>1172723.6488600001</v>
       </c>
-      <c r="J10" s="75">
+      <c r="J10" s="66">
         <f t="shared" si="0"/>
         <v>0.99340197181519507</v>
       </c>
-      <c r="K10" s="75">
+      <c r="K10" s="66">
         <f t="shared" si="1"/>
         <v>0.73345839969234483</v>
       </c>
-      <c r="L10" s="75">
+      <c r="L10" s="66">
         <f t="shared" si="2"/>
         <v>0.74373582595171506</v>
       </c>
-      <c r="M10" s="75">
+      <c r="M10" s="66">
         <f t="shared" si="3"/>
         <v>5.0283462924160874E-2</v>
       </c>
-      <c r="N10" s="75">
+      <c r="N10" s="66">
         <f t="shared" si="4"/>
         <v>0.14085372951999781</v>
       </c>
-      <c r="O10" s="75">
+      <c r="O10" s="66">
         <f t="shared" si="5"/>
         <v>2.087417080911088E-2</v>
       </c>
-      <c r="P10" s="75">
+      <c r="P10" s="66">
         <f t="shared" si="6"/>
         <v>1.9662594945557173E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="75">
+      <c r="B11" s="66">
         <v>248801500.19999999</v>
       </c>
-      <c r="C11" s="75">
+      <c r="C11" s="66">
         <v>4715956.1624400001</v>
       </c>
-      <c r="D11" s="75">
+      <c r="D11" s="66">
         <v>253422519.59999999</v>
       </c>
-      <c r="E11" s="75">
+      <c r="E11" s="66">
         <v>7220355.8324800003</v>
       </c>
-      <c r="F11" s="75">
+      <c r="F11" s="66">
         <v>266081221.40000001</v>
       </c>
-      <c r="G11" s="75">
+      <c r="G11" s="66">
         <v>4012746.4544000002</v>
       </c>
-      <c r="H11" s="75">
+      <c r="H11" s="66">
         <v>271198856.39999998</v>
       </c>
-      <c r="I11" s="75">
+      <c r="I11" s="66">
         <v>752691.83418200002</v>
       </c>
-      <c r="J11" s="75">
+      <c r="J11" s="66">
         <f t="shared" si="0"/>
         <v>1.0185731171085599</v>
       </c>
-      <c r="K11" s="75">
+      <c r="K11" s="66">
         <f t="shared" si="1"/>
         <v>1.069451836850299</v>
       </c>
-      <c r="L11" s="75">
+      <c r="L11" s="66">
         <f t="shared" si="2"/>
         <v>1.0900209853316631</v>
       </c>
-      <c r="M11" s="75">
+      <c r="M11" s="66">
         <f t="shared" si="3"/>
         <v>1.8954693434923269E-2</v>
       </c>
-      <c r="N11" s="75">
+      <c r="N11" s="66">
         <f t="shared" si="4"/>
         <v>2.9020547812918698E-2</v>
       </c>
-      <c r="O11" s="75">
+      <c r="O11" s="66">
         <f t="shared" si="5"/>
         <v>1.6128304898380193E-2</v>
       </c>
-      <c r="P11" s="75">
+      <c r="P11" s="66">
         <f t="shared" si="6"/>
         <v>3.0252704809936677E-3</v>
       </c>
@@ -8417,27 +8761,27 @@
   <sheetData>
     <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="31" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="31"/>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61" t="s">
+      <c r="C2" s="74"/>
+      <c r="D2" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="61"/>
-      <c r="F2" s="62" t="s">
+      <c r="E2" s="74"/>
+      <c r="F2" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="61"/>
-      <c r="H2" s="59" t="s">
+      <c r="G2" s="74"/>
+      <c r="H2" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="60"/>
+      <c r="I2" s="73"/>
       <c r="J2" s="53" t="s">
         <v>45</v>
       </c>
@@ -8447,11 +8791,11 @@
       <c r="L2" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="62" t="s">
+      <c r="M2" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="61"/>
-      <c r="O2" s="61"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
     </row>
     <row r="3" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="31"/>
@@ -8991,22 +9335,22 @@
     </row>
     <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="31"/>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61" t="s">
+      <c r="C3" s="74"/>
+      <c r="D3" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="61"/>
-      <c r="F3" s="62" t="s">
+      <c r="E3" s="74"/>
+      <c r="F3" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="59" t="s">
+      <c r="G3" s="74"/>
+      <c r="H3" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="60"/>
+      <c r="I3" s="73"/>
       <c r="J3" s="53" t="s">
         <v>45</v>
       </c>
@@ -9016,11 +9360,11 @@
       <c r="L3" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="62" t="s">
+      <c r="M3" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
     </row>
     <row r="4" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="31"/>
@@ -9537,7 +9881,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="H3" sqref="H3:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9560,22 +9904,22 @@
     </row>
     <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="31"/>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61" t="s">
+      <c r="C3" s="74"/>
+      <c r="D3" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="61"/>
-      <c r="F3" s="62" t="s">
+      <c r="E3" s="74"/>
+      <c r="F3" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="59" t="s">
+      <c r="G3" s="74"/>
+      <c r="H3" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="60"/>
+      <c r="I3" s="73"/>
       <c r="J3" s="53" t="s">
         <v>45</v>
       </c>
@@ -9585,11 +9929,11 @@
       <c r="L3" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="62" t="s">
+      <c r="M3" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
     </row>
     <row r="4" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="31"/>
@@ -10103,10 +10447,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60957CB0-6CA6-420F-AE12-73B8B97534D5}">
-  <dimension ref="A2:C15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10116,6 +10460,11 @@
     <col min="3" max="3" width="30" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="83" t="s">
+        <v>140</v>
+      </c>
+    </row>
     <row r="2" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="23" t="s">
         <v>76</v>
@@ -10124,141 +10473,142 @@
         <v>121</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="A3" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="80" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="A4" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="80" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="C5" t="s">
-        <v>126</v>
+      <c r="B5" s="80" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="80" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="A6" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="80" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="A7" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="80" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="A8" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="80" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="A9" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="80" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B11" t="s">
-        <v>122</v>
-      </c>
-      <c r="C11" t="s">
-        <v>127</v>
+      <c r="A11" s="80" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="80" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="80" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+      <c r="A13" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="B13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13" t="s">
-        <v>123</v>
+      <c r="B13" s="80" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="80" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>145</v>
-      </c>
-      <c r="B14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C14" t="s">
-        <v>128</v>
+      <c r="A14" s="80" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="80" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="A15" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="80" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65049047-28B8-4D24-A307-ABB41DE3392E}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10266,10 +10616,12 @@
     <col min="1" max="1" width="32.86328125" customWidth="1"/>
     <col min="2" max="2" width="17.9296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.9296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.73046875" customWidth="1"/>
+    <col min="9" max="9" width="17.9296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
@@ -10320,7 +10672,7 @@
       <c r="K3" s="25"/>
       <c r="L3" s="25"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" s="80" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="25"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -10334,288 +10686,557 @@
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
     </row>
-    <row r="5" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="2"/>
-      <c r="B5" s="61" t="s">
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="83" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+    </row>
+    <row r="6" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="2"/>
+      <c r="B6" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61" t="s">
+      <c r="C6" s="74"/>
+      <c r="D6" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="61"/>
-      <c r="F5" s="62" t="s">
+      <c r="E6" s="74"/>
+      <c r="F6" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="61"/>
-      <c r="H5" s="8" t="s">
+      <c r="G6" s="74"/>
+      <c r="H6" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="62" t="s">
+      <c r="J6" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
-    </row>
-    <row r="6" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
+      <c r="K6" s="74"/>
+      <c r="L6" s="74"/>
+    </row>
+    <row r="7" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3" t="s">
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L7" s="8" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="6">
-        <v>155488099780</v>
-      </c>
-      <c r="C7" s="6">
-        <v>109256561.01800001</v>
-      </c>
-      <c r="D7" s="6">
-        <v>155651878039</v>
-      </c>
-      <c r="E7" s="6">
-        <v>1240169394.24</v>
-      </c>
-      <c r="F7" s="6">
-        <v>155396097352</v>
-      </c>
-      <c r="G7" s="6">
-        <v>1092945842.3599999</v>
-      </c>
-      <c r="H7" s="6">
-        <f>D7/B7</f>
-        <v>1.0010533170013123</v>
-      </c>
-      <c r="I7" s="6">
-        <f>F7/B7</f>
-        <v>0.99940829923235175</v>
-      </c>
-      <c r="J7" s="6">
-        <f>C7/B7</f>
-        <v>7.0266831463364102E-4</v>
-      </c>
-      <c r="K7" s="6">
-        <f>E7/B7</f>
-        <v>7.9759762708188908E-3</v>
-      </c>
-      <c r="L7" s="6">
-        <f>G7/B7</f>
-        <v>7.0291285565030901E-3</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="6">
-        <v>333482308492</v>
+        <v>155488099780</v>
       </c>
       <c r="C8" s="6">
-        <v>396439847.07999998</v>
+        <v>109256561.01800001</v>
       </c>
       <c r="D8" s="6">
-        <v>328381134082</v>
+        <v>155651878039</v>
       </c>
       <c r="E8" s="6">
-        <v>10031617594</v>
+        <v>1240169394.24</v>
       </c>
       <c r="F8" s="6">
-        <v>331966609845</v>
+        <v>155396097352</v>
       </c>
       <c r="G8" s="6">
-        <v>3160684862.4499998</v>
+        <v>1092945842.3599999</v>
       </c>
       <c r="H8" s="6">
-        <f t="shared" ref="H8:H11" si="0">D8/B8</f>
-        <v>0.98470331324900739</v>
+        <f>D8/B8</f>
+        <v>1.0010533170013123</v>
       </c>
       <c r="I8" s="6">
-        <f t="shared" ref="I8:I11" si="1">F8/B8</f>
-        <v>0.99545493536417584</v>
+        <f>F8/B8</f>
+        <v>0.99940829923235175</v>
       </c>
       <c r="J8" s="6">
-        <f t="shared" ref="J8:J11" si="2">C8/B8</f>
-        <v>1.1887882414893091E-3</v>
+        <f>C8/B8</f>
+        <v>7.0266831463364102E-4</v>
       </c>
       <c r="K8" s="6">
-        <f t="shared" ref="K8:K11" si="3">E8/B8</f>
-        <v>3.0081408634127442E-2</v>
+        <f>E8/B8</f>
+        <v>7.9759762708188908E-3</v>
       </c>
       <c r="L8" s="6">
-        <f t="shared" ref="L8:L11" si="4">G8/B8</f>
-        <v>9.477818708712166E-3</v>
+        <f>G8/B8</f>
+        <v>7.0291285565030901E-3</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="B9" s="6">
-        <v>78271163.599999994</v>
+        <v>333482308492</v>
       </c>
       <c r="C9" s="6">
-        <v>1433465.8790899999</v>
+        <v>396439847.07999998</v>
       </c>
       <c r="D9" s="6">
-        <v>68326073.599999994</v>
+        <v>328381134082</v>
       </c>
       <c r="E9" s="6">
-        <v>1214110.2608099999</v>
+        <v>10031617594</v>
       </c>
       <c r="F9" s="6">
-        <v>62405817.399999999</v>
+        <v>331966609845</v>
       </c>
       <c r="G9" s="6">
-        <v>806169.35760300001</v>
+        <v>3160684862.4499998</v>
       </c>
       <c r="H9" s="6">
-        <f t="shared" si="0"/>
-        <v>0.87294056274896104</v>
+        <f t="shared" ref="H9:H12" si="0">D9/B9</f>
+        <v>0.98470331324900739</v>
       </c>
       <c r="I9" s="6">
-        <f t="shared" si="1"/>
-        <v>0.79730279364340517</v>
+        <f t="shared" ref="I9:I12" si="1">F9/B9</f>
+        <v>0.99545493536417584</v>
       </c>
       <c r="J9" s="6">
-        <f t="shared" si="2"/>
-        <v>1.8314099511994478E-2</v>
+        <f t="shared" ref="J9:J12" si="2">C9/B9</f>
+        <v>1.1887882414893091E-3</v>
       </c>
       <c r="K9" s="6">
-        <f t="shared" si="3"/>
-        <v>1.5511590794978292E-2</v>
+        <f t="shared" ref="K9:K12" si="3">E9/B9</f>
+        <v>3.0081408634127442E-2</v>
       </c>
       <c r="L9" s="6">
-        <f t="shared" si="4"/>
-        <v>1.0299698133055481E-2</v>
+        <f t="shared" ref="L9:L12" si="4">G9/B9</f>
+        <v>9.477818708712166E-3</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="6">
-        <v>32476392.600000001</v>
+        <v>78271163.599999994</v>
       </c>
       <c r="C10" s="6">
-        <v>1704563.7003500001</v>
+        <v>1433465.8790899999</v>
       </c>
       <c r="D10" s="6">
-        <v>26894871.600000001</v>
+        <v>68326073.599999994</v>
       </c>
       <c r="E10" s="6">
-        <v>1063580.79907</v>
+        <v>1214110.2608099999</v>
       </c>
       <c r="F10" s="6">
-        <v>4609278</v>
+        <v>62405817.399999999</v>
       </c>
       <c r="G10" s="6">
-        <v>257185.27273500001</v>
+        <v>806169.35760300001</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" si="0"/>
-        <v>0.82813605350983477</v>
+        <v>0.87294056274896104</v>
       </c>
       <c r="I10" s="6">
         <f t="shared" si="1"/>
-        <v>0.1419270316371283</v>
+        <v>0.79730279364340517</v>
       </c>
       <c r="J10" s="6">
         <f t="shared" si="2"/>
-        <v>5.2486238891877417E-2</v>
+        <v>1.8314099511994478E-2</v>
       </c>
       <c r="K10" s="6">
         <f t="shared" si="3"/>
-        <v>3.2749351572686672E-2</v>
+        <v>1.5511590794978292E-2</v>
       </c>
       <c r="L10" s="6">
         <f t="shared" si="4"/>
-        <v>7.9191453281975653E-3</v>
+        <v>1.0299698133055481E-2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="6">
+        <v>32476392.600000001</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1704563.7003500001</v>
+      </c>
+      <c r="D11" s="6">
+        <v>26894871.600000001</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1063580.79907</v>
+      </c>
+      <c r="F11" s="6">
+        <v>4609278</v>
+      </c>
+      <c r="G11" s="6">
+        <v>257185.27273500001</v>
+      </c>
+      <c r="H11" s="6">
+        <f t="shared" si="0"/>
+        <v>0.82813605350983477</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="1"/>
+        <v>0.1419270316371283</v>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" si="2"/>
+        <v>5.2486238891877417E-2</v>
+      </c>
+      <c r="K11" s="6">
+        <f t="shared" si="3"/>
+        <v>3.2749351572686672E-2</v>
+      </c>
+      <c r="L11" s="6">
+        <f t="shared" si="4"/>
+        <v>7.9191453281975653E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B12" s="6">
         <v>13127022678.4</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C12" s="6">
         <v>210486566.602</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D12" s="6">
         <v>13630958501.799999</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E12" s="6">
         <v>220806167.229</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F12" s="6">
         <v>13408413157</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G12" s="6">
         <v>190294880.90900001</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H12" s="6">
         <f t="shared" si="0"/>
         <v>1.0383891942404584</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I12" s="6">
         <f t="shared" si="1"/>
         <v>1.0214359710875656</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J12" s="6">
         <f t="shared" si="2"/>
         <v>1.6034600667548735E-2</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K12" s="6">
         <f t="shared" si="3"/>
         <v>1.6820734803203157E-2</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L12" s="6">
         <f t="shared" si="4"/>
         <v>1.4496423566184795E-2</v>
       </c>
     </row>
+    <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="83" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+    </row>
+    <row r="17" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A17" s="2"/>
+      <c r="B17" s="74" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="74"/>
+      <c r="F17" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="74"/>
+      <c r="H17" s="72" t="s">
+        <v>114</v>
+      </c>
+      <c r="I17" s="73"/>
+      <c r="J17" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="L17" s="75" t="s">
+        <v>44</v>
+      </c>
+      <c r="M17" s="74"/>
+      <c r="N17" s="74"/>
+    </row>
+    <row r="18" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M18" s="82" t="s">
+        <v>30</v>
+      </c>
+      <c r="N18" s="82" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A19" s="80" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="81"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81">
+        <v>154231498991</v>
+      </c>
+      <c r="E19" s="81">
+        <v>776501347.76400006</v>
+      </c>
+      <c r="H19" s="81">
+        <v>153324861138</v>
+      </c>
+      <c r="I19" s="81">
+        <v>336290655.68900001</v>
+      </c>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A20" s="80" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81">
+        <v>320995802715</v>
+      </c>
+      <c r="E20" s="81">
+        <v>2139277529.4000001</v>
+      </c>
+      <c r="H20" s="81">
+        <v>328914925755</v>
+      </c>
+      <c r="I20" s="81">
+        <v>11811502965.6</v>
+      </c>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A21" s="80" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="81"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81">
+        <v>55426876</v>
+      </c>
+      <c r="E21" s="81">
+        <v>1793666.85338</v>
+      </c>
+      <c r="H21" s="81">
+        <v>46162437.600000001</v>
+      </c>
+      <c r="I21" s="81">
+        <v>1415999.3302199999</v>
+      </c>
+      <c r="J21" s="81"/>
+      <c r="K21" s="81"/>
+      <c r="L21" s="81"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A22" s="80" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="81"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="81">
+        <v>7471985</v>
+      </c>
+      <c r="E22" s="81">
+        <v>261195.06404100001</v>
+      </c>
+      <c r="H22" s="81">
+        <v>3821710</v>
+      </c>
+      <c r="I22" s="81">
+        <v>508277.09580800001</v>
+      </c>
+      <c r="J22" s="81"/>
+      <c r="K22" s="81"/>
+      <c r="L22" s="81"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A23" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="81"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81">
+        <v>13356814029.799999</v>
+      </c>
+      <c r="E23" s="81">
+        <v>244857269.73199999</v>
+      </c>
+      <c r="H23" s="81">
+        <v>13620259009.4</v>
+      </c>
+      <c r="I23" s="81">
+        <v>186564319.986</v>
+      </c>
+      <c r="J23" s="81"/>
+      <c r="K23" s="81"/>
+      <c r="L23" s="81"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A24" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="81">
+        <v>3557269894.1999998</v>
+      </c>
+      <c r="E24" s="81">
+        <v>24548824.4307</v>
+      </c>
+      <c r="H24" s="81">
+        <v>2911940947</v>
+      </c>
+      <c r="I24" s="81">
+        <v>53453576.313600004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A25" s="80" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="81">
+        <v>885658835</v>
+      </c>
+      <c r="E25" s="81">
+        <v>49874908.9133</v>
+      </c>
+      <c r="H25" s="81">
+        <v>379748471.39999998</v>
+      </c>
+      <c r="I25" s="81">
+        <v>8505820.7215299997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A26" s="80" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="81">
+        <v>105115239.59999999</v>
+      </c>
+      <c r="E26" s="81">
+        <v>1651547.44683</v>
+      </c>
+      <c r="H26" s="81">
+        <v>106508726.8</v>
+      </c>
+      <c r="I26" s="81">
+        <v>2375056.0667400002</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="J5:L5"/>
+  <mergeCells count="9">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="H17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated results for postgres
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="820" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{61CD0F8D-C78C-4CB9-AA06-9534A67CC54F}"/>
+  <xr:revisionPtr revIDLastSave="906" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{C6130B6D-0012-4320-BBD5-BCA491E75A9F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="153">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -718,7 +718,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -866,6 +866,12 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3153,10 +3159,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51140CC8-C0B8-469A-8BAE-C9043CBCBC10}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3165,35 +3171,39 @@
     <col min="2" max="2" width="19.19921875" style="25" customWidth="1"/>
     <col min="3" max="3" width="19.46484375" style="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.3984375" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.86328125" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="25" customWidth="1"/>
     <col min="6" max="6" width="19.3984375" style="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.9296875" style="25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.59765625" style="25" customWidth="1"/>
     <col min="9" max="9" width="17" style="25" customWidth="1"/>
-    <col min="10" max="16384" width="9.06640625" style="25"/>
+    <col min="10" max="11" width="9.06640625" style="25"/>
+    <col min="12" max="12" width="13.1328125" style="25" customWidth="1"/>
+    <col min="13" max="15" width="9.06640625" style="25"/>
+    <col min="16" max="16" width="18.73046875" style="25" customWidth="1"/>
+    <col min="17" max="16384" width="9.06640625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" s="23" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" s="24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="83" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
       <c r="B6" s="74" t="s">
         <v>24</v>
@@ -3217,13 +3227,16 @@
       <c r="K6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="L6" s="75" t="s">
+      <c r="L6" s="85" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="M6" s="74"/>
-      <c r="N6" s="74"/>
-    </row>
-    <row r="7" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="N6" s="75"/>
+      <c r="O6" s="75"/>
+    </row>
+    <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -3253,490 +3266,847 @@
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="N7" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="O7" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="P7" s="86" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A8" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="6">
-        <v>946914692983</v>
-      </c>
-      <c r="C8" s="6">
-        <v>1638529605.76</v>
-      </c>
-      <c r="D8" s="6">
-        <v>940390725841</v>
-      </c>
-      <c r="E8" s="6">
-        <v>6669456559.4899998</v>
-      </c>
-      <c r="F8" s="6">
-        <v>944522103276</v>
-      </c>
-      <c r="G8" s="6">
-        <v>6985699539.3500004</v>
-      </c>
-      <c r="J8" s="26">
-        <f>D8/B8</f>
-        <v>0.99311029051471578</v>
+      <c r="D8" s="81">
+        <v>943944726458</v>
+      </c>
+      <c r="E8" s="81">
+        <v>8036919330.3100004</v>
+      </c>
+      <c r="H8" s="81">
+        <v>945025210371</v>
+      </c>
+      <c r="I8" s="81">
+        <v>7415023994.6800003</v>
+      </c>
+      <c r="J8" s="26" t="e">
+        <f>#REF!/D8</f>
+        <v>#REF!</v>
       </c>
       <c r="K8" s="26">
-        <f>F8/B8</f>
-        <v>0.99747327850678624</v>
-      </c>
-      <c r="L8" s="26">
-        <f>C8/B8</f>
-        <v>1.7303877718892007E-3</v>
+        <f>H8/D8</f>
+        <v>1.0011446474382608</v>
       </c>
       <c r="M8" s="26">
-        <f>E8/B8</f>
-        <v>7.0433552345456497E-3</v>
-      </c>
-      <c r="N8" s="26">
-        <f>G8/B8</f>
-        <v>7.3773272197767189E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+        <f>E8/D8</f>
+        <v>8.514184257872006E-3</v>
+      </c>
+      <c r="N8" s="26" t="e">
+        <f>#REF!/D8</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O8" s="26">
+        <f>I8/D8</f>
+        <v>7.8553582501633117E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A9" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="6">
-        <v>1200836800110</v>
-      </c>
-      <c r="C9" s="6">
-        <v>827454901.97399998</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1200772331430</v>
-      </c>
-      <c r="E9" s="6">
-        <v>9214310628.6700001</v>
-      </c>
-      <c r="F9" s="6">
-        <v>1151380231060</v>
-      </c>
-      <c r="G9" s="6">
-        <v>10934220055.700001</v>
-      </c>
-      <c r="J9" s="26">
-        <f>D9/B9</f>
-        <v>0.99994631353736485</v>
+      <c r="D9" s="81">
+        <v>1208883703350</v>
+      </c>
+      <c r="E9" s="81">
+        <v>11754126552.299999</v>
+      </c>
+      <c r="H9" s="81">
+        <v>1150780393290</v>
+      </c>
+      <c r="I9" s="81">
+        <v>10686477064.9</v>
+      </c>
+      <c r="J9" s="26" t="e">
+        <f>#REF!/D9</f>
+        <v>#REF!</v>
       </c>
       <c r="K9" s="26">
-        <f>F9/B9</f>
-        <v>0.95881491219667014</v>
-      </c>
-      <c r="L9" s="26">
-        <f>C9/B9</f>
-        <v>6.8906524341875834E-4</v>
+        <f>H9/D9</f>
+        <v>0.95193639396495555</v>
       </c>
       <c r="M9" s="26">
-        <f>E9/B9</f>
-        <v>7.6732413828639687E-3</v>
-      </c>
-      <c r="N9" s="26">
-        <f>G9/B9</f>
-        <v>9.1055004765829926E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+        <f>E9/D9</f>
+        <v>9.7231243334057142E-3</v>
+      </c>
+      <c r="N9" s="26" t="e">
+        <f>#REF!/D9</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O9" s="26">
+        <f>I9/D9</f>
+        <v>8.8399546087734922E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A10" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="6">
-        <v>451472726.19999999</v>
-      </c>
-      <c r="C10" s="6">
-        <v>4509950.1854800005</v>
-      </c>
-      <c r="D10" s="6">
-        <v>414906363.80000001</v>
-      </c>
-      <c r="E10" s="6">
-        <v>5076230.1852000002</v>
-      </c>
-      <c r="F10" s="6">
-        <v>83253569.799999997</v>
-      </c>
-      <c r="G10" s="6">
-        <v>4087614.1338900002</v>
-      </c>
-      <c r="J10" s="26">
-        <f>D10/B10</f>
-        <v>0.9190064863767623</v>
+      <c r="D10" s="81">
+        <v>429044136.60000002</v>
+      </c>
+      <c r="E10" s="81">
+        <v>17035425.073100001</v>
+      </c>
+      <c r="H10" s="81">
+        <v>107691606.59999999</v>
+      </c>
+      <c r="I10" s="81">
+        <v>978641.49078600004</v>
+      </c>
+      <c r="J10" s="26" t="e">
+        <f>#REF!/D10</f>
+        <v>#REF!</v>
       </c>
       <c r="K10" s="26">
-        <f>F10/B10</f>
-        <v>0.18440442792798764</v>
-      </c>
-      <c r="L10" s="26">
-        <f>C10/B10</f>
-        <v>9.9894189034181371E-3</v>
+        <f>H10/D10</f>
+        <v>0.25100356213561642</v>
       </c>
       <c r="M10" s="26">
-        <f>E10/B10</f>
-        <v>1.1243713940210991E-2</v>
-      </c>
-      <c r="N10" s="26">
-        <f>G10/B10</f>
-        <v>9.0539558575221859E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+        <f>E10/D10</f>
+        <v>3.9705530550070686E-2</v>
+      </c>
+      <c r="N10" s="26" t="e">
+        <f>#REF!/D10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O10" s="26">
+        <f>I10/D10</f>
+        <v>2.2809809231780559E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A11" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="6">
-        <v>266369123.40000001</v>
-      </c>
-      <c r="C11" s="6">
-        <v>3466899.5721100001</v>
-      </c>
-      <c r="D11" s="6">
-        <v>245947677.80000001</v>
-      </c>
-      <c r="E11" s="6">
-        <v>2917717.71747</v>
-      </c>
-      <c r="F11" s="6">
-        <v>127109755.2</v>
-      </c>
-      <c r="G11" s="6">
-        <v>665387.35145299998</v>
-      </c>
-      <c r="J11" s="26">
-        <f>D11/B11</f>
-        <v>0.92333403609496578</v>
+      <c r="D11" s="81">
+        <v>248961865.19999999</v>
+      </c>
+      <c r="E11" s="81">
+        <v>11418958.505999999</v>
+      </c>
+      <c r="H11" s="81">
+        <v>126322180.8</v>
+      </c>
+      <c r="I11" s="81">
+        <v>768366.61140000005</v>
+      </c>
+      <c r="J11" s="26" t="e">
+        <f>#REF!/D11</f>
+        <v>#REF!</v>
       </c>
       <c r="K11" s="26">
-        <f>F11/B11</f>
-        <v>0.47719402901334923</v>
-      </c>
-      <c r="L11" s="26">
-        <f>C11/B11</f>
-        <v>1.3015395808108891E-2</v>
+        <f>H11/D11</f>
+        <v>0.50739570374973231</v>
       </c>
       <c r="M11" s="26">
-        <f>E11/B11</f>
-        <v>1.0953663398473309E-2</v>
-      </c>
-      <c r="N11" s="26">
-        <f>G11/B11</f>
-        <v>2.4979897931105329E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+        <f>E11/D11</f>
+        <v>4.5866295614497989E-2</v>
+      </c>
+      <c r="N11" s="26" t="e">
+        <f>#REF!/D11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O11" s="26">
+        <f>I11/D11</f>
+        <v>3.0862823540574922E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A12" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="6">
-        <v>13444549014</v>
-      </c>
-      <c r="C12" s="6">
-        <v>307569910.05299997</v>
-      </c>
-      <c r="D12" s="6">
-        <v>13667780586.799999</v>
-      </c>
-      <c r="E12" s="6">
-        <v>113540871.403</v>
-      </c>
-      <c r="F12" s="6">
-        <v>13323831275.6</v>
-      </c>
-      <c r="G12" s="6">
-        <v>250385375.715</v>
-      </c>
-      <c r="J12" s="26">
-        <f>D12/B12</f>
-        <v>1.0166038721393738</v>
+      <c r="D12" s="81">
+        <v>50032630234.599998</v>
+      </c>
+      <c r="E12" s="81">
+        <v>402589850.713</v>
+      </c>
+      <c r="H12" s="81">
+        <v>50738369301</v>
+      </c>
+      <c r="I12" s="81">
+        <v>441963416.24599999</v>
+      </c>
+      <c r="J12" s="26" t="e">
+        <f>#REF!/D12</f>
+        <v>#REF!</v>
       </c>
       <c r="K12" s="26">
-        <f>F12/B12</f>
-        <v>0.99102106450173266</v>
-      </c>
-      <c r="L12" s="26">
-        <f>C12/B12</f>
-        <v>2.2876922813306944E-2</v>
+        <f>H12/D12</f>
+        <v>1.0141055759629432</v>
       </c>
       <c r="M12" s="26">
-        <f>E12/B12</f>
-        <v>8.4451230967114085E-3</v>
-      </c>
-      <c r="N12" s="26">
-        <f>G12/B12</f>
-        <v>1.8623560779485435E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="83" t="s">
+        <f>E12/D12</f>
+        <v>8.0465458007160599E-3</v>
+      </c>
+      <c r="N12" s="26" t="e">
+        <f>#REF!/D12</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O12" s="26">
+        <f>I12/D12</f>
+        <v>8.8335035390636092E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A13" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="81">
+        <v>21680931744.599998</v>
+      </c>
+      <c r="E13" s="81">
+        <v>236688616.986</v>
+      </c>
+      <c r="H13" s="81">
+        <v>8207865959.8000002</v>
+      </c>
+      <c r="I13" s="81">
+        <v>102438436.20299999</v>
+      </c>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26">
+        <f>H13/D13</f>
+        <v>0.37857533322313547</v>
+      </c>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26">
+        <f>E13/D13</f>
+        <v>1.0916902454847279E-2</v>
+      </c>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26">
+        <f>I13/D13</f>
+        <v>4.7248170608956419E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A14" s="80" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="81">
+        <v>17982740923.200001</v>
+      </c>
+      <c r="E14" s="81">
+        <v>219770850.15400001</v>
+      </c>
+      <c r="H14" s="81">
+        <v>11542933099.4</v>
+      </c>
+      <c r="I14" s="81">
+        <v>145744926.20699999</v>
+      </c>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26">
+        <f>H14/D14</f>
+        <v>0.64188952889312678</v>
+      </c>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26">
+        <f>E14/D14</f>
+        <v>1.2221209830725412E-2</v>
+      </c>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26">
+        <f>I14/D14</f>
+        <v>8.1047114469057751E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A15" s="80" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="81">
+        <v>71249580938.399994</v>
+      </c>
+      <c r="E15" s="81">
+        <v>594405628.78699994</v>
+      </c>
+      <c r="H15" s="81">
+        <v>72147459341.199997</v>
+      </c>
+      <c r="I15" s="81">
+        <v>106593048.45</v>
+      </c>
+      <c r="K15" s="26">
+        <f>H15/D15</f>
+        <v>1.0126018762633324</v>
+      </c>
+      <c r="M15" s="26">
+        <f>E15/D15</f>
+        <v>8.3425842083324417E-3</v>
+      </c>
+      <c r="O15" s="26">
+        <f>I15/D15</f>
+        <v>1.4960515843897636E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="83" t="s">
         <v>152</v>
       </c>
-      <c r="M15" s="80"/>
-      <c r="N15" s="80"/>
-    </row>
-    <row r="16" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A16" s="2"/>
-      <c r="B16" s="74" t="s">
+      <c r="M17" s="80"/>
+      <c r="N17" s="80"/>
+    </row>
+    <row r="18" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A18" s="2"/>
+      <c r="B18" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="74"/>
-      <c r="D16" s="74" t="s">
+      <c r="C18" s="74"/>
+      <c r="D18" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="74"/>
-      <c r="F16" s="75" t="s">
+      <c r="E18" s="74"/>
+      <c r="F18" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="74"/>
-      <c r="H16" s="72" t="s">
+      <c r="G18" s="74"/>
+      <c r="H18" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="I16" s="73"/>
-      <c r="J16" s="82" t="s">
+      <c r="I18" s="73"/>
+      <c r="J18" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="K16" s="82" t="s">
+      <c r="K18" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="L16" s="75" t="s">
+      <c r="L18" s="85" t="s">
+        <v>115</v>
+      </c>
+      <c r="M18" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="M16" s="74"/>
-      <c r="N16" s="74"/>
-    </row>
-    <row r="17" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A17" s="3" t="s">
+      <c r="N18" s="74"/>
+      <c r="O18" s="74"/>
+    </row>
+    <row r="19" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="H19" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="I19" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3" t="s">
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="M19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M17" s="82" t="s">
+      <c r="N19" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="N17" s="82" t="s">
+      <c r="O19" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A18" s="80" t="s">
+      <c r="P19" s="86" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A20" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="81"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81">
+      <c r="B20" s="81">
+        <v>950961617600</v>
+      </c>
+      <c r="C20" s="81">
+        <v>3342695208.5900002</v>
+      </c>
+      <c r="D20" s="81">
         <v>947044998803</v>
       </c>
-      <c r="E18" s="81">
+      <c r="E20" s="81">
         <v>4671101663.8400002</v>
       </c>
-      <c r="H18" s="81">
+      <c r="F20" s="81">
+        <v>942333772624</v>
+      </c>
+      <c r="G20" s="81">
+        <v>1806397218.3</v>
+      </c>
+      <c r="H20" s="81">
         <v>944883191889</v>
       </c>
-      <c r="I18" s="81">
+      <c r="I20" s="81">
         <v>6989132626.8100004</v>
       </c>
-      <c r="J18" s="81"/>
-      <c r="K18" s="81"/>
-      <c r="L18" s="81"/>
-      <c r="M18" s="80"/>
-      <c r="N18" s="80"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A19" s="80" t="s">
+      <c r="J20" s="81">
+        <f>D20/B20</f>
+        <v>0.99588141232567873</v>
+      </c>
+      <c r="K20" s="81">
+        <f>F20/B20</f>
+        <v>0.99092724162960999</v>
+      </c>
+      <c r="L20" s="81">
+        <f>H20/B20</f>
+        <v>0.99360812718567915</v>
+      </c>
+      <c r="M20" s="81">
+        <f>C20/B20</f>
+        <v>3.5150684809195187E-3</v>
+      </c>
+      <c r="N20" s="81">
+        <f>E20/B20</f>
+        <v>4.9119770739314856E-3</v>
+      </c>
+      <c r="O20" s="26">
+        <f>G20/B20</f>
+        <v>1.8995479784546037E-3</v>
+      </c>
+      <c r="P20" s="26">
+        <f>I20/B20</f>
+        <v>7.3495422921998699E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A21" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="81"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81">
+      <c r="B21" s="81">
+        <v>1196533593690</v>
+      </c>
+      <c r="C21" s="81">
+        <v>3862807717.6399999</v>
+      </c>
+      <c r="D21" s="81">
         <v>1203651140030</v>
       </c>
-      <c r="E19" s="81">
+      <c r="E21" s="81">
         <v>9785263329.6399994</v>
       </c>
-      <c r="H19" s="81">
+      <c r="F21" s="81">
+        <v>1133790186310</v>
+      </c>
+      <c r="G21" s="81">
+        <v>1801538523.27</v>
+      </c>
+      <c r="H21" s="81">
         <v>1145899823710</v>
       </c>
-      <c r="I19" s="81">
+      <c r="I21" s="81">
         <v>10497091805.6</v>
       </c>
-      <c r="J19" s="81"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="80"/>
-      <c r="N19" s="80"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A20" s="80" t="s">
+      <c r="J21" s="81">
+        <f t="shared" ref="J21:J27" si="0">D21/B21</f>
+        <v>1.0059484718001523</v>
+      </c>
+      <c r="K21" s="81">
+        <f t="shared" ref="K21:K27" si="1">F21/B21</f>
+        <v>0.94756235202180572</v>
+      </c>
+      <c r="L21" s="81">
+        <f t="shared" ref="L21:L27" si="2">H21/B21</f>
+        <v>0.95768295161371098</v>
+      </c>
+      <c r="M21" s="81">
+        <f t="shared" ref="M21:M27" si="3">C21/B21</f>
+        <v>3.2283320234473773E-3</v>
+      </c>
+      <c r="N21" s="81">
+        <f t="shared" ref="N21:N27" si="4">E21/B21</f>
+        <v>8.1780096950417776E-3</v>
+      </c>
+      <c r="O21" s="26">
+        <f t="shared" ref="O21:O27" si="5">G21/B21</f>
+        <v>1.5056313778154947E-3</v>
+      </c>
+      <c r="P21" s="26">
+        <f t="shared" ref="P21:P27" si="6">I21/B21</f>
+        <v>8.7729185882929796E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A22" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="81"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81">
+      <c r="B22" s="81">
+        <v>387762805.60000002</v>
+      </c>
+      <c r="C22" s="81">
+        <v>6409107.8970799996</v>
+      </c>
+      <c r="D22" s="81">
         <v>373726151.39999998</v>
       </c>
-      <c r="E20" s="81">
+      <c r="E22" s="81">
         <v>11967060.9714</v>
       </c>
-      <c r="H20" s="81">
+      <c r="F22" s="81">
+        <v>84708735.599999994</v>
+      </c>
+      <c r="G22" s="81">
+        <v>3917699.6093700002</v>
+      </c>
+      <c r="H22" s="81">
         <v>109409320.40000001</v>
       </c>
-      <c r="I20" s="81">
+      <c r="I22" s="81">
         <v>3682064.03516</v>
       </c>
-      <c r="J20" s="81"/>
-      <c r="K20" s="81"/>
-      <c r="L20" s="81"/>
-      <c r="M20" s="80"/>
-      <c r="N20" s="80"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A21" s="80" t="s">
+      <c r="J22" s="81">
+        <f t="shared" si="0"/>
+        <v>0.96380092675912898</v>
+      </c>
+      <c r="K22" s="81">
+        <f t="shared" si="1"/>
+        <v>0.21845503069570318</v>
+      </c>
+      <c r="L22" s="81">
+        <f t="shared" si="2"/>
+        <v>0.2821552733267102</v>
+      </c>
+      <c r="M22" s="81">
+        <f t="shared" si="3"/>
+        <v>1.6528423573692028E-2</v>
+      </c>
+      <c r="N22" s="81">
+        <f t="shared" si="4"/>
+        <v>3.086180726612733E-2</v>
+      </c>
+      <c r="O22" s="26">
+        <f t="shared" si="5"/>
+        <v>1.0103340374041279E-2</v>
+      </c>
+      <c r="P22" s="26">
+        <f t="shared" si="6"/>
+        <v>9.4956607028428199E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A23" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="81"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81">
+      <c r="B23" s="81">
+        <v>197721030.40000001</v>
+      </c>
+      <c r="C23" s="81">
+        <v>3206633.6842399999</v>
+      </c>
+      <c r="D23" s="81">
         <v>178376300</v>
       </c>
-      <c r="E21" s="81">
+      <c r="E23" s="81">
         <v>7016479.1470799996</v>
       </c>
-      <c r="H21" s="81">
+      <c r="F23" s="81">
+        <v>74518004.200000003</v>
+      </c>
+      <c r="G23" s="81">
+        <v>603428.89475700003</v>
+      </c>
+      <c r="H23" s="81">
         <v>72696324.200000003</v>
       </c>
-      <c r="I21" s="81">
+      <c r="I23" s="81">
         <v>1204122.4476600001</v>
       </c>
-      <c r="J21" s="81"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="81"/>
-      <c r="M21" s="80"/>
-      <c r="N21" s="80"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A22" s="80" t="s">
+      <c r="J23" s="81">
+        <f t="shared" si="0"/>
+        <v>0.90216149308515836</v>
+      </c>
+      <c r="K23" s="81">
+        <f t="shared" si="1"/>
+        <v>0.3768845633124922</v>
+      </c>
+      <c r="L23" s="81">
+        <f t="shared" si="2"/>
+        <v>0.36767117818944972</v>
+      </c>
+      <c r="M23" s="81">
+        <f t="shared" si="3"/>
+        <v>1.6217969721039852E-2</v>
+      </c>
+      <c r="N23" s="81">
+        <f t="shared" si="4"/>
+        <v>3.5486761994337652E-2</v>
+      </c>
+      <c r="O23" s="26">
+        <f t="shared" si="5"/>
+        <v>3.0519206456502464E-3</v>
+      </c>
+      <c r="P23" s="26">
+        <f t="shared" si="6"/>
+        <v>6.090006941719843E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A24" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="81"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81">
+      <c r="B24" s="81">
+        <v>51646439040</v>
+      </c>
+      <c r="C24" s="81">
+        <v>427666677.69199997</v>
+      </c>
+      <c r="D24" s="81">
         <v>50047193757.599998</v>
       </c>
-      <c r="E22" s="81">
+      <c r="E24" s="81">
         <v>256065872.794</v>
       </c>
-      <c r="H22" s="81">
+      <c r="F24" s="81">
+        <v>50863014412</v>
+      </c>
+      <c r="G24" s="81">
+        <v>255246866.58399999</v>
+      </c>
+      <c r="H24" s="81">
         <v>49480147960.800003</v>
       </c>
-      <c r="I22" s="81">
+      <c r="I24" s="81">
         <v>676041009.45899999</v>
       </c>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="80"/>
-      <c r="N22" s="80"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A23" s="80" t="s">
+      <c r="J24" s="81">
+        <f t="shared" si="0"/>
+        <v>0.96903474252772026</v>
+      </c>
+      <c r="K24" s="81">
+        <f t="shared" si="1"/>
+        <v>0.98483100398474244</v>
+      </c>
+      <c r="L24" s="81">
+        <f t="shared" si="2"/>
+        <v>0.95805536413609826</v>
+      </c>
+      <c r="M24" s="81">
+        <f t="shared" si="3"/>
+        <v>8.2806614674977592E-3</v>
+      </c>
+      <c r="N24" s="81">
+        <f t="shared" si="4"/>
+        <v>4.9580547575734666E-3</v>
+      </c>
+      <c r="O24" s="26">
+        <f t="shared" si="5"/>
+        <v>4.9421968160537092E-3</v>
+      </c>
+      <c r="P24" s="26">
+        <f t="shared" si="6"/>
+        <v>1.3089789383841323E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A25" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="81">
+      <c r="B25" s="81">
+        <v>21131880797.200001</v>
+      </c>
+      <c r="C25" s="81">
+        <v>480889559.88700002</v>
+      </c>
+      <c r="D25" s="81">
         <v>19963233833.799999</v>
       </c>
-      <c r="E23" s="81">
+      <c r="E25" s="81">
         <v>208319673.255</v>
       </c>
-      <c r="H23" s="81">
+      <c r="F25" s="81">
+        <v>6226879954.8000002</v>
+      </c>
+      <c r="G25" s="81">
+        <v>204481330.852</v>
+      </c>
+      <c r="H25" s="81">
         <v>8088796149.8000002</v>
       </c>
-      <c r="I23" s="81">
+      <c r="I25" s="81">
         <v>104743077.28399999</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A24" s="80" t="s">
+      <c r="J25" s="81">
+        <f t="shared" si="0"/>
+        <v>0.94469744673390132</v>
+      </c>
+      <c r="K25" s="81">
+        <f t="shared" si="1"/>
+        <v>0.29466756956271822</v>
+      </c>
+      <c r="L25" s="81">
+        <f t="shared" si="2"/>
+        <v>0.38277691547795289</v>
+      </c>
+      <c r="M25" s="81">
+        <f t="shared" si="3"/>
+        <v>2.275659059891718E-2</v>
+      </c>
+      <c r="N25" s="81">
+        <f t="shared" si="4"/>
+        <v>9.8580753532644672E-3</v>
+      </c>
+      <c r="O25" s="26">
+        <f t="shared" si="5"/>
+        <v>9.6764378341133751E-3</v>
+      </c>
+      <c r="P25" s="26">
+        <f t="shared" si="6"/>
+        <v>4.9566377119578762E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A26" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="81">
+      <c r="B26" s="81">
+        <v>11957535869.799999</v>
+      </c>
+      <c r="C26" s="81">
+        <v>180159381.93700001</v>
+      </c>
+      <c r="D26" s="81">
         <v>11291216904.799999</v>
       </c>
-      <c r="E24" s="81">
+      <c r="E26" s="81">
         <v>101645055.061</v>
       </c>
-      <c r="H24" s="81">
+      <c r="F26" s="81">
+        <v>4954524262.3999996</v>
+      </c>
+      <c r="G26" s="81">
+        <v>72885506.043899998</v>
+      </c>
+      <c r="H26" s="81">
         <v>4792947991</v>
       </c>
-      <c r="I24" s="81">
+      <c r="I26" s="81">
         <v>250072949.72400001</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A25" s="80" t="s">
+      <c r="J26" s="81">
+        <f t="shared" si="0"/>
+        <v>0.9442762311353079</v>
+      </c>
+      <c r="K26" s="81">
+        <f t="shared" si="1"/>
+        <v>0.41434324900610719</v>
+      </c>
+      <c r="L26" s="81">
+        <f t="shared" si="2"/>
+        <v>0.40083074332271823</v>
+      </c>
+      <c r="M26" s="81">
+        <f t="shared" si="3"/>
+        <v>1.5066597658470026E-2</v>
+      </c>
+      <c r="N26" s="81">
+        <f t="shared" si="4"/>
+        <v>8.5005017896467427E-3</v>
+      </c>
+      <c r="O26" s="26">
+        <f t="shared" si="5"/>
+        <v>6.0953616896922656E-3</v>
+      </c>
+      <c r="P26" s="26">
+        <f t="shared" si="6"/>
+        <v>2.0913418320206361E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A27" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="81">
+      <c r="B27" s="81">
+        <v>63735346968.599998</v>
+      </c>
+      <c r="C27" s="81">
+        <v>70283082.364500001</v>
+      </c>
+      <c r="D27" s="81">
         <v>63401290363.800003</v>
       </c>
-      <c r="E25" s="81">
+      <c r="E27" s="81">
         <v>105764495.332</v>
       </c>
-      <c r="H25" s="81">
+      <c r="F27" s="81">
+        <v>62937469818.199997</v>
+      </c>
+      <c r="G27" s="81">
+        <v>118134134.51100001</v>
+      </c>
+      <c r="H27" s="81">
         <v>63760215368.599998</v>
       </c>
-      <c r="I25" s="81">
+      <c r="I27" s="81">
         <v>554303853.73599994</v>
+      </c>
+      <c r="J27" s="81">
+        <f t="shared" si="0"/>
+        <v>0.99475869167285502</v>
+      </c>
+      <c r="K27" s="81">
+        <f t="shared" si="1"/>
+        <v>0.9874814025756683</v>
+      </c>
+      <c r="L27" s="81">
+        <f t="shared" si="2"/>
+        <v>1.0003901822329806</v>
+      </c>
+      <c r="M27" s="81">
+        <f t="shared" si="3"/>
+        <v>1.1027331882122776E-3</v>
+      </c>
+      <c r="N27" s="81">
+        <f t="shared" si="4"/>
+        <v>1.6594323301339551E-3</v>
+      </c>
+      <c r="O27" s="26">
+        <f t="shared" si="5"/>
+        <v>1.853510495035043E-3</v>
+      </c>
+      <c r="P27" s="26">
+        <f t="shared" si="6"/>
+        <v>8.696961420937812E-3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="M6:O6"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="M18:O18"/>
     <mergeCell ref="H6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4113,7 +4483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5A357B-AD95-4B57-AFAC-6E90E36724A8}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="D39" sqref="D39:D51"/>
     </sheetView>
   </sheetViews>
@@ -9880,8 +10250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EB1957-8C0E-4A2E-90B7-11EE02C0E28A}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10605,26 +10975,28 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65049047-28B8-4D24-A307-ABB41DE3392E}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:E17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="32.86328125" customWidth="1"/>
-    <col min="2" max="2" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.06640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.06640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.73046875" customWidth="1"/>
     <col min="9" max="9" width="17.9296875" customWidth="1"/>
+    <col min="12" max="12" width="13.86328125" customWidth="1"/>
+    <col min="16" max="16" width="16.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" s="23" t="s">
         <v>117</v>
       </c>
@@ -10640,7 +11012,7 @@
       <c r="K1" s="25"/>
       <c r="L1" s="25"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" s="24" t="s">
         <v>48</v>
       </c>
@@ -10656,7 +11028,7 @@
       <c r="K2" s="25"/>
       <c r="L2" s="25"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="25" t="s">
         <v>49</v>
       </c>
@@ -10672,7 +11044,7 @@
       <c r="K3" s="25"/>
       <c r="L3" s="25"/>
     </row>
-    <row r="4" spans="1:12" s="80" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="25"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -10686,7 +11058,7 @@
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
     </row>
-    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="83" t="s">
         <v>151</v>
       </c>
@@ -10702,7 +11074,7 @@
       <c r="K5" s="25"/>
       <c r="L5" s="25"/>
     </row>
-    <row r="6" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
       <c r="B6" s="74" t="s">
         <v>24</v>
@@ -10716,19 +11088,26 @@
         <v>42</v>
       </c>
       <c r="G6" s="74"/>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="72" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" s="73"/>
+      <c r="J6" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="K6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="75" t="s">
+      <c r="L6" s="85" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="K6" s="74"/>
-      <c r="L6" s="74"/>
-    </row>
-    <row r="7" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="N6" s="74"/>
+      <c r="O6" s="74"/>
+    </row>
+    <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -10750,491 +11129,824 @@
       <c r="G7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3" t="s">
+      <c r="H7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="M7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="N7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="O7" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="P7" s="86" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A8" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="6">
-        <v>155488099780</v>
-      </c>
-      <c r="C8" s="6">
-        <v>109256561.01800001</v>
-      </c>
-      <c r="D8" s="6">
-        <v>155651878039</v>
-      </c>
-      <c r="E8" s="6">
-        <v>1240169394.24</v>
-      </c>
-      <c r="F8" s="6">
-        <v>155396097352</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1092945842.3599999</v>
-      </c>
-      <c r="H8" s="6">
-        <f>D8/B8</f>
-        <v>1.0010533170013123</v>
-      </c>
-      <c r="I8" s="6">
-        <f>F8/B8</f>
-        <v>0.99940829923235175</v>
-      </c>
-      <c r="J8" s="6">
-        <f>C8/B8</f>
-        <v>7.0266831463364102E-4</v>
+      <c r="D8" s="81">
+        <v>154918952634</v>
+      </c>
+      <c r="E8" s="81">
+        <v>280351869.92900002</v>
+      </c>
+      <c r="H8" s="81">
+        <v>155317428173</v>
+      </c>
+      <c r="I8" s="81">
+        <v>1411292601.6199999</v>
+      </c>
+      <c r="J8" s="6" t="e">
+        <f>#REF!/D8</f>
+        <v>#REF!</v>
       </c>
       <c r="K8" s="6">
-        <f>E8/B8</f>
-        <v>7.9759762708188908E-3</v>
-      </c>
-      <c r="L8" s="6">
-        <f>G8/B8</f>
-        <v>7.0291285565030901E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+        <f>H8/D8</f>
+        <v>1.0025721548734028</v>
+      </c>
+      <c r="M8" s="6">
+        <f>E8/D8</f>
+        <v>1.809667991955371E-3</v>
+      </c>
+      <c r="N8" s="6" t="e">
+        <f>#REF!/D8</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O8" s="6">
+        <f>I8/D8</f>
+        <v>9.1098769880933479E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A9" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="6">
-        <v>333482308492</v>
-      </c>
-      <c r="C9" s="6">
-        <v>396439847.07999998</v>
-      </c>
-      <c r="D9" s="6">
-        <v>328381134082</v>
-      </c>
-      <c r="E9" s="6">
-        <v>10031617594</v>
-      </c>
-      <c r="F9" s="6">
-        <v>331966609845</v>
-      </c>
-      <c r="G9" s="6">
-        <v>3160684862.4499998</v>
-      </c>
-      <c r="H9" s="6">
-        <f t="shared" ref="H9:H12" si="0">D9/B9</f>
-        <v>0.98470331324900739</v>
-      </c>
-      <c r="I9" s="6">
-        <f t="shared" ref="I9:I12" si="1">F9/B9</f>
-        <v>0.99545493536417584</v>
-      </c>
-      <c r="J9" s="6">
-        <f t="shared" ref="J9:J12" si="2">C9/B9</f>
-        <v>1.1887882414893091E-3</v>
+      <c r="D9" s="81">
+        <v>323888734975</v>
+      </c>
+      <c r="E9" s="81">
+        <v>1799069197.0699999</v>
+      </c>
+      <c r="H9" s="81">
+        <v>324404115108</v>
+      </c>
+      <c r="I9" s="81">
+        <v>3561778733.0300002</v>
+      </c>
+      <c r="J9" s="6" t="e">
+        <f>#REF!/D9</f>
+        <v>#REF!</v>
       </c>
       <c r="K9" s="6">
-        <f t="shared" ref="K9:K12" si="3">E9/B9</f>
-        <v>3.0081408634127442E-2</v>
-      </c>
-      <c r="L9" s="6">
-        <f t="shared" ref="L9:L12" si="4">G9/B9</f>
-        <v>9.477818708712166E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+        <f>H9/D9</f>
+        <v>1.0015912258666229</v>
+      </c>
+      <c r="M9" s="6">
+        <f>E9/D9</f>
+        <v>5.5545902120024788E-3</v>
+      </c>
+      <c r="N9" s="6" t="e">
+        <f>#REF!/D9</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O9" s="6">
+        <f>I9/D9</f>
+        <v>1.0996920696562426E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A10" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="6">
-        <v>78271163.599999994</v>
-      </c>
-      <c r="C10" s="6">
-        <v>1433465.8790899999</v>
-      </c>
-      <c r="D10" s="6">
-        <v>68326073.599999994</v>
-      </c>
-      <c r="E10" s="6">
-        <v>1214110.2608099999</v>
-      </c>
-      <c r="F10" s="6">
-        <v>62405817.399999999</v>
-      </c>
-      <c r="G10" s="6">
-        <v>806169.35760300001</v>
-      </c>
-      <c r="H10" s="6">
-        <f t="shared" si="0"/>
-        <v>0.87294056274896104</v>
-      </c>
-      <c r="I10" s="6">
-        <f t="shared" si="1"/>
-        <v>0.79730279364340517</v>
-      </c>
-      <c r="J10" s="6">
-        <f t="shared" si="2"/>
-        <v>1.8314099511994478E-2</v>
+      <c r="D10" s="81">
+        <v>67105167.399999999</v>
+      </c>
+      <c r="E10" s="81">
+        <v>851354.688035</v>
+      </c>
+      <c r="H10" s="81">
+        <v>54168281.200000003</v>
+      </c>
+      <c r="I10" s="81">
+        <v>275826.63121700002</v>
+      </c>
+      <c r="J10" s="6" t="e">
+        <f>#REF!/D10</f>
+        <v>#REF!</v>
       </c>
       <c r="K10" s="6">
-        <f t="shared" si="3"/>
-        <v>1.5511590794978292E-2</v>
-      </c>
-      <c r="L10" s="6">
-        <f t="shared" si="4"/>
-        <v>1.0299698133055481E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+        <f>H10/D10</f>
+        <v>0.80721475407570487</v>
+      </c>
+      <c r="M10" s="6">
+        <f>E10/D10</f>
+        <v>1.2686872278557195E-2</v>
+      </c>
+      <c r="N10" s="6" t="e">
+        <f>#REF!/D10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O10" s="6">
+        <f>I10/D10</f>
+        <v>4.1103635070732277E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A11" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="6">
-        <v>32476392.600000001</v>
-      </c>
-      <c r="C11" s="6">
-        <v>1704563.7003500001</v>
-      </c>
-      <c r="D11" s="6">
-        <v>26894871.600000001</v>
-      </c>
-      <c r="E11" s="6">
-        <v>1063580.79907</v>
-      </c>
-      <c r="F11" s="6">
-        <v>4609278</v>
-      </c>
-      <c r="G11" s="6">
-        <v>257185.27273500001</v>
-      </c>
-      <c r="H11" s="6">
-        <f t="shared" si="0"/>
-        <v>0.82813605350983477</v>
-      </c>
-      <c r="I11" s="6">
-        <f t="shared" si="1"/>
-        <v>0.1419270316371283</v>
-      </c>
-      <c r="J11" s="6">
-        <f t="shared" si="2"/>
-        <v>5.2486238891877417E-2</v>
+      <c r="D11" s="81">
+        <v>15824359</v>
+      </c>
+      <c r="E11" s="81">
+        <v>1011097.01176</v>
+      </c>
+      <c r="H11" s="81">
+        <v>4744871.2</v>
+      </c>
+      <c r="I11" s="81">
+        <v>436397.91209400003</v>
+      </c>
+      <c r="J11" s="6" t="e">
+        <f>#REF!/D11</f>
+        <v>#REF!</v>
       </c>
       <c r="K11" s="6">
-        <f t="shared" si="3"/>
-        <v>3.2749351572686672E-2</v>
-      </c>
-      <c r="L11" s="6">
-        <f t="shared" si="4"/>
-        <v>7.9191453281975653E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+        <f>H11/D11</f>
+        <v>0.29984602851843795</v>
+      </c>
+      <c r="M11" s="6">
+        <f>E11/D11</f>
+        <v>6.3894974308911973E-2</v>
+      </c>
+      <c r="N11" s="6" t="e">
+        <f>#REF!/D11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O11" s="6">
+        <f>I11/D11</f>
+        <v>2.7577604381574004E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A12" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="6">
-        <v>13127022678.4</v>
-      </c>
-      <c r="C12" s="6">
-        <v>210486566.602</v>
-      </c>
-      <c r="D12" s="6">
-        <v>13630958501.799999</v>
-      </c>
-      <c r="E12" s="6">
-        <v>220806167.229</v>
-      </c>
-      <c r="F12" s="6">
-        <v>13408413157</v>
-      </c>
-      <c r="G12" s="6">
-        <v>190294880.90900001</v>
-      </c>
-      <c r="H12" s="6">
-        <f t="shared" si="0"/>
-        <v>1.0383891942404584</v>
-      </c>
-      <c r="I12" s="6">
-        <f t="shared" si="1"/>
-        <v>1.0214359710875656</v>
-      </c>
-      <c r="J12" s="6">
-        <f t="shared" si="2"/>
-        <v>1.6034600667548735E-2</v>
+      <c r="D12" s="81">
+        <v>13571559205.200001</v>
+      </c>
+      <c r="E12" s="81">
+        <v>124870350.419</v>
+      </c>
+      <c r="H12" s="81">
+        <v>13403081932.200001</v>
+      </c>
+      <c r="I12" s="81">
+        <v>112712714.513</v>
+      </c>
+      <c r="J12" s="6" t="e">
+        <f>#REF!/D12</f>
+        <v>#REF!</v>
       </c>
       <c r="K12" s="6">
-        <f t="shared" si="3"/>
-        <v>1.6820734803203157E-2</v>
-      </c>
-      <c r="L12" s="6">
-        <f t="shared" si="4"/>
-        <v>1.4496423566184795E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="83" t="s">
+        <f>H12/D12</f>
+        <v>0.98758600464009716</v>
+      </c>
+      <c r="M12" s="6">
+        <f>E12/D12</f>
+        <v>9.2008846243072338E-3</v>
+      </c>
+      <c r="N12" s="6" t="e">
+        <f>#REF!/D12</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O12" s="6">
+        <f>I12/D12</f>
+        <v>8.3050674435265794E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A13" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="81">
+        <v>3810031732.5999999</v>
+      </c>
+      <c r="E13" s="81">
+        <v>38318967.155400001</v>
+      </c>
+      <c r="H13" s="81">
+        <v>3431107693.1999998</v>
+      </c>
+      <c r="I13" s="81">
+        <v>54530811.428999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A14" s="80" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="81">
+        <v>1822701831.4000001</v>
+      </c>
+      <c r="E14" s="81">
+        <v>38027087.5339</v>
+      </c>
+      <c r="H14" s="81">
+        <v>504405128.39999998</v>
+      </c>
+      <c r="I14" s="81">
+        <v>39336546.523500003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="80" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="81">
+        <v>2019444030</v>
+      </c>
+      <c r="E15" s="81">
+        <v>44096097.7223</v>
+      </c>
+      <c r="H15" s="81">
+        <v>1934053663.5999999</v>
+      </c>
+      <c r="I15" s="81">
+        <v>150295057.50999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="18" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="83" t="s">
         <v>152</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-    </row>
-    <row r="17" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A17" s="2"/>
-      <c r="B17" s="74" t="s">
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+    </row>
+    <row r="19" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A19" s="2"/>
+      <c r="B19" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74" t="s">
+      <c r="C19" s="74"/>
+      <c r="D19" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="74"/>
-      <c r="F17" s="75" t="s">
+      <c r="E19" s="74"/>
+      <c r="F19" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="74"/>
-      <c r="H17" s="72" t="s">
+      <c r="G19" s="74"/>
+      <c r="H19" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="I17" s="73"/>
-      <c r="J17" s="82" t="s">
+      <c r="I19" s="73"/>
+      <c r="J19" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="K17" s="82" t="s">
+      <c r="K19" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="L17" s="75" t="s">
+      <c r="L19" s="85" t="s">
+        <v>115</v>
+      </c>
+      <c r="M19" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="M17" s="74"/>
-      <c r="N17" s="74"/>
-    </row>
-    <row r="18" spans="1:14" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A18" s="3" t="s">
+      <c r="N19" s="74"/>
+      <c r="O19" s="74"/>
+    </row>
+    <row r="20" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="H20" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="I20" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3" t="s">
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M18" s="82" t="s">
+      <c r="N20" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="N18" s="82" t="s">
+      <c r="O20" s="82" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A19" s="80" t="s">
+      <c r="P20" s="86" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A21" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="81"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81">
+      <c r="B21" s="81">
+        <v>154224661811</v>
+      </c>
+      <c r="C21" s="81">
+        <v>396037299.84799999</v>
+      </c>
+      <c r="D21" s="81">
         <v>154231498991</v>
       </c>
-      <c r="E19" s="81">
+      <c r="E21" s="81">
         <v>776501347.76400006</v>
       </c>
-      <c r="H19" s="81">
+      <c r="F21" s="81">
+        <v>151858466289</v>
+      </c>
+      <c r="G21" s="81">
+        <v>357254358.009</v>
+      </c>
+      <c r="H21" s="81">
         <v>153324861138</v>
       </c>
-      <c r="I19" s="81">
+      <c r="I21" s="81">
         <v>336290655.68900001</v>
       </c>
-      <c r="J19" s="81"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A20" s="80" t="s">
+      <c r="J21" s="81">
+        <f>D21/B21</f>
+        <v>1.0000443325984296</v>
+      </c>
+      <c r="K21" s="81">
+        <f>F21/B21</f>
+        <v>0.98465747634512735</v>
+      </c>
+      <c r="L21" s="81">
+        <f>H21/B21</f>
+        <v>0.99416564988741751</v>
+      </c>
+      <c r="M21" s="81">
+        <f>C21/B21</f>
+        <v>2.5679245796196831E-3</v>
+      </c>
+      <c r="N21" s="81">
+        <f>E21/B21</f>
+        <v>5.0348714573003293E-3</v>
+      </c>
+      <c r="O21" s="81">
+        <f>G21/B21</f>
+        <v>2.3164541508076692E-3</v>
+      </c>
+      <c r="P21" s="81">
+        <f>I21/B21</f>
+        <v>2.180524513654756E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A22" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="81"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81">
+      <c r="B22" s="81">
+        <v>334478074273</v>
+      </c>
+      <c r="C22" s="81">
+        <v>1257152096.21</v>
+      </c>
+      <c r="D22" s="81">
         <v>320995802715</v>
       </c>
-      <c r="E20" s="81">
+      <c r="E22" s="81">
         <v>2139277529.4000001</v>
       </c>
-      <c r="H20" s="81">
+      <c r="F22" s="81">
+        <v>326887773402</v>
+      </c>
+      <c r="G22" s="81">
+        <v>1119009493.4200001</v>
+      </c>
+      <c r="H22" s="81">
         <v>328914925755</v>
       </c>
-      <c r="I20" s="81">
+      <c r="I22" s="81">
         <v>11811502965.6</v>
       </c>
-      <c r="J20" s="81"/>
-      <c r="K20" s="81"/>
-      <c r="L20" s="81"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A21" s="80" t="s">
+      <c r="J22" s="81">
+        <f t="shared" ref="J22:J28" si="0">D22/B22</f>
+        <v>0.95969161330737685</v>
+      </c>
+      <c r="K22" s="81">
+        <f t="shared" ref="K22:K28" si="1">F22/B22</f>
+        <v>0.97730703010205444</v>
+      </c>
+      <c r="L22" s="81">
+        <f t="shared" ref="L22:L28" si="2">H22/B22</f>
+        <v>0.98336767356098986</v>
+      </c>
+      <c r="M22" s="81">
+        <f t="shared" ref="M22:M28" si="3">C22/B22</f>
+        <v>3.7585485952777767E-3</v>
+      </c>
+      <c r="N22" s="81">
+        <f t="shared" ref="N22:N28" si="4">E22/B22</f>
+        <v>6.3958677532146048E-3</v>
+      </c>
+      <c r="O22" s="81">
+        <f t="shared" ref="O22:O28" si="5">G22/B22</f>
+        <v>3.3455391533576814E-3</v>
+      </c>
+      <c r="P22" s="81">
+        <f t="shared" ref="P22:P28" si="6">I22/B22</f>
+        <v>3.5313235378051977E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A23" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="81"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81">
+      <c r="B23" s="81">
+        <v>91553547.599999994</v>
+      </c>
+      <c r="C23" s="81">
+        <v>1407369.3687</v>
+      </c>
+      <c r="D23" s="81">
         <v>55426876</v>
       </c>
-      <c r="E21" s="81">
+      <c r="E23" s="81">
         <v>1793666.85338</v>
       </c>
-      <c r="H21" s="81">
+      <c r="F23" s="81">
+        <v>71791787.599999994</v>
+      </c>
+      <c r="G23" s="81">
+        <v>2846669.9186200001</v>
+      </c>
+      <c r="H23" s="81">
         <v>46162437.600000001</v>
       </c>
-      <c r="I21" s="81">
+      <c r="I23" s="81">
         <v>1415999.3302199999</v>
       </c>
-      <c r="J21" s="81"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="81"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A22" s="80" t="s">
+      <c r="J23" s="81">
+        <f t="shared" si="0"/>
+        <v>0.60540391337058364</v>
+      </c>
+      <c r="K23" s="81">
+        <f t="shared" si="1"/>
+        <v>0.7841508000723284</v>
+      </c>
+      <c r="L23" s="81">
+        <f t="shared" si="2"/>
+        <v>0.50421243971544372</v>
+      </c>
+      <c r="M23" s="81">
+        <f t="shared" si="3"/>
+        <v>1.5372089947282393E-2</v>
+      </c>
+      <c r="N23" s="81">
+        <f t="shared" si="4"/>
+        <v>1.9591451127776945E-2</v>
+      </c>
+      <c r="O23" s="81">
+        <f t="shared" si="5"/>
+        <v>3.1092950445319505E-2</v>
+      </c>
+      <c r="P23" s="81">
+        <f t="shared" si="6"/>
+        <v>1.546635130302695E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A24" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="81"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81">
+      <c r="B24" s="81">
+        <v>11773123.6</v>
+      </c>
+      <c r="C24" s="81">
+        <v>488609.35972299997</v>
+      </c>
+      <c r="D24" s="81">
         <v>7471985</v>
       </c>
-      <c r="E22" s="81">
+      <c r="E24" s="81">
         <v>261195.06404100001</v>
       </c>
-      <c r="H22" s="81">
+      <c r="F24" s="81">
+        <v>14173087.6</v>
+      </c>
+      <c r="G24" s="81">
+        <v>6172868.7977600005</v>
+      </c>
+      <c r="H24" s="81">
         <v>3821710</v>
       </c>
-      <c r="I22" s="81">
+      <c r="I24" s="81">
         <v>508277.09580800001</v>
       </c>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A23" s="80" t="s">
+      <c r="J24" s="81">
+        <f t="shared" si="0"/>
+        <v>0.63466461865736301</v>
+      </c>
+      <c r="K24" s="81">
+        <f t="shared" si="1"/>
+        <v>1.2038510833267733</v>
+      </c>
+      <c r="L24" s="81">
+        <f t="shared" si="2"/>
+        <v>0.32461308738829514</v>
+      </c>
+      <c r="M24" s="81">
+        <f t="shared" si="3"/>
+        <v>4.1502100574481351E-2</v>
+      </c>
+      <c r="N24" s="81">
+        <f t="shared" si="4"/>
+        <v>2.2185706437414791E-2</v>
+      </c>
+      <c r="O24" s="81">
+        <f t="shared" si="5"/>
+        <v>0.52431869463767466</v>
+      </c>
+      <c r="P24" s="81">
+        <f t="shared" si="6"/>
+        <v>4.3172662844378873E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A25" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="81"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="81">
+      <c r="B25" s="81">
+        <v>13403983485.6</v>
+      </c>
+      <c r="C25" s="81">
+        <v>121796591.243</v>
+      </c>
+      <c r="D25" s="81">
         <v>13356814029.799999</v>
       </c>
-      <c r="E23" s="81">
+      <c r="E25" s="81">
         <v>244857269.73199999</v>
       </c>
-      <c r="H23" s="81">
+      <c r="F25" s="81">
+        <v>13099183008.6</v>
+      </c>
+      <c r="G25" s="81">
+        <v>86653181.352899998</v>
+      </c>
+      <c r="H25" s="81">
         <v>13620259009.4</v>
       </c>
-      <c r="I23" s="81">
+      <c r="I25" s="81">
         <v>186564319.986</v>
       </c>
-      <c r="J23" s="81"/>
-      <c r="K23" s="81"/>
-      <c r="L23" s="81"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A24" s="80" t="s">
+      <c r="J25" s="81">
+        <f t="shared" si="0"/>
+        <v>0.99648093748767474</v>
+      </c>
+      <c r="K25" s="81">
+        <f t="shared" si="1"/>
+        <v>0.97726045564533492</v>
+      </c>
+      <c r="L25" s="81">
+        <f t="shared" si="2"/>
+        <v>1.0161351678799326</v>
+      </c>
+      <c r="M25" s="81">
+        <f t="shared" si="3"/>
+        <v>9.0865966355335327E-3</v>
+      </c>
+      <c r="N25" s="81">
+        <f t="shared" si="4"/>
+        <v>1.8267500105103231E-2</v>
+      </c>
+      <c r="O25" s="81">
+        <f t="shared" si="5"/>
+        <v>6.4647335208963931E-3</v>
+      </c>
+      <c r="P25" s="81">
+        <f t="shared" si="6"/>
+        <v>1.3918572802363376E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A26" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="81">
+      <c r="B26" s="81">
+        <v>4207290989</v>
+      </c>
+      <c r="C26" s="81">
+        <v>47812624.160400003</v>
+      </c>
+      <c r="D26" s="81">
         <v>3557269894.1999998</v>
       </c>
-      <c r="E24" s="81">
+      <c r="E26" s="81">
         <v>24548824.4307</v>
       </c>
-      <c r="H24" s="81">
+      <c r="F26" s="81">
+        <v>3744450908.5999999</v>
+      </c>
+      <c r="G26" s="81">
+        <v>52157654.794100001</v>
+      </c>
+      <c r="H26" s="81">
         <v>2911940947</v>
       </c>
-      <c r="I24" s="81">
+      <c r="I26" s="81">
         <v>53453576.313600004</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A25" s="80" t="s">
+      <c r="J26" s="81">
+        <f t="shared" si="0"/>
+        <v>0.84550127469207947</v>
+      </c>
+      <c r="K26" s="81">
+        <f t="shared" si="1"/>
+        <v>0.88999095103949322</v>
+      </c>
+      <c r="L26" s="81">
+        <f t="shared" si="2"/>
+        <v>0.69211779138008178</v>
+      </c>
+      <c r="M26" s="81">
+        <f t="shared" si="3"/>
+        <v>1.1364230400370818E-2</v>
+      </c>
+      <c r="N26" s="81">
+        <f t="shared" si="4"/>
+        <v>5.8348292273776928E-3</v>
+      </c>
+      <c r="O26" s="81">
+        <f t="shared" si="5"/>
+        <v>1.2396968721789544E-2</v>
+      </c>
+      <c r="P26" s="81">
+        <f t="shared" si="6"/>
+        <v>1.2704986760686356E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A27" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="81">
+      <c r="B27" s="81">
+        <v>1591523887.2</v>
+      </c>
+      <c r="C27" s="81">
+        <v>46781665.820299998</v>
+      </c>
+      <c r="D27" s="81">
         <v>885658835</v>
       </c>
-      <c r="E25" s="81">
+      <c r="E27" s="81">
         <v>49874908.9133</v>
       </c>
-      <c r="H25" s="81">
+      <c r="F27" s="81">
+        <v>852721605.60000002</v>
+      </c>
+      <c r="G27" s="81">
+        <v>74307902.240899995</v>
+      </c>
+      <c r="H27" s="81">
         <v>379748471.39999998</v>
       </c>
-      <c r="I25" s="81">
+      <c r="I27" s="81">
         <v>8505820.7215299997</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A26" s="80" t="s">
+      <c r="J27" s="81">
+        <f t="shared" si="0"/>
+        <v>0.55648478927837985</v>
+      </c>
+      <c r="K27" s="81">
+        <f t="shared" si="1"/>
+        <v>0.5357893855430661</v>
+      </c>
+      <c r="L27" s="81">
+        <f t="shared" si="2"/>
+        <v>0.23860683113471773</v>
+      </c>
+      <c r="M27" s="81">
+        <f t="shared" si="3"/>
+        <v>2.9394259298617203E-2</v>
+      </c>
+      <c r="N27" s="81">
+        <f t="shared" si="4"/>
+        <v>3.1337832447520426E-2</v>
+      </c>
+      <c r="O27" s="81">
+        <f t="shared" si="5"/>
+        <v>4.668978130867478E-2</v>
+      </c>
+      <c r="P27" s="81">
+        <f t="shared" si="6"/>
+        <v>5.3444505545527567E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A28" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="81">
+      <c r="B28" s="81">
+        <v>103376374</v>
+      </c>
+      <c r="C28" s="81">
+        <v>2023324.2933499999</v>
+      </c>
+      <c r="D28" s="81">
         <v>105115239.59999999</v>
       </c>
-      <c r="E26" s="81">
+      <c r="E28" s="81">
         <v>1651547.44683</v>
       </c>
-      <c r="H26" s="81">
+      <c r="F28" s="81">
+        <v>101048964</v>
+      </c>
+      <c r="G28" s="81">
+        <v>2492931.63693</v>
+      </c>
+      <c r="H28" s="81">
         <v>106508726.8</v>
       </c>
-      <c r="I26" s="81">
+      <c r="I28" s="81">
         <v>2375056.0667400002</v>
       </c>
+      <c r="J28" s="81">
+        <f t="shared" si="0"/>
+        <v>1.0168207254009509</v>
+      </c>
+      <c r="K28" s="81">
+        <f t="shared" si="1"/>
+        <v>0.97748605498583263</v>
+      </c>
+      <c r="L28" s="81">
+        <f t="shared" si="2"/>
+        <v>1.030300470782618</v>
+      </c>
+      <c r="M28" s="81">
+        <f t="shared" si="3"/>
+        <v>1.9572405328803659E-2</v>
+      </c>
+      <c r="N28" s="81">
+        <f t="shared" si="4"/>
+        <v>1.5976062836465903E-2</v>
+      </c>
+      <c r="O28" s="81">
+        <f t="shared" si="5"/>
+        <v>2.4115100389669308E-2</v>
+      </c>
+      <c r="P28" s="81">
+        <f t="shared" si="6"/>
+        <v>2.2974844007780736E-2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
added results for octane
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="971" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{58A10D46-473E-4078-9D5B-D0A3C73830ED}"/>
+  <xr:revisionPtr revIDLastSave="999" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{B02C1C1D-519F-40D7-A33A-E3CCCDF66C15}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <sheet name="postgres-4GB-usr" sheetId="8" r:id="rId10"/>
     <sheet name="postgres-1GB-os" sheetId="18" r:id="rId11"/>
     <sheet name="postgres-1GB-usr" sheetId="19" r:id="rId12"/>
-    <sheet name="postgres_stats" sheetId="9" r:id="rId13"/>
+    <sheet name="octane-os" sheetId="20" r:id="rId13"/>
+    <sheet name="octane-usr" sheetId="21" r:id="rId14"/>
+    <sheet name="postgres_stats" sheetId="9" r:id="rId15"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="155">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -519,6 +521,9 @@
   </si>
   <si>
     <t>1GB/2MB * 2 # of super pages for each iteration</t>
+  </si>
+  <si>
+    <t>node run.js for 4 iterations</t>
   </si>
 </sst>
 </file>
@@ -864,6 +869,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -885,25 +903,12 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1213,22 +1218,22 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="57" x14ac:dyDescent="0.45">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72" t="s">
+      <c r="C3" s="79"/>
+      <c r="D3" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72" t="s">
+      <c r="E3" s="79"/>
+      <c r="F3" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="72"/>
-      <c r="H3" s="73" t="s">
+      <c r="G3" s="79"/>
+      <c r="H3" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="74"/>
+      <c r="I3" s="81"/>
       <c r="J3" s="33" t="s">
         <v>45</v>
       </c>
@@ -1238,12 +1243,12 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="72" t="s">
+      <c r="M3" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="79"/>
     </row>
     <row r="4" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
@@ -3197,927 +3202,927 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="35" style="80" customWidth="1"/>
-    <col min="2" max="2" width="19.19921875" style="80" customWidth="1"/>
-    <col min="3" max="3" width="19.46484375" style="80" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.3984375" style="80" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="80" customWidth="1"/>
-    <col min="6" max="6" width="19.3984375" style="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.9296875" style="80" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.59765625" style="80" customWidth="1"/>
-    <col min="9" max="9" width="17" style="80" customWidth="1"/>
-    <col min="10" max="11" width="9.06640625" style="80"/>
-    <col min="12" max="12" width="13.1328125" style="80" customWidth="1"/>
-    <col min="13" max="15" width="9.06640625" style="80"/>
-    <col min="16" max="16" width="18.73046875" style="80" customWidth="1"/>
-    <col min="17" max="16384" width="9.06640625" style="80"/>
+    <col min="1" max="1" width="35" style="73" customWidth="1"/>
+    <col min="2" max="2" width="19.19921875" style="73" customWidth="1"/>
+    <col min="3" max="3" width="19.46484375" style="73" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" style="73" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="73" customWidth="1"/>
+    <col min="6" max="6" width="19.3984375" style="73" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.9296875" style="73" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.59765625" style="73" customWidth="1"/>
+    <col min="9" max="9" width="17" style="73" customWidth="1"/>
+    <col min="10" max="11" width="9.06640625" style="73"/>
+    <col min="12" max="12" width="13.1328125" style="73" customWidth="1"/>
+    <col min="13" max="15" width="9.06640625" style="73"/>
+    <col min="16" max="16" width="18.73046875" style="73" customWidth="1"/>
+    <col min="17" max="16384" width="9.06640625" style="73"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="72" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="72" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="73" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="74" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82" t="s">
+      <c r="C6" s="86"/>
+      <c r="D6" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82" t="s">
+      <c r="E6" s="86"/>
+      <c r="F6" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="82"/>
-      <c r="H6" s="83" t="s">
+      <c r="G6" s="86"/>
+      <c r="H6" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="83"/>
-      <c r="J6" s="84" t="s">
+      <c r="I6" s="87"/>
+      <c r="J6" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="84" t="s">
+      <c r="K6" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="L6" s="85" t="s">
+      <c r="L6" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="82" t="s">
+      <c r="M6" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="82"/>
-      <c r="O6" s="82"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="86"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="84" t="s">
+      <c r="E7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="84" t="s">
+      <c r="F7" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="84" t="s">
+      <c r="G7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="84" t="s">
+      <c r="H7" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="84" t="s">
+      <c r="I7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="84"/>
-      <c r="K7" s="84"/>
-      <c r="M7" s="84" t="s">
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="M7" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="N7" s="84" t="s">
+      <c r="N7" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="84" t="s">
+      <c r="O7" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="P7" s="86" t="s">
+      <c r="P7" s="77" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="87">
+      <c r="D8" s="78">
         <v>943944726458</v>
       </c>
-      <c r="E8" s="87">
+      <c r="E8" s="78">
         <v>8036919330.3100004</v>
       </c>
-      <c r="H8" s="87">
+      <c r="H8" s="78">
         <v>945025210371</v>
       </c>
-      <c r="I8" s="87">
+      <c r="I8" s="78">
         <v>7415023994.6800003</v>
       </c>
-      <c r="J8" s="87" t="e">
+      <c r="J8" s="78" t="e">
         <f>#REF!/D8</f>
         <v>#REF!</v>
       </c>
-      <c r="K8" s="87">
+      <c r="K8" s="78">
         <f t="shared" ref="K8:K15" si="0">H8/D8</f>
         <v>1.0011446474382608</v>
       </c>
-      <c r="M8" s="87">
+      <c r="M8" s="78">
         <f t="shared" ref="M8:M15" si="1">E8/D8</f>
         <v>8.514184257872006E-3</v>
       </c>
-      <c r="N8" s="87" t="e">
+      <c r="N8" s="78" t="e">
         <f>#REF!/D8</f>
         <v>#REF!</v>
       </c>
-      <c r="O8" s="87">
+      <c r="O8" s="78">
         <f t="shared" ref="O8:O15" si="2">I8/D8</f>
         <v>7.8553582501633117E-3</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A9" s="80" t="s">
+      <c r="A9" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="87">
+      <c r="D9" s="78">
         <v>1208883703350</v>
       </c>
-      <c r="E9" s="87">
+      <c r="E9" s="78">
         <v>11754126552.299999</v>
       </c>
-      <c r="H9" s="87">
+      <c r="H9" s="78">
         <v>1150780393290</v>
       </c>
-      <c r="I9" s="87">
+      <c r="I9" s="78">
         <v>10686477064.9</v>
       </c>
-      <c r="J9" s="87" t="e">
+      <c r="J9" s="78" t="e">
         <f>#REF!/D9</f>
         <v>#REF!</v>
       </c>
-      <c r="K9" s="87">
+      <c r="K9" s="78">
         <f t="shared" si="0"/>
         <v>0.95193639396495555</v>
       </c>
-      <c r="M9" s="87">
+      <c r="M9" s="78">
         <f t="shared" si="1"/>
         <v>9.7231243334057142E-3</v>
       </c>
-      <c r="N9" s="87" t="e">
+      <c r="N9" s="78" t="e">
         <f>#REF!/D9</f>
         <v>#REF!</v>
       </c>
-      <c r="O9" s="87">
+      <c r="O9" s="78">
         <f t="shared" si="2"/>
         <v>8.8399546087734922E-3</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A10" s="80" t="s">
+      <c r="A10" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="87">
+      <c r="D10" s="78">
         <v>429044136.60000002</v>
       </c>
-      <c r="E10" s="87">
+      <c r="E10" s="78">
         <v>17035425.073100001</v>
       </c>
-      <c r="H10" s="87">
+      <c r="H10" s="78">
         <v>107691606.59999999</v>
       </c>
-      <c r="I10" s="87">
+      <c r="I10" s="78">
         <v>978641.49078600004</v>
       </c>
-      <c r="J10" s="87" t="e">
+      <c r="J10" s="78" t="e">
         <f>#REF!/D10</f>
         <v>#REF!</v>
       </c>
-      <c r="K10" s="87">
+      <c r="K10" s="78">
         <f t="shared" si="0"/>
         <v>0.25100356213561642</v>
       </c>
-      <c r="M10" s="87">
+      <c r="M10" s="78">
         <f t="shared" si="1"/>
         <v>3.9705530550070686E-2</v>
       </c>
-      <c r="N10" s="87" t="e">
+      <c r="N10" s="78" t="e">
         <f>#REF!/D10</f>
         <v>#REF!</v>
       </c>
-      <c r="O10" s="87">
+      <c r="O10" s="78">
         <f t="shared" si="2"/>
         <v>2.2809809231780559E-3</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A11" s="80" t="s">
+      <c r="A11" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="87">
+      <c r="D11" s="78">
         <v>248961865.19999999</v>
       </c>
-      <c r="E11" s="87">
+      <c r="E11" s="78">
         <v>11418958.505999999</v>
       </c>
-      <c r="H11" s="87">
+      <c r="H11" s="78">
         <v>126322180.8</v>
       </c>
-      <c r="I11" s="87">
+      <c r="I11" s="78">
         <v>768366.61140000005</v>
       </c>
-      <c r="J11" s="87" t="e">
+      <c r="J11" s="78" t="e">
         <f>#REF!/D11</f>
         <v>#REF!</v>
       </c>
-      <c r="K11" s="87">
+      <c r="K11" s="78">
         <f t="shared" si="0"/>
         <v>0.50739570374973231</v>
       </c>
-      <c r="M11" s="87">
+      <c r="M11" s="78">
         <f t="shared" si="1"/>
         <v>4.5866295614497989E-2</v>
       </c>
-      <c r="N11" s="87" t="e">
+      <c r="N11" s="78" t="e">
         <f>#REF!/D11</f>
         <v>#REF!</v>
       </c>
-      <c r="O11" s="87">
+      <c r="O11" s="78">
         <f t="shared" si="2"/>
         <v>3.0862823540574922E-3</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="87">
+      <c r="D12" s="78">
         <v>50032630234.599998</v>
       </c>
-      <c r="E12" s="87">
+      <c r="E12" s="78">
         <v>402589850.713</v>
       </c>
-      <c r="H12" s="87">
+      <c r="H12" s="78">
         <v>50738369301</v>
       </c>
-      <c r="I12" s="87">
+      <c r="I12" s="78">
         <v>441963416.24599999</v>
       </c>
-      <c r="J12" s="87" t="e">
+      <c r="J12" s="78" t="e">
         <f>#REF!/D12</f>
         <v>#REF!</v>
       </c>
-      <c r="K12" s="87">
+      <c r="K12" s="78">
         <f t="shared" si="0"/>
         <v>1.0141055759629432</v>
       </c>
-      <c r="M12" s="87">
+      <c r="M12" s="78">
         <f t="shared" si="1"/>
         <v>8.0465458007160599E-3</v>
       </c>
-      <c r="N12" s="87" t="e">
+      <c r="N12" s="78" t="e">
         <f>#REF!/D12</f>
         <v>#REF!</v>
       </c>
-      <c r="O12" s="87">
+      <c r="O12" s="78">
         <f t="shared" si="2"/>
         <v>8.8335035390636092E-3</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="87">
+      <c r="D13" s="78">
         <v>21680931744.599998</v>
       </c>
-      <c r="E13" s="87">
+      <c r="E13" s="78">
         <v>236688616.986</v>
       </c>
-      <c r="H13" s="87">
+      <c r="H13" s="78">
         <v>8207865959.8000002</v>
       </c>
-      <c r="I13" s="87">
+      <c r="I13" s="78">
         <v>102438436.20299999</v>
       </c>
-      <c r="J13" s="87"/>
-      <c r="K13" s="87">
+      <c r="J13" s="78"/>
+      <c r="K13" s="78">
         <f t="shared" si="0"/>
         <v>0.37857533322313547</v>
       </c>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87">
+      <c r="L13" s="78"/>
+      <c r="M13" s="78">
         <f t="shared" si="1"/>
         <v>1.0916902454847279E-2</v>
       </c>
-      <c r="N13" s="87"/>
-      <c r="O13" s="87">
+      <c r="N13" s="78"/>
+      <c r="O13" s="78">
         <f t="shared" si="2"/>
         <v>4.7248170608956419E-3</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="87">
+      <c r="D14" s="78">
         <v>17982740923.200001</v>
       </c>
-      <c r="E14" s="87">
+      <c r="E14" s="78">
         <v>219770850.15400001</v>
       </c>
-      <c r="H14" s="87">
+      <c r="H14" s="78">
         <v>11542933099.4</v>
       </c>
-      <c r="I14" s="87">
+      <c r="I14" s="78">
         <v>145744926.20699999</v>
       </c>
-      <c r="J14" s="87"/>
-      <c r="K14" s="87">
+      <c r="J14" s="78"/>
+      <c r="K14" s="78">
         <f t="shared" si="0"/>
         <v>0.64188952889312678</v>
       </c>
-      <c r="L14" s="87"/>
-      <c r="M14" s="87">
+      <c r="L14" s="78"/>
+      <c r="M14" s="78">
         <f t="shared" si="1"/>
         <v>1.2221209830725412E-2</v>
       </c>
-      <c r="N14" s="87"/>
-      <c r="O14" s="87">
+      <c r="N14" s="78"/>
+      <c r="O14" s="78">
         <f t="shared" si="2"/>
         <v>8.1047114469057751E-3</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A15" s="80" t="s">
+      <c r="A15" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="87">
+      <c r="D15" s="78">
         <v>71249580938.399994</v>
       </c>
-      <c r="E15" s="87">
+      <c r="E15" s="78">
         <v>594405628.78699994</v>
       </c>
-      <c r="H15" s="87">
+      <c r="H15" s="78">
         <v>72147459341.199997</v>
       </c>
-      <c r="I15" s="87">
+      <c r="I15" s="78">
         <v>106593048.45</v>
       </c>
-      <c r="K15" s="87">
+      <c r="K15" s="78">
         <f t="shared" si="0"/>
         <v>1.0126018762633324</v>
       </c>
-      <c r="M15" s="87">
+      <c r="M15" s="78">
         <f t="shared" si="1"/>
         <v>8.3425842083324417E-3</v>
       </c>
-      <c r="O15" s="87">
+      <c r="O15" s="78">
         <f t="shared" si="2"/>
         <v>1.4960515843897636E-3</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="81" t="s">
+      <c r="A17" s="74" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B18" s="82" t="s">
+      <c r="B18" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="82"/>
-      <c r="D18" s="82" t="s">
+      <c r="C18" s="86"/>
+      <c r="D18" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="82"/>
-      <c r="F18" s="82" t="s">
+      <c r="E18" s="86"/>
+      <c r="F18" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="82"/>
-      <c r="H18" s="83" t="s">
+      <c r="G18" s="86"/>
+      <c r="H18" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="I18" s="83"/>
-      <c r="J18" s="84" t="s">
+      <c r="I18" s="87"/>
+      <c r="J18" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="K18" s="84" t="s">
+      <c r="K18" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="L18" s="85" t="s">
+      <c r="L18" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="M18" s="82" t="s">
+      <c r="M18" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="N18" s="82"/>
-      <c r="O18" s="82"/>
+      <c r="N18" s="86"/>
+      <c r="O18" s="86"/>
     </row>
     <row r="19" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A19" s="84" t="s">
+      <c r="A19" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="84" t="s">
+      <c r="B19" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="84" t="s">
+      <c r="C19" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="84" t="s">
+      <c r="D19" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="84" t="s">
+      <c r="E19" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="84" t="s">
+      <c r="F19" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="84" t="s">
+      <c r="G19" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="84" t="s">
+      <c r="H19" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="84" t="s">
+      <c r="I19" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="84"/>
-      <c r="K19" s="84"/>
-      <c r="M19" s="84" t="s">
+      <c r="J19" s="75"/>
+      <c r="K19" s="75"/>
+      <c r="M19" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="N19" s="84" t="s">
+      <c r="N19" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="O19" s="84" t="s">
+      <c r="O19" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="P19" s="86" t="s">
+      <c r="P19" s="77" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A20" s="80" t="s">
+      <c r="A20" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="87">
+      <c r="B20" s="78">
         <v>950961617600</v>
       </c>
-      <c r="C20" s="87">
+      <c r="C20" s="78">
         <v>3342695208.5900002</v>
       </c>
-      <c r="D20" s="87">
+      <c r="D20" s="78">
         <v>947044998803</v>
       </c>
-      <c r="E20" s="87">
+      <c r="E20" s="78">
         <v>4671101663.8400002</v>
       </c>
-      <c r="F20" s="87">
+      <c r="F20" s="78">
         <v>942333772624</v>
       </c>
-      <c r="G20" s="87">
+      <c r="G20" s="78">
         <v>1806397218.3</v>
       </c>
-      <c r="H20" s="87">
+      <c r="H20" s="78">
         <v>944883191889</v>
       </c>
-      <c r="I20" s="87">
+      <c r="I20" s="78">
         <v>6989132626.8100004</v>
       </c>
-      <c r="J20" s="87">
+      <c r="J20" s="78">
         <f>D20/B20</f>
         <v>0.99588141232567873</v>
       </c>
-      <c r="K20" s="87">
+      <c r="K20" s="78">
         <f>F20/B20</f>
         <v>0.99092724162960999</v>
       </c>
-      <c r="L20" s="87">
+      <c r="L20" s="78">
         <f>H20/B20</f>
         <v>0.99360812718567915</v>
       </c>
-      <c r="M20" s="87">
+      <c r="M20" s="78">
         <f>C20/B20</f>
         <v>3.5150684809195187E-3</v>
       </c>
-      <c r="N20" s="87">
+      <c r="N20" s="78">
         <f>E20/B20</f>
         <v>4.9119770739314856E-3</v>
       </c>
-      <c r="O20" s="87">
+      <c r="O20" s="78">
         <f>G20/B20</f>
         <v>1.8995479784546037E-3</v>
       </c>
-      <c r="P20" s="87">
+      <c r="P20" s="78">
         <f>I20/B20</f>
         <v>7.3495422921998699E-3</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A21" s="80" t="s">
+      <c r="A21" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="87">
+      <c r="B21" s="78">
         <v>1196533593690</v>
       </c>
-      <c r="C21" s="87">
+      <c r="C21" s="78">
         <v>3862807717.6399999</v>
       </c>
-      <c r="D21" s="87">
+      <c r="D21" s="78">
         <v>1203651140030</v>
       </c>
-      <c r="E21" s="87">
+      <c r="E21" s="78">
         <v>9785263329.6399994</v>
       </c>
-      <c r="F21" s="87">
+      <c r="F21" s="78">
         <v>1133790186310</v>
       </c>
-      <c r="G21" s="87">
+      <c r="G21" s="78">
         <v>1801538523.27</v>
       </c>
-      <c r="H21" s="87">
+      <c r="H21" s="78">
         <v>1145899823710</v>
       </c>
-      <c r="I21" s="87">
+      <c r="I21" s="78">
         <v>10497091805.6</v>
       </c>
-      <c r="J21" s="87">
+      <c r="J21" s="78">
         <f t="shared" ref="J21:J27" si="3">D21/B21</f>
         <v>1.0059484718001523</v>
       </c>
-      <c r="K21" s="87">
+      <c r="K21" s="78">
         <f t="shared" ref="K21:K27" si="4">F21/B21</f>
         <v>0.94756235202180572</v>
       </c>
-      <c r="L21" s="87">
+      <c r="L21" s="78">
         <f t="shared" ref="L21:L27" si="5">H21/B21</f>
         <v>0.95768295161371098</v>
       </c>
-      <c r="M21" s="87">
+      <c r="M21" s="78">
         <f t="shared" ref="M21:M27" si="6">C21/B21</f>
         <v>3.2283320234473773E-3</v>
       </c>
-      <c r="N21" s="87">
+      <c r="N21" s="78">
         <f t="shared" ref="N21:N27" si="7">E21/B21</f>
         <v>8.1780096950417776E-3</v>
       </c>
-      <c r="O21" s="87">
+      <c r="O21" s="78">
         <f t="shared" ref="O21:O27" si="8">G21/B21</f>
         <v>1.5056313778154947E-3</v>
       </c>
-      <c r="P21" s="87">
+      <c r="P21" s="78">
         <f t="shared" ref="P21:P27" si="9">I21/B21</f>
         <v>8.7729185882929796E-3</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A22" s="80" t="s">
+      <c r="A22" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="87">
+      <c r="B22" s="78">
         <v>387762805.60000002</v>
       </c>
-      <c r="C22" s="87">
+      <c r="C22" s="78">
         <v>6409107.8970799996</v>
       </c>
-      <c r="D22" s="87">
+      <c r="D22" s="78">
         <v>373726151.39999998</v>
       </c>
-      <c r="E22" s="87">
+      <c r="E22" s="78">
         <v>11967060.9714</v>
       </c>
-      <c r="F22" s="87">
+      <c r="F22" s="78">
         <v>84708735.599999994</v>
       </c>
-      <c r="G22" s="87">
+      <c r="G22" s="78">
         <v>3917699.6093700002</v>
       </c>
-      <c r="H22" s="87">
+      <c r="H22" s="78">
         <v>109409320.40000001</v>
       </c>
-      <c r="I22" s="87">
+      <c r="I22" s="78">
         <v>3682064.03516</v>
       </c>
-      <c r="J22" s="87">
+      <c r="J22" s="78">
         <f t="shared" si="3"/>
         <v>0.96380092675912898</v>
       </c>
-      <c r="K22" s="87">
+      <c r="K22" s="78">
         <f t="shared" si="4"/>
         <v>0.21845503069570318</v>
       </c>
-      <c r="L22" s="87">
+      <c r="L22" s="78">
         <f t="shared" si="5"/>
         <v>0.2821552733267102</v>
       </c>
-      <c r="M22" s="87">
+      <c r="M22" s="78">
         <f t="shared" si="6"/>
         <v>1.6528423573692028E-2</v>
       </c>
-      <c r="N22" s="87">
+      <c r="N22" s="78">
         <f t="shared" si="7"/>
         <v>3.086180726612733E-2</v>
       </c>
-      <c r="O22" s="87">
+      <c r="O22" s="78">
         <f t="shared" si="8"/>
         <v>1.0103340374041279E-2</v>
       </c>
-      <c r="P22" s="87">
+      <c r="P22" s="78">
         <f t="shared" si="9"/>
         <v>9.4956607028428199E-3</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A23" s="80" t="s">
+      <c r="A23" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="87">
+      <c r="B23" s="78">
         <v>197721030.40000001</v>
       </c>
-      <c r="C23" s="87">
+      <c r="C23" s="78">
         <v>3206633.6842399999</v>
       </c>
-      <c r="D23" s="87">
+      <c r="D23" s="78">
         <v>178376300</v>
       </c>
-      <c r="E23" s="87">
+      <c r="E23" s="78">
         <v>7016479.1470799996</v>
       </c>
-      <c r="F23" s="87">
+      <c r="F23" s="78">
         <v>74518004.200000003</v>
       </c>
-      <c r="G23" s="87">
+      <c r="G23" s="78">
         <v>603428.89475700003</v>
       </c>
-      <c r="H23" s="87">
+      <c r="H23" s="78">
         <v>72696324.200000003</v>
       </c>
-      <c r="I23" s="87">
+      <c r="I23" s="78">
         <v>1204122.4476600001</v>
       </c>
-      <c r="J23" s="87">
+      <c r="J23" s="78">
         <f t="shared" si="3"/>
         <v>0.90216149308515836</v>
       </c>
-      <c r="K23" s="87">
+      <c r="K23" s="78">
         <f t="shared" si="4"/>
         <v>0.3768845633124922</v>
       </c>
-      <c r="L23" s="87">
+      <c r="L23" s="78">
         <f t="shared" si="5"/>
         <v>0.36767117818944972</v>
       </c>
-      <c r="M23" s="87">
+      <c r="M23" s="78">
         <f t="shared" si="6"/>
         <v>1.6217969721039852E-2</v>
       </c>
-      <c r="N23" s="87">
+      <c r="N23" s="78">
         <f t="shared" si="7"/>
         <v>3.5486761994337652E-2</v>
       </c>
-      <c r="O23" s="87">
+      <c r="O23" s="78">
         <f t="shared" si="8"/>
         <v>3.0519206456502464E-3</v>
       </c>
-      <c r="P23" s="87">
+      <c r="P23" s="78">
         <f t="shared" si="9"/>
         <v>6.090006941719843E-3</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A24" s="80" t="s">
+      <c r="A24" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="87">
+      <c r="B24" s="78">
         <v>51646439040</v>
       </c>
-      <c r="C24" s="87">
+      <c r="C24" s="78">
         <v>427666677.69199997</v>
       </c>
-      <c r="D24" s="87">
+      <c r="D24" s="78">
         <v>50047193757.599998</v>
       </c>
-      <c r="E24" s="87">
+      <c r="E24" s="78">
         <v>256065872.794</v>
       </c>
-      <c r="F24" s="87">
+      <c r="F24" s="78">
         <v>50863014412</v>
       </c>
-      <c r="G24" s="87">
+      <c r="G24" s="78">
         <v>255246866.58399999</v>
       </c>
-      <c r="H24" s="87">
+      <c r="H24" s="78">
         <v>49480147960.800003</v>
       </c>
-      <c r="I24" s="87">
+      <c r="I24" s="78">
         <v>676041009.45899999</v>
       </c>
-      <c r="J24" s="87">
+      <c r="J24" s="78">
         <f t="shared" si="3"/>
         <v>0.96903474252772026</v>
       </c>
-      <c r="K24" s="87">
+      <c r="K24" s="78">
         <f t="shared" si="4"/>
         <v>0.98483100398474244</v>
       </c>
-      <c r="L24" s="87">
+      <c r="L24" s="78">
         <f t="shared" si="5"/>
         <v>0.95805536413609826</v>
       </c>
-      <c r="M24" s="87">
+      <c r="M24" s="78">
         <f t="shared" si="6"/>
         <v>8.2806614674977592E-3</v>
       </c>
-      <c r="N24" s="87">
+      <c r="N24" s="78">
         <f t="shared" si="7"/>
         <v>4.9580547575734666E-3</v>
       </c>
-      <c r="O24" s="87">
+      <c r="O24" s="78">
         <f t="shared" si="8"/>
         <v>4.9421968160537092E-3</v>
       </c>
-      <c r="P24" s="87">
+      <c r="P24" s="78">
         <f t="shared" si="9"/>
         <v>1.3089789383841323E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A25" s="80" t="s">
+      <c r="A25" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="87">
+      <c r="B25" s="78">
         <v>21131880797.200001</v>
       </c>
-      <c r="C25" s="87">
+      <c r="C25" s="78">
         <v>480889559.88700002</v>
       </c>
-      <c r="D25" s="87">
+      <c r="D25" s="78">
         <v>19963233833.799999</v>
       </c>
-      <c r="E25" s="87">
+      <c r="E25" s="78">
         <v>208319673.255</v>
       </c>
-      <c r="F25" s="87">
+      <c r="F25" s="78">
         <v>6226879954.8000002</v>
       </c>
-      <c r="G25" s="87">
+      <c r="G25" s="78">
         <v>204481330.852</v>
       </c>
-      <c r="H25" s="87">
+      <c r="H25" s="78">
         <v>8088796149.8000002</v>
       </c>
-      <c r="I25" s="87">
+      <c r="I25" s="78">
         <v>104743077.28399999</v>
       </c>
-      <c r="J25" s="87">
+      <c r="J25" s="78">
         <f t="shared" si="3"/>
         <v>0.94469744673390132</v>
       </c>
-      <c r="K25" s="87">
+      <c r="K25" s="78">
         <f t="shared" si="4"/>
         <v>0.29466756956271822</v>
       </c>
-      <c r="L25" s="87">
+      <c r="L25" s="78">
         <f t="shared" si="5"/>
         <v>0.38277691547795289</v>
       </c>
-      <c r="M25" s="87">
+      <c r="M25" s="78">
         <f t="shared" si="6"/>
         <v>2.275659059891718E-2</v>
       </c>
-      <c r="N25" s="87">
+      <c r="N25" s="78">
         <f t="shared" si="7"/>
         <v>9.8580753532644672E-3</v>
       </c>
-      <c r="O25" s="87">
+      <c r="O25" s="78">
         <f t="shared" si="8"/>
         <v>9.6764378341133751E-3</v>
       </c>
-      <c r="P25" s="87">
+      <c r="P25" s="78">
         <f t="shared" si="9"/>
         <v>4.9566377119578762E-3</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A26" s="80" t="s">
+      <c r="A26" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="87">
+      <c r="B26" s="78">
         <v>11957535869.799999</v>
       </c>
-      <c r="C26" s="87">
+      <c r="C26" s="78">
         <v>180159381.93700001</v>
       </c>
-      <c r="D26" s="87">
+      <c r="D26" s="78">
         <v>11291216904.799999</v>
       </c>
-      <c r="E26" s="87">
+      <c r="E26" s="78">
         <v>101645055.061</v>
       </c>
-      <c r="F26" s="87">
+      <c r="F26" s="78">
         <v>4954524262.3999996</v>
       </c>
-      <c r="G26" s="87">
+      <c r="G26" s="78">
         <v>72885506.043899998</v>
       </c>
-      <c r="H26" s="87">
+      <c r="H26" s="78">
         <v>4792947991</v>
       </c>
-      <c r="I26" s="87">
+      <c r="I26" s="78">
         <v>250072949.72400001</v>
       </c>
-      <c r="J26" s="87">
+      <c r="J26" s="78">
         <f t="shared" si="3"/>
         <v>0.9442762311353079</v>
       </c>
-      <c r="K26" s="87">
+      <c r="K26" s="78">
         <f t="shared" si="4"/>
         <v>0.41434324900610719</v>
       </c>
-      <c r="L26" s="87">
+      <c r="L26" s="78">
         <f t="shared" si="5"/>
         <v>0.40083074332271823</v>
       </c>
-      <c r="M26" s="87">
+      <c r="M26" s="78">
         <f t="shared" si="6"/>
         <v>1.5066597658470026E-2</v>
       </c>
-      <c r="N26" s="87">
+      <c r="N26" s="78">
         <f t="shared" si="7"/>
         <v>8.5005017896467427E-3</v>
       </c>
-      <c r="O26" s="87">
+      <c r="O26" s="78">
         <f t="shared" si="8"/>
         <v>6.0953616896922656E-3</v>
       </c>
-      <c r="P26" s="87">
+      <c r="P26" s="78">
         <f t="shared" si="9"/>
         <v>2.0913418320206361E-2</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A27" s="80" t="s">
+      <c r="A27" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="87">
+      <c r="B27" s="78">
         <v>63735346968.599998</v>
       </c>
-      <c r="C27" s="87">
+      <c r="C27" s="78">
         <v>70283082.364500001</v>
       </c>
-      <c r="D27" s="87">
+      <c r="D27" s="78">
         <v>63401290363.800003</v>
       </c>
-      <c r="E27" s="87">
+      <c r="E27" s="78">
         <v>105764495.332</v>
       </c>
-      <c r="F27" s="87">
+      <c r="F27" s="78">
         <v>62937469818.199997</v>
       </c>
-      <c r="G27" s="87">
+      <c r="G27" s="78">
         <v>118134134.51100001</v>
       </c>
-      <c r="H27" s="87">
+      <c r="H27" s="78">
         <v>63760215368.599998</v>
       </c>
-      <c r="I27" s="87">
+      <c r="I27" s="78">
         <v>554303853.73599994</v>
       </c>
-      <c r="J27" s="87">
+      <c r="J27" s="78">
         <f t="shared" si="3"/>
         <v>0.99475869167285502</v>
       </c>
-      <c r="K27" s="87">
+      <c r="K27" s="78">
         <f t="shared" si="4"/>
         <v>0.9874814025756683</v>
       </c>
-      <c r="L27" s="87">
+      <c r="L27" s="78">
         <f t="shared" si="5"/>
         <v>1.0003901822329806</v>
       </c>
-      <c r="M27" s="87">
+      <c r="M27" s="78">
         <f t="shared" si="6"/>
         <v>1.1027331882122776E-3</v>
       </c>
-      <c r="N27" s="87">
+      <c r="N27" s="78">
         <f t="shared" si="7"/>
         <v>1.6594323301339551E-3</v>
       </c>
-      <c r="O27" s="87">
+      <c r="O27" s="78">
         <f t="shared" si="8"/>
         <v>1.853510495035043E-3</v>
       </c>
-      <c r="P27" s="87">
+      <c r="P27" s="78">
         <f t="shared" si="9"/>
         <v>8.696961420937812E-3</v>
       </c>
@@ -4144,7 +4149,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+      <selection activeCell="A6" sqref="A6:P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4161,95 +4166,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="72" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="72" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="73" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="80"/>
-      <c r="B6" s="82" t="s">
+      <c r="A6" s="73"/>
+      <c r="B6" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82" t="s">
+      <c r="C6" s="86"/>
+      <c r="D6" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82" t="s">
+      <c r="E6" s="86"/>
+      <c r="F6" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="82"/>
-      <c r="H6" s="83" t="s">
+      <c r="G6" s="86"/>
+      <c r="H6" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="83"/>
-      <c r="J6" s="84" t="s">
+      <c r="I6" s="87"/>
+      <c r="J6" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="84" t="s">
+      <c r="K6" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="L6" s="85" t="s">
+      <c r="L6" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="82" t="s">
+      <c r="M6" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="82"/>
-      <c r="O6" s="82"/>
-      <c r="P6" s="80"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="84" t="s">
+      <c r="E7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="84" t="s">
+      <c r="F7" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="84" t="s">
+      <c r="G7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="84" t="s">
+      <c r="H7" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="84" t="s">
+      <c r="I7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="84"/>
-      <c r="K7" s="84"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="84" t="s">
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="N7" s="84" t="s">
+      <c r="N7" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="84" t="s">
+      <c r="O7" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="P7" s="86" t="s">
+      <c r="P7" s="77" t="s">
         <v>118</v>
       </c>
     </row>
@@ -4725,7 +4730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1814E241-F455-4452-B5DE-B4EE59F14CFA}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -4743,95 +4748,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="72" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="72" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="73" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="80"/>
-      <c r="B6" s="82" t="s">
+      <c r="A6" s="73"/>
+      <c r="B6" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82" t="s">
+      <c r="C6" s="86"/>
+      <c r="D6" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82" t="s">
+      <c r="E6" s="86"/>
+      <c r="F6" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="82"/>
-      <c r="H6" s="83" t="s">
+      <c r="G6" s="86"/>
+      <c r="H6" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="83"/>
-      <c r="J6" s="84" t="s">
+      <c r="I6" s="87"/>
+      <c r="J6" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="84" t="s">
+      <c r="K6" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="L6" s="85" t="s">
+      <c r="L6" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="82" t="s">
+      <c r="M6" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="82"/>
-      <c r="O6" s="82"/>
-      <c r="P6" s="80"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="84" t="s">
+      <c r="E7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="84" t="s">
+      <c r="F7" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="84" t="s">
+      <c r="G7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="84" t="s">
+      <c r="H7" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="84" t="s">
+      <c r="I7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="84"/>
-      <c r="K7" s="84"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="84" t="s">
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="N7" s="84" t="s">
+      <c r="N7" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="84" t="s">
+      <c r="O7" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="P7" s="86" t="s">
+      <c r="P7" s="77" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5304,6 +5309,1151 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC958D8-824A-4FFE-8EFB-EA4CAF2DCC74}">
+  <dimension ref="A1:P12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.73046875" customWidth="1"/>
+    <col min="3" max="3" width="16.796875" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A3" s="73"/>
+      <c r="B3" s="86" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="86"/>
+      <c r="H3" s="87" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="87"/>
+      <c r="J3" s="75" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="76" t="s">
+        <v>115</v>
+      </c>
+      <c r="M3" s="86" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="73"/>
+    </row>
+    <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A4" s="75" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="75" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="75" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4" s="77" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A5" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="66">
+        <v>496591292</v>
+      </c>
+      <c r="C5" s="66">
+        <v>4018490.6334899999</v>
+      </c>
+      <c r="D5" s="66">
+        <v>500136116.60000002</v>
+      </c>
+      <c r="E5" s="66">
+        <v>11596117.205800001</v>
+      </c>
+      <c r="F5" s="66">
+        <v>493339560.19999999</v>
+      </c>
+      <c r="G5" s="66">
+        <v>4525908.4988099998</v>
+      </c>
+      <c r="H5" s="66">
+        <v>499474230.60000002</v>
+      </c>
+      <c r="I5" s="66">
+        <v>4383930.4332499998</v>
+      </c>
+      <c r="J5" s="66">
+        <f>D5/B5</f>
+        <v>1.0071383140564616</v>
+      </c>
+      <c r="K5" s="66">
+        <f>F5/B5</f>
+        <v>0.99345189524587951</v>
+      </c>
+      <c r="L5" s="66">
+        <f>H5/B5</f>
+        <v>1.0058054554045623</v>
+      </c>
+      <c r="M5" s="66">
+        <f>C5/B5</f>
+        <v>8.0921488117636983E-3</v>
+      </c>
+      <c r="N5" s="66">
+        <f>E5/B5</f>
+        <v>2.3351430829761714E-2</v>
+      </c>
+      <c r="O5" s="66">
+        <f>G5/B5</f>
+        <v>9.1139505901968176E-3</v>
+      </c>
+      <c r="P5" s="66">
+        <f>I5/B5</f>
+        <v>8.8280453239401539E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A6" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="66">
+        <v>24622719852.200001</v>
+      </c>
+      <c r="C6" s="66">
+        <v>97892683.567200005</v>
+      </c>
+      <c r="D6" s="66">
+        <v>24559805519.200001</v>
+      </c>
+      <c r="E6" s="66">
+        <v>202827566.98300001</v>
+      </c>
+      <c r="F6" s="66">
+        <v>24641323621.400002</v>
+      </c>
+      <c r="G6" s="66">
+        <v>80281137.797900006</v>
+      </c>
+      <c r="H6" s="66">
+        <v>24600659012.200001</v>
+      </c>
+      <c r="I6" s="66">
+        <v>43789347.406800002</v>
+      </c>
+      <c r="J6" s="66">
+        <f t="shared" ref="J6:J12" si="0">D6/B6</f>
+        <v>0.99744486663627541</v>
+      </c>
+      <c r="K6" s="66">
+        <f t="shared" ref="K6:K12" si="1">F6/B6</f>
+        <v>1.0007555529735006</v>
+      </c>
+      <c r="L6" s="66">
+        <f t="shared" ref="L6:L12" si="2">H6/B6</f>
+        <v>0.9991040453641018</v>
+      </c>
+      <c r="M6" s="66">
+        <f t="shared" ref="M6:M12" si="3">C6/B6</f>
+        <v>3.9757055335401317E-3</v>
+      </c>
+      <c r="N6" s="66">
+        <f t="shared" ref="N6:N12" si="4">E6/B6</f>
+        <v>8.2374152084127988E-3</v>
+      </c>
+      <c r="O6" s="66">
+        <f t="shared" ref="O6:O12" si="5">G6/B6</f>
+        <v>3.2604496286273189E-3</v>
+      </c>
+      <c r="P6" s="66">
+        <f t="shared" ref="P6:P12" si="6">I6/B6</f>
+        <v>1.7784122822194028E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A7" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="66">
+        <v>1449897.6</v>
+      </c>
+      <c r="C7" s="66">
+        <v>79647.966072199997</v>
+      </c>
+      <c r="D7" s="66">
+        <v>1376036.6</v>
+      </c>
+      <c r="E7" s="66">
+        <v>129459.784594</v>
+      </c>
+      <c r="F7" s="66">
+        <v>1731427</v>
+      </c>
+      <c r="G7" s="66">
+        <v>258471.21077800001</v>
+      </c>
+      <c r="H7" s="66">
+        <v>1690296.6</v>
+      </c>
+      <c r="I7" s="66">
+        <v>78944.221616499999</v>
+      </c>
+      <c r="J7" s="66">
+        <f t="shared" si="0"/>
+        <v>0.9490577817357585</v>
+      </c>
+      <c r="K7" s="66">
+        <f t="shared" si="1"/>
+        <v>1.1941719194514149</v>
+      </c>
+      <c r="L7" s="66">
+        <f t="shared" si="2"/>
+        <v>1.165804122994617</v>
+      </c>
+      <c r="M7" s="66">
+        <f t="shared" si="3"/>
+        <v>5.4933511216378308E-2</v>
+      </c>
+      <c r="N7" s="66">
+        <f t="shared" si="4"/>
+        <v>8.9288915709633557E-2</v>
+      </c>
+      <c r="O7" s="66">
+        <f t="shared" si="5"/>
+        <v>0.17826859688435928</v>
+      </c>
+      <c r="P7" s="66">
+        <f t="shared" si="6"/>
+        <v>5.4448135934910158E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A8" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="66">
+        <v>885541.6</v>
+      </c>
+      <c r="C8" s="66">
+        <v>79049.450307000006</v>
+      </c>
+      <c r="D8" s="66">
+        <v>857580.2</v>
+      </c>
+      <c r="E8" s="66">
+        <v>58765.317007199999</v>
+      </c>
+      <c r="F8" s="66">
+        <v>1004167.8</v>
+      </c>
+      <c r="G8" s="66">
+        <v>31039.264414000001</v>
+      </c>
+      <c r="H8" s="66">
+        <v>963836.8</v>
+      </c>
+      <c r="I8" s="66">
+        <v>22430.258789399999</v>
+      </c>
+      <c r="J8" s="66">
+        <f t="shared" si="0"/>
+        <v>0.96842452121955647</v>
+      </c>
+      <c r="K8" s="66">
+        <f t="shared" si="1"/>
+        <v>1.133958924120561</v>
+      </c>
+      <c r="L8" s="66">
+        <f t="shared" si="2"/>
+        <v>1.0884150445331988</v>
+      </c>
+      <c r="M8" s="66">
+        <f t="shared" si="3"/>
+        <v>8.9266783522084128E-2</v>
+      </c>
+      <c r="N8" s="66">
+        <f t="shared" si="4"/>
+        <v>6.6360876786816111E-2</v>
+      </c>
+      <c r="O8" s="66">
+        <f t="shared" si="5"/>
+        <v>3.5051164636421377E-2</v>
+      </c>
+      <c r="P8" s="66">
+        <f t="shared" si="6"/>
+        <v>2.5329424150598912E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A9" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="66">
+        <v>24183423890.599998</v>
+      </c>
+      <c r="C9" s="66">
+        <v>49716861.902999997</v>
+      </c>
+      <c r="D9" s="66">
+        <v>24266124866</v>
+      </c>
+      <c r="E9" s="66">
+        <v>65766798.660899997</v>
+      </c>
+      <c r="F9" s="66">
+        <v>24232753812</v>
+      </c>
+      <c r="G9" s="66">
+        <v>190061596.18099999</v>
+      </c>
+      <c r="H9" s="66">
+        <v>24276819744.400002</v>
+      </c>
+      <c r="I9" s="66">
+        <v>45453154.373000003</v>
+      </c>
+      <c r="J9" s="66">
+        <f t="shared" si="0"/>
+        <v>1.0034197380724137</v>
+      </c>
+      <c r="K9" s="66">
+        <f t="shared" si="1"/>
+        <v>1.0020398237083037</v>
+      </c>
+      <c r="L9" s="66">
+        <f t="shared" si="2"/>
+        <v>1.0038619781145344</v>
+      </c>
+      <c r="M9" s="66">
+        <f t="shared" si="3"/>
+        <v>2.0558239448602127E-3</v>
+      </c>
+      <c r="N9" s="66">
+        <f t="shared" si="4"/>
+        <v>2.7194990650791714E-3</v>
+      </c>
+      <c r="O9" s="66">
+        <f t="shared" si="5"/>
+        <v>7.8591682071485411E-3</v>
+      </c>
+      <c r="P9" s="66">
+        <f t="shared" si="6"/>
+        <v>1.8795169194659597E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A10" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="66">
+        <v>79511482.400000006</v>
+      </c>
+      <c r="C10" s="66">
+        <v>17135944.8248</v>
+      </c>
+      <c r="D10" s="66">
+        <v>70853788.799999997</v>
+      </c>
+      <c r="E10" s="66">
+        <v>8957880.0904300008</v>
+      </c>
+      <c r="F10" s="66">
+        <v>94122488.400000006</v>
+      </c>
+      <c r="G10" s="66">
+        <v>6327578.3154999996</v>
+      </c>
+      <c r="H10" s="66">
+        <v>80706299.200000003</v>
+      </c>
+      <c r="I10" s="66">
+        <v>4358625.7019400001</v>
+      </c>
+      <c r="J10" s="66">
+        <f t="shared" si="0"/>
+        <v>0.89111392042163706</v>
+      </c>
+      <c r="K10" s="66">
+        <f t="shared" si="1"/>
+        <v>1.1837596980835563</v>
+      </c>
+      <c r="L10" s="66">
+        <f t="shared" si="2"/>
+        <v>1.0150269717521956</v>
+      </c>
+      <c r="M10" s="66">
+        <f t="shared" si="3"/>
+        <v>0.21551534831904981</v>
+      </c>
+      <c r="N10" s="66">
+        <f t="shared" si="4"/>
+        <v>0.11266146498647094</v>
+      </c>
+      <c r="O10" s="66">
+        <f t="shared" si="5"/>
+        <v>7.958068601548296E-2</v>
+      </c>
+      <c r="P10" s="66">
+        <f t="shared" si="6"/>
+        <v>5.4817563078662958E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A11" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="66">
+        <v>88046397.599999994</v>
+      </c>
+      <c r="C11" s="66">
+        <v>1569267.7557900001</v>
+      </c>
+      <c r="D11" s="66">
+        <v>85976030.200000003</v>
+      </c>
+      <c r="E11" s="66">
+        <v>2969156.0773499999</v>
+      </c>
+      <c r="F11" s="66">
+        <v>91692176</v>
+      </c>
+      <c r="G11" s="66">
+        <v>5772566.8047599997</v>
+      </c>
+      <c r="H11" s="66">
+        <v>92064046.799999997</v>
+      </c>
+      <c r="I11" s="66">
+        <v>2940424.5985699999</v>
+      </c>
+      <c r="J11" s="66">
+        <f t="shared" si="0"/>
+        <v>0.97648549564281106</v>
+      </c>
+      <c r="K11" s="66">
+        <f t="shared" si="1"/>
+        <v>1.0414074681006598</v>
+      </c>
+      <c r="L11" s="66">
+        <f t="shared" si="2"/>
+        <v>1.0456310457839788</v>
+      </c>
+      <c r="M11" s="66">
+        <f t="shared" si="3"/>
+        <v>1.7823190937569944E-2</v>
+      </c>
+      <c r="N11" s="66">
+        <f t="shared" si="4"/>
+        <v>3.3722629866573893E-2</v>
+      </c>
+      <c r="O11" s="66">
+        <f t="shared" si="5"/>
+        <v>6.5562782375096287E-2</v>
+      </c>
+      <c r="P11" s="66">
+        <f t="shared" si="6"/>
+        <v>3.3396307841332969E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A12" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="66">
+        <v>869046155.60000002</v>
+      </c>
+      <c r="C12" s="66">
+        <v>7034018.4514300004</v>
+      </c>
+      <c r="D12" s="66">
+        <v>869905585.20000005</v>
+      </c>
+      <c r="E12" s="66">
+        <v>18679104.192200001</v>
+      </c>
+      <c r="F12" s="66">
+        <v>881615632</v>
+      </c>
+      <c r="G12" s="66">
+        <v>11453885.719799999</v>
+      </c>
+      <c r="H12" s="66">
+        <v>910305330.39999998</v>
+      </c>
+      <c r="I12" s="66">
+        <v>8583505.2219900005</v>
+      </c>
+      <c r="J12" s="66">
+        <f t="shared" si="0"/>
+        <v>1.0009889343557439</v>
+      </c>
+      <c r="K12" s="66">
+        <f t="shared" si="1"/>
+        <v>1.0144635314465225</v>
+      </c>
+      <c r="L12" s="66">
+        <f t="shared" si="2"/>
+        <v>1.047476390677448</v>
+      </c>
+      <c r="M12" s="66">
+        <f t="shared" si="3"/>
+        <v>8.0939526699518385E-3</v>
+      </c>
+      <c r="N12" s="66">
+        <f t="shared" si="4"/>
+        <v>2.1493799922863384E-2</v>
+      </c>
+      <c r="O12" s="66">
+        <f t="shared" si="5"/>
+        <v>1.3179835899385687E-2</v>
+      </c>
+      <c r="P12" s="66">
+        <f t="shared" si="6"/>
+        <v>9.8769267508741748E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M3:O3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F72758A-17BC-4C1E-98B0-DDD6331D597C}">
+  <dimension ref="A1:P12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="35.33203125" style="65" customWidth="1"/>
+    <col min="2" max="2" width="21.86328125" style="65" customWidth="1"/>
+    <col min="3" max="3" width="16.796875" style="65" customWidth="1"/>
+    <col min="4" max="4" width="22" style="65" customWidth="1"/>
+    <col min="5" max="5" width="17" style="65" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.3984375" style="65" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.9296875" style="65" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.3984375" style="65" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" style="65" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="65"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A1" s="65" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A3" s="73"/>
+      <c r="B3" s="86" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="86"/>
+      <c r="H3" s="87" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="87"/>
+      <c r="J3" s="75" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="76" t="s">
+        <v>115</v>
+      </c>
+      <c r="M3" s="86" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="73"/>
+    </row>
+    <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A4" s="75" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="75" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="75" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4" s="77" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A5" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="66">
+        <v>16119623394.200001</v>
+      </c>
+      <c r="C5" s="66">
+        <v>31331424.663899999</v>
+      </c>
+      <c r="D5" s="66">
+        <v>16114043027.200001</v>
+      </c>
+      <c r="E5" s="66">
+        <v>37414693.188600004</v>
+      </c>
+      <c r="F5" s="66">
+        <v>16187258378.799999</v>
+      </c>
+      <c r="G5" s="66">
+        <v>39222287.738499999</v>
+      </c>
+      <c r="H5" s="66">
+        <v>16196183193.200001</v>
+      </c>
+      <c r="I5" s="66">
+        <v>39658787.826200001</v>
+      </c>
+      <c r="J5" s="66">
+        <f>D5/B5</f>
+        <v>0.9996538152993073</v>
+      </c>
+      <c r="K5" s="66">
+        <f>F5/B5</f>
+        <v>1.0041958166730083</v>
+      </c>
+      <c r="L5" s="66">
+        <f>H5/B5</f>
+        <v>1.0047494781439836</v>
+      </c>
+      <c r="M5" s="66">
+        <f>C5/B5</f>
+        <v>1.9436821753027651E-3</v>
+      </c>
+      <c r="N5" s="66">
+        <f>E5/B5</f>
+        <v>2.3210649699212066E-3</v>
+      </c>
+      <c r="O5" s="66">
+        <f>G5/B5</f>
+        <v>2.4332012466626585E-3</v>
+      </c>
+      <c r="P5" s="66">
+        <f>I5/B5</f>
+        <v>2.4602800485071892E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A6" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="66">
+        <v>1025374354960</v>
+      </c>
+      <c r="C6" s="66">
+        <v>80567813.380700007</v>
+      </c>
+      <c r="D6" s="66">
+        <v>1025349157960</v>
+      </c>
+      <c r="E6" s="66">
+        <v>144376745.414</v>
+      </c>
+      <c r="F6" s="66">
+        <v>1025289730700</v>
+      </c>
+      <c r="G6" s="66">
+        <v>218362695.77599999</v>
+      </c>
+      <c r="H6" s="66">
+        <v>1025317318150</v>
+      </c>
+      <c r="I6" s="66">
+        <v>197127058.868</v>
+      </c>
+      <c r="J6" s="66">
+        <f t="shared" ref="J6:J12" si="0">D6/B6</f>
+        <v>0.99997542653580318</v>
+      </c>
+      <c r="K6" s="66">
+        <f t="shared" ref="K6:K12" si="1">F6/B6</f>
+        <v>0.99991746988834795</v>
+      </c>
+      <c r="L6" s="66">
+        <f t="shared" ref="L6:L12" si="2">H6/B6</f>
+        <v>0.99994437464744057</v>
+      </c>
+      <c r="M6" s="66">
+        <f t="shared" ref="M6:M12" si="3">C6/B6</f>
+        <v>7.857404760609891E-5</v>
+      </c>
+      <c r="N6" s="66">
+        <f t="shared" ref="N6:N12" si="4">E6/B6</f>
+        <v>1.4080393635320846E-4</v>
+      </c>
+      <c r="O6" s="66">
+        <f t="shared" ref="O6:O12" si="5">G6/B6</f>
+        <v>2.1295899855474574E-4</v>
+      </c>
+      <c r="P6" s="66">
+        <f t="shared" ref="P6:P12" si="6">I6/B6</f>
+        <v>1.9224886785440421E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A7" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="66">
+        <v>381885772.19999999</v>
+      </c>
+      <c r="C7" s="66">
+        <v>42179327.449699998</v>
+      </c>
+      <c r="D7" s="66">
+        <v>400683133</v>
+      </c>
+      <c r="E7" s="66">
+        <v>53422893.307599999</v>
+      </c>
+      <c r="F7" s="66">
+        <v>338308890</v>
+      </c>
+      <c r="G7" s="66">
+        <v>64878043.399300002</v>
+      </c>
+      <c r="H7" s="66">
+        <v>336441413.39999998</v>
+      </c>
+      <c r="I7" s="66">
+        <v>47321905.6809</v>
+      </c>
+      <c r="J7" s="66">
+        <f t="shared" si="0"/>
+        <v>1.0492224695665162</v>
+      </c>
+      <c r="K7" s="66">
+        <f t="shared" si="1"/>
+        <v>0.8858902704100271</v>
+      </c>
+      <c r="L7" s="66">
+        <f t="shared" si="2"/>
+        <v>0.88100012593242139</v>
+      </c>
+      <c r="M7" s="66">
+        <f t="shared" si="3"/>
+        <v>0.11045011498257645</v>
+      </c>
+      <c r="N7" s="66">
+        <f t="shared" si="4"/>
+        <v>0.13989233743859286</v>
+      </c>
+      <c r="O7" s="66">
+        <f t="shared" si="5"/>
+        <v>0.16988861099889913</v>
+      </c>
+      <c r="P7" s="66">
+        <f t="shared" si="6"/>
+        <v>0.12391638842233882</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A8" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="66">
+        <v>79424898.799999997</v>
+      </c>
+      <c r="C8" s="66">
+        <v>847877.90061799996</v>
+      </c>
+      <c r="D8" s="66">
+        <v>79072544</v>
+      </c>
+      <c r="E8" s="66">
+        <v>996438.38698700001</v>
+      </c>
+      <c r="F8" s="66">
+        <v>70296559.200000003</v>
+      </c>
+      <c r="G8" s="66">
+        <v>719304.71276999998</v>
+      </c>
+      <c r="H8" s="66">
+        <v>69900522.400000006</v>
+      </c>
+      <c r="I8" s="66">
+        <v>877772.14083000005</v>
+      </c>
+      <c r="J8" s="66">
+        <f t="shared" si="0"/>
+        <v>0.99556367328981732</v>
+      </c>
+      <c r="K8" s="66">
+        <f t="shared" si="1"/>
+        <v>0.88506954698190943</v>
+      </c>
+      <c r="L8" s="66">
+        <f t="shared" si="2"/>
+        <v>0.88008324160433182</v>
+      </c>
+      <c r="M8" s="66">
+        <f t="shared" si="3"/>
+        <v>1.0675215372361293E-2</v>
+      </c>
+      <c r="N8" s="66">
+        <f t="shared" si="4"/>
+        <v>1.25456676941589E-2</v>
+      </c>
+      <c r="O8" s="66">
+        <f t="shared" si="5"/>
+        <v>9.0564133368464545E-3</v>
+      </c>
+      <c r="P8" s="66">
+        <f t="shared" si="6"/>
+        <v>1.1051599109245577E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A9" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="66">
+        <v>1515158391250</v>
+      </c>
+      <c r="C9" s="66">
+        <v>2662809211.0799999</v>
+      </c>
+      <c r="D9" s="66">
+        <v>1516417403530</v>
+      </c>
+      <c r="E9" s="66">
+        <v>1556357367.26</v>
+      </c>
+      <c r="F9" s="66">
+        <v>1521760798470</v>
+      </c>
+      <c r="G9" s="66">
+        <v>1909699016.1800001</v>
+      </c>
+      <c r="H9" s="66">
+        <v>1521682820950</v>
+      </c>
+      <c r="I9" s="66">
+        <v>3756314077.2399998</v>
+      </c>
+      <c r="J9" s="66">
+        <f t="shared" si="0"/>
+        <v>1.0008309443337877</v>
+      </c>
+      <c r="K9" s="66">
+        <f t="shared" si="1"/>
+        <v>1.0043575689895714</v>
+      </c>
+      <c r="L9" s="66">
+        <f t="shared" si="2"/>
+        <v>1.0043061040599308</v>
+      </c>
+      <c r="M9" s="66">
+        <f t="shared" si="3"/>
+        <v>1.7574461036269564E-3</v>
+      </c>
+      <c r="N9" s="66">
+        <f t="shared" si="4"/>
+        <v>1.0271912007668129E-3</v>
+      </c>
+      <c r="O9" s="66">
+        <f t="shared" si="5"/>
+        <v>1.2603956307198389E-3</v>
+      </c>
+      <c r="P9" s="66">
+        <f t="shared" si="6"/>
+        <v>2.4791560400104803E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A10" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="66">
+        <v>9274971445</v>
+      </c>
+      <c r="C10" s="66">
+        <v>852369149.06700003</v>
+      </c>
+      <c r="D10" s="66">
+        <v>9447663570.2000008</v>
+      </c>
+      <c r="E10" s="66">
+        <v>896254793.89400005</v>
+      </c>
+      <c r="F10" s="66">
+        <v>7547441364.8000002</v>
+      </c>
+      <c r="G10" s="66">
+        <v>769315223.47399998</v>
+      </c>
+      <c r="H10" s="66">
+        <v>7040602809.3999996</v>
+      </c>
+      <c r="I10" s="66">
+        <v>1215518551.96</v>
+      </c>
+      <c r="J10" s="66">
+        <f t="shared" si="0"/>
+        <v>1.0186191543795098</v>
+      </c>
+      <c r="K10" s="66">
+        <f t="shared" si="1"/>
+        <v>0.81374281414836203</v>
+      </c>
+      <c r="L10" s="66">
+        <f t="shared" si="2"/>
+        <v>0.75909697955948796</v>
+      </c>
+      <c r="M10" s="66">
+        <f t="shared" si="3"/>
+        <v>9.189992164628169E-2</v>
+      </c>
+      <c r="N10" s="66">
+        <f t="shared" si="4"/>
+        <v>9.6631542124817837E-2</v>
+      </c>
+      <c r="O10" s="66">
+        <f t="shared" si="5"/>
+        <v>8.2945292935508327E-2</v>
+      </c>
+      <c r="P10" s="66">
+        <f t="shared" si="6"/>
+        <v>0.13105361662490811</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A11" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="66">
+        <v>8978732644.2000008</v>
+      </c>
+      <c r="C11" s="66">
+        <v>75653514.757100001</v>
+      </c>
+      <c r="D11" s="66">
+        <v>8905455713.7999992</v>
+      </c>
+      <c r="E11" s="66">
+        <v>57198923.647100002</v>
+      </c>
+      <c r="F11" s="66">
+        <v>8233739451.8000002</v>
+      </c>
+      <c r="G11" s="66">
+        <v>99356758.617699996</v>
+      </c>
+      <c r="H11" s="66">
+        <v>8250560983.1999998</v>
+      </c>
+      <c r="I11" s="66">
+        <v>60099701.520099998</v>
+      </c>
+      <c r="J11" s="66">
+        <f t="shared" si="0"/>
+        <v>0.99183883368580572</v>
+      </c>
+      <c r="K11" s="66">
+        <f t="shared" si="1"/>
+        <v>0.91702690993018432</v>
+      </c>
+      <c r="L11" s="66">
+        <f t="shared" si="2"/>
+        <v>0.91890039609650498</v>
+      </c>
+      <c r="M11" s="66">
+        <f t="shared" si="3"/>
+        <v>8.4258567166458579E-3</v>
+      </c>
+      <c r="N11" s="66">
+        <f t="shared" si="4"/>
+        <v>6.3704896797488267E-3</v>
+      </c>
+      <c r="O11" s="66">
+        <f t="shared" si="5"/>
+        <v>1.1065788742677572E-2</v>
+      </c>
+      <c r="P11" s="66">
+        <f t="shared" si="6"/>
+        <v>6.6935617644125591E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A12" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="66">
+        <v>73953462243</v>
+      </c>
+      <c r="C12" s="66">
+        <v>461090849.08200002</v>
+      </c>
+      <c r="D12" s="66">
+        <v>72543114524.399994</v>
+      </c>
+      <c r="E12" s="66">
+        <v>639469996.86099994</v>
+      </c>
+      <c r="F12" s="66">
+        <v>73527920768.199997</v>
+      </c>
+      <c r="G12" s="66">
+        <v>258636195.30199999</v>
+      </c>
+      <c r="H12" s="66">
+        <v>74975542371.399994</v>
+      </c>
+      <c r="I12" s="66">
+        <v>618106921.52199996</v>
+      </c>
+      <c r="J12" s="66">
+        <f t="shared" si="0"/>
+        <v>0.98092925367083128</v>
+      </c>
+      <c r="K12" s="66">
+        <f t="shared" si="1"/>
+        <v>0.99424582079197676</v>
+      </c>
+      <c r="L12" s="66">
+        <f t="shared" si="2"/>
+        <v>1.013820585235639</v>
+      </c>
+      <c r="M12" s="66">
+        <f t="shared" si="3"/>
+        <v>6.2348784640660166E-3</v>
+      </c>
+      <c r="N12" s="66">
+        <f t="shared" si="4"/>
+        <v>8.6469243963155813E-3</v>
+      </c>
+      <c r="O12" s="66">
+        <f t="shared" si="5"/>
+        <v>3.4972831218119333E-3</v>
+      </c>
+      <c r="P12" s="66">
+        <f t="shared" si="6"/>
+        <v>8.3580525208000831E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M3:O3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5A357B-AD95-4B57-AFAC-6E90E36724A8}">
   <dimension ref="A1:H59"/>
   <sheetViews>
@@ -6014,22 +7164,22 @@
     </row>
     <row r="3" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75" t="s">
+      <c r="C3" s="82"/>
+      <c r="D3" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="75"/>
-      <c r="F3" s="76" t="s">
+      <c r="E3" s="82"/>
+      <c r="F3" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="75"/>
-      <c r="H3" s="73" t="s">
+      <c r="G3" s="82"/>
+      <c r="H3" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="74"/>
+      <c r="I3" s="81"/>
       <c r="J3" s="48" t="s">
         <v>45</v>
       </c>
@@ -6039,11 +7189,11 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="76" t="s">
+      <c r="M3" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
     </row>
     <row r="4" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -7875,29 +9025,29 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75" t="s">
+      <c r="C3" s="82"/>
+      <c r="D3" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="75"/>
-      <c r="F3" s="76" t="s">
+      <c r="E3" s="82"/>
+      <c r="F3" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="75"/>
+      <c r="G3" s="82"/>
       <c r="H3" s="7" t="s">
         <v>45</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="76" t="s">
+      <c r="J3" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -9389,22 +10539,22 @@
     </row>
     <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="52"/>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77" t="s">
+      <c r="C2" s="84"/>
+      <c r="D2" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77" t="s">
+      <c r="E2" s="84"/>
+      <c r="F2" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="77"/>
-      <c r="H2" s="78" t="s">
+      <c r="G2" s="84"/>
+      <c r="H2" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="78"/>
+      <c r="I2" s="85"/>
       <c r="J2" s="54" t="s">
         <v>45</v>
       </c>
@@ -9414,11 +10564,11 @@
       <c r="L2" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="77" t="s">
+      <c r="M2" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
     </row>
     <row r="3" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="52"/>
@@ -9960,22 +11110,22 @@
     </row>
     <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="26"/>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="75"/>
-      <c r="F2" s="76" t="s">
+      <c r="E2" s="82"/>
+      <c r="F2" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="75"/>
-      <c r="H2" s="73" t="s">
+      <c r="G2" s="82"/>
+      <c r="H2" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="74"/>
+      <c r="I2" s="81"/>
       <c r="J2" s="48" t="s">
         <v>45</v>
       </c>
@@ -9985,11 +11135,11 @@
       <c r="L2" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="76" t="s">
+      <c r="M2" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
     </row>
     <row r="3" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26"/>
@@ -10529,22 +11679,22 @@
     </row>
     <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26"/>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75" t="s">
+      <c r="C3" s="82"/>
+      <c r="D3" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="75"/>
-      <c r="F3" s="76" t="s">
+      <c r="E3" s="82"/>
+      <c r="F3" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="75"/>
-      <c r="H3" s="73" t="s">
+      <c r="G3" s="82"/>
+      <c r="H3" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="74"/>
+      <c r="I3" s="81"/>
       <c r="J3" s="48" t="s">
         <v>45</v>
       </c>
@@ -10554,11 +11704,11 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="76" t="s">
+      <c r="M3" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
     </row>
     <row r="4" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="26"/>
@@ -11098,22 +12248,22 @@
     </row>
     <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26"/>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75" t="s">
+      <c r="C3" s="82"/>
+      <c r="D3" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="75"/>
-      <c r="F3" s="76" t="s">
+      <c r="E3" s="82"/>
+      <c r="F3" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="75"/>
-      <c r="H3" s="73" t="s">
+      <c r="G3" s="82"/>
+      <c r="H3" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="74"/>
+      <c r="I3" s="81"/>
       <c r="J3" s="48" t="s">
         <v>45</v>
       </c>
@@ -11123,11 +12273,11 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="76" t="s">
+      <c r="M3" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
     </row>
     <row r="4" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="26"/>
@@ -11900,22 +13050,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75" t="s">
+      <c r="C6" s="82"/>
+      <c r="D6" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="75"/>
-      <c r="F6" s="76" t="s">
+      <c r="E6" s="82"/>
+      <c r="F6" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="75"/>
-      <c r="H6" s="73" t="s">
+      <c r="G6" s="82"/>
+      <c r="H6" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="74"/>
+      <c r="I6" s="81"/>
       <c r="J6" s="7" t="s">
         <v>45</v>
       </c>
@@ -11925,11 +13075,11 @@
       <c r="L6" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="76" t="s">
+      <c r="M6" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="75"/>
-      <c r="O6" s="75"/>
+      <c r="N6" s="82"/>
+      <c r="O6" s="82"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
@@ -12229,22 +13379,22 @@
     </row>
     <row r="19" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A19" s="2"/>
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75" t="s">
+      <c r="C19" s="82"/>
+      <c r="D19" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="75"/>
-      <c r="F19" s="76" t="s">
+      <c r="E19" s="82"/>
+      <c r="F19" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="75"/>
-      <c r="H19" s="73" t="s">
+      <c r="G19" s="82"/>
+      <c r="H19" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="I19" s="74"/>
+      <c r="I19" s="81"/>
       <c r="J19" s="67" t="s">
         <v>45</v>
       </c>
@@ -12254,11 +13404,11 @@
       <c r="L19" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="M19" s="76" t="s">
+      <c r="M19" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="N19" s="75"/>
-      <c r="O19" s="75"/>
+      <c r="N19" s="82"/>
+      <c r="O19" s="82"/>
     </row>
     <row r="20" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">

</xml_diff>

<commit_message>
added procstat -v results for octane
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="999" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{B02C1C1D-519F-40D7-A33A-E3CCCDF66C15}"/>
+  <xr:revisionPtr revIDLastSave="1018" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{8AD85566-7D3D-4018-8561-5C401B6B2183}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -22,7 +22,8 @@
     <sheet name="postgres-1GB-usr" sheetId="19" r:id="rId12"/>
     <sheet name="octane-os" sheetId="20" r:id="rId13"/>
     <sheet name="octane-usr" sheetId="21" r:id="rId14"/>
-    <sheet name="postgres_stats" sheetId="9" r:id="rId15"/>
+    <sheet name="octane-stats" sheetId="22" r:id="rId15"/>
+    <sheet name="postgres_stats" sheetId="9" r:id="rId16"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="180">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -524,6 +525,81 @@
   </si>
   <si>
     <t>node run.js for 4 iterations</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.promotions: 130</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.mappings: 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 159280K,     86</t>
+  </si>
+  <si>
+    <t>vm.reserv.fullpop: 70</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 2562</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.promotions: 156</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.p_failures: 11</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.mappings: 10</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.demotions: 54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 171248K,     98</t>
+  </si>
+  <si>
+    <t>vm.reserv.fullpop: 71</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 3337</t>
+  </si>
+  <si>
+    <t>after running one round of "node run.js" (octane)</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.promotions: 179</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.p_failures: 21</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.mappings: 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 173284K,     99</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 4084</t>
+  </si>
+  <si>
+    <t>after running second round of "node run.js" (octane)</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.promotions: 204</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.p_failures: 32</t>
+  </si>
+  <si>
+    <t>vm.pmap.pde.mappings: 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -1: 173280K,     99</t>
+  </si>
+  <si>
+    <t>vm.reserv.freed: 4929</t>
+  </si>
+  <si>
+    <t>after running third round of "node run.js" (octane)</t>
   </si>
 </sst>
 </file>
@@ -5884,7 +5960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F72758A-17BC-4C1E-98B0-DDD6331D597C}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -6454,11 +6530,201 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C510FE-BA24-4F4C-B882-A73942D255FE}">
+  <dimension ref="A2:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="27.3984375" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.19921875" customWidth="1"/>
+    <col min="4" max="4" width="27.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="69" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="69" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" t="s">
+        <v>172</v>
+      </c>
+      <c r="D14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5A357B-AD95-4B57-AFAC-6E90E36724A8}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39:D51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
added results for postgresql 8GB database
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1018" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{8AD85566-7D3D-4018-8561-5C401B6B2183}"/>
+  <xr:revisionPtr revIDLastSave="1044" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{97162284-6534-4B07-815A-C8E559C0961A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -16,14 +16,16 @@
     <sheet name="clang-2core-os" sheetId="15" r:id="rId6"/>
     <sheet name="clang-2core-usr" sheetId="16" r:id="rId7"/>
     <sheet name="clang-stats" sheetId="17" r:id="rId8"/>
-    <sheet name="postgres-4GB-os" sheetId="11" r:id="rId9"/>
-    <sheet name="postgres-4GB-usr" sheetId="8" r:id="rId10"/>
-    <sheet name="postgres-1GB-os" sheetId="18" r:id="rId11"/>
-    <sheet name="postgres-1GB-usr" sheetId="19" r:id="rId12"/>
-    <sheet name="octane-os" sheetId="20" r:id="rId13"/>
-    <sheet name="octane-usr" sheetId="21" r:id="rId14"/>
-    <sheet name="octane-stats" sheetId="22" r:id="rId15"/>
-    <sheet name="postgres_stats" sheetId="9" r:id="rId16"/>
+    <sheet name="postgres-8GB-os" sheetId="23" r:id="rId9"/>
+    <sheet name="postgres-8GB-usr" sheetId="24" r:id="rId10"/>
+    <sheet name="postgres-4GB-os" sheetId="11" r:id="rId11"/>
+    <sheet name="postgres-4GB-usr" sheetId="8" r:id="rId12"/>
+    <sheet name="postgres-1GB-os" sheetId="18" r:id="rId13"/>
+    <sheet name="postgres-1GB-usr" sheetId="19" r:id="rId14"/>
+    <sheet name="octane-os" sheetId="20" r:id="rId15"/>
+    <sheet name="octane-usr" sheetId="21" r:id="rId16"/>
+    <sheet name="octane-stats" sheetId="22" r:id="rId17"/>
+    <sheet name="postgres_stats" sheetId="9" r:id="rId18"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="182">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -600,6 +602,12 @@
   </si>
   <si>
     <t>after running third round of "node run.js" (octane)</t>
+  </si>
+  <si>
+    <t>database size = 8GB</t>
+  </si>
+  <si>
+    <t>8GB/2MB * 2 # of super pages for each iteration</t>
   </si>
 </sst>
 </file>
@@ -3269,10 +3277,1653 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEB844F-EF6D-4427-9E28-001A58A9FD5B}">
+  <dimension ref="A1:P15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="34.86328125" customWidth="1"/>
+    <col min="2" max="2" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A1" s="72" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A2" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A3" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A4" s="65"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
+      <c r="N4" s="65"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A5" s="65"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
+    </row>
+    <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="73"/>
+      <c r="B6" s="86" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="86"/>
+      <c r="H6" s="87" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" s="87"/>
+      <c r="J6" s="75" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="76" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6" s="86" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="86"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="73"/>
+    </row>
+    <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="75" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="75" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="75" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="75" t="s">
+        <v>43</v>
+      </c>
+      <c r="P7" s="77" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A8" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="66">
+        <v>51788007274.599998</v>
+      </c>
+      <c r="C8" s="66">
+        <v>428699322.86000001</v>
+      </c>
+      <c r="D8" s="66">
+        <v>49945315764.599998</v>
+      </c>
+      <c r="E8" s="66">
+        <v>744176256.85500002</v>
+      </c>
+      <c r="F8" s="66">
+        <v>51154787569</v>
+      </c>
+      <c r="G8" s="66">
+        <v>225767672.954</v>
+      </c>
+      <c r="H8" s="66">
+        <v>49897799664.599998</v>
+      </c>
+      <c r="I8" s="66">
+        <v>796827727.65799999</v>
+      </c>
+      <c r="J8" s="66">
+        <f>D8/B8</f>
+        <v>0.96441856702017248</v>
+      </c>
+      <c r="K8" s="66">
+        <f>F8/B8</f>
+        <v>0.98777285053193065</v>
+      </c>
+      <c r="L8" s="66">
+        <f>H8/B8</f>
+        <v>0.96350105537026387</v>
+      </c>
+      <c r="M8" s="66">
+        <f>C8/B8</f>
+        <v>8.2779652166740225E-3</v>
+      </c>
+      <c r="N8" s="66">
+        <f>E8/B8</f>
+        <v>1.4369663866560656E-2</v>
+      </c>
+      <c r="O8" s="66">
+        <f>G8/B8</f>
+        <v>4.3594585857859459E-3</v>
+      </c>
+      <c r="P8" s="66">
+        <f>I8/B8</f>
+        <v>1.5386336906784459E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A9" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="66">
+        <v>1193613749360</v>
+      </c>
+      <c r="C9" s="66">
+        <v>4888467322.5299997</v>
+      </c>
+      <c r="D9" s="66">
+        <v>1198964106530</v>
+      </c>
+      <c r="E9" s="66">
+        <v>9694727370.6200008</v>
+      </c>
+      <c r="F9" s="66">
+        <v>1143131210900</v>
+      </c>
+      <c r="G9" s="66">
+        <v>10465606984.5</v>
+      </c>
+      <c r="H9" s="66">
+        <v>1156708988360</v>
+      </c>
+      <c r="I9" s="66">
+        <v>1469223720.0999999</v>
+      </c>
+      <c r="J9" s="66">
+        <f t="shared" ref="J9:J15" si="0">D9/B9</f>
+        <v>1.0044824862086825</v>
+      </c>
+      <c r="K9" s="66">
+        <f t="shared" ref="K9:K15" si="1">F9/B9</f>
+        <v>0.9577061352660623</v>
+      </c>
+      <c r="L9" s="66">
+        <f t="shared" ref="L9:L15" si="2">H9/B9</f>
+        <v>0.96908148802760707</v>
+      </c>
+      <c r="M9" s="66">
+        <f t="shared" ref="M9:M15" si="3">C9/B9</f>
+        <v>4.0955186090568512E-3</v>
+      </c>
+      <c r="N9" s="66">
+        <f t="shared" ref="N9:N15" si="4">E9/B9</f>
+        <v>8.1221646247106195E-3</v>
+      </c>
+      <c r="O9" s="66">
+        <f t="shared" ref="O9:O15" si="5">G9/B9</f>
+        <v>8.7680013656943213E-3</v>
+      </c>
+      <c r="P9" s="66">
+        <f t="shared" ref="P9:P15" si="6">I9/B9</f>
+        <v>1.2309038169908636E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A10" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="66">
+        <v>390152279.19999999</v>
+      </c>
+      <c r="C10" s="66">
+        <v>3561803.4116799999</v>
+      </c>
+      <c r="D10" s="66">
+        <v>361214159</v>
+      </c>
+      <c r="E10" s="66">
+        <v>14024582.6665</v>
+      </c>
+      <c r="F10" s="66">
+        <v>86523027.200000003</v>
+      </c>
+      <c r="G10" s="66">
+        <v>4865573.5198299997</v>
+      </c>
+      <c r="H10" s="66">
+        <v>105286045.59999999</v>
+      </c>
+      <c r="I10" s="66">
+        <v>1932588.55125</v>
+      </c>
+      <c r="J10" s="66">
+        <f t="shared" si="0"/>
+        <v>0.9258286527011016</v>
+      </c>
+      <c r="K10" s="66">
+        <f t="shared" si="1"/>
+        <v>0.22176732474154418</v>
+      </c>
+      <c r="L10" s="66">
+        <f t="shared" si="2"/>
+        <v>0.26985885053878728</v>
+      </c>
+      <c r="M10" s="66">
+        <f t="shared" si="3"/>
+        <v>9.1292646527233214E-3</v>
+      </c>
+      <c r="N10" s="66">
+        <f t="shared" si="4"/>
+        <v>3.5946432749943552E-2</v>
+      </c>
+      <c r="O10" s="66">
+        <f t="shared" si="5"/>
+        <v>1.2470960133327345E-2</v>
+      </c>
+      <c r="P10" s="66">
+        <f t="shared" si="6"/>
+        <v>4.9534211493336318E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A11" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="66">
+        <v>211631907.59999999</v>
+      </c>
+      <c r="C11" s="66">
+        <v>2993638.6393900001</v>
+      </c>
+      <c r="D11" s="66">
+        <v>186811746.59999999</v>
+      </c>
+      <c r="E11" s="66">
+        <v>11166333.873400001</v>
+      </c>
+      <c r="F11" s="66">
+        <v>80349971.799999997</v>
+      </c>
+      <c r="G11" s="66">
+        <v>780433.75305399997</v>
+      </c>
+      <c r="H11" s="66">
+        <v>76407676.400000006</v>
+      </c>
+      <c r="I11" s="66">
+        <v>2191805.6304899999</v>
+      </c>
+      <c r="J11" s="66">
+        <f t="shared" si="0"/>
+        <v>0.88272013761312429</v>
+      </c>
+      <c r="K11" s="66">
+        <f t="shared" si="1"/>
+        <v>0.37966851365280613</v>
+      </c>
+      <c r="L11" s="66">
+        <f t="shared" si="2"/>
+        <v>0.36104043698559946</v>
+      </c>
+      <c r="M11" s="66">
+        <f t="shared" si="3"/>
+        <v>1.4145497592207122E-2</v>
+      </c>
+      <c r="N11" s="66">
+        <f t="shared" si="4"/>
+        <v>5.2762997791926537E-2</v>
+      </c>
+      <c r="O11" s="66">
+        <f t="shared" si="5"/>
+        <v>3.6876941757245682E-3</v>
+      </c>
+      <c r="P11" s="66">
+        <f t="shared" si="6"/>
+        <v>1.0356687965184698E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A12" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="66">
+        <v>952568389258</v>
+      </c>
+      <c r="C12" s="66">
+        <v>1426578775.8399999</v>
+      </c>
+      <c r="D12" s="66">
+        <v>944588372622</v>
+      </c>
+      <c r="E12" s="66">
+        <v>6698761902.3400002</v>
+      </c>
+      <c r="F12" s="66">
+        <v>945064389940</v>
+      </c>
+      <c r="G12" s="66">
+        <v>8654323503.8500004</v>
+      </c>
+      <c r="H12" s="66">
+        <v>942033089233</v>
+      </c>
+      <c r="I12" s="66">
+        <v>6835264884.6199999</v>
+      </c>
+      <c r="J12" s="66">
+        <f t="shared" si="0"/>
+        <v>0.99162263127142403</v>
+      </c>
+      <c r="K12" s="66">
+        <f t="shared" si="1"/>
+        <v>0.99212235110610247</v>
+      </c>
+      <c r="L12" s="66">
+        <f t="shared" si="2"/>
+        <v>0.98894011165622819</v>
+      </c>
+      <c r="M12" s="66">
+        <f t="shared" si="3"/>
+        <v>1.4976129713387075E-3</v>
+      </c>
+      <c r="N12" s="66">
+        <f t="shared" si="4"/>
+        <v>7.0323159763447315E-3</v>
+      </c>
+      <c r="O12" s="66">
+        <f t="shared" si="5"/>
+        <v>9.0852516222916617E-3</v>
+      </c>
+      <c r="P12" s="66">
+        <f t="shared" si="6"/>
+        <v>7.1756159050630547E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A13" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="66">
+        <v>21723174024.599998</v>
+      </c>
+      <c r="C13" s="66">
+        <v>293488626.32099998</v>
+      </c>
+      <c r="D13" s="66">
+        <v>18947435442.799999</v>
+      </c>
+      <c r="E13" s="66">
+        <v>202936932.23100001</v>
+      </c>
+      <c r="F13" s="66">
+        <v>6087735250.1999998</v>
+      </c>
+      <c r="G13" s="66">
+        <v>178764457.546</v>
+      </c>
+      <c r="H13" s="66">
+        <v>8038467759.1999998</v>
+      </c>
+      <c r="I13" s="66">
+        <v>170620592.71200001</v>
+      </c>
+      <c r="J13" s="66">
+        <f t="shared" si="0"/>
+        <v>0.87222223701487334</v>
+      </c>
+      <c r="K13" s="66">
+        <f t="shared" si="1"/>
+        <v>0.28024151734484376</v>
+      </c>
+      <c r="L13" s="66">
+        <f t="shared" si="2"/>
+        <v>0.37004112521020127</v>
+      </c>
+      <c r="M13" s="66">
+        <f t="shared" si="3"/>
+        <v>1.3510393370169771E-2</v>
+      </c>
+      <c r="N13" s="66">
+        <f t="shared" si="4"/>
+        <v>9.341955830266235E-3</v>
+      </c>
+      <c r="O13" s="66">
+        <f t="shared" si="5"/>
+        <v>8.2292052415342976E-3</v>
+      </c>
+      <c r="P13" s="66">
+        <f t="shared" si="6"/>
+        <v>7.8543122896674276E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A14" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="66">
+        <v>12876858062.4</v>
+      </c>
+      <c r="C14" s="66">
+        <v>228036295.20899999</v>
+      </c>
+      <c r="D14" s="66">
+        <v>11130724132.200001</v>
+      </c>
+      <c r="E14" s="66">
+        <v>140016916.71200001</v>
+      </c>
+      <c r="F14" s="66">
+        <v>5346155452</v>
+      </c>
+      <c r="G14" s="66">
+        <v>58497580.384900004</v>
+      </c>
+      <c r="H14" s="66">
+        <v>5527889551.6000004</v>
+      </c>
+      <c r="I14" s="66">
+        <v>41264571.025399998</v>
+      </c>
+      <c r="J14" s="66">
+        <f t="shared" si="0"/>
+        <v>0.86439751671266363</v>
+      </c>
+      <c r="K14" s="66">
+        <f t="shared" si="1"/>
+        <v>0.41517545864783562</v>
+      </c>
+      <c r="L14" s="66">
+        <f t="shared" si="2"/>
+        <v>0.42928869176101703</v>
+      </c>
+      <c r="M14" s="66">
+        <f t="shared" si="3"/>
+        <v>1.7709001225606303E-2</v>
+      </c>
+      <c r="N14" s="66">
+        <f t="shared" si="4"/>
+        <v>1.0873531107782013E-2</v>
+      </c>
+      <c r="O14" s="66">
+        <f t="shared" si="5"/>
+        <v>4.5428457859383424E-3</v>
+      </c>
+      <c r="P14" s="66">
+        <f t="shared" si="6"/>
+        <v>3.2045527585561561E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A15" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="66">
+        <v>70611116528.399994</v>
+      </c>
+      <c r="C15" s="66">
+        <v>124618292.34999999</v>
+      </c>
+      <c r="D15" s="66">
+        <v>70588304130.399994</v>
+      </c>
+      <c r="E15" s="66">
+        <v>556079933.59899998</v>
+      </c>
+      <c r="F15" s="66">
+        <v>70272609435.199997</v>
+      </c>
+      <c r="G15" s="66">
+        <v>663786584.04799998</v>
+      </c>
+      <c r="H15" s="66">
+        <v>70235095344</v>
+      </c>
+      <c r="I15" s="66">
+        <v>422516914.92000002</v>
+      </c>
+      <c r="J15" s="66">
+        <f t="shared" si="0"/>
+        <v>0.9996769290853682</v>
+      </c>
+      <c r="K15" s="66">
+        <f t="shared" si="1"/>
+        <v>0.99520603681342656</v>
+      </c>
+      <c r="L15" s="66">
+        <f t="shared" si="2"/>
+        <v>0.99467475940210126</v>
+      </c>
+      <c r="M15" s="66">
+        <f t="shared" si="3"/>
+        <v>1.7648537295098308E-3</v>
+      </c>
+      <c r="N15" s="66">
+        <f t="shared" si="4"/>
+        <v>7.8752462917838582E-3</v>
+      </c>
+      <c r="O15" s="66">
+        <f t="shared" si="5"/>
+        <v>9.4005960631003919E-3</v>
+      </c>
+      <c r="P15" s="66">
+        <f t="shared" si="6"/>
+        <v>5.9837166680413913E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="M6:O6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65049047-28B8-4D24-A307-ABB41DE3392E}">
+  <dimension ref="A1:P28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="32.86328125" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.06640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.06640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.73046875" customWidth="1"/>
+    <col min="9" max="9" width="17.9296875" customWidth="1"/>
+    <col min="12" max="12" width="13.86328125" customWidth="1"/>
+    <col min="16" max="16" width="16.53125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A1" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A2" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A3" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+    </row>
+    <row r="4" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+    </row>
+    <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="68" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+    </row>
+    <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="2"/>
+      <c r="B6" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="82"/>
+      <c r="F6" s="83" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="82"/>
+      <c r="H6" s="80" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" s="81"/>
+      <c r="J6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="82"/>
+      <c r="O6" s="82"/>
+    </row>
+    <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="M7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="P7" s="71" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A8" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="66">
+        <v>154918952634</v>
+      </c>
+      <c r="E8" s="66">
+        <v>280351869.92900002</v>
+      </c>
+      <c r="H8" s="66">
+        <v>155317428173</v>
+      </c>
+      <c r="I8" s="66">
+        <v>1411292601.6199999</v>
+      </c>
+      <c r="J8" s="5" t="e">
+        <f>#REF!/D8</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K8" s="5">
+        <f>H8/D8</f>
+        <v>1.0025721548734028</v>
+      </c>
+      <c r="M8" s="5">
+        <f>E8/D8</f>
+        <v>1.809667991955371E-3</v>
+      </c>
+      <c r="N8" s="5" t="e">
+        <f>#REF!/D8</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O8" s="5">
+        <f>I8/D8</f>
+        <v>9.1098769880933479E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A9" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="66">
+        <v>323888734975</v>
+      </c>
+      <c r="E9" s="66">
+        <v>1799069197.0699999</v>
+      </c>
+      <c r="H9" s="66">
+        <v>324404115108</v>
+      </c>
+      <c r="I9" s="66">
+        <v>3561778733.0300002</v>
+      </c>
+      <c r="J9" s="5" t="e">
+        <f>#REF!/D9</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K9" s="5">
+        <f>H9/D9</f>
+        <v>1.0015912258666229</v>
+      </c>
+      <c r="M9" s="5">
+        <f>E9/D9</f>
+        <v>5.5545902120024788E-3</v>
+      </c>
+      <c r="N9" s="5" t="e">
+        <f>#REF!/D9</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O9" s="5">
+        <f>I9/D9</f>
+        <v>1.0996920696562426E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A10" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="66">
+        <v>67105167.399999999</v>
+      </c>
+      <c r="E10" s="66">
+        <v>851354.688035</v>
+      </c>
+      <c r="H10" s="66">
+        <v>54168281.200000003</v>
+      </c>
+      <c r="I10" s="66">
+        <v>275826.63121700002</v>
+      </c>
+      <c r="J10" s="5" t="e">
+        <f>#REF!/D10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K10" s="5">
+        <f>H10/D10</f>
+        <v>0.80721475407570487</v>
+      </c>
+      <c r="M10" s="5">
+        <f>E10/D10</f>
+        <v>1.2686872278557195E-2</v>
+      </c>
+      <c r="N10" s="5" t="e">
+        <f>#REF!/D10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O10" s="5">
+        <f>I10/D10</f>
+        <v>4.1103635070732277E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A11" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="66">
+        <v>15824359</v>
+      </c>
+      <c r="E11" s="66">
+        <v>1011097.01176</v>
+      </c>
+      <c r="H11" s="66">
+        <v>4744871.2</v>
+      </c>
+      <c r="I11" s="66">
+        <v>436397.91209400003</v>
+      </c>
+      <c r="J11" s="5" t="e">
+        <f>#REF!/D11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K11" s="5">
+        <f>H11/D11</f>
+        <v>0.29984602851843795</v>
+      </c>
+      <c r="M11" s="5">
+        <f>E11/D11</f>
+        <v>6.3894974308911973E-2</v>
+      </c>
+      <c r="N11" s="5" t="e">
+        <f>#REF!/D11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O11" s="5">
+        <f>I11/D11</f>
+        <v>2.7577604381574004E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A12" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="66">
+        <v>13571559205.200001</v>
+      </c>
+      <c r="E12" s="66">
+        <v>124870350.419</v>
+      </c>
+      <c r="H12" s="66">
+        <v>13403081932.200001</v>
+      </c>
+      <c r="I12" s="66">
+        <v>112712714.513</v>
+      </c>
+      <c r="J12" s="5" t="e">
+        <f>#REF!/D12</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K12" s="5">
+        <f>H12/D12</f>
+        <v>0.98758600464009716</v>
+      </c>
+      <c r="M12" s="5">
+        <f>E12/D12</f>
+        <v>9.2008846243072338E-3</v>
+      </c>
+      <c r="N12" s="5" t="e">
+        <f>#REF!/D12</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O12" s="5">
+        <f>I12/D12</f>
+        <v>8.3050674435265794E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A13" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="66">
+        <v>3810031732.5999999</v>
+      </c>
+      <c r="E13" s="66">
+        <v>38318967.155400001</v>
+      </c>
+      <c r="H13" s="66">
+        <v>3431107693.1999998</v>
+      </c>
+      <c r="I13" s="66">
+        <v>54530811.428999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A14" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="66">
+        <v>1822701831.4000001</v>
+      </c>
+      <c r="E14" s="66">
+        <v>38027087.5339</v>
+      </c>
+      <c r="H14" s="66">
+        <v>504405128.39999998</v>
+      </c>
+      <c r="I14" s="66">
+        <v>39336546.523500003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="66">
+        <v>2019444030</v>
+      </c>
+      <c r="E15" s="66">
+        <v>44096097.7223</v>
+      </c>
+      <c r="H15" s="66">
+        <v>1934053663.5999999</v>
+      </c>
+      <c r="I15" s="66">
+        <v>150295057.50999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="18" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="68" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+    </row>
+    <row r="19" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A19" s="2"/>
+      <c r="B19" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="82"/>
+      <c r="F19" s="83" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="82"/>
+      <c r="H19" s="80" t="s">
+        <v>114</v>
+      </c>
+      <c r="I19" s="81"/>
+      <c r="J19" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="L19" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="M19" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="N19" s="82"/>
+      <c r="O19" s="82"/>
+    </row>
+    <row r="20" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N20" s="67" t="s">
+        <v>30</v>
+      </c>
+      <c r="O20" s="67" t="s">
+        <v>43</v>
+      </c>
+      <c r="P20" s="71" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A21" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="66">
+        <v>154224661811</v>
+      </c>
+      <c r="C21" s="66">
+        <v>396037299.84799999</v>
+      </c>
+      <c r="D21" s="66">
+        <v>154231498991</v>
+      </c>
+      <c r="E21" s="66">
+        <v>776501347.76400006</v>
+      </c>
+      <c r="F21" s="66">
+        <v>151858466289</v>
+      </c>
+      <c r="G21" s="66">
+        <v>357254358.009</v>
+      </c>
+      <c r="H21" s="66">
+        <v>153324861138</v>
+      </c>
+      <c r="I21" s="66">
+        <v>336290655.68900001</v>
+      </c>
+      <c r="J21" s="66">
+        <f>D21/B21</f>
+        <v>1.0000443325984296</v>
+      </c>
+      <c r="K21" s="66">
+        <f>F21/B21</f>
+        <v>0.98465747634512735</v>
+      </c>
+      <c r="L21" s="66">
+        <f>H21/B21</f>
+        <v>0.99416564988741751</v>
+      </c>
+      <c r="M21" s="66">
+        <f>C21/B21</f>
+        <v>2.5679245796196831E-3</v>
+      </c>
+      <c r="N21" s="66">
+        <f>E21/B21</f>
+        <v>5.0348714573003293E-3</v>
+      </c>
+      <c r="O21" s="66">
+        <f>G21/B21</f>
+        <v>2.3164541508076692E-3</v>
+      </c>
+      <c r="P21" s="66">
+        <f>I21/B21</f>
+        <v>2.180524513654756E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A22" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="66">
+        <v>334478074273</v>
+      </c>
+      <c r="C22" s="66">
+        <v>1257152096.21</v>
+      </c>
+      <c r="D22" s="66">
+        <v>320995802715</v>
+      </c>
+      <c r="E22" s="66">
+        <v>2139277529.4000001</v>
+      </c>
+      <c r="F22" s="66">
+        <v>326887773402</v>
+      </c>
+      <c r="G22" s="66">
+        <v>1119009493.4200001</v>
+      </c>
+      <c r="H22" s="66">
+        <v>328914925755</v>
+      </c>
+      <c r="I22" s="66">
+        <v>11811502965.6</v>
+      </c>
+      <c r="J22" s="66">
+        <f t="shared" ref="J22:J28" si="0">D22/B22</f>
+        <v>0.95969161330737685</v>
+      </c>
+      <c r="K22" s="66">
+        <f t="shared" ref="K22:K28" si="1">F22/B22</f>
+        <v>0.97730703010205444</v>
+      </c>
+      <c r="L22" s="66">
+        <f t="shared" ref="L22:L28" si="2">H22/B22</f>
+        <v>0.98336767356098986</v>
+      </c>
+      <c r="M22" s="66">
+        <f t="shared" ref="M22:M28" si="3">C22/B22</f>
+        <v>3.7585485952777767E-3</v>
+      </c>
+      <c r="N22" s="66">
+        <f t="shared" ref="N22:N28" si="4">E22/B22</f>
+        <v>6.3958677532146048E-3</v>
+      </c>
+      <c r="O22" s="66">
+        <f t="shared" ref="O22:O28" si="5">G22/B22</f>
+        <v>3.3455391533576814E-3</v>
+      </c>
+      <c r="P22" s="66">
+        <f t="shared" ref="P22:P28" si="6">I22/B22</f>
+        <v>3.5313235378051977E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A23" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="66">
+        <v>91553547.599999994</v>
+      </c>
+      <c r="C23" s="66">
+        <v>1407369.3687</v>
+      </c>
+      <c r="D23" s="66">
+        <v>55426876</v>
+      </c>
+      <c r="E23" s="66">
+        <v>1793666.85338</v>
+      </c>
+      <c r="F23" s="66">
+        <v>71791787.599999994</v>
+      </c>
+      <c r="G23" s="66">
+        <v>2846669.9186200001</v>
+      </c>
+      <c r="H23" s="66">
+        <v>46162437.600000001</v>
+      </c>
+      <c r="I23" s="66">
+        <v>1415999.3302199999</v>
+      </c>
+      <c r="J23" s="66">
+        <f t="shared" si="0"/>
+        <v>0.60540391337058364</v>
+      </c>
+      <c r="K23" s="66">
+        <f t="shared" si="1"/>
+        <v>0.7841508000723284</v>
+      </c>
+      <c r="L23" s="66">
+        <f t="shared" si="2"/>
+        <v>0.50421243971544372</v>
+      </c>
+      <c r="M23" s="66">
+        <f t="shared" si="3"/>
+        <v>1.5372089947282393E-2</v>
+      </c>
+      <c r="N23" s="66">
+        <f t="shared" si="4"/>
+        <v>1.9591451127776945E-2</v>
+      </c>
+      <c r="O23" s="66">
+        <f t="shared" si="5"/>
+        <v>3.1092950445319505E-2</v>
+      </c>
+      <c r="P23" s="66">
+        <f t="shared" si="6"/>
+        <v>1.546635130302695E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A24" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="66">
+        <v>11773123.6</v>
+      </c>
+      <c r="C24" s="66">
+        <v>488609.35972299997</v>
+      </c>
+      <c r="D24" s="66">
+        <v>7471985</v>
+      </c>
+      <c r="E24" s="66">
+        <v>261195.06404100001</v>
+      </c>
+      <c r="F24" s="66">
+        <v>14173087.6</v>
+      </c>
+      <c r="G24" s="66">
+        <v>6172868.7977600005</v>
+      </c>
+      <c r="H24" s="66">
+        <v>3821710</v>
+      </c>
+      <c r="I24" s="66">
+        <v>508277.09580800001</v>
+      </c>
+      <c r="J24" s="66">
+        <f t="shared" si="0"/>
+        <v>0.63466461865736301</v>
+      </c>
+      <c r="K24" s="66">
+        <f t="shared" si="1"/>
+        <v>1.2038510833267733</v>
+      </c>
+      <c r="L24" s="66">
+        <f t="shared" si="2"/>
+        <v>0.32461308738829514</v>
+      </c>
+      <c r="M24" s="66">
+        <f t="shared" si="3"/>
+        <v>4.1502100574481351E-2</v>
+      </c>
+      <c r="N24" s="66">
+        <f t="shared" si="4"/>
+        <v>2.2185706437414791E-2</v>
+      </c>
+      <c r="O24" s="66">
+        <f t="shared" si="5"/>
+        <v>0.52431869463767466</v>
+      </c>
+      <c r="P24" s="66">
+        <f t="shared" si="6"/>
+        <v>4.3172662844378873E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A25" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="66">
+        <v>13403983485.6</v>
+      </c>
+      <c r="C25" s="66">
+        <v>121796591.243</v>
+      </c>
+      <c r="D25" s="66">
+        <v>13356814029.799999</v>
+      </c>
+      <c r="E25" s="66">
+        <v>244857269.73199999</v>
+      </c>
+      <c r="F25" s="66">
+        <v>13099183008.6</v>
+      </c>
+      <c r="G25" s="66">
+        <v>86653181.352899998</v>
+      </c>
+      <c r="H25" s="66">
+        <v>13620259009.4</v>
+      </c>
+      <c r="I25" s="66">
+        <v>186564319.986</v>
+      </c>
+      <c r="J25" s="66">
+        <f t="shared" si="0"/>
+        <v>0.99648093748767474</v>
+      </c>
+      <c r="K25" s="66">
+        <f t="shared" si="1"/>
+        <v>0.97726045564533492</v>
+      </c>
+      <c r="L25" s="66">
+        <f t="shared" si="2"/>
+        <v>1.0161351678799326</v>
+      </c>
+      <c r="M25" s="66">
+        <f t="shared" si="3"/>
+        <v>9.0865966355335327E-3</v>
+      </c>
+      <c r="N25" s="66">
+        <f t="shared" si="4"/>
+        <v>1.8267500105103231E-2</v>
+      </c>
+      <c r="O25" s="66">
+        <f t="shared" si="5"/>
+        <v>6.4647335208963931E-3</v>
+      </c>
+      <c r="P25" s="66">
+        <f t="shared" si="6"/>
+        <v>1.3918572802363376E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A26" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="66">
+        <v>4207290989</v>
+      </c>
+      <c r="C26" s="66">
+        <v>47812624.160400003</v>
+      </c>
+      <c r="D26" s="66">
+        <v>3557269894.1999998</v>
+      </c>
+      <c r="E26" s="66">
+        <v>24548824.4307</v>
+      </c>
+      <c r="F26" s="66">
+        <v>3744450908.5999999</v>
+      </c>
+      <c r="G26" s="66">
+        <v>52157654.794100001</v>
+      </c>
+      <c r="H26" s="66">
+        <v>2911940947</v>
+      </c>
+      <c r="I26" s="66">
+        <v>53453576.313600004</v>
+      </c>
+      <c r="J26" s="66">
+        <f t="shared" si="0"/>
+        <v>0.84550127469207947</v>
+      </c>
+      <c r="K26" s="66">
+        <f t="shared" si="1"/>
+        <v>0.88999095103949322</v>
+      </c>
+      <c r="L26" s="66">
+        <f t="shared" si="2"/>
+        <v>0.69211779138008178</v>
+      </c>
+      <c r="M26" s="66">
+        <f t="shared" si="3"/>
+        <v>1.1364230400370818E-2</v>
+      </c>
+      <c r="N26" s="66">
+        <f t="shared" si="4"/>
+        <v>5.8348292273776928E-3</v>
+      </c>
+      <c r="O26" s="66">
+        <f t="shared" si="5"/>
+        <v>1.2396968721789544E-2</v>
+      </c>
+      <c r="P26" s="66">
+        <f t="shared" si="6"/>
+        <v>1.2704986760686356E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A27" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="66">
+        <v>1591523887.2</v>
+      </c>
+      <c r="C27" s="66">
+        <v>46781665.820299998</v>
+      </c>
+      <c r="D27" s="66">
+        <v>885658835</v>
+      </c>
+      <c r="E27" s="66">
+        <v>49874908.9133</v>
+      </c>
+      <c r="F27" s="66">
+        <v>852721605.60000002</v>
+      </c>
+      <c r="G27" s="66">
+        <v>74307902.240899995</v>
+      </c>
+      <c r="H27" s="66">
+        <v>379748471.39999998</v>
+      </c>
+      <c r="I27" s="66">
+        <v>8505820.7215299997</v>
+      </c>
+      <c r="J27" s="66">
+        <f t="shared" si="0"/>
+        <v>0.55648478927837985</v>
+      </c>
+      <c r="K27" s="66">
+        <f t="shared" si="1"/>
+        <v>0.5357893855430661</v>
+      </c>
+      <c r="L27" s="66">
+        <f t="shared" si="2"/>
+        <v>0.23860683113471773</v>
+      </c>
+      <c r="M27" s="66">
+        <f t="shared" si="3"/>
+        <v>2.9394259298617203E-2</v>
+      </c>
+      <c r="N27" s="66">
+        <f t="shared" si="4"/>
+        <v>3.1337832447520426E-2</v>
+      </c>
+      <c r="O27" s="66">
+        <f t="shared" si="5"/>
+        <v>4.668978130867478E-2</v>
+      </c>
+      <c r="P27" s="66">
+        <f t="shared" si="6"/>
+        <v>5.3444505545527567E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A28" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="66">
+        <v>103376374</v>
+      </c>
+      <c r="C28" s="66">
+        <v>2023324.2933499999</v>
+      </c>
+      <c r="D28" s="66">
+        <v>105115239.59999999</v>
+      </c>
+      <c r="E28" s="66">
+        <v>1651547.44683</v>
+      </c>
+      <c r="F28" s="66">
+        <v>101048964</v>
+      </c>
+      <c r="G28" s="66">
+        <v>2492931.63693</v>
+      </c>
+      <c r="H28" s="66">
+        <v>106508726.8</v>
+      </c>
+      <c r="I28" s="66">
+        <v>2375056.0667400002</v>
+      </c>
+      <c r="J28" s="66">
+        <f t="shared" si="0"/>
+        <v>1.0168207254009509</v>
+      </c>
+      <c r="K28" s="66">
+        <f t="shared" si="1"/>
+        <v>0.97748605498583263</v>
+      </c>
+      <c r="L28" s="66">
+        <f t="shared" si="2"/>
+        <v>1.030300470782618</v>
+      </c>
+      <c r="M28" s="66">
+        <f t="shared" si="3"/>
+        <v>1.9572405328803659E-2</v>
+      </c>
+      <c r="N28" s="66">
+        <f t="shared" si="4"/>
+        <v>1.5976062836465903E-2</v>
+      </c>
+      <c r="O28" s="66">
+        <f t="shared" si="5"/>
+        <v>2.4115100389669308E-2</v>
+      </c>
+      <c r="P28" s="66">
+        <f t="shared" si="6"/>
+        <v>2.2974844007780736E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H6:I6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51140CC8-C0B8-469A-8BAE-C9043CBCBC10}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="C11" workbookViewId="0">
       <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
@@ -4220,7 +5871,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD3A0CC-C87B-4B2D-914D-368FCFB476B0}">
   <dimension ref="A1:P15"/>
   <sheetViews>
@@ -4802,12 +6453,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1814E241-F455-4452-B5DE-B4EE59F14CFA}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5384,7 +7035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC958D8-824A-4FFE-8EFB-EA4CAF2DCC74}">
   <dimension ref="A1:P12"/>
   <sheetViews>
@@ -5956,7 +7607,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F72758A-17BC-4C1E-98B0-DDD6331D597C}">
   <dimension ref="A1:P12"/>
   <sheetViews>
@@ -6529,11 +8180,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C510FE-BA24-4F4C-B882-A73942D255FE}">
   <dimension ref="A2:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -6719,7 +8370,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5A357B-AD95-4B57-AFAC-6E90E36724A8}">
   <dimension ref="A1:H59"/>
   <sheetViews>
@@ -13214,981 +14865,664 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65049047-28B8-4D24-A307-ABB41DE3392E}">
-  <dimension ref="A1:P28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99183D17-15E5-4DA6-B476-6E21D829BB49}">
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="32.86328125" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.06640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.06640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.06640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.73046875" customWidth="1"/>
-    <col min="9" max="9" width="17.9296875" customWidth="1"/>
-    <col min="12" max="12" width="13.86328125" customWidth="1"/>
-    <col min="16" max="16" width="16.53125" customWidth="1"/>
+    <col min="1" max="1" width="36.1328125" customWidth="1"/>
+    <col min="2" max="2" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A2" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
+      <c r="A2" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A3" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-    </row>
-    <row r="4" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-    </row>
-    <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="68" t="s">
-        <v>150</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
+      <c r="A3" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A4" s="65"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
+      <c r="N4" s="65"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A5" s="65"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="2"/>
-      <c r="B6" s="82" t="s">
+      <c r="A6" s="73"/>
+      <c r="B6" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82" t="s">
+      <c r="C6" s="86"/>
+      <c r="D6" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="82"/>
-      <c r="F6" s="83" t="s">
+      <c r="E6" s="86"/>
+      <c r="F6" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="82"/>
-      <c r="H6" s="80" t="s">
+      <c r="G6" s="86"/>
+      <c r="H6" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="81"/>
-      <c r="J6" s="7" t="s">
+      <c r="I6" s="87"/>
+      <c r="J6" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="L6" s="70" t="s">
+      <c r="L6" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="83" t="s">
+      <c r="M6" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="82"/>
-      <c r="O6" s="82"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="M7" s="3" t="s">
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="N7" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="O7" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="P7" s="71" t="s">
+      <c r="P7" s="77" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="66" t="s">
         <v>1</v>
       </c>
+      <c r="B8" s="66">
+        <v>13563151726</v>
+      </c>
+      <c r="C8" s="66">
+        <v>93351086.245000005</v>
+      </c>
       <c r="D8" s="66">
-        <v>154918952634</v>
+        <v>13364827557.6</v>
       </c>
       <c r="E8" s="66">
-        <v>280351869.92900002</v>
+        <v>146986924.491</v>
+      </c>
+      <c r="F8" s="66">
+        <v>13582753150.799999</v>
+      </c>
+      <c r="G8" s="66">
+        <v>1401281353.04</v>
       </c>
       <c r="H8" s="66">
-        <v>155317428173</v>
+        <v>14365139458.200001</v>
       </c>
       <c r="I8" s="66">
-        <v>1411292601.6199999</v>
-      </c>
-      <c r="J8" s="5" t="e">
-        <f>#REF!/D8</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K8" s="5">
-        <f>H8/D8</f>
-        <v>1.0025721548734028</v>
-      </c>
-      <c r="M8" s="5">
-        <f>E8/D8</f>
-        <v>1.809667991955371E-3</v>
-      </c>
-      <c r="N8" s="5" t="e">
-        <f>#REF!/D8</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O8" s="5">
-        <f>I8/D8</f>
-        <v>9.1098769880933479E-3</v>
+        <v>1279732382.5799999</v>
+      </c>
+      <c r="J8" s="66">
+        <f>D8/B8</f>
+        <v>0.98537772249352484</v>
+      </c>
+      <c r="K8" s="66">
+        <f>F8/B8</f>
+        <v>1.0014451968978879</v>
+      </c>
+      <c r="L8" s="66">
+        <f>H8/B8</f>
+        <v>1.0591298946145846</v>
+      </c>
+      <c r="M8" s="66">
+        <f>C8/B8</f>
+        <v>6.8826986625866492E-3</v>
+      </c>
+      <c r="N8" s="66">
+        <f>E8/B8</f>
+        <v>1.0837224817682468E-2</v>
+      </c>
+      <c r="O8" s="66">
+        <f>G8/B8</f>
+        <v>0.10331531942931831</v>
+      </c>
+      <c r="P8" s="66">
+        <f>I8/B8</f>
+        <v>9.4353614000115174E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="66" t="s">
         <v>2</v>
       </c>
+      <c r="B9" s="66">
+        <v>334355105530</v>
+      </c>
+      <c r="C9" s="66">
+        <v>262052286.92399999</v>
+      </c>
       <c r="D9" s="66">
-        <v>323888734975</v>
+        <v>332263518861</v>
       </c>
       <c r="E9" s="66">
-        <v>1799069197.0699999</v>
+        <v>17801899819.900002</v>
+      </c>
+      <c r="F9" s="66">
+        <v>329292059095</v>
+      </c>
+      <c r="G9" s="66">
+        <v>10898951281.200001</v>
       </c>
       <c r="H9" s="66">
-        <v>324404115108</v>
+        <v>334514741490</v>
       </c>
       <c r="I9" s="66">
-        <v>3561778733.0300002</v>
-      </c>
-      <c r="J9" s="5" t="e">
-        <f>#REF!/D9</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K9" s="5">
-        <f>H9/D9</f>
-        <v>1.0015912258666229</v>
-      </c>
-      <c r="M9" s="5">
-        <f>E9/D9</f>
-        <v>5.5545902120024788E-3</v>
-      </c>
-      <c r="N9" s="5" t="e">
-        <f>#REF!/D9</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O9" s="5">
-        <f>I9/D9</f>
-        <v>1.0996920696562426E-2</v>
+        <v>18754581602.700001</v>
+      </c>
+      <c r="J9" s="66">
+        <f t="shared" ref="J9:J15" si="0">D9/B9</f>
+        <v>0.99374441534043711</v>
+      </c>
+      <c r="K9" s="66">
+        <f t="shared" ref="K9:K15" si="1">F9/B9</f>
+        <v>0.98485727793217226</v>
+      </c>
+      <c r="L9" s="66">
+        <f t="shared" ref="L9:L15" si="2">H9/B9</f>
+        <v>1.0004774443618767</v>
+      </c>
+      <c r="M9" s="66">
+        <f t="shared" ref="M9:M15" si="3">C9/B9</f>
+        <v>7.8375440539067036E-4</v>
+      </c>
+      <c r="N9" s="66">
+        <f t="shared" ref="N9:N15" si="4">E9/B9</f>
+        <v>5.324249435845007E-2</v>
+      </c>
+      <c r="O9" s="66">
+        <f t="shared" ref="O9:O15" si="5">G9/B9</f>
+        <v>3.2596933921268008E-2</v>
+      </c>
+      <c r="P9" s="66">
+        <f t="shared" ref="P9:P15" si="6">I9/B9</f>
+        <v>5.6091805665630087E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="66" t="s">
         <v>35</v>
       </c>
+      <c r="B10" s="66">
+        <v>89023452.400000006</v>
+      </c>
+      <c r="C10" s="66">
+        <v>954956.12547500001</v>
+      </c>
       <c r="D10" s="66">
-        <v>67105167.399999999</v>
+        <v>53305900.200000003</v>
       </c>
       <c r="E10" s="66">
-        <v>851354.688035</v>
+        <v>1130037.8262499999</v>
+      </c>
+      <c r="F10" s="66">
+        <v>76088356</v>
+      </c>
+      <c r="G10" s="66">
+        <v>4772971.2505999999</v>
       </c>
       <c r="H10" s="66">
-        <v>54168281.200000003</v>
+        <v>45756372</v>
       </c>
       <c r="I10" s="66">
-        <v>275826.63121700002</v>
-      </c>
-      <c r="J10" s="5" t="e">
-        <f>#REF!/D10</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K10" s="5">
-        <f>H10/D10</f>
-        <v>0.80721475407570487</v>
-      </c>
-      <c r="M10" s="5">
-        <f>E10/D10</f>
-        <v>1.2686872278557195E-2</v>
-      </c>
-      <c r="N10" s="5" t="e">
-        <f>#REF!/D10</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O10" s="5">
-        <f>I10/D10</f>
-        <v>4.1103635070732277E-3</v>
+        <v>3295743.5932900002</v>
+      </c>
+      <c r="J10" s="66">
+        <f t="shared" si="0"/>
+        <v>0.59878491299670156</v>
+      </c>
+      <c r="K10" s="66">
+        <f t="shared" si="1"/>
+        <v>0.85470012618832103</v>
+      </c>
+      <c r="L10" s="66">
+        <f t="shared" si="2"/>
+        <v>0.51398110010840237</v>
+      </c>
+      <c r="M10" s="66">
+        <f t="shared" si="3"/>
+        <v>1.0727017428892703E-2</v>
+      </c>
+      <c r="N10" s="66">
+        <f t="shared" si="4"/>
+        <v>1.2693709306762405E-2</v>
+      </c>
+      <c r="O10" s="66">
+        <f t="shared" si="5"/>
+        <v>5.3614762424109265E-2</v>
+      </c>
+      <c r="P10" s="66">
+        <f t="shared" si="6"/>
+        <v>3.7021071464197676E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="66" t="s">
         <v>36</v>
       </c>
+      <c r="B11" s="66">
+        <v>11554263.4</v>
+      </c>
+      <c r="C11" s="66">
+        <v>648866.92103199998</v>
+      </c>
       <c r="D11" s="66">
-        <v>15824359</v>
+        <v>8492568</v>
       </c>
       <c r="E11" s="66">
-        <v>1011097.01176</v>
+        <v>208867.300303</v>
+      </c>
+      <c r="F11" s="66">
+        <v>7906681.5999999996</v>
+      </c>
+      <c r="G11" s="66">
+        <v>7852306.4089599997</v>
       </c>
       <c r="H11" s="66">
-        <v>4744871.2</v>
+        <v>7801803.2000000002</v>
       </c>
       <c r="I11" s="66">
-        <v>436397.91209400003</v>
-      </c>
-      <c r="J11" s="5" t="e">
-        <f>#REF!/D11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K11" s="5">
-        <f>H11/D11</f>
-        <v>0.29984602851843795</v>
-      </c>
-      <c r="M11" s="5">
-        <f>E11/D11</f>
-        <v>6.3894974308911973E-2</v>
-      </c>
-      <c r="N11" s="5" t="e">
-        <f>#REF!/D11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O11" s="5">
-        <f>I11/D11</f>
-        <v>2.7577604381574004E-2</v>
+        <v>7452421.4309700001</v>
+      </c>
+      <c r="J11" s="66">
+        <f t="shared" si="0"/>
+        <v>0.73501595956346288</v>
+      </c>
+      <c r="K11" s="66">
+        <f t="shared" si="1"/>
+        <v>0.68430858171365549</v>
+      </c>
+      <c r="L11" s="66">
+        <f t="shared" si="2"/>
+        <v>0.67523155132502866</v>
+      </c>
+      <c r="M11" s="66">
+        <f t="shared" si="3"/>
+        <v>5.6158224766799061E-2</v>
+      </c>
+      <c r="N11" s="66">
+        <f t="shared" si="4"/>
+        <v>1.8077076233436049E-2</v>
+      </c>
+      <c r="O11" s="66">
+        <f t="shared" si="5"/>
+        <v>0.6796025100968357</v>
+      </c>
+      <c r="P11" s="66">
+        <f t="shared" si="6"/>
+        <v>0.64499320925728587</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="66" t="s">
         <v>15</v>
       </c>
+      <c r="B12" s="66">
+        <v>154266408196</v>
+      </c>
+      <c r="C12" s="66">
+        <v>333540127.14300001</v>
+      </c>
       <c r="D12" s="66">
-        <v>13571559205.200001</v>
+        <v>153708667247</v>
       </c>
       <c r="E12" s="66">
-        <v>124870350.419</v>
+        <v>1125204248.3900001</v>
+      </c>
+      <c r="F12" s="66">
+        <v>151315685357</v>
+      </c>
+      <c r="G12" s="66">
+        <v>505401413.60900003</v>
       </c>
       <c r="H12" s="66">
-        <v>13403081932.200001</v>
+        <v>152691956895</v>
       </c>
       <c r="I12" s="66">
-        <v>112712714.513</v>
-      </c>
-      <c r="J12" s="5" t="e">
-        <f>#REF!/D12</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K12" s="5">
-        <f>H12/D12</f>
-        <v>0.98758600464009716</v>
-      </c>
-      <c r="M12" s="5">
-        <f>E12/D12</f>
-        <v>9.2008846243072338E-3</v>
-      </c>
-      <c r="N12" s="5" t="e">
-        <f>#REF!/D12</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O12" s="5">
-        <f>I12/D12</f>
-        <v>8.3050674435265794E-3</v>
+        <v>1049509775.46</v>
+      </c>
+      <c r="J12" s="66">
+        <f t="shared" si="0"/>
+        <v>0.99638455996012187</v>
+      </c>
+      <c r="K12" s="66">
+        <f t="shared" si="1"/>
+        <v>0.98087255110489757</v>
+      </c>
+      <c r="L12" s="66">
+        <f t="shared" si="2"/>
+        <v>0.98979394594447534</v>
+      </c>
+      <c r="M12" s="66">
+        <f t="shared" si="3"/>
+        <v>2.1621047060305411E-3</v>
+      </c>
+      <c r="N12" s="66">
+        <f t="shared" si="4"/>
+        <v>7.2939031999785398E-3</v>
+      </c>
+      <c r="O12" s="66">
+        <f t="shared" si="5"/>
+        <v>3.2761598556626322E-3</v>
+      </c>
+      <c r="P12" s="66">
+        <f t="shared" si="6"/>
+        <v>6.8032294764169728E-3</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="66" t="s">
         <v>4</v>
       </c>
+      <c r="B13" s="66">
+        <v>4339882189</v>
+      </c>
+      <c r="C13" s="66">
+        <v>94571446.819900006</v>
+      </c>
       <c r="D13" s="66">
-        <v>3810031732.5999999</v>
+        <v>3521968783.8000002</v>
       </c>
       <c r="E13" s="66">
-        <v>38318967.155400001</v>
+        <v>46258535.239299998</v>
+      </c>
+      <c r="F13" s="66">
+        <v>3772166970</v>
+      </c>
+      <c r="G13" s="66">
+        <v>46064277.778800003</v>
       </c>
       <c r="H13" s="66">
-        <v>3431107693.1999998</v>
+        <v>2916716897.8000002</v>
       </c>
       <c r="I13" s="66">
-        <v>54530811.428999998</v>
+        <v>36696330.085299999</v>
+      </c>
+      <c r="J13" s="66">
+        <f t="shared" si="0"/>
+        <v>0.81153557410541965</v>
+      </c>
+      <c r="K13" s="66">
+        <f t="shared" si="1"/>
+        <v>0.86918649072111942</v>
+      </c>
+      <c r="L13" s="66">
+        <f t="shared" si="2"/>
+        <v>0.67207282842672578</v>
+      </c>
+      <c r="M13" s="66">
+        <f t="shared" si="3"/>
+        <v>2.1791247481234337E-2</v>
+      </c>
+      <c r="N13" s="66">
+        <f t="shared" si="4"/>
+        <v>1.065893801369731E-2</v>
+      </c>
+      <c r="O13" s="66">
+        <f t="shared" si="5"/>
+        <v>1.0614177015117127E-2</v>
+      </c>
+      <c r="P13" s="66">
+        <f t="shared" si="6"/>
+        <v>8.4556051264045029E-3</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A14" s="65" t="s">
+      <c r="A14" s="66" t="s">
         <v>6</v>
       </c>
+      <c r="B14" s="66">
+        <v>1476198697</v>
+      </c>
+      <c r="C14" s="66">
+        <v>71316578.637799993</v>
+      </c>
       <c r="D14" s="66">
-        <v>1822701831.4000001</v>
+        <v>1043094764.4</v>
       </c>
       <c r="E14" s="66">
-        <v>38027087.5339</v>
+        <v>43551366.377800003</v>
+      </c>
+      <c r="F14" s="66">
+        <v>430432636.19999999</v>
+      </c>
+      <c r="G14" s="66">
+        <v>29782884.002</v>
       </c>
       <c r="H14" s="66">
-        <v>504405128.39999998</v>
+        <v>404692467.80000001</v>
       </c>
       <c r="I14" s="66">
-        <v>39336546.523500003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="65" t="s">
+        <v>17091650.657299999</v>
+      </c>
+      <c r="J14" s="66">
+        <f t="shared" si="0"/>
+        <v>0.70660864727751482</v>
+      </c>
+      <c r="K14" s="66">
+        <f t="shared" si="1"/>
+        <v>0.29158177491603626</v>
+      </c>
+      <c r="L14" s="66">
+        <f t="shared" si="2"/>
+        <v>0.27414498374943358</v>
+      </c>
+      <c r="M14" s="66">
+        <f t="shared" si="3"/>
+        <v>4.8310961649493986E-2</v>
+      </c>
+      <c r="N14" s="66">
+        <f t="shared" si="4"/>
+        <v>2.9502374217174915E-2</v>
+      </c>
+      <c r="O14" s="66">
+        <f t="shared" si="5"/>
+        <v>2.0175389710427309E-2</v>
+      </c>
+      <c r="P14" s="66">
+        <f t="shared" si="6"/>
+        <v>1.157815048342371E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A15" s="66" t="s">
         <v>20</v>
       </c>
+      <c r="B15" s="66">
+        <v>166283139.19999999</v>
+      </c>
+      <c r="C15" s="66">
+        <v>3557251.2152300002</v>
+      </c>
       <c r="D15" s="66">
-        <v>2019444030</v>
+        <v>164423405.80000001</v>
       </c>
       <c r="E15" s="66">
-        <v>44096097.7223</v>
+        <v>3329099.5423099999</v>
+      </c>
+      <c r="F15" s="66">
+        <v>162008092</v>
+      </c>
+      <c r="G15" s="66">
+        <v>1281746.34726</v>
       </c>
       <c r="H15" s="66">
-        <v>1934053663.5999999</v>
+        <v>166116687.19999999</v>
       </c>
       <c r="I15" s="66">
-        <v>150295057.50999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" s="65" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="18" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="68" t="s">
-        <v>151</v>
-      </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-    </row>
-    <row r="19" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A19" s="2"/>
-      <c r="B19" s="82" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="82"/>
-      <c r="D19" s="82" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="82"/>
-      <c r="F19" s="83" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" s="82"/>
-      <c r="H19" s="80" t="s">
-        <v>114</v>
-      </c>
-      <c r="I19" s="81"/>
-      <c r="J19" s="67" t="s">
-        <v>45</v>
-      </c>
-      <c r="K19" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="L19" s="70" t="s">
-        <v>115</v>
-      </c>
-      <c r="M19" s="83" t="s">
-        <v>44</v>
-      </c>
-      <c r="N19" s="82"/>
-      <c r="O19" s="82"/>
-    </row>
-    <row r="20" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="M20" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N20" s="67" t="s">
-        <v>30</v>
-      </c>
-      <c r="O20" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="P20" s="71" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A21" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="66">
-        <v>154224661811</v>
-      </c>
-      <c r="C21" s="66">
-        <v>396037299.84799999</v>
-      </c>
-      <c r="D21" s="66">
-        <v>154231498991</v>
-      </c>
-      <c r="E21" s="66">
-        <v>776501347.76400006</v>
-      </c>
-      <c r="F21" s="66">
-        <v>151858466289</v>
-      </c>
-      <c r="G21" s="66">
-        <v>357254358.009</v>
-      </c>
-      <c r="H21" s="66">
-        <v>153324861138</v>
-      </c>
-      <c r="I21" s="66">
-        <v>336290655.68900001</v>
-      </c>
-      <c r="J21" s="66">
-        <f>D21/B21</f>
-        <v>1.0000443325984296</v>
-      </c>
-      <c r="K21" s="66">
-        <f>F21/B21</f>
-        <v>0.98465747634512735</v>
-      </c>
-      <c r="L21" s="66">
-        <f>H21/B21</f>
-        <v>0.99416564988741751</v>
-      </c>
-      <c r="M21" s="66">
-        <f>C21/B21</f>
-        <v>2.5679245796196831E-3</v>
-      </c>
-      <c r="N21" s="66">
-        <f>E21/B21</f>
-        <v>5.0348714573003293E-3</v>
-      </c>
-      <c r="O21" s="66">
-        <f>G21/B21</f>
-        <v>2.3164541508076692E-3</v>
-      </c>
-      <c r="P21" s="66">
-        <f>I21/B21</f>
-        <v>2.180524513654756E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A22" s="65" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="66">
-        <v>334478074273</v>
-      </c>
-      <c r="C22" s="66">
-        <v>1257152096.21</v>
-      </c>
-      <c r="D22" s="66">
-        <v>320995802715</v>
-      </c>
-      <c r="E22" s="66">
-        <v>2139277529.4000001</v>
-      </c>
-      <c r="F22" s="66">
-        <v>326887773402</v>
-      </c>
-      <c r="G22" s="66">
-        <v>1119009493.4200001</v>
-      </c>
-      <c r="H22" s="66">
-        <v>328914925755</v>
-      </c>
-      <c r="I22" s="66">
-        <v>11811502965.6</v>
-      </c>
-      <c r="J22" s="66">
-        <f t="shared" ref="J22:J28" si="0">D22/B22</f>
-        <v>0.95969161330737685</v>
-      </c>
-      <c r="K22" s="66">
-        <f t="shared" ref="K22:K28" si="1">F22/B22</f>
-        <v>0.97730703010205444</v>
-      </c>
-      <c r="L22" s="66">
-        <f t="shared" ref="L22:L28" si="2">H22/B22</f>
-        <v>0.98336767356098986</v>
-      </c>
-      <c r="M22" s="66">
-        <f t="shared" ref="M22:M28" si="3">C22/B22</f>
-        <v>3.7585485952777767E-3</v>
-      </c>
-      <c r="N22" s="66">
-        <f t="shared" ref="N22:N28" si="4">E22/B22</f>
-        <v>6.3958677532146048E-3</v>
-      </c>
-      <c r="O22" s="66">
-        <f t="shared" ref="O22:O28" si="5">G22/B22</f>
-        <v>3.3455391533576814E-3</v>
-      </c>
-      <c r="P22" s="66">
-        <f t="shared" ref="P22:P28" si="6">I22/B22</f>
-        <v>3.5313235378051977E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A23" s="65" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="66">
-        <v>91553547.599999994</v>
-      </c>
-      <c r="C23" s="66">
-        <v>1407369.3687</v>
-      </c>
-      <c r="D23" s="66">
-        <v>55426876</v>
-      </c>
-      <c r="E23" s="66">
-        <v>1793666.85338</v>
-      </c>
-      <c r="F23" s="66">
-        <v>71791787.599999994</v>
-      </c>
-      <c r="G23" s="66">
-        <v>2846669.9186200001</v>
-      </c>
-      <c r="H23" s="66">
-        <v>46162437.600000001</v>
-      </c>
-      <c r="I23" s="66">
-        <v>1415999.3302199999</v>
-      </c>
-      <c r="J23" s="66">
-        <f t="shared" si="0"/>
-        <v>0.60540391337058364</v>
-      </c>
-      <c r="K23" s="66">
-        <f t="shared" si="1"/>
-        <v>0.7841508000723284</v>
-      </c>
-      <c r="L23" s="66">
-        <f t="shared" si="2"/>
-        <v>0.50421243971544372</v>
-      </c>
-      <c r="M23" s="66">
-        <f t="shared" si="3"/>
-        <v>1.5372089947282393E-2</v>
-      </c>
-      <c r="N23" s="66">
-        <f t="shared" si="4"/>
-        <v>1.9591451127776945E-2</v>
-      </c>
-      <c r="O23" s="66">
+        <v>2042722.8918000001</v>
+      </c>
+      <c r="J15" s="66">
+        <f t="shared" si="0"/>
+        <v>0.98881586305775027</v>
+      </c>
+      <c r="K15" s="66">
+        <f t="shared" si="1"/>
+        <v>0.97429055513043872</v>
+      </c>
+      <c r="L15" s="66">
+        <f t="shared" si="2"/>
+        <v>0.99899898449836333</v>
+      </c>
+      <c r="M15" s="66">
+        <f t="shared" si="3"/>
+        <v>2.1392735501291286E-2</v>
+      </c>
+      <c r="N15" s="66">
+        <f t="shared" si="4"/>
+        <v>2.0020668110588571E-2</v>
+      </c>
+      <c r="O15" s="66">
         <f t="shared" si="5"/>
-        <v>3.1092950445319505E-2</v>
-      </c>
-      <c r="P23" s="66">
+        <v>7.7082159587951778E-3</v>
+      </c>
+      <c r="P15" s="66">
         <f t="shared" si="6"/>
-        <v>1.546635130302695E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A24" s="65" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="66">
-        <v>11773123.6</v>
-      </c>
-      <c r="C24" s="66">
-        <v>488609.35972299997</v>
-      </c>
-      <c r="D24" s="66">
-        <v>7471985</v>
-      </c>
-      <c r="E24" s="66">
-        <v>261195.06404100001</v>
-      </c>
-      <c r="F24" s="66">
-        <v>14173087.6</v>
-      </c>
-      <c r="G24" s="66">
-        <v>6172868.7977600005</v>
-      </c>
-      <c r="H24" s="66">
-        <v>3821710</v>
-      </c>
-      <c r="I24" s="66">
-        <v>508277.09580800001</v>
-      </c>
-      <c r="J24" s="66">
-        <f t="shared" si="0"/>
-        <v>0.63466461865736301</v>
-      </c>
-      <c r="K24" s="66">
-        <f t="shared" si="1"/>
-        <v>1.2038510833267733</v>
-      </c>
-      <c r="L24" s="66">
-        <f t="shared" si="2"/>
-        <v>0.32461308738829514</v>
-      </c>
-      <c r="M24" s="66">
-        <f t="shared" si="3"/>
-        <v>4.1502100574481351E-2</v>
-      </c>
-      <c r="N24" s="66">
-        <f t="shared" si="4"/>
-        <v>2.2185706437414791E-2</v>
-      </c>
-      <c r="O24" s="66">
-        <f t="shared" si="5"/>
-        <v>0.52431869463767466</v>
-      </c>
-      <c r="P24" s="66">
-        <f t="shared" si="6"/>
-        <v>4.3172662844378873E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A25" s="65" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="66">
-        <v>13403983485.6</v>
-      </c>
-      <c r="C25" s="66">
-        <v>121796591.243</v>
-      </c>
-      <c r="D25" s="66">
-        <v>13356814029.799999</v>
-      </c>
-      <c r="E25" s="66">
-        <v>244857269.73199999</v>
-      </c>
-      <c r="F25" s="66">
-        <v>13099183008.6</v>
-      </c>
-      <c r="G25" s="66">
-        <v>86653181.352899998</v>
-      </c>
-      <c r="H25" s="66">
-        <v>13620259009.4</v>
-      </c>
-      <c r="I25" s="66">
-        <v>186564319.986</v>
-      </c>
-      <c r="J25" s="66">
-        <f t="shared" si="0"/>
-        <v>0.99648093748767474</v>
-      </c>
-      <c r="K25" s="66">
-        <f t="shared" si="1"/>
-        <v>0.97726045564533492</v>
-      </c>
-      <c r="L25" s="66">
-        <f t="shared" si="2"/>
-        <v>1.0161351678799326</v>
-      </c>
-      <c r="M25" s="66">
-        <f t="shared" si="3"/>
-        <v>9.0865966355335327E-3</v>
-      </c>
-      <c r="N25" s="66">
-        <f t="shared" si="4"/>
-        <v>1.8267500105103231E-2</v>
-      </c>
-      <c r="O25" s="66">
-        <f t="shared" si="5"/>
-        <v>6.4647335208963931E-3</v>
-      </c>
-      <c r="P25" s="66">
-        <f t="shared" si="6"/>
-        <v>1.3918572802363376E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A26" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="66">
-        <v>4207290989</v>
-      </c>
-      <c r="C26" s="66">
-        <v>47812624.160400003</v>
-      </c>
-      <c r="D26" s="66">
-        <v>3557269894.1999998</v>
-      </c>
-      <c r="E26" s="66">
-        <v>24548824.4307</v>
-      </c>
-      <c r="F26" s="66">
-        <v>3744450908.5999999</v>
-      </c>
-      <c r="G26" s="66">
-        <v>52157654.794100001</v>
-      </c>
-      <c r="H26" s="66">
-        <v>2911940947</v>
-      </c>
-      <c r="I26" s="66">
-        <v>53453576.313600004</v>
-      </c>
-      <c r="J26" s="66">
-        <f t="shared" si="0"/>
-        <v>0.84550127469207947</v>
-      </c>
-      <c r="K26" s="66">
-        <f t="shared" si="1"/>
-        <v>0.88999095103949322</v>
-      </c>
-      <c r="L26" s="66">
-        <f t="shared" si="2"/>
-        <v>0.69211779138008178</v>
-      </c>
-      <c r="M26" s="66">
-        <f t="shared" si="3"/>
-        <v>1.1364230400370818E-2</v>
-      </c>
-      <c r="N26" s="66">
-        <f t="shared" si="4"/>
-        <v>5.8348292273776928E-3</v>
-      </c>
-      <c r="O26" s="66">
-        <f t="shared" si="5"/>
-        <v>1.2396968721789544E-2</v>
-      </c>
-      <c r="P26" s="66">
-        <f t="shared" si="6"/>
-        <v>1.2704986760686356E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A27" s="65" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="66">
-        <v>1591523887.2</v>
-      </c>
-      <c r="C27" s="66">
-        <v>46781665.820299998</v>
-      </c>
-      <c r="D27" s="66">
-        <v>885658835</v>
-      </c>
-      <c r="E27" s="66">
-        <v>49874908.9133</v>
-      </c>
-      <c r="F27" s="66">
-        <v>852721605.60000002</v>
-      </c>
-      <c r="G27" s="66">
-        <v>74307902.240899995</v>
-      </c>
-      <c r="H27" s="66">
-        <v>379748471.39999998</v>
-      </c>
-      <c r="I27" s="66">
-        <v>8505820.7215299997</v>
-      </c>
-      <c r="J27" s="66">
-        <f t="shared" si="0"/>
-        <v>0.55648478927837985</v>
-      </c>
-      <c r="K27" s="66">
-        <f t="shared" si="1"/>
-        <v>0.5357893855430661</v>
-      </c>
-      <c r="L27" s="66">
-        <f t="shared" si="2"/>
-        <v>0.23860683113471773</v>
-      </c>
-      <c r="M27" s="66">
-        <f t="shared" si="3"/>
-        <v>2.9394259298617203E-2</v>
-      </c>
-      <c r="N27" s="66">
-        <f t="shared" si="4"/>
-        <v>3.1337832447520426E-2</v>
-      </c>
-      <c r="O27" s="66">
-        <f t="shared" si="5"/>
-        <v>4.668978130867478E-2</v>
-      </c>
-      <c r="P27" s="66">
-        <f t="shared" si="6"/>
-        <v>5.3444505545527567E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A28" s="65" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="66">
-        <v>103376374</v>
-      </c>
-      <c r="C28" s="66">
-        <v>2023324.2933499999</v>
-      </c>
-      <c r="D28" s="66">
-        <v>105115239.59999999</v>
-      </c>
-      <c r="E28" s="66">
-        <v>1651547.44683</v>
-      </c>
-      <c r="F28" s="66">
-        <v>101048964</v>
-      </c>
-      <c r="G28" s="66">
-        <v>2492931.63693</v>
-      </c>
-      <c r="H28" s="66">
-        <v>106508726.8</v>
-      </c>
-      <c r="I28" s="66">
-        <v>2375056.0667400002</v>
-      </c>
-      <c r="J28" s="66">
-        <f t="shared" si="0"/>
-        <v>1.0168207254009509</v>
-      </c>
-      <c r="K28" s="66">
-        <f t="shared" si="1"/>
-        <v>0.97748605498583263</v>
-      </c>
-      <c r="L28" s="66">
-        <f t="shared" si="2"/>
-        <v>1.030300470782618</v>
-      </c>
-      <c r="M28" s="66">
-        <f t="shared" si="3"/>
-        <v>1.9572405328803659E-2</v>
-      </c>
-      <c r="N28" s="66">
-        <f t="shared" si="4"/>
-        <v>1.5976062836465903E-2</v>
-      </c>
-      <c r="O28" s="66">
-        <f t="shared" si="5"/>
-        <v>2.4115100389669308E-2</v>
-      </c>
-      <c r="P28" s="66">
-        <f t="shared" si="6"/>
-        <v>2.2974844007780736E-2</v>
+        <v>1.2284606254294244E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="5">
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="M6:O6"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added plots of ITLB and DTLB postgresql performance with varying database size
Database size ranges from 1GB to 12GB
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1084" documentId="3E3A0F759595214EF5B7DC1E59180F3A328511B7" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{D58D87AE-4730-49CF-8A66-6F2079E2654C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -16,18 +15,19 @@
     <sheet name="clang-2core-os" sheetId="15" r:id="rId6"/>
     <sheet name="clang-2core-usr" sheetId="16" r:id="rId7"/>
     <sheet name="clang-stats" sheetId="17" r:id="rId8"/>
-    <sheet name="postgres-12GB-os" sheetId="25" r:id="rId9"/>
-    <sheet name="postgres-12GB-usr" sheetId="26" r:id="rId10"/>
-    <sheet name="postgres-8GB-os" sheetId="23" r:id="rId11"/>
-    <sheet name="postgres-8GB-usr" sheetId="24" r:id="rId12"/>
-    <sheet name="postgres-4GB-os" sheetId="11" r:id="rId13"/>
-    <sheet name="postgres-4GB-usr" sheetId="8" r:id="rId14"/>
-    <sheet name="postgres-1GB-os" sheetId="18" r:id="rId15"/>
-    <sheet name="postgres-1GB-usr" sheetId="19" r:id="rId16"/>
-    <sheet name="octane-os" sheetId="20" r:id="rId17"/>
-    <sheet name="octane-usr" sheetId="21" r:id="rId18"/>
-    <sheet name="octane-stats" sheetId="22" r:id="rId19"/>
-    <sheet name="postgres_stats" sheetId="9" r:id="rId20"/>
+    <sheet name="postgres summary" sheetId="27" r:id="rId9"/>
+    <sheet name="postgres-12GB-os" sheetId="25" r:id="rId10"/>
+    <sheet name="postgres-12GB-usr" sheetId="26" r:id="rId11"/>
+    <sheet name="postgres-8GB-os" sheetId="23" r:id="rId12"/>
+    <sheet name="postgres-8GB-usr" sheetId="24" r:id="rId13"/>
+    <sheet name="postgres-4GB-os" sheetId="11" r:id="rId14"/>
+    <sheet name="postgres-4GB-usr" sheetId="8" r:id="rId15"/>
+    <sheet name="postgres-1GB-os" sheetId="18" r:id="rId16"/>
+    <sheet name="postgres-1GB-usr" sheetId="19" r:id="rId17"/>
+    <sheet name="octane-os" sheetId="20" r:id="rId18"/>
+    <sheet name="octane-usr" sheetId="21" r:id="rId19"/>
+    <sheet name="octane-stats" sheetId="22" r:id="rId20"/>
+    <sheet name="postgres_stats" sheetId="9" r:id="rId21"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="208">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -673,6 +673,21 @@
   </si>
   <si>
     <t>12GB/2MB * 2 # of super pages for each iteration</t>
+  </si>
+  <si>
+    <t>Database Size (GB)</t>
+  </si>
+  <si>
+    <t>Code super page</t>
+  </si>
+  <si>
+    <t>shared ptp + code super page</t>
+  </si>
+  <si>
+    <t>std. dev.</t>
+  </si>
+  <si>
+    <t>Shared ptp + code super page</t>
   </si>
 </sst>
 </file>
@@ -899,7 +914,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1064,6 +1079,13 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1080,6 +1102,2373 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'postgres summary'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Shared ptp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'postgres summary'!$A$4:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'postgres summary'!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.9356013083638639</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94469744673390132</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.87222223701487334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90400805184937105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0E3C-48C1-9DE2-0D8FD0EBBDCF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'postgres summary'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Code super page</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'postgres summary'!$A$4:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'postgres summary'!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.29882809452770503</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29466756956271822</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28024151734484376</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29114478875725908</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0E3C-48C1-9DE2-0D8FD0EBBDCF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'postgres summary'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>shared ptp + code super page</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'postgres summary'!$A$4:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'postgres summary'!$D$4:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.38405980306350745</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.38277691547795289</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.37004112521020127</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.36980716829392185</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0E3C-48C1-9DE2-0D8FD0EBBDCF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="128257352"/>
+        <c:axId val="128257680"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="128257352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Database</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Size (GB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="128257680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="128257680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ITLB_MISSES.WALK_PENDING normalized to the baseline</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="128257352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'postgres summary'!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Shared ptp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'postgres summary'!$A$13:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'postgres summary'!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.96271978203603858</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9442762311353079</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.86439751671266363</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.91955706039378737</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0BDE-4399-B19A-7A01C9B4C1E1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'postgres summary'!$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Code super page</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'postgres summary'!$A$13:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'postgres summary'!$C$13:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.38730105438735418</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41434324900610719</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.41517545864783562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.44375153500032488</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0BDE-4399-B19A-7A01C9B4C1E1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'postgres summary'!$D$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Shared ptp + code super page</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'postgres summary'!$A$13:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'postgres summary'!$D$13:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.36957921312384739</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.40083074332271823</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42928869176101703</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4494151032037067</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0BDE-4399-B19A-7A01C9B4C1E1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="731787936"/>
+        <c:axId val="731788264"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="731787936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Database</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Size (GB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="731788264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="731788264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>DTLB_LOAD_MISSES.WALK_PENDING normalized</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> to the baseline</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="731787936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>931068</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>40481</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>604838</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E51531F6-5503-42DD-B658-9F14AD3AA697}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1288256</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>173830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>481013</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0487063C-0E93-4F41-B001-2C1E33205431}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3348,11 +5737,674 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638ACDA3-EFA6-47B5-8321-84E7AF859506}">
+  <dimension ref="A1:P15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A1" s="72" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A2" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A3" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A4" s="65"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
+      <c r="N4" s="65"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A5" s="65"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
+    </row>
+    <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="73"/>
+      <c r="B6" s="88" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="88"/>
+      <c r="H6" s="89" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" s="89"/>
+      <c r="J6" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6" s="88" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="88"/>
+      <c r="O6" s="88"/>
+      <c r="P6" s="73"/>
+    </row>
+    <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="77" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="77" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="77" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="P7" s="79" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A8" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="66">
+        <v>13300161702.799999</v>
+      </c>
+      <c r="C8" s="66">
+        <v>125241443.06</v>
+      </c>
+      <c r="D8" s="66">
+        <v>13677965368.200001</v>
+      </c>
+      <c r="E8" s="66">
+        <v>107651978.021</v>
+      </c>
+      <c r="F8" s="66">
+        <v>13946645014</v>
+      </c>
+      <c r="G8" s="66">
+        <v>1806520616.8599999</v>
+      </c>
+      <c r="H8" s="66">
+        <v>14593221457</v>
+      </c>
+      <c r="I8" s="66">
+        <v>2113898519.0799999</v>
+      </c>
+      <c r="J8" s="66">
+        <f>D8/B8</f>
+        <v>1.0284059452691063</v>
+      </c>
+      <c r="K8" s="66">
+        <f>F8/B8</f>
+        <v>1.0486071767882266</v>
+      </c>
+      <c r="L8" s="66">
+        <f>H8/B8</f>
+        <v>1.0972213558822959</v>
+      </c>
+      <c r="M8" s="66">
+        <f>C8/B8</f>
+        <v>9.4165353669071333E-3</v>
+      </c>
+      <c r="N8" s="66">
+        <f>E8/B8</f>
+        <v>8.0940352776565638E-3</v>
+      </c>
+      <c r="O8" s="66">
+        <f>G8/B8</f>
+        <v>0.13582696641046738</v>
+      </c>
+      <c r="P8" s="66">
+        <f>I8/B8</f>
+        <v>0.15893780589411738</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A9" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="66">
+        <v>338061420427</v>
+      </c>
+      <c r="C9" s="66">
+        <v>10187269073.299999</v>
+      </c>
+      <c r="D9" s="66">
+        <v>326696879273</v>
+      </c>
+      <c r="E9" s="66">
+        <v>4678703300.5900002</v>
+      </c>
+      <c r="F9" s="66">
+        <v>334503842865</v>
+      </c>
+      <c r="G9" s="66">
+        <v>13832307230.5</v>
+      </c>
+      <c r="H9" s="66">
+        <v>343959204435</v>
+      </c>
+      <c r="I9" s="66">
+        <v>19087632535.599998</v>
+      </c>
+      <c r="J9" s="66">
+        <f t="shared" ref="J9:J15" si="0">D9/B9</f>
+        <v>0.96638320592853921</v>
+      </c>
+      <c r="K9" s="66">
+        <f t="shared" ref="K9:K15" si="1">F9/B9</f>
+        <v>0.98947653489266396</v>
+      </c>
+      <c r="L9" s="66">
+        <f t="shared" ref="L9:L15" si="2">H9/B9</f>
+        <v>1.0174458948925631</v>
+      </c>
+      <c r="M9" s="66">
+        <f t="shared" ref="M9:M15" si="3">C9/B9</f>
+        <v>3.0134373394138325E-2</v>
+      </c>
+      <c r="N9" s="66">
+        <f t="shared" ref="N9:N15" si="4">E9/B9</f>
+        <v>1.3839802526654489E-2</v>
+      </c>
+      <c r="O9" s="66">
+        <f t="shared" ref="O9:O15" si="5">G9/B9</f>
+        <v>4.0916550646413995E-2</v>
+      </c>
+      <c r="P9" s="66">
+        <f t="shared" ref="P9:P15" si="6">I9/B9</f>
+        <v>5.6462025484868145E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A10" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="66">
+        <v>84120736.599999994</v>
+      </c>
+      <c r="C10" s="66">
+        <v>1942491.9396200001</v>
+      </c>
+      <c r="D10" s="66">
+        <v>54650354.399999999</v>
+      </c>
+      <c r="E10" s="66">
+        <v>2110333.1493700002</v>
+      </c>
+      <c r="F10" s="66">
+        <v>73058279</v>
+      </c>
+      <c r="G10" s="66">
+        <v>5535577.3796300003</v>
+      </c>
+      <c r="H10" s="66">
+        <v>48964596.799999997</v>
+      </c>
+      <c r="I10" s="66">
+        <v>6379096.9760699999</v>
+      </c>
+      <c r="J10" s="66">
+        <f t="shared" si="0"/>
+        <v>0.64966566638457135</v>
+      </c>
+      <c r="K10" s="66">
+        <f t="shared" si="1"/>
+        <v>0.86849309638593919</v>
+      </c>
+      <c r="L10" s="66">
+        <f t="shared" si="2"/>
+        <v>0.58207522638359777</v>
+      </c>
+      <c r="M10" s="66">
+        <f t="shared" si="3"/>
+        <v>2.3091713388776962E-2</v>
+      </c>
+      <c r="N10" s="66">
+        <f t="shared" si="4"/>
+        <v>2.5086955186861742E-2</v>
+      </c>
+      <c r="O10" s="66">
+        <f t="shared" si="5"/>
+        <v>6.5805146309548604E-2</v>
+      </c>
+      <c r="P10" s="66">
+        <f t="shared" si="6"/>
+        <v>7.5832633354163959E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A11" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="66">
+        <v>16749914.4</v>
+      </c>
+      <c r="C11" s="66">
+        <v>4948842.44814</v>
+      </c>
+      <c r="D11" s="66">
+        <v>7749925.4000000004</v>
+      </c>
+      <c r="E11" s="66">
+        <v>515495.68698100001</v>
+      </c>
+      <c r="F11" s="66">
+        <v>10514158.199999999</v>
+      </c>
+      <c r="G11" s="66">
+        <v>12573631.119999999</v>
+      </c>
+      <c r="H11" s="66">
+        <v>15665488.4</v>
+      </c>
+      <c r="I11" s="66">
+        <v>12819897.091499999</v>
+      </c>
+      <c r="J11" s="66">
+        <f t="shared" si="0"/>
+        <v>0.46268447795769035</v>
+      </c>
+      <c r="K11" s="66">
+        <f t="shared" si="1"/>
+        <v>0.62771414521378088</v>
+      </c>
+      <c r="L11" s="66">
+        <f t="shared" si="2"/>
+        <v>0.93525781839219424</v>
+      </c>
+      <c r="M11" s="66">
+        <f t="shared" si="3"/>
+        <v>0.29545479039224226</v>
+      </c>
+      <c r="N11" s="66">
+        <f t="shared" si="4"/>
+        <v>3.0776019188551794E-2</v>
+      </c>
+      <c r="O11" s="66">
+        <f t="shared" si="5"/>
+        <v>0.75066838072915754</v>
+      </c>
+      <c r="P11" s="66">
+        <f t="shared" si="6"/>
+        <v>0.76537090192532564</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A12" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="66">
+        <v>153785542243</v>
+      </c>
+      <c r="C12" s="66">
+        <v>190866239.28099999</v>
+      </c>
+      <c r="D12" s="66">
+        <v>152907857946</v>
+      </c>
+      <c r="E12" s="66">
+        <v>514095111.53100002</v>
+      </c>
+      <c r="F12" s="66">
+        <v>151698784971</v>
+      </c>
+      <c r="G12" s="66">
+        <v>1058535319.75</v>
+      </c>
+      <c r="H12" s="66">
+        <v>152793389151</v>
+      </c>
+      <c r="I12" s="66">
+        <v>529403644.43300003</v>
+      </c>
+      <c r="J12" s="66">
+        <f t="shared" si="0"/>
+        <v>0.99429280357438832</v>
+      </c>
+      <c r="K12" s="66">
+        <f t="shared" si="1"/>
+        <v>0.98643073177384477</v>
+      </c>
+      <c r="L12" s="66">
+        <f t="shared" si="2"/>
+        <v>0.99354846315505863</v>
+      </c>
+      <c r="M12" s="66">
+        <f t="shared" si="3"/>
+        <v>1.2411195259136125E-3</v>
+      </c>
+      <c r="N12" s="66">
+        <f t="shared" si="4"/>
+        <v>3.3429352592759779E-3</v>
+      </c>
+      <c r="O12" s="66">
+        <f t="shared" si="5"/>
+        <v>6.8831913865959162E-3</v>
+      </c>
+      <c r="P12" s="66">
+        <f t="shared" si="6"/>
+        <v>3.4424799412969354E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A13" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="66">
+        <v>4266685843.5999999</v>
+      </c>
+      <c r="C13" s="66">
+        <v>49406518.2016</v>
+      </c>
+      <c r="D13" s="66">
+        <v>3535419423.8000002</v>
+      </c>
+      <c r="E13" s="66">
+        <v>96266867.696799994</v>
+      </c>
+      <c r="F13" s="66">
+        <v>3874049893</v>
+      </c>
+      <c r="G13" s="66">
+        <v>34933171.063000001</v>
+      </c>
+      <c r="H13" s="66">
+        <v>2914015164.8000002</v>
+      </c>
+      <c r="I13" s="66">
+        <v>46608971.733800001</v>
+      </c>
+      <c r="J13" s="66">
+        <f t="shared" si="0"/>
+        <v>0.82861020318688461</v>
+      </c>
+      <c r="K13" s="66">
+        <f t="shared" si="1"/>
+        <v>0.90797636268699011</v>
+      </c>
+      <c r="L13" s="66">
+        <f t="shared" si="2"/>
+        <v>0.68296923458074688</v>
+      </c>
+      <c r="M13" s="66">
+        <f t="shared" si="3"/>
+        <v>1.1579600657899257E-2</v>
+      </c>
+      <c r="N13" s="66">
+        <f t="shared" si="4"/>
+        <v>2.2562445707410037E-2</v>
+      </c>
+      <c r="O13" s="66">
+        <f t="shared" si="5"/>
+        <v>8.1874251687406342E-3</v>
+      </c>
+      <c r="P13" s="66">
+        <f t="shared" si="6"/>
+        <v>1.0923928651487932E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A14" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="66">
+        <v>1427529350.4000001</v>
+      </c>
+      <c r="C14" s="66">
+        <v>54266504.609499998</v>
+      </c>
+      <c r="D14" s="66">
+        <v>978358233.20000005</v>
+      </c>
+      <c r="E14" s="66">
+        <v>29110680.692299999</v>
+      </c>
+      <c r="F14" s="66">
+        <v>466778888.39999998</v>
+      </c>
+      <c r="G14" s="66">
+        <v>24326412.497499999</v>
+      </c>
+      <c r="H14" s="66">
+        <v>846131783.39999998</v>
+      </c>
+      <c r="I14" s="66">
+        <v>601232379.42200005</v>
+      </c>
+      <c r="J14" s="66">
+        <f t="shared" si="0"/>
+        <v>0.68535069553971673</v>
+      </c>
+      <c r="K14" s="66">
+        <f t="shared" si="1"/>
+        <v>0.32698374171375633</v>
+      </c>
+      <c r="L14" s="66">
+        <f t="shared" si="2"/>
+        <v>0.59272461414745004</v>
+      </c>
+      <c r="M14" s="66">
+        <f t="shared" si="3"/>
+        <v>3.8014282924756879E-2</v>
+      </c>
+      <c r="N14" s="66">
+        <f t="shared" si="4"/>
+        <v>2.0392351781869184E-2</v>
+      </c>
+      <c r="O14" s="66">
+        <f t="shared" si="5"/>
+        <v>1.7040919327286425E-2</v>
+      </c>
+      <c r="P14" s="66">
+        <f t="shared" si="6"/>
+        <v>0.4211698899595529</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A15" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="66">
+        <v>218581302.80000001</v>
+      </c>
+      <c r="C15" s="66">
+        <v>1818257.88693</v>
+      </c>
+      <c r="D15" s="66">
+        <v>220467523.59999999</v>
+      </c>
+      <c r="E15" s="66">
+        <v>1871631.13164</v>
+      </c>
+      <c r="F15" s="66">
+        <v>213248411.40000001</v>
+      </c>
+      <c r="G15" s="66">
+        <v>3947465.8204199998</v>
+      </c>
+      <c r="H15" s="66">
+        <v>222067635.59999999</v>
+      </c>
+      <c r="I15" s="66">
+        <v>2133921.9328299998</v>
+      </c>
+      <c r="J15" s="66">
+        <f t="shared" si="0"/>
+        <v>1.008629378523404</v>
+      </c>
+      <c r="K15" s="66">
+        <f t="shared" si="1"/>
+        <v>0.97560225265525313</v>
+      </c>
+      <c r="L15" s="66">
+        <f t="shared" si="2"/>
+        <v>1.0159498216697425</v>
+      </c>
+      <c r="M15" s="66">
+        <f t="shared" si="3"/>
+        <v>8.3184511375782692E-3</v>
+      </c>
+      <c r="N15" s="66">
+        <f t="shared" si="4"/>
+        <v>8.562631422105331E-3</v>
+      </c>
+      <c r="O15" s="66">
+        <f t="shared" si="5"/>
+        <v>1.8059485280092307E-2</v>
+      </c>
+      <c r="P15" s="66">
+        <f t="shared" si="6"/>
+        <v>9.7626004854702506E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="M6:O6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819BCD50-CCED-4858-989E-30CB05A9C1BE}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14:P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4005,7 +7057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99183D17-15E5-4DA6-B476-6E21D829BB49}">
   <dimension ref="A1:P15"/>
   <sheetViews>
@@ -4668,12 +7720,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEB844F-EF6D-4427-9E28-001A58A9FD5B}">
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView topLeftCell="D6" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="N13" sqref="N13:P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5331,12 +8383,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65049047-28B8-4D24-A307-ABB41DE3392E}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6311,12 +9363,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51140CC8-C0B8-469A-8BAE-C9043CBCBC10}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView topLeftCell="E15" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView topLeftCell="D18" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26:P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7263,12 +10315,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD3A0CC-C87B-4B2D-914D-368FCFB476B0}">
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:P15"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7845,12 +10897,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1814E241-F455-4452-B5DE-B4EE59F14CFA}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:P15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N14" sqref="N14:P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8427,7 +11479,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC958D8-824A-4FFE-8EFB-EA4CAF2DCC74}">
   <dimension ref="A1:P12"/>
   <sheetViews>
@@ -8999,7 +12051,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F72758A-17BC-4C1E-98B0-DDD6331D597C}">
   <dimension ref="A1:P12"/>
   <sheetViews>
@@ -9569,374 +12621,6 @@
     <mergeCell ref="M3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C510FE-BA24-4F4C-B882-A73942D255FE}">
-  <dimension ref="A1:D31"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="27.3984375" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.19921875" customWidth="1"/>
-    <col min="4" max="4" width="27.265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="25" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="69" t="s">
-        <v>167</v>
-      </c>
-      <c r="C2" s="69" t="s">
-        <v>173</v>
-      </c>
-      <c r="D2" s="69" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" t="s">
-        <v>161</v>
-      </c>
-      <c r="C4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>163</v>
-      </c>
-      <c r="C6" t="s">
-        <v>163</v>
-      </c>
-      <c r="D6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>157</v>
-      </c>
-      <c r="B11" t="s">
-        <v>164</v>
-      </c>
-      <c r="C11" t="s">
-        <v>171</v>
-      </c>
-      <c r="D11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>158</v>
-      </c>
-      <c r="B13" t="s">
-        <v>165</v>
-      </c>
-      <c r="C13" t="s">
-        <v>165</v>
-      </c>
-      <c r="D13" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>159</v>
-      </c>
-      <c r="B14" t="s">
-        <v>166</v>
-      </c>
-      <c r="C14" t="s">
-        <v>172</v>
-      </c>
-      <c r="D14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A17" s="25" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="69" t="s">
-        <v>167</v>
-      </c>
-      <c r="C18" s="69" t="s">
-        <v>173</v>
-      </c>
-      <c r="D18" s="69" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>155</v>
-      </c>
-      <c r="B19" t="s">
-        <v>187</v>
-      </c>
-      <c r="C19" t="s">
-        <v>191</v>
-      </c>
-      <c r="D19" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" t="s">
-        <v>188</v>
-      </c>
-      <c r="C20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D20" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>184</v>
-      </c>
-      <c r="B21" t="s">
-        <v>156</v>
-      </c>
-      <c r="C21" t="s">
-        <v>193</v>
-      </c>
-      <c r="D21" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>185</v>
-      </c>
-      <c r="B27" t="s">
-        <v>189</v>
-      </c>
-      <c r="C27" t="s">
-        <v>194</v>
-      </c>
-      <c r="D27" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>158</v>
-      </c>
-      <c r="B29" t="s">
-        <v>165</v>
-      </c>
-      <c r="C29" t="s">
-        <v>165</v>
-      </c>
-      <c r="D29" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>186</v>
-      </c>
-      <c r="B30" t="s">
-        <v>190</v>
-      </c>
-      <c r="C30" t="s">
-        <v>195</v>
-      </c>
-      <c r="D30" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11803,6 +14487,374 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C510FE-BA24-4F4C-B882-A73942D255FE}">
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="27.3984375" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.19921875" customWidth="1"/>
+    <col min="4" max="4" width="27.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A1" s="25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="69" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="69" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" t="s">
+        <v>172</v>
+      </c>
+      <c r="D14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A17" s="25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="69" t="s">
+        <v>167</v>
+      </c>
+      <c r="C18" s="69" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" s="69" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" t="s">
+        <v>187</v>
+      </c>
+      <c r="C19" t="s">
+        <v>191</v>
+      </c>
+      <c r="D19" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" t="s">
+        <v>192</v>
+      </c>
+      <c r="D20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>184</v>
+      </c>
+      <c r="B21" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" t="s">
+        <v>193</v>
+      </c>
+      <c r="D21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B27" t="s">
+        <v>189</v>
+      </c>
+      <c r="C27" t="s">
+        <v>194</v>
+      </c>
+      <c r="D27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>158</v>
+      </c>
+      <c r="B29" t="s">
+        <v>165</v>
+      </c>
+      <c r="C29" t="s">
+        <v>165</v>
+      </c>
+      <c r="D29" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>186</v>
+      </c>
+      <c r="B30" t="s">
+        <v>190</v>
+      </c>
+      <c r="C30" t="s">
+        <v>195</v>
+      </c>
+      <c r="D30" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5A357B-AD95-4B57-AFAC-6E90E36724A8}">
   <dimension ref="A1:H59"/>
   <sheetViews>
@@ -16435,664 +19487,281 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638ACDA3-EFA6-47B5-8321-84E7AF859506}">
-  <dimension ref="A1:P15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DCC425-F9E0-4DC1-9C1B-7FD63E026DA8}">
+  <dimension ref="A2:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:I15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.46484375" customWidth="1"/>
+    <col min="2" max="2" width="13.06640625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.1328125" customWidth="1"/>
+    <col min="7" max="7" width="19.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A1" s="72" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A2" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A3" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A4" s="65"/>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
-      <c r="O4" s="65"/>
-      <c r="P4" s="65"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A5" s="65"/>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="65"/>
-    </row>
-    <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="73"/>
-      <c r="B6" s="88" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="91" t="s">
+        <v>206</v>
+      </c>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+    </row>
+    <row r="3" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="88"/>
-      <c r="H6" s="89" t="s">
-        <v>114</v>
-      </c>
-      <c r="I6" s="89"/>
-      <c r="J6" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="77" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" s="78" t="s">
-        <v>115</v>
-      </c>
-      <c r="M6" s="88" t="s">
-        <v>44</v>
-      </c>
-      <c r="N6" s="88"/>
-      <c r="O6" s="88"/>
-      <c r="P6" s="73"/>
-    </row>
-    <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="77" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="77" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="77" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" s="77" t="s">
-        <v>30</v>
-      </c>
-      <c r="O7" s="77" t="s">
-        <v>43</v>
-      </c>
-      <c r="P7" s="79" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A8" s="66" t="s">
+      <c r="C3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D3" s="90" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="90" t="s">
+        <v>204</v>
+      </c>
+      <c r="G3" s="90" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B8" s="66">
-        <v>13300161702.799999</v>
-      </c>
-      <c r="C8" s="66">
-        <v>125241443.06</v>
-      </c>
-      <c r="D8" s="66">
-        <v>13677965368.200001</v>
-      </c>
-      <c r="E8" s="66">
-        <v>107651978.021</v>
-      </c>
-      <c r="F8" s="66">
-        <v>13946645014</v>
-      </c>
-      <c r="G8" s="66">
-        <v>1806520616.8599999</v>
-      </c>
-      <c r="H8" s="66">
-        <v>14593221457</v>
-      </c>
-      <c r="I8" s="66">
-        <v>2113898519.0799999</v>
-      </c>
-      <c r="J8" s="66">
-        <f>D8/B8</f>
-        <v>1.0284059452691063</v>
-      </c>
-      <c r="K8" s="66">
-        <f>F8/B8</f>
-        <v>1.0486071767882266</v>
-      </c>
-      <c r="L8" s="66">
-        <f>H8/B8</f>
-        <v>1.0972213558822959</v>
-      </c>
-      <c r="M8" s="66">
-        <f>C8/B8</f>
-        <v>9.4165353669071333E-3</v>
-      </c>
-      <c r="N8" s="66">
-        <f>E8/B8</f>
-        <v>8.0940352776565638E-3</v>
-      </c>
-      <c r="O8" s="66">
-        <f>G8/B8</f>
-        <v>0.13582696641046738</v>
-      </c>
-      <c r="P8" s="66">
-        <f>I8/B8</f>
-        <v>0.15893780589411738</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A9" s="66" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="66">
-        <v>338061420427</v>
-      </c>
-      <c r="C9" s="66">
-        <v>10187269073.299999</v>
-      </c>
-      <c r="D9" s="66">
-        <v>326696879273</v>
-      </c>
-      <c r="E9" s="66">
-        <v>4678703300.5900002</v>
-      </c>
-      <c r="F9" s="66">
-        <v>334503842865</v>
-      </c>
-      <c r="G9" s="66">
-        <v>13832307230.5</v>
-      </c>
-      <c r="H9" s="66">
-        <v>343959204435</v>
-      </c>
-      <c r="I9" s="66">
-        <v>19087632535.599998</v>
-      </c>
-      <c r="J9" s="66">
-        <f t="shared" ref="J9:J15" si="0">D9/B9</f>
-        <v>0.96638320592853921</v>
-      </c>
-      <c r="K9" s="66">
-        <f t="shared" ref="K9:K15" si="1">F9/B9</f>
-        <v>0.98947653489266396</v>
-      </c>
-      <c r="L9" s="66">
-        <f t="shared" ref="L9:L15" si="2">H9/B9</f>
-        <v>1.0174458948925631</v>
-      </c>
-      <c r="M9" s="66">
-        <f t="shared" ref="M9:M15" si="3">C9/B9</f>
-        <v>3.0134373394138325E-2</v>
-      </c>
-      <c r="N9" s="66">
-        <f t="shared" ref="N9:N15" si="4">E9/B9</f>
-        <v>1.3839802526654489E-2</v>
-      </c>
-      <c r="O9" s="66">
-        <f t="shared" ref="O9:O15" si="5">G9/B9</f>
-        <v>4.0916550646413995E-2</v>
-      </c>
-      <c r="P9" s="66">
-        <f t="shared" ref="P9:P15" si="6">I9/B9</f>
-        <v>5.6462025484868145E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A10" s="66" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="66">
-        <v>84120736.599999994</v>
-      </c>
-      <c r="C10" s="66">
-        <v>1942491.9396200001</v>
-      </c>
-      <c r="D10" s="66">
-        <v>54650354.399999999</v>
-      </c>
-      <c r="E10" s="66">
-        <v>2110333.1493700002</v>
-      </c>
-      <c r="F10" s="66">
-        <v>73058279</v>
-      </c>
-      <c r="G10" s="66">
-        <v>5535577.3796300003</v>
-      </c>
-      <c r="H10" s="66">
-        <v>48964596.799999997</v>
-      </c>
-      <c r="I10" s="66">
-        <v>6379096.9760699999</v>
-      </c>
-      <c r="J10" s="66">
-        <f t="shared" si="0"/>
-        <v>0.64966566638457135</v>
-      </c>
-      <c r="K10" s="66">
-        <f t="shared" si="1"/>
-        <v>0.86849309638593919</v>
-      </c>
-      <c r="L10" s="66">
-        <f t="shared" si="2"/>
-        <v>0.58207522638359777</v>
-      </c>
-      <c r="M10" s="66">
-        <f t="shared" si="3"/>
-        <v>2.3091713388776962E-2</v>
-      </c>
-      <c r="N10" s="66">
-        <f t="shared" si="4"/>
-        <v>2.5086955186861742E-2</v>
-      </c>
-      <c r="O10" s="66">
-        <f t="shared" si="5"/>
-        <v>6.5805146309548604E-2</v>
-      </c>
-      <c r="P10" s="66">
-        <f t="shared" si="6"/>
-        <v>7.5832633354163959E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="B4" s="92">
+        <v>0.9356013083638639</v>
+      </c>
+      <c r="C4" s="92">
+        <v>0.29882809452770503</v>
+      </c>
+      <c r="D4" s="92">
+        <v>0.38405980306350745</v>
+      </c>
+      <c r="E4" s="92">
+        <v>3.4640422932770171E-2</v>
+      </c>
+      <c r="F4" s="92">
+        <v>1.2445591937164885E-2</v>
+      </c>
+      <c r="G4" s="92">
+        <v>1.0409780317991439E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="92">
+        <v>0.94469744673390132</v>
+      </c>
+      <c r="C5" s="92">
+        <v>0.29466756956271822</v>
+      </c>
+      <c r="D5" s="92">
+        <v>0.38277691547795289</v>
+      </c>
+      <c r="E5" s="92">
+        <v>9.8580753532644672E-3</v>
+      </c>
+      <c r="F5" s="92">
+        <v>9.6764378341133751E-3</v>
+      </c>
+      <c r="G5" s="92">
+        <v>4.9566377119578762E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6" s="92">
+        <v>0.87222223701487334</v>
+      </c>
+      <c r="C6" s="92">
+        <v>0.28024151734484376</v>
+      </c>
+      <c r="D6" s="92">
+        <v>0.37004112521020127</v>
+      </c>
+      <c r="E6" s="92">
+        <v>9.341955830266235E-3</v>
+      </c>
+      <c r="F6" s="92">
+        <v>8.2292052415342976E-3</v>
+      </c>
+      <c r="G6" s="92">
+        <v>7.8543122896674276E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7" s="92">
+        <v>0.90400805184937105</v>
+      </c>
+      <c r="C7" s="92">
+        <v>0.29114478875725908</v>
+      </c>
+      <c r="D7" s="92">
+        <v>0.36980716829392185</v>
+      </c>
+      <c r="E7" s="92">
+        <v>1.8841533980046916E-2</v>
+      </c>
+      <c r="F7" s="92">
+        <v>9.4314524537784418E-3</v>
+      </c>
+      <c r="G7" s="92">
+        <v>1.1562533614423927E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="66" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="66">
-        <v>16749914.4</v>
-      </c>
-      <c r="C11" s="66">
-        <v>4948842.44814</v>
-      </c>
-      <c r="D11" s="66">
-        <v>7749925.4000000004</v>
-      </c>
-      <c r="E11" s="66">
-        <v>515495.68698100001</v>
-      </c>
-      <c r="F11" s="66">
-        <v>10514158.199999999</v>
-      </c>
-      <c r="G11" s="66">
-        <v>12573631.119999999</v>
-      </c>
-      <c r="H11" s="66">
-        <v>15665488.4</v>
-      </c>
-      <c r="I11" s="66">
-        <v>12819897.091499999</v>
-      </c>
-      <c r="J11" s="66">
-        <f t="shared" si="0"/>
-        <v>0.46268447795769035</v>
-      </c>
-      <c r="K11" s="66">
-        <f t="shared" si="1"/>
-        <v>0.62771414521378088</v>
-      </c>
-      <c r="L11" s="66">
-        <f t="shared" si="2"/>
-        <v>0.93525781839219424</v>
-      </c>
-      <c r="M11" s="66">
-        <f t="shared" si="3"/>
-        <v>0.29545479039224226</v>
-      </c>
-      <c r="N11" s="66">
-        <f t="shared" si="4"/>
-        <v>3.0776019188551794E-2</v>
-      </c>
-      <c r="O11" s="66">
-        <f t="shared" si="5"/>
-        <v>0.75066838072915754</v>
-      </c>
-      <c r="P11" s="66">
-        <f t="shared" si="6"/>
-        <v>0.76537090192532564</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A12" s="66" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="66">
-        <v>153785542243</v>
-      </c>
-      <c r="C12" s="66">
-        <v>190866239.28099999</v>
-      </c>
-      <c r="D12" s="66">
-        <v>152907857946</v>
-      </c>
-      <c r="E12" s="66">
-        <v>514095111.53100002</v>
-      </c>
-      <c r="F12" s="66">
-        <v>151698784971</v>
-      </c>
-      <c r="G12" s="66">
-        <v>1058535319.75</v>
-      </c>
-      <c r="H12" s="66">
-        <v>152793389151</v>
-      </c>
-      <c r="I12" s="66">
-        <v>529403644.43300003</v>
-      </c>
-      <c r="J12" s="66">
-        <f t="shared" si="0"/>
-        <v>0.99429280357438832</v>
-      </c>
-      <c r="K12" s="66">
-        <f t="shared" si="1"/>
-        <v>0.98643073177384477</v>
-      </c>
-      <c r="L12" s="66">
-        <f t="shared" si="2"/>
-        <v>0.99354846315505863</v>
-      </c>
-      <c r="M12" s="66">
-        <f t="shared" si="3"/>
-        <v>1.2411195259136125E-3</v>
-      </c>
-      <c r="N12" s="66">
-        <f t="shared" si="4"/>
-        <v>3.3429352592759779E-3</v>
-      </c>
-      <c r="O12" s="66">
-        <f t="shared" si="5"/>
-        <v>6.8831913865959162E-3</v>
-      </c>
-      <c r="P12" s="66">
-        <f t="shared" si="6"/>
-        <v>3.4424799412969354E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A13" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="91" t="s">
+        <v>206</v>
+      </c>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
+    </row>
+    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A12" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="B12" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="D12" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="E12" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="90" t="s">
+        <v>204</v>
+      </c>
+      <c r="G12" s="90" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="65">
+        <v>1</v>
+      </c>
+      <c r="B13" s="92">
+        <v>0.96271978203603858</v>
+      </c>
+      <c r="C13" s="92">
+        <v>0.38730105438735418</v>
+      </c>
+      <c r="D13" s="92">
+        <v>0.36957921312384739</v>
+      </c>
+      <c r="E13" s="92">
+        <v>5.1252841937856744E-2</v>
+      </c>
+      <c r="F13" s="92">
+        <v>5.5295311611507636E-3</v>
+      </c>
+      <c r="G13" s="92">
+        <v>3.1795331807251317E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="65">
         <v>4</v>
       </c>
-      <c r="B13" s="66">
-        <v>4266685843.5999999</v>
-      </c>
-      <c r="C13" s="66">
-        <v>49406518.2016</v>
-      </c>
-      <c r="D13" s="66">
-        <v>3535419423.8000002</v>
-      </c>
-      <c r="E13" s="66">
-        <v>96266867.696799994</v>
-      </c>
-      <c r="F13" s="66">
-        <v>3874049893</v>
-      </c>
-      <c r="G13" s="66">
-        <v>34933171.063000001</v>
-      </c>
-      <c r="H13" s="66">
-        <v>2914015164.8000002</v>
-      </c>
-      <c r="I13" s="66">
-        <v>46608971.733800001</v>
-      </c>
-      <c r="J13" s="66">
-        <f t="shared" si="0"/>
-        <v>0.82861020318688461</v>
-      </c>
-      <c r="K13" s="66">
-        <f t="shared" si="1"/>
-        <v>0.90797636268699011</v>
-      </c>
-      <c r="L13" s="66">
-        <f t="shared" si="2"/>
-        <v>0.68296923458074688</v>
-      </c>
-      <c r="M13" s="66">
-        <f t="shared" si="3"/>
-        <v>1.1579600657899257E-2</v>
-      </c>
-      <c r="N13" s="66">
-        <f t="shared" si="4"/>
-        <v>2.2562445707410037E-2</v>
-      </c>
-      <c r="O13" s="66">
-        <f t="shared" si="5"/>
-        <v>8.1874251687406342E-3</v>
-      </c>
-      <c r="P13" s="66">
-        <f t="shared" si="6"/>
-        <v>1.0923928651487932E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A14" s="66" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="66">
-        <v>1427529350.4000001</v>
-      </c>
-      <c r="C14" s="66">
-        <v>54266504.609499998</v>
-      </c>
-      <c r="D14" s="66">
-        <v>978358233.20000005</v>
-      </c>
-      <c r="E14" s="66">
-        <v>29110680.692299999</v>
-      </c>
-      <c r="F14" s="66">
-        <v>466778888.39999998</v>
-      </c>
-      <c r="G14" s="66">
-        <v>24326412.497499999</v>
-      </c>
-      <c r="H14" s="66">
-        <v>846131783.39999998</v>
-      </c>
-      <c r="I14" s="66">
-        <v>601232379.42200005</v>
-      </c>
-      <c r="J14" s="66">
-        <f t="shared" si="0"/>
-        <v>0.68535069553971673</v>
-      </c>
-      <c r="K14" s="66">
-        <f t="shared" si="1"/>
-        <v>0.32698374171375633</v>
-      </c>
-      <c r="L14" s="66">
-        <f t="shared" si="2"/>
-        <v>0.59272461414745004</v>
-      </c>
-      <c r="M14" s="66">
-        <f t="shared" si="3"/>
-        <v>3.8014282924756879E-2</v>
-      </c>
-      <c r="N14" s="66">
-        <f t="shared" si="4"/>
-        <v>2.0392351781869184E-2</v>
-      </c>
-      <c r="O14" s="66">
-        <f t="shared" si="5"/>
-        <v>1.7040919327286425E-2</v>
-      </c>
-      <c r="P14" s="66">
-        <f t="shared" si="6"/>
-        <v>0.4211698899595529</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A15" s="66" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="66">
-        <v>218581302.80000001</v>
-      </c>
-      <c r="C15" s="66">
-        <v>1818257.88693</v>
-      </c>
-      <c r="D15" s="66">
-        <v>220467523.59999999</v>
-      </c>
-      <c r="E15" s="66">
-        <v>1871631.13164</v>
-      </c>
-      <c r="F15" s="66">
-        <v>213248411.40000001</v>
-      </c>
-      <c r="G15" s="66">
-        <v>3947465.8204199998</v>
-      </c>
-      <c r="H15" s="66">
-        <v>222067635.59999999</v>
-      </c>
-      <c r="I15" s="66">
-        <v>2133921.9328299998</v>
-      </c>
-      <c r="J15" s="66">
-        <f t="shared" si="0"/>
-        <v>1.008629378523404</v>
-      </c>
-      <c r="K15" s="66">
-        <f t="shared" si="1"/>
-        <v>0.97560225265525313</v>
-      </c>
-      <c r="L15" s="66">
-        <f t="shared" si="2"/>
-        <v>1.0159498216697425</v>
-      </c>
-      <c r="M15" s="66">
-        <f t="shared" si="3"/>
-        <v>8.3184511375782692E-3</v>
-      </c>
-      <c r="N15" s="66">
-        <f t="shared" si="4"/>
-        <v>8.562631422105331E-3</v>
-      </c>
-      <c r="O15" s="66">
-        <f t="shared" si="5"/>
-        <v>1.8059485280092307E-2</v>
-      </c>
-      <c r="P15" s="66">
-        <f t="shared" si="6"/>
-        <v>9.7626004854702506E-3</v>
+      <c r="B14" s="92">
+        <v>0.9442762311353079</v>
+      </c>
+      <c r="C14" s="92">
+        <v>0.41434324900610719</v>
+      </c>
+      <c r="D14" s="92">
+        <v>0.40083074332271823</v>
+      </c>
+      <c r="E14" s="92">
+        <v>8.5005017896467427E-3</v>
+      </c>
+      <c r="F14" s="92">
+        <v>6.0953616896922656E-3</v>
+      </c>
+      <c r="G14" s="92">
+        <v>2.0913418320206361E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="65">
+        <v>8</v>
+      </c>
+      <c r="B15" s="92">
+        <v>0.86439751671266363</v>
+      </c>
+      <c r="C15" s="92">
+        <v>0.41517545864783562</v>
+      </c>
+      <c r="D15" s="92">
+        <v>0.42928869176101703</v>
+      </c>
+      <c r="E15" s="92">
+        <v>1.0873531107782013E-2</v>
+      </c>
+      <c r="F15" s="92">
+        <v>4.5428457859383424E-3</v>
+      </c>
+      <c r="G15" s="92">
+        <v>3.2045527585561561E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="65">
+        <v>12</v>
+      </c>
+      <c r="B16" s="92">
+        <v>0.91955706039378737</v>
+      </c>
+      <c r="C16" s="92">
+        <v>0.44375153500032488</v>
+      </c>
+      <c r="D16" s="92">
+        <v>0.4494151032037067</v>
+      </c>
+      <c r="E16" s="92">
+        <v>2.0072354924216499E-2</v>
+      </c>
+      <c r="F16" s="92">
+        <v>9.5140644989271071E-3</v>
+      </c>
+      <c r="G16" s="92">
+        <v>1.2858348739257596E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="M6:O6"/>
+  <mergeCells count="2">
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added results for SPECjvm2008 derby
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="81D8B261ABBD5CBDED69DEB44BA5B0CD337C6AB9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{4C5B0F60-B89A-477E-BCF4-1ADBD8CC82DC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -15,21 +16,22 @@
     <sheet name="clang-2core-os" sheetId="15" r:id="rId6"/>
     <sheet name="clang-2core-usr" sheetId="16" r:id="rId7"/>
     <sheet name="clang-stats" sheetId="17" r:id="rId8"/>
-    <sheet name="postgres summary" sheetId="27" r:id="rId9"/>
-    <sheet name="postgres-12GB-os" sheetId="25" r:id="rId10"/>
-    <sheet name="postgres-12GB-usr" sheetId="26" r:id="rId11"/>
-    <sheet name="postgres-10GB-os" sheetId="28" r:id="rId12"/>
-    <sheet name="postgres-10GB-usr" sheetId="29" r:id="rId13"/>
-    <sheet name="postgres-8GB-os" sheetId="23" r:id="rId14"/>
-    <sheet name="postgres-8GB-usr" sheetId="24" r:id="rId15"/>
-    <sheet name="postgres-4GB-os" sheetId="11" r:id="rId16"/>
-    <sheet name="postgres-4GB-usr" sheetId="8" r:id="rId17"/>
-    <sheet name="postgres-1GB-os" sheetId="18" r:id="rId18"/>
-    <sheet name="postgres-1GB-usr" sheetId="19" r:id="rId19"/>
-    <sheet name="octane-os" sheetId="20" r:id="rId20"/>
-    <sheet name="octane-usr" sheetId="21" r:id="rId21"/>
-    <sheet name="octane-stats" sheetId="22" r:id="rId22"/>
-    <sheet name="postgres_stats" sheetId="9" r:id="rId23"/>
+    <sheet name="SPECjvm2008-derby" sheetId="30" r:id="rId9"/>
+    <sheet name="postgres summary" sheetId="27" r:id="rId10"/>
+    <sheet name="postgres-12GB-os" sheetId="25" r:id="rId11"/>
+    <sheet name="postgres-12GB-usr" sheetId="26" r:id="rId12"/>
+    <sheet name="postgres-10GB-os" sheetId="28" r:id="rId13"/>
+    <sheet name="postgres-10GB-usr" sheetId="29" r:id="rId14"/>
+    <sheet name="postgres-8GB-os" sheetId="23" r:id="rId15"/>
+    <sheet name="postgres-8GB-usr" sheetId="24" r:id="rId16"/>
+    <sheet name="postgres-4GB-os" sheetId="11" r:id="rId17"/>
+    <sheet name="postgres-4GB-usr" sheetId="8" r:id="rId18"/>
+    <sheet name="postgres-1GB-os" sheetId="18" r:id="rId19"/>
+    <sheet name="postgres-1GB-usr" sheetId="19" r:id="rId20"/>
+    <sheet name="octane-os" sheetId="20" r:id="rId21"/>
+    <sheet name="octane-usr" sheetId="21" r:id="rId22"/>
+    <sheet name="octane-stats" sheetId="22" r:id="rId23"/>
+    <sheet name="postgres_stats" sheetId="9" r:id="rId24"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="213">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -697,6 +699,15 @@
   <si>
     <t>10GB/2MB * 2 # of super pages for each iteration</t>
   </si>
+  <si>
+    <t>java -jar SPECjvm2008.jar -ikv derby -ctf false -chf false</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>USR</t>
+  </si>
 </sst>
 </file>
 
@@ -922,7 +933,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1066,6 +1077,10 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1087,19 +1102,22 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3812,22 +3830,22 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="57" x14ac:dyDescent="0.45">
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="85"/>
+      <c r="D3" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83" t="s">
+      <c r="E3" s="85"/>
+      <c r="F3" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="83"/>
-      <c r="H3" s="84" t="s">
+      <c r="G3" s="85"/>
+      <c r="H3" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="85"/>
+      <c r="I3" s="87"/>
       <c r="J3" s="33" t="s">
         <v>45</v>
       </c>
@@ -3837,12 +3855,12 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="83" t="s">
+      <c r="M3" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="83"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
     </row>
     <row r="4" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
@@ -5787,11 +5805,337 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DCC425-F9E0-4DC1-9C1B-7FD63E026DA8}">
+  <dimension ref="A2:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="19.46484375" customWidth="1"/>
+    <col min="2" max="2" width="13.06640625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.1328125" customWidth="1"/>
+    <col min="7" max="7" width="19.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="92" t="s">
+        <v>206</v>
+      </c>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+    </row>
+    <row r="3" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D3" s="83" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="83" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="83" t="s">
+        <v>204</v>
+      </c>
+      <c r="G3" s="83" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="84">
+        <v>0.9356013083638639</v>
+      </c>
+      <c r="C4" s="84">
+        <v>0.29882809452770503</v>
+      </c>
+      <c r="D4" s="84">
+        <v>0.38405980306350745</v>
+      </c>
+      <c r="E4" s="84">
+        <v>3.4640422932770171E-2</v>
+      </c>
+      <c r="F4" s="84">
+        <v>1.2445591937164885E-2</v>
+      </c>
+      <c r="G4" s="84">
+        <v>1.0409780317991439E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="84">
+        <v>0.94469744673390132</v>
+      </c>
+      <c r="C5" s="84">
+        <v>0.29466756956271822</v>
+      </c>
+      <c r="D5" s="84">
+        <v>0.38277691547795289</v>
+      </c>
+      <c r="E5" s="84">
+        <v>9.8580753532644672E-3</v>
+      </c>
+      <c r="F5" s="84">
+        <v>9.6764378341133751E-3</v>
+      </c>
+      <c r="G5" s="84">
+        <v>4.9566377119578762E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6" s="84">
+        <v>0.87222223701487334</v>
+      </c>
+      <c r="C6" s="84">
+        <v>0.28024151734484376</v>
+      </c>
+      <c r="D6" s="84">
+        <v>0.37004112521020127</v>
+      </c>
+      <c r="E6" s="84">
+        <v>9.341955830266235E-3</v>
+      </c>
+      <c r="F6" s="84">
+        <v>8.2292052415342976E-3</v>
+      </c>
+      <c r="G6" s="84">
+        <v>7.8543122896674276E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" s="84">
+        <v>0.8835802154119029</v>
+      </c>
+      <c r="C7" s="84">
+        <v>0.2790662450692325</v>
+      </c>
+      <c r="D7" s="84">
+        <v>0.36589759015925816</v>
+      </c>
+      <c r="E7" s="84">
+        <v>1.78778409257737E-2</v>
+      </c>
+      <c r="F7" s="84">
+        <v>3.6076317302390845E-3</v>
+      </c>
+      <c r="G7" s="84">
+        <v>3.7763396325711275E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8" s="84">
+        <v>0.90400805184937105</v>
+      </c>
+      <c r="C8" s="84">
+        <v>0.29114478875725908</v>
+      </c>
+      <c r="D8" s="84">
+        <v>0.36980716829392185</v>
+      </c>
+      <c r="E8" s="84">
+        <v>1.8841533980046916E-2</v>
+      </c>
+      <c r="F8" s="84">
+        <v>9.4314524537784418E-3</v>
+      </c>
+      <c r="G8" s="84">
+        <v>1.1562533614423927E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="92" t="s">
+        <v>206</v>
+      </c>
+      <c r="F11" s="92"/>
+      <c r="G11" s="92"/>
+    </row>
+    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A12" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="B12" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="D12" s="83" t="s">
+        <v>207</v>
+      </c>
+      <c r="E12" s="83" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="83" t="s">
+        <v>204</v>
+      </c>
+      <c r="G12" s="83" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="65">
+        <v>1</v>
+      </c>
+      <c r="B13" s="84">
+        <v>0.96271978203603858</v>
+      </c>
+      <c r="C13" s="84">
+        <v>0.38730105438735418</v>
+      </c>
+      <c r="D13" s="84">
+        <v>0.36957921312384739</v>
+      </c>
+      <c r="E13" s="84">
+        <v>5.1252841937856744E-2</v>
+      </c>
+      <c r="F13" s="84">
+        <v>5.5295311611507636E-3</v>
+      </c>
+      <c r="G13" s="84">
+        <v>3.1795331807251317E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="65">
+        <v>4</v>
+      </c>
+      <c r="B14" s="84">
+        <v>0.9442762311353079</v>
+      </c>
+      <c r="C14" s="84">
+        <v>0.41434324900610719</v>
+      </c>
+      <c r="D14" s="84">
+        <v>0.40083074332271823</v>
+      </c>
+      <c r="E14" s="84">
+        <v>8.5005017896467427E-3</v>
+      </c>
+      <c r="F14" s="84">
+        <v>6.0953616896922656E-3</v>
+      </c>
+      <c r="G14" s="84">
+        <v>2.0913418320206361E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="65">
+        <v>8</v>
+      </c>
+      <c r="B15" s="84">
+        <v>0.86439751671266363</v>
+      </c>
+      <c r="C15" s="84">
+        <v>0.41517545864783562</v>
+      </c>
+      <c r="D15" s="84">
+        <v>0.42928869176101703</v>
+      </c>
+      <c r="E15" s="84">
+        <v>1.0873531107782013E-2</v>
+      </c>
+      <c r="F15" s="84">
+        <v>4.5428457859383424E-3</v>
+      </c>
+      <c r="G15" s="84">
+        <v>3.2045527585561561E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" s="84">
+        <v>0.87182608862774247</v>
+      </c>
+      <c r="C16" s="84">
+        <v>0.4396266532861684</v>
+      </c>
+      <c r="D16" s="84">
+        <v>0.40648641375508454</v>
+      </c>
+      <c r="E16" s="84">
+        <v>2.966505280632557E-2</v>
+      </c>
+      <c r="F16" s="84">
+        <v>3.8832662288856685E-3</v>
+      </c>
+      <c r="G16" s="84">
+        <v>1.9088334041327464E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="65">
+        <v>12</v>
+      </c>
+      <c r="B17" s="84">
+        <v>0.91955706039378737</v>
+      </c>
+      <c r="C17" s="84">
+        <v>0.44375153500032488</v>
+      </c>
+      <c r="D17" s="84">
+        <v>0.4494151032037067</v>
+      </c>
+      <c r="E17" s="84">
+        <v>2.0072354924216499E-2</v>
+      </c>
+      <c r="F17" s="84">
+        <v>9.5140644989271071E-3</v>
+      </c>
+      <c r="G17" s="84">
+        <v>1.2858348739257596E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E11:G11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638ACDA3-EFA6-47B5-8321-84E7AF859506}">
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P7"/>
+      <selection activeCell="A6" sqref="A6:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5905,22 +6249,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90" t="s">
+      <c r="C6" s="93"/>
+      <c r="D6" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90" t="s">
+      <c r="E6" s="93"/>
+      <c r="F6" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="90"/>
-      <c r="H6" s="91" t="s">
+      <c r="G6" s="93"/>
+      <c r="H6" s="94" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="91"/>
+      <c r="I6" s="94"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -5930,11 +6274,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="90" t="s">
+      <c r="M6" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="90"/>
-      <c r="O6" s="90"/>
+      <c r="N6" s="93"/>
+      <c r="O6" s="93"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -5983,7 +6327,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" s="66" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B8" s="66">
         <v>13300161702.799999</v>
@@ -6211,7 +6555,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" s="66" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B12" s="66">
         <v>153785542243</v>
@@ -6449,12 +6793,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819BCD50-CCED-4858-989E-30CB05A9C1BE}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:T15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6648,7 +6992,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" s="66" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B8" s="66">
         <v>51992876606.199997</v>
@@ -6876,7 +7220,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" s="66" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B12" s="66">
         <v>950956907531</v>
@@ -7107,12 +7451,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E2C13C-499C-4223-89FD-CBE0858897C8}">
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="A8" sqref="A8:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7332,7 +7676,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A8" s="66" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B8" s="66">
         <v>13262885030.6</v>
@@ -7576,7 +7920,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A12" s="66" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B12" s="66">
         <v>153829362033</v>
@@ -7823,12 +8167,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD324841-F3D6-48B1-BFDE-305D75F58DD9}">
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14:P14"/>
+      <selection activeCell="A8" sqref="A8:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8048,7 +8392,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A8" s="66" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B8" s="66">
         <v>52469169049.800003</v>
@@ -8292,7 +8636,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A12" s="66" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B12" s="66">
         <v>950995779400</v>
@@ -8539,11 +8883,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99183D17-15E5-4DA6-B476-6E21D829BB49}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:P15"/>
     </sheetView>
   </sheetViews>
@@ -8658,22 +9002,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90" t="s">
+      <c r="C6" s="93"/>
+      <c r="D6" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90" t="s">
+      <c r="E6" s="93"/>
+      <c r="F6" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="90"/>
-      <c r="H6" s="91" t="s">
+      <c r="G6" s="93"/>
+      <c r="H6" s="94" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="91"/>
+      <c r="I6" s="94"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -8683,11 +9027,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="90" t="s">
+      <c r="M6" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="90"/>
-      <c r="O6" s="90"/>
+      <c r="N6" s="93"/>
+      <c r="O6" s="93"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -9202,11 +9546,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEB844F-EF6D-4427-9E28-001A58A9FD5B}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView topLeftCell="D6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="N13" sqref="N13:P13"/>
     </sheetView>
   </sheetViews>
@@ -9321,22 +9665,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90" t="s">
+      <c r="C6" s="93"/>
+      <c r="D6" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90" t="s">
+      <c r="E6" s="93"/>
+      <c r="F6" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="90"/>
-      <c r="H6" s="91" t="s">
+      <c r="G6" s="93"/>
+      <c r="H6" s="94" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="91"/>
+      <c r="I6" s="94"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -9346,11 +9690,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="90" t="s">
+      <c r="M6" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="90"/>
-      <c r="O6" s="90"/>
+      <c r="N6" s="93"/>
+      <c r="O6" s="93"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -9865,12 +10209,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65049047-28B8-4D24-A307-ABB41DE3392E}">
   <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9968,22 +10312,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86" t="s">
+      <c r="C6" s="88"/>
+      <c r="D6" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="86"/>
-      <c r="F6" s="87" t="s">
+      <c r="E6" s="88"/>
+      <c r="F6" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="86"/>
-      <c r="H6" s="84" t="s">
+      <c r="G6" s="88"/>
+      <c r="H6" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="85"/>
+      <c r="I6" s="87"/>
       <c r="J6" s="7" t="s">
         <v>45</v>
       </c>
@@ -9993,11 +10337,11 @@
       <c r="L6" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="87" t="s">
+      <c r="M6" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="86"/>
-      <c r="O6" s="86"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="88"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
@@ -10297,22 +10641,22 @@
     </row>
     <row r="19" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A19" s="2"/>
-      <c r="B19" s="86" t="s">
+      <c r="B19" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86" t="s">
+      <c r="C19" s="88"/>
+      <c r="D19" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="86"/>
-      <c r="F19" s="87" t="s">
+      <c r="E19" s="88"/>
+      <c r="F19" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="86"/>
-      <c r="H19" s="84" t="s">
+      <c r="G19" s="88"/>
+      <c r="H19" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="I19" s="85"/>
+      <c r="I19" s="87"/>
       <c r="J19" s="67" t="s">
         <v>45</v>
       </c>
@@ -10322,11 +10666,11 @@
       <c r="L19" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="M19" s="87" t="s">
+      <c r="M19" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="N19" s="86"/>
-      <c r="O19" s="86"/>
+      <c r="N19" s="88"/>
+      <c r="O19" s="88"/>
     </row>
     <row r="20" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
@@ -10845,11 +11189,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51140CC8-C0B8-469A-8BAE-C9043CBCBC10}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView topLeftCell="D18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="N26" sqref="N26:P26"/>
     </sheetView>
   </sheetViews>
@@ -10892,22 +11236,22 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90" t="s">
+      <c r="C6" s="93"/>
+      <c r="D6" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90" t="s">
+      <c r="E6" s="93"/>
+      <c r="F6" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="90"/>
-      <c r="H6" s="91" t="s">
+      <c r="G6" s="93"/>
+      <c r="H6" s="94" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="91"/>
+      <c r="I6" s="94"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -10917,11 +11261,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="90" t="s">
+      <c r="M6" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="90"/>
-      <c r="O6" s="90"/>
+      <c r="N6" s="93"/>
+      <c r="O6" s="93"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A7" s="77" t="s">
@@ -11250,22 +11594,22 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B18" s="90" t="s">
+      <c r="B18" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="90"/>
-      <c r="D18" s="90" t="s">
+      <c r="C18" s="93"/>
+      <c r="D18" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="90"/>
-      <c r="F18" s="90" t="s">
+      <c r="E18" s="93"/>
+      <c r="F18" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="90"/>
-      <c r="H18" s="91" t="s">
+      <c r="G18" s="93"/>
+      <c r="H18" s="94" t="s">
         <v>114</v>
       </c>
-      <c r="I18" s="91"/>
+      <c r="I18" s="94"/>
       <c r="J18" s="77" t="s">
         <v>45</v>
       </c>
@@ -11275,11 +11619,11 @@
       <c r="L18" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M18" s="90" t="s">
+      <c r="M18" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="N18" s="90"/>
-      <c r="O18" s="90"/>
+      <c r="N18" s="93"/>
+      <c r="O18" s="93"/>
     </row>
     <row r="19" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A19" s="77" t="s">
@@ -11797,7 +12141,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD3A0CC-C87B-4B2D-914D-368FCFB476B0}">
   <dimension ref="A1:P15"/>
   <sheetViews>
@@ -11835,22 +12179,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90" t="s">
+      <c r="C6" s="93"/>
+      <c r="D6" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90" t="s">
+      <c r="E6" s="93"/>
+      <c r="F6" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="90"/>
-      <c r="H6" s="91" t="s">
+      <c r="G6" s="93"/>
+      <c r="H6" s="94" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="91"/>
+      <c r="I6" s="94"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -11860,11 +12204,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="90" t="s">
+      <c r="M6" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="90"/>
-      <c r="O6" s="90"/>
+      <c r="N6" s="93"/>
+      <c r="O6" s="93"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -12365,588 +12709,6 @@
       <c r="P15" s="66">
         <f t="shared" si="6"/>
         <v>2.5963681417960943E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="M6:O6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1814E241-F455-4452-B5DE-B4EE59F14CFA}">
-  <dimension ref="A1:P15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14:P14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="32.265625" customWidth="1"/>
-    <col min="2" max="2" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.9296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.9296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.46484375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.9296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A1" s="72" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A2" s="72" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A3" s="73" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="73"/>
-      <c r="B6" s="90" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="90"/>
-      <c r="H6" s="91" t="s">
-        <v>114</v>
-      </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="77" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" s="78" t="s">
-        <v>115</v>
-      </c>
-      <c r="M6" s="90" t="s">
-        <v>44</v>
-      </c>
-      <c r="N6" s="90"/>
-      <c r="O6" s="90"/>
-      <c r="P6" s="73"/>
-    </row>
-    <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="77" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="77" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="77" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" s="77" t="s">
-        <v>30</v>
-      </c>
-      <c r="O7" s="77" t="s">
-        <v>43</v>
-      </c>
-      <c r="P7" s="79" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A8" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="66">
-        <v>927274396101</v>
-      </c>
-      <c r="C8" s="66">
-        <v>2252129313.96</v>
-      </c>
-      <c r="D8" s="66">
-        <v>928584523878</v>
-      </c>
-      <c r="E8" s="66">
-        <v>6426468418.3100004</v>
-      </c>
-      <c r="F8" s="66">
-        <v>935859695818</v>
-      </c>
-      <c r="G8" s="66">
-        <v>1303543522.45</v>
-      </c>
-      <c r="H8" s="66">
-        <v>931436628179</v>
-      </c>
-      <c r="I8" s="66">
-        <v>5821397551.7399998</v>
-      </c>
-      <c r="J8" s="66">
-        <f>D8/B8</f>
-        <v>1.0014128803539804</v>
-      </c>
-      <c r="K8" s="66">
-        <f>F8/B8</f>
-        <v>1.0092586398946195</v>
-      </c>
-      <c r="L8" s="66">
-        <f>H8/B8</f>
-        <v>1.0044886735744041</v>
-      </c>
-      <c r="M8" s="66">
-        <f>C8/B8</f>
-        <v>2.4287625361271111E-3</v>
-      </c>
-      <c r="N8" s="66">
-        <f>E8/B8</f>
-        <v>6.93049268407711E-3</v>
-      </c>
-      <c r="O8" s="66">
-        <f>G8/B8</f>
-        <v>1.4057797000878436E-3</v>
-      </c>
-      <c r="P8" s="66">
-        <f>I8/B8</f>
-        <v>6.2779664533149961E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A9" s="66" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="66">
-        <v>1167899698070</v>
-      </c>
-      <c r="C9" s="66">
-        <v>1572343407.77</v>
-      </c>
-      <c r="D9" s="66">
-        <v>1178943655390</v>
-      </c>
-      <c r="E9" s="66">
-        <v>10362118961.700001</v>
-      </c>
-      <c r="F9" s="66">
-        <v>1129500984560</v>
-      </c>
-      <c r="G9" s="66">
-        <v>944174208.25399995</v>
-      </c>
-      <c r="H9" s="66">
-        <v>1133772596540</v>
-      </c>
-      <c r="I9" s="66">
-        <v>8461901884.1800003</v>
-      </c>
-      <c r="J9" s="66">
-        <f t="shared" ref="J9:J15" si="0">D9/B9</f>
-        <v>1.0094562549662873</v>
-      </c>
-      <c r="K9" s="66">
-        <f t="shared" ref="K9:K15" si="1">F9/B9</f>
-        <v>0.9671215656845743</v>
-      </c>
-      <c r="L9" s="66">
-        <f t="shared" ref="L9:L15" si="2">H9/B9</f>
-        <v>0.97077908181122374</v>
-      </c>
-      <c r="M9" s="66">
-        <f t="shared" ref="M9:M15" si="3">C9/B9</f>
-        <v>1.346300037895685E-3</v>
-      </c>
-      <c r="N9" s="66">
-        <f t="shared" ref="N9:N15" si="4">E9/B9</f>
-        <v>8.8724391134134273E-3</v>
-      </c>
-      <c r="O9" s="66">
-        <f t="shared" ref="O9:O15" si="5">G9/B9</f>
-        <v>8.0843775352822231E-4</v>
-      </c>
-      <c r="P9" s="66">
-        <f t="shared" ref="P9:P15" si="6">I9/B9</f>
-        <v>7.2454012088226626E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A10" s="66" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="66">
-        <v>368205228.60000002</v>
-      </c>
-      <c r="C10" s="66">
-        <v>6887574.7414600002</v>
-      </c>
-      <c r="D10" s="66">
-        <v>362294137.80000001</v>
-      </c>
-      <c r="E10" s="66">
-        <v>20204685.2766</v>
-      </c>
-      <c r="F10" s="66">
-        <v>88088658.400000006</v>
-      </c>
-      <c r="G10" s="66">
-        <v>9483474.11558</v>
-      </c>
-      <c r="H10" s="66">
-        <v>108439750</v>
-      </c>
-      <c r="I10" s="66">
-        <v>3555898.5149500002</v>
-      </c>
-      <c r="J10" s="66">
-        <f t="shared" si="0"/>
-        <v>0.98394620624352536</v>
-      </c>
-      <c r="K10" s="66">
-        <f t="shared" si="1"/>
-        <v>0.23923793460221385</v>
-      </c>
-      <c r="L10" s="66">
-        <f t="shared" si="2"/>
-        <v>0.29450899003339137</v>
-      </c>
-      <c r="M10" s="66">
-        <f t="shared" si="3"/>
-        <v>1.8705803737899446E-2</v>
-      </c>
-      <c r="N10" s="66">
-        <f t="shared" si="4"/>
-        <v>5.4873433909189195E-2</v>
-      </c>
-      <c r="O10" s="66">
-        <f t="shared" si="5"/>
-        <v>2.5755946355347326E-2</v>
-      </c>
-      <c r="P10" s="66">
-        <f t="shared" si="6"/>
-        <v>9.6573819129900321E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A11" s="66" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="66">
-        <v>174362730.59999999</v>
-      </c>
-      <c r="C11" s="66">
-        <v>2663219.4407000002</v>
-      </c>
-      <c r="D11" s="66">
-        <v>168909930.40000001</v>
-      </c>
-      <c r="E11" s="66">
-        <v>13591693.936100001</v>
-      </c>
-      <c r="F11" s="66">
-        <v>61109618.799999997</v>
-      </c>
-      <c r="G11" s="66">
-        <v>1312040.0078100001</v>
-      </c>
-      <c r="H11" s="66">
-        <v>54860028.799999997</v>
-      </c>
-      <c r="I11" s="66">
-        <v>2739627.79629</v>
-      </c>
-      <c r="J11" s="66">
-        <f t="shared" si="0"/>
-        <v>0.96872726080145488</v>
-      </c>
-      <c r="K11" s="66">
-        <f t="shared" si="1"/>
-        <v>0.35047408692049925</v>
-      </c>
-      <c r="L11" s="66">
-        <f t="shared" si="2"/>
-        <v>0.31463162231527936</v>
-      </c>
-      <c r="M11" s="66">
-        <f t="shared" si="3"/>
-        <v>1.527401774183961E-2</v>
-      </c>
-      <c r="N11" s="66">
-        <f t="shared" si="4"/>
-        <v>7.7950682977546815E-2</v>
-      </c>
-      <c r="O11" s="66">
-        <f t="shared" si="5"/>
-        <v>7.5247732316139817E-3</v>
-      </c>
-      <c r="P11" s="66">
-        <f t="shared" si="6"/>
-        <v>1.5712232693664872E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A12" s="66" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="66">
-        <v>50721089984.400002</v>
-      </c>
-      <c r="C12" s="66">
-        <v>327032611.59600002</v>
-      </c>
-      <c r="D12" s="66">
-        <v>49851101330.800003</v>
-      </c>
-      <c r="E12" s="66">
-        <v>853331810.60500002</v>
-      </c>
-      <c r="F12" s="66">
-        <v>51061339932.400002</v>
-      </c>
-      <c r="G12" s="66">
-        <v>257035844.535</v>
-      </c>
-      <c r="H12" s="66">
-        <v>49624355425.800003</v>
-      </c>
-      <c r="I12" s="66">
-        <v>1672872144.6199999</v>
-      </c>
-      <c r="J12" s="66">
-        <f t="shared" si="0"/>
-        <v>0.98284759547029499</v>
-      </c>
-      <c r="K12" s="66">
-        <f t="shared" si="1"/>
-        <v>1.0067082538664813</v>
-      </c>
-      <c r="L12" s="66">
-        <f t="shared" si="2"/>
-        <v>0.97837714925019725</v>
-      </c>
-      <c r="M12" s="66">
-        <f t="shared" si="3"/>
-        <v>6.4476652945862087E-3</v>
-      </c>
-      <c r="N12" s="66">
-        <f t="shared" si="4"/>
-        <v>1.6824003799355544E-2</v>
-      </c>
-      <c r="O12" s="66">
-        <f t="shared" si="5"/>
-        <v>5.0676325097519601E-3</v>
-      </c>
-      <c r="P12" s="66">
-        <f t="shared" si="6"/>
-        <v>3.2981786178777221E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A13" s="66" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="66">
-        <v>20660583393.799999</v>
-      </c>
-      <c r="C13" s="66">
-        <v>537639626.39699996</v>
-      </c>
-      <c r="D13" s="66">
-        <v>19330068854.799999</v>
-      </c>
-      <c r="E13" s="66">
-        <v>715691346.79900002</v>
-      </c>
-      <c r="F13" s="66">
-        <v>6173962767.3999996</v>
-      </c>
-      <c r="G13" s="66">
-        <v>257133190.10299999</v>
-      </c>
-      <c r="H13" s="66">
-        <v>7934899589.3999996</v>
-      </c>
-      <c r="I13" s="66">
-        <v>215072134.37099999</v>
-      </c>
-      <c r="J13" s="66">
-        <f t="shared" si="0"/>
-        <v>0.9356013083638639</v>
-      </c>
-      <c r="K13" s="66">
-        <f t="shared" si="1"/>
-        <v>0.29882809452770503</v>
-      </c>
-      <c r="L13" s="66">
-        <f t="shared" si="2"/>
-        <v>0.38405980306350745</v>
-      </c>
-      <c r="M13" s="66">
-        <f t="shared" si="3"/>
-        <v>2.6022480398996833E-2</v>
-      </c>
-      <c r="N13" s="66">
-        <f t="shared" si="4"/>
-        <v>3.4640422932770171E-2</v>
-      </c>
-      <c r="O13" s="66">
-        <f t="shared" si="5"/>
-        <v>1.2445591937164885E-2</v>
-      </c>
-      <c r="P13" s="66">
-        <f t="shared" si="6"/>
-        <v>1.0409780317991439E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A14" s="66" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="66">
-        <v>10561923505.4</v>
-      </c>
-      <c r="C14" s="66">
-        <v>151274963.77000001</v>
-      </c>
-      <c r="D14" s="66">
-        <v>10168172695</v>
-      </c>
-      <c r="E14" s="66">
-        <v>541328595.98199999</v>
-      </c>
-      <c r="F14" s="66">
-        <v>4090644110</v>
-      </c>
-      <c r="G14" s="66">
-        <v>58402485.1448</v>
-      </c>
-      <c r="H14" s="66">
-        <v>3903467378.1999998</v>
-      </c>
-      <c r="I14" s="66">
-        <v>335819862.37699997</v>
-      </c>
-      <c r="J14" s="66">
-        <f t="shared" si="0"/>
-        <v>0.96271978203603858</v>
-      </c>
-      <c r="K14" s="66">
-        <f t="shared" si="1"/>
-        <v>0.38730105438735418</v>
-      </c>
-      <c r="L14" s="66">
-        <f t="shared" si="2"/>
-        <v>0.36957921312384739</v>
-      </c>
-      <c r="M14" s="66">
-        <f t="shared" si="3"/>
-        <v>1.4322671783473682E-2</v>
-      </c>
-      <c r="N14" s="66">
-        <f t="shared" si="4"/>
-        <v>5.1252841937856744E-2</v>
-      </c>
-      <c r="O14" s="66">
-        <f t="shared" si="5"/>
-        <v>5.5295311611507636E-3</v>
-      </c>
-      <c r="P14" s="66">
-        <f t="shared" si="6"/>
-        <v>3.1795331807251317E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A15" s="66" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="66">
-        <v>54820958103.199997</v>
-      </c>
-      <c r="C15" s="66">
-        <v>152868415.64500001</v>
-      </c>
-      <c r="D15" s="66">
-        <v>55418587635.599998</v>
-      </c>
-      <c r="E15" s="66">
-        <v>261534004.36199999</v>
-      </c>
-      <c r="F15" s="66">
-        <v>55428470726.599998</v>
-      </c>
-      <c r="G15" s="66">
-        <v>162601301.75799999</v>
-      </c>
-      <c r="H15" s="66">
-        <v>55030507401.199997</v>
-      </c>
-      <c r="I15" s="66">
-        <v>211962712.59099999</v>
-      </c>
-      <c r="J15" s="66">
-        <f t="shared" si="0"/>
-        <v>1.0109014791619471</v>
-      </c>
-      <c r="K15" s="66">
-        <f t="shared" si="1"/>
-        <v>1.0110817585905076</v>
-      </c>
-      <c r="L15" s="66">
-        <f t="shared" si="2"/>
-        <v>1.0038224304216925</v>
-      </c>
-      <c r="M15" s="66">
-        <f t="shared" si="3"/>
-        <v>2.7885031734984729E-3</v>
-      </c>
-      <c r="N15" s="66">
-        <f t="shared" si="4"/>
-        <v>4.7706937895843488E-3</v>
-      </c>
-      <c r="O15" s="66">
-        <f t="shared" si="5"/>
-        <v>2.9660426848415232E-3</v>
-      </c>
-      <c r="P15" s="66">
-        <f t="shared" si="6"/>
-        <v>3.86645399724649E-3</v>
       </c>
     </row>
   </sheetData>
@@ -12990,22 +12752,22 @@
     </row>
     <row r="3" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86" t="s">
+      <c r="C3" s="88"/>
+      <c r="D3" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="86"/>
-      <c r="F3" s="87" t="s">
+      <c r="E3" s="88"/>
+      <c r="F3" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="86"/>
-      <c r="H3" s="84" t="s">
+      <c r="G3" s="88"/>
+      <c r="H3" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="85"/>
+      <c r="I3" s="87"/>
       <c r="J3" s="48" t="s">
         <v>45</v>
       </c>
@@ -13015,11 +12777,11 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="87" t="s">
+      <c r="M3" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="88"/>
     </row>
     <row r="4" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -14824,11 +14586,593 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1814E241-F455-4452-B5DE-B4EE59F14CFA}">
+  <dimension ref="A1:P15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N14" sqref="N14:P14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="32.265625" customWidth="1"/>
+    <col min="2" max="2" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.9296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A1" s="72" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A2" s="72" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A3" s="73" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="73"/>
+      <c r="B6" s="93" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="93"/>
+      <c r="D6" s="93" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="93"/>
+      <c r="F6" s="93" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="93"/>
+      <c r="H6" s="94" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" s="94"/>
+      <c r="J6" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6" s="93" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="93"/>
+      <c r="O6" s="93"/>
+      <c r="P6" s="73"/>
+    </row>
+    <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="77" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="77" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="77" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="P7" s="79" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A8" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="66">
+        <v>927274396101</v>
+      </c>
+      <c r="C8" s="66">
+        <v>2252129313.96</v>
+      </c>
+      <c r="D8" s="66">
+        <v>928584523878</v>
+      </c>
+      <c r="E8" s="66">
+        <v>6426468418.3100004</v>
+      </c>
+      <c r="F8" s="66">
+        <v>935859695818</v>
+      </c>
+      <c r="G8" s="66">
+        <v>1303543522.45</v>
+      </c>
+      <c r="H8" s="66">
+        <v>931436628179</v>
+      </c>
+      <c r="I8" s="66">
+        <v>5821397551.7399998</v>
+      </c>
+      <c r="J8" s="66">
+        <f>D8/B8</f>
+        <v>1.0014128803539804</v>
+      </c>
+      <c r="K8" s="66">
+        <f>F8/B8</f>
+        <v>1.0092586398946195</v>
+      </c>
+      <c r="L8" s="66">
+        <f>H8/B8</f>
+        <v>1.0044886735744041</v>
+      </c>
+      <c r="M8" s="66">
+        <f>C8/B8</f>
+        <v>2.4287625361271111E-3</v>
+      </c>
+      <c r="N8" s="66">
+        <f>E8/B8</f>
+        <v>6.93049268407711E-3</v>
+      </c>
+      <c r="O8" s="66">
+        <f>G8/B8</f>
+        <v>1.4057797000878436E-3</v>
+      </c>
+      <c r="P8" s="66">
+        <f>I8/B8</f>
+        <v>6.2779664533149961E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A9" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="66">
+        <v>1167899698070</v>
+      </c>
+      <c r="C9" s="66">
+        <v>1572343407.77</v>
+      </c>
+      <c r="D9" s="66">
+        <v>1178943655390</v>
+      </c>
+      <c r="E9" s="66">
+        <v>10362118961.700001</v>
+      </c>
+      <c r="F9" s="66">
+        <v>1129500984560</v>
+      </c>
+      <c r="G9" s="66">
+        <v>944174208.25399995</v>
+      </c>
+      <c r="H9" s="66">
+        <v>1133772596540</v>
+      </c>
+      <c r="I9" s="66">
+        <v>8461901884.1800003</v>
+      </c>
+      <c r="J9" s="66">
+        <f t="shared" ref="J9:J15" si="0">D9/B9</f>
+        <v>1.0094562549662873</v>
+      </c>
+      <c r="K9" s="66">
+        <f t="shared" ref="K9:K15" si="1">F9/B9</f>
+        <v>0.9671215656845743</v>
+      </c>
+      <c r="L9" s="66">
+        <f t="shared" ref="L9:L15" si="2">H9/B9</f>
+        <v>0.97077908181122374</v>
+      </c>
+      <c r="M9" s="66">
+        <f t="shared" ref="M9:M15" si="3">C9/B9</f>
+        <v>1.346300037895685E-3</v>
+      </c>
+      <c r="N9" s="66">
+        <f t="shared" ref="N9:N15" si="4">E9/B9</f>
+        <v>8.8724391134134273E-3</v>
+      </c>
+      <c r="O9" s="66">
+        <f t="shared" ref="O9:O15" si="5">G9/B9</f>
+        <v>8.0843775352822231E-4</v>
+      </c>
+      <c r="P9" s="66">
+        <f t="shared" ref="P9:P15" si="6">I9/B9</f>
+        <v>7.2454012088226626E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A10" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="66">
+        <v>368205228.60000002</v>
+      </c>
+      <c r="C10" s="66">
+        <v>6887574.7414600002</v>
+      </c>
+      <c r="D10" s="66">
+        <v>362294137.80000001</v>
+      </c>
+      <c r="E10" s="66">
+        <v>20204685.2766</v>
+      </c>
+      <c r="F10" s="66">
+        <v>88088658.400000006</v>
+      </c>
+      <c r="G10" s="66">
+        <v>9483474.11558</v>
+      </c>
+      <c r="H10" s="66">
+        <v>108439750</v>
+      </c>
+      <c r="I10" s="66">
+        <v>3555898.5149500002</v>
+      </c>
+      <c r="J10" s="66">
+        <f t="shared" si="0"/>
+        <v>0.98394620624352536</v>
+      </c>
+      <c r="K10" s="66">
+        <f t="shared" si="1"/>
+        <v>0.23923793460221385</v>
+      </c>
+      <c r="L10" s="66">
+        <f t="shared" si="2"/>
+        <v>0.29450899003339137</v>
+      </c>
+      <c r="M10" s="66">
+        <f t="shared" si="3"/>
+        <v>1.8705803737899446E-2</v>
+      </c>
+      <c r="N10" s="66">
+        <f t="shared" si="4"/>
+        <v>5.4873433909189195E-2</v>
+      </c>
+      <c r="O10" s="66">
+        <f t="shared" si="5"/>
+        <v>2.5755946355347326E-2</v>
+      </c>
+      <c r="P10" s="66">
+        <f t="shared" si="6"/>
+        <v>9.6573819129900321E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A11" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="66">
+        <v>174362730.59999999</v>
+      </c>
+      <c r="C11" s="66">
+        <v>2663219.4407000002</v>
+      </c>
+      <c r="D11" s="66">
+        <v>168909930.40000001</v>
+      </c>
+      <c r="E11" s="66">
+        <v>13591693.936100001</v>
+      </c>
+      <c r="F11" s="66">
+        <v>61109618.799999997</v>
+      </c>
+      <c r="G11" s="66">
+        <v>1312040.0078100001</v>
+      </c>
+      <c r="H11" s="66">
+        <v>54860028.799999997</v>
+      </c>
+      <c r="I11" s="66">
+        <v>2739627.79629</v>
+      </c>
+      <c r="J11" s="66">
+        <f t="shared" si="0"/>
+        <v>0.96872726080145488</v>
+      </c>
+      <c r="K11" s="66">
+        <f t="shared" si="1"/>
+        <v>0.35047408692049925</v>
+      </c>
+      <c r="L11" s="66">
+        <f t="shared" si="2"/>
+        <v>0.31463162231527936</v>
+      </c>
+      <c r="M11" s="66">
+        <f t="shared" si="3"/>
+        <v>1.527401774183961E-2</v>
+      </c>
+      <c r="N11" s="66">
+        <f t="shared" si="4"/>
+        <v>7.7950682977546815E-2</v>
+      </c>
+      <c r="O11" s="66">
+        <f t="shared" si="5"/>
+        <v>7.5247732316139817E-3</v>
+      </c>
+      <c r="P11" s="66">
+        <f t="shared" si="6"/>
+        <v>1.5712232693664872E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A12" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="66">
+        <v>50721089984.400002</v>
+      </c>
+      <c r="C12" s="66">
+        <v>327032611.59600002</v>
+      </c>
+      <c r="D12" s="66">
+        <v>49851101330.800003</v>
+      </c>
+      <c r="E12" s="66">
+        <v>853331810.60500002</v>
+      </c>
+      <c r="F12" s="66">
+        <v>51061339932.400002</v>
+      </c>
+      <c r="G12" s="66">
+        <v>257035844.535</v>
+      </c>
+      <c r="H12" s="66">
+        <v>49624355425.800003</v>
+      </c>
+      <c r="I12" s="66">
+        <v>1672872144.6199999</v>
+      </c>
+      <c r="J12" s="66">
+        <f t="shared" si="0"/>
+        <v>0.98284759547029499</v>
+      </c>
+      <c r="K12" s="66">
+        <f t="shared" si="1"/>
+        <v>1.0067082538664813</v>
+      </c>
+      <c r="L12" s="66">
+        <f t="shared" si="2"/>
+        <v>0.97837714925019725</v>
+      </c>
+      <c r="M12" s="66">
+        <f t="shared" si="3"/>
+        <v>6.4476652945862087E-3</v>
+      </c>
+      <c r="N12" s="66">
+        <f t="shared" si="4"/>
+        <v>1.6824003799355544E-2</v>
+      </c>
+      <c r="O12" s="66">
+        <f t="shared" si="5"/>
+        <v>5.0676325097519601E-3</v>
+      </c>
+      <c r="P12" s="66">
+        <f t="shared" si="6"/>
+        <v>3.2981786178777221E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A13" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="66">
+        <v>20660583393.799999</v>
+      </c>
+      <c r="C13" s="66">
+        <v>537639626.39699996</v>
+      </c>
+      <c r="D13" s="66">
+        <v>19330068854.799999</v>
+      </c>
+      <c r="E13" s="66">
+        <v>715691346.79900002</v>
+      </c>
+      <c r="F13" s="66">
+        <v>6173962767.3999996</v>
+      </c>
+      <c r="G13" s="66">
+        <v>257133190.10299999</v>
+      </c>
+      <c r="H13" s="66">
+        <v>7934899589.3999996</v>
+      </c>
+      <c r="I13" s="66">
+        <v>215072134.37099999</v>
+      </c>
+      <c r="J13" s="66">
+        <f t="shared" si="0"/>
+        <v>0.9356013083638639</v>
+      </c>
+      <c r="K13" s="66">
+        <f t="shared" si="1"/>
+        <v>0.29882809452770503</v>
+      </c>
+      <c r="L13" s="66">
+        <f t="shared" si="2"/>
+        <v>0.38405980306350745</v>
+      </c>
+      <c r="M13" s="66">
+        <f t="shared" si="3"/>
+        <v>2.6022480398996833E-2</v>
+      </c>
+      <c r="N13" s="66">
+        <f t="shared" si="4"/>
+        <v>3.4640422932770171E-2</v>
+      </c>
+      <c r="O13" s="66">
+        <f t="shared" si="5"/>
+        <v>1.2445591937164885E-2</v>
+      </c>
+      <c r="P13" s="66">
+        <f t="shared" si="6"/>
+        <v>1.0409780317991439E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A14" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="66">
+        <v>10561923505.4</v>
+      </c>
+      <c r="C14" s="66">
+        <v>151274963.77000001</v>
+      </c>
+      <c r="D14" s="66">
+        <v>10168172695</v>
+      </c>
+      <c r="E14" s="66">
+        <v>541328595.98199999</v>
+      </c>
+      <c r="F14" s="66">
+        <v>4090644110</v>
+      </c>
+      <c r="G14" s="66">
+        <v>58402485.1448</v>
+      </c>
+      <c r="H14" s="66">
+        <v>3903467378.1999998</v>
+      </c>
+      <c r="I14" s="66">
+        <v>335819862.37699997</v>
+      </c>
+      <c r="J14" s="66">
+        <f t="shared" si="0"/>
+        <v>0.96271978203603858</v>
+      </c>
+      <c r="K14" s="66">
+        <f t="shared" si="1"/>
+        <v>0.38730105438735418</v>
+      </c>
+      <c r="L14" s="66">
+        <f t="shared" si="2"/>
+        <v>0.36957921312384739</v>
+      </c>
+      <c r="M14" s="66">
+        <f t="shared" si="3"/>
+        <v>1.4322671783473682E-2</v>
+      </c>
+      <c r="N14" s="66">
+        <f t="shared" si="4"/>
+        <v>5.1252841937856744E-2</v>
+      </c>
+      <c r="O14" s="66">
+        <f t="shared" si="5"/>
+        <v>5.5295311611507636E-3</v>
+      </c>
+      <c r="P14" s="66">
+        <f t="shared" si="6"/>
+        <v>3.1795331807251317E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A15" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="66">
+        <v>54820958103.199997</v>
+      </c>
+      <c r="C15" s="66">
+        <v>152868415.64500001</v>
+      </c>
+      <c r="D15" s="66">
+        <v>55418587635.599998</v>
+      </c>
+      <c r="E15" s="66">
+        <v>261534004.36199999</v>
+      </c>
+      <c r="F15" s="66">
+        <v>55428470726.599998</v>
+      </c>
+      <c r="G15" s="66">
+        <v>162601301.75799999</v>
+      </c>
+      <c r="H15" s="66">
+        <v>55030507401.199997</v>
+      </c>
+      <c r="I15" s="66">
+        <v>211962712.59099999</v>
+      </c>
+      <c r="J15" s="66">
+        <f t="shared" si="0"/>
+        <v>1.0109014791619471</v>
+      </c>
+      <c r="K15" s="66">
+        <f t="shared" si="1"/>
+        <v>1.0110817585905076</v>
+      </c>
+      <c r="L15" s="66">
+        <f t="shared" si="2"/>
+        <v>1.0038224304216925</v>
+      </c>
+      <c r="M15" s="66">
+        <f t="shared" si="3"/>
+        <v>2.7885031734984729E-3</v>
+      </c>
+      <c r="N15" s="66">
+        <f t="shared" si="4"/>
+        <v>4.7706937895843488E-3</v>
+      </c>
+      <c r="O15" s="66">
+        <f t="shared" si="5"/>
+        <v>2.9660426848415232E-3</v>
+      </c>
+      <c r="P15" s="66">
+        <f t="shared" si="6"/>
+        <v>3.86645399724649E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="M6:O6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC958D8-824A-4FFE-8EFB-EA4CAF2DCC74}">
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="A5" sqref="A5:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14851,22 +15195,22 @@
     </row>
     <row r="3" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="73"/>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90" t="s">
+      <c r="C3" s="93"/>
+      <c r="D3" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90" t="s">
+      <c r="E3" s="93"/>
+      <c r="F3" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="90"/>
-      <c r="H3" s="91" t="s">
+      <c r="G3" s="93"/>
+      <c r="H3" s="94" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="91"/>
+      <c r="I3" s="94"/>
       <c r="J3" s="77" t="s">
         <v>45</v>
       </c>
@@ -14876,11 +15220,11 @@
       <c r="L3" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="90" t="s">
+      <c r="M3" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
       <c r="P3" s="73"/>
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -15395,7 +15739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F72758A-17BC-4C1E-98B0-DDD6331D597C}">
   <dimension ref="A1:P12"/>
   <sheetViews>
@@ -15424,22 +15768,22 @@
     </row>
     <row r="3" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="73"/>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90" t="s">
+      <c r="C3" s="93"/>
+      <c r="D3" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90" t="s">
+      <c r="E3" s="93"/>
+      <c r="F3" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="90"/>
-      <c r="H3" s="91" t="s">
+      <c r="G3" s="93"/>
+      <c r="H3" s="94" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="91"/>
+      <c r="I3" s="94"/>
       <c r="J3" s="77" t="s">
         <v>45</v>
       </c>
@@ -15449,11 +15793,11 @@
       <c r="L3" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="90" t="s">
+      <c r="M3" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
       <c r="P3" s="73"/>
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -15968,7 +16312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C510FE-BA24-4F4C-B882-A73942D255FE}">
   <dimension ref="A1:D31"/>
   <sheetViews>
@@ -16336,7 +16680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5A357B-AD95-4B57-AFAC-6E90E36724A8}">
   <dimension ref="A1:H59"/>
   <sheetViews>
@@ -17046,29 +17390,29 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86" t="s">
+      <c r="C3" s="88"/>
+      <c r="D3" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="86"/>
-      <c r="F3" s="87" t="s">
+      <c r="E3" s="88"/>
+      <c r="F3" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="86"/>
+      <c r="G3" s="88"/>
       <c r="H3" s="7" t="s">
         <v>45</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="87" t="s">
+      <c r="J3" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="88"/>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -18560,22 +18904,22 @@
     </row>
     <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="52"/>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88" t="s">
+      <c r="C2" s="90"/>
+      <c r="D2" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88" t="s">
+      <c r="E2" s="90"/>
+      <c r="F2" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="88"/>
-      <c r="H2" s="89" t="s">
+      <c r="G2" s="90"/>
+      <c r="H2" s="91" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="89"/>
+      <c r="I2" s="91"/>
       <c r="J2" s="54" t="s">
         <v>45</v>
       </c>
@@ -18585,11 +18929,11 @@
       <c r="L2" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="88" t="s">
+      <c r="M2" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
     </row>
     <row r="3" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="52"/>
@@ -19131,22 +19475,22 @@
     </row>
     <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="26"/>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86" t="s">
+      <c r="C2" s="88"/>
+      <c r="D2" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="86"/>
-      <c r="F2" s="87" t="s">
+      <c r="E2" s="88"/>
+      <c r="F2" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="86"/>
-      <c r="H2" s="84" t="s">
+      <c r="G2" s="88"/>
+      <c r="H2" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="85"/>
+      <c r="I2" s="87"/>
       <c r="J2" s="48" t="s">
         <v>45</v>
       </c>
@@ -19156,11 +19500,11 @@
       <c r="L2" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="87" t="s">
+      <c r="M2" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
     </row>
     <row r="3" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26"/>
@@ -19700,22 +20044,22 @@
     </row>
     <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26"/>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86" t="s">
+      <c r="C3" s="88"/>
+      <c r="D3" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="86"/>
-      <c r="F3" s="87" t="s">
+      <c r="E3" s="88"/>
+      <c r="F3" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="86"/>
-      <c r="H3" s="84" t="s">
+      <c r="G3" s="88"/>
+      <c r="H3" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="85"/>
+      <c r="I3" s="87"/>
       <c r="J3" s="48" t="s">
         <v>45</v>
       </c>
@@ -19725,11 +20069,11 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="87" t="s">
+      <c r="M3" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="88"/>
     </row>
     <row r="4" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="26"/>
@@ -20269,22 +20613,22 @@
     </row>
     <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26"/>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86" t="s">
+      <c r="C3" s="88"/>
+      <c r="D3" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="86"/>
-      <c r="F3" s="87" t="s">
+      <c r="E3" s="88"/>
+      <c r="F3" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="86"/>
-      <c r="H3" s="84" t="s">
+      <c r="G3" s="88"/>
+      <c r="H3" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="85"/>
+      <c r="I3" s="87"/>
       <c r="J3" s="48" t="s">
         <v>45</v>
       </c>
@@ -20294,11 +20638,11 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="87" t="s">
+      <c r="M3" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="88"/>
     </row>
     <row r="4" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="26"/>
@@ -20969,327 +21313,253 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DCC425-F9E0-4DC1-9C1B-7FD63E026DA8}">
-  <dimension ref="A2:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F173229C-1150-4B07-9313-8228C415AB22}">
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.46484375" customWidth="1"/>
-    <col min="2" max="2" width="13.06640625" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="22.1328125" customWidth="1"/>
-    <col min="7" max="7" width="19.59765625" customWidth="1"/>
+    <col min="1" max="1" width="34.9296875" customWidth="1"/>
+    <col min="2" max="2" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="66" t="s">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A1" s="25" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="22" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="80"/>
+      <c r="B4" s="95" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="95"/>
+    </row>
+    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="96" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="96" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="96" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="66">
+        <v>65403223.600000001</v>
+      </c>
+      <c r="C6" s="66">
+        <v>3289023.0558799999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="66">
+        <v>31458333486.799999</v>
+      </c>
+      <c r="C7" s="66">
+        <v>93140878.649000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="66">
+        <v>713763</v>
+      </c>
+      <c r="C8" s="66">
+        <v>4668.7681030399999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="66">
+        <v>1461786</v>
+      </c>
+      <c r="C9" s="66">
+        <v>24201.016011700001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="66">
+        <v>42183725662</v>
+      </c>
+      <c r="C10" s="66">
+        <v>62319091.303900003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="93" t="s">
-        <v>206</v>
-      </c>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-    </row>
-    <row r="3" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D3" s="92" t="s">
-        <v>205</v>
-      </c>
-      <c r="E3" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="92" t="s">
-        <v>204</v>
-      </c>
-      <c r="G3" s="92" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4">
+      <c r="B11" s="66">
+        <v>22172169.800000001</v>
+      </c>
+      <c r="C11" s="66">
+        <v>450762.66297800001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="66">
+        <v>64846325.799999997</v>
+      </c>
+      <c r="C12" s="66">
+        <v>4044395.09381</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="66">
+        <v>416160398</v>
+      </c>
+      <c r="C13" s="66">
+        <v>21823144.353399999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="97" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="80"/>
+      <c r="B17" s="95" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="95"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="96" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="96" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="96" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="66">
+        <v>151772</v>
+      </c>
+      <c r="C19" s="66">
+        <v>31250.017708799998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="66">
+        <v>6585151.4000000004</v>
+      </c>
+      <c r="C20" s="66">
+        <v>1286932.6227599999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="66">
+        <v>13998.4</v>
+      </c>
+      <c r="C21" s="66">
+        <v>810.24381515699997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="66">
+        <v>11084.2</v>
+      </c>
+      <c r="C22" s="66">
+        <v>697.57935749299997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="94">
-        <v>0.9356013083638639</v>
-      </c>
-      <c r="C4" s="94">
-        <v>0.29882809452770503</v>
-      </c>
-      <c r="D4" s="94">
-        <v>0.38405980306350745</v>
-      </c>
-      <c r="E4" s="94">
-        <v>3.4640422932770171E-2</v>
-      </c>
-      <c r="F4" s="94">
-        <v>1.2445591937164885E-2</v>
-      </c>
-      <c r="G4" s="94">
-        <v>1.0409780317991439E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5">
+      <c r="B23" s="66">
+        <v>8731488.4000000004</v>
+      </c>
+      <c r="C23" s="66">
+        <v>6201094.71172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="94">
-        <v>0.94469744673390132</v>
-      </c>
-      <c r="C5" s="94">
-        <v>0.29466756956271822</v>
-      </c>
-      <c r="D5" s="94">
-        <v>0.38277691547795289</v>
-      </c>
-      <c r="E5" s="94">
-        <v>9.8580753532644672E-3</v>
-      </c>
-      <c r="F5" s="94">
-        <v>9.6764378341133751E-3</v>
-      </c>
-      <c r="G5" s="94">
-        <v>4.9566377119578762E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>8</v>
-      </c>
-      <c r="B6" s="94">
-        <v>0.87222223701487334</v>
-      </c>
-      <c r="C6" s="94">
-        <v>0.28024151734484376</v>
-      </c>
-      <c r="D6" s="94">
-        <v>0.37004112521020127</v>
-      </c>
-      <c r="E6" s="94">
-        <v>9.341955830266235E-3</v>
-      </c>
-      <c r="F6" s="94">
-        <v>8.2292052415342976E-3</v>
-      </c>
-      <c r="G6" s="94">
-        <v>7.8543122896674276E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>10</v>
-      </c>
-      <c r="B7" s="94">
-        <v>0.8835802154119029</v>
-      </c>
-      <c r="C7" s="94">
-        <v>0.2790662450692325</v>
-      </c>
-      <c r="D7" s="94">
-        <v>0.36589759015925816</v>
-      </c>
-      <c r="E7" s="94">
-        <v>1.78778409257737E-2</v>
-      </c>
-      <c r="F7" s="94">
-        <v>3.6076317302390845E-3</v>
-      </c>
-      <c r="G7" s="94">
-        <v>3.7763396325711275E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>12</v>
-      </c>
-      <c r="B8" s="94">
-        <v>0.90400805184937105</v>
-      </c>
-      <c r="C8" s="94">
-        <v>0.29114478875725908</v>
-      </c>
-      <c r="D8" s="94">
-        <v>0.36980716829392185</v>
-      </c>
-      <c r="E8" s="94">
-        <v>1.8841533980046916E-2</v>
-      </c>
-      <c r="F8" s="94">
-        <v>9.4314524537784418E-3</v>
-      </c>
-      <c r="G8" s="94">
-        <v>1.1562533614423927E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" s="66" t="s">
+      <c r="B24" s="66">
+        <v>571030.19999999995</v>
+      </c>
+      <c r="C24" s="66">
+        <v>54596.198817900004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="93" t="s">
-        <v>206</v>
-      </c>
-      <c r="F11" s="93"/>
-      <c r="G11" s="93"/>
-    </row>
-    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A12" s="65" t="s">
-        <v>203</v>
-      </c>
-      <c r="B12" s="65" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="65" t="s">
-        <v>204</v>
-      </c>
-      <c r="D12" s="92" t="s">
-        <v>207</v>
-      </c>
-      <c r="E12" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="92" t="s">
-        <v>204</v>
-      </c>
-      <c r="G12" s="92" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="65">
-        <v>1</v>
-      </c>
-      <c r="B13" s="94">
-        <v>0.96271978203603858</v>
-      </c>
-      <c r="C13" s="94">
-        <v>0.38730105438735418</v>
-      </c>
-      <c r="D13" s="94">
-        <v>0.36957921312384739</v>
-      </c>
-      <c r="E13" s="94">
-        <v>5.1252841937856744E-2</v>
-      </c>
-      <c r="F13" s="94">
-        <v>5.5295311611507636E-3</v>
-      </c>
-      <c r="G13" s="94">
-        <v>3.1795331807251317E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="65">
-        <v>4</v>
-      </c>
-      <c r="B14" s="94">
-        <v>0.9442762311353079</v>
-      </c>
-      <c r="C14" s="94">
-        <v>0.41434324900610719</v>
-      </c>
-      <c r="D14" s="94">
-        <v>0.40083074332271823</v>
-      </c>
-      <c r="E14" s="94">
-        <v>8.5005017896467427E-3</v>
-      </c>
-      <c r="F14" s="94">
-        <v>6.0953616896922656E-3</v>
-      </c>
-      <c r="G14" s="94">
-        <v>2.0913418320206361E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="65">
-        <v>8</v>
-      </c>
-      <c r="B15" s="94">
-        <v>0.86439751671266363</v>
-      </c>
-      <c r="C15" s="94">
-        <v>0.41517545864783562</v>
-      </c>
-      <c r="D15" s="94">
-        <v>0.42928869176101703</v>
-      </c>
-      <c r="E15" s="94">
-        <v>1.0873531107782013E-2</v>
-      </c>
-      <c r="F15" s="94">
-        <v>4.5428457859383424E-3</v>
-      </c>
-      <c r="G15" s="94">
-        <v>3.2045527585561561E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16">
-        <v>10</v>
-      </c>
-      <c r="B16" s="94">
-        <v>0.87182608862774247</v>
-      </c>
-      <c r="C16" s="94">
-        <v>0.4396266532861684</v>
-      </c>
-      <c r="D16" s="94">
-        <v>0.40648641375508454</v>
-      </c>
-      <c r="E16" s="94">
-        <v>2.966505280632557E-2</v>
-      </c>
-      <c r="F16" s="94">
-        <v>3.8832662288856685E-3</v>
-      </c>
-      <c r="G16" s="94">
-        <v>1.9088334041327464E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="65">
-        <v>12</v>
-      </c>
-      <c r="B17" s="94">
-        <v>0.91955706039378737</v>
-      </c>
-      <c r="C17" s="94">
-        <v>0.44375153500032488</v>
-      </c>
-      <c r="D17" s="94">
-        <v>0.4494151032037067</v>
-      </c>
-      <c r="E17" s="94">
-        <v>2.0072354924216499E-2</v>
-      </c>
-      <c r="F17" s="94">
-        <v>9.5140644989271071E-3</v>
-      </c>
-      <c r="G17" s="94">
-        <v>1.2858348739257596E-2</v>
+      <c r="B25" s="66">
+        <v>427796.4</v>
+      </c>
+      <c r="C25" s="66">
+        <v>61332.597051199999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="66">
+        <v>1947502.6</v>
+      </c>
+      <c r="C26" s="66">
+        <v>987191.93594800006</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added results of SPECjvm derby with Alan's patch of using large pages on the code and data heap
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="25" documentId="81D8B261ABBD5CBDED69DEB44BA5B0CD337C6AB9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{4C5B0F60-B89A-477E-BCF4-1ADBD8CC82DC}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="81D8B261ABBD5CBDED69DEB44BA5B0CD337C6AB9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{579568F4-A4B7-4F6B-8548-3455D4D6DB74}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="216">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -708,6 +708,15 @@
   <si>
     <t>USR</t>
   </si>
+  <si>
+    <t xml:space="preserve"> Enable UseLargePage in jvm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Disable UseLargePage in jvm</t>
+  </si>
+  <si>
+    <t>Results are normalized to the baseline</t>
+  </si>
 </sst>
 </file>
 
@@ -933,7 +942,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1081,6 +1090,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1102,6 +1115,9 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1111,13 +1127,9 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2376,6 +2388,618 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'postgres summary'!$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Shared ptp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'postgres summary'!$A$22:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'postgres summary'!$B$22:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.0094562549662873</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0059484718001523</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0044824862086825</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0125669639090009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0031291270585641</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4CB7-4733-8173-334A3BB87992}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'postgres summary'!$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Code super page</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'postgres summary'!$A$22:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'postgres summary'!$C$22:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.9671215656845743</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94756235202180572</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9577061352660623</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95545547272293507</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94905852788502132</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4CB7-4733-8173-334A3BB87992}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'postgres summary'!$D$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Shared ptp + code super page</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'postgres summary'!$A$22:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'postgres summary'!$D$22:$D$26</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.97077908181122374</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95768295161371098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96908148802760707</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96531645829242818</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96926551111416337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4CB7-4733-8173-334A3BB87992}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="892226856"/>
+        <c:axId val="892223904"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="892226856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Database Size (GB)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="892223904"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="892223904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>CPU_CLK_UNHALTED.THREAD_P normalized to the baseline</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="892226856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2417,6 +3041,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3462,20 +4126,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>931068</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>40481</xdr:rowOff>
+      <xdr:colOff>188118</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>116681</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>604838</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>80963</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>509588</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>157163</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3503,15 +4670,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1288256</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>173830</xdr:rowOff>
+      <xdr:colOff>216694</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>102393</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>481013</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3531,6 +4698,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>169067</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>97631</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>619124</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{599CFAE2-5DB8-4C17-9E87-B35DF7B82AD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3830,22 +5033,22 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="57" x14ac:dyDescent="0.45">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85" t="s">
+      <c r="C3" s="87"/>
+      <c r="D3" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85" t="s">
+      <c r="E3" s="87"/>
+      <c r="F3" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="85"/>
-      <c r="H3" s="86" t="s">
+      <c r="G3" s="87"/>
+      <c r="H3" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="87"/>
+      <c r="I3" s="89"/>
       <c r="J3" s="33" t="s">
         <v>45</v>
       </c>
@@ -3855,12 +5058,12 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="85" t="s">
+      <c r="M3" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
     </row>
     <row r="4" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
@@ -5806,11 +7009,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DCC425-F9E0-4DC1-9C1B-7FD63E026DA8}">
-  <dimension ref="A2:G17"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -5821,15 +7022,20 @@
     <col min="7" max="7" width="19.59765625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="22" t="s">
+        <v>215</v>
+      </c>
+    </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="92" t="s">
+      <c r="E2" s="95" t="s">
         <v>206</v>
       </c>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
     </row>
     <row r="3" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -5976,11 +7182,11 @@
       <c r="B11" s="65"/>
       <c r="C11" s="65"/>
       <c r="D11" s="65"/>
-      <c r="E11" s="92" t="s">
+      <c r="E11" s="95" t="s">
         <v>206</v>
       </c>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92"/>
+      <c r="F11" s="95"/>
+      <c r="G11" s="95"/>
     </row>
     <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="65" t="s">
@@ -6120,13 +7326,163 @@
         <v>1.2858348739257596E-2</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="95" t="s">
+        <v>206</v>
+      </c>
+      <c r="F20" s="95"/>
+      <c r="G20" s="95"/>
+    </row>
+    <row r="21" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A21" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="B21" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="D21" s="83" t="s">
+        <v>207</v>
+      </c>
+      <c r="E21" s="83" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="83" t="s">
+        <v>204</v>
+      </c>
+      <c r="G21" s="83" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="65">
+        <v>1</v>
+      </c>
+      <c r="B22" s="84">
+        <v>1.0094562549662873</v>
+      </c>
+      <c r="C22" s="84">
+        <v>0.9671215656845743</v>
+      </c>
+      <c r="D22" s="84">
+        <v>0.97077908181122374</v>
+      </c>
+      <c r="E22" s="84">
+        <v>8.8724391134134273E-3</v>
+      </c>
+      <c r="F22" s="84">
+        <v>8.0843775352822231E-4</v>
+      </c>
+      <c r="G22" s="84">
+        <v>7.2454012088226626E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="65">
+        <v>4</v>
+      </c>
+      <c r="B23" s="84">
+        <v>1.0059484718001523</v>
+      </c>
+      <c r="C23" s="84">
+        <v>0.94756235202180572</v>
+      </c>
+      <c r="D23" s="84">
+        <v>0.95768295161371098</v>
+      </c>
+      <c r="E23" s="84">
+        <v>8.1780096950417776E-3</v>
+      </c>
+      <c r="F23" s="84">
+        <v>1.5056313778154947E-3</v>
+      </c>
+      <c r="G23" s="84">
+        <v>8.7729185882929796E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="65">
+        <v>8</v>
+      </c>
+      <c r="B24" s="84">
+        <v>1.0044824862086825</v>
+      </c>
+      <c r="C24" s="84">
+        <v>0.9577061352660623</v>
+      </c>
+      <c r="D24" s="84">
+        <v>0.96908148802760707</v>
+      </c>
+      <c r="E24" s="84">
+        <v>8.1221646247106195E-3</v>
+      </c>
+      <c r="F24" s="84">
+        <v>8.7680013656943213E-3</v>
+      </c>
+      <c r="G24" s="84">
+        <v>1.2309038169908636E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" s="65">
+        <v>10</v>
+      </c>
+      <c r="B25" s="84">
+        <v>1.0125669639090009</v>
+      </c>
+      <c r="C25" s="84">
+        <v>0.95545547272293507</v>
+      </c>
+      <c r="D25" s="84">
+        <v>0.96531645829242818</v>
+      </c>
+      <c r="E25" s="84">
+        <v>7.094640920187089E-3</v>
+      </c>
+      <c r="F25" s="84">
+        <v>9.7277594852813887E-3</v>
+      </c>
+      <c r="G25" s="84">
+        <v>1.1418859023494183E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="65">
+        <v>12</v>
+      </c>
+      <c r="B26" s="84">
+        <v>1.0031291270585641</v>
+      </c>
+      <c r="C26" s="84">
+        <v>0.94905852788502132</v>
+      </c>
+      <c r="D26" s="84">
+        <v>0.96926551111416337</v>
+      </c>
+      <c r="E26" s="84">
+        <v>7.5384279310884246E-3</v>
+      </c>
+      <c r="F26" s="84">
+        <v>9.1452993911554203E-4</v>
+      </c>
+      <c r="G26" s="84">
+        <v>1.2846948576943572E-3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6135,7 +7491,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C15"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6249,22 +7605,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93" t="s">
+      <c r="C6" s="96"/>
+      <c r="D6" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93" t="s">
+      <c r="E6" s="96"/>
+      <c r="F6" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="93"/>
-      <c r="H6" s="94" t="s">
+      <c r="G6" s="96"/>
+      <c r="H6" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="94"/>
+      <c r="I6" s="97"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -6274,11 +7630,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="93" t="s">
+      <c r="M6" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="93"/>
-      <c r="O6" s="93"/>
+      <c r="N6" s="96"/>
+      <c r="O6" s="96"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -6797,8 +8153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819BCD50-CCED-4858-989E-30CB05A9C1BE}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A15"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8171,8 +9527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD324841-F3D6-48B1-BFDE-305D75F58DD9}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A15"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9002,22 +10358,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93" t="s">
+      <c r="C6" s="96"/>
+      <c r="D6" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93" t="s">
+      <c r="E6" s="96"/>
+      <c r="F6" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="93"/>
-      <c r="H6" s="94" t="s">
+      <c r="G6" s="96"/>
+      <c r="H6" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="94"/>
+      <c r="I6" s="97"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -9027,11 +10383,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="93" t="s">
+      <c r="M6" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="93"/>
-      <c r="O6" s="93"/>
+      <c r="N6" s="96"/>
+      <c r="O6" s="96"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -9550,8 +10906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEB844F-EF6D-4427-9E28-001A58A9FD5B}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13:P13"/>
+    <sheetView topLeftCell="E6" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9665,22 +11021,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93" t="s">
+      <c r="C6" s="96"/>
+      <c r="D6" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93" t="s">
+      <c r="E6" s="96"/>
+      <c r="F6" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="93"/>
-      <c r="H6" s="94" t="s">
+      <c r="G6" s="96"/>
+      <c r="H6" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="94"/>
+      <c r="I6" s="97"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -9690,11 +11046,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="93" t="s">
+      <c r="M6" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="93"/>
-      <c r="O6" s="93"/>
+      <c r="N6" s="96"/>
+      <c r="O6" s="96"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -9827,31 +11183,31 @@
         <v>1469223720.0999999</v>
       </c>
       <c r="J9" s="66">
-        <f t="shared" ref="J9:J15" si="0">D9/B9</f>
+        <f>D9/B9</f>
         <v>1.0044824862086825</v>
       </c>
       <c r="K9" s="66">
-        <f t="shared" ref="K9:K15" si="1">F9/B9</f>
+        <f t="shared" ref="K9:K15" si="0">F9/B9</f>
         <v>0.9577061352660623</v>
       </c>
       <c r="L9" s="66">
-        <f t="shared" ref="L9:L15" si="2">H9/B9</f>
+        <f t="shared" ref="L9:L15" si="1">H9/B9</f>
         <v>0.96908148802760707</v>
       </c>
       <c r="M9" s="66">
-        <f t="shared" ref="M9:M15" si="3">C9/B9</f>
+        <f t="shared" ref="M9:M15" si="2">C9/B9</f>
         <v>4.0955186090568512E-3</v>
       </c>
       <c r="N9" s="66">
-        <f t="shared" ref="N9:N15" si="4">E9/B9</f>
+        <f t="shared" ref="N9:N15" si="3">E9/B9</f>
         <v>8.1221646247106195E-3</v>
       </c>
       <c r="O9" s="66">
-        <f t="shared" ref="O9:O15" si="5">G9/B9</f>
+        <f t="shared" ref="O9:O15" si="4">G9/B9</f>
         <v>8.7680013656943213E-3</v>
       </c>
       <c r="P9" s="66">
-        <f t="shared" ref="P9:P15" si="6">I9/B9</f>
+        <f t="shared" ref="P9:P15" si="5">I9/B9</f>
         <v>1.2309038169908636E-3</v>
       </c>
     </row>
@@ -9884,31 +11240,31 @@
         <v>1932588.55125</v>
       </c>
       <c r="J10" s="66">
+        <f t="shared" ref="J9:J15" si="6">D10/B10</f>
+        <v>0.9258286527011016</v>
+      </c>
+      <c r="K10" s="66">
         <f t="shared" si="0"/>
-        <v>0.9258286527011016</v>
-      </c>
-      <c r="K10" s="66">
+        <v>0.22176732474154418</v>
+      </c>
+      <c r="L10" s="66">
         <f t="shared" si="1"/>
-        <v>0.22176732474154418</v>
-      </c>
-      <c r="L10" s="66">
+        <v>0.26985885053878728</v>
+      </c>
+      <c r="M10" s="66">
         <f t="shared" si="2"/>
-        <v>0.26985885053878728</v>
-      </c>
-      <c r="M10" s="66">
+        <v>9.1292646527233214E-3</v>
+      </c>
+      <c r="N10" s="66">
         <f t="shared" si="3"/>
-        <v>9.1292646527233214E-3</v>
-      </c>
-      <c r="N10" s="66">
+        <v>3.5946432749943552E-2</v>
+      </c>
+      <c r="O10" s="66">
         <f t="shared" si="4"/>
-        <v>3.5946432749943552E-2</v>
-      </c>
-      <c r="O10" s="66">
+        <v>1.2470960133327345E-2</v>
+      </c>
+      <c r="P10" s="66">
         <f t="shared" si="5"/>
-        <v>1.2470960133327345E-2</v>
-      </c>
-      <c r="P10" s="66">
-        <f t="shared" si="6"/>
         <v>4.9534211493336318E-3</v>
       </c>
     </row>
@@ -9941,31 +11297,31 @@
         <v>2191805.6304899999</v>
       </c>
       <c r="J11" s="66">
+        <f t="shared" si="6"/>
+        <v>0.88272013761312429</v>
+      </c>
+      <c r="K11" s="66">
         <f t="shared" si="0"/>
-        <v>0.88272013761312429</v>
-      </c>
-      <c r="K11" s="66">
+        <v>0.37966851365280613</v>
+      </c>
+      <c r="L11" s="66">
         <f t="shared" si="1"/>
-        <v>0.37966851365280613</v>
-      </c>
-      <c r="L11" s="66">
+        <v>0.36104043698559946</v>
+      </c>
+      <c r="M11" s="66">
         <f t="shared" si="2"/>
-        <v>0.36104043698559946</v>
-      </c>
-      <c r="M11" s="66">
+        <v>1.4145497592207122E-2</v>
+      </c>
+      <c r="N11" s="66">
         <f t="shared" si="3"/>
-        <v>1.4145497592207122E-2</v>
-      </c>
-      <c r="N11" s="66">
+        <v>5.2762997791926537E-2</v>
+      </c>
+      <c r="O11" s="66">
         <f t="shared" si="4"/>
-        <v>5.2762997791926537E-2</v>
-      </c>
-      <c r="O11" s="66">
+        <v>3.6876941757245682E-3</v>
+      </c>
+      <c r="P11" s="66">
         <f t="shared" si="5"/>
-        <v>3.6876941757245682E-3</v>
-      </c>
-      <c r="P11" s="66">
-        <f t="shared" si="6"/>
         <v>1.0356687965184698E-2</v>
       </c>
     </row>
@@ -9998,31 +11354,31 @@
         <v>6835264884.6199999</v>
       </c>
       <c r="J12" s="66">
+        <f t="shared" si="6"/>
+        <v>0.99162263127142403</v>
+      </c>
+      <c r="K12" s="66">
         <f t="shared" si="0"/>
-        <v>0.99162263127142403</v>
-      </c>
-      <c r="K12" s="66">
+        <v>0.99212235110610247</v>
+      </c>
+      <c r="L12" s="66">
         <f t="shared" si="1"/>
-        <v>0.99212235110610247</v>
-      </c>
-      <c r="L12" s="66">
+        <v>0.98894011165622819</v>
+      </c>
+      <c r="M12" s="66">
         <f t="shared" si="2"/>
-        <v>0.98894011165622819</v>
-      </c>
-      <c r="M12" s="66">
+        <v>1.4976129713387075E-3</v>
+      </c>
+      <c r="N12" s="66">
         <f t="shared" si="3"/>
-        <v>1.4976129713387075E-3</v>
-      </c>
-      <c r="N12" s="66">
+        <v>7.0323159763447315E-3</v>
+      </c>
+      <c r="O12" s="66">
         <f t="shared" si="4"/>
-        <v>7.0323159763447315E-3</v>
-      </c>
-      <c r="O12" s="66">
+        <v>9.0852516222916617E-3</v>
+      </c>
+      <c r="P12" s="66">
         <f t="shared" si="5"/>
-        <v>9.0852516222916617E-3</v>
-      </c>
-      <c r="P12" s="66">
-        <f t="shared" si="6"/>
         <v>7.1756159050630547E-3</v>
       </c>
     </row>
@@ -10055,31 +11411,31 @@
         <v>170620592.71200001</v>
       </c>
       <c r="J13" s="66">
+        <f t="shared" si="6"/>
+        <v>0.87222223701487334</v>
+      </c>
+      <c r="K13" s="66">
         <f t="shared" si="0"/>
-        <v>0.87222223701487334</v>
-      </c>
-      <c r="K13" s="66">
+        <v>0.28024151734484376</v>
+      </c>
+      <c r="L13" s="66">
         <f t="shared" si="1"/>
-        <v>0.28024151734484376</v>
-      </c>
-      <c r="L13" s="66">
+        <v>0.37004112521020127</v>
+      </c>
+      <c r="M13" s="66">
         <f t="shared" si="2"/>
-        <v>0.37004112521020127</v>
-      </c>
-      <c r="M13" s="66">
+        <v>1.3510393370169771E-2</v>
+      </c>
+      <c r="N13" s="66">
         <f t="shared" si="3"/>
-        <v>1.3510393370169771E-2</v>
-      </c>
-      <c r="N13" s="66">
+        <v>9.341955830266235E-3</v>
+      </c>
+      <c r="O13" s="66">
         <f t="shared" si="4"/>
-        <v>9.341955830266235E-3</v>
-      </c>
-      <c r="O13" s="66">
+        <v>8.2292052415342976E-3</v>
+      </c>
+      <c r="P13" s="66">
         <f t="shared" si="5"/>
-        <v>8.2292052415342976E-3</v>
-      </c>
-      <c r="P13" s="66">
-        <f t="shared" si="6"/>
         <v>7.8543122896674276E-3</v>
       </c>
     </row>
@@ -10112,31 +11468,31 @@
         <v>41264571.025399998</v>
       </c>
       <c r="J14" s="66">
+        <f t="shared" si="6"/>
+        <v>0.86439751671266363</v>
+      </c>
+      <c r="K14" s="66">
         <f t="shared" si="0"/>
-        <v>0.86439751671266363</v>
-      </c>
-      <c r="K14" s="66">
+        <v>0.41517545864783562</v>
+      </c>
+      <c r="L14" s="66">
         <f t="shared" si="1"/>
-        <v>0.41517545864783562</v>
-      </c>
-      <c r="L14" s="66">
+        <v>0.42928869176101703</v>
+      </c>
+      <c r="M14" s="66">
         <f t="shared" si="2"/>
-        <v>0.42928869176101703</v>
-      </c>
-      <c r="M14" s="66">
+        <v>1.7709001225606303E-2</v>
+      </c>
+      <c r="N14" s="66">
         <f t="shared" si="3"/>
-        <v>1.7709001225606303E-2</v>
-      </c>
-      <c r="N14" s="66">
+        <v>1.0873531107782013E-2</v>
+      </c>
+      <c r="O14" s="66">
         <f t="shared" si="4"/>
-        <v>1.0873531107782013E-2</v>
-      </c>
-      <c r="O14" s="66">
+        <v>4.5428457859383424E-3</v>
+      </c>
+      <c r="P14" s="66">
         <f t="shared" si="5"/>
-        <v>4.5428457859383424E-3</v>
-      </c>
-      <c r="P14" s="66">
-        <f t="shared" si="6"/>
         <v>3.2045527585561561E-3</v>
       </c>
     </row>
@@ -10169,31 +11525,31 @@
         <v>422516914.92000002</v>
       </c>
       <c r="J15" s="66">
+        <f t="shared" si="6"/>
+        <v>0.9996769290853682</v>
+      </c>
+      <c r="K15" s="66">
         <f t="shared" si="0"/>
-        <v>0.9996769290853682</v>
-      </c>
-      <c r="K15" s="66">
+        <v>0.99520603681342656</v>
+      </c>
+      <c r="L15" s="66">
         <f t="shared" si="1"/>
-        <v>0.99520603681342656</v>
-      </c>
-      <c r="L15" s="66">
+        <v>0.99467475940210126</v>
+      </c>
+      <c r="M15" s="66">
         <f t="shared" si="2"/>
-        <v>0.99467475940210126</v>
-      </c>
-      <c r="M15" s="66">
+        <v>1.7648537295098308E-3</v>
+      </c>
+      <c r="N15" s="66">
         <f t="shared" si="3"/>
-        <v>1.7648537295098308E-3</v>
-      </c>
-      <c r="N15" s="66">
+        <v>7.8752462917838582E-3</v>
+      </c>
+      <c r="O15" s="66">
         <f t="shared" si="4"/>
-        <v>7.8752462917838582E-3</v>
-      </c>
-      <c r="O15" s="66">
+        <v>9.4005960631003919E-3</v>
+      </c>
+      <c r="P15" s="66">
         <f t="shared" si="5"/>
-        <v>9.4005960631003919E-3</v>
-      </c>
-      <c r="P15" s="66">
-        <f t="shared" si="6"/>
         <v>5.9837166680413913E-3</v>
       </c>
     </row>
@@ -10312,22 +11668,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88" t="s">
+      <c r="C6" s="90"/>
+      <c r="D6" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="88"/>
-      <c r="F6" s="89" t="s">
+      <c r="E6" s="90"/>
+      <c r="F6" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="88"/>
-      <c r="H6" s="86" t="s">
+      <c r="G6" s="90"/>
+      <c r="H6" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="87"/>
+      <c r="I6" s="89"/>
       <c r="J6" s="7" t="s">
         <v>45</v>
       </c>
@@ -10337,11 +11693,11 @@
       <c r="L6" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="89" t="s">
+      <c r="M6" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="88"/>
-      <c r="O6" s="88"/>
+      <c r="N6" s="90"/>
+      <c r="O6" s="90"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
@@ -10641,22 +11997,22 @@
     </row>
     <row r="19" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A19" s="2"/>
-      <c r="B19" s="88" t="s">
+      <c r="B19" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="88"/>
-      <c r="D19" s="88" t="s">
+      <c r="C19" s="90"/>
+      <c r="D19" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="88"/>
-      <c r="F19" s="89" t="s">
+      <c r="E19" s="90"/>
+      <c r="F19" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="88"/>
-      <c r="H19" s="86" t="s">
+      <c r="G19" s="90"/>
+      <c r="H19" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I19" s="87"/>
+      <c r="I19" s="89"/>
       <c r="J19" s="67" t="s">
         <v>45</v>
       </c>
@@ -10666,11 +12022,11 @@
       <c r="L19" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="M19" s="89" t="s">
+      <c r="M19" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N19" s="88"/>
-      <c r="O19" s="88"/>
+      <c r="N19" s="90"/>
+      <c r="O19" s="90"/>
     </row>
     <row r="20" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
@@ -11193,8 +12549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51140CC8-C0B8-469A-8BAE-C9043CBCBC10}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26:P26"/>
+    <sheetView topLeftCell="F19" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21:P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11236,22 +12592,22 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93" t="s">
+      <c r="C6" s="96"/>
+      <c r="D6" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93" t="s">
+      <c r="E6" s="96"/>
+      <c r="F6" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="93"/>
-      <c r="H6" s="94" t="s">
+      <c r="G6" s="96"/>
+      <c r="H6" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="94"/>
+      <c r="I6" s="97"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -11261,11 +12617,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="93" t="s">
+      <c r="M6" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="93"/>
-      <c r="O6" s="93"/>
+      <c r="N6" s="96"/>
+      <c r="O6" s="96"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A7" s="77" t="s">
@@ -11594,22 +12950,22 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B18" s="93" t="s">
+      <c r="B18" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93" t="s">
+      <c r="C18" s="96"/>
+      <c r="D18" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93" t="s">
+      <c r="E18" s="96"/>
+      <c r="F18" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="93"/>
-      <c r="H18" s="94" t="s">
+      <c r="G18" s="96"/>
+      <c r="H18" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I18" s="94"/>
+      <c r="I18" s="97"/>
       <c r="J18" s="77" t="s">
         <v>45</v>
       </c>
@@ -11619,11 +12975,11 @@
       <c r="L18" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M18" s="93" t="s">
+      <c r="M18" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N18" s="93"/>
-      <c r="O18" s="93"/>
+      <c r="N18" s="96"/>
+      <c r="O18" s="96"/>
     </row>
     <row r="19" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A19" s="77" t="s">
@@ -12179,22 +13535,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93" t="s">
+      <c r="C6" s="96"/>
+      <c r="D6" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93" t="s">
+      <c r="E6" s="96"/>
+      <c r="F6" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="93"/>
-      <c r="H6" s="94" t="s">
+      <c r="G6" s="96"/>
+      <c r="H6" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="94"/>
+      <c r="I6" s="97"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -12204,11 +13560,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="93" t="s">
+      <c r="M6" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="93"/>
-      <c r="O6" s="93"/>
+      <c r="N6" s="96"/>
+      <c r="O6" s="96"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -12752,22 +14108,22 @@
     </row>
     <row r="3" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88" t="s">
+      <c r="C3" s="90"/>
+      <c r="D3" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="88"/>
-      <c r="F3" s="89" t="s">
+      <c r="E3" s="90"/>
+      <c r="F3" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="88"/>
-      <c r="H3" s="86" t="s">
+      <c r="G3" s="90"/>
+      <c r="H3" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="87"/>
+      <c r="I3" s="89"/>
       <c r="J3" s="48" t="s">
         <v>45</v>
       </c>
@@ -12777,11 +14133,11 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="89" t="s">
+      <c r="M3" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
     </row>
     <row r="4" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -14589,8 +15945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1814E241-F455-4452-B5DE-B4EE59F14CFA}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14:P14"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14623,22 +15979,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93" t="s">
+      <c r="C6" s="96"/>
+      <c r="D6" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93" t="s">
+      <c r="E6" s="96"/>
+      <c r="F6" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="93"/>
-      <c r="H6" s="94" t="s">
+      <c r="G6" s="96"/>
+      <c r="H6" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="94"/>
+      <c r="I6" s="97"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -14648,11 +16004,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="93" t="s">
+      <c r="M6" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="93"/>
-      <c r="O6" s="93"/>
+      <c r="N6" s="96"/>
+      <c r="O6" s="96"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -15195,22 +16551,22 @@
     </row>
     <row r="3" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="73"/>
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93" t="s">
+      <c r="C3" s="96"/>
+      <c r="D3" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93" t="s">
+      <c r="E3" s="96"/>
+      <c r="F3" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="93"/>
-      <c r="H3" s="94" t="s">
+      <c r="G3" s="96"/>
+      <c r="H3" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="94"/>
+      <c r="I3" s="97"/>
       <c r="J3" s="77" t="s">
         <v>45</v>
       </c>
@@ -15220,11 +16576,11 @@
       <c r="L3" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="93" t="s">
+      <c r="M3" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
       <c r="P3" s="73"/>
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -15768,22 +17124,22 @@
     </row>
     <row r="3" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="73"/>
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93" t="s">
+      <c r="C3" s="96"/>
+      <c r="D3" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93" t="s">
+      <c r="E3" s="96"/>
+      <c r="F3" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="93"/>
-      <c r="H3" s="94" t="s">
+      <c r="G3" s="96"/>
+      <c r="H3" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="94"/>
+      <c r="I3" s="97"/>
       <c r="J3" s="77" t="s">
         <v>45</v>
       </c>
@@ -15793,11 +17149,11 @@
       <c r="L3" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="93" t="s">
+      <c r="M3" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
       <c r="P3" s="73"/>
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -17390,29 +18746,29 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88" t="s">
+      <c r="C3" s="90"/>
+      <c r="D3" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="88"/>
-      <c r="F3" s="89" t="s">
+      <c r="E3" s="90"/>
+      <c r="F3" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="88"/>
+      <c r="G3" s="90"/>
       <c r="H3" s="7" t="s">
         <v>45</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="89" t="s">
+      <c r="J3" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -18904,22 +20260,22 @@
     </row>
     <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="52"/>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90" t="s">
+      <c r="C2" s="92"/>
+      <c r="D2" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90" t="s">
+      <c r="E2" s="92"/>
+      <c r="F2" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="90"/>
-      <c r="H2" s="91" t="s">
+      <c r="G2" s="92"/>
+      <c r="H2" s="93" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="91"/>
+      <c r="I2" s="93"/>
       <c r="J2" s="54" t="s">
         <v>45</v>
       </c>
@@ -18929,11 +20285,11 @@
       <c r="L2" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="90" t="s">
+      <c r="M2" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
     </row>
     <row r="3" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="52"/>
@@ -19475,22 +20831,22 @@
     </row>
     <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="26"/>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88" t="s">
+      <c r="C2" s="90"/>
+      <c r="D2" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="88"/>
-      <c r="F2" s="89" t="s">
+      <c r="E2" s="90"/>
+      <c r="F2" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="88"/>
-      <c r="H2" s="86" t="s">
+      <c r="G2" s="90"/>
+      <c r="H2" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="87"/>
+      <c r="I2" s="89"/>
       <c r="J2" s="48" t="s">
         <v>45</v>
       </c>
@@ -19500,11 +20856,11 @@
       <c r="L2" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="89" t="s">
+      <c r="M2" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
     </row>
     <row r="3" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26"/>
@@ -20044,22 +21400,22 @@
     </row>
     <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26"/>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88" t="s">
+      <c r="C3" s="90"/>
+      <c r="D3" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="88"/>
-      <c r="F3" s="89" t="s">
+      <c r="E3" s="90"/>
+      <c r="F3" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="88"/>
-      <c r="H3" s="86" t="s">
+      <c r="G3" s="90"/>
+      <c r="H3" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="87"/>
+      <c r="I3" s="89"/>
       <c r="J3" s="48" t="s">
         <v>45</v>
       </c>
@@ -20069,11 +21425,11 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="89" t="s">
+      <c r="M3" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
     </row>
     <row r="4" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="26"/>
@@ -20613,22 +21969,22 @@
     </row>
     <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26"/>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88" t="s">
+      <c r="C3" s="90"/>
+      <c r="D3" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="88"/>
-      <c r="F3" s="89" t="s">
+      <c r="E3" s="90"/>
+      <c r="F3" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="88"/>
-      <c r="H3" s="86" t="s">
+      <c r="G3" s="90"/>
+      <c r="H3" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="87"/>
+      <c r="I3" s="89"/>
       <c r="J3" s="48" t="s">
         <v>45</v>
       </c>
@@ -20638,11 +21994,11 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="89" t="s">
+      <c r="M3" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
     </row>
     <row r="4" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="26"/>
@@ -21314,10 +22670,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F173229C-1150-4B07-9313-8228C415AB22}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:C26"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -21325,239 +22681,361 @@
     <col min="1" max="1" width="34.9296875" customWidth="1"/>
     <col min="2" max="2" width="17.9296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.86328125" customWidth="1"/>
+    <col min="6" max="6" width="15.19921875" customWidth="1"/>
+    <col min="7" max="7" width="20.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="25" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="80"/>
-      <c r="B4" s="95" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="95"/>
-    </row>
-    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="96" t="s">
+      <c r="B4" s="98" t="s">
+        <v>213</v>
+      </c>
+      <c r="C4" s="94"/>
+      <c r="D4" s="98" t="s">
+        <v>214</v>
+      </c>
+      <c r="E4" s="94"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="96" t="s">
+      <c r="C5" s="85" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D5" s="85" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="85" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="66" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="66">
-        <v>65403223.600000001</v>
+        <v>83495490.400000006</v>
       </c>
       <c r="C6" s="66">
-        <v>3289023.0558799999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+        <v>15365890.752599999</v>
+      </c>
+      <c r="D6" s="66">
+        <v>80472677</v>
+      </c>
+      <c r="E6" s="66">
+        <v>10602970.279999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="66" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="66">
-        <v>31458333486.799999</v>
+        <v>31892287022.799999</v>
       </c>
       <c r="C7" s="66">
-        <v>93140878.649000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+        <v>294743606.00199997</v>
+      </c>
+      <c r="D7" s="66">
+        <v>31753582481.599998</v>
+      </c>
+      <c r="E7" s="66">
+        <v>222896080.50299999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="66" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="66">
-        <v>713763</v>
+        <v>711202.2</v>
       </c>
       <c r="C8" s="66">
-        <v>4668.7681030399999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+        <v>4471.9511356900002</v>
+      </c>
+      <c r="D8" s="66">
+        <v>707988.2</v>
+      </c>
+      <c r="E8" s="66">
+        <v>5871.9051559099998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="66" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="66">
-        <v>1461786</v>
+        <v>1483456.6</v>
       </c>
       <c r="C9" s="66">
-        <v>24201.016011700001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+        <v>21049.434895999999</v>
+      </c>
+      <c r="D9" s="66">
+        <v>1471555.2</v>
+      </c>
+      <c r="E9" s="66">
+        <v>35417.194905299999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="66" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="66">
-        <v>42183725662</v>
+        <v>42389392245</v>
       </c>
       <c r="C10" s="66">
-        <v>62319091.303900003</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+        <v>147337456.426</v>
+      </c>
+      <c r="D10" s="66">
+        <v>42602583568.800003</v>
+      </c>
+      <c r="E10" s="66">
+        <v>183113427.19299999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="66" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="66">
-        <v>22172169.800000001</v>
+        <v>22405457.600000001</v>
       </c>
       <c r="C11" s="66">
-        <v>450762.66297800001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+        <v>321401.23202400003</v>
+      </c>
+      <c r="D11" s="66">
+        <v>22175558</v>
+      </c>
+      <c r="E11" s="66">
+        <v>367514.69018099998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="66" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="66">
-        <v>64846325.799999997</v>
+        <v>66990423</v>
       </c>
       <c r="C12" s="66">
-        <v>4044395.09381</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+        <v>3559547.2307699998</v>
+      </c>
+      <c r="D12" s="66">
+        <v>67300587.599999994</v>
+      </c>
+      <c r="E12" s="66">
+        <v>1743471.8024800001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="66" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="66">
-        <v>416160398</v>
+        <v>892289521</v>
       </c>
       <c r="C13" s="66">
-        <v>21823144.353399999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="97" t="s">
+        <v>249422286.264</v>
+      </c>
+      <c r="D13" s="66">
+        <v>1212366021.4000001</v>
+      </c>
+      <c r="E13" s="66">
+        <v>445878619.82300001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="86" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="80"/>
-      <c r="B17" s="95" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="95"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="96" t="s">
+      <c r="B17" s="98" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" s="94"/>
+      <c r="D17" s="98" t="s">
+        <v>214</v>
+      </c>
+      <c r="E17" s="94"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="96" t="s">
+      <c r="B18" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="96" t="s">
+      <c r="C18" s="85" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D18" s="85" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="85" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="66" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="66">
-        <v>151772</v>
+        <v>165326.39999999999</v>
       </c>
       <c r="C19" s="66">
-        <v>31250.017708799998</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+        <v>88552.537543800005</v>
+      </c>
+      <c r="D19" s="66">
+        <v>162785.4</v>
+      </c>
+      <c r="E19" s="66">
+        <v>43077.178359799997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="66" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="66">
-        <v>6585151.4000000004</v>
+        <v>9269186.1999999993</v>
       </c>
       <c r="C20" s="66">
-        <v>1286932.6227599999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+        <v>8168144.4918200001</v>
+      </c>
+      <c r="D20" s="66">
+        <v>8735535</v>
+      </c>
+      <c r="E20" s="66">
+        <v>4701053.9160500001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="66" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="66">
-        <v>13998.4</v>
+        <v>13532.2</v>
       </c>
       <c r="C21" s="66">
-        <v>810.24381515699997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+        <v>1372.35584307</v>
+      </c>
+      <c r="D21" s="66">
+        <v>13889.4</v>
+      </c>
+      <c r="E21" s="66">
+        <v>899.22513310099998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="66" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="66">
-        <v>11084.2</v>
+        <v>10918.4</v>
       </c>
       <c r="C22" s="66">
-        <v>697.57935749299997</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+        <v>1371.3629133100001</v>
+      </c>
+      <c r="D22" s="66">
+        <v>11177.8</v>
+      </c>
+      <c r="E22" s="66">
+        <v>877.566726808</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="66" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="66">
-        <v>8731488.4000000004</v>
+        <v>29825266</v>
       </c>
       <c r="C23" s="66">
-        <v>6201094.71172</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+        <v>53445126.699500002</v>
+      </c>
+      <c r="D23" s="66">
+        <v>14200475.4</v>
+      </c>
+      <c r="E23" s="66">
+        <v>15759577.400699999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="66" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="66">
-        <v>571030.19999999995</v>
+        <v>599135</v>
       </c>
       <c r="C24" s="66">
-        <v>54596.198817900004</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+        <v>161460.95392100001</v>
+      </c>
+      <c r="D24" s="66">
+        <v>555900</v>
+      </c>
+      <c r="E24" s="66">
+        <v>47786.972325100003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="66" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="66">
-        <v>427796.4</v>
+        <v>471554.6</v>
       </c>
       <c r="C25" s="66">
-        <v>61332.597051199999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+        <v>172266.862287</v>
+      </c>
+      <c r="D25" s="66">
+        <v>429188.2</v>
+      </c>
+      <c r="E25" s="66">
+        <v>58791.971517899998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="66" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="66">
-        <v>1947502.6</v>
+        <v>2258070.6</v>
       </c>
       <c r="C26" s="66">
-        <v>987191.93594800006</v>
+        <v>1873577.88075</v>
+      </c>
+      <c r="D26" s="66">
+        <v>2198244.7999999998</v>
+      </c>
+      <c r="E26" s="66">
+        <v>1095869.89809</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated the results of derby with Alan's patch of using large pages on the code and date heaps
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="127" documentId="81D8B261ABBD5CBDED69DEB44BA5B0CD337C6AB9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{579568F4-A4B7-4F6B-8548-3455D4D6DB74}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="81D8B261ABBD5CBDED69DEB44BA5B0CD337C6AB9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{24E69823-C136-4C1A-90B8-79EEC686A0BC}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22672,8 +22672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F173229C-1150-4B07-9313-8228C415AB22}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -22730,16 +22730,16 @@
         <v>15</v>
       </c>
       <c r="B6" s="66">
-        <v>83495490.400000006</v>
+        <v>80605206</v>
       </c>
       <c r="C6" s="66">
-        <v>15365890.752599999</v>
+        <v>3040886.0836800002</v>
       </c>
       <c r="D6" s="66">
-        <v>80472677</v>
+        <v>78093460</v>
       </c>
       <c r="E6" s="66">
-        <v>10602970.279999999</v>
+        <v>14128786.833900001</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -22747,16 +22747,16 @@
         <v>2</v>
       </c>
       <c r="B7" s="66">
-        <v>31892287022.799999</v>
+        <v>33732068734.799999</v>
       </c>
       <c r="C7" s="66">
-        <v>294743606.00199997</v>
+        <v>58260190.090400003</v>
       </c>
       <c r="D7" s="66">
-        <v>31753582481.599998</v>
+        <v>33651012757</v>
       </c>
       <c r="E7" s="66">
-        <v>222896080.50299999</v>
+        <v>274588285.99800003</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
@@ -22764,16 +22764,16 @@
         <v>35</v>
       </c>
       <c r="B8" s="66">
-        <v>711202.2</v>
+        <v>754610</v>
       </c>
       <c r="C8" s="66">
-        <v>4471.9511356900002</v>
+        <v>2780.1559668499999</v>
       </c>
       <c r="D8" s="66">
-        <v>707988.2</v>
+        <v>749986.6</v>
       </c>
       <c r="E8" s="66">
-        <v>5871.9051559099998</v>
+        <v>4289.0407132600003</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -22781,16 +22781,16 @@
         <v>36</v>
       </c>
       <c r="B9" s="66">
-        <v>1483456.6</v>
+        <v>1579060.8</v>
       </c>
       <c r="C9" s="66">
-        <v>21049.434895999999</v>
+        <v>14561.519829999999</v>
       </c>
       <c r="D9" s="66">
-        <v>1471555.2</v>
+        <v>1547285.2</v>
       </c>
       <c r="E9" s="66">
-        <v>35417.194905299999</v>
+        <v>20143.231998899999</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -22798,16 +22798,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="66">
-        <v>42389392245</v>
+        <v>45152519547.400002</v>
       </c>
       <c r="C10" s="66">
-        <v>147337456.426</v>
+        <v>157726254.31900001</v>
       </c>
       <c r="D10" s="66">
-        <v>42602583568.800003</v>
+        <v>45389923102.199997</v>
       </c>
       <c r="E10" s="66">
-        <v>183113427.19299999</v>
+        <v>145877111.773</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
@@ -22815,16 +22815,16 @@
         <v>4</v>
       </c>
       <c r="B11" s="66">
-        <v>22405457.600000001</v>
+        <v>23503844.399999999</v>
       </c>
       <c r="C11" s="66">
-        <v>321401.23202400003</v>
+        <v>93035.3229727</v>
       </c>
       <c r="D11" s="66">
-        <v>22175558</v>
+        <v>23728844.800000001</v>
       </c>
       <c r="E11" s="66">
-        <v>367514.69018099998</v>
+        <v>114092.69380199999</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
@@ -22832,16 +22832,16 @@
         <v>6</v>
       </c>
       <c r="B12" s="66">
-        <v>66990423</v>
+        <v>69054272.400000006</v>
       </c>
       <c r="C12" s="66">
-        <v>3559547.2307699998</v>
+        <v>2506304.57883</v>
       </c>
       <c r="D12" s="66">
-        <v>67300587.599999994</v>
+        <v>70737430</v>
       </c>
       <c r="E12" s="66">
-        <v>1743471.8024800001</v>
+        <v>4009965.6546399998</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
@@ -22849,16 +22849,16 @@
         <v>20</v>
       </c>
       <c r="B13" s="66">
-        <v>892289521</v>
+        <v>871772778.79999995</v>
       </c>
       <c r="C13" s="66">
-        <v>249422286.264</v>
+        <v>302583081.12199998</v>
       </c>
       <c r="D13" s="66">
-        <v>1212366021.4000001</v>
+        <v>1239314739.8</v>
       </c>
       <c r="E13" s="66">
-        <v>445878619.82300001</v>
+        <v>190482375.76899999</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
@@ -22899,16 +22899,16 @@
         <v>15</v>
       </c>
       <c r="B19" s="66">
-        <v>165326.39999999999</v>
+        <v>148546.6</v>
       </c>
       <c r="C19" s="66">
-        <v>88552.537543800005</v>
+        <v>69071.475822099994</v>
       </c>
       <c r="D19" s="66">
-        <v>162785.4</v>
+        <v>175029.2</v>
       </c>
       <c r="E19" s="66">
-        <v>43077.178359799997</v>
+        <v>108651.97558100001</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
@@ -22916,16 +22916,16 @@
         <v>2</v>
       </c>
       <c r="B20" s="66">
-        <v>9269186.1999999993</v>
+        <v>8681713.8000000007</v>
       </c>
       <c r="C20" s="66">
-        <v>8168144.4918200001</v>
+        <v>7071760.9311199998</v>
       </c>
       <c r="D20" s="66">
-        <v>8735535</v>
+        <v>10152415.6</v>
       </c>
       <c r="E20" s="66">
-        <v>4701053.9160500001</v>
+        <v>9167515.1956799999</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
@@ -22933,16 +22933,16 @@
         <v>35</v>
       </c>
       <c r="B21" s="66">
-        <v>13532.2</v>
+        <v>13856.8</v>
       </c>
       <c r="C21" s="66">
-        <v>1372.35584307</v>
+        <v>923.38927868999997</v>
       </c>
       <c r="D21" s="66">
-        <v>13889.4</v>
+        <v>14505</v>
       </c>
       <c r="E21" s="66">
-        <v>899.22513310099998</v>
+        <v>1580.7342597700001</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
@@ -22950,16 +22950,16 @@
         <v>36</v>
       </c>
       <c r="B22" s="66">
-        <v>10918.4</v>
+        <v>11095</v>
       </c>
       <c r="C22" s="66">
-        <v>1371.3629133100001</v>
+        <v>875.22271451300003</v>
       </c>
       <c r="D22" s="66">
-        <v>11177.8</v>
+        <v>11752.8</v>
       </c>
       <c r="E22" s="66">
-        <v>877.566726808</v>
+        <v>1641.8301252000001</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
@@ -22967,16 +22967,16 @@
         <v>1</v>
       </c>
       <c r="B23" s="66">
-        <v>29825266</v>
+        <v>4214593</v>
       </c>
       <c r="C23" s="66">
-        <v>53445126.699500002</v>
+        <v>1191655.77477</v>
       </c>
       <c r="D23" s="66">
-        <v>14200475.4</v>
+        <v>5982800.5999999996</v>
       </c>
       <c r="E23" s="66">
-        <v>15759577.400699999</v>
+        <v>4689357.86436</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
@@ -22984,16 +22984,16 @@
         <v>4</v>
       </c>
       <c r="B24" s="66">
-        <v>599135</v>
+        <v>559252.4</v>
       </c>
       <c r="C24" s="66">
-        <v>161460.95392100001</v>
+        <v>20181.5485887</v>
       </c>
       <c r="D24" s="66">
-        <v>555900</v>
+        <v>549325.4</v>
       </c>
       <c r="E24" s="66">
-        <v>47786.972325100003</v>
+        <v>25316.881392499999</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
@@ -23001,16 +23001,16 @@
         <v>6</v>
       </c>
       <c r="B25" s="66">
-        <v>471554.6</v>
+        <v>391445.6</v>
       </c>
       <c r="C25" s="66">
-        <v>172266.862287</v>
+        <v>6316.7423122999999</v>
       </c>
       <c r="D25" s="66">
-        <v>429188.2</v>
+        <v>403337.4</v>
       </c>
       <c r="E25" s="66">
-        <v>58791.971517899998</v>
+        <v>33208.869915099996</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
@@ -23018,16 +23018,16 @@
         <v>20</v>
       </c>
       <c r="B26" s="66">
-        <v>2258070.6</v>
+        <v>1360418.8</v>
       </c>
       <c r="C26" s="66">
-        <v>1873577.88075</v>
+        <v>368852.98791999999</v>
       </c>
       <c r="D26" s="66">
-        <v>2198244.7999999998</v>
+        <v>1688186.8</v>
       </c>
       <c r="E26" s="66">
-        <v>1095869.89809</v>
+        <v>819883.52055100002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added statistics regarding SPECjvm2008 workloads
I/O activities, the size of the JIT code
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="142" documentId="81D8B261ABBD5CBDED69DEB44BA5B0CD337C6AB9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{2A7FE782-B088-48F6-98EA-C6F0D758B12C}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="81D8B261ABBD5CBDED69DEB44BA5B0CD337C6AB9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{12D60D06-7029-430A-B238-6AE367976E04}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -17,21 +17,22 @@
     <sheet name="clang-2core-usr" sheetId="16" r:id="rId7"/>
     <sheet name="clang-stats" sheetId="17" r:id="rId8"/>
     <sheet name="SPECjvm2008-derby" sheetId="30" r:id="rId9"/>
-    <sheet name="postgres summary" sheetId="27" r:id="rId10"/>
-    <sheet name="postgres-12GB-os" sheetId="25" r:id="rId11"/>
-    <sheet name="postgres-12GB-usr" sheetId="26" r:id="rId12"/>
-    <sheet name="postgres-10GB-os" sheetId="28" r:id="rId13"/>
-    <sheet name="postgres-10GB-usr" sheetId="29" r:id="rId14"/>
-    <sheet name="postgres-8GB-os" sheetId="23" r:id="rId15"/>
-    <sheet name="postgres-8GB-usr" sheetId="24" r:id="rId16"/>
-    <sheet name="postgres-4GB-os" sheetId="11" r:id="rId17"/>
-    <sheet name="postgres-4GB-usr" sheetId="8" r:id="rId18"/>
-    <sheet name="postgres-1GB-os" sheetId="18" r:id="rId19"/>
-    <sheet name="postgres-1GB-usr" sheetId="19" r:id="rId20"/>
-    <sheet name="octane-os" sheetId="20" r:id="rId21"/>
-    <sheet name="octane-usr" sheetId="21" r:id="rId22"/>
-    <sheet name="octane-stats" sheetId="22" r:id="rId23"/>
-    <sheet name="postgres_stats" sheetId="9" r:id="rId24"/>
+    <sheet name="SPECjvm2008-summary" sheetId="31" r:id="rId10"/>
+    <sheet name="postgres summary" sheetId="27" r:id="rId11"/>
+    <sheet name="postgres-12GB-os" sheetId="25" r:id="rId12"/>
+    <sheet name="postgres-12GB-usr" sheetId="26" r:id="rId13"/>
+    <sheet name="postgres-10GB-os" sheetId="28" r:id="rId14"/>
+    <sheet name="postgres-10GB-usr" sheetId="29" r:id="rId15"/>
+    <sheet name="postgres-8GB-os" sheetId="23" r:id="rId16"/>
+    <sheet name="postgres-8GB-usr" sheetId="24" r:id="rId17"/>
+    <sheet name="postgres-4GB-os" sheetId="11" r:id="rId18"/>
+    <sheet name="postgres-4GB-usr" sheetId="8" r:id="rId19"/>
+    <sheet name="postgres-1GB-os" sheetId="18" r:id="rId20"/>
+    <sheet name="postgres-1GB-usr" sheetId="19" r:id="rId21"/>
+    <sheet name="octane-os" sheetId="20" r:id="rId22"/>
+    <sheet name="octane-usr" sheetId="21" r:id="rId23"/>
+    <sheet name="octane-stats" sheetId="22" r:id="rId24"/>
+    <sheet name="postgres_stats" sheetId="9" r:id="rId25"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="254">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -700,9 +701,6 @@
     <t>10GB/2MB * 2 # of super pages for each iteration</t>
   </si>
   <si>
-    <t>java -jar SPECjvm2008.jar -ikv derby -ctf false -chf false</t>
-  </si>
-  <si>
     <t>OS</t>
   </si>
   <si>
@@ -725,6 +723,114 @@
   </si>
   <si>
     <t>ops/m</t>
+  </si>
+  <si>
+    <t>java -jar SPECjvm2008.jar derby</t>
+  </si>
+  <si>
+    <t>compiler.compiler</t>
+  </si>
+  <si>
+    <t>compiler.sunflow</t>
+  </si>
+  <si>
+    <t>compress</t>
+  </si>
+  <si>
+    <t>crypto.aes</t>
+  </si>
+  <si>
+    <t>crypto.rsa</t>
+  </si>
+  <si>
+    <t>crypto.signverify</t>
+  </si>
+  <si>
+    <t>derby</t>
+  </si>
+  <si>
+    <t>mpegaudio</t>
+  </si>
+  <si>
+    <t>scimark.fft.large</t>
+  </si>
+  <si>
+    <t>scimark.lu.large</t>
+  </si>
+  <si>
+    <t>scimark.sor.large</t>
+  </si>
+  <si>
+    <t>scimark.sparse.large</t>
+  </si>
+  <si>
+    <t>scimark.monte_carlo</t>
+  </si>
+  <si>
+    <t>serial</t>
+  </si>
+  <si>
+    <t>sunflow</t>
+  </si>
+  <si>
+    <t>xml.transform</t>
+  </si>
+  <si>
+    <t>xml.validation</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Occationally medium (300, 400 kBpS for writes),usually none</t>
+  </si>
+  <si>
+    <t>Sometimes 40 - 400 kBps for writes</t>
+  </si>
+  <si>
+    <t>Sometimes 8 - 600 kBps for writes</t>
+  </si>
+  <si>
+    <t>Sometimes 8 - 400 kBps for writes</t>
+  </si>
+  <si>
+    <t>a lot of IO</t>
+  </si>
+  <si>
+    <t>some IO 40 - 500 KBps for writes</t>
+  </si>
+  <si>
+    <t>IO 4 - 400 KbpS for writes</t>
+  </si>
+  <si>
+    <t>IO 4-400 Kbps for writes</t>
+  </si>
+  <si>
+    <t>Occationally 32 KbpS for writes</t>
+  </si>
+  <si>
+    <t>4-300 KBps for writes</t>
+  </si>
+  <si>
+    <t>12 - 300 KBps for writes</t>
+  </si>
+  <si>
+    <t>I/O (output of gstat)</t>
+  </si>
+  <si>
+    <t>4 - 415 KBps for writes</t>
+  </si>
+  <si>
+    <t>Sometimes 32, 64 KBps for writes, at the beginning it is 64 - 700</t>
+  </si>
+  <si>
+    <t>Ocationally 5 - 300 KBps for writes</t>
+  </si>
+  <si>
+    <t>Sometimes 15 - 300 KBps for writes</t>
+  </si>
+  <si>
+    <t>JIT code size (# of 4KB pages)</t>
   </si>
 </sst>
 </file>
@@ -951,7 +1057,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1124,6 +1230,9 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="43" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1136,8 +1245,8 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7017,6 +7126,222 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9BAF00-EAB6-4E4C-AFCD-518EB49BC392}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="83" customWidth="1"/>
+    <col min="3" max="3" width="23.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="99" t="s">
+        <v>236</v>
+      </c>
+      <c r="C2" s="4">
+        <v>5183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="99" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" s="4">
+        <v>4720</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A4" s="65" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4" s="83" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="65" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" s="83" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="65" t="s">
+        <v>223</v>
+      </c>
+      <c r="B6" s="83" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="65" t="s">
+        <v>224</v>
+      </c>
+      <c r="B7" s="83" t="s">
+        <v>240</v>
+      </c>
+      <c r="C7">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="65" t="s">
+        <v>225</v>
+      </c>
+      <c r="B8" s="83" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8">
+        <v>3131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="65" t="s">
+        <v>226</v>
+      </c>
+      <c r="B9" s="83" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="65" t="s">
+        <v>227</v>
+      </c>
+      <c r="B10" s="83" t="s">
+        <v>244</v>
+      </c>
+      <c r="C10">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="65" t="s">
+        <v>228</v>
+      </c>
+      <c r="B11" s="83" t="s">
+        <v>243</v>
+      </c>
+      <c r="C11">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="65" t="s">
+        <v>229</v>
+      </c>
+      <c r="B12" s="83" t="s">
+        <v>245</v>
+      </c>
+      <c r="C12">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="65" t="s">
+        <v>230</v>
+      </c>
+      <c r="B13" s="83" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="65" t="s">
+        <v>231</v>
+      </c>
+      <c r="B14" s="83" t="s">
+        <v>247</v>
+      </c>
+      <c r="C14">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="65" t="s">
+        <v>232</v>
+      </c>
+      <c r="B15" s="83" t="s">
+        <v>252</v>
+      </c>
+      <c r="C15">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="65" t="s">
+        <v>233</v>
+      </c>
+      <c r="B16" s="83" t="s">
+        <v>249</v>
+      </c>
+      <c r="C16">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+      <c r="A17" s="65" t="s">
+        <v>234</v>
+      </c>
+      <c r="B17" s="83" t="s">
+        <v>250</v>
+      </c>
+      <c r="C17">
+        <v>4685</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="65" t="s">
+        <v>235</v>
+      </c>
+      <c r="B18" s="83" t="s">
+        <v>251</v>
+      </c>
+      <c r="C18">
+        <v>2490</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DCC425-F9E0-4DC1-9C1B-7FD63E026DA8}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -7033,18 +7358,18 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="95" t="s">
+      <c r="E2" s="96" t="s">
         <v>206</v>
       </c>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
     </row>
     <row r="3" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -7191,11 +7516,11 @@
       <c r="B11" s="65"/>
       <c r="C11" s="65"/>
       <c r="D11" s="65"/>
-      <c r="E11" s="95" t="s">
+      <c r="E11" s="96" t="s">
         <v>206</v>
       </c>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
     </row>
     <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="65" t="s">
@@ -7339,11 +7664,11 @@
       <c r="A20" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="95" t="s">
+      <c r="E20" s="96" t="s">
         <v>206</v>
       </c>
-      <c r="F20" s="95"/>
-      <c r="G20" s="95"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="96"/>
     </row>
     <row r="21" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" s="65" t="s">
@@ -7495,7 +7820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638ACDA3-EFA6-47B5-8321-84E7AF859506}">
   <dimension ref="A1:P15"/>
   <sheetViews>
@@ -7614,22 +7939,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96" t="s">
+      <c r="C6" s="97"/>
+      <c r="D6" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96" t="s">
+      <c r="E6" s="97"/>
+      <c r="F6" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="97" t="s">
+      <c r="G6" s="97"/>
+      <c r="H6" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="97"/>
+      <c r="I6" s="98"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -7639,11 +7964,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="96" t="s">
+      <c r="M6" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="96"/>
-      <c r="O6" s="96"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -8158,7 +8483,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819BCD50-CCED-4858-989E-30CB05A9C1BE}">
   <dimension ref="A1:P15"/>
   <sheetViews>
@@ -8816,7 +9141,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E2C13C-499C-4223-89FD-CBE0858897C8}">
   <dimension ref="A1:T15"/>
   <sheetViews>
@@ -9532,7 +9857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD324841-F3D6-48B1-BFDE-305D75F58DD9}">
   <dimension ref="A1:T15"/>
   <sheetViews>
@@ -10248,7 +10573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99183D17-15E5-4DA6-B476-6E21D829BB49}">
   <dimension ref="A1:P15"/>
   <sheetViews>
@@ -10367,22 +10692,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96" t="s">
+      <c r="C6" s="97"/>
+      <c r="D6" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96" t="s">
+      <c r="E6" s="97"/>
+      <c r="F6" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="97" t="s">
+      <c r="G6" s="97"/>
+      <c r="H6" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="97"/>
+      <c r="I6" s="98"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -10392,11 +10717,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="96" t="s">
+      <c r="M6" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="96"/>
-      <c r="O6" s="96"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -10911,7 +11236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEB844F-EF6D-4427-9E28-001A58A9FD5B}">
   <dimension ref="A1:P15"/>
   <sheetViews>
@@ -11030,22 +11355,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96" t="s">
+      <c r="C6" s="97"/>
+      <c r="D6" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96" t="s">
+      <c r="E6" s="97"/>
+      <c r="F6" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="97" t="s">
+      <c r="G6" s="97"/>
+      <c r="H6" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="97"/>
+      <c r="I6" s="98"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -11055,11 +11380,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="96" t="s">
+      <c r="M6" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="96"/>
-      <c r="O6" s="96"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -11249,7 +11574,7 @@
         <v>1932588.55125</v>
       </c>
       <c r="J10" s="66">
-        <f t="shared" ref="J9:J15" si="6">D10/B10</f>
+        <f t="shared" ref="J10:J15" si="6">D10/B10</f>
         <v>0.9258286527011016</v>
       </c>
       <c r="K10" s="66">
@@ -11574,7 +11899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65049047-28B8-4D24-A307-ABB41DE3392E}">
   <dimension ref="A1:P28"/>
   <sheetViews>
@@ -12554,7 +12879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51140CC8-C0B8-469A-8BAE-C9043CBCBC10}">
   <dimension ref="A1:P27"/>
   <sheetViews>
@@ -12601,22 +12926,22 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96" t="s">
+      <c r="C6" s="97"/>
+      <c r="D6" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96" t="s">
+      <c r="E6" s="97"/>
+      <c r="F6" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="97" t="s">
+      <c r="G6" s="97"/>
+      <c r="H6" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="97"/>
+      <c r="I6" s="98"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -12626,11 +12951,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="96" t="s">
+      <c r="M6" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="96"/>
-      <c r="O6" s="96"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A7" s="77" t="s">
@@ -12959,22 +13284,22 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B18" s="96" t="s">
+      <c r="B18" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="96"/>
-      <c r="D18" s="96" t="s">
+      <c r="C18" s="97"/>
+      <c r="D18" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="96"/>
-      <c r="F18" s="96" t="s">
+      <c r="E18" s="97"/>
+      <c r="F18" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="96"/>
-      <c r="H18" s="97" t="s">
+      <c r="G18" s="97"/>
+      <c r="H18" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I18" s="97"/>
+      <c r="I18" s="98"/>
       <c r="J18" s="77" t="s">
         <v>45</v>
       </c>
@@ -12984,11 +13309,11 @@
       <c r="L18" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M18" s="96" t="s">
+      <c r="M18" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N18" s="96"/>
-      <c r="O18" s="96"/>
+      <c r="N18" s="97"/>
+      <c r="O18" s="97"/>
     </row>
     <row r="19" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A19" s="77" t="s">
@@ -13501,588 +13826,6 @@
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="M18:O18"/>
     <mergeCell ref="H6:I6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD3A0CC-C87B-4B2D-914D-368FCFB476B0}">
-  <dimension ref="A1:P15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.9296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.9296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A1" s="72" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A2" s="72" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A3" s="73" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="73"/>
-      <c r="B6" s="96" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="97" t="s">
-        <v>114</v>
-      </c>
-      <c r="I6" s="97"/>
-      <c r="J6" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="77" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" s="78" t="s">
-        <v>115</v>
-      </c>
-      <c r="M6" s="96" t="s">
-        <v>44</v>
-      </c>
-      <c r="N6" s="96"/>
-      <c r="O6" s="96"/>
-      <c r="P6" s="73"/>
-    </row>
-    <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="77" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="77" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="77" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" s="77" t="s">
-        <v>30</v>
-      </c>
-      <c r="O7" s="77" t="s">
-        <v>43</v>
-      </c>
-      <c r="P7" s="79" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A8" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="66">
-        <v>152191676326</v>
-      </c>
-      <c r="C8" s="66">
-        <v>361244554.66000003</v>
-      </c>
-      <c r="D8" s="66">
-        <v>153390874835</v>
-      </c>
-      <c r="E8" s="66">
-        <v>1330183544.27</v>
-      </c>
-      <c r="F8" s="66">
-        <v>152201793910</v>
-      </c>
-      <c r="G8" s="66">
-        <v>1149440198.28</v>
-      </c>
-      <c r="H8" s="66">
-        <v>151870700503</v>
-      </c>
-      <c r="I8" s="66">
-        <v>759082047.57500005</v>
-      </c>
-      <c r="J8" s="66">
-        <f>D8/B8</f>
-        <v>1.0078795275664831</v>
-      </c>
-      <c r="K8" s="66">
-        <f>F8/B8</f>
-        <v>1.0000664792204426</v>
-      </c>
-      <c r="L8" s="66">
-        <f>H8/B8</f>
-        <v>0.99789097649261405</v>
-      </c>
-      <c r="M8" s="66">
-        <f>C8/B8</f>
-        <v>2.3736157152655399E-3</v>
-      </c>
-      <c r="N8" s="66">
-        <f>E8/B8</f>
-        <v>8.7401859049157163E-3</v>
-      </c>
-      <c r="O8" s="66">
-        <f>G8/B8</f>
-        <v>7.552582546090484E-3</v>
-      </c>
-      <c r="P8" s="66">
-        <f>I8/B8</f>
-        <v>4.9876712439188807E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A9" s="66" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="66">
-        <v>329076787597</v>
-      </c>
-      <c r="C9" s="66">
-        <v>412474474.41000003</v>
-      </c>
-      <c r="D9" s="66">
-        <v>333412643633</v>
-      </c>
-      <c r="E9" s="66">
-        <v>10225280940.5</v>
-      </c>
-      <c r="F9" s="66">
-        <v>327746794941</v>
-      </c>
-      <c r="G9" s="66">
-        <v>2835431253.3299999</v>
-      </c>
-      <c r="H9" s="66">
-        <v>326503011286</v>
-      </c>
-      <c r="I9" s="66">
-        <v>14249038008</v>
-      </c>
-      <c r="J9" s="66">
-        <f t="shared" ref="J9:J15" si="0">D9/B9</f>
-        <v>1.013175818530567</v>
-      </c>
-      <c r="K9" s="66">
-        <f t="shared" ref="K9:K15" si="1">F9/B9</f>
-        <v>0.99595841242491778</v>
-      </c>
-      <c r="L9" s="66">
-        <f t="shared" ref="L9:L15" si="2">H9/B9</f>
-        <v>0.99217879714399082</v>
-      </c>
-      <c r="M9" s="66">
-        <f t="shared" ref="M9:M15" si="3">C9/B9</f>
-        <v>1.2534292601492512E-3</v>
-      </c>
-      <c r="N9" s="66">
-        <f t="shared" ref="N9:N15" si="4">E9/B9</f>
-        <v>3.1072629021230966E-2</v>
-      </c>
-      <c r="O9" s="66">
-        <f t="shared" ref="O9:O15" si="5">G9/B9</f>
-        <v>8.6163210539248886E-3</v>
-      </c>
-      <c r="P9" s="66">
-        <f t="shared" ref="P9:P15" si="6">I9/B9</f>
-        <v>4.3300039823683696E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A10" s="66" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="66">
-        <v>89180840.200000003</v>
-      </c>
-      <c r="C10" s="66">
-        <v>2451957.1950300001</v>
-      </c>
-      <c r="D10" s="66">
-        <v>58644676.600000001</v>
-      </c>
-      <c r="E10" s="66">
-        <v>823780.93678700004</v>
-      </c>
-      <c r="F10" s="66">
-        <v>74403713.599999994</v>
-      </c>
-      <c r="G10" s="66">
-        <v>3040391.5781800002</v>
-      </c>
-      <c r="H10" s="66">
-        <v>45688361.600000001</v>
-      </c>
-      <c r="I10" s="66">
-        <v>1261450.3099700001</v>
-      </c>
-      <c r="J10" s="66">
-        <f t="shared" si="0"/>
-        <v>0.65759277966524476</v>
-      </c>
-      <c r="K10" s="66">
-        <f t="shared" si="1"/>
-        <v>0.83430155438252973</v>
-      </c>
-      <c r="L10" s="66">
-        <f t="shared" si="2"/>
-        <v>0.51231140565100886</v>
-      </c>
-      <c r="M10" s="66">
-        <f t="shared" si="3"/>
-        <v>2.7494215007743333E-2</v>
-      </c>
-      <c r="N10" s="66">
-        <f t="shared" si="4"/>
-        <v>9.2371964083267297E-3</v>
-      </c>
-      <c r="O10" s="66">
-        <f t="shared" si="5"/>
-        <v>3.4092430295134181E-2</v>
-      </c>
-      <c r="P10" s="66">
-        <f t="shared" si="6"/>
-        <v>1.4144857876882843E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A11" s="66" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="66">
-        <v>9365000.4000000004</v>
-      </c>
-      <c r="C11" s="66">
-        <v>228787.049768</v>
-      </c>
-      <c r="D11" s="66">
-        <v>8007886.7999999998</v>
-      </c>
-      <c r="E11" s="66">
-        <v>399759.497836</v>
-      </c>
-      <c r="F11" s="66">
-        <v>2663329.2000000002</v>
-      </c>
-      <c r="G11" s="66">
-        <v>75350.234408100005</v>
-      </c>
-      <c r="H11" s="66">
-        <v>2482229.6</v>
-      </c>
-      <c r="I11" s="66">
-        <v>173898.34443699999</v>
-      </c>
-      <c r="J11" s="66">
-        <f t="shared" si="0"/>
-        <v>0.85508664794077316</v>
-      </c>
-      <c r="K11" s="66">
-        <f t="shared" si="1"/>
-        <v>0.28439178710552965</v>
-      </c>
-      <c r="L11" s="66">
-        <f t="shared" si="2"/>
-        <v>0.2650538701525309</v>
-      </c>
-      <c r="M11" s="66">
-        <f t="shared" si="3"/>
-        <v>2.4430009609823399E-2</v>
-      </c>
-      <c r="N11" s="66">
-        <f t="shared" si="4"/>
-        <v>4.2686543594381475E-2</v>
-      </c>
-      <c r="O11" s="66">
-        <f t="shared" si="5"/>
-        <v>8.045940329922464E-3</v>
-      </c>
-      <c r="P11" s="66">
-        <f t="shared" si="6"/>
-        <v>1.8568962841368376E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A12" s="66" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="66">
-        <v>13314226111.799999</v>
-      </c>
-      <c r="C12" s="66">
-        <v>69454845.720300004</v>
-      </c>
-      <c r="D12" s="66">
-        <v>13399672688.4</v>
-      </c>
-      <c r="E12" s="66">
-        <v>103191540.17900001</v>
-      </c>
-      <c r="F12" s="66">
-        <v>13040676172</v>
-      </c>
-      <c r="G12" s="66">
-        <v>90360710.352699995</v>
-      </c>
-      <c r="H12" s="66">
-        <v>13422847444.200001</v>
-      </c>
-      <c r="I12" s="66">
-        <v>149206640.58399999</v>
-      </c>
-      <c r="J12" s="66">
-        <f t="shared" si="0"/>
-        <v>1.006417690061931</v>
-      </c>
-      <c r="K12" s="66">
-        <f t="shared" si="1"/>
-        <v>0.97945431168864105</v>
-      </c>
-      <c r="L12" s="66">
-        <f t="shared" si="2"/>
-        <v>1.0081582911006546</v>
-      </c>
-      <c r="M12" s="66">
-        <f t="shared" si="3"/>
-        <v>5.2165890181738962E-3</v>
-      </c>
-      <c r="N12" s="66">
-        <f t="shared" si="4"/>
-        <v>7.7504722627133723E-3</v>
-      </c>
-      <c r="O12" s="66">
-        <f t="shared" si="5"/>
-        <v>6.7867790132102391E-3</v>
-      </c>
-      <c r="P12" s="66">
-        <f t="shared" si="6"/>
-        <v>1.120655750706852E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A13" s="66" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="66">
-        <v>4249181412.4000001</v>
-      </c>
-      <c r="C13" s="66">
-        <v>74875268.073799998</v>
-      </c>
-      <c r="D13" s="66">
-        <v>3608770196.1999998</v>
-      </c>
-      <c r="E13" s="66">
-        <v>42084565.060699999</v>
-      </c>
-      <c r="F13" s="66">
-        <v>3709863843.8000002</v>
-      </c>
-      <c r="G13" s="66">
-        <v>38265556.192500003</v>
-      </c>
-      <c r="H13" s="66">
-        <v>2956884482.8000002</v>
-      </c>
-      <c r="I13" s="66">
-        <v>58635839.859700002</v>
-      </c>
-      <c r="J13" s="66">
-        <f t="shared" si="0"/>
-        <v>0.84928597909913983</v>
-      </c>
-      <c r="K13" s="66">
-        <f t="shared" si="1"/>
-        <v>0.87307730213020363</v>
-      </c>
-      <c r="L13" s="66">
-        <f t="shared" si="2"/>
-        <v>0.6958715563828819</v>
-      </c>
-      <c r="M13" s="66">
-        <f t="shared" si="3"/>
-        <v>1.7621104115559366E-2</v>
-      </c>
-      <c r="N13" s="66">
-        <f t="shared" si="4"/>
-        <v>9.9041582310156109E-3</v>
-      </c>
-      <c r="O13" s="66">
-        <f t="shared" si="5"/>
-        <v>9.0053947992978379E-3</v>
-      </c>
-      <c r="P13" s="66">
-        <f t="shared" si="6"/>
-        <v>1.3799326074567764E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A14" s="66" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="66">
-        <v>1200047302.5999999</v>
-      </c>
-      <c r="C14" s="66">
-        <v>31685201.2073</v>
-      </c>
-      <c r="D14" s="66">
-        <v>959150403</v>
-      </c>
-      <c r="E14" s="66">
-        <v>33065051.145599999</v>
-      </c>
-      <c r="F14" s="66">
-        <v>345116464.19999999</v>
-      </c>
-      <c r="G14" s="66">
-        <v>8786793.3537900001</v>
-      </c>
-      <c r="H14" s="66">
-        <v>314148983</v>
-      </c>
-      <c r="I14" s="66">
-        <v>15612839.249600001</v>
-      </c>
-      <c r="J14" s="66">
-        <f t="shared" si="0"/>
-        <v>0.79926049658369536</v>
-      </c>
-      <c r="K14" s="66">
-        <f t="shared" si="1"/>
-        <v>0.28758571720654441</v>
-      </c>
-      <c r="L14" s="66">
-        <f t="shared" si="2"/>
-        <v>0.26178050008476395</v>
-      </c>
-      <c r="M14" s="66">
-        <f t="shared" si="3"/>
-        <v>2.6403293552388674E-2</v>
-      </c>
-      <c r="N14" s="66">
-        <f t="shared" si="4"/>
-        <v>2.7553123176029714E-2</v>
-      </c>
-      <c r="O14" s="66">
-        <f t="shared" si="5"/>
-        <v>7.3220391685833545E-3</v>
-      </c>
-      <c r="P14" s="66">
-        <f t="shared" si="6"/>
-        <v>1.3010186528292274E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A15" s="66" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="66">
-        <v>54409205.399999999</v>
-      </c>
-      <c r="C15" s="66">
-        <v>1367307.0280200001</v>
-      </c>
-      <c r="D15" s="66">
-        <v>55558445.600000001</v>
-      </c>
-      <c r="E15" s="66">
-        <v>8566182.6584099997</v>
-      </c>
-      <c r="F15" s="66">
-        <v>53866379.200000003</v>
-      </c>
-      <c r="G15" s="66">
-        <v>1758501.7690600001</v>
-      </c>
-      <c r="H15" s="66">
-        <v>53714283.799999997</v>
-      </c>
-      <c r="I15" s="66">
-        <v>1412663.2752100001</v>
-      </c>
-      <c r="J15" s="66">
-        <f t="shared" si="0"/>
-        <v>1.0211221647431006</v>
-      </c>
-      <c r="K15" s="66">
-        <f t="shared" si="1"/>
-        <v>0.99002326543809449</v>
-      </c>
-      <c r="L15" s="66">
-        <f t="shared" si="2"/>
-        <v>0.98722786714323163</v>
-      </c>
-      <c r="M15" s="66">
-        <f t="shared" si="3"/>
-        <v>2.5130067935526221E-2</v>
-      </c>
-      <c r="N15" s="66">
-        <f t="shared" si="4"/>
-        <v>0.15743995148309958</v>
-      </c>
-      <c r="O15" s="66">
-        <f t="shared" si="5"/>
-        <v>3.2319931087617028E-2</v>
-      </c>
-      <c r="P15" s="66">
-        <f t="shared" si="6"/>
-        <v>2.5963681417960943E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="M6:O6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15951,6 +15694,588 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD3A0CC-C87B-4B2D-914D-368FCFB476B0}">
+  <dimension ref="A1:P15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A1" s="72" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A2" s="72" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A3" s="73" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="73"/>
+      <c r="B6" s="97" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="97"/>
+      <c r="H6" s="98" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" s="98"/>
+      <c r="J6" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6" s="97" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
+      <c r="P6" s="73"/>
+    </row>
+    <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="77" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="77" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="77" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="77" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="P7" s="79" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A8" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="66">
+        <v>152191676326</v>
+      </c>
+      <c r="C8" s="66">
+        <v>361244554.66000003</v>
+      </c>
+      <c r="D8" s="66">
+        <v>153390874835</v>
+      </c>
+      <c r="E8" s="66">
+        <v>1330183544.27</v>
+      </c>
+      <c r="F8" s="66">
+        <v>152201793910</v>
+      </c>
+      <c r="G8" s="66">
+        <v>1149440198.28</v>
+      </c>
+      <c r="H8" s="66">
+        <v>151870700503</v>
+      </c>
+      <c r="I8" s="66">
+        <v>759082047.57500005</v>
+      </c>
+      <c r="J8" s="66">
+        <f>D8/B8</f>
+        <v>1.0078795275664831</v>
+      </c>
+      <c r="K8" s="66">
+        <f>F8/B8</f>
+        <v>1.0000664792204426</v>
+      </c>
+      <c r="L8" s="66">
+        <f>H8/B8</f>
+        <v>0.99789097649261405</v>
+      </c>
+      <c r="M8" s="66">
+        <f>C8/B8</f>
+        <v>2.3736157152655399E-3</v>
+      </c>
+      <c r="N8" s="66">
+        <f>E8/B8</f>
+        <v>8.7401859049157163E-3</v>
+      </c>
+      <c r="O8" s="66">
+        <f>G8/B8</f>
+        <v>7.552582546090484E-3</v>
+      </c>
+      <c r="P8" s="66">
+        <f>I8/B8</f>
+        <v>4.9876712439188807E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A9" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="66">
+        <v>329076787597</v>
+      </c>
+      <c r="C9" s="66">
+        <v>412474474.41000003</v>
+      </c>
+      <c r="D9" s="66">
+        <v>333412643633</v>
+      </c>
+      <c r="E9" s="66">
+        <v>10225280940.5</v>
+      </c>
+      <c r="F9" s="66">
+        <v>327746794941</v>
+      </c>
+      <c r="G9" s="66">
+        <v>2835431253.3299999</v>
+      </c>
+      <c r="H9" s="66">
+        <v>326503011286</v>
+      </c>
+      <c r="I9" s="66">
+        <v>14249038008</v>
+      </c>
+      <c r="J9" s="66">
+        <f t="shared" ref="J9:J15" si="0">D9/B9</f>
+        <v>1.013175818530567</v>
+      </c>
+      <c r="K9" s="66">
+        <f t="shared" ref="K9:K15" si="1">F9/B9</f>
+        <v>0.99595841242491778</v>
+      </c>
+      <c r="L9" s="66">
+        <f t="shared" ref="L9:L15" si="2">H9/B9</f>
+        <v>0.99217879714399082</v>
+      </c>
+      <c r="M9" s="66">
+        <f t="shared" ref="M9:M15" si="3">C9/B9</f>
+        <v>1.2534292601492512E-3</v>
+      </c>
+      <c r="N9" s="66">
+        <f t="shared" ref="N9:N15" si="4">E9/B9</f>
+        <v>3.1072629021230966E-2</v>
+      </c>
+      <c r="O9" s="66">
+        <f t="shared" ref="O9:O15" si="5">G9/B9</f>
+        <v>8.6163210539248886E-3</v>
+      </c>
+      <c r="P9" s="66">
+        <f t="shared" ref="P9:P15" si="6">I9/B9</f>
+        <v>4.3300039823683696E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A10" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="66">
+        <v>89180840.200000003</v>
+      </c>
+      <c r="C10" s="66">
+        <v>2451957.1950300001</v>
+      </c>
+      <c r="D10" s="66">
+        <v>58644676.600000001</v>
+      </c>
+      <c r="E10" s="66">
+        <v>823780.93678700004</v>
+      </c>
+      <c r="F10" s="66">
+        <v>74403713.599999994</v>
+      </c>
+      <c r="G10" s="66">
+        <v>3040391.5781800002</v>
+      </c>
+      <c r="H10" s="66">
+        <v>45688361.600000001</v>
+      </c>
+      <c r="I10" s="66">
+        <v>1261450.3099700001</v>
+      </c>
+      <c r="J10" s="66">
+        <f t="shared" si="0"/>
+        <v>0.65759277966524476</v>
+      </c>
+      <c r="K10" s="66">
+        <f t="shared" si="1"/>
+        <v>0.83430155438252973</v>
+      </c>
+      <c r="L10" s="66">
+        <f t="shared" si="2"/>
+        <v>0.51231140565100886</v>
+      </c>
+      <c r="M10" s="66">
+        <f t="shared" si="3"/>
+        <v>2.7494215007743333E-2</v>
+      </c>
+      <c r="N10" s="66">
+        <f t="shared" si="4"/>
+        <v>9.2371964083267297E-3</v>
+      </c>
+      <c r="O10" s="66">
+        <f t="shared" si="5"/>
+        <v>3.4092430295134181E-2</v>
+      </c>
+      <c r="P10" s="66">
+        <f t="shared" si="6"/>
+        <v>1.4144857876882843E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A11" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="66">
+        <v>9365000.4000000004</v>
+      </c>
+      <c r="C11" s="66">
+        <v>228787.049768</v>
+      </c>
+      <c r="D11" s="66">
+        <v>8007886.7999999998</v>
+      </c>
+      <c r="E11" s="66">
+        <v>399759.497836</v>
+      </c>
+      <c r="F11" s="66">
+        <v>2663329.2000000002</v>
+      </c>
+      <c r="G11" s="66">
+        <v>75350.234408100005</v>
+      </c>
+      <c r="H11" s="66">
+        <v>2482229.6</v>
+      </c>
+      <c r="I11" s="66">
+        <v>173898.34443699999</v>
+      </c>
+      <c r="J11" s="66">
+        <f t="shared" si="0"/>
+        <v>0.85508664794077316</v>
+      </c>
+      <c r="K11" s="66">
+        <f t="shared" si="1"/>
+        <v>0.28439178710552965</v>
+      </c>
+      <c r="L11" s="66">
+        <f t="shared" si="2"/>
+        <v>0.2650538701525309</v>
+      </c>
+      <c r="M11" s="66">
+        <f t="shared" si="3"/>
+        <v>2.4430009609823399E-2</v>
+      </c>
+      <c r="N11" s="66">
+        <f t="shared" si="4"/>
+        <v>4.2686543594381475E-2</v>
+      </c>
+      <c r="O11" s="66">
+        <f t="shared" si="5"/>
+        <v>8.045940329922464E-3</v>
+      </c>
+      <c r="P11" s="66">
+        <f t="shared" si="6"/>
+        <v>1.8568962841368376E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A12" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="66">
+        <v>13314226111.799999</v>
+      </c>
+      <c r="C12" s="66">
+        <v>69454845.720300004</v>
+      </c>
+      <c r="D12" s="66">
+        <v>13399672688.4</v>
+      </c>
+      <c r="E12" s="66">
+        <v>103191540.17900001</v>
+      </c>
+      <c r="F12" s="66">
+        <v>13040676172</v>
+      </c>
+      <c r="G12" s="66">
+        <v>90360710.352699995</v>
+      </c>
+      <c r="H12" s="66">
+        <v>13422847444.200001</v>
+      </c>
+      <c r="I12" s="66">
+        <v>149206640.58399999</v>
+      </c>
+      <c r="J12" s="66">
+        <f t="shared" si="0"/>
+        <v>1.006417690061931</v>
+      </c>
+      <c r="K12" s="66">
+        <f t="shared" si="1"/>
+        <v>0.97945431168864105</v>
+      </c>
+      <c r="L12" s="66">
+        <f t="shared" si="2"/>
+        <v>1.0081582911006546</v>
+      </c>
+      <c r="M12" s="66">
+        <f t="shared" si="3"/>
+        <v>5.2165890181738962E-3</v>
+      </c>
+      <c r="N12" s="66">
+        <f t="shared" si="4"/>
+        <v>7.7504722627133723E-3</v>
+      </c>
+      <c r="O12" s="66">
+        <f t="shared" si="5"/>
+        <v>6.7867790132102391E-3</v>
+      </c>
+      <c r="P12" s="66">
+        <f t="shared" si="6"/>
+        <v>1.120655750706852E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A13" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="66">
+        <v>4249181412.4000001</v>
+      </c>
+      <c r="C13" s="66">
+        <v>74875268.073799998</v>
+      </c>
+      <c r="D13" s="66">
+        <v>3608770196.1999998</v>
+      </c>
+      <c r="E13" s="66">
+        <v>42084565.060699999</v>
+      </c>
+      <c r="F13" s="66">
+        <v>3709863843.8000002</v>
+      </c>
+      <c r="G13" s="66">
+        <v>38265556.192500003</v>
+      </c>
+      <c r="H13" s="66">
+        <v>2956884482.8000002</v>
+      </c>
+      <c r="I13" s="66">
+        <v>58635839.859700002</v>
+      </c>
+      <c r="J13" s="66">
+        <f t="shared" si="0"/>
+        <v>0.84928597909913983</v>
+      </c>
+      <c r="K13" s="66">
+        <f t="shared" si="1"/>
+        <v>0.87307730213020363</v>
+      </c>
+      <c r="L13" s="66">
+        <f t="shared" si="2"/>
+        <v>0.6958715563828819</v>
+      </c>
+      <c r="M13" s="66">
+        <f t="shared" si="3"/>
+        <v>1.7621104115559366E-2</v>
+      </c>
+      <c r="N13" s="66">
+        <f t="shared" si="4"/>
+        <v>9.9041582310156109E-3</v>
+      </c>
+      <c r="O13" s="66">
+        <f t="shared" si="5"/>
+        <v>9.0053947992978379E-3</v>
+      </c>
+      <c r="P13" s="66">
+        <f t="shared" si="6"/>
+        <v>1.3799326074567764E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A14" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="66">
+        <v>1200047302.5999999</v>
+      </c>
+      <c r="C14" s="66">
+        <v>31685201.2073</v>
+      </c>
+      <c r="D14" s="66">
+        <v>959150403</v>
+      </c>
+      <c r="E14" s="66">
+        <v>33065051.145599999</v>
+      </c>
+      <c r="F14" s="66">
+        <v>345116464.19999999</v>
+      </c>
+      <c r="G14" s="66">
+        <v>8786793.3537900001</v>
+      </c>
+      <c r="H14" s="66">
+        <v>314148983</v>
+      </c>
+      <c r="I14" s="66">
+        <v>15612839.249600001</v>
+      </c>
+      <c r="J14" s="66">
+        <f t="shared" si="0"/>
+        <v>0.79926049658369536</v>
+      </c>
+      <c r="K14" s="66">
+        <f t="shared" si="1"/>
+        <v>0.28758571720654441</v>
+      </c>
+      <c r="L14" s="66">
+        <f t="shared" si="2"/>
+        <v>0.26178050008476395</v>
+      </c>
+      <c r="M14" s="66">
+        <f t="shared" si="3"/>
+        <v>2.6403293552388674E-2</v>
+      </c>
+      <c r="N14" s="66">
+        <f t="shared" si="4"/>
+        <v>2.7553123176029714E-2</v>
+      </c>
+      <c r="O14" s="66">
+        <f t="shared" si="5"/>
+        <v>7.3220391685833545E-3</v>
+      </c>
+      <c r="P14" s="66">
+        <f t="shared" si="6"/>
+        <v>1.3010186528292274E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A15" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="66">
+        <v>54409205.399999999</v>
+      </c>
+      <c r="C15" s="66">
+        <v>1367307.0280200001</v>
+      </c>
+      <c r="D15" s="66">
+        <v>55558445.600000001</v>
+      </c>
+      <c r="E15" s="66">
+        <v>8566182.6584099997</v>
+      </c>
+      <c r="F15" s="66">
+        <v>53866379.200000003</v>
+      </c>
+      <c r="G15" s="66">
+        <v>1758501.7690600001</v>
+      </c>
+      <c r="H15" s="66">
+        <v>53714283.799999997</v>
+      </c>
+      <c r="I15" s="66">
+        <v>1412663.2752100001</v>
+      </c>
+      <c r="J15" s="66">
+        <f t="shared" si="0"/>
+        <v>1.0211221647431006</v>
+      </c>
+      <c r="K15" s="66">
+        <f t="shared" si="1"/>
+        <v>0.99002326543809449</v>
+      </c>
+      <c r="L15" s="66">
+        <f t="shared" si="2"/>
+        <v>0.98722786714323163</v>
+      </c>
+      <c r="M15" s="66">
+        <f t="shared" si="3"/>
+        <v>2.5130067935526221E-2</v>
+      </c>
+      <c r="N15" s="66">
+        <f t="shared" si="4"/>
+        <v>0.15743995148309958</v>
+      </c>
+      <c r="O15" s="66">
+        <f t="shared" si="5"/>
+        <v>3.2319931087617028E-2</v>
+      </c>
+      <c r="P15" s="66">
+        <f t="shared" si="6"/>
+        <v>2.5963681417960943E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="M6:O6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1814E241-F455-4452-B5DE-B4EE59F14CFA}">
   <dimension ref="A1:P15"/>
   <sheetViews>
@@ -15988,22 +16313,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96" t="s">
+      <c r="C6" s="97"/>
+      <c r="D6" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96" t="s">
+      <c r="E6" s="97"/>
+      <c r="F6" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="97" t="s">
+      <c r="G6" s="97"/>
+      <c r="H6" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="97"/>
+      <c r="I6" s="98"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -16013,11 +16338,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="96" t="s">
+      <c r="M6" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="96"/>
-      <c r="O6" s="96"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -16532,7 +16857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC958D8-824A-4FFE-8EFB-EA4CAF2DCC74}">
   <dimension ref="A1:P12"/>
   <sheetViews>
@@ -16560,22 +16885,22 @@
     </row>
     <row r="3" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="73"/>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96" t="s">
+      <c r="C3" s="97"/>
+      <c r="D3" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96" t="s">
+      <c r="E3" s="97"/>
+      <c r="F3" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="96"/>
-      <c r="H3" s="97" t="s">
+      <c r="G3" s="97"/>
+      <c r="H3" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="97"/>
+      <c r="I3" s="98"/>
       <c r="J3" s="77" t="s">
         <v>45</v>
       </c>
@@ -16585,11 +16910,11 @@
       <c r="L3" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="96" t="s">
+      <c r="M3" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
       <c r="P3" s="73"/>
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -17104,7 +17429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F72758A-17BC-4C1E-98B0-DDD6331D597C}">
   <dimension ref="A1:P12"/>
   <sheetViews>
@@ -17133,22 +17458,22 @@
     </row>
     <row r="3" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="73"/>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96" t="s">
+      <c r="C3" s="97"/>
+      <c r="D3" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96" t="s">
+      <c r="E3" s="97"/>
+      <c r="F3" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="96"/>
-      <c r="H3" s="97" t="s">
+      <c r="G3" s="97"/>
+      <c r="H3" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="97"/>
+      <c r="I3" s="98"/>
       <c r="J3" s="77" t="s">
         <v>45</v>
       </c>
@@ -17158,11 +17483,11 @@
       <c r="L3" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="96" t="s">
+      <c r="M3" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
       <c r="P3" s="73"/>
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -17677,7 +18002,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C510FE-BA24-4F4C-B882-A73942D255FE}">
   <dimension ref="A1:D31"/>
   <sheetViews>
@@ -18045,7 +18370,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5A357B-AD95-4B57-AFAC-6E90E36724A8}">
   <dimension ref="A1:H59"/>
   <sheetViews>
@@ -22681,9 +23006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F173229C-1150-4B07-9313-8228C415AB22}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -22698,24 +23021,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="25" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="80"/>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="94" t="s">
+        <v>213</v>
+      </c>
+      <c r="C4" s="95"/>
+      <c r="D4" s="94" t="s">
         <v>214</v>
       </c>
-      <c r="C4" s="94"/>
-      <c r="D4" s="98" t="s">
-        <v>215</v>
-      </c>
-      <c r="E4" s="94"/>
+      <c r="E4" s="95"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="85" t="s">
@@ -22872,19 +23195,19 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="86" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="80"/>
-      <c r="B17" s="98" t="s">
+      <c r="B17" s="94" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" s="95"/>
+      <c r="D17" s="94" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="94"/>
-      <c r="D17" s="98" t="s">
-        <v>215</v>
-      </c>
-      <c r="E17" s="94"/>
+      <c r="E17" s="95"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="85" t="s">
@@ -23041,12 +23364,12 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B28" s="65" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="66" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B29" s="65">
         <v>215.28</v>
@@ -23057,7 +23380,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="66" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B30">
         <v>216.15</v>

</xml_diff>

<commit_message>
added results of disable UseLargePage for specjvm compiler.compiler
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="253" documentId="81D8B261ABBD5CBDED69DEB44BA5B0CD337C6AB9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{212A868A-9151-41A2-BB5E-ED6FE34DAF66}"/>
+  <xr:revisionPtr revIDLastSave="257" documentId="81D8B261ABBD5CBDED69DEB44BA5B0CD337C6AB9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{0E7C9352-FA9F-4958-BD75-7AA0B4249CD6}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7134,15 +7134,16 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="35.19921875" customWidth="1"/>
-    <col min="2" max="2" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
@@ -7191,105 +7192,137 @@
       <c r="A6" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="66">
         <v>848515828.20000005</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="66">
         <v>31125912.630600002</v>
       </c>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
+      <c r="D6" s="66">
+        <v>840330563</v>
+      </c>
+      <c r="E6" s="66">
+        <v>24387713.008200001</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="66">
         <v>140402962470</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="66">
         <v>651623475.11199999</v>
       </c>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
+      <c r="D7" s="66">
+        <v>140348996038</v>
+      </c>
+      <c r="E7" s="66">
+        <v>616223577.551</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="66">
         <v>2644396</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="66">
         <v>779678.30018699996</v>
       </c>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
+      <c r="D8" s="66">
+        <v>2330265.7999999998</v>
+      </c>
+      <c r="E8" s="66">
+        <v>420625.344896</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="66">
         <v>3505292.4</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="66">
         <v>394822.744389</v>
       </c>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
+      <c r="D9" s="66">
+        <v>3674564</v>
+      </c>
+      <c r="E9" s="66">
+        <v>26949.256546299999</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="66">
         <v>209033496735</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="66">
         <v>1325523106.99</v>
       </c>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
+      <c r="D10" s="66">
+        <v>208488972487</v>
+      </c>
+      <c r="E10" s="66">
+        <v>890197947.329</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="66">
         <v>138323111.59999999</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="66">
         <v>19480498.205499999</v>
       </c>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
+      <c r="D11" s="66">
+        <v>153799543</v>
+      </c>
+      <c r="E11" s="66">
+        <v>42691851.003799997</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="66">
         <v>171923672.59999999</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="66">
         <v>6170074.2861400004</v>
       </c>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
+      <c r="D12" s="66">
+        <v>177880719.59999999</v>
+      </c>
+      <c r="E12" s="66">
+        <v>10236150.110099999</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="31">
+      <c r="B13" s="66">
         <v>2547202360.8000002</v>
       </c>
-      <c r="C13" s="31">
+      <c r="C13" s="66">
         <v>123523596.719</v>
       </c>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
+      <c r="D13" s="66">
+        <v>2446884702.4000001</v>
+      </c>
+      <c r="E13" s="66">
+        <v>135724290.56</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="66"/>
@@ -7346,105 +7379,137 @@
       <c r="A19" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="31">
+      <c r="B19" s="66">
         <v>64023665052.199997</v>
       </c>
-      <c r="C19" s="31">
+      <c r="C19" s="66">
         <v>901945315.08700001</v>
       </c>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
+      <c r="D19" s="66">
+        <v>64170277315</v>
+      </c>
+      <c r="E19" s="66">
+        <v>1127219042.1600001</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="31">
+      <c r="B20" s="66">
         <v>2473983034190</v>
       </c>
-      <c r="C20" s="31">
+      <c r="C20" s="66">
         <v>14971484657</v>
       </c>
-      <c r="D20" s="66"/>
-      <c r="E20" s="66"/>
+      <c r="D20" s="66">
+        <v>2478098843780</v>
+      </c>
+      <c r="E20" s="66">
+        <v>16463842483</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="31">
+      <c r="B21" s="66">
         <v>19486541.199999999</v>
       </c>
-      <c r="C21" s="31">
+      <c r="C21" s="66">
         <v>1957661.6367800001</v>
       </c>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
+      <c r="D21" s="66">
+        <v>19266334</v>
+      </c>
+      <c r="E21" s="66">
+        <v>1437223.44961</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="31">
+      <c r="B22" s="66">
         <v>217977453.80000001</v>
       </c>
-      <c r="C22" s="31">
+      <c r="C22" s="66">
         <v>11480066.7805</v>
       </c>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
+      <c r="D22" s="66">
+        <v>203274321</v>
+      </c>
+      <c r="E22" s="66">
+        <v>10443566.922800001</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="31">
+      <c r="B23" s="66">
         <v>2713558839040</v>
       </c>
-      <c r="C23" s="31">
+      <c r="C23" s="66">
         <v>20899612744.799999</v>
       </c>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
+      <c r="D23" s="66">
+        <v>2708449528150</v>
+      </c>
+      <c r="E23" s="66">
+        <v>23185814766.799999</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="31">
+      <c r="B24" s="66">
         <v>1733947706</v>
       </c>
-      <c r="C24" s="31">
+      <c r="C24" s="66">
         <v>645790981.324</v>
       </c>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
+      <c r="D24" s="66">
+        <v>1349642605.8</v>
+      </c>
+      <c r="E24" s="66">
+        <v>165785934.153</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="31">
+      <c r="B25" s="66">
         <v>15451772579</v>
       </c>
-      <c r="C25" s="31">
+      <c r="C25" s="66">
         <v>768428597.255</v>
       </c>
-      <c r="D25" s="66"/>
-      <c r="E25" s="66"/>
+      <c r="D25" s="66">
+        <v>15726153788.200001</v>
+      </c>
+      <c r="E25" s="66">
+        <v>948509332.69700003</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="31">
+      <c r="B26" s="66">
         <v>255258511247</v>
       </c>
-      <c r="C26" s="31">
+      <c r="C26" s="66">
         <v>1877302684.26</v>
       </c>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
+      <c r="D26" s="66">
+        <v>254163773567</v>
+      </c>
+      <c r="E26" s="66">
+        <v>1935192897</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
added ITLB VS DTLB misses for SPECJvm workloads
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="257" documentId="81D8B261ABBD5CBDED69DEB44BA5B0CD337C6AB9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{0E7C9352-FA9F-4958-BD75-7AA0B4249CD6}"/>
+  <xr:revisionPtr revIDLastSave="285" documentId="81D8B261ABBD5CBDED69DEB44BA5B0CD337C6AB9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{0BC0448A-BADD-4B8B-A3D0-2E5C76B871F9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="257">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -835,6 +835,12 @@
   </si>
   <si>
     <t>java -jar SPECjvm2008.jar compiler.compiler</t>
+  </si>
+  <si>
+    <t>Disable UseLargePage in jvm (Disable alignment)</t>
+  </si>
+  <si>
+    <t>rerun shared_ptp to reduce the standard deviation from rows 21 to 23</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1067,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1213,9 +1219,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1251,6 +1254,19 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5155,22 +5171,22 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="57" x14ac:dyDescent="0.45">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88" t="s">
+      <c r="C3" s="87"/>
+      <c r="D3" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88" t="s">
+      <c r="E3" s="87"/>
+      <c r="F3" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="88"/>
-      <c r="H3" s="89" t="s">
+      <c r="G3" s="87"/>
+      <c r="H3" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="90"/>
+      <c r="I3" s="89"/>
       <c r="J3" s="33" t="s">
         <v>45</v>
       </c>
@@ -5180,12 +5196,12 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="88" t="s">
+      <c r="M3" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
-      <c r="P3" s="88"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
     </row>
     <row r="4" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
@@ -7133,8 +7149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735095F3-7CED-46DA-BF91-AC87A8D06A06}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7162,14 +7178,14 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="80"/>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="94" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="95" t="s">
-        <v>214</v>
-      </c>
-      <c r="E4" s="96"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="99" t="s">
+        <v>255</v>
+      </c>
+      <c r="E4" s="100"/>
     </row>
     <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="85" t="s">
@@ -7349,14 +7365,14 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="80"/>
-      <c r="B17" s="95" t="s">
+      <c r="B17" s="94" t="s">
         <v>213</v>
       </c>
-      <c r="C17" s="96"/>
-      <c r="D17" s="95" t="s">
+      <c r="C17" s="95"/>
+      <c r="D17" s="94" t="s">
         <v>214</v>
       </c>
-      <c r="E17" s="96"/>
+      <c r="E17" s="95"/>
     </row>
     <row r="18" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="85" t="s">
@@ -7524,10 +7540,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9BAF00-EAB6-4E4C-AFCD-518EB49BC392}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7535,40 +7551,60 @@
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" style="83" customWidth="1"/>
     <col min="3" max="3" width="23.19921875" customWidth="1"/>
+    <col min="4" max="4" width="18.06640625" style="101" customWidth="1"/>
+    <col min="5" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="57" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>247</v>
       </c>
       <c r="C1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
+      <c r="D1" s="102" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="102" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="103" t="s">
         <v>253</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="20">
         <v>5183</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="4" t="s">
+      <c r="D2" s="31">
+        <v>22461837</v>
+      </c>
+      <c r="E2" s="31">
+        <v>234230712</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="103" t="s">
         <v>253</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="20">
         <v>4720</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A4" s="65" t="s">
+      <c r="D3" s="31">
+        <v>19273052</v>
+      </c>
+      <c r="E3" s="31">
+        <v>164835403</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A4" s="4" t="s">
         <v>221</v>
       </c>
       <c r="B4" s="83" t="s">
@@ -7577,9 +7613,15 @@
       <c r="C4">
         <v>603</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="65" t="s">
+      <c r="D4" s="31">
+        <v>1750817</v>
+      </c>
+      <c r="E4" s="31">
+        <v>2099095</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
         <v>222</v>
       </c>
       <c r="B5" s="83" t="s">
@@ -7588,9 +7630,15 @@
       <c r="C5">
         <v>678</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="65" t="s">
+      <c r="D5" s="31">
+        <v>1866777</v>
+      </c>
+      <c r="E5" s="31">
+        <v>2288612</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="4" t="s">
         <v>223</v>
       </c>
       <c r="B6" s="83" t="s">
@@ -7599,9 +7647,15 @@
       <c r="C6">
         <v>898</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="65" t="s">
+      <c r="D6" s="31">
+        <v>5567804</v>
+      </c>
+      <c r="E6" s="31">
+        <v>7934715</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
         <v>224</v>
       </c>
       <c r="B7" s="83" t="s">
@@ -7610,8 +7664,14 @@
       <c r="C7">
         <v>923</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D7" s="31">
+        <v>6453022</v>
+      </c>
+      <c r="E7" s="31">
+        <v>7174248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="65" t="s">
         <v>225</v>
       </c>
@@ -7621,9 +7681,15 @@
       <c r="C8">
         <v>3131</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="65" t="s">
+      <c r="D8" s="31">
+        <v>68753598</v>
+      </c>
+      <c r="E8" s="31">
+        <v>131915011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="4" t="s">
         <v>226</v>
       </c>
       <c r="B9" s="83" t="s">
@@ -7632,9 +7698,15 @@
       <c r="C9">
         <v>875</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="65" t="s">
+      <c r="D9" s="31">
+        <v>4009599</v>
+      </c>
+      <c r="E9" s="31">
+        <v>5617691</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
         <v>227</v>
       </c>
       <c r="B10" s="83" t="s">
@@ -7643,8 +7715,14 @@
       <c r="C10">
         <v>501</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D10" s="31">
+        <v>1050761</v>
+      </c>
+      <c r="E10" s="31">
+        <v>2009094</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="65" t="s">
         <v>228</v>
       </c>
@@ -7654,8 +7732,14 @@
       <c r="C11">
         <v>469</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D11" s="31">
+        <v>842540</v>
+      </c>
+      <c r="E11" s="31">
+        <v>20425597</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="65" t="s">
         <v>229</v>
       </c>
@@ -7665,8 +7749,14 @@
       <c r="C12">
         <v>486</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D12" s="31">
+        <v>689792</v>
+      </c>
+      <c r="E12" s="31">
+        <v>5395646</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="65" t="s">
         <v>230</v>
       </c>
@@ -7676,9 +7766,15 @@
       <c r="C13">
         <v>479</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="65" t="s">
+      <c r="D13" s="31">
+        <v>746177</v>
+      </c>
+      <c r="E13" s="31">
+        <v>2798645</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="4" t="s">
         <v>231</v>
       </c>
       <c r="B14" s="83" t="s">
@@ -7687,8 +7783,14 @@
       <c r="C14">
         <v>582</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D14" s="31">
+        <v>1153442</v>
+      </c>
+      <c r="E14" s="31">
+        <v>1195215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="65" t="s">
         <v>232</v>
       </c>
@@ -7698,8 +7800,14 @@
       <c r="C15">
         <v>1368</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D15" s="31">
+        <v>10310539</v>
+      </c>
+      <c r="E15" s="31">
+        <v>45385911</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="65" t="s">
         <v>233</v>
       </c>
@@ -7709,8 +7817,14 @@
       <c r="C16">
         <v>1352</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+      <c r="D16" s="31">
+        <v>5801726</v>
+      </c>
+      <c r="E16" s="31">
+        <v>15956099</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="57" x14ac:dyDescent="0.45">
       <c r="A17" s="65" t="s">
         <v>234</v>
       </c>
@@ -7720,8 +7834,14 @@
       <c r="C17">
         <v>4685</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D17" s="31">
+        <v>16926746</v>
+      </c>
+      <c r="E17" s="31">
+        <v>47436162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="65" t="s">
         <v>235</v>
       </c>
@@ -7730,6 +7850,12 @@
       </c>
       <c r="C18">
         <v>2490</v>
+      </c>
+      <c r="D18" s="31">
+        <v>4921673</v>
+      </c>
+      <c r="E18" s="31">
+        <v>15650890</v>
       </c>
     </row>
   </sheetData>
@@ -7742,7 +7868,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DCC425-F9E0-4DC1-9C1B-7FD63E026DA8}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -7762,11 +7890,11 @@
       <c r="A2" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="97" t="s">
+      <c r="E2" s="96" t="s">
         <v>206</v>
       </c>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
     </row>
     <row r="3" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -7913,11 +8041,11 @@
       <c r="B11" s="65"/>
       <c r="C11" s="65"/>
       <c r="D11" s="65"/>
-      <c r="E11" s="97" t="s">
+      <c r="E11" s="96" t="s">
         <v>206</v>
       </c>
-      <c r="F11" s="97"/>
-      <c r="G11" s="97"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
     </row>
     <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="65" t="s">
@@ -8061,11 +8189,11 @@
       <c r="A20" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="97" t="s">
+      <c r="E20" s="96" t="s">
         <v>206</v>
       </c>
-      <c r="F20" s="97"/>
-      <c r="G20" s="97"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="96"/>
     </row>
     <row r="21" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" s="65" t="s">
@@ -8336,22 +8464,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98" t="s">
+      <c r="C6" s="97"/>
+      <c r="D6" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98" t="s">
+      <c r="E6" s="97"/>
+      <c r="F6" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="98"/>
-      <c r="H6" s="99" t="s">
+      <c r="G6" s="97"/>
+      <c r="H6" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="99"/>
+      <c r="I6" s="98"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -8361,11 +8489,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="98" t="s">
+      <c r="M6" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="98"/>
-      <c r="O6" s="98"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -10258,7 +10386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD324841-F3D6-48B1-BFDE-305D75F58DD9}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="N9" sqref="N9:P9"/>
     </sheetView>
   </sheetViews>
@@ -11089,22 +11217,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98" t="s">
+      <c r="C6" s="97"/>
+      <c r="D6" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98" t="s">
+      <c r="E6" s="97"/>
+      <c r="F6" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="98"/>
-      <c r="H6" s="99" t="s">
+      <c r="G6" s="97"/>
+      <c r="H6" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="99"/>
+      <c r="I6" s="98"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -11114,11 +11242,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="98" t="s">
+      <c r="M6" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="98"/>
-      <c r="O6" s="98"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -11752,22 +11880,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98" t="s">
+      <c r="C6" s="97"/>
+      <c r="D6" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98" t="s">
+      <c r="E6" s="97"/>
+      <c r="F6" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="98"/>
-      <c r="H6" s="99" t="s">
+      <c r="G6" s="97"/>
+      <c r="H6" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="99"/>
+      <c r="I6" s="98"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -11777,11 +11905,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="98" t="s">
+      <c r="M6" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="98"/>
-      <c r="O6" s="98"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -12399,22 +12527,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
-      <c r="B6" s="91" t="s">
+      <c r="B6" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91" t="s">
+      <c r="C6" s="90"/>
+      <c r="D6" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="91"/>
-      <c r="F6" s="92" t="s">
+      <c r="E6" s="90"/>
+      <c r="F6" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="91"/>
-      <c r="H6" s="89" t="s">
+      <c r="G6" s="90"/>
+      <c r="H6" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="90"/>
+      <c r="I6" s="89"/>
       <c r="J6" s="7" t="s">
         <v>45</v>
       </c>
@@ -12424,11 +12552,11 @@
       <c r="L6" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="92" t="s">
+      <c r="M6" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="91"/>
-      <c r="O6" s="91"/>
+      <c r="N6" s="90"/>
+      <c r="O6" s="90"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
@@ -12728,22 +12856,22 @@
     </row>
     <row r="19" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A19" s="2"/>
-      <c r="B19" s="91" t="s">
+      <c r="B19" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="91"/>
-      <c r="D19" s="91" t="s">
+      <c r="C19" s="90"/>
+      <c r="D19" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="91"/>
-      <c r="F19" s="92" t="s">
+      <c r="E19" s="90"/>
+      <c r="F19" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="91"/>
-      <c r="H19" s="89" t="s">
+      <c r="G19" s="90"/>
+      <c r="H19" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I19" s="90"/>
+      <c r="I19" s="89"/>
       <c r="J19" s="67" t="s">
         <v>45</v>
       </c>
@@ -12753,11 +12881,11 @@
       <c r="L19" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="M19" s="92" t="s">
+      <c r="M19" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N19" s="91"/>
-      <c r="O19" s="91"/>
+      <c r="N19" s="90"/>
+      <c r="O19" s="90"/>
     </row>
     <row r="20" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
@@ -13305,22 +13433,22 @@
     </row>
     <row r="3" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91" t="s">
+      <c r="C3" s="90"/>
+      <c r="D3" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="91"/>
-      <c r="F3" s="92" t="s">
+      <c r="E3" s="90"/>
+      <c r="F3" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="91"/>
-      <c r="H3" s="89" t="s">
+      <c r="G3" s="90"/>
+      <c r="H3" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="90"/>
+      <c r="I3" s="89"/>
       <c r="J3" s="48" t="s">
         <v>45</v>
       </c>
@@ -13330,11 +13458,11 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="92" t="s">
+      <c r="M3" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
     </row>
     <row r="4" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -15140,10 +15268,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51140CC8-C0B8-469A-8BAE-C9043CBCBC10}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView topLeftCell="F19" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21:P21"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -15185,22 +15313,22 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98" t="s">
+      <c r="C6" s="97"/>
+      <c r="D6" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98" t="s">
+      <c r="E6" s="97"/>
+      <c r="F6" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="98"/>
-      <c r="H6" s="99" t="s">
+      <c r="G6" s="97"/>
+      <c r="H6" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="99"/>
+      <c r="I6" s="98"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -15210,11 +15338,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="98" t="s">
+      <c r="M6" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="98"/>
-      <c r="O6" s="98"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A7" s="77" t="s">
@@ -15543,22 +15671,22 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B18" s="98" t="s">
+      <c r="B18" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="98"/>
-      <c r="D18" s="98" t="s">
+      <c r="C18" s="97"/>
+      <c r="D18" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="98"/>
-      <c r="F18" s="98" t="s">
+      <c r="E18" s="97"/>
+      <c r="F18" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="98"/>
-      <c r="H18" s="99" t="s">
+      <c r="G18" s="97"/>
+      <c r="H18" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I18" s="99"/>
+      <c r="I18" s="98"/>
       <c r="J18" s="77" t="s">
         <v>45</v>
       </c>
@@ -15568,11 +15696,11 @@
       <c r="L18" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M18" s="98" t="s">
+      <c r="M18" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N18" s="98"/>
-      <c r="O18" s="98"/>
+      <c r="N18" s="97"/>
+      <c r="O18" s="97"/>
     </row>
     <row r="19" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A19" s="77" t="s">
@@ -16071,6 +16199,11 @@
       <c r="P27" s="80">
         <f t="shared" si="9"/>
         <v>8.696961420937812E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="D29" s="29" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -16128,22 +16261,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98" t="s">
+      <c r="C6" s="97"/>
+      <c r="D6" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98" t="s">
+      <c r="E6" s="97"/>
+      <c r="F6" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="98"/>
-      <c r="H6" s="99" t="s">
+      <c r="G6" s="97"/>
+      <c r="H6" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="99"/>
+      <c r="I6" s="98"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -16153,11 +16286,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="98" t="s">
+      <c r="M6" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="98"/>
-      <c r="O6" s="98"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -16676,7 +16809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1814E241-F455-4452-B5DE-B4EE59F14CFA}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N9" sqref="N9:P9"/>
     </sheetView>
   </sheetViews>
@@ -16710,22 +16843,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98" t="s">
+      <c r="C6" s="97"/>
+      <c r="D6" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98" t="s">
+      <c r="E6" s="97"/>
+      <c r="F6" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="98"/>
-      <c r="H6" s="99" t="s">
+      <c r="G6" s="97"/>
+      <c r="H6" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="99"/>
+      <c r="I6" s="98"/>
       <c r="J6" s="77" t="s">
         <v>45</v>
       </c>
@@ -16735,11 +16868,11 @@
       <c r="L6" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="98" t="s">
+      <c r="M6" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="98"/>
-      <c r="O6" s="98"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -17282,22 +17415,22 @@
     </row>
     <row r="3" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="73"/>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98" t="s">
+      <c r="C3" s="97"/>
+      <c r="D3" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98" t="s">
+      <c r="E3" s="97"/>
+      <c r="F3" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="98"/>
-      <c r="H3" s="99" t="s">
+      <c r="G3" s="97"/>
+      <c r="H3" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="99"/>
+      <c r="I3" s="98"/>
       <c r="J3" s="77" t="s">
         <v>45</v>
       </c>
@@ -17307,11 +17440,11 @@
       <c r="L3" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="98" t="s">
+      <c r="M3" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
       <c r="P3" s="73"/>
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -17855,22 +17988,22 @@
     </row>
     <row r="3" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="73"/>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98" t="s">
+      <c r="C3" s="97"/>
+      <c r="D3" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98" t="s">
+      <c r="E3" s="97"/>
+      <c r="F3" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="98"/>
-      <c r="H3" s="99" t="s">
+      <c r="G3" s="97"/>
+      <c r="H3" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="99"/>
+      <c r="I3" s="98"/>
       <c r="J3" s="77" t="s">
         <v>45</v>
       </c>
@@ -17880,11 +18013,11 @@
       <c r="L3" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="98" t="s">
+      <c r="M3" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
       <c r="P3" s="73"/>
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -19477,29 +19610,29 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91" t="s">
+      <c r="C3" s="90"/>
+      <c r="D3" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="91"/>
-      <c r="F3" s="92" t="s">
+      <c r="E3" s="90"/>
+      <c r="F3" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="91"/>
+      <c r="G3" s="90"/>
       <c r="H3" s="7" t="s">
         <v>45</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="92" t="s">
+      <c r="J3" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -20991,22 +21124,22 @@
     </row>
     <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="52"/>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93" t="s">
+      <c r="C2" s="92"/>
+      <c r="D2" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93" t="s">
+      <c r="E2" s="92"/>
+      <c r="F2" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="93"/>
-      <c r="H2" s="94" t="s">
+      <c r="G2" s="92"/>
+      <c r="H2" s="93" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="94"/>
+      <c r="I2" s="93"/>
       <c r="J2" s="54" t="s">
         <v>45</v>
       </c>
@@ -21016,11 +21149,11 @@
       <c r="L2" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="93" t="s">
+      <c r="M2" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="93"/>
-      <c r="O2" s="93"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
     </row>
     <row r="3" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="52"/>
@@ -21562,22 +21695,22 @@
     </row>
     <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="26"/>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91" t="s">
+      <c r="C2" s="90"/>
+      <c r="D2" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="91"/>
-      <c r="F2" s="92" t="s">
+      <c r="E2" s="90"/>
+      <c r="F2" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="91"/>
-      <c r="H2" s="89" t="s">
+      <c r="G2" s="90"/>
+      <c r="H2" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="90"/>
+      <c r="I2" s="89"/>
       <c r="J2" s="48" t="s">
         <v>45</v>
       </c>
@@ -21587,11 +21720,11 @@
       <c r="L2" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="92" t="s">
+      <c r="M2" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
     </row>
     <row r="3" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26"/>
@@ -22131,22 +22264,22 @@
     </row>
     <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26"/>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91" t="s">
+      <c r="C3" s="90"/>
+      <c r="D3" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="91"/>
-      <c r="F3" s="92" t="s">
+      <c r="E3" s="90"/>
+      <c r="F3" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="91"/>
-      <c r="H3" s="89" t="s">
+      <c r="G3" s="90"/>
+      <c r="H3" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="90"/>
+      <c r="I3" s="89"/>
       <c r="J3" s="48" t="s">
         <v>45</v>
       </c>
@@ -22156,11 +22289,11 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="92" t="s">
+      <c r="M3" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
     </row>
     <row r="4" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="26"/>
@@ -22700,22 +22833,22 @@
     </row>
     <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26"/>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91" t="s">
+      <c r="C3" s="90"/>
+      <c r="D3" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="91"/>
-      <c r="F3" s="92" t="s">
+      <c r="E3" s="90"/>
+      <c r="F3" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="91"/>
-      <c r="H3" s="89" t="s">
+      <c r="G3" s="90"/>
+      <c r="H3" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="90"/>
+      <c r="I3" s="89"/>
       <c r="J3" s="48" t="s">
         <v>45</v>
       </c>
@@ -22725,11 +22858,11 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="92" t="s">
+      <c r="M3" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
     </row>
     <row r="4" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="26"/>
@@ -23430,14 +23563,14 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="80"/>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="94" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="95" t="s">
+      <c r="C4" s="95"/>
+      <c r="D4" s="94" t="s">
         <v>214</v>
       </c>
-      <c r="E4" s="96"/>
+      <c r="E4" s="95"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="85" t="s">
@@ -23535,14 +23668,14 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="80"/>
-      <c r="B17" s="95" t="s">
+      <c r="B17" s="94" t="s">
         <v>213</v>
       </c>
-      <c r="C17" s="96"/>
-      <c r="D17" s="95" t="s">
+      <c r="C17" s="95"/>
+      <c r="D17" s="94" t="s">
         <v>214</v>
       </c>
-      <c r="E17" s="96"/>
+      <c r="E17" s="95"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="85" t="s">

</xml_diff>

<commit_message>
added results of specjvm2008 with jvm option UseLargePage
The jit code and data heaps are large-page-aligned.
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="409" documentId="81D8B261ABBD5CBDED69DEB44BA5B0CD337C6AB9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{FB43F406-A668-41E7-925F-2DCF9A32BCED}"/>
+  <xr:revisionPtr revIDLastSave="441" documentId="81D8B261ABBD5CBDED69DEB44BA5B0CD337C6AB9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{32A96FE8-C57D-45F6-B521-45A4542122E5}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="249">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -806,6 +806,9 @@
   </si>
   <si>
     <t>Disabling large page</t>
+  </si>
+  <si>
+    <t>JVM UseLargePage option</t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1027,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1165,9 +1168,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1203,9 +1203,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5122,22 +5119,22 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="57" x14ac:dyDescent="0.45">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88" t="s">
+      <c r="C3" s="87"/>
+      <c r="D3" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88" t="s">
+      <c r="E3" s="87"/>
+      <c r="F3" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="88"/>
-      <c r="H3" s="89" t="s">
+      <c r="G3" s="87"/>
+      <c r="H3" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="90"/>
+      <c r="I3" s="89"/>
       <c r="J3" s="33" t="s">
         <v>45</v>
       </c>
@@ -5147,12 +5144,12 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="88" t="s">
+      <c r="M3" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
-      <c r="P3" s="88"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
     </row>
     <row r="4" spans="1:16" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
@@ -7098,10 +7095,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A67B38-292E-4CA0-8E76-A7B2040A6BB6}">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67"/>
+      <selection activeCell="D59" sqref="D59:E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7109,32 +7106,38 @@
     <col min="1" max="1" width="35.59765625" customWidth="1"/>
     <col min="2" max="2" width="19.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" style="66" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.9296875" style="66" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="100" t="s">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A1" s="98" t="s">
         <v>244</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="66" t="s">
         <v>245</v>
       </c>
       <c r="B2" s="66"/>
       <c r="C2" s="66"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A3" s="100" t="s">
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A3" s="98" t="s">
         <v>211</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="94" t="s">
         <v>247</v>
       </c>
-      <c r="C3" s="95"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C3" s="94"/>
+      <c r="D3" s="94" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3" s="94"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="66"/>
       <c r="B4" s="66" t="s">
         <v>27</v>
@@ -7142,8 +7145,14 @@
       <c r="C4" s="66" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D4" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="66" t="s">
         <v>15</v>
       </c>
@@ -7153,8 +7162,14 @@
       <c r="C5" s="66">
         <v>378925074.94800001</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D5" s="66">
+        <v>85809134662.199997</v>
+      </c>
+      <c r="E5" s="66">
+        <v>764596703.148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="66" t="s">
         <v>2</v>
       </c>
@@ -7164,8 +7179,14 @@
       <c r="C6" s="66">
         <v>12345783540.700001</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D6" s="66">
+        <v>2496480524770</v>
+      </c>
+      <c r="E6" s="66">
+        <v>356465032.57700002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="66" t="s">
         <v>35</v>
       </c>
@@ -7175,8 +7196,14 @@
       <c r="C7" s="66">
         <v>365362.88185599999</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D7" s="66">
+        <v>1868902</v>
+      </c>
+      <c r="E7" s="66">
+        <v>223780.34701600001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="66" t="s">
         <v>36</v>
       </c>
@@ -7186,8 +7213,14 @@
       <c r="C8" s="66">
         <v>281972.89983200002</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D8" s="66">
+        <v>2381881.6</v>
+      </c>
+      <c r="E8" s="66">
+        <v>195956.82455200001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="66" t="s">
         <v>1</v>
       </c>
@@ -7197,8 +7230,14 @@
       <c r="C9" s="66">
         <v>9189227442.0599995</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D9" s="66">
+        <v>3241560128780</v>
+      </c>
+      <c r="E9" s="66">
+        <v>12686939398</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="66" t="s">
         <v>4</v>
       </c>
@@ -7208,8 +7247,14 @@
       <c r="C10" s="66">
         <v>167367014.83399999</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D10" s="66">
+        <v>272713376.80000001</v>
+      </c>
+      <c r="E10" s="66">
+        <v>270773758.31199998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="66" t="s">
         <v>6</v>
       </c>
@@ -7219,8 +7264,14 @@
       <c r="C11" s="66">
         <v>6291224.5249100002</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D11" s="66">
+        <v>156461014.80000001</v>
+      </c>
+      <c r="E11" s="66">
+        <v>8377484.2311800001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="66" t="s">
         <v>20</v>
       </c>
@@ -7230,22 +7281,32 @@
       <c r="C12" s="66">
         <v>120187680.292</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D12" s="66">
+        <v>1898321356.2</v>
+      </c>
+      <c r="E12" s="66">
+        <v>620101156.01699996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="66"/>
       <c r="B13" s="66"/>
       <c r="C13" s="66"/>
     </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A14" s="100" t="s">
+    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A14" s="98" t="s">
         <v>212</v>
       </c>
-      <c r="B14" s="95" t="s">
+      <c r="B14" s="94" t="s">
         <v>247</v>
       </c>
-      <c r="C14" s="95"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C14" s="94"/>
+      <c r="D14" s="94" t="s">
+        <v>248</v>
+      </c>
+      <c r="E14" s="94"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="66"/>
       <c r="B15" s="66" t="s">
         <v>27</v>
@@ -7253,8 +7314,14 @@
       <c r="C15" s="66" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D15" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="66" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="66" t="s">
         <v>15</v>
       </c>
@@ -7264,8 +7331,14 @@
       <c r="C16" s="66">
         <v>63286475.464400001</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D16" s="66">
+        <v>2240429227</v>
+      </c>
+      <c r="E16" s="66">
+        <v>47357527.493799999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="66" t="s">
         <v>2</v>
       </c>
@@ -7275,8 +7348,14 @@
       <c r="C17" s="66">
         <v>13443432764.799999</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D17" s="66">
+        <v>2530614734600</v>
+      </c>
+      <c r="E17" s="66">
+        <v>11236549837.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="66" t="s">
         <v>35</v>
       </c>
@@ -7286,8 +7365,14 @@
       <c r="C18" s="66">
         <v>446243.07650999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D18" s="66">
+        <v>3209626.2</v>
+      </c>
+      <c r="E18" s="66">
+        <v>1593167.1845199999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="66" t="s">
         <v>36</v>
       </c>
@@ -7297,8 +7382,14 @@
       <c r="C19" s="66">
         <v>296501.54971799999</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D19" s="66">
+        <v>2389406.6</v>
+      </c>
+      <c r="E19" s="66">
+        <v>208478.24429199999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="66" t="s">
         <v>1</v>
       </c>
@@ -7308,8 +7399,14 @@
       <c r="C20" s="66">
         <v>41806844543.099998</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D20" s="66">
+        <v>5101011400440</v>
+      </c>
+      <c r="E20" s="66">
+        <v>30374819122.099998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="66" t="s">
         <v>4</v>
       </c>
@@ -7319,8 +7416,14 @@
       <c r="C21" s="66">
         <v>3180826.1693299999</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D21" s="66">
+        <v>136936514</v>
+      </c>
+      <c r="E21" s="66">
+        <v>50896741.250200003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="66" t="s">
         <v>6</v>
       </c>
@@ -7330,8 +7433,14 @@
       <c r="C22" s="66">
         <v>5664526.7246300001</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D22" s="66">
+        <v>176584489.40000001</v>
+      </c>
+      <c r="E22" s="66">
+        <v>19873294.455499999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="66" t="s">
         <v>20</v>
       </c>
@@ -7341,22 +7450,32 @@
       <c r="C23" s="66">
         <v>34007592.8495</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D23" s="66">
+        <v>3561687479.8000002</v>
+      </c>
+      <c r="E23" s="66">
+        <v>145421983.42500001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="66"/>
       <c r="B24" s="66"/>
       <c r="C24" s="66"/>
     </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A25" s="100" t="s">
+    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A25" s="98" t="s">
         <v>213</v>
       </c>
-      <c r="B25" s="95" t="s">
+      <c r="B25" s="94" t="s">
         <v>247</v>
       </c>
-      <c r="C25" s="95"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C25" s="94"/>
+      <c r="D25" s="94" t="s">
+        <v>248</v>
+      </c>
+      <c r="E25" s="94"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="66"/>
       <c r="B26" s="66" t="s">
         <v>27</v>
@@ -7364,8 +7483,14 @@
       <c r="C26" s="66" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D26" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="66" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="66" t="s">
         <v>15</v>
       </c>
@@ -7375,8 +7500,14 @@
       <c r="C27" s="66">
         <v>30922099.335499998</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D27" s="66">
+        <v>1241489272.5999999</v>
+      </c>
+      <c r="E27" s="66">
+        <v>27399273.483399998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="66" t="s">
         <v>2</v>
       </c>
@@ -7386,8 +7517,14 @@
       <c r="C28" s="66">
         <v>983254684.33399999</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D28" s="66">
+        <v>2493671755080</v>
+      </c>
+      <c r="E28" s="66">
+        <v>2406771683.4000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="66" t="s">
         <v>35</v>
       </c>
@@ -7397,8 +7534,14 @@
       <c r="C29" s="66">
         <v>403671.21094899997</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D29" s="66">
+        <v>6954931.2000000002</v>
+      </c>
+      <c r="E29" s="66">
+        <v>2914010.7823100002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="66" t="s">
         <v>36</v>
       </c>
@@ -7408,8 +7551,14 @@
       <c r="C30" s="66">
         <v>240964.33450699999</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D30" s="66">
+        <v>8150452.5999999996</v>
+      </c>
+      <c r="E30" s="66">
+        <v>155363.36829099999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="66" t="s">
         <v>1</v>
       </c>
@@ -7419,8 +7568,14 @@
       <c r="C31" s="66">
         <v>22916285503.599998</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D31" s="66">
+        <v>4798326030420</v>
+      </c>
+      <c r="E31" s="66">
+        <v>26698891828.700001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="66" t="s">
         <v>4</v>
       </c>
@@ -7430,8 +7585,14 @@
       <c r="C32" s="66">
         <v>11663517.0461</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D32" s="66">
+        <v>435256532</v>
+      </c>
+      <c r="E32" s="66">
+        <v>299441646.55699998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="66" t="s">
         <v>6</v>
       </c>
@@ -7441,8 +7602,14 @@
       <c r="C33" s="66">
         <v>42876590.606799997</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D33" s="66">
+        <v>656935750.39999998</v>
+      </c>
+      <c r="E33" s="66">
+        <v>166482376.817</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="66" t="s">
         <v>20</v>
       </c>
@@ -7452,31 +7619,47 @@
       <c r="C34" s="66">
         <v>69875378.624899998</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D34" s="66">
+        <v>673616089.79999995</v>
+      </c>
+      <c r="E34" s="66">
+        <v>7898672.1684600003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" s="66"/>
       <c r="B35" s="66"/>
       <c r="C35" s="66"/>
     </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A36" s="100" t="s">
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A36" s="98" t="s">
         <v>214</v>
       </c>
-      <c r="B36" s="95" t="s">
+      <c r="B36" s="94" t="s">
         <v>247</v>
       </c>
-      <c r="C36" s="95"/>
-    </row>
-    <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="101"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="94" t="s">
+        <v>248</v>
+      </c>
+      <c r="E36" s="94"/>
+    </row>
+    <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="99"/>
       <c r="B37" s="66" t="s">
         <v>27</v>
       </c>
       <c r="C37" s="66" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D37" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="66" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" s="66" t="s">
         <v>15</v>
       </c>
@@ -7486,8 +7669,14 @@
       <c r="C38" s="66">
         <v>197261402.081</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D38" s="66">
+        <v>4841383742.3999996</v>
+      </c>
+      <c r="E38" s="66">
+        <v>154824785.83899999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" s="66" t="s">
         <v>2</v>
       </c>
@@ -7497,8 +7686,14 @@
       <c r="C39" s="66">
         <v>1471358751.97</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D39" s="66">
+        <v>2497107247450</v>
+      </c>
+      <c r="E39" s="66">
+        <v>920187736.73500001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" s="66" t="s">
         <v>35</v>
       </c>
@@ -7508,8 +7703,14 @@
       <c r="C40" s="66">
         <v>66342.843210100007</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D40" s="66">
+        <v>9615897.5999999996</v>
+      </c>
+      <c r="E40" s="66">
+        <v>5772763.6471100003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" s="66" t="s">
         <v>36</v>
       </c>
@@ -7519,8 +7720,14 @@
       <c r="C41" s="66">
         <v>249511.52518600001</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D41" s="66">
+        <v>7128517.5999999996</v>
+      </c>
+      <c r="E41" s="66">
+        <v>75471.941595800003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="66" t="s">
         <v>1</v>
       </c>
@@ -7530,8 +7737,14 @@
       <c r="C42" s="66">
         <v>18373280108.799999</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D42" s="66">
+        <v>4737179485360</v>
+      </c>
+      <c r="E42" s="66">
+        <v>15049173668</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="66" t="s">
         <v>4</v>
       </c>
@@ -7541,8 +7754,14 @@
       <c r="C43" s="66">
         <v>15212714.154899999</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D43" s="66">
+        <v>497466808.60000002</v>
+      </c>
+      <c r="E43" s="66">
+        <v>253963295.05899999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" s="66" t="s">
         <v>6</v>
       </c>
@@ -7552,8 +7771,14 @@
       <c r="C44" s="66">
         <v>10469600.8805</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D44" s="66">
+        <v>454664977</v>
+      </c>
+      <c r="E44" s="66">
+        <v>5122739</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" s="66" t="s">
         <v>20</v>
       </c>
@@ -7563,31 +7788,47 @@
       <c r="C45" s="66">
         <v>58382264.978100002</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D45" s="66">
+        <v>1494125647.4000001</v>
+      </c>
+      <c r="E45" s="66">
+        <v>20023914.6558</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" s="66"/>
       <c r="B46" s="66"/>
       <c r="C46" s="66"/>
     </row>
-    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A47" s="100" t="s">
+    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A47" s="98" t="s">
         <v>216</v>
       </c>
-      <c r="B47" s="95" t="s">
+      <c r="B47" s="94" t="s">
         <v>247</v>
       </c>
-      <c r="C47" s="95"/>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A48" s="100"/>
+      <c r="C47" s="94"/>
+      <c r="D47" s="94" t="s">
+        <v>248</v>
+      </c>
+      <c r="E47" s="94"/>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A48" s="98"/>
       <c r="B48" s="66" t="s">
         <v>27</v>
       </c>
       <c r="C48" s="66" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D48" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" s="66" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="66" t="s">
         <v>15</v>
       </c>
@@ -7597,8 +7838,14 @@
       <c r="C49" s="66">
         <v>120477411.669</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D49" s="66">
+        <v>6377164573.3999996</v>
+      </c>
+      <c r="E49" s="66">
+        <v>208790822.65900001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="66" t="s">
         <v>2</v>
       </c>
@@ -7608,8 +7855,14 @@
       <c r="C50" s="66">
         <v>11078130492.799999</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D50" s="66">
+        <v>2513806135820</v>
+      </c>
+      <c r="E50" s="66">
+        <v>10634461937.700001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" s="66" t="s">
         <v>35</v>
       </c>
@@ -7619,8 +7872,14 @@
       <c r="C51" s="66">
         <v>1274865.7178700001</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D51" s="66">
+        <v>4473245.4000000004</v>
+      </c>
+      <c r="E51" s="66">
+        <v>622229.35078199999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="66" t="s">
         <v>36</v>
       </c>
@@ -7630,8 +7889,14 @@
       <c r="C52" s="66">
         <v>190061.40458500001</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D52" s="66">
+        <v>5717564.7999999998</v>
+      </c>
+      <c r="E52" s="66">
+        <v>233003.043729</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="66" t="s">
         <v>1</v>
       </c>
@@ -7641,8 +7906,14 @@
       <c r="C53" s="66">
         <v>30193828357.799999</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D53" s="66">
+        <v>4006031494590</v>
+      </c>
+      <c r="E53" s="66">
+        <v>16125274268.4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" s="66" t="s">
         <v>4</v>
       </c>
@@ -7652,8 +7923,14 @@
       <c r="C54" s="66">
         <v>98763874.267199993</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D54" s="66">
+        <v>365051462.80000001</v>
+      </c>
+      <c r="E54" s="66">
+        <v>235344848.553</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="66" t="s">
         <v>6</v>
       </c>
@@ -7663,8 +7940,14 @@
       <c r="C55" s="66">
         <v>74471418.124799997</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D55" s="66">
+        <v>1206091961.2</v>
+      </c>
+      <c r="E55" s="66">
+        <v>47903481.994999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="66" t="s">
         <v>20</v>
       </c>
@@ -7674,36 +7957,50 @@
       <c r="C56" s="66">
         <v>96789709.229499996</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D56" s="66">
+        <v>1400747536.4000001</v>
+      </c>
+      <c r="E56" s="66">
+        <v>33666990.807700001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" s="66"/>
       <c r="B57" s="66"/>
       <c r="C57" s="66"/>
     </row>
-    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A58" s="100"/>
-      <c r="B58" s="95"/>
-      <c r="C58" s="95"/>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A59" s="100" t="s">
+    <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A58" s="98"/>
+      <c r="B58" s="94"/>
+      <c r="C58" s="94"/>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A59" s="98" t="s">
         <v>221</v>
       </c>
-      <c r="B59" s="95" t="s">
+      <c r="B59" s="94" t="s">
         <v>247</v>
       </c>
-      <c r="C59" s="95"/>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A60" s="100"/>
+      <c r="C59" s="94"/>
+      <c r="D59" s="94" t="s">
+        <v>248</v>
+      </c>
+      <c r="E59" s="94"/>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A60" s="98"/>
       <c r="B60" s="66" t="s">
         <v>27</v>
       </c>
       <c r="C60" s="66" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D60" s="94" t="s">
+        <v>248</v>
+      </c>
+      <c r="E60" s="94"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" s="66" t="s">
         <v>15</v>
       </c>
@@ -7713,8 +8010,14 @@
       <c r="C61" s="66">
         <v>1076302.1475</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D61" s="66">
+        <v>94497164.400000006</v>
+      </c>
+      <c r="E61" s="66">
+        <v>1657129.5503499999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" s="66" t="s">
         <v>2</v>
       </c>
@@ -7724,8 +8027,14 @@
       <c r="C62" s="66">
         <v>880322425.48800004</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D62" s="66">
+        <v>2492751669680</v>
+      </c>
+      <c r="E62" s="66">
+        <v>752773655.06500006</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" s="66" t="s">
         <v>35</v>
       </c>
@@ -7735,8 +8044,14 @@
       <c r="C63" s="66">
         <v>39581.562361299999</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D63" s="66">
+        <v>2600616.7999999998</v>
+      </c>
+      <c r="E63" s="66">
+        <v>2131550.9088599999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64" s="66" t="s">
         <v>36</v>
       </c>
@@ -7746,8 +8061,14 @@
       <c r="C64" s="66">
         <v>6318.8227890999997</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D64" s="66">
+        <v>1159288.3999999999</v>
+      </c>
+      <c r="E64" s="66">
+        <v>6664.0119327599996</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65" s="66" t="s">
         <v>1</v>
       </c>
@@ -7757,8 +8078,14 @@
       <c r="C65" s="66">
         <v>2252842596.8000002</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D65" s="66">
+        <v>5508323108560</v>
+      </c>
+      <c r="E65" s="66">
+        <v>3508530635.8699999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66" s="66" t="s">
         <v>4</v>
       </c>
@@ -7768,8 +8095,14 @@
       <c r="C66" s="66">
         <v>8528438.0449499991</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D66" s="66">
+        <v>311308041.39999998</v>
+      </c>
+      <c r="E66" s="66">
+        <v>373472800.54299998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67" s="66" t="s">
         <v>6</v>
       </c>
@@ -7779,8 +8112,14 @@
       <c r="C67" s="66">
         <v>473789.90292099997</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D67" s="66">
+        <v>59142649.399999999</v>
+      </c>
+      <c r="E67" s="66">
+        <v>839422.56346500001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68" s="66" t="s">
         <v>20</v>
       </c>
@@ -7790,10 +8129,23 @@
       <c r="C68" s="66">
         <v>1007390.79641</v>
       </c>
+      <c r="D68" s="66">
+        <v>119147428.59999999</v>
+      </c>
+      <c r="E68" s="66">
+        <v>1016777.71449</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="14">
+    <mergeCell ref="D60:E60"/>
     <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D59:E59"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B25:C25"/>
@@ -7818,7 +8170,7 @@
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" style="80" customWidth="1"/>
     <col min="3" max="3" width="23.19921875" customWidth="1"/>
-    <col min="4" max="4" width="18.06640625" style="85" customWidth="1"/>
+    <col min="4" max="4" width="18.06640625" style="84" customWidth="1"/>
     <col min="5" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7829,10 +8181,10 @@
       <c r="C1" t="s">
         <v>242</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="86" t="s">
+      <c r="E1" s="85" t="s">
         <v>36</v>
       </c>
     </row>
@@ -7840,7 +8192,7 @@
       <c r="A2" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="86" t="s">
         <v>243</v>
       </c>
       <c r="C2" s="20">
@@ -7857,7 +8209,7 @@
       <c r="A3" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="86" t="s">
         <v>243</v>
       </c>
       <c r="C3" s="20">
@@ -8157,11 +8509,11 @@
       <c r="A2" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="97" t="s">
+      <c r="E2" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
     </row>
     <row r="3" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -8308,11 +8660,11 @@
       <c r="B11" s="65"/>
       <c r="C11" s="65"/>
       <c r="D11" s="65"/>
-      <c r="E11" s="97" t="s">
+      <c r="E11" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="F11" s="97"/>
-      <c r="G11" s="97"/>
+      <c r="F11" s="95"/>
+      <c r="G11" s="95"/>
     </row>
     <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="65" t="s">
@@ -8456,11 +8808,11 @@
       <c r="A20" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="97" t="s">
+      <c r="E20" s="95" t="s">
         <v>204</v>
       </c>
-      <c r="F20" s="97"/>
-      <c r="G20" s="97"/>
+      <c r="F20" s="95"/>
+      <c r="G20" s="95"/>
     </row>
     <row r="21" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" s="65" t="s">
@@ -8731,22 +9083,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98" t="s">
+      <c r="C6" s="96"/>
+      <c r="D6" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98" t="s">
+      <c r="E6" s="96"/>
+      <c r="F6" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="98"/>
-      <c r="H6" s="99" t="s">
+      <c r="G6" s="96"/>
+      <c r="H6" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="99"/>
+      <c r="I6" s="97"/>
       <c r="J6" s="76" t="s">
         <v>45</v>
       </c>
@@ -8756,11 +9108,11 @@
       <c r="L6" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="98" t="s">
+      <c r="M6" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="98"/>
-      <c r="O6" s="98"/>
+      <c r="N6" s="96"/>
+      <c r="O6" s="96"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -9361,22 +9713,22 @@
     </row>
     <row r="23" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A23" s="73"/>
-      <c r="B23" s="83" t="s">
+      <c r="B23" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="83"/>
-      <c r="D23" s="83" t="s">
+      <c r="C23" s="82"/>
+      <c r="D23" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83" t="s">
+      <c r="E23" s="82"/>
+      <c r="F23" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="83"/>
-      <c r="H23" s="84" t="s">
+      <c r="G23" s="82"/>
+      <c r="H23" s="83" t="s">
         <v>114</v>
       </c>
-      <c r="I23" s="84"/>
+      <c r="I23" s="83"/>
       <c r="J23" s="76" t="s">
         <v>45</v>
       </c>
@@ -9386,11 +9738,11 @@
       <c r="L23" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M23" s="83" t="s">
+      <c r="M23" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="N23" s="83"/>
-      <c r="O23" s="83"/>
+      <c r="N23" s="82"/>
+      <c r="O23" s="82"/>
       <c r="P23" s="73"/>
     </row>
     <row r="24" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -9991,22 +10343,22 @@
     </row>
     <row r="41" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A41" s="73"/>
-      <c r="B41" s="98" t="s">
+      <c r="B41" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C41" s="98"/>
-      <c r="D41" s="98" t="s">
+      <c r="C41" s="96"/>
+      <c r="D41" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E41" s="98"/>
-      <c r="F41" s="98" t="s">
+      <c r="E41" s="96"/>
+      <c r="F41" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G41" s="98"/>
-      <c r="H41" s="99" t="s">
+      <c r="G41" s="96"/>
+      <c r="H41" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I41" s="99"/>
+      <c r="I41" s="97"/>
       <c r="J41" s="76" t="s">
         <v>45</v>
       </c>
@@ -10016,11 +10368,11 @@
       <c r="L41" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M41" s="98" t="s">
+      <c r="M41" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N41" s="98"/>
-      <c r="O41" s="98"/>
+      <c r="N41" s="96"/>
+      <c r="O41" s="96"/>
       <c r="P41" s="73"/>
     </row>
     <row r="42" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -10540,22 +10892,22 @@
     </row>
     <row r="57" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A57" s="2"/>
-      <c r="B57" s="91" t="s">
+      <c r="B57" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="91"/>
-      <c r="D57" s="91" t="s">
+      <c r="C57" s="90"/>
+      <c r="D57" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E57" s="91"/>
-      <c r="F57" s="92" t="s">
+      <c r="E57" s="90"/>
+      <c r="F57" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G57" s="91"/>
-      <c r="H57" s="89" t="s">
+      <c r="G57" s="90"/>
+      <c r="H57" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I57" s="90"/>
+      <c r="I57" s="89"/>
       <c r="J57" s="67" t="s">
         <v>45</v>
       </c>
@@ -10565,11 +10917,11 @@
       <c r="L57" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="M57" s="92" t="s">
+      <c r="M57" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N57" s="91"/>
-      <c r="O57" s="91"/>
+      <c r="N57" s="90"/>
+      <c r="O57" s="90"/>
       <c r="P57" s="65"/>
     </row>
     <row r="58" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -11170,22 +11522,22 @@
     </row>
     <row r="74" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A74" s="73"/>
-      <c r="B74" s="98" t="s">
+      <c r="B74" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C74" s="98"/>
-      <c r="D74" s="98" t="s">
+      <c r="C74" s="96"/>
+      <c r="D74" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E74" s="98"/>
-      <c r="F74" s="98" t="s">
+      <c r="E74" s="96"/>
+      <c r="F74" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G74" s="98"/>
-      <c r="H74" s="99" t="s">
+      <c r="G74" s="96"/>
+      <c r="H74" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I74" s="99"/>
+      <c r="I74" s="97"/>
       <c r="J74" s="76" t="s">
         <v>45</v>
       </c>
@@ -11195,11 +11547,11 @@
       <c r="L74" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M74" s="98" t="s">
+      <c r="M74" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N74" s="98"/>
-      <c r="O74" s="98"/>
+      <c r="N74" s="96"/>
+      <c r="O74" s="96"/>
       <c r="P74" s="73"/>
     </row>
     <row r="75" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -12480,22 +12832,22 @@
     </row>
     <row r="24" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A24" s="73"/>
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="83"/>
-      <c r="D24" s="83" t="s">
+      <c r="C24" s="82"/>
+      <c r="D24" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83" t="s">
+      <c r="E24" s="82"/>
+      <c r="F24" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="G24" s="83"/>
-      <c r="H24" s="84" t="s">
+      <c r="G24" s="82"/>
+      <c r="H24" s="83" t="s">
         <v>114</v>
       </c>
-      <c r="I24" s="84"/>
+      <c r="I24" s="83"/>
       <c r="J24" s="76" t="s">
         <v>45</v>
       </c>
@@ -12505,11 +12857,11 @@
       <c r="L24" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M24" s="83" t="s">
+      <c r="M24" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="N24" s="83"/>
-      <c r="O24" s="83"/>
+      <c r="N24" s="82"/>
+      <c r="O24" s="82"/>
       <c r="P24" s="73"/>
     </row>
     <row r="25" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -13090,22 +13442,22 @@
     </row>
     <row r="40" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A40" s="73"/>
-      <c r="B40" s="98" t="s">
+      <c r="B40" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="98"/>
-      <c r="D40" s="98" t="s">
+      <c r="C40" s="96"/>
+      <c r="D40" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E40" s="98"/>
-      <c r="F40" s="98" t="s">
+      <c r="E40" s="96"/>
+      <c r="F40" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G40" s="98"/>
-      <c r="H40" s="99" t="s">
+      <c r="G40" s="96"/>
+      <c r="H40" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I40" s="99"/>
+      <c r="I40" s="97"/>
       <c r="J40" s="76" t="s">
         <v>45</v>
       </c>
@@ -13115,11 +13467,11 @@
       <c r="L40" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M40" s="98" t="s">
+      <c r="M40" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N40" s="98"/>
-      <c r="O40" s="98"/>
+      <c r="N40" s="96"/>
+      <c r="O40" s="96"/>
       <c r="P40" s="73"/>
     </row>
     <row r="41" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -13634,22 +13986,22 @@
     </row>
     <row r="54" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A54" s="73"/>
-      <c r="B54" s="98" t="s">
+      <c r="B54" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="98"/>
-      <c r="D54" s="98" t="s">
+      <c r="C54" s="96"/>
+      <c r="D54" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E54" s="98"/>
-      <c r="F54" s="98" t="s">
+      <c r="E54" s="96"/>
+      <c r="F54" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G54" s="98"/>
-      <c r="H54" s="99" t="s">
+      <c r="G54" s="96"/>
+      <c r="H54" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I54" s="99"/>
+      <c r="I54" s="97"/>
       <c r="J54" s="76" t="s">
         <v>45</v>
       </c>
@@ -13659,11 +14011,11 @@
       <c r="L54" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M54" s="98" t="s">
+      <c r="M54" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N54" s="98"/>
-      <c r="O54" s="98"/>
+      <c r="N54" s="96"/>
+      <c r="O54" s="96"/>
       <c r="P54" s="73"/>
     </row>
     <row r="55" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -14262,22 +14614,22 @@
     </row>
     <row r="70" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A70" s="73"/>
-      <c r="B70" s="98" t="s">
+      <c r="B70" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C70" s="98"/>
-      <c r="D70" s="98" t="s">
+      <c r="C70" s="96"/>
+      <c r="D70" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E70" s="98"/>
-      <c r="F70" s="98" t="s">
+      <c r="E70" s="96"/>
+      <c r="F70" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G70" s="98"/>
-      <c r="H70" s="99" t="s">
+      <c r="G70" s="96"/>
+      <c r="H70" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I70" s="99"/>
+      <c r="I70" s="97"/>
       <c r="J70" s="76" t="s">
         <v>45</v>
       </c>
@@ -14287,11 +14639,11 @@
       <c r="L70" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M70" s="98" t="s">
+      <c r="M70" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N70" s="98"/>
-      <c r="O70" s="98"/>
+      <c r="N70" s="96"/>
+      <c r="O70" s="96"/>
       <c r="P70" s="73"/>
     </row>
     <row r="71" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -14844,22 +15196,22 @@
     </row>
     <row r="3" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="73"/>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98" t="s">
+      <c r="C3" s="96"/>
+      <c r="D3" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98" t="s">
+      <c r="E3" s="96"/>
+      <c r="F3" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="98"/>
-      <c r="H3" s="99" t="s">
+      <c r="G3" s="96"/>
+      <c r="H3" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="99"/>
+      <c r="I3" s="97"/>
       <c r="J3" s="76" t="s">
         <v>45</v>
       </c>
@@ -14869,11 +15221,11 @@
       <c r="L3" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="98" t="s">
+      <c r="M3" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
       <c r="P3" s="73"/>
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -15417,22 +15769,22 @@
     </row>
     <row r="3" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="73"/>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98" t="s">
+      <c r="C3" s="96"/>
+      <c r="D3" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98" t="s">
+      <c r="E3" s="96"/>
+      <c r="F3" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="98"/>
-      <c r="H3" s="99" t="s">
+      <c r="G3" s="96"/>
+      <c r="H3" s="97" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="99"/>
+      <c r="I3" s="97"/>
       <c r="J3" s="76" t="s">
         <v>45</v>
       </c>
@@ -15442,11 +15794,11 @@
       <c r="L3" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="98" t="s">
+      <c r="M3" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
       <c r="P3" s="73"/>
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -17040,22 +17392,22 @@
     </row>
     <row r="3" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91" t="s">
+      <c r="C3" s="90"/>
+      <c r="D3" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="91"/>
-      <c r="F3" s="92" t="s">
+      <c r="E3" s="90"/>
+      <c r="F3" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="91"/>
-      <c r="H3" s="89" t="s">
+      <c r="G3" s="90"/>
+      <c r="H3" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="90"/>
+      <c r="I3" s="89"/>
       <c r="J3" s="48" t="s">
         <v>45</v>
       </c>
@@ -17065,11 +17417,11 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="92" t="s">
+      <c r="M3" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
     </row>
     <row r="4" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -18901,29 +19253,29 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91" t="s">
+      <c r="C3" s="90"/>
+      <c r="D3" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="91"/>
-      <c r="F3" s="92" t="s">
+      <c r="E3" s="90"/>
+      <c r="F3" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="91"/>
+      <c r="G3" s="90"/>
       <c r="H3" s="7" t="s">
         <v>45</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="92" t="s">
+      <c r="J3" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
@@ -20415,22 +20767,22 @@
     </row>
     <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="52"/>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93" t="s">
+      <c r="C2" s="92"/>
+      <c r="D2" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93" t="s">
+      <c r="E2" s="92"/>
+      <c r="F2" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="93"/>
-      <c r="H2" s="94" t="s">
+      <c r="G2" s="92"/>
+      <c r="H2" s="93" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="94"/>
+      <c r="I2" s="93"/>
       <c r="J2" s="54" t="s">
         <v>45</v>
       </c>
@@ -20440,11 +20792,11 @@
       <c r="L2" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="93" t="s">
+      <c r="M2" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="93"/>
-      <c r="O2" s="93"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
     </row>
     <row r="3" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="52"/>
@@ -20986,22 +21338,22 @@
     </row>
     <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="26"/>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91" t="s">
+      <c r="C2" s="90"/>
+      <c r="D2" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="91"/>
-      <c r="F2" s="92" t="s">
+      <c r="E2" s="90"/>
+      <c r="F2" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="91"/>
-      <c r="H2" s="89" t="s">
+      <c r="G2" s="90"/>
+      <c r="H2" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="90"/>
+      <c r="I2" s="89"/>
       <c r="J2" s="48" t="s">
         <v>45</v>
       </c>
@@ -21011,11 +21363,11 @@
       <c r="L2" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="92" t="s">
+      <c r="M2" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
     </row>
     <row r="3" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26"/>
@@ -21555,22 +21907,22 @@
     </row>
     <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26"/>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91" t="s">
+      <c r="C3" s="90"/>
+      <c r="D3" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="91"/>
-      <c r="F3" s="92" t="s">
+      <c r="E3" s="90"/>
+      <c r="F3" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="91"/>
-      <c r="H3" s="89" t="s">
+      <c r="G3" s="90"/>
+      <c r="H3" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="90"/>
+      <c r="I3" s="89"/>
       <c r="J3" s="48" t="s">
         <v>45</v>
       </c>
@@ -21580,11 +21932,11 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="92" t="s">
+      <c r="M3" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
     </row>
     <row r="4" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="26"/>
@@ -22124,22 +22476,22 @@
     </row>
     <row r="3" spans="1:16" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26"/>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91" t="s">
+      <c r="C3" s="90"/>
+      <c r="D3" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="91"/>
-      <c r="F3" s="92" t="s">
+      <c r="E3" s="90"/>
+      <c r="F3" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="91"/>
-      <c r="H3" s="89" t="s">
+      <c r="G3" s="90"/>
+      <c r="H3" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="90"/>
+      <c r="I3" s="89"/>
       <c r="J3" s="48" t="s">
         <v>45</v>
       </c>
@@ -22149,11 +22501,11 @@
       <c r="L3" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="92" t="s">
+      <c r="M3" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
     </row>
     <row r="4" spans="1:16" ht="100.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="26"/>
@@ -22827,8 +23179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F173229C-1150-4B07-9313-8228C415AB22}">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59:E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -22836,14 +23188,14 @@
     <col min="1" max="1" width="36.53125" customWidth="1"/>
     <col min="2" max="2" width="17.9296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.86328125" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="66" customWidth="1"/>
+    <col min="5" max="5" width="17.86328125" style="66" customWidth="1"/>
     <col min="6" max="6" width="15.19921875" customWidth="1"/>
     <col min="7" max="7" width="20.06640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="98" t="s">
         <v>244</v>
       </c>
       <c r="B1" s="66"/>
@@ -22857,13 +23209,17 @@
       <c r="C2" s="66"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="98" t="s">
         <v>211</v>
       </c>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="94" t="s">
         <v>247</v>
       </c>
-      <c r="C3" s="95"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3" s="94"/>
     </row>
     <row r="4" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="66"/>
@@ -22873,6 +23229,12 @@
       <c r="C4" s="66" t="s">
         <v>246</v>
       </c>
+      <c r="D4" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="66" t="s">
@@ -22884,8 +23246,12 @@
       <c r="C5" s="66">
         <v>5562643.7099799998</v>
       </c>
-      <c r="D5" s="95"/>
-      <c r="E5" s="96"/>
+      <c r="D5" s="66">
+        <v>140507084.19999999</v>
+      </c>
+      <c r="E5" s="66">
+        <v>7423709.5413899999</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="66" t="s">
@@ -22897,8 +23263,12 @@
       <c r="C6" s="66">
         <v>266917755.016</v>
       </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
+      <c r="D6" s="66">
+        <v>109584081420</v>
+      </c>
+      <c r="E6" s="66">
+        <v>291757821.61199999</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="66" t="s">
@@ -22910,8 +23280,12 @@
       <c r="C7" s="66">
         <v>110103.667866</v>
       </c>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
+      <c r="D7" s="66">
+        <v>3102582.6</v>
+      </c>
+      <c r="E7" s="66">
+        <v>3743908.1998399999</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="66" t="s">
@@ -22923,8 +23297,12 @@
       <c r="C8" s="66">
         <v>51695.933227300004</v>
       </c>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
+      <c r="D8" s="66">
+        <v>1974205.2</v>
+      </c>
+      <c r="E8" s="66">
+        <v>384777.404606</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="66" t="s">
@@ -22936,8 +23314,12 @@
       <c r="C9" s="66">
         <v>272231505.95099998</v>
       </c>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
+      <c r="D9" s="66">
+        <v>177105035513</v>
+      </c>
+      <c r="E9" s="66">
+        <v>311176819.338</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="66" t="s">
@@ -22949,8 +23331,12 @@
       <c r="C10" s="66">
         <v>5179857.5691900002</v>
       </c>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
+      <c r="D10" s="66">
+        <v>130848795.8</v>
+      </c>
+      <c r="E10" s="66">
+        <v>171232725.26199999</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="66" t="s">
@@ -22962,8 +23348,12 @@
       <c r="C11" s="66">
         <v>3675826.6224699998</v>
       </c>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
+      <c r="D11" s="66">
+        <v>77559277</v>
+      </c>
+      <c r="E11" s="66">
+        <v>4549899.54103</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="66" t="s">
@@ -22975,8 +23365,12 @@
       <c r="C12" s="66">
         <v>5455521.9034799999</v>
       </c>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
+      <c r="D12" s="66">
+        <v>119057604.8</v>
+      </c>
+      <c r="E12" s="66">
+        <v>10288982.711200001</v>
+      </c>
     </row>
     <row r="13" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="66"/>
@@ -22986,15 +23380,17 @@
       <c r="E13" s="66"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="98" t="s">
         <v>212</v>
       </c>
-      <c r="B14" s="95" t="s">
+      <c r="B14" s="94" t="s">
         <v>247</v>
       </c>
-      <c r="C14" s="95"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94" t="s">
+        <v>248</v>
+      </c>
+      <c r="E14" s="94"/>
     </row>
     <row r="15" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="66"/>
@@ -23004,8 +23400,12 @@
       <c r="C15" s="66" t="s">
         <v>246</v>
       </c>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
+      <c r="D15" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="66" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="66" t="s">
@@ -23017,8 +23417,12 @@
       <c r="C16" s="66">
         <v>2475963.8639099998</v>
       </c>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
+      <c r="D16" s="66">
+        <v>68454870</v>
+      </c>
+      <c r="E16" s="66">
+        <v>3490367.6106699998</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="66" t="s">
@@ -23030,6 +23434,12 @@
       <c r="C17" s="66">
         <v>278025822.32700002</v>
       </c>
+      <c r="D17" s="66">
+        <v>110467705371</v>
+      </c>
+      <c r="E17" s="66">
+        <v>254081561.78999999</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="66" t="s">
@@ -23041,6 +23451,12 @@
       <c r="C18" s="66">
         <v>71439.602914899995</v>
       </c>
+      <c r="D18" s="66">
+        <v>1936812.2</v>
+      </c>
+      <c r="E18" s="66">
+        <v>724311.367753</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="66" t="s">
@@ -23052,6 +23468,12 @@
       <c r="C19" s="66">
         <v>131485.37587600001</v>
       </c>
+      <c r="D19" s="66">
+        <v>2162128</v>
+      </c>
+      <c r="E19" s="66">
+        <v>94677.016163399996</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="66" t="s">
@@ -23063,8 +23485,12 @@
       <c r="C20" s="66">
         <v>362827147.80500001</v>
       </c>
-      <c r="D20" s="95"/>
-      <c r="E20" s="96"/>
+      <c r="D20" s="66">
+        <v>178278349585</v>
+      </c>
+      <c r="E20" s="66">
+        <v>296906861.25400001</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="66" t="s">
@@ -23076,8 +23502,12 @@
       <c r="C21" s="66">
         <v>8145547.4997800002</v>
       </c>
-      <c r="D21" s="82"/>
-      <c r="E21" s="82"/>
+      <c r="D21" s="66">
+        <v>49585662.799999997</v>
+      </c>
+      <c r="E21" s="66">
+        <v>8105395.9591899998</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="66" t="s">
@@ -23089,8 +23519,12 @@
       <c r="C22" s="66">
         <v>1689310.1185600001</v>
       </c>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
+      <c r="D22" s="66">
+        <v>74519491.400000006</v>
+      </c>
+      <c r="E22" s="66">
+        <v>4605892.6965699997</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="66" t="s">
@@ -23102,8 +23536,12 @@
       <c r="C23" s="66">
         <v>2255689.88907</v>
       </c>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
+      <c r="D23" s="66">
+        <v>154853984.80000001</v>
+      </c>
+      <c r="E23" s="66">
+        <v>6741885.7954799999</v>
+      </c>
     </row>
     <row r="24" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="66"/>
@@ -23113,15 +23551,17 @@
       <c r="E24" s="66"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="98" t="s">
         <v>213</v>
       </c>
-      <c r="B25" s="95" t="s">
+      <c r="B25" s="94" t="s">
         <v>247</v>
       </c>
-      <c r="C25" s="95"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="66"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="94" t="s">
+        <v>248</v>
+      </c>
+      <c r="E25" s="94"/>
     </row>
     <row r="26" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="66"/>
@@ -23131,8 +23571,12 @@
       <c r="C26" s="66" t="s">
         <v>246</v>
       </c>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
+      <c r="D26" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="66" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="66" t="s">
@@ -23144,8 +23588,12 @@
       <c r="C27" s="66">
         <v>2714820.20946</v>
       </c>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
+      <c r="D27" s="66">
+        <v>126606713.2</v>
+      </c>
+      <c r="E27" s="66">
+        <v>5208346.3876400003</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="66" t="s">
@@ -23157,8 +23605,12 @@
       <c r="C28" s="66">
         <v>154369292.24599999</v>
       </c>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
+      <c r="D28" s="66">
+        <v>110305965844</v>
+      </c>
+      <c r="E28" s="66">
+        <v>201496586.58199999</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="66" t="s">
@@ -23170,8 +23622,12 @@
       <c r="C29" s="66">
         <v>104099.279755</v>
       </c>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66"/>
+      <c r="D29" s="66">
+        <v>1941495.4</v>
+      </c>
+      <c r="E29" s="66">
+        <v>183110.868411</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="66" t="s">
@@ -23183,8 +23639,12 @@
       <c r="C30" s="66">
         <v>78603.873984899998</v>
       </c>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
+      <c r="D30" s="66">
+        <v>2239316.7999999998</v>
+      </c>
+      <c r="E30" s="66">
+        <v>247239.329952</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="66" t="s">
@@ -23196,8 +23656,12 @@
       <c r="C31" s="66">
         <v>99989037.071999997</v>
       </c>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
+      <c r="D31" s="66">
+        <v>178998060625</v>
+      </c>
+      <c r="E31" s="66">
+        <v>165378286.26100001</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="66" t="s">
@@ -23209,8 +23673,14 @@
       <c r="C32" s="66">
         <v>24665525.0524</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D32" s="66">
+        <v>56291125.399999999</v>
+      </c>
+      <c r="E32" s="66">
+        <v>7380528.4371300004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="66" t="s">
         <v>6</v>
       </c>
@@ -23220,8 +23690,14 @@
       <c r="C33" s="66">
         <v>1411621.13934</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D33" s="66">
+        <v>76966460.200000003</v>
+      </c>
+      <c r="E33" s="66">
+        <v>3508916.4789100001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="66" t="s">
         <v>20</v>
       </c>
@@ -23231,31 +23707,49 @@
       <c r="C34" s="66">
         <v>2124486.4452999998</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" s="65" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D34" s="66">
+        <v>57667330.399999999</v>
+      </c>
+      <c r="E34" s="66">
+        <v>769966.25150400004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A35" s="66"/>
       <c r="B35" s="66"/>
       <c r="C35" s="66"/>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A36" s="100" t="s">
+      <c r="D35" s="66"/>
+      <c r="E35" s="66"/>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A36" s="98" t="s">
         <v>214</v>
       </c>
-      <c r="B36" s="95" t="s">
+      <c r="B36" s="94" t="s">
         <v>247</v>
       </c>
-      <c r="C36" s="95"/>
-    </row>
-    <row r="37" spans="1:3" s="65" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="101"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="94" t="s">
+        <v>248</v>
+      </c>
+      <c r="E36" s="94"/>
+    </row>
+    <row r="37" spans="1:5" s="65" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="99"/>
       <c r="B37" s="66" t="s">
         <v>27</v>
       </c>
       <c r="C37" s="66" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D37" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="66" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" s="66" t="s">
         <v>15</v>
       </c>
@@ -23265,8 +23759,14 @@
       <c r="C38" s="66">
         <v>7333563.0097599998</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D38" s="66">
+        <v>154876486.19999999</v>
+      </c>
+      <c r="E38" s="66">
+        <v>3902159.5551499999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" s="66" t="s">
         <v>2</v>
       </c>
@@ -23276,8 +23776,14 @@
       <c r="C39" s="66">
         <v>162055593.63600001</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D39" s="66">
+        <v>109843069901</v>
+      </c>
+      <c r="E39" s="66">
+        <v>141359482.09099999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" s="66" t="s">
         <v>35</v>
       </c>
@@ -23287,8 +23793,14 @@
       <c r="C40" s="66">
         <v>184028.060192</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D40" s="66">
+        <v>2195633</v>
+      </c>
+      <c r="E40" s="66">
+        <v>565382.58637200005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" s="66" t="s">
         <v>36</v>
       </c>
@@ -23298,8 +23810,14 @@
       <c r="C41" s="66">
         <v>142184.520797</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D41" s="66">
+        <v>2296027.7999999998</v>
+      </c>
+      <c r="E41" s="66">
+        <v>66437.594427899996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="66" t="s">
         <v>1</v>
       </c>
@@ -23309,8 +23827,14 @@
       <c r="C42" s="66">
         <v>172826087.759</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D42" s="66">
+        <v>177108684090</v>
+      </c>
+      <c r="E42" s="66">
+        <v>34473622.656199999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="66" t="s">
         <v>4</v>
       </c>
@@ -23320,8 +23844,14 @@
       <c r="C43" s="66">
         <v>8767991.1419300009</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D43" s="66">
+        <v>78047389.599999994</v>
+      </c>
+      <c r="E43" s="66">
+        <v>17949252.723200001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" s="66" t="s">
         <v>6</v>
       </c>
@@ -23331,8 +23861,14 @@
       <c r="C44" s="66">
         <v>798964.64845600002</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D44" s="66">
+        <v>85129981.799999997</v>
+      </c>
+      <c r="E44" s="66">
+        <v>6259223.48587</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" s="66" t="s">
         <v>20</v>
       </c>
@@ -23342,31 +23878,49 @@
       <c r="C45" s="66">
         <v>5348658.7459100001</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" s="65" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D45" s="66">
+        <v>360259678.39999998</v>
+      </c>
+      <c r="E45" s="66">
+        <v>7467498.1551700002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A46" s="66"/>
       <c r="B46" s="66"/>
       <c r="C46" s="66"/>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A47" s="100" t="s">
+      <c r="D46" s="66"/>
+      <c r="E46" s="66"/>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A47" s="98" t="s">
         <v>216</v>
       </c>
-      <c r="B47" s="95" t="s">
+      <c r="B47" s="94" t="s">
         <v>247</v>
       </c>
-      <c r="C47" s="95"/>
-    </row>
-    <row r="48" spans="1:3" s="65" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A48" s="100"/>
+      <c r="C47" s="94"/>
+      <c r="D47" s="94" t="s">
+        <v>248</v>
+      </c>
+      <c r="E47" s="94"/>
+    </row>
+    <row r="48" spans="1:5" s="65" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A48" s="98"/>
       <c r="B48" s="66" t="s">
         <v>27</v>
       </c>
       <c r="C48" s="66" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D48" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" s="66" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="66" t="s">
         <v>15</v>
       </c>
@@ -23376,8 +23930,14 @@
       <c r="C49" s="66">
         <v>3062836.7971899998</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D49" s="66">
+        <v>424724617.19999999</v>
+      </c>
+      <c r="E49" s="66">
+        <v>5288755.3796100002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="66" t="s">
         <v>2</v>
       </c>
@@ -23387,8 +23947,14 @@
       <c r="C50" s="66">
         <v>1041967512.6900001</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D50" s="66">
+        <v>112649802716</v>
+      </c>
+      <c r="E50" s="66">
+        <v>607205835.21000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" s="66" t="s">
         <v>35</v>
       </c>
@@ -23398,8 +23964,14 @@
       <c r="C51" s="66">
         <v>59474.552194999997</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D51" s="66">
+        <v>1411865.4</v>
+      </c>
+      <c r="E51" s="66">
+        <v>116826.332635</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="66" t="s">
         <v>36</v>
       </c>
@@ -23409,8 +23981,14 @@
       <c r="C52" s="66">
         <v>165029.68992100001</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D52" s="66">
+        <v>2693496</v>
+      </c>
+      <c r="E52" s="66">
+        <v>89565.3032217</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="66" t="s">
         <v>1</v>
       </c>
@@ -23420,8 +23998,14 @@
       <c r="C53" s="66">
         <v>621877562.13800001</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D53" s="66">
+        <v>179082100682</v>
+      </c>
+      <c r="E53" s="66">
+        <v>714628998.153</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" s="66" t="s">
         <v>4</v>
       </c>
@@ -23431,8 +24015,14 @@
       <c r="C54" s="66">
         <v>234791241.579</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D54" s="66">
+        <v>75997480.599999994</v>
+      </c>
+      <c r="E54" s="66">
+        <v>35186909.071599998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="66" t="s">
         <v>6</v>
       </c>
@@ -23442,8 +24032,14 @@
       <c r="C55" s="66">
         <v>4667878.6997499997</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D55" s="66">
+        <v>113291532</v>
+      </c>
+      <c r="E55" s="66">
+        <v>6932359.8661000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="66" t="s">
         <v>20</v>
       </c>
@@ -23453,36 +24049,54 @@
       <c r="C56" s="66">
         <v>47738362.114399999</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" s="65" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D56" s="66">
+        <v>790296623.39999998</v>
+      </c>
+      <c r="E56" s="66">
+        <v>45006982.528200001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A57" s="66"/>
       <c r="B57" s="66"/>
       <c r="C57" s="66"/>
-    </row>
-    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A58" s="100"/>
-      <c r="B58" s="95"/>
-      <c r="C58" s="95"/>
-    </row>
-    <row r="59" spans="1:3" s="65" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A59" s="100" t="s">
+      <c r="D57" s="66"/>
+      <c r="E57" s="66"/>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A58" s="98"/>
+      <c r="B58" s="94"/>
+      <c r="C58" s="94"/>
+    </row>
+    <row r="59" spans="1:5" s="65" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A59" s="98" t="s">
         <v>221</v>
       </c>
-      <c r="B59" s="95" t="s">
+      <c r="B59" s="94" t="s">
         <v>247</v>
       </c>
-      <c r="C59" s="95"/>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A60" s="100"/>
+      <c r="C59" s="94"/>
+      <c r="D59" s="94" t="s">
+        <v>248</v>
+      </c>
+      <c r="E59" s="94"/>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A60" s="98"/>
       <c r="B60" s="66" t="s">
         <v>27</v>
       </c>
       <c r="C60" s="66" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D60" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" s="66" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" s="66" t="s">
         <v>15</v>
       </c>
@@ -23492,8 +24106,14 @@
       <c r="C61" s="66">
         <v>12768737.4175</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D61" s="66">
+        <v>25562806.199999999</v>
+      </c>
+      <c r="E61" s="66">
+        <v>321733.28533599997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" s="66" t="s">
         <v>2</v>
       </c>
@@ -23503,8 +24123,14 @@
       <c r="C62" s="66">
         <v>225536804.248</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D62" s="66">
+        <v>113379659884</v>
+      </c>
+      <c r="E62" s="66">
+        <v>831762911.65699995</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" s="66" t="s">
         <v>35</v>
       </c>
@@ -23514,8 +24140,14 @@
       <c r="C63" s="66">
         <v>75762.627542600007</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D63" s="66">
+        <v>2859571.2000000002</v>
+      </c>
+      <c r="E63" s="66">
+        <v>3661431.6962899999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64" s="66" t="s">
         <v>36</v>
       </c>
@@ -23525,8 +24157,14 @@
       <c r="C64" s="66">
         <v>28461.100852899999</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D64" s="66">
+        <v>2045564.2</v>
+      </c>
+      <c r="E64" s="66">
+        <v>86572.937890300003</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65" s="66" t="s">
         <v>1</v>
       </c>
@@ -23536,8 +24174,14 @@
       <c r="C65" s="66">
         <v>394443241.889</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D65" s="66">
+        <v>181408620461</v>
+      </c>
+      <c r="E65" s="66">
+        <v>890616601.94799995</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66" s="66" t="s">
         <v>4</v>
       </c>
@@ -23547,8 +24191,14 @@
       <c r="C66" s="66">
         <v>10422934.581800001</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D66" s="66">
+        <v>120825261.40000001</v>
+      </c>
+      <c r="E66" s="66">
+        <v>126606042.023</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67" s="66" t="s">
         <v>6</v>
       </c>
@@ -23558,8 +24208,14 @@
       <c r="C67" s="66">
         <v>2084831.63961</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" s="65" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D67" s="66">
+        <v>67914320</v>
+      </c>
+      <c r="E67" s="66">
+        <v>4807809.9957299996</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A68" s="66" t="s">
         <v>20</v>
       </c>
@@ -23569,19 +24225,32 @@
       <c r="C68" s="66">
         <v>257053.50531899999</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" s="65" customFormat="1" x14ac:dyDescent="0.45"/>
+      <c r="D68" s="66">
+        <v>22640884.199999999</v>
+      </c>
+      <c r="E68" s="66">
+        <v>505498.69384899997</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D70" s="66"/>
+      <c r="E70" s="66"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D59:E59"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B58:C58"/>
     <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D20:E20"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
put back results for compiler.compiler
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="441" documentId="81D8B261ABBD5CBDED69DEB44BA5B0CD337C6AB9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{32A96FE8-C57D-45F6-B521-45A4542122E5}"/>
+  <xr:revisionPtr revIDLastSave="448" documentId="81D8B261ABBD5CBDED69DEB44BA5B0CD337C6AB9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{AFC8E04A-FB76-4F65-86EC-3DCE3A29B7F6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -18,14 +18,15 @@
     <sheet name="clang-stats" sheetId="17" r:id="rId8"/>
     <sheet name="SPECjvm2008-os" sheetId="30" r:id="rId9"/>
     <sheet name="SPECjvm2008-usr" sheetId="33" r:id="rId10"/>
-    <sheet name="SPECjvm2008-summary" sheetId="31" r:id="rId11"/>
-    <sheet name="postgres summary" sheetId="27" r:id="rId12"/>
-    <sheet name="postgres-os" sheetId="25" r:id="rId13"/>
-    <sheet name="postgres-usr" sheetId="26" r:id="rId14"/>
-    <sheet name="octane-os" sheetId="20" r:id="rId15"/>
-    <sheet name="octane-usr" sheetId="21" r:id="rId16"/>
-    <sheet name="octane-stats" sheetId="22" r:id="rId17"/>
-    <sheet name="postgres_stats" sheetId="9" r:id="rId18"/>
+    <sheet name="SPECjvm2008-old-results" sheetId="34" r:id="rId11"/>
+    <sheet name="SPECjvm2008-summary" sheetId="31" r:id="rId12"/>
+    <sheet name="postgres summary" sheetId="27" r:id="rId13"/>
+    <sheet name="postgres-os" sheetId="25" r:id="rId14"/>
+    <sheet name="postgres-usr" sheetId="26" r:id="rId15"/>
+    <sheet name="octane-os" sheetId="20" r:id="rId16"/>
+    <sheet name="octane-usr" sheetId="21" r:id="rId17"/>
+    <sheet name="octane-stats" sheetId="22" r:id="rId18"/>
+    <sheet name="postgres_stats" sheetId="9" r:id="rId19"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="255">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -688,6 +689,18 @@
     <t>10GB/2MB * 2 # of super pages for each iteration</t>
   </si>
   <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>USR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enable UseLargePage in jvm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Disable UseLargePage in jvm</t>
+  </si>
+  <si>
     <t>Results are normalized to the baseline</t>
   </si>
   <si>
@@ -794,6 +807,12 @@
   </si>
   <si>
     <t>some IO</t>
+  </si>
+  <si>
+    <t>java -jar SPECjvm2008.jar compiler.compiler</t>
+  </si>
+  <si>
+    <t>Disable UseLargePage in jvm (Disable alignment)</t>
   </si>
   <si>
     <t>java -jar SPECjvm2008.jar BENCHMARK</t>
@@ -1027,7 +1046,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1205,6 +1224,9 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1216,6 +1238,18 @@
     </xf>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -7097,8 +7131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A67B38-292E-4CA0-8E76-A7B2040A6BB6}">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59:E60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7111,29 +7145,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="98" t="s">
-        <v>244</v>
+      <c r="A1" s="99" t="s">
+        <v>250</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="66" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="B2" s="66"/>
       <c r="C2" s="66"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A3" s="98" t="s">
-        <v>211</v>
+      <c r="A3" s="99" t="s">
+        <v>215</v>
       </c>
       <c r="B3" s="94" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C3" s="94"/>
       <c r="D3" s="94" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E3" s="94"/>
     </row>
@@ -7143,13 +7177,13 @@
         <v>27</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D4" s="66" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -7294,15 +7328,15 @@
       <c r="C13" s="66"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A14" s="98" t="s">
-        <v>212</v>
+      <c r="A14" s="99" t="s">
+        <v>216</v>
       </c>
       <c r="B14" s="94" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C14" s="94"/>
       <c r="D14" s="94" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E14" s="94"/>
     </row>
@@ -7312,13 +7346,13 @@
         <v>27</v>
       </c>
       <c r="C15" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D15" s="66" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
@@ -7463,15 +7497,15 @@
       <c r="C24" s="66"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A25" s="98" t="s">
-        <v>213</v>
+      <c r="A25" s="99" t="s">
+        <v>217</v>
       </c>
       <c r="B25" s="94" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C25" s="94"/>
       <c r="D25" s="94" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E25" s="94"/>
     </row>
@@ -7481,13 +7515,13 @@
         <v>27</v>
       </c>
       <c r="C26" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D26" s="66" t="s">
         <v>27</v>
       </c>
       <c r="E26" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
@@ -7632,31 +7666,31 @@
       <c r="C35" s="66"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A36" s="98" t="s">
-        <v>214</v>
+      <c r="A36" s="99" t="s">
+        <v>218</v>
       </c>
       <c r="B36" s="94" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C36" s="94"/>
       <c r="D36" s="94" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E36" s="94"/>
     </row>
     <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="99"/>
+      <c r="A37" s="100"/>
       <c r="B37" s="66" t="s">
         <v>27</v>
       </c>
       <c r="C37" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D37" s="66" t="s">
         <v>27</v>
       </c>
       <c r="E37" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.45">
@@ -7801,31 +7835,31 @@
       <c r="C46" s="66"/>
     </row>
     <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A47" s="98" t="s">
-        <v>216</v>
+      <c r="A47" s="99" t="s">
+        <v>220</v>
       </c>
       <c r="B47" s="94" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C47" s="94"/>
       <c r="D47" s="94" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E47" s="94"/>
     </row>
     <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A48" s="98"/>
+      <c r="A48" s="99"/>
       <c r="B48" s="66" t="s">
         <v>27</v>
       </c>
       <c r="C48" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D48" s="66" t="s">
         <v>27</v>
       </c>
       <c r="E48" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.45">
@@ -7970,35 +8004,37 @@
       <c r="C57" s="66"/>
     </row>
     <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A58" s="98"/>
+      <c r="A58" s="99"/>
       <c r="B58" s="94"/>
       <c r="C58" s="94"/>
     </row>
     <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A59" s="98" t="s">
-        <v>221</v>
+      <c r="A59" s="99" t="s">
+        <v>225</v>
       </c>
       <c r="B59" s="94" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C59" s="94"/>
       <c r="D59" s="94" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E59" s="94"/>
     </row>
     <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A60" s="98"/>
+      <c r="A60" s="99"/>
       <c r="B60" s="66" t="s">
         <v>27</v>
       </c>
       <c r="C60" s="66" t="s">
-        <v>246</v>
-      </c>
-      <c r="D60" s="94" t="s">
-        <v>248</v>
-      </c>
-      <c r="E60" s="94"/>
+        <v>252</v>
+      </c>
+      <c r="D60" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" s="66" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" s="66" t="s">
@@ -8137,8 +8173,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="D60:E60"/>
+  <mergeCells count="13">
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D14:E14"/>
@@ -8158,10 +8193,414 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CDBF21-342B-4234-A56D-2C760D6B9FBB}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="35.19921875" customWidth="1"/>
+    <col min="2" max="2" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A1" s="99" t="s">
+        <v>248</v>
+      </c>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="103"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="106" t="s">
+        <v>208</v>
+      </c>
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="104"/>
+      <c r="B4" s="94" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" s="101"/>
+      <c r="D4" s="95" t="s">
+        <v>249</v>
+      </c>
+      <c r="E4" s="102"/>
+    </row>
+    <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="105" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="105" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="105" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="105" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="103" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="103">
+        <v>848515828.20000005</v>
+      </c>
+      <c r="C6" s="103">
+        <v>31125912.630600002</v>
+      </c>
+      <c r="D6" s="103">
+        <v>840330563</v>
+      </c>
+      <c r="E6" s="103">
+        <v>24387713.008200001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="103" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="103">
+        <v>140402962470</v>
+      </c>
+      <c r="C7" s="103">
+        <v>651623475.11199999</v>
+      </c>
+      <c r="D7" s="103">
+        <v>140348996038</v>
+      </c>
+      <c r="E7" s="103">
+        <v>616223577.551</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="103" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="103">
+        <v>2644396</v>
+      </c>
+      <c r="C8" s="103">
+        <v>779678.30018699996</v>
+      </c>
+      <c r="D8" s="103">
+        <v>2330265.7999999998</v>
+      </c>
+      <c r="E8" s="103">
+        <v>420625.344896</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="103">
+        <v>3505292.4</v>
+      </c>
+      <c r="C9" s="103">
+        <v>394822.744389</v>
+      </c>
+      <c r="D9" s="103">
+        <v>3674564</v>
+      </c>
+      <c r="E9" s="103">
+        <v>26949.256546299999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="103" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="103">
+        <v>209033496735</v>
+      </c>
+      <c r="C10" s="103">
+        <v>1325523106.99</v>
+      </c>
+      <c r="D10" s="103">
+        <v>208488972487</v>
+      </c>
+      <c r="E10" s="103">
+        <v>890197947.329</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" s="103" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="103">
+        <v>138323111.59999999</v>
+      </c>
+      <c r="C11" s="103">
+        <v>19480498.205499999</v>
+      </c>
+      <c r="D11" s="103">
+        <v>153799543</v>
+      </c>
+      <c r="E11" s="103">
+        <v>42691851.003799997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="103">
+        <v>171923672.59999999</v>
+      </c>
+      <c r="C12" s="103">
+        <v>6170074.2861400004</v>
+      </c>
+      <c r="D12" s="103">
+        <v>177880719.59999999</v>
+      </c>
+      <c r="E12" s="103">
+        <v>10236150.110099999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" s="103" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="103">
+        <v>2547202360.8000002</v>
+      </c>
+      <c r="C13" s="103">
+        <v>123523596.719</v>
+      </c>
+      <c r="D13" s="103">
+        <v>2446884702.4000001</v>
+      </c>
+      <c r="E13" s="103">
+        <v>135724290.56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="103"/>
+      <c r="B14" s="103"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="103"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="103"/>
+      <c r="B15" s="103"/>
+      <c r="C15" s="103"/>
+      <c r="D15" s="103"/>
+      <c r="E15" s="103"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="106" t="s">
+        <v>209</v>
+      </c>
+      <c r="B16" s="103"/>
+      <c r="C16" s="103"/>
+      <c r="D16" s="103"/>
+      <c r="E16" s="103"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="104"/>
+      <c r="B17" s="94" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" s="101"/>
+      <c r="D17" s="94" t="s">
+        <v>211</v>
+      </c>
+      <c r="E17" s="101"/>
+    </row>
+    <row r="18" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="105" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="105" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="105" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="105" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="105" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="103" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="103">
+        <v>64023665052.199997</v>
+      </c>
+      <c r="C19" s="103">
+        <v>901945315.08700001</v>
+      </c>
+      <c r="D19" s="103">
+        <v>64170277315</v>
+      </c>
+      <c r="E19" s="103">
+        <v>1127219042.1600001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="103" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="103">
+        <v>2473983034190</v>
+      </c>
+      <c r="C20" s="103">
+        <v>14971484657</v>
+      </c>
+      <c r="D20" s="103">
+        <v>2478098843780</v>
+      </c>
+      <c r="E20" s="103">
+        <v>16463842483</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="103" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="103">
+        <v>19486541.199999999</v>
+      </c>
+      <c r="C21" s="103">
+        <v>1957661.6367800001</v>
+      </c>
+      <c r="D21" s="103">
+        <v>19266334</v>
+      </c>
+      <c r="E21" s="103">
+        <v>1437223.44961</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="103">
+        <v>217977453.80000001</v>
+      </c>
+      <c r="C22" s="103">
+        <v>11480066.7805</v>
+      </c>
+      <c r="D22" s="103">
+        <v>203274321</v>
+      </c>
+      <c r="E22" s="103">
+        <v>10443566.922800001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" s="103" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="103">
+        <v>2713558839040</v>
+      </c>
+      <c r="C23" s="103">
+        <v>20899612744.799999</v>
+      </c>
+      <c r="D23" s="103">
+        <v>2708449528150</v>
+      </c>
+      <c r="E23" s="103">
+        <v>23185814766.799999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" s="103" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="103">
+        <v>1733947706</v>
+      </c>
+      <c r="C24" s="103">
+        <v>645790981.324</v>
+      </c>
+      <c r="D24" s="103">
+        <v>1349642605.8</v>
+      </c>
+      <c r="E24" s="103">
+        <v>165785934.153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="103">
+        <v>15451772579</v>
+      </c>
+      <c r="C25" s="103">
+        <v>768428597.255</v>
+      </c>
+      <c r="D25" s="103">
+        <v>15726153788.200001</v>
+      </c>
+      <c r="E25" s="103">
+        <v>948509332.69700003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" s="103" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="103">
+        <v>255258511247</v>
+      </c>
+      <c r="C26" s="103">
+        <v>1877302684.26</v>
+      </c>
+      <c r="D26" s="103">
+        <v>254163773567</v>
+      </c>
+      <c r="E26" s="103">
+        <v>1935192897</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9BAF00-EAB6-4E4C-AFCD-518EB49BC392}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
@@ -8176,10 +8615,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="57" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C1" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D1" s="85" t="s">
         <v>35</v>
@@ -8190,10 +8629,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="20" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B2" s="86" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C2" s="20">
         <v>5183</v>
@@ -8207,10 +8646,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="20" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B3" s="86" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C3" s="20">
         <v>4720</v>
@@ -8224,10 +8663,10 @@
     </row>
     <row r="4" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B4" s="80" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C4">
         <v>603</v>
@@ -8241,10 +8680,10 @@
     </row>
     <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B5" s="80" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C5">
         <v>678</v>
@@ -8258,10 +8697,10 @@
     </row>
     <row r="6" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B6" s="80" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C6">
         <v>898</v>
@@ -8275,10 +8714,10 @@
     </row>
     <row r="7" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B7" s="80" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C7">
         <v>923</v>
@@ -8292,10 +8731,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="65" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B8" s="80" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C8">
         <v>3131</v>
@@ -8309,10 +8748,10 @@
     </row>
     <row r="9" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B9" s="80" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C9">
         <v>875</v>
@@ -8326,10 +8765,10 @@
     </row>
     <row r="10" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B10" s="80" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C10">
         <v>501</v>
@@ -8343,10 +8782,10 @@
     </row>
     <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="65" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B11" s="80" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C11">
         <v>469</v>
@@ -8360,10 +8799,10 @@
     </row>
     <row r="12" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="65" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B12" s="80" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C12">
         <v>486</v>
@@ -8377,10 +8816,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="65" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B13" s="80" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="C13">
         <v>479</v>
@@ -8394,10 +8833,10 @@
     </row>
     <row r="14" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B14" s="80" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C14">
         <v>582</v>
@@ -8411,10 +8850,10 @@
     </row>
     <row r="15" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="65" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B15" s="80" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C15">
         <v>1368</v>
@@ -8428,10 +8867,10 @@
     </row>
     <row r="16" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="65" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B16" s="80" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C16">
         <v>1352</v>
@@ -8445,10 +8884,10 @@
     </row>
     <row r="17" spans="1:5" ht="57" x14ac:dyDescent="0.45">
       <c r="A17" s="65" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B17" s="80" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C17">
         <v>4685</v>
@@ -8462,10 +8901,10 @@
     </row>
     <row r="18" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="65" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B18" s="80" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C18">
         <v>2490</v>
@@ -8483,7 +8922,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DCC425-F9E0-4DC1-9C1B-7FD63E026DA8}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -8502,18 +8941,18 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="22" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="95" t="s">
+      <c r="E2" s="96" t="s">
         <v>204</v>
       </c>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
     </row>
     <row r="3" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -8660,11 +9099,11 @@
       <c r="B11" s="65"/>
       <c r="C11" s="65"/>
       <c r="D11" s="65"/>
-      <c r="E11" s="95" t="s">
+      <c r="E11" s="96" t="s">
         <v>204</v>
       </c>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
     </row>
     <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="65" t="s">
@@ -8808,11 +9247,11 @@
       <c r="A20" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="95" t="s">
+      <c r="E20" s="96" t="s">
         <v>204</v>
       </c>
-      <c r="F20" s="95"/>
-      <c r="G20" s="95"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="96"/>
     </row>
     <row r="21" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" s="65" t="s">
@@ -8964,7 +9403,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638ACDA3-EFA6-47B5-8321-84E7AF859506}">
   <dimension ref="A1:P83"/>
   <sheetViews>
@@ -9083,22 +9522,22 @@
     </row>
     <row r="6" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="73"/>
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96" t="s">
+      <c r="C6" s="97"/>
+      <c r="D6" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96" t="s">
+      <c r="E6" s="97"/>
+      <c r="F6" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="97" t="s">
+      <c r="G6" s="97"/>
+      <c r="H6" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="97"/>
+      <c r="I6" s="98"/>
       <c r="J6" s="76" t="s">
         <v>45</v>
       </c>
@@ -9108,11 +9547,11 @@
       <c r="L6" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="96" t="s">
+      <c r="M6" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="96"/>
-      <c r="O6" s="96"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
       <c r="P6" s="73"/>
     </row>
     <row r="7" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -10343,22 +10782,22 @@
     </row>
     <row r="41" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A41" s="73"/>
-      <c r="B41" s="96" t="s">
+      <c r="B41" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C41" s="96"/>
-      <c r="D41" s="96" t="s">
+      <c r="C41" s="97"/>
+      <c r="D41" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E41" s="96"/>
-      <c r="F41" s="96" t="s">
+      <c r="E41" s="97"/>
+      <c r="F41" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G41" s="96"/>
-      <c r="H41" s="97" t="s">
+      <c r="G41" s="97"/>
+      <c r="H41" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I41" s="97"/>
+      <c r="I41" s="98"/>
       <c r="J41" s="76" t="s">
         <v>45</v>
       </c>
@@ -10368,11 +10807,11 @@
       <c r="L41" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M41" s="96" t="s">
+      <c r="M41" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N41" s="96"/>
-      <c r="O41" s="96"/>
+      <c r="N41" s="97"/>
+      <c r="O41" s="97"/>
       <c r="P41" s="73"/>
     </row>
     <row r="42" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -11522,22 +11961,22 @@
     </row>
     <row r="74" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A74" s="73"/>
-      <c r="B74" s="96" t="s">
+      <c r="B74" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C74" s="96"/>
-      <c r="D74" s="96" t="s">
+      <c r="C74" s="97"/>
+      <c r="D74" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E74" s="96"/>
-      <c r="F74" s="96" t="s">
+      <c r="E74" s="97"/>
+      <c r="F74" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G74" s="96"/>
-      <c r="H74" s="97" t="s">
+      <c r="G74" s="97"/>
+      <c r="H74" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I74" s="97"/>
+      <c r="I74" s="98"/>
       <c r="J74" s="76" t="s">
         <v>45</v>
       </c>
@@ -11547,11 +11986,11 @@
       <c r="L74" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M74" s="96" t="s">
+      <c r="M74" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N74" s="96"/>
-      <c r="O74" s="96"/>
+      <c r="N74" s="97"/>
+      <c r="O74" s="97"/>
       <c r="P74" s="73"/>
     </row>
     <row r="75" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -12081,7 +12520,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819BCD50-CCED-4858-989E-30CB05A9C1BE}">
   <dimension ref="A1:P79"/>
   <sheetViews>
@@ -13442,22 +13881,22 @@
     </row>
     <row r="40" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A40" s="73"/>
-      <c r="B40" s="96" t="s">
+      <c r="B40" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="96"/>
-      <c r="D40" s="96" t="s">
+      <c r="C40" s="97"/>
+      <c r="D40" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E40" s="96"/>
-      <c r="F40" s="96" t="s">
+      <c r="E40" s="97"/>
+      <c r="F40" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G40" s="96"/>
-      <c r="H40" s="97" t="s">
+      <c r="G40" s="97"/>
+      <c r="H40" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I40" s="97"/>
+      <c r="I40" s="98"/>
       <c r="J40" s="76" t="s">
         <v>45</v>
       </c>
@@ -13467,11 +13906,11 @@
       <c r="L40" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M40" s="96" t="s">
+      <c r="M40" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N40" s="96"/>
-      <c r="O40" s="96"/>
+      <c r="N40" s="97"/>
+      <c r="O40" s="97"/>
       <c r="P40" s="73"/>
     </row>
     <row r="41" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -13986,22 +14425,22 @@
     </row>
     <row r="54" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A54" s="73"/>
-      <c r="B54" s="96" t="s">
+      <c r="B54" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="96"/>
-      <c r="D54" s="96" t="s">
+      <c r="C54" s="97"/>
+      <c r="D54" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E54" s="96"/>
-      <c r="F54" s="96" t="s">
+      <c r="E54" s="97"/>
+      <c r="F54" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G54" s="96"/>
-      <c r="H54" s="97" t="s">
+      <c r="G54" s="97"/>
+      <c r="H54" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I54" s="97"/>
+      <c r="I54" s="98"/>
       <c r="J54" s="76" t="s">
         <v>45</v>
       </c>
@@ -14011,11 +14450,11 @@
       <c r="L54" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M54" s="96" t="s">
+      <c r="M54" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N54" s="96"/>
-      <c r="O54" s="96"/>
+      <c r="N54" s="97"/>
+      <c r="O54" s="97"/>
       <c r="P54" s="73"/>
     </row>
     <row r="55" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -14614,22 +15053,22 @@
     </row>
     <row r="70" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A70" s="73"/>
-      <c r="B70" s="96" t="s">
+      <c r="B70" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C70" s="96"/>
-      <c r="D70" s="96" t="s">
+      <c r="C70" s="97"/>
+      <c r="D70" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E70" s="96"/>
-      <c r="F70" s="96" t="s">
+      <c r="E70" s="97"/>
+      <c r="F70" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G70" s="96"/>
-      <c r="H70" s="97" t="s">
+      <c r="G70" s="97"/>
+      <c r="H70" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I70" s="97"/>
+      <c r="I70" s="98"/>
       <c r="J70" s="76" t="s">
         <v>45</v>
       </c>
@@ -14639,11 +15078,11 @@
       <c r="L70" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M70" s="96" t="s">
+      <c r="M70" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N70" s="96"/>
-      <c r="O70" s="96"/>
+      <c r="N70" s="97"/>
+      <c r="O70" s="97"/>
       <c r="P70" s="73"/>
     </row>
     <row r="71" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -15168,7 +15607,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC958D8-824A-4FFE-8EFB-EA4CAF2DCC74}">
   <dimension ref="A1:P12"/>
   <sheetViews>
@@ -15196,22 +15635,22 @@
     </row>
     <row r="3" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="73"/>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96" t="s">
+      <c r="C3" s="97"/>
+      <c r="D3" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96" t="s">
+      <c r="E3" s="97"/>
+      <c r="F3" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="96"/>
-      <c r="H3" s="97" t="s">
+      <c r="G3" s="97"/>
+      <c r="H3" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="97"/>
+      <c r="I3" s="98"/>
       <c r="J3" s="76" t="s">
         <v>45</v>
       </c>
@@ -15221,11 +15660,11 @@
       <c r="L3" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="96" t="s">
+      <c r="M3" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
       <c r="P3" s="73"/>
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -15740,7 +16179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F72758A-17BC-4C1E-98B0-DDD6331D597C}">
   <dimension ref="A1:P12"/>
   <sheetViews>
@@ -15769,22 +16208,22 @@
     </row>
     <row r="3" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="73"/>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96" t="s">
+      <c r="C3" s="97"/>
+      <c r="D3" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96" t="s">
+      <c r="E3" s="97"/>
+      <c r="F3" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="96"/>
-      <c r="H3" s="97" t="s">
+      <c r="G3" s="97"/>
+      <c r="H3" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="97"/>
+      <c r="I3" s="98"/>
       <c r="J3" s="76" t="s">
         <v>45</v>
       </c>
@@ -15794,11 +16233,11 @@
       <c r="L3" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M3" s="96" t="s">
+      <c r="M3" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
       <c r="P3" s="73"/>
     </row>
     <row r="4" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
@@ -16313,7 +16752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C510FE-BA24-4F4C-B882-A73942D255FE}">
   <dimension ref="A1:D31"/>
   <sheetViews>
@@ -16681,7 +17120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5A357B-AD95-4B57-AFAC-6E90E36724A8}">
   <dimension ref="A1:H59"/>
   <sheetViews>
@@ -23179,8 +23618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F173229C-1150-4B07-9313-8228C415AB22}">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59:E60"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -23195,29 +23634,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="98" t="s">
-        <v>244</v>
+      <c r="A1" s="99" t="s">
+        <v>250</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="66" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="B2" s="66"/>
       <c r="C2" s="66"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A3" s="98" t="s">
-        <v>211</v>
+      <c r="A3" s="99" t="s">
+        <v>215</v>
       </c>
       <c r="B3" s="94" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C3" s="94"/>
       <c r="D3" s="94" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E3" s="94"/>
     </row>
@@ -23227,13 +23666,13 @@
         <v>27</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D4" s="66" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -23380,15 +23819,15 @@
       <c r="E13" s="66"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A14" s="98" t="s">
-        <v>212</v>
+      <c r="A14" s="99" t="s">
+        <v>216</v>
       </c>
       <c r="B14" s="94" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C14" s="94"/>
       <c r="D14" s="94" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E14" s="94"/>
     </row>
@@ -23398,13 +23837,13 @@
         <v>27</v>
       </c>
       <c r="C15" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D15" s="66" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
@@ -23551,15 +23990,15 @@
       <c r="E24" s="66"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A25" s="98" t="s">
-        <v>213</v>
+      <c r="A25" s="99" t="s">
+        <v>217</v>
       </c>
       <c r="B25" s="94" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C25" s="94"/>
       <c r="D25" s="94" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E25" s="94"/>
     </row>
@@ -23569,13 +24008,13 @@
         <v>27</v>
       </c>
       <c r="C26" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D26" s="66" t="s">
         <v>27</v>
       </c>
       <c r="E26" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
@@ -23722,31 +24161,31 @@
       <c r="E35" s="66"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A36" s="98" t="s">
-        <v>214</v>
+      <c r="A36" s="99" t="s">
+        <v>218</v>
       </c>
       <c r="B36" s="94" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C36" s="94"/>
       <c r="D36" s="94" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E36" s="94"/>
     </row>
     <row r="37" spans="1:5" s="65" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="99"/>
+      <c r="A37" s="100"/>
       <c r="B37" s="66" t="s">
         <v>27</v>
       </c>
       <c r="C37" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D37" s="66" t="s">
         <v>27</v>
       </c>
       <c r="E37" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.45">
@@ -23893,31 +24332,31 @@
       <c r="E46" s="66"/>
     </row>
     <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A47" s="98" t="s">
-        <v>216</v>
+      <c r="A47" s="99" t="s">
+        <v>220</v>
       </c>
       <c r="B47" s="94" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C47" s="94"/>
       <c r="D47" s="94" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E47" s="94"/>
     </row>
     <row r="48" spans="1:5" s="65" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A48" s="98"/>
+      <c r="A48" s="99"/>
       <c r="B48" s="66" t="s">
         <v>27</v>
       </c>
       <c r="C48" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D48" s="66" t="s">
         <v>27</v>
       </c>
       <c r="E48" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.45">
@@ -24064,36 +24503,36 @@
       <c r="E57" s="66"/>
     </row>
     <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A58" s="98"/>
+      <c r="A58" s="99"/>
       <c r="B58" s="94"/>
       <c r="C58" s="94"/>
     </row>
     <row r="59" spans="1:5" s="65" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A59" s="98" t="s">
-        <v>221</v>
+      <c r="A59" s="99" t="s">
+        <v>225</v>
       </c>
       <c r="B59" s="94" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C59" s="94"/>
       <c r="D59" s="94" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E59" s="94"/>
     </row>
     <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A60" s="98"/>
+      <c r="A60" s="99"/>
       <c r="B60" s="66" t="s">
         <v>27</v>
       </c>
       <c r="C60" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D60" s="66" t="s">
         <v>27</v>
       </c>
       <c r="E60" s="66" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
added results for padded postgres code
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="536" documentId="81D8B261ABBD5CBDED69DEB44BA5B0CD337C6AB9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{48A877A6-EE7A-47F4-93D3-AE08A096CFB3}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="9E001895F985C8961FD5BD0910042522F195CEDD" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{C225736E-9255-4090-B326-F3A0AD72D41E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="262">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -832,6 +832,24 @@
   <si>
     <t>ops/min</t>
   </si>
+  <si>
+    <t>code super page with padding /baseline</t>
+  </si>
+  <si>
+    <t>code super page with padding</t>
+  </si>
+  <si>
+    <t>shared_ptp + super_page (col I/col B)</t>
+  </si>
+  <si>
+    <t>super page with padding (col K/ col B)</t>
+  </si>
+  <si>
+    <t>code super page with padding / baseline</t>
+  </si>
+  <si>
+    <t>code super page with padding (col k / col B)</t>
+  </si>
 </sst>
 </file>
 
@@ -1049,7 +1067,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1253,6 +1271,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -7134,8 +7153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A67B38-292E-4CA0-8E76-A7B2040A6BB6}">
   <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8846,14 +8865,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
     <mergeCell ref="B103:C103"/>
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="D56:E56"/>
@@ -8867,6 +8878,14 @@
     <mergeCell ref="B80:C80"/>
     <mergeCell ref="B91:C91"/>
     <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9281,7 +9300,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="D1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10112,10 +10131,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638ACDA3-EFA6-47B5-8321-84E7AF859506}">
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:T83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="E51" workbookViewId="0">
+      <selection activeCell="T59" sqref="T59:T66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10129,6 +10148,9 @@
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.45">
@@ -11907,7 +11929,7 @@
         <v>8.4556051264045029E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A49" s="66" t="s">
         <v>6</v>
       </c>
@@ -11964,7 +11986,7 @@
         <v>1.157815048342371E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A50" s="66" t="s">
         <v>20</v>
       </c>
@@ -12021,22 +12043,22 @@
         <v>1.2284606254294244E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A53" s="22" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A54" s="23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A55" s="24" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:20" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A57" s="2"/>
       <c r="B57" s="96" t="s">
         <v>24</v>
@@ -12054,23 +12076,31 @@
         <v>114</v>
       </c>
       <c r="I57" s="95"/>
-      <c r="J57" s="67" t="s">
+      <c r="J57" s="104" t="s">
+        <v>257</v>
+      </c>
+      <c r="K57" s="104"/>
+      <c r="L57" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="K57" s="67" t="s">
+      <c r="M57" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="L57" s="70" t="s">
+      <c r="N57" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="M57" s="97" t="s">
+      <c r="O57" s="71" t="s">
+        <v>260</v>
+      </c>
+      <c r="P57" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="N57" s="96"/>
-      <c r="O57" s="96"/>
-      <c r="P57" s="65"/>
-    </row>
-    <row r="58" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="Q57" s="97"/>
+      <c r="R57" s="97"/>
+      <c r="S57" s="97"/>
+      <c r="T57" s="97"/>
+    </row>
+    <row r="58" spans="1:20" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
         <v>23</v>
       </c>
@@ -12098,23 +12128,32 @@
       <c r="I58" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
-      <c r="L58" s="65"/>
-      <c r="M58" s="3" t="s">
+      <c r="J58" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="K58" s="76" t="s">
+        <v>26</v>
+      </c>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="65"/>
+      <c r="P58" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N58" s="67" t="s">
+      <c r="Q58" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="O58" s="67" t="s">
+      <c r="R58" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="P58" s="71" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="S58" s="71" t="s">
+        <v>258</v>
+      </c>
+      <c r="T58" s="71" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A59" s="65" t="s">
         <v>1</v>
       </c>
@@ -12142,36 +12181,50 @@
       <c r="I59" s="66">
         <v>336290655.68900001</v>
       </c>
-      <c r="J59" s="66">
+      <c r="J59" s="89">
+        <v>152349812576</v>
+      </c>
+      <c r="K59" s="89">
+        <v>610749918.77499998</v>
+      </c>
+      <c r="L59" s="66">
         <f>D59/B59</f>
         <v>1.0000443325984296</v>
       </c>
-      <c r="K59" s="66">
+      <c r="M59" s="66">
         <f>F59/B59</f>
         <v>0.98465747634512735</v>
       </c>
-      <c r="L59" s="66">
+      <c r="N59" s="66">
         <f>H59/B59</f>
         <v>0.99416564988741751</v>
       </c>
-      <c r="M59" s="66">
+      <c r="O59" s="89">
+        <f>J59/B59</f>
+        <v>0.98784338890431411</v>
+      </c>
+      <c r="P59" s="66">
         <f>C59/B59</f>
         <v>2.5679245796196831E-3</v>
       </c>
-      <c r="N59" s="66">
+      <c r="Q59" s="66">
         <f>E59/B59</f>
         <v>5.0348714573003293E-3</v>
       </c>
-      <c r="O59" s="66">
+      <c r="R59" s="66">
         <f>G59/B59</f>
         <v>2.3164541508076692E-3</v>
       </c>
-      <c r="P59" s="66">
+      <c r="S59" s="66">
         <f>I59/B59</f>
         <v>2.180524513654756E-3</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="T59" s="89">
+        <f>K59/B59</f>
+        <v>3.9601313538522448E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A60" s="65" t="s">
         <v>2</v>
       </c>
@@ -12199,36 +12252,50 @@
       <c r="I60" s="66">
         <v>11811502965.6</v>
       </c>
-      <c r="J60" s="66">
-        <f t="shared" ref="J60:J66" si="21">D60/B60</f>
+      <c r="J60" s="89">
+        <v>333899737888</v>
+      </c>
+      <c r="K60" s="89">
+        <v>295526922.85100001</v>
+      </c>
+      <c r="L60" s="66">
+        <f>D60/B60</f>
         <v>0.95969161330737685</v>
       </c>
-      <c r="K60" s="66">
-        <f t="shared" ref="K60:K66" si="22">F60/B60</f>
+      <c r="M60" s="66">
+        <f>F60/B60</f>
         <v>0.97730703010205444</v>
       </c>
-      <c r="L60" s="66">
-        <f t="shared" ref="L60:L66" si="23">H60/B60</f>
+      <c r="N60" s="66">
+        <f>H60/B60</f>
         <v>0.98336767356098986</v>
       </c>
-      <c r="M60" s="66">
-        <f t="shared" ref="M60:M66" si="24">C60/B60</f>
+      <c r="O60" s="89">
+        <f t="shared" ref="O60:O66" si="21">J60/B60</f>
+        <v>0.99827092886056268</v>
+      </c>
+      <c r="P60" s="66">
+        <f>C60/B60</f>
         <v>3.7585485952777767E-3</v>
       </c>
-      <c r="N60" s="66">
-        <f t="shared" ref="N60:N66" si="25">E60/B60</f>
+      <c r="Q60" s="66">
+        <f>E60/B60</f>
         <v>6.3958677532146048E-3</v>
       </c>
-      <c r="O60" s="66">
-        <f t="shared" ref="O60:O66" si="26">G60/B60</f>
+      <c r="R60" s="66">
+        <f>G60/B60</f>
         <v>3.3455391533576814E-3</v>
       </c>
-      <c r="P60" s="66">
-        <f t="shared" ref="P60:P66" si="27">I60/B60</f>
+      <c r="S60" s="66">
+        <f>I60/B60</f>
         <v>3.5313235378051977E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="T60" s="89">
+        <f t="shared" ref="T60:T66" si="22">K60/B60</f>
+        <v>8.835464730934555E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A61" s="65" t="s">
         <v>35</v>
       </c>
@@ -12256,36 +12323,50 @@
       <c r="I61" s="66">
         <v>1415999.3302199999</v>
       </c>
-      <c r="J61" s="66">
+      <c r="J61" s="89">
+        <v>38564055.600000001</v>
+      </c>
+      <c r="K61" s="89">
+        <v>1614908.7911</v>
+      </c>
+      <c r="L61" s="66">
+        <f>D61/B61</f>
+        <v>0.60540391337058364</v>
+      </c>
+      <c r="M61" s="66">
+        <f>F61/B61</f>
+        <v>0.7841508000723284</v>
+      </c>
+      <c r="N61" s="66">
+        <f>H61/B61</f>
+        <v>0.50421243971544372</v>
+      </c>
+      <c r="O61" s="89">
         <f t="shared" si="21"/>
-        <v>0.60540391337058364</v>
-      </c>
-      <c r="K61" s="66">
+        <v>0.42121858312347915</v>
+      </c>
+      <c r="P61" s="66">
+        <f>C61/B61</f>
+        <v>1.5372089947282393E-2</v>
+      </c>
+      <c r="Q61" s="66">
+        <f>E61/B61</f>
+        <v>1.9591451127776945E-2</v>
+      </c>
+      <c r="R61" s="66">
+        <f>G61/B61</f>
+        <v>3.1092950445319505E-2</v>
+      </c>
+      <c r="S61" s="66">
+        <f>I61/B61</f>
+        <v>1.546635130302695E-2</v>
+      </c>
+      <c r="T61" s="89">
         <f t="shared" si="22"/>
-        <v>0.7841508000723284</v>
-      </c>
-      <c r="L61" s="66">
-        <f t="shared" si="23"/>
-        <v>0.50421243971544372</v>
-      </c>
-      <c r="M61" s="66">
-        <f t="shared" si="24"/>
-        <v>1.5372089947282393E-2</v>
-      </c>
-      <c r="N61" s="66">
-        <f t="shared" si="25"/>
-        <v>1.9591451127776945E-2</v>
-      </c>
-      <c r="O61" s="66">
-        <f t="shared" si="26"/>
-        <v>3.1092950445319505E-2</v>
-      </c>
-      <c r="P61" s="66">
-        <f t="shared" si="27"/>
-        <v>1.546635130302695E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.45">
+        <v>1.7638953742738422E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A62" s="65" t="s">
         <v>36</v>
       </c>
@@ -12313,36 +12394,50 @@
       <c r="I62" s="66">
         <v>508277.09580800001</v>
       </c>
-      <c r="J62" s="66">
+      <c r="J62" s="89">
+        <v>28255273</v>
+      </c>
+      <c r="K62" s="89">
+        <v>4510084.6777999997</v>
+      </c>
+      <c r="L62" s="66">
+        <f>D62/B62</f>
+        <v>0.63466461865736301</v>
+      </c>
+      <c r="M62" s="66">
+        <f>F62/B62</f>
+        <v>1.2038510833267733</v>
+      </c>
+      <c r="N62" s="66">
+        <f>H62/B62</f>
+        <v>0.32461308738829514</v>
+      </c>
+      <c r="O62" s="89">
         <f t="shared" si="21"/>
-        <v>0.63466461865736301</v>
-      </c>
-      <c r="K62" s="66">
+        <v>2.399981004191615</v>
+      </c>
+      <c r="P62" s="66">
+        <f>C62/B62</f>
+        <v>4.1502100574481351E-2</v>
+      </c>
+      <c r="Q62" s="66">
+        <f>E62/B62</f>
+        <v>2.2185706437414791E-2</v>
+      </c>
+      <c r="R62" s="66">
+        <f>G62/B62</f>
+        <v>0.52431869463767466</v>
+      </c>
+      <c r="S62" s="66">
+        <f>I62/B62</f>
+        <v>4.3172662844378873E-2</v>
+      </c>
+      <c r="T62" s="89">
         <f t="shared" si="22"/>
-        <v>1.2038510833267733</v>
-      </c>
-      <c r="L62" s="66">
-        <f t="shared" si="23"/>
-        <v>0.32461308738829514</v>
-      </c>
-      <c r="M62" s="66">
-        <f t="shared" si="24"/>
-        <v>4.1502100574481351E-2</v>
-      </c>
-      <c r="N62" s="66">
-        <f t="shared" si="25"/>
-        <v>2.2185706437414791E-2</v>
-      </c>
-      <c r="O62" s="66">
-        <f t="shared" si="26"/>
-        <v>0.52431869463767466</v>
-      </c>
-      <c r="P62" s="66">
-        <f t="shared" si="27"/>
-        <v>4.3172662844378873E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.45">
+        <v>0.38308309935691154</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A63" s="65" t="s">
         <v>15</v>
       </c>
@@ -12370,36 +12465,50 @@
       <c r="I63" s="66">
         <v>186564319.986</v>
       </c>
-      <c r="J63" s="66">
+      <c r="J63" s="89">
+        <v>13733318987</v>
+      </c>
+      <c r="K63" s="89">
+        <v>230056561.917</v>
+      </c>
+      <c r="L63" s="66">
+        <f>D63/B63</f>
+        <v>0.99648093748767474</v>
+      </c>
+      <c r="M63" s="66">
+        <f>F63/B63</f>
+        <v>0.97726045564533492</v>
+      </c>
+      <c r="N63" s="66">
+        <f>H63/B63</f>
+        <v>1.0161351678799326</v>
+      </c>
+      <c r="O63" s="89">
         <f t="shared" si="21"/>
-        <v>0.99648093748767474</v>
-      </c>
-      <c r="K63" s="66">
+        <v>1.0245699721842993</v>
+      </c>
+      <c r="P63" s="66">
+        <f>C63/B63</f>
+        <v>9.0865966355335327E-3</v>
+      </c>
+      <c r="Q63" s="66">
+        <f>E63/B63</f>
+        <v>1.8267500105103231E-2</v>
+      </c>
+      <c r="R63" s="66">
+        <f>G63/B63</f>
+        <v>6.4647335208963931E-3</v>
+      </c>
+      <c r="S63" s="66">
+        <f>I63/B63</f>
+        <v>1.3918572802363376E-2</v>
+      </c>
+      <c r="T63" s="89">
         <f t="shared" si="22"/>
-        <v>0.97726045564533492</v>
-      </c>
-      <c r="L63" s="66">
-        <f t="shared" si="23"/>
-        <v>1.0161351678799326</v>
-      </c>
-      <c r="M63" s="66">
-        <f t="shared" si="24"/>
-        <v>9.0865966355335327E-3</v>
-      </c>
-      <c r="N63" s="66">
-        <f t="shared" si="25"/>
-        <v>1.8267500105103231E-2</v>
-      </c>
-      <c r="O63" s="66">
-        <f t="shared" si="26"/>
-        <v>6.4647335208963931E-3</v>
-      </c>
-      <c r="P63" s="66">
-        <f t="shared" si="27"/>
-        <v>1.3918572802363376E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.45">
+        <v>1.7163297922901163E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A64" s="65" t="s">
         <v>4</v>
       </c>
@@ -12427,36 +12536,50 @@
       <c r="I64" s="66">
         <v>53453576.313600004</v>
       </c>
-      <c r="J64" s="66">
+      <c r="J64" s="89">
+        <v>2119472151.8</v>
+      </c>
+      <c r="K64" s="89">
+        <v>78561700.676100001</v>
+      </c>
+      <c r="L64" s="66">
+        <f>D64/B64</f>
+        <v>0.84550127469207947</v>
+      </c>
+      <c r="M64" s="66">
+        <f>F64/B64</f>
+        <v>0.88999095103949322</v>
+      </c>
+      <c r="N64" s="66">
+        <f>H64/B64</f>
+        <v>0.69211779138008178</v>
+      </c>
+      <c r="O64" s="89">
         <f t="shared" si="21"/>
-        <v>0.84550127469207947</v>
-      </c>
-      <c r="K64" s="66">
+        <v>0.50376172157841681</v>
+      </c>
+      <c r="P64" s="66">
+        <f>C64/B64</f>
+        <v>1.1364230400370818E-2</v>
+      </c>
+      <c r="Q64" s="66">
+        <f>E64/B64</f>
+        <v>5.8348292273776928E-3</v>
+      </c>
+      <c r="R64" s="66">
+        <f>G64/B64</f>
+        <v>1.2396968721789544E-2</v>
+      </c>
+      <c r="S64" s="66">
+        <f>I64/B64</f>
+        <v>1.2704986760686356E-2</v>
+      </c>
+      <c r="T64" s="89">
         <f t="shared" si="22"/>
-        <v>0.88999095103949322</v>
-      </c>
-      <c r="L64" s="66">
-        <f t="shared" si="23"/>
-        <v>0.69211779138008178</v>
-      </c>
-      <c r="M64" s="66">
-        <f t="shared" si="24"/>
-        <v>1.1364230400370818E-2</v>
-      </c>
-      <c r="N64" s="66">
-        <f t="shared" si="25"/>
-        <v>5.8348292273776928E-3</v>
-      </c>
-      <c r="O64" s="66">
-        <f t="shared" si="26"/>
-        <v>1.2396968721789544E-2</v>
-      </c>
-      <c r="P64" s="66">
-        <f t="shared" si="27"/>
-        <v>1.2704986760686356E-2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.45">
+        <v>1.8672751868482659E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A65" s="65" t="s">
         <v>6</v>
       </c>
@@ -12484,36 +12607,50 @@
       <c r="I65" s="66">
         <v>8505820.7215299997</v>
       </c>
-      <c r="J65" s="66">
+      <c r="J65" s="89">
+        <v>2018861338</v>
+      </c>
+      <c r="K65" s="89">
+        <v>625092452.051</v>
+      </c>
+      <c r="L65" s="66">
+        <f>D65/B65</f>
+        <v>0.55648478927837985</v>
+      </c>
+      <c r="M65" s="66">
+        <f>F65/B65</f>
+        <v>0.5357893855430661</v>
+      </c>
+      <c r="N65" s="66">
+        <f>H65/B65</f>
+        <v>0.23860683113471773</v>
+      </c>
+      <c r="O65" s="89">
         <f t="shared" si="21"/>
-        <v>0.55648478927837985</v>
-      </c>
-      <c r="K65" s="66">
+        <v>1.2685083486568483</v>
+      </c>
+      <c r="P65" s="66">
+        <f>C65/B65</f>
+        <v>2.9394259298617203E-2</v>
+      </c>
+      <c r="Q65" s="66">
+        <f>E65/B65</f>
+        <v>3.1337832447520426E-2</v>
+      </c>
+      <c r="R65" s="66">
+        <f>G65/B65</f>
+        <v>4.668978130867478E-2</v>
+      </c>
+      <c r="S65" s="66">
+        <f>I65/B65</f>
+        <v>5.3444505545527567E-3</v>
+      </c>
+      <c r="T65" s="89">
         <f t="shared" si="22"/>
-        <v>0.5357893855430661</v>
-      </c>
-      <c r="L65" s="66">
-        <f t="shared" si="23"/>
-        <v>0.23860683113471773</v>
-      </c>
-      <c r="M65" s="66">
-        <f t="shared" si="24"/>
-        <v>2.9394259298617203E-2</v>
-      </c>
-      <c r="N65" s="66">
-        <f t="shared" si="25"/>
-        <v>3.1337832447520426E-2</v>
-      </c>
-      <c r="O65" s="66">
-        <f t="shared" si="26"/>
-        <v>4.668978130867478E-2</v>
-      </c>
-      <c r="P65" s="66">
-        <f t="shared" si="27"/>
-        <v>5.3444505545527567E-3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.45">
+        <v>0.39276347472907724</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A66" s="65" t="s">
         <v>20</v>
       </c>
@@ -12541,36 +12678,50 @@
       <c r="I66" s="66">
         <v>2375056.0667400002</v>
       </c>
-      <c r="J66" s="66">
+      <c r="J66" s="89">
+        <v>128485884</v>
+      </c>
+      <c r="K66" s="89">
+        <v>49094371.382399999</v>
+      </c>
+      <c r="L66" s="66">
+        <f>D66/B66</f>
+        <v>1.0168207254009509</v>
+      </c>
+      <c r="M66" s="66">
+        <f>F66/B66</f>
+        <v>0.97748605498583263</v>
+      </c>
+      <c r="N66" s="66">
+        <f>H66/B66</f>
+        <v>1.030300470782618</v>
+      </c>
+      <c r="O66" s="89">
         <f t="shared" si="21"/>
-        <v>1.0168207254009509</v>
-      </c>
-      <c r="K66" s="66">
+        <v>1.2428940871924952</v>
+      </c>
+      <c r="P66" s="66">
+        <f>C66/B66</f>
+        <v>1.9572405328803659E-2</v>
+      </c>
+      <c r="Q66" s="66">
+        <f>E66/B66</f>
+        <v>1.5976062836465903E-2</v>
+      </c>
+      <c r="R66" s="66">
+        <f>G66/B66</f>
+        <v>2.4115100389669308E-2</v>
+      </c>
+      <c r="S66" s="66">
+        <f>I66/B66</f>
+        <v>2.2974844007780736E-2</v>
+      </c>
+      <c r="T66" s="89">
         <f t="shared" si="22"/>
-        <v>0.97748605498583263</v>
-      </c>
-      <c r="L66" s="66">
-        <f t="shared" si="23"/>
-        <v>1.030300470782618</v>
-      </c>
-      <c r="M66" s="66">
-        <f t="shared" si="24"/>
-        <v>1.9572405328803659E-2</v>
-      </c>
-      <c r="N66" s="66">
-        <f t="shared" si="25"/>
-        <v>1.5976062836465903E-2</v>
-      </c>
-      <c r="O66" s="66">
-        <f t="shared" si="26"/>
-        <v>2.4115100389669308E-2</v>
-      </c>
-      <c r="P66" s="66">
-        <f t="shared" si="27"/>
-        <v>2.2974844007780736E-2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.45">
+        <v>0.47490900950346737</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A69" s="72" t="s">
         <v>117</v>
       </c>
@@ -12590,7 +12741,7 @@
       <c r="O69" s="65"/>
       <c r="P69" s="65"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A70" s="72" t="s">
         <v>150</v>
       </c>
@@ -12610,7 +12761,7 @@
       <c r="O70" s="65"/>
       <c r="P70" s="65"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A71" s="73" t="s">
         <v>151</v>
       </c>
@@ -12630,7 +12781,7 @@
       <c r="O71" s="65"/>
       <c r="P71" s="65"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A72" s="65"/>
       <c r="B72" s="65"/>
       <c r="C72" s="65"/>
@@ -12648,7 +12799,7 @@
       <c r="O72" s="65"/>
       <c r="P72" s="65"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A73" s="65"/>
       <c r="B73" s="65"/>
       <c r="C73" s="65"/>
@@ -12666,7 +12817,7 @@
       <c r="O73" s="65"/>
       <c r="P73" s="65"/>
     </row>
-    <row r="74" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:20" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A74" s="73"/>
       <c r="B74" s="105" t="s">
         <v>24</v>
@@ -12700,7 +12851,7 @@
       <c r="O74" s="105"/>
       <c r="P74" s="73"/>
     </row>
-    <row r="75" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:20" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A75" s="76" t="s">
         <v>23</v>
       </c>
@@ -12744,7 +12895,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A76" s="66" t="s">
         <v>1</v>
       </c>
@@ -12801,7 +12952,7 @@
         <v>4.9876712439188807E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A77" s="66" t="s">
         <v>2</v>
       </c>
@@ -12830,35 +12981,35 @@
         <v>14249038008</v>
       </c>
       <c r="J77" s="66">
-        <f t="shared" ref="J77:J83" si="28">D77/B77</f>
+        <f t="shared" ref="J77:J83" si="23">D77/B77</f>
         <v>1.013175818530567</v>
       </c>
       <c r="K77" s="66">
-        <f t="shared" ref="K77:K83" si="29">F77/B77</f>
+        <f t="shared" ref="K77:K83" si="24">F77/B77</f>
         <v>0.99595841242491778</v>
       </c>
       <c r="L77" s="66">
-        <f t="shared" ref="L77:L83" si="30">H77/B77</f>
+        <f t="shared" ref="L77:L83" si="25">H77/B77</f>
         <v>0.99217879714399082</v>
       </c>
       <c r="M77" s="66">
-        <f t="shared" ref="M77:M83" si="31">C77/B77</f>
+        <f t="shared" ref="M77:M83" si="26">C77/B77</f>
         <v>1.2534292601492512E-3</v>
       </c>
       <c r="N77" s="66">
-        <f t="shared" ref="N77:N83" si="32">E77/B77</f>
+        <f t="shared" ref="N77:N83" si="27">E77/B77</f>
         <v>3.1072629021230966E-2</v>
       </c>
       <c r="O77" s="66">
-        <f t="shared" ref="O77:O83" si="33">G77/B77</f>
+        <f t="shared" ref="O77:O83" si="28">G77/B77</f>
         <v>8.6163210539248886E-3</v>
       </c>
       <c r="P77" s="66">
-        <f t="shared" ref="P77:P83" si="34">I77/B77</f>
+        <f t="shared" ref="P77:P83" si="29">I77/B77</f>
         <v>4.3300039823683696E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A78" s="66" t="s">
         <v>35</v>
       </c>
@@ -12887,35 +13038,35 @@
         <v>1261450.3099700001</v>
       </c>
       <c r="J78" s="66">
+        <f t="shared" si="23"/>
+        <v>0.65759277966524476</v>
+      </c>
+      <c r="K78" s="66">
+        <f t="shared" si="24"/>
+        <v>0.83430155438252973</v>
+      </c>
+      <c r="L78" s="66">
+        <f t="shared" si="25"/>
+        <v>0.51231140565100886</v>
+      </c>
+      <c r="M78" s="66">
+        <f t="shared" si="26"/>
+        <v>2.7494215007743333E-2</v>
+      </c>
+      <c r="N78" s="66">
+        <f t="shared" si="27"/>
+        <v>9.2371964083267297E-3</v>
+      </c>
+      <c r="O78" s="66">
         <f t="shared" si="28"/>
-        <v>0.65759277966524476</v>
-      </c>
-      <c r="K78" s="66">
+        <v>3.4092430295134181E-2</v>
+      </c>
+      <c r="P78" s="66">
         <f t="shared" si="29"/>
-        <v>0.83430155438252973</v>
-      </c>
-      <c r="L78" s="66">
-        <f t="shared" si="30"/>
-        <v>0.51231140565100886</v>
-      </c>
-      <c r="M78" s="66">
-        <f t="shared" si="31"/>
-        <v>2.7494215007743333E-2</v>
-      </c>
-      <c r="N78" s="66">
-        <f t="shared" si="32"/>
-        <v>9.2371964083267297E-3</v>
-      </c>
-      <c r="O78" s="66">
-        <f t="shared" si="33"/>
-        <v>3.4092430295134181E-2</v>
-      </c>
-      <c r="P78" s="66">
-        <f t="shared" si="34"/>
         <v>1.4144857876882843E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A79" s="66" t="s">
         <v>36</v>
       </c>
@@ -12944,35 +13095,35 @@
         <v>173898.34443699999</v>
       </c>
       <c r="J79" s="66">
+        <f t="shared" si="23"/>
+        <v>0.85508664794077316</v>
+      </c>
+      <c r="K79" s="66">
+        <f t="shared" si="24"/>
+        <v>0.28439178710552965</v>
+      </c>
+      <c r="L79" s="66">
+        <f t="shared" si="25"/>
+        <v>0.2650538701525309</v>
+      </c>
+      <c r="M79" s="66">
+        <f t="shared" si="26"/>
+        <v>2.4430009609823399E-2</v>
+      </c>
+      <c r="N79" s="66">
+        <f t="shared" si="27"/>
+        <v>4.2686543594381475E-2</v>
+      </c>
+      <c r="O79" s="66">
         <f t="shared" si="28"/>
-        <v>0.85508664794077316</v>
-      </c>
-      <c r="K79" s="66">
+        <v>8.045940329922464E-3</v>
+      </c>
+      <c r="P79" s="66">
         <f t="shared" si="29"/>
-        <v>0.28439178710552965</v>
-      </c>
-      <c r="L79" s="66">
-        <f t="shared" si="30"/>
-        <v>0.2650538701525309</v>
-      </c>
-      <c r="M79" s="66">
-        <f t="shared" si="31"/>
-        <v>2.4430009609823399E-2</v>
-      </c>
-      <c r="N79" s="66">
-        <f t="shared" si="32"/>
-        <v>4.2686543594381475E-2</v>
-      </c>
-      <c r="O79" s="66">
-        <f t="shared" si="33"/>
-        <v>8.045940329922464E-3</v>
-      </c>
-      <c r="P79" s="66">
-        <f t="shared" si="34"/>
         <v>1.8568962841368376E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A80" s="66" t="s">
         <v>15</v>
       </c>
@@ -13001,31 +13152,31 @@
         <v>149206640.58399999</v>
       </c>
       <c r="J80" s="66">
+        <f t="shared" si="23"/>
+        <v>1.006417690061931</v>
+      </c>
+      <c r="K80" s="66">
+        <f t="shared" si="24"/>
+        <v>0.97945431168864105</v>
+      </c>
+      <c r="L80" s="66">
+        <f t="shared" si="25"/>
+        <v>1.0081582911006546</v>
+      </c>
+      <c r="M80" s="66">
+        <f t="shared" si="26"/>
+        <v>5.2165890181738962E-3</v>
+      </c>
+      <c r="N80" s="66">
+        <f t="shared" si="27"/>
+        <v>7.7504722627133723E-3</v>
+      </c>
+      <c r="O80" s="66">
         <f t="shared" si="28"/>
-        <v>1.006417690061931</v>
-      </c>
-      <c r="K80" s="66">
+        <v>6.7867790132102391E-3</v>
+      </c>
+      <c r="P80" s="66">
         <f t="shared" si="29"/>
-        <v>0.97945431168864105</v>
-      </c>
-      <c r="L80" s="66">
-        <f t="shared" si="30"/>
-        <v>1.0081582911006546</v>
-      </c>
-      <c r="M80" s="66">
-        <f t="shared" si="31"/>
-        <v>5.2165890181738962E-3</v>
-      </c>
-      <c r="N80" s="66">
-        <f t="shared" si="32"/>
-        <v>7.7504722627133723E-3</v>
-      </c>
-      <c r="O80" s="66">
-        <f t="shared" si="33"/>
-        <v>6.7867790132102391E-3</v>
-      </c>
-      <c r="P80" s="66">
-        <f t="shared" si="34"/>
         <v>1.120655750706852E-2</v>
       </c>
     </row>
@@ -13058,31 +13209,31 @@
         <v>58635839.859700002</v>
       </c>
       <c r="J81" s="66">
+        <f t="shared" si="23"/>
+        <v>0.84928597909913983</v>
+      </c>
+      <c r="K81" s="66">
+        <f t="shared" si="24"/>
+        <v>0.87307730213020363</v>
+      </c>
+      <c r="L81" s="66">
+        <f t="shared" si="25"/>
+        <v>0.6958715563828819</v>
+      </c>
+      <c r="M81" s="66">
+        <f t="shared" si="26"/>
+        <v>1.7621104115559366E-2</v>
+      </c>
+      <c r="N81" s="66">
+        <f t="shared" si="27"/>
+        <v>9.9041582310156109E-3</v>
+      </c>
+      <c r="O81" s="66">
         <f t="shared" si="28"/>
-        <v>0.84928597909913983</v>
-      </c>
-      <c r="K81" s="66">
+        <v>9.0053947992978379E-3</v>
+      </c>
+      <c r="P81" s="66">
         <f t="shared" si="29"/>
-        <v>0.87307730213020363</v>
-      </c>
-      <c r="L81" s="66">
-        <f t="shared" si="30"/>
-        <v>0.6958715563828819</v>
-      </c>
-      <c r="M81" s="66">
-        <f t="shared" si="31"/>
-        <v>1.7621104115559366E-2</v>
-      </c>
-      <c r="N81" s="66">
-        <f t="shared" si="32"/>
-        <v>9.9041582310156109E-3</v>
-      </c>
-      <c r="O81" s="66">
-        <f t="shared" si="33"/>
-        <v>9.0053947992978379E-3</v>
-      </c>
-      <c r="P81" s="66">
-        <f t="shared" si="34"/>
         <v>1.3799326074567764E-2</v>
       </c>
     </row>
@@ -13115,31 +13266,31 @@
         <v>15612839.249600001</v>
       </c>
       <c r="J82" s="66">
+        <f t="shared" si="23"/>
+        <v>0.79926049658369536</v>
+      </c>
+      <c r="K82" s="66">
+        <f t="shared" si="24"/>
+        <v>0.28758571720654441</v>
+      </c>
+      <c r="L82" s="66">
+        <f t="shared" si="25"/>
+        <v>0.26178050008476395</v>
+      </c>
+      <c r="M82" s="66">
+        <f t="shared" si="26"/>
+        <v>2.6403293552388674E-2</v>
+      </c>
+      <c r="N82" s="66">
+        <f t="shared" si="27"/>
+        <v>2.7553123176029714E-2</v>
+      </c>
+      <c r="O82" s="66">
         <f t="shared" si="28"/>
-        <v>0.79926049658369536</v>
-      </c>
-      <c r="K82" s="66">
+        <v>7.3220391685833545E-3</v>
+      </c>
+      <c r="P82" s="66">
         <f t="shared" si="29"/>
-        <v>0.28758571720654441</v>
-      </c>
-      <c r="L82" s="66">
-        <f t="shared" si="30"/>
-        <v>0.26178050008476395</v>
-      </c>
-      <c r="M82" s="66">
-        <f t="shared" si="31"/>
-        <v>2.6403293552388674E-2</v>
-      </c>
-      <c r="N82" s="66">
-        <f t="shared" si="32"/>
-        <v>2.7553123176029714E-2</v>
-      </c>
-      <c r="O82" s="66">
-        <f t="shared" si="33"/>
-        <v>7.3220391685833545E-3</v>
-      </c>
-      <c r="P82" s="66">
-        <f t="shared" si="34"/>
         <v>1.3010186528292274E-2</v>
       </c>
     </row>
@@ -13172,56 +13323,57 @@
         <v>1412663.2752100001</v>
       </c>
       <c r="J83" s="66">
+        <f t="shared" si="23"/>
+        <v>1.0211221647431006</v>
+      </c>
+      <c r="K83" s="66">
+        <f t="shared" si="24"/>
+        <v>0.99002326543809449</v>
+      </c>
+      <c r="L83" s="66">
+        <f t="shared" si="25"/>
+        <v>0.98722786714323163</v>
+      </c>
+      <c r="M83" s="66">
+        <f t="shared" si="26"/>
+        <v>2.5130067935526221E-2</v>
+      </c>
+      <c r="N83" s="66">
+        <f t="shared" si="27"/>
+        <v>0.15743995148309958</v>
+      </c>
+      <c r="O83" s="66">
         <f t="shared" si="28"/>
-        <v>1.0211221647431006</v>
-      </c>
-      <c r="K83" s="66">
+        <v>3.2319931087617028E-2</v>
+      </c>
+      <c r="P83" s="66">
         <f t="shared" si="29"/>
-        <v>0.99002326543809449</v>
-      </c>
-      <c r="L83" s="66">
-        <f t="shared" si="30"/>
-        <v>0.98722786714323163</v>
-      </c>
-      <c r="M83" s="66">
-        <f t="shared" si="31"/>
-        <v>2.5130067935526221E-2</v>
-      </c>
-      <c r="N83" s="66">
-        <f t="shared" si="32"/>
-        <v>0.15743995148309958</v>
-      </c>
-      <c r="O83" s="66">
-        <f t="shared" si="33"/>
-        <v>3.2319931087617028E-2</v>
-      </c>
-      <c r="P83" s="66">
-        <f t="shared" si="34"/>
         <v>2.5963681417960943E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="21">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="M41:O41"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="P57:T57"/>
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="D74:E74"/>
     <mergeCell ref="F74:G74"/>
     <mergeCell ref="H74:I74"/>
     <mergeCell ref="M74:O74"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="M57:O57"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="M41:O41"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="M6:O6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13229,10 +13381,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819BCD50-CCED-4858-989E-30CB05A9C1BE}">
-  <dimension ref="A1:P79"/>
+  <dimension ref="A1:T79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
+      <selection activeCell="R57" sqref="R57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -13248,6 +13400,7 @@
     <col min="9" max="9" width="17.06640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.3984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.53125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.45">
@@ -15063,7 +15216,7 @@
         <v>3.2045527585561561E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A49" s="66" t="s">
         <v>20</v>
       </c>
@@ -15120,17 +15273,17 @@
         <v>5.9837166680413913E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A52" s="72" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A53" s="73" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:20" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A54" s="73"/>
       <c r="B54" s="105" t="s">
         <v>24</v>
@@ -15148,23 +15301,31 @@
         <v>114</v>
       </c>
       <c r="I54" s="106"/>
-      <c r="J54" s="76" t="s">
+      <c r="J54" s="104" t="s">
+        <v>257</v>
+      </c>
+      <c r="K54" s="104"/>
+      <c r="L54" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="K54" s="76" t="s">
+      <c r="M54" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="L54" s="77" t="s">
+      <c r="N54" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="M54" s="105" t="s">
+      <c r="O54" s="71" t="s">
+        <v>256</v>
+      </c>
+      <c r="P54" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="N54" s="105"/>
-      <c r="O54" s="105"/>
-      <c r="P54" s="73"/>
-    </row>
-    <row r="55" spans="1:16" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="Q54" s="105"/>
+      <c r="R54" s="105"/>
+      <c r="S54" s="105"/>
+      <c r="T54" s="105"/>
+    </row>
+    <row r="55" spans="1:20" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A55" s="76" t="s">
         <v>23</v>
       </c>
@@ -15192,23 +15353,32 @@
       <c r="I55" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="J55" s="76"/>
-      <c r="K55" s="76"/>
-      <c r="L55" s="73"/>
-      <c r="M55" s="76" t="s">
+      <c r="J55" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="K55" s="76" t="s">
+        <v>26</v>
+      </c>
+      <c r="L55" s="76"/>
+      <c r="M55" s="76"/>
+      <c r="N55" s="73"/>
+      <c r="P55" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="N55" s="76" t="s">
+      <c r="Q55" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="O55" s="76" t="s">
+      <c r="R55" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="P55" s="78" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="S55" s="71" t="s">
+        <v>258</v>
+      </c>
+      <c r="T55" s="71" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A56" s="73" t="s">
         <v>1</v>
       </c>
@@ -15236,36 +15406,50 @@
       <c r="I56" s="79">
         <v>6989132626.8100004</v>
       </c>
-      <c r="J56" s="79">
-        <f>D56/B56</f>
+      <c r="J56" s="89">
+        <v>944650499294</v>
+      </c>
+      <c r="K56" s="89">
+        <v>2210716835.1999998</v>
+      </c>
+      <c r="L56" s="79">
+        <f t="shared" ref="L56:L63" si="21">D56/B56</f>
         <v>0.99588141232567873</v>
       </c>
-      <c r="K56" s="79">
-        <f>F56/B56</f>
+      <c r="M56" s="79">
+        <f t="shared" ref="M56:M63" si="22">F56/B56</f>
         <v>0.99092724162960999</v>
       </c>
-      <c r="L56" s="79">
-        <f>H56/B56</f>
+      <c r="N56" s="79">
+        <f t="shared" ref="N56:N63" si="23">H56/B56</f>
         <v>0.99360812718567915</v>
       </c>
-      <c r="M56" s="79">
-        <f>C56/B56</f>
+      <c r="O56" s="89">
+        <f>J56/B56</f>
+        <v>0.99336343529623439</v>
+      </c>
+      <c r="P56" s="79">
+        <f t="shared" ref="P56:P63" si="24">C56/B56</f>
         <v>3.5150684809195187E-3</v>
       </c>
-      <c r="N56" s="79">
-        <f>E56/B56</f>
+      <c r="Q56" s="79">
+        <f t="shared" ref="Q56:Q63" si="25">E56/B56</f>
         <v>4.9119770739314856E-3</v>
       </c>
-      <c r="O56" s="79">
-        <f>G56/B56</f>
+      <c r="R56" s="79">
+        <f t="shared" ref="R56:R63" si="26">G56/B56</f>
         <v>1.8995479784546037E-3</v>
       </c>
-      <c r="P56" s="79">
-        <f>I56/B56</f>
+      <c r="S56" s="79">
+        <f t="shared" ref="S56:S63" si="27">I56/B56</f>
         <v>7.3495422921998699E-3</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="T56" s="89">
+        <f>K56/B56</f>
+        <v>2.3247172065464861E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A57" s="73" t="s">
         <v>2</v>
       </c>
@@ -15293,36 +15477,50 @@
       <c r="I57" s="79">
         <v>10497091805.6</v>
       </c>
-      <c r="J57" s="79">
-        <f t="shared" ref="J57:J63" si="21">D57/B57</f>
+      <c r="J57" s="89">
+        <v>1127172832440</v>
+      </c>
+      <c r="K57" s="89">
+        <v>910911070.87199998</v>
+      </c>
+      <c r="L57" s="79">
+        <f t="shared" si="21"/>
         <v>1.0059484718001523</v>
       </c>
-      <c r="K57" s="79">
-        <f t="shared" ref="K57:K63" si="22">F57/B57</f>
+      <c r="M57" s="79">
+        <f t="shared" si="22"/>
         <v>0.94756235202180572</v>
       </c>
-      <c r="L57" s="79">
-        <f t="shared" ref="L57:L63" si="23">H57/B57</f>
+      <c r="N57" s="79">
+        <f t="shared" si="23"/>
         <v>0.95768295161371098</v>
       </c>
-      <c r="M57" s="79">
-        <f t="shared" ref="M57:M63" si="24">C57/B57</f>
+      <c r="O57" s="89">
+        <f t="shared" ref="O57:O63" si="28">J57/B57</f>
+        <v>0.94203191484486637</v>
+      </c>
+      <c r="P57" s="79">
+        <f t="shared" si="24"/>
         <v>3.2283320234473773E-3</v>
       </c>
-      <c r="N57" s="79">
-        <f t="shared" ref="N57:N63" si="25">E57/B57</f>
+      <c r="Q57" s="79">
+        <f t="shared" si="25"/>
         <v>8.1780096950417776E-3</v>
       </c>
-      <c r="O57" s="79">
-        <f t="shared" ref="O57:O63" si="26">G57/B57</f>
+      <c r="R57" s="79">
+        <f t="shared" si="26"/>
         <v>1.5056313778154947E-3</v>
       </c>
-      <c r="P57" s="79">
-        <f t="shared" ref="P57:P63" si="27">I57/B57</f>
+      <c r="S57" s="79">
+        <f t="shared" si="27"/>
         <v>8.7729185882929796E-3</v>
       </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="T57" s="89">
+        <f t="shared" ref="T57:T63" si="29">K57/B57</f>
+        <v>7.6129168096554121E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A58" s="73" t="s">
         <v>35</v>
       </c>
@@ -15350,36 +15548,50 @@
       <c r="I58" s="79">
         <v>3682064.03516</v>
       </c>
-      <c r="J58" s="79">
+      <c r="J58" s="89">
+        <v>19356565.800000001</v>
+      </c>
+      <c r="K58" s="89">
+        <v>761415.23543500004</v>
+      </c>
+      <c r="L58" s="79">
         <f t="shared" si="21"/>
         <v>0.96380092675912898</v>
       </c>
-      <c r="K58" s="79">
+      <c r="M58" s="79">
         <f t="shared" si="22"/>
         <v>0.21845503069570318</v>
       </c>
-      <c r="L58" s="79">
+      <c r="N58" s="79">
         <f t="shared" si="23"/>
         <v>0.2821552733267102</v>
       </c>
-      <c r="M58" s="79">
+      <c r="O58" s="107">
+        <f t="shared" si="28"/>
+        <v>4.9918572695616989E-2</v>
+      </c>
+      <c r="P58" s="79">
         <f t="shared" si="24"/>
         <v>1.6528423573692028E-2</v>
       </c>
-      <c r="N58" s="79">
+      <c r="Q58" s="79">
         <f t="shared" si="25"/>
         <v>3.086180726612733E-2</v>
       </c>
-      <c r="O58" s="79">
+      <c r="R58" s="79">
         <f t="shared" si="26"/>
         <v>1.0103340374041279E-2</v>
       </c>
-      <c r="P58" s="79">
+      <c r="S58" s="79">
         <f t="shared" si="27"/>
         <v>9.4956607028428199E-3</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="T58" s="89">
+        <f t="shared" si="29"/>
+        <v>1.9636108065002097E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A59" s="73" t="s">
         <v>36</v>
       </c>
@@ -15407,36 +15619,50 @@
       <c r="I59" s="79">
         <v>1204122.4476600001</v>
       </c>
-      <c r="J59" s="79">
+      <c r="J59" s="89">
+        <v>83903431.799999997</v>
+      </c>
+      <c r="K59" s="89">
+        <v>958651.13287600002</v>
+      </c>
+      <c r="L59" s="79">
         <f t="shared" si="21"/>
         <v>0.90216149308515836</v>
       </c>
-      <c r="K59" s="79">
+      <c r="M59" s="79">
         <f t="shared" si="22"/>
         <v>0.3768845633124922</v>
       </c>
-      <c r="L59" s="79">
+      <c r="N59" s="79">
         <f t="shared" si="23"/>
         <v>0.36767117818944972</v>
       </c>
-      <c r="M59" s="79">
+      <c r="O59" s="107">
+        <f t="shared" si="28"/>
+        <v>0.42435259228752226</v>
+      </c>
+      <c r="P59" s="79">
         <f t="shared" si="24"/>
         <v>1.6217969721039852E-2</v>
       </c>
-      <c r="N59" s="79">
+      <c r="Q59" s="79">
         <f t="shared" si="25"/>
         <v>3.5486761994337652E-2</v>
       </c>
-      <c r="O59" s="79">
+      <c r="R59" s="79">
         <f t="shared" si="26"/>
         <v>3.0519206456502464E-3</v>
       </c>
-      <c r="P59" s="79">
+      <c r="S59" s="79">
         <f t="shared" si="27"/>
         <v>6.090006941719843E-3</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="T59" s="89">
+        <f t="shared" si="29"/>
+        <v>4.8485036262283206E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A60" s="73" t="s">
         <v>15</v>
       </c>
@@ -15464,36 +15690,50 @@
       <c r="I60" s="79">
         <v>676041009.45899999</v>
       </c>
-      <c r="J60" s="79">
+      <c r="J60" s="89">
+        <v>50887462587.400002</v>
+      </c>
+      <c r="K60" s="89">
+        <v>246650670.877</v>
+      </c>
+      <c r="L60" s="79">
         <f t="shared" si="21"/>
         <v>0.96903474252772026</v>
       </c>
-      <c r="K60" s="79">
+      <c r="M60" s="79">
         <f t="shared" si="22"/>
         <v>0.98483100398474244</v>
       </c>
-      <c r="L60" s="79">
+      <c r="N60" s="79">
         <f t="shared" si="23"/>
         <v>0.95805536413609826</v>
       </c>
-      <c r="M60" s="79">
+      <c r="O60" s="89">
+        <f t="shared" si="28"/>
+        <v>0.9853043798041492</v>
+      </c>
+      <c r="P60" s="79">
         <f t="shared" si="24"/>
         <v>8.2806614674977592E-3</v>
       </c>
-      <c r="N60" s="79">
+      <c r="Q60" s="79">
         <f t="shared" si="25"/>
         <v>4.9580547575734666E-3</v>
       </c>
-      <c r="O60" s="79">
+      <c r="R60" s="79">
         <f t="shared" si="26"/>
         <v>4.9421968160537092E-3</v>
       </c>
-      <c r="P60" s="79">
+      <c r="S60" s="79">
         <f t="shared" si="27"/>
         <v>1.3089789383841323E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="T60" s="89">
+        <f t="shared" si="29"/>
+        <v>4.7757536717288459E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A61" s="73" t="s">
         <v>4</v>
       </c>
@@ -15521,36 +15761,50 @@
       <c r="I61" s="79">
         <v>104743077.28399999</v>
       </c>
-      <c r="J61" s="79">
+      <c r="J61" s="89">
+        <v>3117494396.8000002</v>
+      </c>
+      <c r="K61" s="89">
+        <v>129994248.771</v>
+      </c>
+      <c r="L61" s="79">
         <f t="shared" si="21"/>
         <v>0.94469744673390132</v>
       </c>
-      <c r="K61" s="79">
+      <c r="M61" s="79">
         <f t="shared" si="22"/>
         <v>0.29466756956271822</v>
       </c>
-      <c r="L61" s="79">
+      <c r="N61" s="79">
         <f t="shared" si="23"/>
         <v>0.38277691547795289</v>
       </c>
-      <c r="M61" s="79">
+      <c r="O61" s="89">
+        <f t="shared" si="28"/>
+        <v>0.14752564746688671</v>
+      </c>
+      <c r="P61" s="79">
         <f t="shared" si="24"/>
         <v>2.275659059891718E-2</v>
       </c>
-      <c r="N61" s="79">
+      <c r="Q61" s="79">
         <f t="shared" si="25"/>
         <v>9.8580753532644672E-3</v>
       </c>
-      <c r="O61" s="79">
+      <c r="R61" s="79">
         <f t="shared" si="26"/>
         <v>9.6764378341133751E-3</v>
       </c>
-      <c r="P61" s="79">
+      <c r="S61" s="79">
         <f t="shared" si="27"/>
         <v>4.9566377119578762E-3</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="T61" s="89">
+        <f t="shared" si="29"/>
+        <v>6.1515702278722101E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A62" s="73" t="s">
         <v>6</v>
       </c>
@@ -15578,36 +15832,50 @@
       <c r="I62" s="79">
         <v>250072949.72400001</v>
       </c>
-      <c r="J62" s="79">
+      <c r="J62" s="89">
+        <v>5890316559.3999996</v>
+      </c>
+      <c r="K62" s="89">
+        <v>85332909.139300004</v>
+      </c>
+      <c r="L62" s="79">
         <f t="shared" si="21"/>
         <v>0.9442762311353079</v>
       </c>
-      <c r="K62" s="79">
+      <c r="M62" s="79">
         <f t="shared" si="22"/>
         <v>0.41434324900610719</v>
       </c>
-      <c r="L62" s="79">
+      <c r="N62" s="79">
         <f t="shared" si="23"/>
         <v>0.40083074332271823</v>
       </c>
-      <c r="M62" s="79">
+      <c r="O62" s="89">
+        <f t="shared" si="28"/>
+        <v>0.49260287600529862</v>
+      </c>
+      <c r="P62" s="79">
         <f t="shared" si="24"/>
         <v>1.5066597658470026E-2</v>
       </c>
-      <c r="N62" s="79">
+      <c r="Q62" s="79">
         <f t="shared" si="25"/>
         <v>8.5005017896467427E-3</v>
       </c>
-      <c r="O62" s="79">
+      <c r="R62" s="79">
         <f t="shared" si="26"/>
         <v>6.0953616896922656E-3</v>
       </c>
-      <c r="P62" s="79">
+      <c r="S62" s="79">
         <f t="shared" si="27"/>
         <v>2.0913418320206361E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="T62" s="89">
+        <f t="shared" si="29"/>
+        <v>7.1363289283385839E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A63" s="73" t="s">
         <v>20</v>
       </c>
@@ -15635,36 +15903,50 @@
       <c r="I63" s="79">
         <v>554303853.73599994</v>
       </c>
-      <c r="J63" s="79">
+      <c r="J63" s="89">
+        <v>63285963155.199997</v>
+      </c>
+      <c r="K63" s="89">
+        <v>182338858.338</v>
+      </c>
+      <c r="L63" s="79">
         <f t="shared" si="21"/>
         <v>0.99475869167285502</v>
       </c>
-      <c r="K63" s="79">
+      <c r="M63" s="79">
         <f t="shared" si="22"/>
         <v>0.9874814025756683</v>
       </c>
-      <c r="L63" s="79">
+      <c r="N63" s="79">
         <f t="shared" si="23"/>
         <v>1.0003901822329806</v>
       </c>
-      <c r="M63" s="79">
+      <c r="O63" s="89">
+        <f t="shared" si="28"/>
+        <v>0.99294922151092402</v>
+      </c>
+      <c r="P63" s="79">
         <f t="shared" si="24"/>
         <v>1.1027331882122776E-3</v>
       </c>
-      <c r="N63" s="79">
+      <c r="Q63" s="79">
         <f t="shared" si="25"/>
         <v>1.6594323301339551E-3</v>
       </c>
-      <c r="O63" s="79">
+      <c r="R63" s="79">
         <f t="shared" si="26"/>
         <v>1.853510495035043E-3</v>
       </c>
-      <c r="P63" s="79">
+      <c r="S63" s="79">
         <f t="shared" si="27"/>
         <v>8.696961420937812E-3</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="T63" s="89">
+        <f t="shared" si="29"/>
+        <v>2.8608749620180379E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A64" s="73"/>
       <c r="B64" s="73"/>
       <c r="C64" s="73"/>
@@ -15922,31 +16204,31 @@
         <v>8461901884.1800003</v>
       </c>
       <c r="J73" s="66">
-        <f t="shared" ref="J73:J79" si="28">D73/B73</f>
+        <f t="shared" ref="J73:J79" si="30">D73/B73</f>
         <v>1.0094562549662873</v>
       </c>
       <c r="K73" s="66">
-        <f t="shared" ref="K73:K79" si="29">F73/B73</f>
+        <f t="shared" ref="K73:K79" si="31">F73/B73</f>
         <v>0.9671215656845743</v>
       </c>
       <c r="L73" s="66">
-        <f t="shared" ref="L73:L79" si="30">H73/B73</f>
+        <f t="shared" ref="L73:L79" si="32">H73/B73</f>
         <v>0.97077908181122374</v>
       </c>
       <c r="M73" s="66">
-        <f t="shared" ref="M73:M79" si="31">C73/B73</f>
+        <f t="shared" ref="M73:M79" si="33">C73/B73</f>
         <v>1.346300037895685E-3</v>
       </c>
       <c r="N73" s="66">
-        <f t="shared" ref="N73:N79" si="32">E73/B73</f>
+        <f t="shared" ref="N73:N79" si="34">E73/B73</f>
         <v>8.8724391134134273E-3</v>
       </c>
       <c r="O73" s="66">
-        <f t="shared" ref="O73:O79" si="33">G73/B73</f>
+        <f t="shared" ref="O73:O79" si="35">G73/B73</f>
         <v>8.0843775352822231E-4</v>
       </c>
       <c r="P73" s="66">
-        <f t="shared" ref="P73:P79" si="34">I73/B73</f>
+        <f t="shared" ref="P73:P79" si="36">I73/B73</f>
         <v>7.2454012088226626E-3</v>
       </c>
     </row>
@@ -15979,31 +16261,31 @@
         <v>3555898.5149500002</v>
       </c>
       <c r="J74" s="66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>0.98394620624352536</v>
       </c>
       <c r="K74" s="66">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.23923793460221385</v>
       </c>
       <c r="L74" s="66">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.29450899003339137</v>
       </c>
       <c r="M74" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1.8705803737899446E-2</v>
       </c>
       <c r="N74" s="66">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>5.4873433909189195E-2</v>
       </c>
       <c r="O74" s="66">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>2.5755946355347326E-2</v>
       </c>
       <c r="P74" s="66">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>9.6573819129900321E-3</v>
       </c>
     </row>
@@ -16036,31 +16318,31 @@
         <v>2739627.79629</v>
       </c>
       <c r="J75" s="66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>0.96872726080145488</v>
       </c>
       <c r="K75" s="66">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.35047408692049925</v>
       </c>
       <c r="L75" s="66">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.31463162231527936</v>
       </c>
       <c r="M75" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1.527401774183961E-2</v>
       </c>
       <c r="N75" s="66">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>7.7950682977546815E-2</v>
       </c>
       <c r="O75" s="66">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>7.5247732316139817E-3</v>
       </c>
       <c r="P75" s="66">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>1.5712232693664872E-2</v>
       </c>
     </row>
@@ -16093,31 +16375,31 @@
         <v>1672872144.6199999</v>
       </c>
       <c r="J76" s="66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>0.98284759547029499</v>
       </c>
       <c r="K76" s="66">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>1.0067082538664813</v>
       </c>
       <c r="L76" s="66">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.97837714925019725</v>
       </c>
       <c r="M76" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>6.4476652945862087E-3</v>
       </c>
       <c r="N76" s="66">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>1.6824003799355544E-2</v>
       </c>
       <c r="O76" s="66">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>5.0676325097519601E-3</v>
       </c>
       <c r="P76" s="66">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>3.2981786178777221E-2</v>
       </c>
     </row>
@@ -16150,31 +16432,31 @@
         <v>215072134.37099999</v>
       </c>
       <c r="J77" s="66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>0.9356013083638639</v>
       </c>
       <c r="K77" s="66">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.29882809452770503</v>
       </c>
       <c r="L77" s="66">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.38405980306350745</v>
       </c>
       <c r="M77" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>2.6022480398996833E-2</v>
       </c>
       <c r="N77" s="66">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>3.4640422932770171E-2</v>
       </c>
       <c r="O77" s="66">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>1.2445591937164885E-2</v>
       </c>
       <c r="P77" s="66">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>1.0409780317991439E-2</v>
       </c>
     </row>
@@ -16207,31 +16489,31 @@
         <v>335819862.37699997</v>
       </c>
       <c r="J78" s="66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>0.96271978203603858</v>
       </c>
       <c r="K78" s="66">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.38730105438735418</v>
       </c>
       <c r="L78" s="66">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.36957921312384739</v>
       </c>
       <c r="M78" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1.4322671783473682E-2</v>
       </c>
       <c r="N78" s="66">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>5.1252841937856744E-2</v>
       </c>
       <c r="O78" s="66">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>5.5295311611507636E-3</v>
       </c>
       <c r="P78" s="66">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>3.1795331807251317E-2</v>
       </c>
     </row>
@@ -16264,53 +16546,55 @@
         <v>211962712.59099999</v>
       </c>
       <c r="J79" s="66">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>1.0109014791619471</v>
       </c>
       <c r="K79" s="66">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>1.0110817585905076</v>
       </c>
       <c r="L79" s="66">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>1.0038224304216925</v>
       </c>
       <c r="M79" s="66">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>2.7885031734984729E-3</v>
       </c>
       <c r="N79" s="66">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>4.7706937895843488E-3</v>
       </c>
       <c r="O79" s="66">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>2.9660426848415232E-3</v>
       </c>
       <c r="P79" s="66">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>3.86645399724649E-3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="M40:O40"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="P54:T54"/>
     <mergeCell ref="B70:C70"/>
     <mergeCell ref="D70:E70"/>
     <mergeCell ref="F70:G70"/>
     <mergeCell ref="H70:I70"/>
     <mergeCell ref="M70:O70"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="M40:O40"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="F54:G54"/>
     <mergeCell ref="H54:I54"/>
-    <mergeCell ref="M54:O54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -26026,6 +26310,19 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B103:C103"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="B3:C3"/>
@@ -26034,19 +26331,6 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D69:E69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
added results for microbenchmark
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="210" documentId="9E001895F985C8961FD5BD0910042522F195CEDD" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{8CFC7A8E-F9B6-47B0-8748-066C7703C391}"/>
+  <xr:revisionPtr revIDLastSave="252" documentId="9E001895F985C8961FD5BD0910042522F195CEDD" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{692A55FC-7DBB-4090-973E-0E00558FBA54}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clang-os" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="275">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -880,6 +880,15 @@
   </si>
   <si>
     <t>Conclusion: (1) The TLB hierarchy is inclusive. (2) A lot of ITLB flushes are involved.</t>
+  </si>
+  <si>
+    <t>kern.hz = 1000</t>
+  </si>
+  <si>
+    <t>kern.hz = 100</t>
+  </si>
+  <si>
+    <t>5E+10 iterations, 1 code page, 1 data page</t>
   </si>
 </sst>
 </file>
@@ -8926,7 +8935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CDBF21-342B-4234-A56D-2C760D6B9FBB}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -13544,7 +13553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819BCD50-CCED-4858-989E-30CB05A9C1BE}">
   <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="M75" sqref="M75"/>
     </sheetView>
   </sheetViews>
@@ -16888,16 +16897,17 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E42A5A-17BB-451B-A796-6BF4F5724A44}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" customWidth="1"/>
-    <col min="3" max="4" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.796875" customWidth="1"/>
+    <col min="2" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.86328125" customWidth="1"/>
   </cols>
@@ -16922,7 +16932,11 @@
         <v>269</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="65" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="5" spans="1:6" s="65" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="65" t="s">
+        <v>272</v>
+      </c>
+    </row>
     <row r="6" spans="1:6" s="65" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="65" t="s">
         <v>208</v>
@@ -16932,6 +16946,9 @@
       <c r="A7" t="s">
         <v>264</v>
       </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
       <c r="C7">
         <v>10</v>
       </c>
@@ -16996,86 +17013,240 @@
         <v>149267</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" s="65" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="C11" s="89"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="57" x14ac:dyDescent="0.45">
-      <c r="A12" s="65" t="s">
+    <row r="13" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A13" s="65" t="s">
         <v>264</v>
       </c>
-      <c r="B12" s="65"/>
-      <c r="C12" s="65">
+      <c r="B13" s="65">
+        <v>1</v>
+      </c>
+      <c r="C13" s="65">
         <v>10</v>
       </c>
-      <c r="D12" s="65">
+      <c r="D13" s="65">
         <v>20</v>
       </c>
-      <c r="E12" s="65">
+      <c r="E13" s="65">
         <v>768</v>
       </c>
-      <c r="F12" s="80" t="s">
+      <c r="F13" s="80" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="89" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="89" t="s">
         <v>37</v>
-      </c>
-      <c r="B13" s="65"/>
-      <c r="C13" s="89">
-        <v>223</v>
-      </c>
-      <c r="D13" s="89">
-        <v>2000</v>
-      </c>
-      <c r="E13" s="89">
-        <v>1379366</v>
-      </c>
-      <c r="F13" s="89">
-        <v>1752433</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="65" t="s">
-        <v>22</v>
       </c>
       <c r="B14" s="65"/>
       <c r="C14" s="89">
-        <v>54</v>
+        <v>223</v>
       </c>
       <c r="D14" s="89">
-        <v>280</v>
+        <v>2000</v>
       </c>
       <c r="E14" s="89">
-        <v>16203</v>
+        <v>1379366</v>
       </c>
       <c r="F14" s="89">
-        <v>13502</v>
+        <v>1752433</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="65" t="s">
-        <v>266</v>
+        <v>22</v>
       </c>
       <c r="B15" s="65"/>
       <c r="C15" s="89">
+        <v>54</v>
+      </c>
+      <c r="D15" s="89">
+        <v>280</v>
+      </c>
+      <c r="E15" s="89">
+        <v>16203</v>
+      </c>
+      <c r="F15" s="89">
+        <v>13502</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="65" t="s">
+        <v>266</v>
+      </c>
+      <c r="B16" s="65"/>
+      <c r="C16" s="89">
         <v>116</v>
       </c>
-      <c r="D15" s="89">
+      <c r="D16" s="89">
         <v>190</v>
       </c>
-      <c r="E15" s="89">
+      <c r="E16" s="89">
         <v>5892</v>
       </c>
-      <c r="F15" s="89">
+      <c r="F16" s="89">
         <v>7657</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>271</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="65" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="65" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="65" t="s">
+        <v>264</v>
+      </c>
+      <c r="E22" s="65">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" s="89" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="89">
+        <v>43867</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="89">
+        <v>32050</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" s="65" t="s">
+        <v>266</v>
+      </c>
+      <c r="E25" s="89">
+        <v>69518</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" s="65" t="s">
+        <v>209</v>
+      </c>
+      <c r="B27" s="65"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" s="65" t="s">
+        <v>264</v>
+      </c>
+      <c r="B28" s="65"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" s="89" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="65"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="89">
+        <v>1387929</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="89">
+        <v>16231</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" s="65" t="s">
+        <v>266</v>
+      </c>
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="89">
+        <v>5877</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
+        <v>208</v>
+      </c>
+      <c r="C35" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" s="65" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" s="89" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="89">
+        <v>57122</v>
+      </c>
+      <c r="C37" s="89">
+        <v>15050</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="89">
+        <v>39617</v>
+      </c>
+      <c r="C38" s="89">
+        <v>19567</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" s="65" t="s">
+        <v>266</v>
+      </c>
+      <c r="B39" s="89">
+        <v>84892</v>
+      </c>
+      <c r="C39" s="89">
+        <v>7115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added results for the microbenchmark
</commit_message>
<xml_diff>
--- a/shared_ptp.xlsx
+++ b/shared_ptp.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="252" documentId="9E001895F985C8961FD5BD0910042522F195CEDD" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{692A55FC-7DBB-4090-973E-0E00558FBA54}"/>
+  <xr:revisionPtr revIDLastSave="321" documentId="9E001895F985C8961FD5BD0910042522F195CEDD" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{DDC29808-40F3-46F3-84E0-688313965091}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9465" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="276">
   <si>
     <t>PAGE_FAULT.ALL</t>
   </si>
@@ -889,6 +889,9 @@
   </si>
   <si>
     <t>5E+10 iterations, 1 code page, 1 data page</t>
+  </si>
+  <si>
+    <t># of iterations</t>
   </si>
 </sst>
 </file>
@@ -1107,7 +1110,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1312,6 +1315,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -16897,18 +16901,18 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E42A5A-17BB-451B-A796-6BF4F5724A44}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34.796875" customWidth="1"/>
-    <col min="2" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.86328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17198,55 +17202,179 @@
         <v>5877</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B35" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
         <v>208</v>
       </c>
-      <c r="C35" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="65" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+        <v>275</v>
+      </c>
+      <c r="B36" s="108">
+        <v>10000000000</v>
+      </c>
+      <c r="C36" s="108">
+        <v>20000000000</v>
+      </c>
+      <c r="D36" s="108">
+        <v>40000000000</v>
+      </c>
+      <c r="E36" s="108">
+        <v>80000000000</v>
+      </c>
+      <c r="F36" s="108">
+        <v>160000000000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="89" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="89">
-        <v>57122</v>
+        <v>9856</v>
       </c>
       <c r="C37" s="89">
-        <v>15050</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+        <v>19853</v>
+      </c>
+      <c r="D37" s="89">
+        <v>40033</v>
+      </c>
+      <c r="E37" s="89">
+        <v>81070</v>
+      </c>
+      <c r="F37" s="89">
+        <v>161931</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="65" t="s">
         <v>22</v>
       </c>
       <c r="B38" s="89">
-        <v>39617</v>
+        <v>6985</v>
       </c>
       <c r="C38" s="89">
-        <v>19567</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+        <v>13976</v>
+      </c>
+      <c r="D38" s="89">
+        <v>27834</v>
+      </c>
+      <c r="E38" s="89">
+        <v>55557</v>
+      </c>
+      <c r="F38" s="89">
+        <v>111007</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="65" t="s">
         <v>266</v>
       </c>
       <c r="B39" s="89">
-        <v>84892</v>
+        <v>24624</v>
       </c>
       <c r="C39" s="89">
-        <v>7115</v>
+        <v>48771</v>
+      </c>
+      <c r="D39" s="89">
+        <v>96873</v>
+      </c>
+      <c r="E39" s="89">
+        <v>196563</v>
+      </c>
+      <c r="F39" s="89">
+        <v>387181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" s="65" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="65" t="s">
+        <v>275</v>
+      </c>
+      <c r="B42" s="108">
+        <v>10000000000</v>
+      </c>
+      <c r="C42" s="108">
+        <v>20000000000</v>
+      </c>
+      <c r="D42" s="108">
+        <v>40000000000</v>
+      </c>
+      <c r="E42" s="108">
+        <v>80000000000</v>
+      </c>
+      <c r="F42" s="108">
+        <v>160000000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="89" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="89">
+        <v>3392</v>
+      </c>
+      <c r="C43" s="89">
+        <v>5354</v>
+      </c>
+      <c r="D43" s="89">
+        <v>10674</v>
+      </c>
+      <c r="E43" s="89">
+        <v>21389</v>
+      </c>
+      <c r="F43" s="89">
+        <v>42728</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="89">
+        <v>3508</v>
+      </c>
+      <c r="C44" s="89">
+        <v>6990</v>
+      </c>
+      <c r="D44" s="89">
+        <v>13979</v>
+      </c>
+      <c r="E44" s="89">
+        <v>27968</v>
+      </c>
+      <c r="F44" s="89">
+        <v>55818</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="65" t="s">
+        <v>266</v>
+      </c>
+      <c r="B45" s="89">
+        <v>2671</v>
+      </c>
+      <c r="C45" s="89">
+        <v>2595</v>
+      </c>
+      <c r="D45" s="89">
+        <v>5209</v>
+      </c>
+      <c r="E45" s="89">
+        <v>10151</v>
+      </c>
+      <c r="F45" s="89">
+        <v>20364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>